<commit_message>
fixed some text regexp bugs, now text comes out much cleaner.
</commit_message>
<xml_diff>
--- a/mapp/server/SheetWithDataFetched.xlsx
+++ b/mapp/server/SheetWithDataFetched.xlsx
@@ -372,7 +372,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:E28"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
@@ -393,16 +393,7 @@
         <v>App</v>
       </c>
       <c r="C2" t="str">
-        <v>WhatsApp :: Home WhatsApp Messenger :: cross-platform mobile messaging app for iPhone, BlackBerry, Android, Windows Phone and Nokia. Send text, video, images, audio for free. WhatsApp Simple. Personal.Real Time Messaging. Download WhatsApp How it works Why we don't sell ads WhatsApp for your phone Help Translate WhatsApp Share WhatsApp with Friends About WhatsApp WhatsApp Get in touch Download Home Download WhatsApp Web FAQ Blog Contact Azərbaycanca Bahasa Indonesia Bahasa Melayu Català Česky Dansk Deutsch eesti English Español Français Hrvatski Italiano Latviešu Lietuviškai Magyar Nederlands Norsk Pilipino Polski Português Română Slovenčina Slovenščina suomi Tiếng Việt Türkçe Ελληνικά Български Македонски Pусский српски Oʻzbekcha Українська ‏עברית‏ العربية فارسی বাংলা  हिंदी ગુજરાતી தமிழ் ภาษาไทย 简体中文 繁體中文 日本語 한국어 Help translate WhatsApp into your language                                 Group Chats                                                          Send photos &amp; videos                                                         Share locations                                                           iPhone                                        BlackBerry                                    Nokia S40                                    Symbian                                    Windows Phone     for iPhone for Android for BlackBerry for Nokia for Windows Phone About Jobs Press Brand Center Privacy &amp; Terms Open Source Contact Us Facebook Twitter for iPhone for Android for BlackBerry for Nokia S60 for Nokia S40 for Windows Phone JavaScript seem to be disabled in your browser. You better have JavaScript enabled to utilize the functionality of this website. WhatsApp Messenger is a cross-platform mobile messaging app which allows you to exchange messages without having to pay for SMS. WhatsApp Messenger is available for iPhone, BlackBerry, Android, Windows Phone and Nokia and yes, those phones can all message each other! Because WhatsApp Messenger uses the same internet data plan that you use for email and web browsing, there is no cost to message and stay in touch with your friends. In addition to basic messaging WhatsApp users can create groups, send each other unlimited images, video and audio media messages.                                     Advertising has us chasing cars and clothes, working jobs we hate so we can buy shit we dont need. - Tyler Durden, Fight Club                                                    Brian and I spent a combined 20 years at Yahoo! working hard to keep the site working. And yes, working hard to sell ads, because that's what Yahoo! did. It gathered data and it served pages and it sold ads. We watched Yahoo! get eclipsed in size by Google...                 Read more in our blog WhatsApp Messenger is a cross-platform mobile messaging app which allows you to exchange messages without having to pay for SMS. WhatsApp Messenger is available for iPhone, BlackBerry, Windows Phone, Android and Nokia. © 2016 WhatsApp Inc  WhatsApp Home Download WhatsApp Web FAQ Blog Contact                                                               Available for Android Azərbaycanca Bahasa Indonesia Bahasa Melayu Català Česky Dansk Deutsch eesti English Español Français Hrvatski Italiano Latviešu Lietuviškai Magyar Nederlands Norsk Pilipino Polski Português Română Slovenčina Slovenščina suomi Tiếng Việt Türkçe Ελληνικά Български Македонски Pусский српски Oʻzbekcha Українська ‏עברית‏ العربية فارسی বাংলা  हिंदी ગુજરાતી தமிழ் ภาษาไทย 简体中文 繁體中文 日本語 한국어 Help translate WhatsApp into your language Download WhatsApp                                iPhone                                    BlackBerry                                    Nokia S40                                    Symbian                                    Windows Phone     Download Why we don't sell ads Read more in our blog for iPhone for Android for BlackBerry for Nokia for Windows Phone Let's make WhatsApp available to everyone in the world! Tweet web.whatsapp.com @WhatsApp About Jobs Press Brand Center Privacy &amp; Terms Open Source Contact Us Facebook Twitter for iPhone for Android for BlackBerry for Nokia S60 for Nokia S40 for Windows Phone Available for ▾ ▾ &amp;                   Advertising has us chasing cars and clothes, working jobs we hate so we can buy shit we dont need. - Tyler Durden, Fight Club                  11 months ago @WhatsApp</v>
-      </c>
-      <c r="D2" t="str">
-        <v>WhatsApp :: Home WhatsApp Messenger :: cross-platform mobile messaging app for iPhone, BlackBerry, Android, Windows Phone and Nokia. Send text, video, images, audio for free. WhatsApp Simple. Personal.Real Time Messaging. Download WhatsApp How it works Why we don't sell ads WhatsApp for your phone Help Translate WhatsApp Share WhatsApp with Friends About WhatsApp WhatsApp Get in touch Download Home Download WhatsApp Web FAQ Blog Contact Azərbaycanca Bahasa Indonesia Bahasa Melayu Català Česky Dansk Deutsch eesti English Español Français Hrvatski Italiano Latviešu Lietuviškai Magyar Nederlands Norsk Pilipino Polski Português Română Slovenčina Slovenščina suomi Tiếng Việt Türkçe Ελληνικά Български Македонски Pусский српски Oʻzbekcha Українська ‏עברית‏ العربية فارسی বাংলা  हिंदी ગુજરાતી தமிழ் ภาษาไทย 简体中文 繁體中文 日本語 한국어 Help translate WhatsApp into your language                                 Group Chats                                                          Send photos &amp; videos                                                         Share locations                                                           iPhone                                        BlackBerry                                    Nokia S40                                    Symbian                                    Windows Phone     for iPhone for Android for BlackBerry for Nokia for Windows Phone About Jobs Press Brand Center Privacy &amp; Terms Open Source Contact Us Facebook Twitter for iPhone for Android for BlackBerry for Nokia S60 for Nokia S40 for Windows Phone JavaScript seem to be disabled in your browser. You better have JavaScript enabled to utilize the functionality of this website. WhatsApp Messenger is a cross-platform mobile messaging app which allows you to exchange messages without having to pay for SMS. WhatsApp Messenger is available for iPhone, BlackBerry, Android, Windows Phone and Nokia and yes, those phones can all message each other! Because WhatsApp Messenger uses the same internet data plan that you use for email and web browsing, there is no cost to message and stay in touch with your friends. In addition to basic messaging WhatsApp users can create groups, send each other unlimited images, video and audio media messages.                                     Advertising has us chasing cars and clothes, working jobs we hate so we can buy shit we dont need. - Tyler Durden, Fight Club                                                    Brian and I spent a combined 20 years at Yahoo! working hard to keep the site working. And yes, working hard to sell ads, because that's what Yahoo! did. It gathered data and it served pages and it sold ads. We watched Yahoo! get eclipsed in size by Google...                 Read more in our blog WhatsApp Messenger is a cross-platform mobile messaging app which allows you to exchange messages without having to pay for SMS. WhatsApp Messenger is available for iPhone, BlackBerry, Windows Phone, Android and Nokia. © 2016 WhatsApp Inc  WhatsApp Home Download WhatsApp Web FAQ Blog Contact                                                               Available for Android Azərbaycanca Bahasa Indonesia Bahasa Melayu Català Česky Dansk Deutsch eesti English Español Français Hrvatski Italiano Latviešu Lietuviškai Magyar Nederlands Norsk Pilipino Polski Português Română Slovenčina Slovenščina suomi Tiếng Việt Türkçe Ελληνικά Български Македонски Pусский српски Oʻzbekcha Українська ‏עברית‏ العربية فارسی বাংলা  हिंदी ગુજરાતી தமிழ் ภาษาไทย 简体中文 繁體中文 日本語 한국어 Help translate WhatsApp into your language Download WhatsApp                                iPhone                                    BlackBerry                                    Nokia S40                                    Symbian                                    Windows Phone     Download Why we don't sell ads Read more in our blog for iPhone for Android for BlackBerry for Nokia for Windows Phone Let's make WhatsApp available to everyone in the world! Tweet web.whatsapp.com @WhatsApp About Jobs Press Brand Center Privacy &amp; Terms Open Source Contact Us Facebook Twitter for iPhone for Android for BlackBerry for Nokia S60 for Nokia S40 for Windows Phone Available for ▾ ▾ &amp;                   Advertising has us chasing cars and clothes, working jobs we hate so we can buy shit we dont need. - Tyler Durden, Fight Club                  11 months ago @WhatsApp</v>
-      </c>
-      <c r="E2" t="str">
-        <v>WhatsApp :: Home WhatsApp Messenger :: cross-platform mobile messaging app for iPhone, BlackBerry, Android, Windows Phone and Nokia. Send text, video, images, audio for free. WhatsApp Simple. Personal.Real Time Messaging. Download WhatsApp How it works Why we don't sell ads WhatsApp for your phone Help Translate WhatsApp Share WhatsApp with Friends About WhatsApp WhatsApp Get in touch Download Home Download WhatsApp Web FAQ Blog Contact Azərbaycanca Bahasa Indonesia Bahasa Melayu Català Česky Dansk Deutsch eesti English Español Français Hrvatski Italiano Latviešu Lietuviškai Magyar Nederlands Norsk Pilipino Polski Português Română Slovenčina Slovenščina suomi Tiếng Việt Türkçe Ελληνικά Български Македонски Pусский српски Oʻzbekcha Українська ‏עברית‏ العربية فارسی বাংলা  हिंदी ગુજરાતી தமிழ் ภาษาไทย 简体中文 繁體中文 日本語 한국어 Help translate WhatsApp into your language                                 Group Chats                                                          Send photos &amp; videos                                                         Share locations                                                           iPhone                                        BlackBerry                                    Nokia S40                                    Symbian                                    Windows Phone     for iPhone for Android for BlackBerry for Nokia for Windows Phone About Jobs Press Brand Center Privacy &amp; Terms Open Source Contact Us Facebook Twitter for iPhone for Android for BlackBerry for Nokia S60 for Nokia S40 for Windows Phone JavaScript seem to be disabled in your browser. You better have JavaScript enabled to utilize the functionality of this website. WhatsApp Messenger is a cross-platform mobile messaging app which allows you to exchange messages without having to pay for SMS. WhatsApp Messenger is available for iPhone, BlackBerry, Android, Windows Phone and Nokia and yes, those phones can all message each other! Because WhatsApp Messenger uses the same internet data plan that you use for email and web browsing, there is no cost to message and stay in touch with your friends. In addition to basic messaging WhatsApp users can create groups, send each other unlimited images, video and audio media messages.                                     Advertising has us chasing cars and clothes, working jobs we hate so we can buy shit we dont need. - Tyler Durden, Fight Club                                                    Brian and I spent a combined 20 years at Yahoo! working hard to keep the site working. And yes, working hard to sell ads, because that's what Yahoo! did. It gathered data and it served pages and it sold ads. We watched Yahoo! get eclipsed in size by Google...                 Read more in our blog WhatsApp Messenger is a cross-platform mobile messaging app which allows you to exchange messages without having to pay for SMS. WhatsApp Messenger is available for iPhone, BlackBerry, Windows Phone, Android and Nokia. © 2016 WhatsApp Inc  WhatsApp Home Download WhatsApp Web FAQ Blog Contact                                                               Available for Android Azərbaycanca Bahasa Indonesia Bahasa Melayu Català Česky Dansk Deutsch eesti English Español Français Hrvatski Italiano Latviešu Lietuviškai Magyar Nederlands Norsk Pilipino Polski Português Română Slovenčina Slovenščina suomi Tiếng Việt Türkçe Ελληνικά Български Македонски Pусский српски Oʻzbekcha Українська ‏עברית‏ العربية فارسی বাংলা  हिंदी ગુજરાતી தமிழ் ภาษาไทย 简体中文 繁體中文 日本語 한국어 Help translate WhatsApp into your language Download WhatsApp                                iPhone                                    BlackBerry                                    Nokia S40                                    Symbian                                    Windows Phone     Download Why we don't sell ads Read more in our blog for iPhone for Android for BlackBerry for Nokia for Windows Phone Let's make WhatsApp available to everyone in the world! Tweet web.whatsapp.com @WhatsApp About Jobs Press Brand Center Privacy &amp; Terms Open Source Contact Us Facebook Twitter for iPhone for Android for BlackBerry for Nokia S60 for Nokia S40 for Windows Phone Available for ▾ ▾ &amp;                   Advertising has us chasing cars and clothes, working jobs we hate so we can buy shit we dont need. - Tyler Durden, Fight Club                  11 months ago @WhatsApp</v>
-      </c>
-      <c r="F2" t="str">
-        <v>WhatsApp :: Home WhatsApp Messenger :: cross-platform mobile messaging app for iPhone, BlackBerry, Android, Windows Phone and Nokia. Send text, video, images, audio for free. WhatsApp Simple. Personal.Real Time Messaging. Download WhatsApp How it works Why we don't sell ads WhatsApp for your phone Help Translate WhatsApp Share WhatsApp with Friends About WhatsApp WhatsApp Get in touch Download Home Download WhatsApp Web FAQ Blog Contact Azərbaycanca Bahasa Indonesia Bahasa Melayu Català Česky Dansk Deutsch eesti English Español Français Hrvatski Italiano Latviešu Lietuviškai Magyar Nederlands Norsk Pilipino Polski Português Română Slovenčina Slovenščina suomi Tiếng Việt Türkçe Ελληνικά Български Македонски Pусский српски Oʻzbekcha Українська ‏עברית‏ العربية فارسی বাংলা  हिंदी ગુજરાતી தமிழ் ภาษาไทย 简体中文 繁體中文 日本語 한국어 Help translate WhatsApp into your language                                 Group Chats                                                          Send photos &amp; videos                                                         Share locations                                                           iPhone                                        BlackBerry                                    Nokia S40                                    Symbian                                    Windows Phone     for iPhone for Android for BlackBerry for Nokia for Windows Phone About Jobs Press Brand Center Privacy &amp; Terms Open Source Contact Us Facebook Twitter for iPhone for Android for BlackBerry for Nokia S60 for Nokia S40 for Windows Phone JavaScript seem to be disabled in your browser. You better have JavaScript enabled to utilize the functionality of this website. WhatsApp Messenger is a cross-platform mobile messaging app which allows you to exchange messages without having to pay for SMS. WhatsApp Messenger is available for iPhone, BlackBerry, Android, Windows Phone and Nokia and yes, those phones can all message each other! Because WhatsApp Messenger uses the same internet data plan that you use for email and web browsing, there is no cost to message and stay in touch with your friends. In addition to basic messaging WhatsApp users can create groups, send each other unlimited images, video and audio media messages.                                     Advertising has us chasing cars and clothes, working jobs we hate so we can buy shit we dont need. - Tyler Durden, Fight Club                                                    Brian and I spent a combined 20 years at Yahoo! working hard to keep the site working. And yes, working hard to sell ads, because that's what Yahoo! did. It gathered data and it served pages and it sold ads. We watched Yahoo! get eclipsed in size by Google...                 Read more in our blog WhatsApp Messenger is a cross-platform mobile messaging app which allows you to exchange messages without having to pay for SMS. WhatsApp Messenger is available for iPhone, BlackBerry, Windows Phone, Android and Nokia. © 2016 WhatsApp Inc  WhatsApp Home Download WhatsApp Web FAQ Blog Contact                                                               Available for Android Azərbaycanca Bahasa Indonesia Bahasa Melayu Català Česky Dansk Deutsch eesti English Español Français Hrvatski Italiano Latviešu Lietuviškai Magyar Nederlands Norsk Pilipino Polski Português Română Slovenčina Slovenščina suomi Tiếng Việt Türkçe Ελληνικά Български Македонски Pусский српски Oʻzbekcha Українська ‏עברית‏ العربية فارسی বাংলা  हिंदी ગુજરાતી தமிழ் ภาษาไทย 简体中文 繁體中文 日本語 한국어 Help translate WhatsApp into your language Download WhatsApp                                iPhone                                    BlackBerry                                    Nokia S40                                    Symbian                                    Windows Phone     Download Why we don't sell ads Read more in our blog for iPhone for Android for BlackBerry for Nokia for Windows Phone Let's make WhatsApp available to everyone in the world! Tweet web.whatsapp.com @WhatsApp About Jobs Press Brand Center Privacy &amp; Terms Open Source Contact Us Facebook Twitter for iPhone for Android for BlackBerry for Nokia S60 for Nokia S40 for Windows Phone Available for ▾ ▾ &amp;                   Advertising has us chasing cars and clothes, working jobs we hate so we can buy shit we dont need. - Tyler Durden, Fight Club                  11 months ago @WhatsApp</v>
+        <v>WhatsApp Home WhatsApp Messenger crossplatform mobile messaging app for iPhone BlackBerry Android Windows Phone and Nokia Send text video images audio for free WhatsApp Simple PersonalReal Time Messaging Download WhatsApp How it works Why we dont sell ads WhatsApp for your phone Help Translate WhatsApp Share WhatsApp with Friends About WhatsApp WhatsApp Get in touch Download Home Download WhatsApp Web FAQ Blog Contact Azərbaycanca Bahasa Indonesia Bahasa Melayu Català Česky Dansk Deutsch eesti English Español Français Hrvatski Italiano Latviešu Lietuviškai Magyar Nederlands Norsk Pilipino Polski Português Română Slovenčina Slovenščina suomi Tiếng Việt Türkçe Ελληνικά Български Македонски Pусский српски Oʻzbekcha Українська ‏עברית‏ العربية فارسی বাংলা हिंदी ગુજરાતી தமிழ் ภาษาไทย 简体中文 繁體中文 日本語 한국어 Help translate WhatsApp into your language Group Chats Send photos videos Share locations iPhone BlackBerry Nokia S40 Symbian Windows Phone for iPhone for Android for BlackBerry for Nokia for Windows Phone About Jobs Press Brand Center Privacy Terms Open Source Contact Us Facebook Twitter for iPhone for Android for BlackBerry for Nokia S60 for Nokia S40 for Windows Phone JavaScript seem to be disabled in your browser You better have JavaScript enabled to utilize the functionality of this website WhatsApp Messenger is a crossplatform mobile messaging app which allows you to exchange messages without having to pay for SMS WhatsApp Messenger is available for iPhone BlackBerry Android Windows Phone and Nokia and yes those phones can all message each other Because WhatsApp Messenger uses the same internet data plan that you use for email and web browsing there is no cost to message and stay in touch with your friends In addition to basic messaging WhatsApp users can create groups send each other unlimited images video and audio media messages Advertising has us chasing cars and clothes working jobs we hate so we can buy shit we dont need Tyler Durden Fight Club Brian and I spent a combined 20 years at Yahoo working hard to keep the site working And yes working hard to sell ads because thats what Yahoo did It gathered data and it served pages and it sold ads We watched Yahoo get eclipsed in size by Google Read more in our blog WhatsApp Messenger is a crossplatform mobile messaging app which allows you to exchange messages without having to pay for SMS WhatsApp Messenger is available for iPhone BlackBerry Windows Phone Android and Nokia © 2016 WhatsApp Inc WhatsApp Home Download WhatsApp Web FAQ Blog Contact Available for Android Azərbaycanca Bahasa Indonesia Bahasa Melayu Català Česky Dansk Deutsch eesti English Español Français Hrvatski Italiano Latviešu Lietuviškai Magyar Nederlands Norsk Pilipino Polski Português Română Slovenčina Slovenščina suomi Tiếng Việt Türkçe Ελληνικά Български Македонски Pусский српски Oʻzbekcha Українська ‏עברית‏ العربية فارسی বাংলা हिंदी ગુજરાતી தமிழ் ภาษาไทย 简体中文 繁體中文 日本語 한국어 Help translate WhatsApp into your language Download WhatsApp iPhone BlackBerry Nokia S40 Symbian Windows Phone Download Why we dont sell ads Read more in our blog for iPhone for Android for BlackBerry for Nokia for Windows Phone Lets make WhatsApp available to everyone in the world Tweet webwhatsappcom WhatsApp About Jobs Press Brand Center Privacy Terms Open Source Contact Us Facebook Twitter for iPhone for Android for BlackBerry for Nokia S60 for Nokia S40 for Windows Phone Available for ▾ ▾ Advertising has us chasing cars and clothes working jobs we hate so we can buy shit we dont need Tyler Durden Fight Club 11 months ago WhatsApp</v>
       </c>
     </row>
     <row r="3">
@@ -413,16 +404,7 @@
         <v>App</v>
       </c>
       <c r="C3" t="str">
-        <v>Tinder Tinder is how people meet. It's like real life, but better. Get it for free on iPhone and Android</v>
-      </c>
-      <c r="D3" t="str">
-        <v>Tinder Tinder is how people meet. It's like real life, but better. Get it for free on iPhone and Android</v>
-      </c>
-      <c r="E3" t="str">
-        <v>Tinder Tinder is how people meet. It's like real life, but better. Get it for free on iPhone and Android</v>
-      </c>
-      <c r="F3" t="str">
-        <v>Tinder Tinder is how people meet. It's like real life, but better. Get it for free on iPhone and Android</v>
+        <v>Tinder Tinder is how people meet Its like real life but better Get it for free on iPhone and Android</v>
       </c>
     </row>
     <row r="4">
@@ -433,16 +415,7 @@
         <v>App</v>
       </c>
       <c r="C4" t="str">
-        <v>Snapchat Snapchat lets you easily talk with friends, view Live Stories from around the world, and explore news in Discover. Life's more fun when you live in the moment! snapchat                                  Home Blog Jobs Brand Guidelines Support Twitter Snapchat for iOS Snapchat for Android Snapcodes Geofilters Safety Center Community Guidelines Overview and FAQ General Guidelines Political Guidelines Inquiries Terms of Service Privacy Policy Copyright</v>
-      </c>
-      <c r="D4" t="str">
-        <v>Snapchat Snapchat lets you easily talk with friends, view Live Stories from around the world, and explore news in Discover. Life's more fun when you live in the moment! snapchat                                  Home Blog Jobs Brand Guidelines Support Twitter Snapchat for iOS Snapchat for Android Snapcodes Geofilters Safety Center Community Guidelines Overview and FAQ General Guidelines Political Guidelines Inquiries Terms of Service Privacy Policy Copyright</v>
-      </c>
-      <c r="E4" t="str">
-        <v>Snapchat Snapchat lets you easily talk with friends, view Live Stories from around the world, and explore news in Discover. Life's more fun when you live in the moment! snapchat                                  Home Blog Jobs Brand Guidelines Support Twitter Snapchat for iOS Snapchat for Android Snapcodes Geofilters Safety Center Community Guidelines Overview and FAQ General Guidelines Political Guidelines Inquiries Terms of Service Privacy Policy Copyright</v>
-      </c>
-      <c r="F4" t="str">
-        <v>Snapchat Snapchat lets you easily talk with friends, view Live Stories from around the world, and explore news in Discover. Life's more fun when you live in the moment! snapchat                                  Home Blog Jobs Brand Guidelines Support Twitter Snapchat for iOS Snapchat for Android Snapcodes Geofilters Safety Center Community Guidelines Overview and FAQ General Guidelines Political Guidelines Inquiries Terms of Service Privacy Policy Copyright</v>
+        <v>Snapchat Snapchat lets you easily talk with friends view Live Stories from around the world and explore news in Discover Lifes more fun when you live in the moment snapchat Home Blog Jobs Brand Guidelines Support Twitter Snapchat for iOS Snapchat for Android Snapcodes Geofilters Safety Center Community Guidelines Overview and FAQ General Guidelines Political Guidelines Inquiries Terms of Service Privacy Policy Copyright</v>
       </c>
     </row>
     <row r="5">
@@ -453,16 +426,7 @@
         <v>App</v>
       </c>
       <c r="C5" t="str">
-        <v>WeChat - The new way to connect Available for all kinds of platforms; enjoy group chat; support voice,photo,video and text messages. WeChat WeChat chat mobile chatting free send message send photo voice weixin offline message Weibo private message data consumption</v>
-      </c>
-      <c r="D5" t="str">
-        <v>WeChat - The new way to connect Available for all kinds of platforms; enjoy group chat; support voice,photo,video and text messages. WeChat WeChat chat mobile chatting free send message send photo voice weixin offline message Weibo private message data consumption</v>
-      </c>
-      <c r="E5" t="str">
-        <v>WeChat - The new way to connect Available for all kinds of platforms; enjoy group chat; support voice,photo,video and text messages. WeChat WeChat chat mobile chatting free send message send photo voice weixin offline message Weibo private message data consumption</v>
-      </c>
-      <c r="F5" t="str">
-        <v>WeChat - The new way to connect Available for all kinds of platforms; enjoy group chat; support voice,photo,video and text messages. WeChat WeChat chat mobile chatting free send message send photo voice weixin offline message Weibo private message data consumption</v>
+        <v>WeChat The new way to connect Available for all kinds of platforms enjoy group chat support voicephotovideo and text messages WeChat WeChat chat mobile chatting free send message send photo voice weixin offline message Weibo private message data consumption</v>
       </c>
     </row>
     <row r="6">
@@ -473,16 +437,7 @@
         <v>App</v>
       </c>
       <c r="C6" t="str">
-        <v>Uber - Sign up to drive or click and ride Get a taxi, private car or rideshare from your mobile phone. Uber connects you with a driver in minutes. Use our app in cities around the world. Your Ride, On Demand Drive with Uber Her turn to earn Transportation in minutes with the Uber app Your car. Your schedule. Your move. Creating 1,000,000 jobs for women by 2020 The Uber App One Tap to Ride Reliable Pickups Clear Pricing Cashless &amp; Convenient Feedback Matters Split Your Fare Choice is a beautiful thing All around the world One Tapto Ride ReliablePickups ClearPricing Cashless &amp;Convenient FeedbackMatters Split YourFare The low-cost Uber Taxi without the hassle The original Room for everyone Ultimate luxury                         One Tapto Ride                                                                     ReliablePickups                                                                     ClearPricing                                                                     Cashless &amp;Convenient                                                                     FeedbackMatters                                                                     Split YourFare                                                                                        One Tap to Ride             Uber uses your phone's GPS to detect your location and connects you with the nearest available driver. Get picked up anywhere — even if you don't know the exact address.                                                                   Reliable Pickups             When you request a ride, we’ll find a driver and let you track their location on the map. Feel free to put away your phone – we’ll text you when your ride arrives. Your driver’s name and car details appear in the app, and you can message or call if you need to.                                                                   Clear Pricing             View rates for your city in the app. You can also enter your pickup and drop-off locations to get a fare estimate for your trip.                                                                   Cashless &amp; Convenient             You don't need cash when you ride with Uber. Once you arrive at your destination, your fare is automatically charged to your credit card on file – no need to tip. We’ll also e-mail you a receipt.                                                                   Feedback Matters             Drivers not only meet Uber’s standards, they meet your standards. After your trip, you can rate your experience and leave additional feedback about your driver.                                                                   Split Your Fare             Simplify your life and your fractions. Invite your friends to split the fare. If your friends opt in, each person’s credit card will be charged equally. No more pay-me-backs or IOUs.                                     Home                       Our Cities                       Be a Driver             App Features Safety Business Developer About Us Help Center Careers Legal Newsroom                     Log In                                                              Log In                                                                         Sign Up                                                                          Download                             Features Request, ride, and pay via your mobile phone Uber uses your phone's GPS to detect your location and connects you with the nearest available driver. Get picked up anywhere — even if you don't know the exact address. When you request a ride, we’ll find a driver and let you track their location on the map. Feel free to put away your phone – we’ll text you when your ride arrives. Your driver’s name and car details appear in the app, and you can message or call if you need to. View rates for your city in the app. You can also enter your pickup and drop-off locations to get a fare estimate for your trip. You don't need cash when you ride with Uber. Once you arrive at your destination, your fare is automatically charged to your credit card on file – no need to tip. We’ll also e-mail you a receipt. Drivers not only meet Uber’s standards, they meet your standards. After your trip, you can rate your experience and leave additional feedback about your driver. Simplify your life and your fractions. Invite your friends to split the fare. If your friends opt in, each person’s credit card will be charged equally. No more pay-me-backs or IOUs. Options Get a ride that matches your style and budget uberX uberX Everyday cars for everyday use.Better, faster, and smarter than a taxi. uberTAXI Taxi No whistling, no waving, no cash needed. UberBLACK Black Your own private driver, on demand.Expect pickup in a high-end sedan within minutes. UberSUV SUV For those times when you need a bit more space.Seats up to six people in style. UberLUX LUX The finest cars with prices to match.                      uberX uberX Everyday cars for everyday use.Better, faster, and smarter than a taxi. uberTAXI uberTAXI No whistling, no waving, no cash needed. UberBLACK UberBLACK Your own private driver, on demand.Expect pickup in a high-end sedan within minutes. UberSUV UberSUV For those times when you need a bit more space.Seats up to six people in style. UberLUX UberLUX The finest cars with prices to match. Locations Available locally, expanding globally                           Log In                 Sign up                 Home                 Our Cities                 Be a Driver        App Features Safety Business Developer About Us Help Center Careers Legal Newsroom            Log In                                                                                    Become a driver                                                                                     Menu                               Log In                                 Sign Up                                   Download                Uber Sign Up Sign Up Learn More uberX TAXI BLACK SUV LUX            uberX                                           uberTAXI                                           UberBLACK                                           UberSUV                                           UberLUX                                View all cities        Download Uber               Sign up for Uber                   Home                     Cities                     Drive                     Help Center                     Careers                     Developers                     Newsroom                     About Us                   English        Apple Store Google Play Store Windows Store Terms and Conditions Privacy Policy Menu • •</v>
-      </c>
-      <c r="D6" t="str">
-        <v>Uber - Sign up to drive or click and ride Get a taxi, private car or rideshare from your mobile phone. Uber connects you with a driver in minutes. Use our app in cities around the world. Your Ride, On Demand Drive with Uber Her turn to earn Transportation in minutes with the Uber app Your car. Your schedule. Your move. Creating 1,000,000 jobs for women by 2020 The Uber App One Tap to Ride Reliable Pickups Clear Pricing Cashless &amp; Convenient Feedback Matters Split Your Fare Choice is a beautiful thing All around the world One Tapto Ride ReliablePickups ClearPricing Cashless &amp;Convenient FeedbackMatters Split YourFare The low-cost Uber Taxi without the hassle The original Room for everyone Ultimate luxury                         One Tapto Ride                                                                     ReliablePickups                                                                     ClearPricing                                                                     Cashless &amp;Convenient                                                                     FeedbackMatters                                                                     Split YourFare                                                                                        One Tap to Ride             Uber uses your phone's GPS to detect your location and connects you with the nearest available driver. Get picked up anywhere — even if you don't know the exact address.                                                                   Reliable Pickups             When you request a ride, we’ll find a driver and let you track their location on the map. Feel free to put away your phone – we’ll text you when your ride arrives. Your driver’s name and car details appear in the app, and you can message or call if you need to.                                                                   Clear Pricing             View rates for your city in the app. You can also enter your pickup and drop-off locations to get a fare estimate for your trip.                                                                   Cashless &amp; Convenient             You don't need cash when you ride with Uber. Once you arrive at your destination, your fare is automatically charged to your credit card on file – no need to tip. We’ll also e-mail you a receipt.                                                                   Feedback Matters             Drivers not only meet Uber’s standards, they meet your standards. After your trip, you can rate your experience and leave additional feedback about your driver.                                                                   Split Your Fare             Simplify your life and your fractions. Invite your friends to split the fare. If your friends opt in, each person’s credit card will be charged equally. No more pay-me-backs or IOUs.                                     Home                       Our Cities                       Be a Driver             App Features Safety Business Developer About Us Help Center Careers Legal Newsroom                     Log In                                                              Log In                                                                         Sign Up                                                                          Download                             Features Request, ride, and pay via your mobile phone Uber uses your phone's GPS to detect your location and connects you with the nearest available driver. Get picked up anywhere — even if you don't know the exact address. When you request a ride, we’ll find a driver and let you track their location on the map. Feel free to put away your phone – we’ll text you when your ride arrives. Your driver’s name and car details appear in the app, and you can message or call if you need to. View rates for your city in the app. You can also enter your pickup and drop-off locations to get a fare estimate for your trip. You don't need cash when you ride with Uber. Once you arrive at your destination, your fare is automatically charged to your credit card on file – no need to tip. We’ll also e-mail you a receipt. Drivers not only meet Uber’s standards, they meet your standards. After your trip, you can rate your experience and leave additional feedback about your driver. Simplify your life and your fractions. Invite your friends to split the fare. If your friends opt in, each person’s credit card will be charged equally. No more pay-me-backs or IOUs. Options Get a ride that matches your style and budget uberX uberX Everyday cars for everyday use.Better, faster, and smarter than a taxi. uberTAXI Taxi No whistling, no waving, no cash needed. UberBLACK Black Your own private driver, on demand.Expect pickup in a high-end sedan within minutes. UberSUV SUV For those times when you need a bit more space.Seats up to six people in style. UberLUX LUX The finest cars with prices to match.                      uberX uberX Everyday cars for everyday use.Better, faster, and smarter than a taxi. uberTAXI uberTAXI No whistling, no waving, no cash needed. UberBLACK UberBLACK Your own private driver, on demand.Expect pickup in a high-end sedan within minutes. UberSUV UberSUV For those times when you need a bit more space.Seats up to six people in style. UberLUX UberLUX The finest cars with prices to match. Locations Available locally, expanding globally                           Log In                 Sign up                 Home                 Our Cities                 Be a Driver        App Features Safety Business Developer About Us Help Center Careers Legal Newsroom            Log In                                                                                    Become a driver                                                                                     Menu                               Log In                                 Sign Up                                   Download                Uber Sign Up Sign Up Learn More uberX TAXI BLACK SUV LUX            uberX                                           uberTAXI                                           UberBLACK                                           UberSUV                                           UberLUX                                View all cities        Download Uber               Sign up for Uber                   Home                     Cities                     Drive                     Help Center                     Careers                     Developers                     Newsroom                     About Us                   English        Apple Store Google Play Store Windows Store Terms and Conditions Privacy Policy Menu • •</v>
-      </c>
-      <c r="E6" t="str">
-        <v>Uber - Sign up to drive or click and ride Get a taxi, private car or rideshare from your mobile phone. Uber connects you with a driver in minutes. Use our app in cities around the world. Your Ride, On Demand Drive with Uber Her turn to earn Transportation in minutes with the Uber app Your car. Your schedule. Your move. Creating 1,000,000 jobs for women by 2020 The Uber App One Tap to Ride Reliable Pickups Clear Pricing Cashless &amp; Convenient Feedback Matters Split Your Fare Choice is a beautiful thing All around the world One Tapto Ride ReliablePickups ClearPricing Cashless &amp;Convenient FeedbackMatters Split YourFare The low-cost Uber Taxi without the hassle The original Room for everyone Ultimate luxury                         One Tapto Ride                                                                     ReliablePickups                                                                     ClearPricing                                                                     Cashless &amp;Convenient                                                                     FeedbackMatters                                                                     Split YourFare                                                                                        One Tap to Ride             Uber uses your phone's GPS to detect your location and connects you with the nearest available driver. Get picked up anywhere — even if you don't know the exact address.                                                                   Reliable Pickups             When you request a ride, we’ll find a driver and let you track their location on the map. Feel free to put away your phone – we’ll text you when your ride arrives. Your driver’s name and car details appear in the app, and you can message or call if you need to.                                                                   Clear Pricing             View rates for your city in the app. You can also enter your pickup and drop-off locations to get a fare estimate for your trip.                                                                   Cashless &amp; Convenient             You don't need cash when you ride with Uber. Once you arrive at your destination, your fare is automatically charged to your credit card on file – no need to tip. We’ll also e-mail you a receipt.                                                                   Feedback Matters             Drivers not only meet Uber’s standards, they meet your standards. After your trip, you can rate your experience and leave additional feedback about your driver.                                                                   Split Your Fare             Simplify your life and your fractions. Invite your friends to split the fare. If your friends opt in, each person’s credit card will be charged equally. No more pay-me-backs or IOUs.                                     Home                       Our Cities                       Be a Driver             App Features Safety Business Developer About Us Help Center Careers Legal Newsroom                     Log In                                                              Log In                                                                         Sign Up                                                                          Download                             Features Request, ride, and pay via your mobile phone Uber uses your phone's GPS to detect your location and connects you with the nearest available driver. Get picked up anywhere — even if you don't know the exact address. When you request a ride, we’ll find a driver and let you track their location on the map. Feel free to put away your phone – we’ll text you when your ride arrives. Your driver’s name and car details appear in the app, and you can message or call if you need to. View rates for your city in the app. You can also enter your pickup and drop-off locations to get a fare estimate for your trip. You don't need cash when you ride with Uber. Once you arrive at your destination, your fare is automatically charged to your credit card on file – no need to tip. We’ll also e-mail you a receipt. Drivers not only meet Uber’s standards, they meet your standards. After your trip, you can rate your experience and leave additional feedback about your driver. Simplify your life and your fractions. Invite your friends to split the fare. If your friends opt in, each person’s credit card will be charged equally. No more pay-me-backs or IOUs. Options Get a ride that matches your style and budget uberX uberX Everyday cars for everyday use.Better, faster, and smarter than a taxi. uberTAXI Taxi No whistling, no waving, no cash needed. UberBLACK Black Your own private driver, on demand.Expect pickup in a high-end sedan within minutes. UberSUV SUV For those times when you need a bit more space.Seats up to six people in style. UberLUX LUX The finest cars with prices to match.                      uberX uberX Everyday cars for everyday use.Better, faster, and smarter than a taxi. uberTAXI uberTAXI No whistling, no waving, no cash needed. UberBLACK UberBLACK Your own private driver, on demand.Expect pickup in a high-end sedan within minutes. UberSUV UberSUV For those times when you need a bit more space.Seats up to six people in style. UberLUX UberLUX The finest cars with prices to match. Locations Available locally, expanding globally                           Log In                 Sign up                 Home                 Our Cities                 Be a Driver        App Features Safety Business Developer About Us Help Center Careers Legal Newsroom            Log In                                                                                    Become a driver                                                                                     Menu                               Log In                                 Sign Up                                   Download                Uber Sign Up Sign Up Learn More uberX TAXI BLACK SUV LUX            uberX                                           uberTAXI                                           UberBLACK                                           UberSUV                                           UberLUX                                View all cities        Download Uber               Sign up for Uber                   Home                     Cities                     Drive                     Help Center                     Careers                     Developers                     Newsroom                     About Us                   English        Apple Store Google Play Store Windows Store Terms and Conditions Privacy Policy Menu • •</v>
-      </c>
-      <c r="F6" t="str">
-        <v>Uber - Sign up to drive or click and ride Get a taxi, private car or rideshare from your mobile phone. Uber connects you with a driver in minutes. Use our app in cities around the world. Your Ride, On Demand Drive with Uber Her turn to earn Transportation in minutes with the Uber app Your car. Your schedule. Your move. Creating 1,000,000 jobs for women by 2020 The Uber App One Tap to Ride Reliable Pickups Clear Pricing Cashless &amp; Convenient Feedback Matters Split Your Fare Choice is a beautiful thing All around the world One Tapto Ride ReliablePickups ClearPricing Cashless &amp;Convenient FeedbackMatters Split YourFare The low-cost Uber Taxi without the hassle The original Room for everyone Ultimate luxury                         One Tapto Ride                                                                     ReliablePickups                                                                     ClearPricing                                                                     Cashless &amp;Convenient                                                                     FeedbackMatters                                                                     Split YourFare                                                                                        One Tap to Ride             Uber uses your phone's GPS to detect your location and connects you with the nearest available driver. Get picked up anywhere — even if you don't know the exact address.                                                                   Reliable Pickups             When you request a ride, we’ll find a driver and let you track their location on the map. Feel free to put away your phone – we’ll text you when your ride arrives. Your driver’s name and car details appear in the app, and you can message or call if you need to.                                                                   Clear Pricing             View rates for your city in the app. You can also enter your pickup and drop-off locations to get a fare estimate for your trip.                                                                   Cashless &amp; Convenient             You don't need cash when you ride with Uber. Once you arrive at your destination, your fare is automatically charged to your credit card on file – no need to tip. We’ll also e-mail you a receipt.                                                                   Feedback Matters             Drivers not only meet Uber’s standards, they meet your standards. After your trip, you can rate your experience and leave additional feedback about your driver.                                                                   Split Your Fare             Simplify your life and your fractions. Invite your friends to split the fare. If your friends opt in, each person’s credit card will be charged equally. No more pay-me-backs or IOUs.                                     Home                       Our Cities                       Be a Driver             App Features Safety Business Developer About Us Help Center Careers Legal Newsroom                     Log In                                                              Log In                                                                         Sign Up                                                                          Download                             Features Request, ride, and pay via your mobile phone Uber uses your phone's GPS to detect your location and connects you with the nearest available driver. Get picked up anywhere — even if you don't know the exact address. When you request a ride, we’ll find a driver and let you track their location on the map. Feel free to put away your phone – we’ll text you when your ride arrives. Your driver’s name and car details appear in the app, and you can message or call if you need to. View rates for your city in the app. You can also enter your pickup and drop-off locations to get a fare estimate for your trip. You don't need cash when you ride with Uber. Once you arrive at your destination, your fare is automatically charged to your credit card on file – no need to tip. We’ll also e-mail you a receipt. Drivers not only meet Uber’s standards, they meet your standards. After your trip, you can rate your experience and leave additional feedback about your driver. Simplify your life and your fractions. Invite your friends to split the fare. If your friends opt in, each person’s credit card will be charged equally. No more pay-me-backs or IOUs. Options Get a ride that matches your style and budget uberX uberX Everyday cars for everyday use.Better, faster, and smarter than a taxi. uberTAXI Taxi No whistling, no waving, no cash needed. UberBLACK Black Your own private driver, on demand.Expect pickup in a high-end sedan within minutes. UberSUV SUV For those times when you need a bit more space.Seats up to six people in style. UberLUX LUX The finest cars with prices to match.                      uberX uberX Everyday cars for everyday use.Better, faster, and smarter than a taxi. uberTAXI uberTAXI No whistling, no waving, no cash needed. UberBLACK UberBLACK Your own private driver, on demand.Expect pickup in a high-end sedan within minutes. UberSUV UberSUV For those times when you need a bit more space.Seats up to six people in style. UberLUX UberLUX The finest cars with prices to match. Locations Available locally, expanding globally                           Log In                 Sign up                 Home                 Our Cities                 Be a Driver        App Features Safety Business Developer About Us Help Center Careers Legal Newsroom            Log In                                                                                    Become a driver                                                                                     Menu                               Log In                                 Sign Up                                   Download                Uber Sign Up Sign Up Learn More uberX TAXI BLACK SUV LUX            uberX                                           uberTAXI                                           UberBLACK                                           UberSUV                                           UberLUX                                View all cities        Download Uber               Sign up for Uber                   Home                     Cities                     Drive                     Help Center                     Careers                     Developers                     Newsroom                     About Us                   English        Apple Store Google Play Store Windows Store Terms and Conditions Privacy Policy Menu • •</v>
+        <v>Uber Sign up to drive or click and ride Get a taxi private car or rideshare from your mobile phone Uber connects you with a driver in minutes Use our app in cities around the world Your Ride On Demand Drive with Uber Her turn to earn Transportation in minutes with the Uber app Your car Your schedule Your move Creating 1000000 jobs for women by 2020 The Uber App One Tap to Ride Reliable Pickups Clear Pricing Cashless Convenient Feedback Matters Split Your Fare Choice is a beautiful thing All around the world One Tapto Ride ReliablePickups ClearPricing Cashless Convenient FeedbackMatters Split YourFare The lowcost Uber Taxi without the hassle The original Room for everyone Ultimate luxury One Tapto Ride ReliablePickups ClearPricing Cashless Convenient FeedbackMatters Split YourFare One Tap to Ride Uber uses your phones GPS to detect your location and connects you with the nearest available driver Get picked up anywhere even if you dont know the exact address Reliable Pickups When you request a ride we’ll find a driver and let you track their location on the map Feel free to put away your phone we’ll text you when your ride arrives Your driver’s name and car details appear in the app and you can message or call if you need to Clear Pricing View rates for your city in the app You can also enter your pickup and dropoff locations to get a fare estimate for your trip Cashless Convenient You dont need cash when you ride with Uber Once you arrive at your destination your fare is automatically charged to your credit card on file no need to tip We’ll also email you a receipt Feedback Matters Drivers not only meet Uber’s standards they meet your standards After your trip you can rate your experience and leave additional feedback about your driver Split Your Fare Simplify your life and your fractions Invite your friends to split the fare If your friends opt in each person’s credit card will be charged equally No more paymebacks or IOUs Home Our Cities Be a Driver App Features Safety Business Developer About Us Help Center Careers Legal Newsroom Log In Log In Sign Up Download Features Request ride and pay via your mobile phone Uber uses your phones GPS to detect your location and connects you with the nearest available driver Get picked up anywhere even if you dont know the exact address When you request a ride we’ll find a driver and let you track their location on the map Feel free to put away your phone we’ll text you when your ride arrives Your driver’s name and car details appear in the app and you can message or call if you need to View rates for your city in the app You can also enter your pickup and dropoff locations to get a fare estimate for your trip You dont need cash when you ride with Uber Once you arrive at your destination your fare is automatically charged to your credit card on file no need to tip We’ll also email you a receipt Drivers not only meet Uber’s standards they meet your standards After your trip you can rate your experience and leave additional feedback about your driver Simplify your life and your fractions Invite your friends to split the fare If your friends opt in each person’s credit card will be charged equally No more paymebacks or IOUs Options Get a ride that matches your style and budget uberX uberX Everyday cars for everyday useBetter faster and smarter than a taxi uberTAXI Taxi No whistling no waving no cash needed UberBLACK Black Your own private driver on demandExpect pickup in a highend sedan within minutes UberSUV SUV For those times when you need a bit more spaceSeats up to six people in style UberLUX LUX The finest cars with prices to match uberX uberX Everyday cars for everyday useBetter faster and smarter than a taxi uberTAXI uberTAXI No whistling no waving no cash needed UberBLACK UberBLACK Your own private driver on demandExpect pickup in a highend sedan within minutes UberSUV UberSUV For those times when you need a bit more spaceSeats up to six people in style UberLUX UberLUX The finest cars with prices to match Locations Available locally expanding globally Log In Sign up Home Our Cities Be a Driver App Features Safety Business Developer About Us Help Center Careers Legal Newsroom Log In Become a driver Menu Log In Sign Up Download Uber Sign Up Sign Up Learn More uberX TAXI BLACK SUV LUX uberX uberTAXI UberBLACK UberSUV UberLUX View all cities Download Uber Sign up for Uber Home Cities Drive Help Center Careers Developers Newsroom About Us English Apple Store Google Play Store Windows Store Terms and Conditions Privacy Policy Menu • •</v>
       </c>
     </row>
     <row r="7">
@@ -493,16 +448,13 @@
         <v>reseller</v>
       </c>
       <c r="C7" t="str">
-        <v>PCM IT Solutions &amp; Services Business-to-business focused computer sales. Mission-critical systems &amp; services, including data storage solutions. PCM. We mean business. PCM, data storage solutions Solutions &amp; Services Cloud Products More than an IT Provider - We're Your Technology Partner! Thank You!                      PCM (Home)                                                  GOVERNMENT (Home)                                                  E-PROCUREMENT                                              Cloud Partners                                       PCM Hybrid Cloud                              Featured                     Hardware                     Software                     Brands          Deal of the Week Lenovo B40-80 80F6 Notebook Managed Print Services Preferred Partners Our Company Support We Provide  PCM Blog  Spiceworks  Facebook  LinkedIn  Twitter  YouTube  Sign in                                                     Order Status                                                Sign In                                   New account?  Register                                                     /* jQuery(function($){                 PCM.tooltipDown.init('#signin-btn-21');             }); */                Cart ()  STARTUPS / ENTREPRENEURS MEDIUM / LARGE BUSINESS ENTERPRISE HEALTHCARE FEDERAL STATE &amp; LOCAL EDUCATION HEALTHCARE PCM BUSINESS DIRECT PCM OPSTRACK Cloud Products Shop Now Learn More Deal of the Week Top Searches Ultrabook Finder Memory Finder Ink/Toner Finder Accessories Cables Computers Memory Monitors &amp; Projectors Networking Printers &amp; Supplies Racks, Power &amp; Cooling Scanners Servers Storage Backup Business Database Desktop &amp; Web Publishing Management Operating Systems Security Unified Collaboration Virtualization Apple Cisco Dell Google HPI HPE Intel Lenovo Microsoft Samsung Symantec VMware                                                                               Picking the Right Printer for your Office [INFOGRAPHIC]                     January 19, 2016 Microsoft Announces Major Change to the Enterprise Agreement Program                     January 6, 2016 How Christmas Gifts Could Impact BYOD                     January 4, 2016 Enhance Your Creativity with Adobe Stock                     December 30, 2015 HP Print Security Seminars: Is Your Network at Risk to Hackers?                     December 22, 2015 Share Costs and Save Time with Hewlett Packard Enterprise Healthcare                     December 21, 2015 Microsoft Announces that Windows Server 2016 will be Launching Next Quarter                     December 11, 2015 Last Chance to Register for Vision Hollywood!                     December 10, 2015 How Big of a Deal is the Apple-Cisco Partnership?                     December 9, 2015 Webcast: ShoreTel Truly Unified Communications                     December 8, 2015 Ergotron StyleView: Fit for Every Body                     December 7, 2015 The Digital Pulse of Tomorrow’s Healthcare with Lenovo                     December 7, 2015          Featured Products                                                 Bestsellers                                                 New Arrivals                                                 Trending                                          &lt;!-- /* You may give each page an identifying name, server, and channel on the next lines. */ s.pageName="Homepage Redesign" s.server="AFS-PL-PCMWS04" s.channel="Home" s.prop1="Home" s.prop2="Home" s.prop3="Home" s.prop4="Home" s.eVar15="06361F3DBD6448308E56B101F5974814"  /************* DO NOT ALTER ANYTHING BELOW THIS LINE ! **************/ var s_code=s.t();if(s_code)document.write(s_code)//--&gt;                                                                                            Menu                                            WELCOME TO PCM!                                                                                                                                                                                                                                     Thank You!                                                         Thank you for subscribing to our newsletter. Be sure to check your email for exclusive offers and discounts.                                   jQuery(document).ready(function() {      PCM.subscribeEmailValidate.init({formNewsLetterEle: '#email-subscribe',          allowPageReload : false});  });      1-800-700-1000    (function(c, h, a, t, _, i, d) {     c[_] = c[_] || function() {         (c[_].q = c[_].q || []).push(arguments)     }, c[_].l = 1 * new Date();     i = h.createElement(a), d = h.getElementsByTagName(a)[0];     i.async = 1;     i.src = t;     d.parentNode.insertBefore(i, d) })(window, document, 'script', 'https://chatidcdn.com/embed/pcm/latest.js', 'CID');            Follow     PCM Blog  Spiceworks  Facebook  LinkedIn  Twitter  YouTube            jQuery(document).ready(function(){  var pcm_tooltip_opts = {};   if('useContentID' == 'useContentID' &amp;&amp; '#follow-us-social' != ''){   pcm_tooltip_opts.customContentID = '#follow-us-social';  }else if('useContentID' == 'customContent' &amp;&amp; '' != ''){   pcm_tooltip_opts.customContent = ''  }   if('' != ''){   pcm_tooltip_opts.isThemeHeader = true;   pcm_tooltip_opts.headerTitle = '';   pcm_tooltip_opts.headerBg = '#1b5d9e';   pcm_tooltip_opts.headerColor = '#000';  }   if('1px' != '0' &amp;&amp; '1px' != '0px'){   pcm_tooltip_opts.tooltipBorderSize = '1px';   pcm_tooltip_opts.tooltipBorderColor = '#e6e6e6';  }    if('' != ''){ pcm_tooltip_opts.width = ''; }  if('25px' != ''){ pcm_tooltip_opts.customArrowPos = '25px'; }  if('bottom' != 'auto'){ pcm_tooltip_opts.tooltipShowDirection = 'bottom'; }  if('#fff' != ''){ pcm_tooltip_opts.contentBGcolor = '#fff'; }  if('10px' != ''){ pcm_tooltip_opts.contentPadding = '10px'; }  if('-4' != ''){ pcm_tooltip_opts.distanceFromBaseElement = '-4'; }  if('800' != ''){ pcm_tooltip_opts.zIndex = '800'; }    pcm_tooltip_opts.eventsArray = 'click'.split(',');    jQuery('#follow-link').pcm_tooltip(pcm_tooltip_opts); });            jQuery(document).ready(function(){  var pcm_tooltip_opts = {};   if('useHref' == 'useContentID' &amp;&amp; '' != ''){   pcm_tooltip_opts.customContentID = '';  }else if('useHref' == 'customContent' &amp;&amp; '' != ''){   pcm_tooltip_opts.customContent = ''  }   if('' != ''){   pcm_tooltip_opts.isThemeHeader = true;   pcm_tooltip_opts.headerTitle = '';   pcm_tooltip_opts.headerBg = '#1b5d9e';   pcm_tooltip_opts.headerColor = '#000';  }   if('1px' != '0' &amp;&amp; '1px' != '0px'){   pcm_tooltip_opts.tooltipBorderSize = '1px';   pcm_tooltip_opts.tooltipBorderColor = '#e6e6e6';  }    if('' != ''){ pcm_tooltip_opts.width = ''; }  if('19px' != ''){ pcm_tooltip_opts.customArrowPos = '19px'; }  if('bottom' != 'auto'){ pcm_tooltip_opts.tooltipShowDirection = 'bottom'; }  if('#fff' != ''){ pcm_tooltip_opts.contentBGcolor = '#fff'; }  if('0' != ''){ pcm_tooltip_opts.contentPadding = '0'; }  if('-4' != ''){ pcm_tooltip_opts.distanceFromBaseElement = '-4'; }  if('800' != ''){ pcm_tooltip_opts.zIndex = '800'; }    pcm_tooltip_opts.eventsArray = 'click'.split(',');    jQuery('.sslink.dropd.ttipdwn').pcm_tooltip(pcm_tooltip_opts); });       Sign in                                                     Order Status                                                Sign In                                   New account?  Register                                                     /* jQuery(function($){                 PCM.tooltipDown.init('#signin-btn-21');             }); */                     Cart ()   var PCM = PCM || {}; PCM.cart=(function($){     function update(){         $.ajax({             url:"/home?op=mall.web.misc.cartLink.cartLink",             type:'POST',             dataType:'json',             data:'false',             success:count         });     }     function count(data){         if(typeof data !== 'undefined'){             $('[data-bind="cart-count"]').text(data.count)         }     }     return {         update:update     }; })(jQuery); PCM.cart.update();                                                                                                                                                                    PCM (Home)                                              STARTUPS / ENTREPRENEURSMEDIUM / LARGE BUSINESSENTERPRISEHEALTHCARE                                                                                                                                              GOVERNMENT (Home)                                              FEDERALSTATE &amp; LOCALEDUCATIONHEALTHCARE                                                                                                                                              E-PROCUREMENT                                              PCM BUSINESS DIRECTPCM OPSTRACK                                                             jQuery(function($){     PCM.changeHomepage.init();     var lastClickedTab = 'last_clicked_tab';     var active = getCookie(lastClickedTab);     var widget=$("#drk-mmenu-13"), $greet=widget.find('.greetings-txt');     if('msc-515,msc-497,msc-428,msc-429,msc-426,msc-427,msc-home,msc-430,msc-425,'.indexOf('msc-home,') &gt; -1){   active = 'msc-home';  }     var txt=widget.find('[navpoint-id="' + active + '"]')     if(txt.length) {         var greetings = txt.attr('greetings');         if(greetings) {             $greet.text(greetings);         }         txt.addClass('actv');     }else{      widget.find('a[navpoint-id]').first().addClass('actv');     }     $greet.show();          var host = window.location.host;     var links= widget.find('a[navpoint-id]')     links.click(function(e){      var navId = $(this).attr('navpoint-id'), href=$(this).attr('href');      if(navId &amp;&amp; href &amp;&amp; (href.charAt(0)=='/' || host===href.split('/')[2])){       document.cookie = lastClickedTab + '=' + navId + '; expires=' + setExpirationDate(30) + '; path=/';      }     });     var setExpirationDate = function(days){      var date = new Date();         date.setTime(date.getTime()+(days*24*60*60*1000));         return date.toUTCString();     };      });  var getCookie = function(name){  var nameEQ = name + "=";     var ca = document.cookie.split(';');     for(var i=0;i &lt; ca.length;i++) {         var c = jQuery.trim(ca[i]);         if (c.indexOf(nameEQ) === 0) return c.substring(nameEQ.length,c.length);     }     return null; };                                        Solutions &amp; Services                Cloud    Products                                                                                               Cloud Partners                                             Shop Now                                                                                                        PCM Hybrid Cloud                                             Learn More                                                                                                                                                   Featured                                    Deal of the Week                  Top Searches                  Ultrabook Finder                  Memory Finder                  Ink/Toner Finder                                                                                               Hardware                                    Accessories                  Cables                  Computers                  Memory                  Monitors &amp; Projectors                  Networking                  Printers &amp; Supplies                  Racks, Power &amp; Cooling                  Scanners                  Servers                  Storage                                           All Categories                                                                              Software                                    Backup                  Business                  Database                  Desktop &amp; Web Publishing                  Management                  Operating Systems                  Security                  Unified Collaboration                  Virtualization                                           All Categories                                                                              Brands                                    Apple                  Cisco                  Dell                  Google                  HPI                  HPE                  Intel                  Lenovo                  Microsoft                  Samsung                  Symantec                  VMware                                           All Brands                                                       jQuery(function($){     PCM.mainNav.init();     var cont=$('.static-links-con,.menu-nav');     cont.show();     $('.menu-nav .static-links-con').each(function(i,t){         var h=0;         $(t).find('.sub-group-name').each(function(i,s){             h=Math.max(h,$(s).height());         }).each(function(i,s){             $(s).height(h);         });     });     cont.hide(); });                            All Products     Mfg Part Number     PCM Part Number                                                      PCM.dropDown = (function($j) {  var init = function($id, $main, inputBar, elem) {   var dropDownDiv;   var textSpan;   var dropSpan;   var inputDiv;   var searchNow = $main.find('.searchInputBtn');      var SEARCH_TEXT = 'Search Products';   var PADDING_SELECT = 30;   var BORDER_WIDTH = 1;    var initEvent = function() {        placeHolder();    elem.selectBoxIt();    elem.change(function(){                 adjustSearchBox();             });    searchNow.click(function(){     checkInputBox();     return false;    });    inputBar.keypress(function(e){     if(e.which === 13){      checkInputBox();      return false;     }    });        adjustSearchBox();   };   var checkInputBox = function(){    var val = $j.trim(inputBar.val()).replace(/\\/g, "");             if(val.length === 0 || val === SEARCH_TEXT){                 alert('Please enter a search keyword');                 //PCM.modalBx('', {'width': 350}).modal().openModal('#error-search');             }else{                 var $type=elem,                 _val = encodeURIComponent(val),                 _q = $type.val().replace(/$0/g, _val),                 url = [$type.attr('href'), _val, _q?"&amp;":"", _q];                 window.location= url.join("");             }   };   var adjustSearchBox = function(){    textSpan = $main.find('.selectboxit-text');    dropSpan = $main.find('.selectboxit');    inputDiv = $main.find('.hm-srch-inpt');        dropSpan.width((textSpan.width() + PADDING_SELECT) + 'px');    inputDiv.width(($main.width() - dropSpan.parent().width() - BORDER_WIDTH ) + 'px');       };   var placeHolder = function(){        var textBox = $id + ' .searchInput';       $j(document).on('blur', textBox, function () {               placeText($j(this), SEARCH_TEXT);           });           $j(document).on('focus', textBox, function () {               clrText($j(this), SEARCH_TEXT);           });           $j(document).on('input', textBox, function () {               placeText($j(this), SEARCH_TEXT);               clrText($j(this), SEARCH_TEXT, true);           });            placeText($j(textBox), SEARCH_TEXT);   };    var placeText = function (base, txt) {           if ($j.trim(base.val()) === '') {               base.val(txt);               base.addClass('plcfont');                          } else if ($j.trim(base.val()) !== txt) {               base.removeClass('plcfont');           }        };       var clrText = function (base, txt, isAddStyle) {           if ($j.trim(base.val()) === txt) {               base.val('');               base.removeClass('plcfont');           }       };   initEvent();  };   return {   init : init  }; })(jQuery);        jQuery(function(j){     var $id='#search-menu-9', $main=j($id), $searchInput = $main.find('.searchInput'), $option = $main.find('[selectit="searchOptions"]');     PCM.dropDown.init($id, $main, $searchInput, $option);     PCM.typeAhead.init($main, $searchInput, "/ajaxCall/typeahead", $option); });   {{#category}} &lt;h3 class="first"&gt;Matching Keywords&lt;/h3&gt; &lt;ul class="first-lvl"&gt;  {{#suggestions}}     &lt;li&gt;&lt;a href="/s?rch&amp;includeImage=true&amp;q={{keyword}}&amp;ssrc=box"&gt;&lt;span class="txt"&gt;{{keyword}}&lt;/span&gt;&lt;span class="count"&gt;({{count}})&lt;/span&gt;&lt;/a&gt;         {{#firstSection}}         &lt;ul class="second-lvl"&gt;             {{#items}}             &lt;li&gt;&lt;a href="/s?rch&amp;includeImage=true&amp;q={{keyword}}&amp;stn={{name}}&amp;ssrc=box" data-keyword="{{keyword}}"&gt;in {{name}}&lt;/a&gt;&lt;/li&gt;             {{/items}}         &lt;/ul&gt;         {{/firstSection}}     &lt;/li&gt;     {{/suggestions}} &lt;/ul&gt; {{/category}} {{#brand}} &lt;h3&gt;Matching Brands&lt;/h3&gt; &lt;ul class="second-lvl"&gt;  {{#items}}  &lt;li&gt;&lt;a href="/s?rch&amp;includeImage=true&amp;q={{keyword}}&amp;man={{name}}&amp;ssrc=box" data-keyword="{{keyword}}"&gt;by {{name}}&lt;/a&gt;&lt;/li&gt;  {{/items}} &lt;/ul&gt; {{/brand}} {{#product}} &lt;h3&gt;Suggestions for {{keyword}}&lt;/h3&gt; &lt;ul class="suggest"&gt;  {{#items}}     &lt;li&gt;         &lt;a href="/p/{{edp}}" title="{{name}}" data-keyword="{{edp}}"&gt;             &lt;span class="tbl"&gt;                 &lt;span class="tr"&gt;                     &lt;span class="td col-img"&gt;&lt;img src="{{#imagePath}}{{imagePath}}{{/imagePath}}{{^imagePath}}/mall/widgetti/images/shared/noImageMed.jpg{{/imagePath}}" e_src="/mall/widgetti/images/shared/noImageMed.jpg" width="67"&gt;&lt;/span&gt;                     &lt;span class="td col-desc"&gt;                         &lt;span class="offer"&gt;{{manufacturer}}&lt;/span&gt;                         &lt;span class="prod-title"&gt;{{name}}&lt;/span&gt;                     &lt;/span&gt;                 &lt;/span&gt;             &lt;/span&gt;         &lt;/a&gt;     &lt;/li&gt;     {{/items}} &lt;/ul&gt; {{/product}}                                                                        document.getElementsByName = function(name){    return jQuery('[name="' + name + '"]');    }                                                                                                                                                                                                                                                             jQuery(function($){     PCM.slideBanner.init($('#sldr-widget-10'), '/home?1453599977565&amp;op=mall.web.misc.layeredSlider.layeredSlider&amp;banners=msc-home-10#banners'); });                               Picking the Right Printer for your Office [INFOGRAPHIC]                     January 19, 2016                     Microsoft Announces Major Change to the Enterprise Agreement Program                     January 6, 2016                     How Christmas Gifts Could Impact BYOD                     January 4, 2016                     Enhance Your Creativity with Adobe Stock                     December 30, 2015                     HP Print Security Seminars: Is Your Network at Risk to Hackers?                     December 22, 2015                     Share Costs and Save Time with Hewlett Packard Enterprise Healthcare                     December 21, 2015                     Microsoft Announces that Windows Server 2016 will be Launching Next Quarter                     December 11, 2015                     Last Chance to Register for Vision Hollywood!                     December 10, 2015                     How Big of a Deal is the Apple-Cisco Partnership?                     December 9, 2015                     Webcast: ShoreTel Truly Unified Communications                     December 8, 2015                     Ergotron StyleView: Fit for Every Body                     December 7, 2015                     The Digital Pulse of Tomorrow’s Healthcare with Lenovo                     December 7, 2015                                                                               jQuery(function($){     PCM.newsFeed.init();     var t8=$('.pcm-nws .trunk8'),li=t8.closest('li');     li.css('display','block');     t8.trunk8().removeClass('trunk8');     li.css('display','');      //Reapply title to support html tags   var rcNws =  jQuery('.hm-nws').find('.rc-nws');   var title = jQuery('.hm-nws').find('.titleTempHolder').val();   rcNws.html(title);   jQuery('.hm-nws').find('.titleTempHolder').remove();    });                                                                                  Deal of the Week                     HP 14" G3 Quad-Core ChromebookOnly $179.99               Shop Now                                                                                    Lenovo B40-80 80F6 Notebook              Reach a New Height inBusiness ComputingOnly $349.99                Shop Now                                                                       Managed Print Services              Save Millions. Gain Visibility. Take Control.               Shop Now                                                                                   Featured Products                                                         Bestsellers                                                         New Arrivals                                                         Trending                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                      &lt;div class="prd-tbl-con rctb hide-avail"&gt;         &lt;div class="tr"&gt; {{#products}}     &lt;div class="tbl-cll itemlist {{first}} {{last}}" data-sku="{{dpno}}"&gt;         &lt;!--if secret sale         &lt;div class="icn-vio-ssp"&gt;&lt;/div&gt;         --&gt;         {{#lowestPrice}}         &lt;div class="icn-vio-gbp"&gt;&lt;/div&gt;         {{/lowestPrice}}         &lt;div class="item {{first}} {{last}}"&gt;             &lt;div class="itm-img"&gt;                 &lt;img class="img-load" src="/widgets/product-view/img/load.gif" /&gt;                 {{^notAvailable}}&lt;a class="prod-image" href="{{link}}" title="{{name}}"&gt;&lt;img class="pro-image" src="{{imgSrc}}"                     e_src="/widgets/product-view/img/noImage_150.jpg"/&gt;&lt;/a&gt;{{/notAvailable}}                 {{#notAvailable}}&lt;img class="pro-image" src="/mall/widgetti/images/shared/notAvailable_150.jpg"                     e_src="/widgets/product-view/img/noImage_150.jpg"/&gt;{{/notAvailable}}             &lt;/div&gt;             {{^savePrice}}             &lt;div class="item-cll npsve"&gt;&lt;/div&gt;             {{/savePrice}}             {{#savePrice}}             &lt;div class="itm-sve"&gt;                 &lt;span&gt;Save&lt;/span&gt; &lt;span class="svprc"&gt;{{savePrice}}&lt;/span&gt;{{#savePercent}} &lt;span class="nrm"&gt;(&lt;/span&gt;&lt;span                     class="sv-prcnt nrm"&gt;{{savePercent}}&lt;/span&gt;&lt;span class="nrm"&gt;)&lt;/span&gt;{{/savePercent}}             &lt;/div&gt;             {{/savePrice}}              &lt;div class="itm-ttl prod-name"&gt;                 &lt;h2&gt;                     {{^notAvailable}}&lt;a href="{{link}}" title="{{name}}"&gt;{{name}}&lt;/a&gt;{{/notAvailable}}                     {{#notAvailable}}&lt;span class="prodName"&gt;Product is No Longer Available&lt;/span&gt;{{/notAvailable}}                 &lt;/h2&gt;             &lt;/div&gt;             &lt;div class="itm-eval prod-avail"&gt;                 {{^notAvailable}}                 &lt;div class="avlb"&gt;                     &lt;span class="avlbs"&gt;Availability:&lt;/span&gt;                     &lt;span class="statavlb"&gt;{{availability}}&lt;/span&gt;                 &lt;/div&gt;                 {{#rateValue}}                 &lt;div class="istr"&gt;                     &lt;div class="str" style="width: {{rate}}%;"&gt;&lt;/div&gt;                 &lt;/div&gt;                 &lt;div class="rater"&gt;                     &lt;a href="{{link}}#pdppdpUserReview" title="Ratings"&gt; ({{rateValue}})&lt;/a&gt;                 &lt;/div&gt;                 {{/rateValue}}                 {{^rateValue}}                 &lt;div class="nstr rater"&gt;&lt;a href="https://www.pcm.com/o/Write-A-Review/msc-66?op=mall.web.zones.pdpRecentReviews.writeReview&amp;amp;dpno={{dpno}}" title="Be the first to write a review"&gt;Be the first to write a review&lt;/a&gt;&lt;/div&gt;                 {{/rateValue}}                 {{/notAvailable}}             &lt;/div&gt;             &lt;div class="itm-prc"&gt;                 &lt;div class="pprcd"&gt;                     &lt;!--if secretsale                     &lt;div class="rprice upp ssp"&gt;                         &lt;span class="ntce"&gt;Secret Sale Price&lt;/span&gt;                     &lt;/div&gt;                     --&gt;                     &lt;!--else--&gt;                      &lt;div class="prc lprc"&gt;                         &lt;p&gt;{{listPrice}}&lt;/p&gt;                     &lt;/div&gt;                     &lt;div class="prc tprc"&gt;                         &lt;p class="prod-price"&gt;{{totalPrice}}&lt;/p&gt;                     &lt;/div&gt;                     &lt;div class="clr"&gt;&lt;/div&gt;                     &lt;!--end--&gt;                 &lt;/div&gt;                 {{#enableCartBtn}}                 &lt;div class="crt-btn"&gt;                 {{#lowestPrice}}                     &lt;div class="crt upp"&gt;                         &lt;a data-action="Button:See Lowest Price" data-label="prod-{{dpno}}" href="{{link}}" class="ga" title="See Lowest Price"&gt;See Lowest Price&lt;/a&gt;                     &lt;/div&gt;                 {{/lowestPrice}}                 {{#callPrice}}                     &lt;div class="crt upp"&gt;                          &lt;a  href="{{link}}" class="upplinks ga" title="Call For Price"&gt;Call For Price&lt;/a&gt;                     &lt;/div&gt;                 {{/callPrice}}                 {{#addCart}}                     &lt;div class="qty"&gt;                         &lt;div class="bl"&gt;&lt;/div&gt;                         &lt;input type="text" id="addCartQty{{dpno}}" value="1" maxlength="3"&gt;                         &lt;div class="br"&gt;&lt;/div&gt;                         &lt;div class="clr"&gt;&lt;/div&gt;                     &lt;/div&gt;                     &lt;div class="crt"&gt;                         &lt;a href="#section=category&amp;amp;sku={{dpno}}" class="mbxlinks" metadata="{{metadata}}"                            title="Add to Cart"&gt;Add to Cart&lt;/a&gt;                     &lt;/div&gt;                 {{/addCart}}                 &lt;div class="clr"&gt;&lt;/div&gt;                 &lt;/div&gt;                 {{/enableCartBtn}}             &lt;/div&gt;         &lt;/div&gt;     &lt;/div&gt; {{/products}}     &lt;/div&gt; &lt;/div&gt;   &lt;div class="pge"&gt;     &lt;div class="num"&gt;         &lt;span class="crnt"&gt;{{startIndex}}&lt;/span&gt;&lt;span&gt;-&lt;/span&gt;&lt;span class="lmtpg"&gt;{{endIndex}}&lt;/span&gt;&lt;/span&gt;         &lt;span&gt;of&lt;/span&gt;&lt;span class="ttl"&gt;{{totalRecords}}&lt;/span&gt;     &lt;/div&gt;     &lt;div class="arw"&gt;         &lt;a href="#" class="lft {{left}}" data-page="{{previousPage}}"&gt;&lt;div class="aim {{left}}"&gt;&lt;/div&gt; &lt;/a&gt;         &lt;a href="#" class="rht {{right}}" data-page="{{nextPage}}"&gt;&lt;div class="aim {{right}}"&gt;&lt;/div&gt;&lt;/a&gt;         &lt;div class="clr"&gt;&lt;/div&gt;     &lt;/div&gt;     &lt;div class="clr"&gt;&lt;/div&gt; &lt;/div&gt;   &lt;div class="cnt bh-enabled"&gt;     &lt;h4&gt;You have no recently viewed items to display.&lt;/h4&gt;     &lt;p&gt;Can't find what you're searching for? Try one of these categories:&lt;/p&gt;     &lt;ul&gt;         {{#links}}&lt;li&gt;&lt;a title="{{label}}" href="{{link}}"{{#newTab}} target="_blank"{{/newTab}}&gt;{{label}}&lt;/a&gt;&lt;/li&gt;{{/links}}     &lt;/ul&gt; &lt;/div&gt; &lt;div class="cnt bh-disabled"&gt;     &lt;h4&gt;Your browsing history is disabled. &lt;a class="onbrowtrigger enable-browsing" href="#enable" url="/ajaxCall/recentlyviewed"&gt;Enable browsing history&lt;/a&gt;&lt;/h4&gt;     &lt;p&gt;Keep track of what you've viewed by turning on your browsing history. See items you've viewed, searches you've conducted and products you've visited.&lt;/p&gt; &lt;/div&gt;    jQuery(function($){     var $id = '#prod-view-tb-36';     PCM.productView.init($id);     PCM.gridRotate.init($($id).width(), $id, '.itemlist'); });                                  test                Preferred Partners                                                                                                                                                                                                   Menu                                            WELCOME TO PCM!                                                                                                                                                                                                                                     Thank You!                                                         Thank you for subscribing to our newsletter. Be sure to check your email for exclusive offers and discounts.                                   jQuery(document).ready(function() {      PCM.subscribeEmailValidate.init({formNewsLetterEle: '#email-subscribe',          allowPageReload : false});  });      1-800-700-1000    (function(c, h, a, t, _, i, d) {     c[_] = c[_] || function() {         (c[_].q = c[_].q || []).push(arguments)     }, c[_].l = 1 * new Date();     i = h.createElement(a), d = h.getElementsByTagName(a)[0];     i.async = 1;     i.src = t;     d.parentNode.insertBefore(i, d) })(window, document, 'script', 'https://chatidcdn.com/embed/pcm/latest.js', 'CID');            Follow     PCM Blog  Spiceworks  Facebook  LinkedIn  Twitter  YouTube            jQuery(document).ready(function(){  var pcm_tooltip_opts = {};   if('useContentID' == 'useContentID' &amp;&amp; '#follow-us-social' != ''){   pcm_tooltip_opts.customContentID = '#follow-us-social';  }else if('useContentID' == 'customContent' &amp;&amp; '' != ''){   pcm_tooltip_opts.customContent = ''  }   if('' != ''){   pcm_tooltip_opts.isThemeHeader = true;   pcm_tooltip_opts.headerTitle = '';   pcm_tooltip_opts.headerBg = '#1b5d9e';   pcm_tooltip_opts.headerColor = '#000';  }   if('1px' != '0' &amp;&amp; '1px' != '0px'){   pcm_tooltip_opts.tooltipBorderSize = '1px';   pcm_tooltip_opts.tooltipBorderColor = '#e6e6e6';  }    if('' != ''){ pcm_tooltip_opts.width = ''; }  if('25px' != ''){ pcm_tooltip_opts.customArrowPos = '25px'; }  if('bottom' != 'auto'){ pcm_tooltip_opts.tooltipShowDirection = 'bottom'; }  if('#fff' != ''){ pcm_tooltip_opts.contentBGcolor = '#fff'; }  if('10px' != ''){ pcm_tooltip_opts.contentPadding = '10px'; }  if('-4' != ''){ pcm_tooltip_opts.distanceFromBaseElement = '-4'; }  if('800' != ''){ pcm_tooltip_opts.zIndex = '800'; }    pcm_tooltip_opts.eventsArray = 'click'.split(',');    jQuery('#follow-link').pcm_tooltip(pcm_tooltip_opts); });            jQuery(document).ready(function(){  var pcm_tooltip_opts = {};   if('useHref' == 'useContentID' &amp;&amp; '' != ''){   pcm_tooltip_opts.customContentID = '';  }else if('useHref' == 'customContent' &amp;&amp; '' != ''){   pcm_tooltip_opts.customContent = ''  }   if('' != ''){   pcm_tooltip_opts.isThemeHeader = true;   pcm_tooltip_opts.headerTitle = '';   pcm_tooltip_opts.headerBg = '#1b5d9e';   pcm_tooltip_opts.headerColor = '#000';  }   if('1px' != '0' &amp;&amp; '1px' != '0px'){   pcm_tooltip_opts.tooltipBorderSize = '1px';   pcm_tooltip_opts.tooltipBorderColor = '#e6e6e6';  }    if('' != ''){ pcm_tooltip_opts.width = ''; }  if('19px' != ''){ pcm_tooltip_opts.customArrowPos = '19px'; }  if('bottom' != 'auto'){ pcm_tooltip_opts.tooltipShowDirection = 'bottom'; }  if('#fff' != ''){ pcm_tooltip_opts.contentBGcolor = '#fff'; }  if('0' != ''){ pcm_tooltip_opts.contentPadding = '0'; }  if('-4' != ''){ pcm_tooltip_opts.distanceFromBaseElement = '-4'; }  if('800' != ''){ pcm_tooltip_opts.zIndex = '800'; }    pcm_tooltip_opts.eventsArray = 'click'.split(',');    jQuery('.sslink.dropd.ttipdwn').pcm_tooltip(pcm_tooltip_opts); });       Sign in                                                     Order Status                                                Sign In                                   New account?  Register                                                     /* jQuery(function($){                 PCM.tooltipDown.init('#signin-btn-21');             }); */                     Cart ()   var PCM = PCM || {}; PCM.cart=(function($){     function update(){         $.ajax({             url:"/home?op=mall.web.misc.cartLink.cartLink",             type:'POST',             dataType:'json',             data:'false',             success:count         });     }     function count(data){         if(typeof data !== 'undefined'){             $('[data-bind="cart-count"]').text(data.count)         }     }     return {         update:update     }; })(jQuery); PCM.cart.update();                                                                                                                                                                    PCM (Home)                                              STARTUPS / ENTREPRENEURSMEDIUM / LARGE BUSINESSENTERPRISEHEALTHCARE                                                                                                                                              GOV</v>
+        <v>PCM IT Solutions Services Businesstobusiness focused computer sales Missioncritical systems services including data storage solutions PCM We mean business PCM data storage solutions Solutions Services Cloud Products More than an IT Provider Were Your Technology Partner Thank You PCM Home GOVERNMENT Home EPROCUREMENT Cloud Partners PCM Hybrid Cloud Featured Hardware Software Brands Deal of the Week Lenovo B4080 80F6 Notebook Managed Print Services Preferred Partners Our Company Support We Provide PCM Blog Spiceworks Facebook LinkedIn Twitter YouTube Sign in Order Status Sign In New account Register jQueryfunction PCMtooltipDowninitsigninbtn21 Cart STARTUPS ENTREPRENEURS MEDIUM LARGE BUSINESS ENTERPRISE HEALTHCARE FEDERAL STATE LOCAL EDUCATION HEALTHCARE PCM BUSINESS DIRECT PCM OPSTRACK Cloud Products Shop Now Learn More Deal of the Week Top Searches Ultrabook Finder Memory Finder InkToner Finder Accessories Cables Computers Memory Monitors Projectors Networking Printers Supplies Racks Power Cooling Scanners Servers Storage Backup Business Database Desktop Web Publishing Management Operating Systems Security Unified Collaboration Virtualization Apple Cisco Dell Google HPI HPE Intel Lenovo Microsoft Samsung Symantec VMware Picking the Right Printer for your Office INFOGRAPHIC January 19 2016 Microsoft Announces Major Change to the Enterprise Agreement Program January 6 2016 How Christmas Gifts Could Impact BYOD January 4 2016 Enhance Your Creativity with Adobe Stock December 30 2015 HP Print Security Seminars Is Your Network at Risk to Hackers December 22 2015 Share Costs and Save Time with Hewlett Packard Enterprise Healthcare December 21 2015 Microsoft Announces that Windows Server 2016 will be Launching Next Quarter December 11 2015 Last Chance to Register for Vision Hollywood December 10 2015 How Big of a Deal is the AppleCisco Partnership December 9 2015 Webcast ShoreTel Truly Unified Communications December 8 2015 Ergotron StyleView Fit for Every Body December 7 2015 The Digital Pulse of Tomorrow’s Healthcare with Lenovo December 7 2015 Featured Products Bestsellers New Arrivals Trending You may give each page an identifying name server and channel on the next lines spageNameHomepage Redesign sserverAFSPLPCMWS03 schannelHome sprop1Home sprop2Home sprop3Home sprop4Home seVar15AFB49840F39445DDB175335A2CD47BDB DO NOT ALTER ANYTHING BELOW THIS LINE var scodestifscodedocumentwritescode Menu WELCOME TO PCM Thank You Thank you for subscribing to our newsletter Be sure to check your email for exclusive offers and discounts jQuerydocumentreadyfunction PCMsubscribeEmailValidateinitformNewsLetterEle emailsubscribe allowPageReload false 18007001000 functionc h a t i d c c function cq cq pusharguments cl 1 new Date i hcreateElementa d hgetElementsByTagNamea0 iasync 1 isrc t dparentNodeinsertBeforei d window document script httpschatidcdncomembedpcmlatestjs CID Follow PCM Blog Spiceworks Facebook LinkedIn Twitter YouTube jQuerydocumentreadyfunction var pcmtooltipopts ifuseContentID useContentID followussocial pcmtooltipoptscustomContentID followussocial else ifuseContentID customContent pcmtooltipoptscustomContent if pcmtooltipoptsisThemeHeader true pcmtooltipoptsheaderTitle pcmtooltipoptsheaderBg 1b5d9e pcmtooltipoptsheaderColor 000 if1px 0 1px 0px pcmtooltipoptstooltipBorderSize 1px pcmtooltipoptstooltipBorderColor e6e6e6 if pcmtooltipoptswidth if25px pcmtooltipoptscustomArrowPos 25px ifbottom auto pcmtooltipoptstooltipShowDirection bottom iffff pcmtooltipoptscontentBGcolor fff if10px pcmtooltipoptscontentPadding 10px if4 pcmtooltipoptsdistanceFromBaseElement 4 if800 pcmtooltipoptszIndex 800 pcmtooltipoptseventsArray clicksplit jQueryfollowlinkpcmtooltippcmtooltipopts jQuerydocumentreadyfunction var pcmtooltipopts ifuseHref useContentID pcmtooltipoptscustomContentID else ifuseHref customContent pcmtooltipoptscustomContent if pcmtooltipoptsisThemeHeader true pcmtooltipoptsheaderTitle pcmtooltipoptsheaderBg 1b5d9e pcmtooltipoptsheaderColor 000 if1px 0 1px 0px pcmtooltipoptstooltipBorderSize 1px pcmtooltipoptstooltipBorderColor e6e6e6 if pcmtooltipoptswidth if19px pcmtooltipoptscustomArrowPos 19px ifbottom auto pcmtooltipoptstooltipShowDirection bottom iffff pcmtooltipoptscontentBGcolor fff if0 pcmtooltipoptscontentPadding 0 if4 pcmtooltipoptsdistanceFromBaseElement 4 if800 pcmtooltipoptszIndex 800 pcmtooltipoptseventsArray clicksplit jQuerysslinkdropdttipdwnpcmtooltippcmtooltipopts Sign in Order Status Sign In New account Register jQueryfunction PCMtooltipDowninitsigninbtn21 Cart var PCM PCM PCMcartfunction function update ajax urlhomeopmallwebmisccartLinkcartLink typePOST dataTypejson datafalse successcount function countdata iftypeof data undefined databindcartcounttextdatacount return updateupdate jQuery PCMcartupdate PCM Home STARTUPS ENTREPRENEURSMEDIUM LARGE BUSINESSENTERPRISEHEALTHCARE GOVERNMENT Home FEDERALSTATE LOCALEDUCATIONHEALTHCARE EPROCUREMENT PCM BUSINESS DIRECTPCM OPSTRACK jQueryfunction PCMchangeHomepageinit var lastClickedTab lastclickedtab var active getCookielastClickedTab var widgetdrkmmenu13 greetwidgetfindgreetingstxt ifmsc515msc497msc428msc429msc426msc427mschomemsc430msc425indexOfmschome 1 active mschome var txtwidgetfindnavpointid active iftxtlength var greetings txtattrgreetings ifgreetings greettextgreetings txtaddClassactv else widgetfindanavpointidfirstaddClassactv greetshow var host windowlocationhost var links widgetfindanavpointid linksclickfunctione var navId thisattrnavpointid hrefthisattrhref ifnavId href hrefcharAt0 hosthrefsplit2 documentcookie lastClickedTab navId expires setExpirationDate30 path var setExpirationDate functiondays var date new Date datesetTimedategetTimedays2460601000 return datetoUTCString var getCookie functionname var nameEQ name var ca documentcookiesplit forvar i0i calengthi var c jQuerytrimcai if cindexOfnameEQ 0 return csubstringnameEQlengthclength return null Solutions Services Cloud Products Cloud Partners Shop Now PCM Hybrid Cloud Learn More Featured Deal of the Week Top Searches Ultrabook Finder Memory Finder InkToner Finder Hardware Accessories Cables Computers Memory Monitors Projectors Networking Printers Supplies Racks Power Cooling Scanners Servers Storage All Categories Software Backup Business Database Desktop Web Publishing Management Operating Systems Security Unified Collaboration Virtualization All Categories Brands Apple Cisco Dell Google HPI HPE Intel Lenovo Microsoft Samsung Symantec VMware All Brands jQueryfunction PCMmainNavinit var contstaticlinksconmenunav contshow menunav staticlinksconeachfunctionit var h0 tfindsubgroupnameeachfunctionis hMathmaxhsheight eachfunctionis sheighth conthide All Products Mfg Part Number PCM Part Number PCMdropDown functionj var init functionid main inputBar elem var dropDownDiv var textSpan var dropSpan var inputDiv var searchNow mainfindsearchInputBtn var SEARCHTEXT Search Products var PADDINGSELECT 30 var BORDERWIDTH 1 var initEvent function placeHolder elemselectBoxIt elemchangefunction adjustSearchBox searchNowclickfunction checkInputBox return false inputBarkeypressfunctione ifewhich 13 checkInputBox return false adjustSearchBox var checkInputBox function var val jtriminputBarvalreplaceg ifvallength 0 val SEARCHTEXT alertPlease enter a search keyword PCMmodalBx width 350modalopenModalerrorsearch else var typeelem val encodeURIComponentval q typevalreplace0g val url typeattrhref val q q windowlocation urljoin var adjustSearchBox function textSpan mainfindselectboxittext dropSpan mainfindselectboxit inputDiv mainfindhmsrchinpt dropSpanwidthtextSpanwidth PADDINGSELECT px inputDivwidthmainwidth dropSpanparentwidth BORDERWIDTH px var placeHolder function var textBox id searchInput jdocumentonblur textBox function placeTextjthis SEARCHTEXT jdocumentonfocus textBox function clrTextjthis SEARCHTEXT jdocumentoninput textBox function placeTextjthis SEARCHTEXT clrTextjthis SEARCHTEXT true placeTextjtextBox SEARCHTEXT var placeText function base txt if jtrimbaseval basevaltxt baseaddClassplcfont else if jtrimbaseval txt baseremoveClassplcfont var clrText function base txt isAddStyle if jtrimbaseval txt baseval baseremoveClassplcfont initEvent return init init jQuery jQueryfunctionj var idsearchmenu9 mainjid searchInput mainfindsearchInput option mainfindselectitsearchOptions PCMdropDowninitid main searchInput option PCMtypeAheadinitmain searchInput ajaxCalltypeahead option category h3 classfirstMatching Keywordsh3 ul classfirstlvl suggestions lia hrefsrchincludeImagetrueqkeywordssrcboxspan classtxtkeywordspanspan classcountcountspana firstSection ul classsecondlvl items lia hrefsrchincludeImagetrueqkeywordstnnamessrcbox datakeywordkeywordin nameali items ul firstSection li suggestions ul category brand h3Matching Brandsh3 ul classsecondlvl items lia hrefsrchincludeImagetrueqkeywordmannamessrcbox datakeywordkeywordby nameali items ul brand product h3Suggestions for keywordh3 ul classsuggest items li a hrefpedp titlename datakeywordedp span classtbl span classtr span classtd colimgimg srcimagePathimagePathimagePathimagePathmallwidgettiimagessharednoImageMedjpgimagePath esrcmallwidgettiimagessharednoImageMedjpg width67span span classtd coldesc span classoffermanufacturerspan span classprodtitlenamespan span span span a li items ul product documentgetElementsByName functionname return jQueryname name jQueryfunction PCMslideBannerinitsldrwidget10 home1453659360039opmallwebmisclayeredSliderlayeredSliderbannersmschome10banners Picking the Right Printer for your Office INFOGRAPHIC January 19 2016 Microsoft Announces Major Change to the Enterprise Agreement Program January 6 2016 How Christmas Gifts Could Impact BYOD January 4 2016 Enhance Your Creativity with Adobe Stock December 30 2015 HP Print Security Seminars Is Your Network at Risk to Hackers December 22 2015 Share Costs and Save Time with Hewlett Packard Enterprise Healthcare December 21 2015 Microsoft Announces that Windows Server 2016 will be Launching Next Quarter December 11 2015 Last Chance to Register for Vision Hollywood December 10 2015 How Big of a Deal is the AppleCisco Partnership December 9 2015 Webcast ShoreTel Truly Unified Communications December 8 2015 Ergotron StyleView Fit for Every Body December 7 2015 The Digital Pulse of Tomorrow’s Healthcare with Lenovo December 7 2015 jQueryfunction PCMnewsFeedinit var t8pcmnws trunk8lit8closestli licssdisplayblock t8trunk8removeClasstrunk8 licssdisplay Reapply title to support html tags var rcNws jQueryhmnwsfindrcnws var title jQueryhmnwsfindtitleTempHolderval rcNwshtmltitle jQueryhmnwsfindtitleTempHolderremove Deal of the Week HP 14 G3 QuadCore ChromebookOnly 17999 Shop Now Lenovo B4080 80F6 Notebook Reach a New Height inBusiness ComputingOnly 34999 Shop Now Managed Print Services Save Millions Gain Visibility Take Control Shop Now Featured Products Bestsellers New Arrivals Trending div classprdtblcon rctb hideavail div classtr products div classtblcll itemlist first last dataskudpno if secret sale div classicnviosspdiv lowestPrice div classicnviogbpdiv lowestPrice div classitem first last div classitmimg img classimgload srcwidgetsproductviewimgloadgif notAvailablea classprodimage hreflink titlenameimg classproimage srcimgSrc esrcwidgetsproductviewimgnoImage150jpganotAvailable notAvailableimg classproimage srcmallwidgettiimagessharednotAvailable150jpg esrcwidgetsproductviewimgnoImage150jpgnotAvailable div savePrice div classitemcll npsvediv savePrice savePrice div classitmsve spanSavespan span classsvprcsavePricespansavePercent span classnrmspanspan classsvprcnt nrmsavePercentspanspan classnrmspansavePercent div savePrice div classitmttl prodname h2 notAvailablea hreflink titlenamenameanotAvailable notAvailablespan classprodNameProduct is No Longer AvailablespannotAvailable h2 div div classitmeval prodavail notAvailable div classavlb span classavlbsAvailabilityspan span classstatavlbavailabilityspan div rateValue div classistr div classstr stylewidth ratediv div div classrater a hreflinkpdppdpUserReview titleRatings rateValuea div rateValue rateValue div classnstr ratera hrefhttpswwwpcmcomoWriteAReviewmsc66opmallwebzonespdpRecentReviewswriteReviewampdpnodpno titleBe the first to write a reviewBe the first to write a reviewadiv rateValue notAvailable div div classitmprc div classpprcd if secretsale div classrprice upp ssp span classntceSecret Sale Pricespan div else div classprc lprc plistPricep div div classprc tprc p classprodpricetotalPricep div div classclrdiv end div enableCartBtn div classcrtbtn lowestPrice div classcrt upp a dataactionButtonSee Lowest Price datalabelproddpno hreflink classga titleSee Lowest PriceSee Lowest Pricea div lowestPrice callPrice div classcrt upp a hreflink classupplinks ga titleCall For PriceCall For Pricea div callPrice addCart div classqty div classbldiv input typetext idaddCartQtydpno value1 maxlength3 div classbrdiv div classclrdiv div div classcrt a hrefsectioncategoryampskudpno classmbxlinks metadatametadata titleAdd to CartAdd to Carta div addCart div classclrdiv div enableCartBtn div div div products div div div classpge div classnum span classcrntstartIndexspanspanspanspan classlmtpgendIndexspanspan spanofspanspan classttltotalRecordsspan div div classarw a href classlft left datapagepreviousPagediv classaim leftdiv a a href classrht right datapagenextPagediv classaim rightdiva div classclrdiv div div classclrdiv div div classcnt bhenabled h4You have no recently viewed items to displayh4 pCant find what youre searching for Try one of these categoriesp ul linkslia titlelabel hreflinknewTab targetblanknewTablabelalilinks ul div div classcnt bhdisabled h4Your browsing history is disabled a classonbrowtrigger enablebrowsing hrefenable urlajaxCallrecentlyviewedEnable browsing historyah4 pKeep track of what youve viewed by turning on your browsing history See items youve viewed searches youve conducted and products youve visitedp div jQueryfunction var id prodviewtb36 PCMproductViewinitid PCMgridRotateinitidwidth id itemlist test Preferred Partners Menu WELCOME TO PCM Thank You Thank you for subscribing to our newsletter Be sure to check your email for exclusive offers and discounts jQuerydocumentreadyfunction PCMsubscribeEmailValidateinitformNewsLetterEle emailsubscribe allowPageReload false 18007001000 functionc h a t i d c c function cq cq pusharguments cl 1 new Date i hcreateElementa d hgetElementsByTagNamea0 iasync 1 isrc t dparentNodeinsertBeforei d window document script httpschatidcdncomembedpcmlatestjs CID Follow PCM Blog Spiceworks Facebook LinkedIn Twitter YouTube jQuerydocumentreadyfunction var pcmtooltipopts ifuseContentID useContentID followussocial pcmtooltipoptscustomContentID followussocial else ifuseContentID customContent pcmtooltipoptscustomContent if pcmtooltipoptsisThemeHeader true pcmtooltipoptsheaderTitle pcmtooltipoptsheaderBg 1b5d9e pcmtooltipoptsheaderColor 000 if1px 0 1px 0px pcmtooltipoptstooltipBorderSize 1px pcmtooltipoptstooltipBorderColor e6e6e6 if pcmtooltipoptswidth if25px pcmtooltipoptscustomArrowPos 25px ifbottom auto pcmtooltipoptstooltipShowDirection bottom iffff pcmtooltipoptscontentBGcolor fff if10px pcmtooltipoptscontentPadding 10px if4 pcmtooltipoptsdistanceFromBaseElement 4 if800 pcmtooltipoptszIndex 800 pcmtooltipoptseventsArray clicksplit jQueryfollowlinkpcmtooltippcmtooltipopts jQuerydocumentreadyfunction var pcmtooltipopts ifuseHref useContentID pcmtooltipoptscustomContentID else ifuseHref customContent pcmtooltipoptscustomContent if pcmtooltipoptsisThemeHeader true pcmtooltipoptsheaderTitle pcmtooltipoptsheaderBg 1b5d9e pcmtooltipoptsheaderColor 000 if1px 0 1px 0px pcmtooltipoptstooltipBorderSize 1px pcmtooltipoptstooltipBorderColor e6e6e6 if pcmtooltipoptswidth if19px pcmtooltipoptscustomArrowPos 19px ifbottom auto pcmtooltipoptstooltipShowDirection bottom iffff pcmtooltipoptscontentBGcolor fff if0 pcmtooltipoptscontentPadding 0 if4 pcmtooltipoptsdistanceFromBaseElement 4 if800 pcmtooltipoptszIndex 800 pcmtooltipoptseventsArray clicksplit jQuerysslinkdropdttipdwnpcmtooltippcmtooltipopts Sign in Order Status Sign In New account Register jQueryfunction PCMtooltipDowninitsigninbtn21 Cart var PCM PCM PCMcartfunction function update ajax urlhomeopmallwebmisccartLinkcartLink typePOST dataTypejson datafalse successcount function countdata iftypeof data undefined databindcartcounttextdatacount return updateupdate jQuery PCMcartupdate PCM Home STARTUPS ENTREPRENEURSMEDIUM LARGE BUSINESSENTERPRISEHEALTHCARE GOVERNMENT Home FEDERALSTATE LOCALEDUCATIONHEALTHCARE EPROCUREMENT PCM BUSINESS DIRECTPCM OPSTRACK jQueryfunction PCMchangeHomepageinit var lastClickedTab lastclickedtab var active getCookielastClickedTab var widgetdrkmmenu13 greetwidgetfindgreetingstxt ifmsc515msc497msc428msc429msc426msc427mschomemsc430msc425indexOfmschome 1 active mschome var txtwidgetfindnavpointid active iftxtlength var greetings txtattrgreetings ifgreetings greettextgreetings txtaddClassactv else widgetfindanavpointidfirstaddClassactv greetshow var host windowlocationhost var links widgetfindanavpointid linksclickfunctione var navId thisattrnavpointid hrefthisattrhref ifnavId href hrefcharAt0 hosthrefsplit2 documentcookie lastClickedTab navId expires setExpirationDate30 path var setExpirationDate functiondays var date new Date datesetTimedategetTimedays2460601000 return datetoUTCString var getCookie functionname var nameEQ name var ca documentcookiesplit forvar i0i calengthi var c jQuerytrimcai if cindexOfnameEQ 0 return csubstringnameEQlengthclength return null Solutions Services Cloud Products Cloud Partners Shop Now PCM Hybrid Cloud Learn More Featured Deal of the Week Top Searches Ultrabook Finder Memory Finder InkToner Finder Hardware Accessories Cables Computers Memory Monitors Projectors Networking Printers Supplies Racks Power Cooling Scanners Servers Storage All Categories Software Backup Business Database Desktop Web Publishing Management Operating Systems Security Unified Collaboration Virtualization All Categories Brands Apple Cisco Dell Google HPI HPE Intel Lenovo Microsoft Samsung Symantec VMware All Brands jQueryfunction PCMmainNavinit var contstaticlinksconmenunav contshow menunav staticlinksconeachfunctionit var h0 tfindsubgroupnameeachfunctionis hMathmaxhsheight eachfunctionis sheighth conthide All Products Mfg Part Number PCM Part Number PCMdropDown functionj var init functionid main inputBar elem var dropDownDiv var textSpan var dropSpan var inputDiv var searchNow mainfindsearchInputBtn var SEARCHTEXT Search Products var PADDINGSELECT 30 var BORDERWIDTH 1 var initEvent function placeHolder elemselectBoxIt elemchangefunction adjustSearchBox searchNowclickfunction checkInputBox return false inputBarkeypressfunctione ifewhich 13 checkInputBox return false adjustSearchBox var checkInputBox function var val jtriminputBarvalreplaceg ifvallength 0 val SEARCHTEXT alertPlease enter a search keyword PCMmodalBx width 350modalopenModalerrorsearch else var typeelem val encodeURIComponentval q typevalreplace0g val url typeattrhref val q q windowlocation urljoin var adjustSearchBox function textSpan mainfindselectboxittext dropSpan mainfindselectboxit inputDiv mainfindhmsrchinpt dropSpanwidthtextSpanwidth PADDINGSELECT px inputDivwidthmainwidth dropSpanparentwidth BORDERWIDTH px var placeHolder function var textBox id searchInput jdocumentonblur textBox function placeTextjthis SEARCHTEXT jdocumentonfocus textBox function clrTextjthis SEARCHTEXT jdocumentoninput textBox function placeTextjthis SEARCHTEXT clrTextjthis SEARCHTEXT true placeTextjtextBox SEARCHTEXT var placeText function base txt if jtrimbaseval basevaltxt baseaddClassplcfont else if jtrimbaseval txt baseremoveClassplcfont var clrText function base txt isAddStyle if jtrimbaseval txt baseval baseremoveClassplcfont initEvent return init init jQuery jQueryfunctionj var idsearchmenu9 mainjid searchInput mainfindsearchInput option mainfindselectitsearchOptions PCMdropDowninitid main searchInput option PCMtypeAheadinitmain searchInput ajaxCalltypeahead option category h3 classfirstMatching Keywordsh3 ul classfirstlvl suggestions lia hrefsrchincludeImagetrueqkeywordssrcboxspan classtxtkeywordspanspan classcountcountspana firstSection ul classsecondlvl items lia hrefsrchincludeImagetrueqkeywordstnnamessrcbox datakeywordkeywordin nameali items ul firstSection li suggestions ul category brand h3Matching Brandsh3 ul classsecondlvl items lia hrefsrchincludeImagetrueqkeywordmannamessrcbox datakeywordkeywordby nameali items ul brand product h3Suggestions for keywordh3 ul classsuggest items li a hrefpedp titlename datakeywordedp span classtbl span classtr span classtd colimgimg srcimagePathimagePathimagePathimagePathmallwidgettiimagessharednoImageMedjpgimagePath esrcmallwidgettiimagessharednoImageMedjpg width67span span classtd coldesc span classoffermanufacturerspan span classprodtitlenamespan span span span a li items ul product documentgetElementsByName functionname return jQueryname name Menu WELCOME TO PCM Thank You Thank you for subscribing to our newsletter Be sure to check your email for exclusive offers and discounts jQuerydocumentreadyfunction PCMsubscribeEmailValidateinitformNewsLetterEle emailsubscribe allowPageReload false 18007001000 functionc h a t i d c c function cq cq pusharguments cl 1 new Date i hcreateElementa d hgetElementsByTagNamea0 iasync 1 isrc t dparentNodeinsertBeforei d window document script httpschatidcdncomembedpcmlatestjs CID Follow PCM Blog Spiceworks Facebook LinkedIn Twitter YouTube jQuerydocumentreadyfunction var pcmtooltipopts ifuseContentID useContentID followussocial pcmtooltipoptscustomContentID followussocial else ifuseContentID customContent pcmtooltipoptscustomContent if pcmtooltipoptsisThemeHeader true pcmtooltipoptsheaderTitle pcmtooltipoptsheaderBg 1b5d9e pcmtooltipoptsheaderColor 000 if1px 0 1px 0px pcmtooltipoptstooltipBorderSize 1px pcmtooltipoptstooltipBorderColor e6e6e6 if pcmtooltipoptswidth if25px pcmtooltipoptscustomArrowPos 25px ifbottom auto pcmtooltipoptstooltipShowDirection bottom iffff pcmtooltipoptscontentBGcolor fff if10px pcmtooltipoptscontentPadding 10px if4 pcmtooltipoptsdistanceFromBaseElement 4 if800 pcmtooltipoptszIndex 800 pcmtooltipoptseventsArray clicksplit jQueryfollowlinkpcmtooltippcmtooltipopts jQuerydocumentreadyfunction var pcmtooltipopts ifuseHref useContentID pcmtooltipoptscustomContentID else ifuseHref customContent pcmtooltipoptscustomContent if pcmtooltipoptsisThemeHeader true pcmtooltipoptsheaderTitle pcmtooltipoptsheaderBg 1b5d9e pcmtooltipoptsheaderColor 000 if1px 0 1px 0px pcmtooltipoptstooltipBorderSize 1px pcmtooltipoptstooltipBorderColor e6e6e6 if pcmtooltipoptswidth if19px pcmtooltipoptscustomArrowPos 19px ifbottom auto pcmtooltipoptstooltipShowDirection bottom iffff pcmtooltipoptscontentBGcolor fff if0 pcmtooltipoptscontentPadding 0 if4 pcmtooltipoptsdistanceFromBaseElement 4 if800 pcmtooltipoptszIndex 800 pcmtooltipoptseventsArray clicksplit jQuerysslinkdropdttipdwnpcmtooltippcmtooltipopts Sign in Order Status Sign In New account Register jQueryfunction PCMtooltipDowninitsigninbtn21 Cart var PCM PCM PCMcartfunction function update ajax urlhomeopmallwebmisccartLinkcartLink typePOST dataTypejson datafalse successcount function countdata iftypeof data undefined databindcartcounttextdatacount return updateupdate jQuery PCMcartupdate PCM Home STARTUPS ENTREPRENEURSMEDIUM LARGE BUSINESSENTERPRISEHEALTHCARE GOVERNMENT Home FEDERALSTATE LOCALEDUCATIONHEALTHCARE EPROCUREMENT PCM BUSINESS DIRECTPCM OPSTRACK jQueryfunction PCMchangeHomepageinit var lastClickedTab lastclickedtab var active getCookielastClickedTab var widgetdrkmmenu13 greetwidgetfindgreetingstxt ifmsc515msc497msc428msc429msc426msc427mschomemsc430msc425indexOfmschome 1 active mschome var txtwidgetfindnavpointid active iftxtlength var greetings txtattrgreetings ifgreetings greettextgreetings txtaddClassactv else widgetfindanavpointidfirstaddClassactv greetshow var host windowlocationhost var links widgetfindanavpointid linksclickfunctione var navId thisattrnavpointid hrefthisattrhref ifnavId href hrefcharAt0 hosthrefsplit2 documentcookie lastClickedTab navId expires setExpirationDate30 path var setExpirationDate functiondays var date new Date datesetTimedategetTimedays2460601000 return datetoUTCString var getCookie functionname var nameEQ name var ca documentcookiesplit forvar i0i calengthi var c jQuerytrimcai if cindexOfnameEQ 0 return csubstringnameEQlengthclength return null Solutions Services Cloud Products Cloud Partners Shop Now PCM Hybrid Cloud Learn More Featured Deal of the Week Top Searches Ultrabook Finder Memory Finder InkToner Finder Hardware Accessories Cables Computers Memory Monitors Projectors Networking Printers Supplies Racks Power Cooling Scanners Servers Storage All Categories Software Backup Business Database Desktop Web Publishing Management Operating Systems Security Unified Collaboration Virtualization All Categories Brands Apple Cisco Dell Google HPI HPE Intel Lenovo Microsoft Samsung Symantec VMware All Brands jQueryfunction PCMmainNavinit var contstaticlinksconmenunav contshow menunav staticlinksconeachfunctionit var h0 tfindsubgroupnameeachfunctionis hMathmaxhsheight eachfunctionis sheighth conthide All Products Mfg Part Number PCM Part Number PCMdropDown functionj var init functionid main inputBar elem var dropDownDiv var textSpan var dropSpan var inputDiv var searchNow mainfindsearchInputBtn var SEARCHTEXT Search Products var PADDINGSELECT 30 var BORDERWIDTH 1 var initEvent function placeHolder elemselectBoxIt elemchangefunction adjustSearchBox searchNowclickfunction checkInputBox return false inputBarkeypressfunctione ifewhich 13 checkInputBox return false adjustSearchBox var checkInputBox function var val jtriminputBarvalreplaceg ifvallength 0 val SEARCHTEXT alertPlease enter a search keyword PCMmodalBx width 350modalopenModalerrorsearch else var typeelem val encodeURIComponentval q typevalreplace0g val url typeattrhref val q q windowlocation urljoin var adjustSearchBox function textSpan mainfindselectboxittext dropSpan mainfindselectboxit inputDiv mainfindhmsrchinpt dropSpanwidthtextSpanwidth PADDINGSELECT px inputDivwidthmainwidth dropSpanparentwidth BORDERWIDTH px var placeHolder function var textBox id searchInput jdocumentonblur textBox function placeTextjthis SEARCHTEXT jdocumentonfocus textBox function clrTextjthis SEARCHTEXT jdocumentoninput textBox function placeTextjthis SEARCHTEXT clrTextjthis SEARCHTEXT true placeTextjtextBox SEARCHTEXT var placeText function base txt if jtrimbaseval basevaltxt baseaddClassplcfont else if jtrimbaseval txt baseremoveClassplcfont var clrText function base txt isAddStyle if jtrimbaseval txt baseval baseremoveClassplcfont initEvent return init init jQuery jQueryfunctionj var idsearchmenu9 mainjid searchInput mainfindsearchInput option mainfindselectitsearchOptions PCMdropDowninitid main searchInput option PCMtypeAheadinitmain searchInput ajaxCalltypeahead option category h3 classfirstMatching Keywordsh3 ul classfirstlvl suggestions lia hrefsrchincludeImagetrueqkeywordssrcboxspan classtxtkeywordspanspan classcountcountspana firstSection ul classsecondlvl items lia hrefsrchincludeImagetrueqkeywordstnnamessrcbox datakeywordkeywordin nameali items ul firstSection li suggestions ul category brand h3Matching Brandsh3 ul classsecondlvl items lia hrefsrchincludeImagetrueqkeywordmannamessrcbox datakeywordkeywordby nameali items ul brand product h3Suggestions for keywordh3 ul classsuggest items li a hrefpedp titlename datakeywordedp span classtbl span classtr span classtd colimgimg srcimagePathimagePathimagePathimagePathmallwidgettiimagessharednoImageMedjpgimagePath esrcmallwidgettiimagessharednoImageMedjpg width67span span classtd coldesc span classoffermanufacturerspan span classprodtitlenamespan span span span a li items ul product documentgetElementsByName functionname return jQueryname name Menu WELCOME TO PCM Thank You Thank you for subscribing to our newsletter Be sure to check your email for exclusive offers and discounts jQuerydocumentreadyfunction PCMsubscribeEmailValidateinitformNewsLetterEle emailsubscribe allowPageReload false 18007001000 functionc h a t i d c c function cq cq pusharguments cl 1 new Date i hcreateElementa d hgetElementsByTagNamea0 iasync 1 isrc t dparentNodeinsertBeforei d window document script httpschatidcdncomembedpcmlatestjs CID Follow PCM Blog Spiceworks Facebook LinkedIn Twitter YouTube jQuerydocumentreadyfunction var pcmtooltipopts ifuseContentID useContentID followussocial pcmtooltipoptscustomContentID followussocial else ifuseContentID customContent pcmtooltipoptscustomContent if pcmtooltipoptsisThemeHeader true pcmtooltipoptsheaderTitle pcmtooltipoptsheaderBg 1b5d9e pcmtooltipoptsheaderColor 000 if1px 0 1px 0px pcmtooltipoptstooltipBorderSize 1px pcmtooltipoptstooltipBorderColor e6e6e6 if pcmtooltipoptswidth if25px pcmtooltipoptscustomArrowPos 25px ifbottom auto pcmtooltipoptstooltipShowDirection bottom iffff pcmtooltipoptscontentBGcolor fff if10px pcmtooltipoptscontentPadding 10px if4 pcmtooltipoptsdistanceFromBaseElement 4 if800 pcmtooltipoptszIndex 800 pcmtooltipoptseventsArray clicksplit jQueryfollowlinkpcmtooltippcmtooltipopts jQuerydocumentreadyfunction var pcmtooltipopts ifuseHref useContentID pcmtooltipoptscustomContentID else ifuseHref customContent pcmtooltipoptscustomContent if pcmtooltipoptsisThemeHeader true pcmtooltipoptsheaderTitle pcmtooltipoptsheaderBg 1b5d9e pcmtooltipoptsheaderColor 000 if1px 0 1px 0px pcmtooltipoptstooltipBorderSize 1px pcmtooltipoptstooltipBorderColor e6e6e6 if pcmtooltipoptswidth if19px pcmtooltipoptscustomArrowPos 19px ifbottom auto pcmtooltipoptstooltipShowDirection bottom iffff pcmtooltipoptscontentBGcolor fff if0 pcmtooltipoptscontentPadding 0 if4 pcmtooltipoptsdistanceFromBaseElement 4 if800 pcmtooltipoptszIndex 800 pcmtooltipoptseventsArray clicksplit jQuerysslinkdropdttipdwnpcmtooltippcmtooltipopts Sign in Order Status Sign In New account Register jQueryfunction PCMtooltipDowninitsigninbtn21 Cart var PCM PCM PCMcartfunction function update ajax urlhomeopmallwebmisccartLinkcartLink typePOST dataTypejson datafalse successcount function countdata iftypeof data undefined databindcartcounttextdatacount return updateupdate jQuery PCMcartupdate PCM Home STARTUPS ENTREPRENEURSMEDIUM LARGE BUSINESSENTERPRISEHEALTHCARE GOVERNMENT Home FEDERALSTATE LOCALEDUCATIONHEALTHCARE EPROCUREMENT PCM BUSINESS DIRECTPCM OPSTRACK jQueryfunction PCMchangeHomepageinit var lastClickedTab lastclickedtab var active getCookielastClickedTab var widgetdrkmmenu13 greetwidgetfindgreetingstxt ifmsc515msc497msc428msc429msc426msc427mschomemsc430msc425indexOfmschome 1 active mschome var txtwidgetfindnavpointid active iftxtlength var greetings txtattrgreetings ifgreetings greettextgreetings txtaddClassactv else widgetfindanavpointidfirstaddClassactv greetshow var host windowlocationhost var links widgetfindanavpointid linksclickfunctione var navId thisattrnavpointid hrefthisattrhref ifnavId href hrefcharAt0 hosthrefsplit2 documentcookie lastClickedTab navId expires setExpirationDate30 path var setExpirationDate functiondays var date new Date datesetTimedategetTimedays2460601000 return datetoUTCString var getCookie functionname var nameEQ name var ca documentcookiesplit forvar i0i calengthi var c jQuerytrimcai if cindexOfnameEQ 0 return csubstringnameEQlengthclength return null Solutions Services Cloud Products Cloud Partners Shop Now PCM Hybrid Cloud Learn More Featured Deal of the Week Top Searches Ultrabook Finder Memory Finder InkToner Finder Hardware Accessories Cables Computers Memory Monitors Projectors Networking Printers Supplies Racks Power Cooling Scanners Servers Storage All Categories Software Backup Business Database Desktop Web Publishing Management Operating Systems Security Unified Collaboration Virtualization All Categories Brands Apple Cisco Dell Google HPI HPE Intel Lenovo Microsoft Samsung Symantec VMware All Brands jQueryfunction PCMmainNavinit var contstaticlinksconmenunav contshow menunav staticlinksconeachfunctionit var h0 tfindsubgroupnameeachfunctionis hMathmaxhsheight eachfunctionis sheighth conthide All Products Mfg Part Number PCM Part Number PCMdropDown functionj var init functionid main inputBar elem var dropDownDiv var textSpan var dropSpan var inputDiv var searchNow mainfindsearchInputBtn var SEARCHTEXT Search Products var PADDINGSELECT 30 var BORDERWIDTH 1 var initEvent function</v>
       </c>
       <c r="D7" t="str">
-        <v>ERNMENT (Home)                                              FEDERALSTATE &amp; LOCALEDUCATIONHEALTHCARE                                                                                                                                              E-PROCUREMENT                                              PCM BUSINESS DIRECTPCM OPSTRACK                                                             jQuery(function($){     PCM.changeHomepage.init();     var lastClickedTab = 'last_clicked_tab';     var active = getCookie(lastClickedTab);     var widget=$("#drk-mmenu-13"), $greet=widget.find('.greetings-txt');     if('msc-515,msc-497,msc-428,msc-429,msc-426,msc-427,msc-home,msc-430,msc-425,'.indexOf('msc-home,') &gt; -1){   active = 'msc-home';  }     var txt=widget.find('[navpoint-id="' + active + '"]')     if(txt.length) {         var greetings = txt.attr('greetings');         if(greetings) {             $greet.text(greetings);         }         txt.addClass('actv');     }else{      widget.find('a[navpoint-id]').first().addClass('actv');     }     $greet.show();          var host = window.location.host;     var links= widget.find('a[navpoint-id]')     links.click(function(e){      var navId = $(this).attr('navpoint-id'), href=$(this).attr('href');      if(navId &amp;&amp; href &amp;&amp; (href.charAt(0)=='/' || host===href.split('/')[2])){       document.cookie = lastClickedTab + '=' + navId + '; expires=' + setExpirationDate(30) + '; path=/';      }     });     var setExpirationDate = function(days){      var date = new Date();         date.setTime(date.getTime()+(days*24*60*60*1000));         return date.toUTCString();     };      });  var getCookie = function(name){  var nameEQ = name + "=";     var ca = document.cookie.split(';');     for(var i=0;i &lt; ca.length;i++) {         var c = jQuery.trim(ca[i]);         if (c.indexOf(nameEQ) === 0) return c.substring(nameEQ.length,c.length);     }     return null; };                                        Solutions &amp; Services                Cloud    Products                                                                                               Cloud Partners                                             Shop Now                                                                                                        PCM Hybrid Cloud                                             Learn More                                                                                                                                                   Featured                                    Deal of the Week                  Top Searches                  Ultrabook Finder                  Memory Finder                  Ink/Toner Finder                                                                                               Hardware                                    Accessories                  Cables                  Computers                  Memory                  Monitors &amp; Projectors                  Networking                  Printers &amp; Supplies                  Racks, Power &amp; Cooling                  Scanners                  Servers                  Storage                                           All Categories                                                                              Software                                    Backup                  Business                  Database                  Desktop &amp; Web Publishing                  Management                  Operating Systems                  Security                  Unified Collaboration                  Virtualization                                           All Categories                                                                              Brands                                    Apple                  Cisco                  Dell                  Google                  HPI                  HPE                  Intel                  Lenovo                  Microsoft                  Samsung                  Symantec                  VMware                                           All Brands                                                       jQuery(function($){     PCM.mainNav.init();     var cont=$('.static-links-con,.menu-nav');     cont.show();     $('.menu-nav .static-links-con').each(function(i,t){         var h=0;         $(t).find('.sub-group-name').each(function(i,s){             h=Math.max(h,$(s).height());         }).each(function(i,s){             $(s).height(h);         });     });     cont.hide(); });                            All Products     Mfg Part Number     PCM Part Number                                                      PCM.dropDown = (function($j) {  var init = function($id, $main, inputBar, elem) {   var dropDownDiv;   var textSpan;   var dropSpan;   var inputDiv;   var searchNow = $main.find('.searchInputBtn');      var SEARCH_TEXT = 'Search Products';   var PADDING_SELECT = 30;   var BORDER_WIDTH = 1;    var initEvent = function() {        placeHolder();    elem.selectBoxIt();    elem.change(function(){                 adjustSearchBox();             });    searchNow.click(function(){     checkInputBox();     return false;    });    inputBar.keypress(function(e){     if(e.which === 13){      checkInputBox();      return false;     }    });        adjustSearchBox();   };   var checkInputBox = function(){    var val = $j.trim(inputBar.val()).replace(/\\/g, "");             if(val.length === 0 || val === SEARCH_TEXT){                 alert('Please enter a search keyword');                 //PCM.modalBx('', {'width': 350}).modal().openModal('#error-search');             }else{                 var $type=elem,                 _val = encodeURIComponent(val),                 _q = $type.val().replace(/$0/g, _val),                 url = [$type.attr('href'), _val, _q?"&amp;":"", _q];                 window.location= url.join("");             }   };   var adjustSearchBox = function(){    textSpan = $main.find('.selectboxit-text');    dropSpan = $main.find('.selectboxit');    inputDiv = $main.find('.hm-srch-inpt');        dropSpan.width((textSpan.width() + PADDING_SELECT) + 'px');    inputDiv.width(($main.width() - dropSpan.parent().width() - BORDER_WIDTH ) + 'px');       };   var placeHolder = function(){        var textBox = $id + ' .searchInput';       $j(document).on('blur', textBox, function () {               placeText($j(this), SEARCH_TEXT);           });           $j(document).on('focus', textBox, function () {               clrText($j(this), SEARCH_TEXT);           });           $j(document).on('input', textBox, function () {               placeText($j(this), SEARCH_TEXT);               clrText($j(this), SEARCH_TEXT, true);           });            placeText($j(textBox), SEARCH_TEXT);   };    var placeText = function (base, txt) {           if ($j.trim(base.val()) === '') {               base.val(txt);               base.addClass('plcfont');                          } else if ($j.trim(base.val()) !== txt) {               base.removeClass('plcfont');           }        };       var clrText = function (base, txt, isAddStyle) {           if ($j.trim(base.val()) === txt) {               base.val('');               base.removeClass('plcfont');           }       };   initEvent();  };   return {   init : init  }; })(jQuery);        jQuery(function(j){     var $id='#search-menu-9', $main=j($id), $searchInput = $main.find('.searchInput'), $option = $main.find('[selectit="searchOptions"]');     PCM.dropDown.init($id, $main, $searchInput, $option);     PCM.typeAhead.init($main, $searchInput, "/ajaxCall/typeahead", $option); });   {{#category}} &lt;h3 class="first"&gt;Matching Keywords&lt;/h3&gt; &lt;ul class="first-lvl"&gt;  {{#suggestions}}     &lt;li&gt;&lt;a href="/s?rch&amp;includeImage=true&amp;q={{keyword}}&amp;ssrc=box"&gt;&lt;span class="txt"&gt;{{keyword}}&lt;/span&gt;&lt;span class="count"&gt;({{count}})&lt;/span&gt;&lt;/a&gt;         {{#firstSection}}         &lt;ul class="second-lvl"&gt;             {{#items}}             &lt;li&gt;&lt;a href="/s?rch&amp;includeImage=true&amp;q={{keyword}}&amp;stn={{name}}&amp;ssrc=box" data-keyword="{{keyword}}"&gt;in {{name}}&lt;/a&gt;&lt;/li&gt;             {{/items}}         &lt;/ul&gt;         {{/firstSection}}     &lt;/li&gt;     {{/suggestions}} &lt;/ul&gt; {{/category}} {{#brand}} &lt;h3&gt;Matching Brands&lt;/h3&gt; &lt;ul class="second-lvl"&gt;  {{#items}}  &lt;li&gt;&lt;a href="/s?rch&amp;includeImage=true&amp;q={{keyword}}&amp;man={{name}}&amp;ssrc=box" data-keyword="{{keyword}}"&gt;by {{name}}&lt;/a&gt;&lt;/li&gt;  {{/items}} &lt;/ul&gt; {{/brand}} {{#product}} &lt;h3&gt;Suggestions for {{keyword}}&lt;/h3&gt; &lt;ul class="suggest"&gt;  {{#items}}     &lt;li&gt;         &lt;a href="/p/{{edp}}" title="{{name}}" data-keyword="{{edp}}"&gt;             &lt;span class="tbl"&gt;                 &lt;span class="tr"&gt;                     &lt;span class="td col-img"&gt;&lt;img src="{{#imagePath}}{{imagePath}}{{/imagePath}}{{^imagePath}}/mall/widgetti/images/shared/noImageMed.jpg{{/imagePath}}" e_src="/mall/widgetti/images/shared/noImageMed.jpg" width="67"&gt;&lt;/span&gt;                     &lt;span class="td col-desc"&gt;                         &lt;span class="offer"&gt;{{manufacturer}}&lt;/span&gt;                         &lt;span class="prod-title"&gt;{{name}}&lt;/span&gt;                     &lt;/span&gt;                 &lt;/span&gt;             &lt;/span&gt;         &lt;/a&gt;     &lt;/li&gt;     {{/items}} &lt;/ul&gt; {{/product}}                                                                        document.getElementsByName = function(name){    return jQuery('[name="' + name + '"]');    }                                                                                                                 Menu                                            WELCOME TO PCM!                                                                                                                                                                                                                                     Thank You!                                                         Thank you for subscribing to our newsletter. Be sure to check your email for exclusive offers and discounts.                                   jQuery(document).ready(function() {      PCM.subscribeEmailValidate.init({formNewsLetterEle: '#email-subscribe',          allowPageReload : false});  });      1-800-700-1000    (function(c, h, a, t, _, i, d) {     c[_] = c[_] || function() {         (c[_].q = c[_].q || []).push(arguments)     }, c[_].l = 1 * new Date();     i = h.createElement(a), d = h.getElementsByTagName(a)[0];     i.async = 1;     i.src = t;     d.parentNode.insertBefore(i, d) })(window, document, 'script', 'https://chatidcdn.com/embed/pcm/latest.js', 'CID');            Follow     PCM Blog  Spiceworks  Facebook  LinkedIn  Twitter  YouTube            jQuery(document).ready(function(){  var pcm_tooltip_opts = {};   if('useContentID' == 'useContentID' &amp;&amp; '#follow-us-social' != ''){   pcm_tooltip_opts.customContentID = '#follow-us-social';  }else if('useContentID' == 'customContent' &amp;&amp; '' != ''){   pcm_tooltip_opts.customContent = ''  }   if('' != ''){   pcm_tooltip_opts.isThemeHeader = true;   pcm_tooltip_opts.headerTitle = '';   pcm_tooltip_opts.headerBg = '#1b5d9e';   pcm_tooltip_opts.headerColor = '#000';  }   if('1px' != '0' &amp;&amp; '1px' != '0px'){   pcm_tooltip_opts.tooltipBorderSize = '1px';   pcm_tooltip_opts.tooltipBorderColor = '#e6e6e6';  }    if('' != ''){ pcm_tooltip_opts.width = ''; }  if('25px' != ''){ pcm_tooltip_opts.customArrowPos = '25px'; }  if('bottom' != 'auto'){ pcm_tooltip_opts.tooltipShowDirection = 'bottom'; }  if('#fff' != ''){ pcm_tooltip_opts.contentBGcolor = '#fff'; }  if('10px' != ''){ pcm_tooltip_opts.contentPadding = '10px'; }  if('-4' != ''){ pcm_tooltip_opts.distanceFromBaseElement = '-4'; }  if('800' != ''){ pcm_tooltip_opts.zIndex = '800'; }    pcm_tooltip_opts.eventsArray = 'click'.split(',');    jQuery('#follow-link').pcm_tooltip(pcm_tooltip_opts); });            jQuery(document).ready(function(){  var pcm_tooltip_opts = {};   if('useHref' == 'useContentID' &amp;&amp; '' != ''){   pcm_tooltip_opts.customContentID = '';  }else if('useHref' == 'customContent' &amp;&amp; '' != ''){   pcm_tooltip_opts.customContent = ''  }   if('' != ''){   pcm_tooltip_opts.isThemeHeader = true;   pcm_tooltip_opts.headerTitle = '';   pcm_tooltip_opts.headerBg = '#1b5d9e';   pcm_tooltip_opts.headerColor = '#000';  }   if('1px' != '0' &amp;&amp; '1px' != '0px'){   pcm_tooltip_opts.tooltipBorderSize = '1px';   pcm_tooltip_opts.tooltipBorderColor = '#e6e6e6';  }    if('' != ''){ pcm_tooltip_opts.width = ''; }  if('19px' != ''){ pcm_tooltip_opts.customArrowPos = '19px'; }  if('bottom' != 'auto'){ pcm_tooltip_opts.tooltipShowDirection = 'bottom'; }  if('#fff' != ''){ pcm_tooltip_opts.contentBGcolor = '#fff'; }  if('0' != ''){ pcm_tooltip_opts.contentPadding = '0'; }  if('-4' != ''){ pcm_tooltip_opts.distanceFromBaseElement = '-4'; }  if('800' != ''){ pcm_tooltip_opts.zIndex = '800'; }    pcm_tooltip_opts.eventsArray = 'click'.split(',');    jQuery('.sslink.dropd.ttipdwn').pcm_tooltip(pcm_tooltip_opts); });       Sign in                                                     Order Status                                                Sign In                                   New account?  Register                                                     /* jQuery(function($){                 PCM.tooltipDown.init('#signin-btn-21');             }); */                     Cart ()   var PCM = PCM || {}; PCM.cart=(function($){     function update(){         $.ajax({             url:"/home?op=mall.web.misc.cartLink.cartLink",             type:'POST',             dataType:'json',             data:'false',             success:count         });     }     function count(data){         if(typeof data !== 'undefined'){             $('[data-bind="cart-count"]').text(data.count)         }     }     return {         update:update     }; })(jQuery); PCM.cart.update();                                                                                                                                                                    PCM (Home)                                              STARTUPS / ENTREPRENEURSMEDIUM / LARGE BUSINESSENTERPRISEHEALTHCARE                                                                                                                                              GOVERNMENT (Home)                                              FEDERALSTATE &amp; LOCALEDUCATIONHEALTHCARE                                                                                                                                              E-PROCUREMENT                                              PCM BUSINESS DIRECTPCM OPSTRACK                                                             jQuery(function($){     PCM.changeHomepage.init();     var lastClickedTab = 'last_clicked_tab';     var active = getCookie(lastClickedTab);     var widget=$("#drk-mmenu-13"), $greet=widget.find('.greetings-txt');     if('msc-515,msc-497,msc-428,msc-429,msc-426,msc-427,msc-home,msc-430,msc-425,'.indexOf('msc-home,') &gt; -1){   active = 'msc-home';  }     var txt=widget.find('[navpoint-id="' + active + '"]')     if(txt.length) {         var greetings = txt.attr('greetings');         if(greetings) {             $greet.text(greetings);         }         txt.addClass('actv');     }else{      widget.find('a[navpoint-id]').first().addClass('actv');     }     $greet.show();          var host = window.location.host;     var links= widget.find('a[navpoint-id]')     links.click(function(e){      var navId = $(this).attr('navpoint-id'), href=$(this).attr('href');      if(navId &amp;&amp; href &amp;&amp; (href.charAt(0)=='/' || host===href.split('/')[2])){       document.cookie = lastClickedTab + '=' + navId + '; expires=' + setExpirationDate(30) + '; path=/';      }     });     var setExpirationDate = function(days){      var date = new Date();         date.setTime(date.getTime()+(days*24*60*60*1000));         return date.toUTCString();     };      });  var getCookie = function(name){  var nameEQ = name + "=";     var ca = document.cookie.split(';');     for(var i=0;i &lt; ca.length;i++) {         var c = jQuery.trim(ca[i]);         if (c.indexOf(nameEQ) === 0) return c.substring(nameEQ.length,c.length);     }     return null; };                                        Solutions &amp; Services                Cloud    Products                                                                                               Cloud Partners                                             Shop Now                                                                                                        PCM Hybrid Cloud                                             Learn More                                                                                                                                                   Featured                                    Deal of the Week                  Top Searches                  Ultrabook Finder                  Memory Finder                  Ink/Toner Finder                                                                                               Hardware                                    Accessories                  Cables                  Computers                  Memory                  Monitors &amp; Projectors                  Networking                  Printers &amp; Supplies                  Racks, Power &amp; Cooling                  Scanners                  Servers                  Storage                                           All Categories                                                                              Software                                    Backup                  Business                  Database                  Desktop &amp; Web Publishing                  Management                  Operating Systems                  Security                  Unified Collaboration                  Virtualization                                           All Categories                                                                              Brands                                    Apple                  Cisco                  Dell                  Google                  HPI                  HPE                  Intel                  Lenovo                  Microsoft                  Samsung                  Symantec                  VMware                                           All Brands                                                       jQuery(function($){     PCM.mainNav.init();     var cont=$('.static-links-con,.menu-nav');     cont.show();     $('.menu-nav .static-links-con').each(function(i,t){         var h=0;         $(t).find('.sub-group-name').each(function(i,s){             h=Math.max(h,$(s).height());         }).each(function(i,s){             $(s).height(h);         });     });     cont.hide(); });                            All Products     Mfg Part Number     PCM Part Number                                                      PCM.dropDown = (function($j) {  var init = function($id, $main, inputBar, elem) {   var dropDownDiv;   var textSpan;   var dropSpan;   var inputDiv;   var searchNow = $main.find('.searchInputBtn');      var SEARCH_TEXT = 'Search Products';   var PADDING_SELECT = 30;   var BORDER_WIDTH = 1;    var initEvent = function() {        placeHolder();    elem.selectBoxIt();    elem.change(function(){                 adjustSearchBox();             });    searchNow.click(function(){     checkInputBox();     return false;    });    inputBar.keypress(function(e){     if(e.which === 13){      checkInputBox();      return false;     }    });        adjustSearchBox();   };   var checkInputBox = function(){    var val = $j.trim(inputBar.val()).replace(/\\/g, "");             if(val.length === 0 || val === SEARCH_TEXT){                 alert('Please enter a search keyword');                 //PCM.modalBx('', {'width': 350}).modal().openModal('#error-search');             }else{                 var $type=elem,                 _val = encodeURIComponent(val),                 _q = $type.val().replace(/$0/g, _val),                 url = [$type.attr('href'), _val, _q?"&amp;":"", _q];                 window.location= url.join("");             }   };   var adjustSearchBox = function(){    textSpan = $main.find('.selectboxit-text');    dropSpan = $main.find('.selectboxit');    inputDiv = $main.find('.hm-srch-inpt');        dropSpan.width((textSpan.width() + PADDING_SELECT) + 'px');    inputDiv.width(($main.width() - dropSpan.parent().width() - BORDER_WIDTH ) + 'px');       };   var placeHolder = function(){        var textBox = $id + ' .searchInput';       $j(document).on('blur', textBox, function () {               placeText($j(this), SEARCH_TEXT);           });           $j(document).on('focus', textBox, function () {               clrText($j(this), SEARCH_TEXT);           });           $j(document).on('input', textBox, function () {               placeText($j(this), SEARCH_TEXT);               clrText($j(this), SEARCH_TEXT, true);           });            placeText($j(textBox), SEARCH_TEXT);   };    var placeText = function (base, txt) {           if ($j.trim(base.val()) === '') {               base.val(txt);               base.addClass('plcfont');                          } else if ($j.trim(base.val()) !== txt) {               base.removeClass('plcfont');           }        };       var clrText = function (base, txt, isAddStyle) {           if ($j.trim(base.val()) === txt) {               base.val('');               base.removeClass('plcfont');           }       };   initEvent();  };   return {   init : init  }; })(jQuery);        jQuery(function(j){     var $id='#search-menu-9', $main=j($id), $searchInput = $main.find('.searchInput'), $option = $main.find('[selectit="searchOptions"]');     PCM.dropDown.init($id, $main, $searchInput, $option);     PCM.typeAhead.init($main, $searchInput, "/ajaxCall/typeahead", $option); });   {{#category}} &lt;h3 class="first"&gt;Matching Keywords&lt;/h3&gt; &lt;ul class="first-lvl"&gt;  {{#suggestions}}     &lt;li&gt;&lt;a href="/s?rch&amp;includeImage=true&amp;q={{keyword}}&amp;ssrc=box"&gt;&lt;span class="txt"&gt;{{keyword}}&lt;/span&gt;&lt;span class="count"&gt;({{count}})&lt;/span&gt;&lt;/a&gt;         {{#firstSection}}         &lt;ul class="second-lvl"&gt;             {{#items}}             &lt;li&gt;&lt;a href="/s?rch&amp;includeImage=true&amp;q={{keyword}}&amp;stn={{name}}&amp;ssrc=box" data-keyword="{{keyword}}"&gt;in {{name}}&lt;/a&gt;&lt;/li&gt;             {{/items}}         &lt;/ul&gt;         {{/firstSection}}     &lt;/li&gt;     {{/suggestions}} &lt;/ul&gt; {{/category}} {{#brand}} &lt;h3&gt;Matching Brands&lt;/h3&gt; &lt;ul class="second-lvl"&gt;  {{#items}}  &lt;li&gt;&lt;a href="/s?rch&amp;includeImage=true&amp;q={{keyword}}&amp;man={{name}}&amp;ssrc=box" data-keyword="{{keyword}}"&gt;by {{name}}&lt;/a&gt;&lt;/li&gt;  {{/items}} &lt;/ul&gt; {{/brand}} {{#product}} &lt;h3&gt;Suggestions for {{keyword}}&lt;/h3&gt; &lt;ul class="suggest"&gt;  {{#items}}     &lt;li&gt;         &lt;a href="/p/{{edp}}" title="{{name}}" data-keyword="{{edp}}"&gt;             &lt;span class="tbl"&gt;                 &lt;span class="tr"&gt;                     &lt;span class="td col-img"&gt;&lt;img src="{{#imagePath}}{{imagePath}}{{/imagePath}}{{^imagePath}}/mall/widgetti/images/shared/noImageMed.jpg{{/imagePath}}" e_src="/mall/widgetti/images/shared/noImageMed.jpg" width="67"&gt;&lt;/span&gt;                     &lt;span class="td col-desc"&gt;                         &lt;span class="offer"&gt;{{manufacturer}}&lt;/span&gt;                         &lt;span class="prod-title"&gt;{{name}}&lt;/span&gt;                     &lt;/span&gt;                 &lt;/span&gt;             &lt;/span&gt;         &lt;/a&gt;     &lt;/li&gt;     {{/items}} &lt;/ul&gt; {{/product}}                                                                        document.getElementsByName = function(name){    return jQuery('[name="' + name + '"]');    }                                                                                           Menu                                            WELCOME TO PCM!                                                                                                                                                                                                                                     Thank You!                                                         Thank you for subscribing to our newsletter. Be sure to check your email for exclusive offers and discounts.                                   jQuery(document).ready(function() {      PCM.subscribeEmailValidate.init({formNewsLetterEle: '#email-subscribe',          allowPageReload : false});  });      1-800-700-1000    (function(c, h, a, t, _, i, d) {     c[_] = c[_] || function() {         (c[_].q = c[_].q || []).push(arguments)     }, c[_].l = 1 * new Date();     i = h.createElement(a), d = h.getElementsByTagName(a)[0];     i.async = 1;     i.src = t;     d.parentNode.insertBefore(i, d) })(window, document, 'script', 'https://chatidcdn.com/embed/pcm/latest.js', 'CID');            Follow     PCM Blog  Spiceworks  Facebook  LinkedIn  Twitter  YouTube            jQuery(document).ready(function(){  var pcm_tooltip_opts = {};   if('useContentID' == 'useContentID' &amp;&amp; '#follow-us-social' != ''){   pcm_tooltip_opts.customContentID = '#follow-us-social';  }else if('useContentID' == 'customContent' &amp;&amp; '' != ''){   pcm_tooltip_opts.customContent = ''  }   if('' != ''){   pcm_tooltip_opts.isThemeHeader = true;   pcm_tooltip_opts.headerTitle = '';   pcm_tooltip_opts.headerBg = '#1b5d9e';   pcm_tooltip_opts.headerColor = '#000';  }   if('1px' != '0' &amp;&amp; '1px' != '0px'){   pcm_tooltip_opts.tooltipBorderSize = '1px';   pcm_tooltip_opts.tooltipBorderColor = '#e6e6e6';  }    if('' != ''){ pcm_tooltip_opts.width = ''; }  if('25px' != ''){ pcm_tooltip_opts.customArrowPos = '25px'; }  if('bottom' != 'auto'){ pcm_tooltip_opts.tooltipShowDirection = 'bottom'; }  if('#fff' != ''){ pcm_tooltip_opts.contentBGcolor = '#fff'; }  if('10px' != ''){ pcm_tooltip_opts.contentPadding = '10px'; }  if('-4' != ''){ pcm_tooltip_opts.distanceFromBaseElement = '-4'; }  if('800' != ''){ pcm_tooltip_opts.zIndex = '800'; }    pcm_tooltip_opts.eventsArray = 'click'.split(',');    jQuery('#follow-link').pcm_tooltip(pcm_tooltip_opts); });            jQuery(document).ready(function(){  var pcm_tooltip_opts = {};   if('useHref' == 'useContentID' &amp;&amp; '' != ''){   pcm_tooltip_opts.customContentID = '';  }else if('useHref' == 'customContent' &amp;&amp; '' != ''){   pcm_tooltip_opts.customContent = ''  }   if('' != ''){   pcm_tooltip_opts.isThemeHeader = true;   pcm_tooltip_opts.headerTitle = '';   pcm_tooltip_opts.headerBg = '#1b5d9e';   pcm_tooltip_opts.headerColor = '#000';  }   if('1px' != '0' &amp;&amp; '1px' != '0px'){   pcm_tooltip_opts.tooltipBorderSize = '1px';   pcm_tooltip_opts.tooltipBorderColor = '#e6e6e6';  }    if('' != ''){ pcm_tooltip_opts.width = ''; }  if('19px' != ''){ pcm_tooltip_opts.customArrowPos = '19px'; }  if('bottom' != 'auto'){ pcm_tooltip_opts.tooltipShowDirection = 'bottom'; }  if('#fff' != ''){ pcm_tooltip_opts.contentBGcolor = '#fff'; }  if('0' != ''){ pcm_tooltip_opts.contentPadding = '0'; }  if('-4' != ''){ pcm_tooltip_opts.distanceFromBaseElement = '-4'; }  if('800' != ''){ pcm_tooltip_opts.zIndex = '800'; }    pcm_tooltip_opts.eventsArray = 'click'.split(',');    jQuery('.sslink.dropd.ttipdwn').pcm_tooltip(pcm_tooltip_opts); });       Sign in                                                     Order Status                                                Sign In                                   New account?  Register                                                     /* jQuery(function($){                 PCM.tooltipDown.init('#signin-btn-21');             }); */                     Cart ()   var PCM = PCM || {}; PCM.cart=(function($){     function update(){         $.ajax({             url:"/home?op=mall.web.misc.cartLink.cartLink",             type:'POST',             dataType:'json',             data:'false',             success:count         });     }     function count(data){         if(typeof data !== 'undefined'){             $('[data-bind="cart-count"]').text(data.count)         }     }     return {         update:update     }; })(jQuery); PCM.cart.update();                                                                                                                                                                    PCM (Home)                                              STARTUPS / ENTREPRENEURSMEDIUM / LARGE BUSINESSENTERPRISEHEALTHCARE                                                                                                                                              GOVERNMENT (Home)                                              FEDERALSTATE &amp; LOCALEDUCATIONHEALTHCARE                                                                                                                                              E-PROCUREMENT                                              PCM BUSINESS DIRECTPCM OPSTRACK                                                             jQuery(function($){     PCM.changeHomepage.init();     var lastClickedTab = 'last_clicked_tab';     var active = getCookie(lastClickedTab);     var widget=$("#drk-mmenu-13"), $greet=widget.find('.greetings-txt');     if('msc-515,msc-497,msc-428,msc-429,msc-426,msc-427,msc-home,msc-430,msc-425,'.indexOf('msc-home,') &gt; -1){   active = 'msc-home';  }     var txt=widget.find('[navpoint-id="' + active + '"]')     if(txt.length) {         var greetings = txt.attr('greetings');         if(greetings) {             $greet.text(greetings);         }         txt.addClass('actv');     }else{      widget.find('a[navpoint-id]').first().addClass('actv');     }     $greet.show();          var host = window.location.host;     var links= widget.find('a[navpoint-id]')     links.click(function(e){      var navId = $(this).attr('navpoint-id'), href=$(this).attr('href');      if(navId &amp;&amp; href &amp;&amp; (href.charAt(0)=='/' || host===href.split('/')[2])){       document.cookie = lastClickedTab + '=' + navId + '; expires=' + setExpirationDate(30) + '; path=/';      }     });     var setExpirationDate = function(days){      var date = new Date();         date.setTime(date.getTime()+(days*24*60*60*1000));         return date.toUTCString();     };      });  var getCookie = function(name){  var nameEQ = name + "=";     var ca = document.cookie.split(';');     for(var i=0;i &lt; ca.length;i++) {         var c = jQuery.trim(ca[i]);         if (c.indexOf(nameEQ) === 0) return c.substring(nameEQ.length,c.length);     }     return null; };                                        Solutions &amp; Services                Cloud    Products                                                                                               Cloud Partners                                             Shop Now                                                                                                        PCM Hybrid Cloud                                             Learn More                                                                                                                                                   Featured                                    Deal of the Week                  Top Searches                  Ultrabook Finder                  Memory Finder                  Ink/Toner Finder                                                                                               Hardware                                    Accessories                  Cables                  Computers                  Memory                  Monitors &amp; Projectors                  Networking                  Printers &amp; Supplies                  Racks, Power &amp; Cooling                  Scanners                  Servers                  Storage                                           All Categories                                                                              Software                                    Backup                  Business                  Database                  Desktop &amp; Web Publishing                  Management                  Operating Systems                  Security                  Unified Collaboration                  Virtualization                                           All Categories                                                                              Brands                                    Apple                  Cisco                  Dell                  Google                  HPI                  HPE                  Intel                  Lenovo                  Microsoft                  Samsung                  Symantec                  VMware                                           All Brands                                                       jQuery(function($){     PCM.mainNav.init();     var cont=$('.static-links-con,.menu-nav');     cont.show();     $('.menu-nav .static-links-con').each(function(i</v>
+        <v xml:space="preserve"> placeHolder elemselectBoxIt elemchangefunction adjustSearchBox searchNowclickfunction checkInputBox return false inputBarkeypressfunctione ifewhich 13 checkInputBox return false adjustSearchBox var checkInputBox function var val jtriminputBarvalreplaceg ifvallength 0 val SEARCHTEXT alertPlease enter a search keyword PCMmodalBx width 350modalopenModalerrorsearch else var typeelem val encodeURIComponentval q typevalreplace0g val url typeattrhref val q q windowlocation urljoin var adjustSearchBox function textSpan mainfindselectboxittext dropSpan mainfindselectboxit inputDiv mainfindhmsrchinpt dropSpanwidthtextSpanwidth PADDINGSELECT px inputDivwidthmainwidth dropSpanparentwidth BORDERWIDTH px var placeHolder function var textBox id searchInput jdocumentonblur textBox function placeTextjthis SEARCHTEXT jdocumentonfocus textBox function clrTextjthis SEARCHTEXT jdocumentoninput textBox function placeTextjthis SEARCHTEXT clrTextjthis SEARCHTEXT true placeTextjtextBox SEARCHTEXT var placeText function base txt if jtrimbaseval basevaltxt baseaddClassplcfont else if jtrimbaseval txt baseremoveClassplcfont var clrText function base txt isAddStyle if jtrimbaseval txt baseval baseremoveClassplcfont initEvent return init init jQuery jQueryfunctionj var idsearchmenu9 mainjid searchInput mainfindsearchInput option mainfindselectitsearchOptions PCMdropDowninitid main searchInput option PCMtypeAheadinitmain searchInput ajaxCalltypeahead option category h3 classfirstMatching Keywordsh3 ul classfirstlvl suggestions lia hrefsrchincludeImagetrueqkeywordssrcboxspan classtxtkeywordspanspan classcountcountspana firstSection ul classsecondlvl items lia hrefsrchincludeImagetrueqkeywordstnnamessrcbox datakeywordkeywordin nameali items ul firstSection li suggestions ul category brand h3Matching Brandsh3 ul classsecondlvl items lia hrefsrchincludeImagetrueqkeywordmannamessrcbox datakeywordkeywordby nameali items ul brand product h3Suggestions for keywordh3 ul classsuggest items li a hrefpedp titlename datakeywordedp span classtbl span classtr span classtd colimgimg srcimagePathimagePathimagePathimagePathmallwidgettiimagessharednoImageMedjpgimagePath esrcmallwidgettiimagessharednoImageMedjpg width67span span classtd coldesc span classoffermanufacturerspan span classprodtitlenamespan span span span a li items ul product Menu WELCOME TO PCM Thank You Thank you for subscribing to our newsletter Be sure to check your email for exclusive offers and discounts jQuerydocumentreadyfunction PCMsubscribeEmailValidateinitformNewsLetterEle emailsubscribe allowPageReload false 18007001000 functionc h a t i d c c function cq cq pusharguments cl 1 new Date i hcreateElementa d hgetElementsByTagNamea0 iasync 1 isrc t dparentNodeinsertBeforei d window document script httpschatidcdncomembedpcmlatestjs CID Follow PCM Blog Spiceworks Facebook LinkedIn Twitter YouTube jQuerydocumentreadyfunction var pcmtooltipopts ifuseContentID useContentID followussocial pcmtooltipoptscustomContentID followussocial else ifuseContentID customContent pcmtooltipoptscustomContent if pcmtooltipoptsisThemeHeader true pcmtooltipoptsheaderTitle pcmtooltipoptsheaderBg 1b5d9e pcmtooltipoptsheaderColor 000 if1px 0 1px 0px pcmtooltipoptstooltipBorderSize 1px pcmtooltipoptstooltipBorderColor e6e6e6 if pcmtooltipoptswidth if25px pcmtooltipoptscustomArrowPos 25px ifbottom auto pcmtooltipoptstooltipShowDirection bottom iffff pcmtooltipoptscontentBGcolor fff if10px pcmtooltipoptscontentPadding 10px if4 pcmtooltipoptsdistanceFromBaseElement 4 if800 pcmtooltipoptszIndex 800 pcmtooltipoptseventsArray clicksplit jQueryfollowlinkpcmtooltippcmtooltipopts jQuerydocumentreadyfunction var pcmtooltipopts ifuseHref useContentID pcmtooltipoptscustomContentID else ifuseHref customContent pcmtooltipoptscustomContent if pcmtooltipoptsisThemeHeader true pcmtooltipoptsheaderTitle pcmtooltipoptsheaderBg 1b5d9e pcmtooltipoptsheaderColor 000 if1px 0 1px 0px pcmtooltipoptstooltipBorderSize 1px pcmtooltipoptstooltipBorderColor e6e6e6 if pcmtooltipoptswidth if19px pcmtooltipoptscustomArrowPos 19px ifbottom auto pcmtooltipoptstooltipShowDirection bottom iffff pcmtooltipoptscontentBGcolor fff if0 pcmtooltipoptscontentPadding 0 if4 pcmtooltipoptsdistanceFromBaseElement 4 if800 pcmtooltipoptszIndex 800 pcmtooltipoptseventsArray clicksplit jQuerysslinkdropdttipdwnpcmtooltippcmtooltipopts Sign in Order Status Sign In New account Register jQueryfunction PCMtooltipDowninitsigninbtn21 Cart var PCM PCM PCMcartfunction function update ajax urlhomeopmallwebmisccartLinkcartLink typePOST dataTypejson datafalse successcount function countdata iftypeof data undefined databindcartcounttextdatacount return updateupdate jQuery PCMcartupdate PCM Home STARTUPS ENTREPRENEURSMEDIUM LARGE BUSINESSENTERPRISEHEALTHCARE GOVERNMENT Home FEDERALSTATE LOCALEDUCATIONHEALTHCARE EPROCUREMENT PCM BUSINESS DIRECTPCM OPSTRACK jQueryfunction PCMchangeHomepageinit var lastClickedTab lastclickedtab var active getCookielastClickedTab var widgetdrkmmenu13 greetwidgetfindgreetingstxt ifmsc515msc497msc428msc429msc426msc427mschomemsc430msc425indexOfmschome 1 active mschome var txtwidgetfindnavpointid active iftxtlength var greetings txtattrgreetings ifgreetings greettextgreetings txtaddClassactv else widgetfindanavpointidfirstaddClassactv greetshow var host windowlocationhost var links widgetfindanavpointid linksclickfunctione var navId thisattrnavpointid hrefthisattrhref ifnavId href hrefcharAt0 hosthrefsplit2 documentcookie lastClickedTab navId expires setExpirationDate30 path var setExpirationDate functiondays var date new Date datesetTimedategetTimedays2460601000 return datetoUTCString var getCookie functionname var nameEQ name var ca documentcookiesplit forvar i0i calengthi var c jQuerytrimcai if cindexOfnameEQ 0 return csubstringnameEQlengthclength return null Solutions Services Cloud Products Cloud Partners Shop Now PCM Hybrid Cloud Learn More Featured Deal of the Week Top Searches Ultrabook Finder Memory Finder InkToner Finder Hardware Accessories Cables Computers Memory Monitors Projectors Networking Printers Supplies Racks Power Cooling Scanners Servers Storage All Categories Software Backup Business Database Desktop Web Publishing Management Operating Systems Security Unified Collaboration Virtualization All Categories Brands Apple Cisco Dell Google HPI HPE Intel Lenovo Microsoft Samsung Symantec VMware All Brands jQueryfunction PCMmainNavinit var contstaticlinksconmenunav contshow menunav staticlinksconeachfunctionit var h0 tfindsubgroupnameeachfunctionis hMathmaxhsheight eachfunctionis sheighth conthide All Products Mfg Part Number PCM Part Number PCMdropDown functionj var init functionid main inputBar elem var dropDownDiv var textSpan var dropSpan var inputDiv var searchNow mainfindsearchInputBtn var SEARCHTEXT Search Products var PADDINGSELECT 30 var BORDERWIDTH 1 var initEvent function placeHolder elemselectBoxIt elemchangefunction adjustSearchBox searchNowclickfunction checkInputBox return false inputBarkeypressfunctione ifewhich 13 checkInputBox return false adjustSearchBox var checkInputBox function var val jtriminputBarvalreplaceg ifvallength 0 val SEARCHTEXT alertPlease enter a search keyword PCMmodalBx width 350modalopenModalerrorsearch else var typeelem val encodeURIComponentval q typevalreplace0g val url typeattrhref val q q windowlocation urljoin var adjustSearchBox function textSpan mainfindselectboxittext dropSpan mainfindselectboxit inputDiv mainfindhmsrchinpt dropSpanwidthtextSpanwidth PADDINGSELECT px inputDivwidthmainwidth dropSpanparentwidth BORDERWIDTH px var placeHolder function var textBox id searchInput jdocumentonblur textBox function placeTextjthis SEARCHTEXT jdocumentonfocus textBox function clrTextjthis SEARCHTEXT jdocumentoninput textBox function placeTextjthis SEARCHTEXT clrTextjthis SEARCHTEXT true placeTextjtextBox SEARCHTEXT var placeText function base txt if jtrimbaseval basevaltxt baseaddClassplcfont else if jtrimbaseval txt baseremoveClassplcfont var clrText function base txt isAddStyle if jtrimbaseval txt baseval baseremoveClassplcfont initEvent return init init jQuery jQueryfunctionj var idsearchmenu9 mainjid searchInput mainfindsearchInput option mainfindselectitsearchOptions PCMdropDowninitid main searchInput option PCMtypeAheadinitmain searchInput ajaxCalltypeahead option category h3 classfirstMatching Keywordsh3 ul classfirstlvl suggestions lia hrefsrchincludeImagetrueqkeywordssrcboxspan classtxtkeywordspanspan classcountcountspana firstSection ul classsecondlvl items lia hrefsrchincludeImagetrueqkeywordstnnamessrcbox datakeywordkeywordin nameali items ul firstSection li suggestions ul category brand h3Matching Brandsh3 ul classsecondlvl items lia hrefsrchincludeImagetrueqkeywordmannamessrcbox datakeywordkeywordby nameali items ul brand product h3Suggestions for keywordh3 ul classsuggest items li a hrefpedp titlename datakeywordedp span classtbl span classtr span classtd colimgimg srcimagePathimagePathimagePathimagePathmallwidgettiimagessharednoImageMedjpgimagePath esrcmallwidgettiimagessharednoImageMedjpg width67span span classtd coldesc span classoffermanufacturerspan span classprodtitlenamespan span span span a li items ul product Menu WELCOME TO PCM Thank You Thank you for subscribing to our newsletter Be sure to check your email for exclusive offers and discounts jQuerydocumentreadyfunction PCMsubscribeEmailValidateinitformNewsLetterEle emailsubscribe allowPageReload false 18007001000 functionc h a t i d c c function cq cq pusharguments cl 1 new Date i hcreateElementa d hgetElementsByTagNamea0 iasync 1 isrc t dparentNodeinsertBeforei d window document script httpschatidcdncomembedpcmlatestjs CID Follow PCM Blog Spiceworks Facebook LinkedIn Twitter YouTube jQuerydocumentreadyfunction var pcmtooltipopts ifuseContentID useContentID followussocial pcmtooltipoptscustomContentID followussocial else ifuseContentID customContent pcmtooltipoptscustomContent if pcmtooltipoptsisThemeHeader true pcmtooltipoptsheaderTitle pcmtooltipoptsheaderBg 1b5d9e pcmtooltipoptsheaderColor 000 if1px 0 1px 0px pcmtooltipoptstooltipBorderSize 1px pcmtooltipoptstooltipBorderColor e6e6e6 if pcmtooltipoptswidth if25px pcmtooltipoptscustomArrowPos 25px ifbottom auto pcmtooltipoptstooltipShowDirection bottom iffff pcmtooltipoptscontentBGcolor fff if10px pcmtooltipoptscontentPadding 10px if4 pcmtooltipoptsdistanceFromBaseElement 4 if800 pcmtooltipoptszIndex 800 pcmtooltipoptseventsArray clicksplit jQueryfollowlinkpcmtooltippcmtooltipopts jQuerydocumentreadyfunction var pcmtooltipopts ifuseHref useContentID pcmtooltipoptscustomContentID else ifuseHref customContent pcmtooltipoptscustomContent if pcmtooltipoptsisThemeHeader true pcmtooltipoptsheaderTitle pcmtooltipoptsheaderBg 1b5d9e pcmtooltipoptsheaderColor 000 if1px 0 1px 0px pcmtooltipoptstooltipBorderSize 1px pcmtooltipoptstooltipBorderColor e6e6e6 if pcmtooltipoptswidth if19px pcmtooltipoptscustomArrowPos 19px ifbottom auto pcmtooltipoptstooltipShowDirection bottom iffff pcmtooltipoptscontentBGcolor fff if0 pcmtooltipoptscontentPadding 0 if4 pcmtooltipoptsdistanceFromBaseElement 4 if800 pcmtooltipoptszIndex 800 pcmtooltipoptseventsArray clicksplit jQuerysslinkdropdttipdwnpcmtooltippcmtooltipopts Sign in Order Status Sign In New account Register jQueryfunction PCMtooltipDowninitsigninbtn21 Cart var PCM PCM PCMcartfunction function update ajax urlhomeopmallwebmisccartLinkcartLink typePOST dataTypejson datafalse successcount function countdata iftypeof data undefined databindcartcounttextdatacount return updateupdate jQuery PCMcartupdate PCM Home STARTUPS ENTREPRENEURSMEDIUM LARGE BUSINESSENTERPRISEHEALTHCARE GOVERNMENT Home FEDERALSTATE LOCALEDUCATIONHEALTHCARE EPROCUREMENT PCM BUSINESS DIRECTPCM OPSTRACK jQueryfunction PCMchangeHomepageinit var lastClickedTab lastclickedtab var active getCookielastClickedTab var widgetdrkmmenu13 greetwidgetfindgreetingstxt ifmsc515msc497msc428msc429msc426msc427mschomemsc430msc425indexOfmschome 1 active mschome var txtwidgetfindnavpointid active iftxtlength var greetings txtattrgreetings ifgreetings greettextgreetings txtaddClassactv else widgetfindanavpointidfirstaddClassactv greetshow var host windowlocationhost var links widgetfindanavpointid linksclickfunctione var navId thisattrnavpointid hrefthisattrhref ifnavId href hrefcharAt0 hosthrefsplit2 documentcookie lastClickedTab navId expires setExpirationDate30 path var setExpirationDate functiondays var date new Date datesetTimedategetTimedays2460601000 return datetoUTCString var getCookie functionname var nameEQ name var ca documentcookiesplit forvar i0i calengthi var c jQuerytrimcai if cindexOfnameEQ 0 return csubstringnameEQlengthclength return null Thank You Thank you for subscribing to our newsletter Be sure to check your email for exclusive offers and discounts jQuerydocumentreadyfunction PCMsubscribeEmailValidateinitformNewsLetterEle emailsubscribe allowPageReload false 18007001000 functionc h a t i d c c function cq cq pusharguments cl 1 new Date i hcreateElementa d hgetElementsByTagNamea0 iasync 1 isrc t dparentNodeinsertBeforei d window document script httpschatidcdncomembedpcmlatestjs CID Follow PCM Blog Spiceworks Facebook LinkedIn Twitter YouTube jQuerydocumentreadyfunction var pcmtooltipopts ifuseContentID useContentID followussocial pcmtooltipoptscustomContentID followussocial else ifuseContentID customContent pcmtooltipoptscustomContent if pcmtooltipoptsisThemeHeader true pcmtooltipoptsheaderTitle pcmtooltipoptsheaderBg 1b5d9e pcmtooltipoptsheaderColor 000 if1px 0 1px 0px pcmtooltipoptstooltipBorderSize 1px pcmtooltipoptstooltipBorderColor e6e6e6 if pcmtooltipoptswidth if25px pcmtooltipoptscustomArrowPos 25px ifbottom auto pcmtooltipoptstooltipShowDirection bottom iffff pcmtooltipoptscontentBGcolor fff if10px pcmtooltipoptscontentPadding 10px if4 pcmtooltipoptsdistanceFromBaseElement 4 if800 pcmtooltipoptszIndex 800 pcmtooltipoptseventsArray clicksplit jQueryfollowlinkpcmtooltippcmtooltipopts jQuerydocumentreadyfunction var pcmtooltipopts ifuseHref useContentID pcmtooltipoptscustomContentID else ifuseHref customContent pcmtooltipoptscustomContent if pcmtooltipoptsisThemeHeader true pcmtooltipoptsheaderTitle pcmtooltipoptsheaderBg 1b5d9e pcmtooltipoptsheaderColor 000 if1px 0 1px 0px pcmtooltipoptstooltipBorderSize 1px pcmtooltipoptstooltipBorderColor e6e6e6 if pcmtooltipoptswidth if19px pcmtooltipoptscustomArrowPos 19px ifbottom auto pcmtooltipoptstooltipShowDirection bottom iffff pcmtooltipoptscontentBGcolor fff if0 pcmtooltipoptscontentPadding 0 if4 pcmtooltipoptsdistanceFromBaseElement 4 if800 pcmtooltipoptszIndex 800 pcmtooltipoptseventsArray clicksplit jQuerysslinkdropdttipdwnpcmtooltippcmtooltipopts Sign in Order Status Sign In New account Register jQueryfunction PCMtooltipDowninitsigninbtn21 Cart var PCM PCM PCMcartfunction function update ajax urlhomeopmallwebmisccartLinkcartLink typePOST dataTypejson datafalse successcount function countdata iftypeof data undefined databindcartcounttextdatacount return updateupdate jQuery PCMcartupdate Thank You Thank you for subscribing to our newsletter Be sure to check your email for exclusive offers and discounts jQuerydocumentreadyfunction PCMsubscribeEmailValidateinitformNewsLetterEle emailsubscribe allowPageReload false 18007001000 functionc h a t i d c c function cq cq pusharguments cl 1 new Date i hcreateElementa d hgetElementsByTagNamea0 iasync 1 isrc t dparentNodeinsertBeforei d window document script httpschatidcdncomembedpcmlatestjs CID Follow PCM Blog Spiceworks Facebook LinkedIn Twitter YouTube jQuerydocumentreadyfunction var pcmtooltipopts ifuseContentID useContentID followussocial pcmtooltipoptscustomContentID followussocial else ifuseContentID customContent pcmtooltipoptscustomContent if pcmtooltipoptsisThemeHeader true pcmtooltipoptsheaderTitle pcmtooltipoptsheaderBg 1b5d9e pcmtooltipoptsheaderColor 000 if1px 0 1px 0px pcmtooltipoptstooltipBorderSize 1px pcmtooltipoptstooltipBorderColor e6e6e6 if pcmtooltipoptswidth if25px pcmtooltipoptscustomArrowPos 25px ifbottom auto pcmtooltipoptstooltipShowDirection bottom iffff pcmtooltipoptscontentBGcolor fff if10px pcmtooltipoptscontentPadding 10px if4 pcmtooltipoptsdistanceFromBaseElement 4 if800 pcmtooltipoptszIndex 800 pcmtooltipoptseventsArray clicksplit jQueryfollowlinkpcmtooltippcmtooltipopts Follow PCM Blog Spiceworks Facebook LinkedIn Twitter YouTube jQuerydocumentreadyfunction var pcmtooltipopts ifuseContentID useContentID followussocial pcmtooltipoptscustomContentID followussocial else ifuseContentID customContent pcmtooltipoptscustomContent if pcmtooltipoptsisThemeHeader true pcmtooltipoptsheaderTitle pcmtooltipoptsheaderBg 1b5d9e pcmtooltipoptsheaderColor 000 if1px 0 1px 0px pcmtooltipoptstooltipBorderSize 1px pcmtooltipoptstooltipBorderColor e6e6e6 if pcmtooltipoptswidth if25px pcmtooltipoptscustomArrowPos 25px ifbottom auto pcmtooltipoptstooltipShowDirection bottom iffff pcmtooltipoptscontentBGcolor fff if10px pcmtooltipoptscontentPadding 10px if4 pcmtooltipoptsdistanceFromBaseElement 4 if800 pcmtooltipoptszIndex 800 pcmtooltipoptseventsArray clicksplit jQueryfollowlinkpcmtooltippcmtooltipopts jQuerydocumentreadyfunction var pcmtooltipopts ifuseHref useContentID pcmtooltipoptscustomContentID else ifuseHref customContent pcmtooltipoptscustomContent if pcmtooltipoptsisThemeHeader true pcmtooltipoptsheaderTitle pcmtooltipoptsheaderBg 1b5d9e pcmtooltipoptsheaderColor 000 if1px 0 1px 0px pcmtooltipoptstooltipBorderSize 1px pcmtooltipoptstooltipBorderColor e6e6e6 if pcmtooltipoptswidth if19px pcmtooltipoptscustomArrowPos 19px ifbottom auto pcmtooltipoptstooltipShowDirection bottom iffff pcmtooltipoptscontentBGcolor fff if0 pcmtooltipoptscontentPadding 0 if4 pcmtooltipoptsdistanceFromBaseElement 4 if800 pcmtooltipoptszIndex 800 pcmtooltipoptseventsArray clicksplit jQuerysslinkdropdttipdwnpcmtooltippcmtooltipopts Sign in Order Status Sign In New account Register jQueryfunction PCMtooltipDowninitsigninbtn21 Cart var PCM PCM PCMcartfunction function update ajax urlhomeopmallwebmisccartLinkcartLink typePOST dataTypejson datafalse successcount function countdata iftypeof data undefined databindcartcounttextdatacount return updateupdate jQuery PCMcartupdate Solutions Services Cloud Products Cloud Partners Shop Now PCM Hybrid Cloud Learn More Featured Deal of the Week Top Searches Ultrabook Finder Memory Finder InkToner Finder Hardware Accessories Cables Computers Memory Monitors Projectors Networking Printers Supplies Racks Power Cooling Scanners Servers Storage All Categories Software Backup Business Database Desktop Web Publishing Management Operating Systems Security Unified Collaboration Virtualization All Categories Brands Apple Cisco Dell Google HPI HPE Intel Lenovo Microsoft Samsung Symantec VMware All Brands jQueryfunction PCMmainNavinit var contstaticlinksconmenunav contshow menunav staticlinksconeachfunctionit var h0 tfindsubgroupnameeachfunctionis hMathmaxhsheight eachfunctionis sheighth conthide All Products Mfg Part Number PCM Part Number PCMdropDown functionj var init functionid main inputBar elem var dropDownDiv var textSpan var dropSpan var inputDiv var searchNow mainfindsearchInputBtn var SEARCHTEXT Search Products var PADDINGSELECT 30 var BORDERWIDTH 1 var initEvent function placeHolder elemselectBoxIt elemchangefunction adjustSearchBox searchNowclickfunction checkInputBox return false inputBarkeypressfunctione ifewhich 13 checkInputBox return false adjustSearchBox var checkInputBox function var val jtriminputBarvalreplaceg ifvallength 0 val SEARCHTEXT alertPlease enter a search keyword PCMmodalBx width 350modalopenModalerrorsearch else var typeelem val encodeURIComponentval q typevalreplace0g val url typeattrhref val q q windowlocation urljoin var adjustSearchBox function textSpan mainfindselectboxittext dropSpan mainfindselectboxit inputDiv mainfindhmsrchinpt dropSpanwidthtextSpanwidth PADDINGSELECT px inputDivwidthmainwidth dropSpanparentwidth BORDERWIDTH px var placeHolder function var textBox id searchInput jdocumentonblur textBox function placeTextjthis SEARCHTEXT jdocumentonfocus textBox function clrTextjthis SEARCHTEXT jdocumentoninput textBox function placeTextjthis SEARCHTEXT clrTextjthis SEARCHTEXT true placeTextjtextBox SEARCHTEXT var placeText function base txt if jtrimbaseval basevaltxt baseaddClassplcfont else if jtrimbaseval txt baseremoveClassplcfont var clrText function base txt isAddStyle if jtrimbaseval txt baseval baseremoveClassplcfont initEvent return init init jQuery jQueryfunctionj var idsearchmenu9 mainjid searchInput mainfindsearchInput option mainfindselectitsearchOptions PCMdropDowninitid main searchInput option PCMtypeAheadinitmain searchInput ajaxCalltypeahead option category h3 classfirstMatching Keywordsh3 ul classfirstlvl suggestions lia hrefsrchincludeImagetrueqkeywordssrcboxspan classtxtkeywordspanspan classcountcountspana firstSection ul classsecondlvl items lia hrefsrchincludeImagetrueqkeywordstnnamessrcbox datakeywordkeywordin nameali items ul firstSection li suggestions ul category brand h3Matching Brandsh3 ul classsecondlvl items lia hrefsrchincludeImagetrueqkeywordmannamessrcbox datakeywordkeywordby nameali items ul brand product h3Suggestions for keywordh3 ul classsuggest items li a hrefpedp titlename datakeywordedp span classtbl span classtr span classtd colimgimg srcimagePathimagePathimagePathimagePathmallwidgettiimagessharednoImageMedjpgimagePath esrcmallwidgettiimagessharednoImageMedjpg width67span span classtd coldesc span classoffermanufacturerspan span classprodtitlenamespan span span span a li items ul product Solutions Services Solutions Services Cloud Products Cloud Partners Shop Now PCM Hybrid Cloud Learn More Featured Deal of the Week Top Searches Ultrabook Finder Memory Finder InkToner Finder Hardware Accessories Cables Computers Memory Monitors Projectors Networking Printers Supplies Racks Power Cooling Scanners Servers Storage All Categories Software Backup Business Database Desktop Web Publishing Management Operating Systems Security Unified Collaboration Virtualization All Categories Brands Apple Cisco Dell Google HPI HPE Intel Lenovo Microsoft Samsung Symantec VMware All Brands jQueryfunction PCMmainNavinit var contstaticlinksconmenunav contshow menunav staticlinksconeachfunctionit var h0 tfindsubgroupnameeachfunctionis hMathmaxhsheight eachfunctionis sheighth conthide All Products Mfg Part Number PCM Part Number PCMdropDown functionj var init functionid main inputBar elem var dropDownDiv var textSpan var dropSpan var inputDiv var searchNow mainfindsearchInputBtn var SEARCHTEXT Search Products var PADDINGSELECT 30 var BORDERWIDTH 1 var initEvent function placeHolder elemselectBoxIt elemchangefunction adjustSearchBox searchNowclickfunction checkInputBox return false inputBarkeypressfunctione ifewhich 13 checkInputBox return false adjustSearchBox var checkInputBox function var val jtriminputBarvalreplaceg ifvallength 0 val SEARCHTEXT alertPlease enter a search keyword PCMmodalBx width 350modalopenModalerrorsearch else var typeelem val encodeURIComponentval q typevalreplace0g val url typeattrhref val q q windowlocation urljoin var adjustSearchBox function textSpan mainfindselectboxittext dropSpan mainfindselectboxit inputDiv mainfindhmsrchinpt dropSpanwidthtextSpanwidth PADDINGSELECT px inputDivwidthmainwidth dropSpanparentwidth BORDERWIDTH px var placeHolder function var textBox id searchInput jdocumentonblur textBox function placeTextjthis SEARCHTEXT jdocumentonfocus textBox function clrTextjthis SEARCHTEXT jdocumentoninput textBox function placeTextjthis SEARCHTEXT clrTextjthis SEARCHTEXT true placeTextjtextBox SEARCHTEXT var placeText function base txt if jtrimbaseval basevaltxt baseaddClassplcfont else if jtrimbaseval txt baseremoveClassplcfont var clrText function base txt isAddStyle if jtrimbaseval txt baseval baseremoveClassplcfont initEvent return init init jQuery jQueryfunctionj var idsearchmenu9 mainjid searchInput mainfindsearchInput option mainfindselectitsearchOptions PCMdropDowninitid main searchInput option PCMtypeAheadinitmain searchInput ajaxCalltypeahead option category h3 classfirstMatching Keywordsh3 ul classfirstlvl suggestions lia hrefsrchincludeImagetrueqkeywordssrcboxspan classtxtkeywordspanspan classcountcountspana firstSection ul classsecondlvl items lia hrefsrchincludeImagetrueqkeywordstnnamessrcbox datakeywordkeywordin nameali items ul firstSection li suggestions ul category brand h3Matching Brandsh3 ul classsecondlvl items lia hrefsrchincludeImagetrueqkeywordmannamessrcbox datakeywordkeywordby nameali items ul brand product h3Suggestions for keywordh3 ul classsuggest items li a hrefpedp titlename datakeywordedp span classtbl span classtr span classtd colimgimg srcimagePathimagePathimagePathimagePathmallwidgettiimagessharednoImageMedjpgimagePath esrcmallwidgettiimagessharednoImageMedjpg width67span span classtd coldesc span classoffermanufacturerspan span classprodtitlenamespan span span span a li items ul product documentgetElementsByName functionname return jQueryname name documentgetElementsByName functionname return jQueryname name documentgetElementsByName functionname return jQueryname name jQueryfunction PCMslideBannerinitsldrwidget10 home1453659360039opmallwebmisclayeredSliderlayeredSliderbannersmschome10banners Picking the Right Printer for your Office INFOGRAPHIC January 19 2016 Microsoft Announces Major Change to the Enterprise Agreement Program January 6 2016 How Christmas Gifts Could Impact BYOD January 4 2016 Enhance Your Creativity with Adobe Stock December 30 2015 HP Print Security Seminars Is Your Network at Risk to Hackers December 22 2015 Share Costs and Save Time with Hewlett Packard Enterprise Healthcare December 21 2015 Microsoft Announces that Windows Server 2016 will be Launching Next Quarter December 11 2015 Last Chance to Register for Vision Hollywood December 10 2015 How Big of a Deal is the AppleCisco Partnership December 9 2015 Webcast ShoreTel Truly Unified Communications December 8 2015 Ergotron StyleView Fit for Every Body December 7 2015 The Digital Pulse of Tomorrow’s Healthcare with Lenovo December 7 2015 jQueryfunction PCMnewsFeedinit var t8pcmnws trunk8lit8closestli licssdisplayblock t8trunk8removeClasstrunk8 licssdisplay Reapply title to support html tags var rcNws jQueryhmnwsfindrcnws var title jQueryhmnwsfindtitleTempHolderval rcNwshtmltitle jQueryhmnwsfindtitleTempHolderremove Deal of the Week HP 14 G3 QuadCore ChromebookOnly 17999 Shop Now Lenovo B4080 80F6 Notebook Reach a New Height inBusiness ComputingOnly 34999 Shop Now Managed Print Services Save Millions Gain Visibility Take Control Shop Now Featured Products Bestsellers New Arrivals Trending div classprdtblcon rctb hideavail div classtr products div classtblcll itemlist first last dataskudpno if secret sale div classicnviosspdiv lowestPrice div classicnviogbpdiv lowestPrice div classitem first last div classitmimg img classimgload srcwidgetsproductviewimgloadgif notAvailablea classprodimage hreflink titlenameimg classproimage srcimgSrc esrcwidgetsproductviewimgnoImage150jpganotAvailable notAvailableimg classproimage srcmallwidgettiimagessharednotAvailable150jpg esrcwidgetsproductviewimgnoImage150jpgnotAvailable div savePrice div classitemcll npsvediv savePrice savePrice div classitmsve spanSavespan span classsvprcsavePricespansavePercent span classnrmspanspan classsvprcnt nrmsavePercentspanspan classnrmspansavePercent div savePrice div classitmttl prodname h2 notAvailablea hreflink titlenamenameanotAvailable notAvailablespan classprodNameProduct is No Longer AvailablespannotAvailable h2 div div classitmeval prodavail notAvailable div classavlb span classavlbsAvailabilityspan span classstatavlbavailabilityspan div rateValue div classistr div classstr stylewidth ratediv div div classrater a hreflinkpdppdpUserReview titleRatings rateValuea div rateValue rateValue div classnstr ratera hrefhttpswwwpcmcomoWriteAReviewmsc66opmallwebzonespdpRecentReviewswriteReviewampdpnodpno titleBe the first to write a reviewBe the first to write a reviewadiv rateValue notAvailable div div classitmprc div classpprcd if secretsale div classrprice upp ssp span classntceSecret Sale Pricespan div else div classprc lprc plistPricep div div classprc tprc p classprodpricetotalPricep div div classclrdiv end div enableCartBtn div classcrtbtn lowestPrice div classcrt upp a dataactionButtonSee Lowest Price datalabelproddpno hreflink classga titleSee Lowest PriceSee Lowest Pricea div lowestPrice callPrice div classcrt upp a hreflink classupplinks ga titleCall For PriceCall For Pricea div callPrice addCart div classqty div classbldiv input typetext idaddCartQtydpno value1 maxlength3 div classbrdiv div classclrdiv div div classcrt a hrefsectioncategoryampskudpno classmbxlinks metadatametadata titleAdd to CartAdd to Carta div addCart div classclrdiv div enableCartBtn div div div products div div div classpge div classnum span classcrntstartIndexspanspanspanspan classlmtpgendIndexspanspan spanofspanspan classttltotalRecordsspan div div classarw a href classlft left datapagepreviousPagediv classaim leftdiv a a href classrht right datapagenextPagediv classaim rightdiva div classclrdiv div div classclrdiv div div classcnt bhenabled h4You have no recently viewed items to displayh4 pCant find what youre searching for Try one of these categoriesp ul linkslia titlelabel hreflinknewTab targetblanknewTablabelalilinks ul div div classcnt bhdisabled h4Your browsing history is disabled a classonbrowtrigger enablebrowsing hrefenable urlajaxCallrecentlyviewedEnable browsing historyah4 pKeep track of what youve viewed by turning on your browsing history See items youve viewed searches youve conducted and products youve visitedp div jQueryfunction var id prodviewtb36 PCMproductViewinitid PCMgridRotateinitidwidth id itemlist test Preferred Partners jQueryfunction PCMslideBannerinitsldrwidget10 home1453659360039opmallwebmisclayeredSliderlayeredSliderbannersmschome10banners Picking the Right Printer for your Office INFOGRAPHIC January 19 2016 Microsoft Announces Major Change to the Enterprise Agreement Program January 6 2016 How Christmas Gifts Could Impact BYOD January 4 2016 Enhance Your Creativity with Adobe Stock December 30 2015 HP Print Security Seminars Is Your Network at Risk to Hackers December 22 2015 Share Costs and Save Time with Hewlett Packard Enterprise Healthcare December 21 2015 Microsoft Announces that Windows Server 2016 will be Launching Next Quarter December 11 2015 Last Chance to Register for Vision Hollywood December 10 2015 How Big of a Deal is the AppleCisco Partnership December 9 2015 Webcast ShoreTel Truly Unified Communications December 8 2015 Ergotron StyleView Fit for Every Body December 7 2015 The Digital Pulse of Tomorrow’s Healthcare with Lenovo December 7 2015 jQueryfunction PCMnewsFeedinit var t8pcmnws trunk8lit8closestli licssdisplayblock t8trunk8removeClasstrunk8 licssdisplay Reapply title to support html tags var rcNws jQueryhmnwsfindrcnws var title jQueryhmnwsfindtitleTempHolderval rcNwshtmltitle jQueryhmnwsfindtitleTempHolderremove Deal of the Week HP 14 G3 QuadCore ChromebookOnly 17999 Shop Now Lenovo B4080 80F6 Notebook Reach a New Height inBusiness ComputingOnly 34999 Shop Now Managed Print Services Save Millions Gain Visibility Take Control Shop Now Deal of the Week HP 14 G3 QuadCore ChromebookOnly 17999 Shop Now Lenovo B4080 80F6 Notebook Reach a New Height inBusiness ComputingOnly 34999 Shop Now Managed Print Services Save Millions Gain Visibility Take Control Shop Now Deal of the Week HP 14 G3 QuadCore ChromebookOnly 17999 Shop Now Deal of the Week HP 14 G3 QuadCore ChromebookOnly 17999 Shop Now Deal of the Week HP 14 G3 QuadCore ChromebookOnly 17999 Shop Now Deal of the Week HP 14 G3 QuadCore ChromebookOnly 17999 Shop Now Lenovo B4080 80F6 Notebook Reach a New Height inBusiness ComputingOnly 34999 Shop Now Lenovo B4080 80F6 Notebook Reach a New Height inBusiness ComputingOnly 34999 Shop Now Lenovo B4080 80F6 Notebook Reach a New Height inBusiness ComputingOnly 34999 Shop Now Lenovo B4080 80F6 Notebook Reach a New Height inBusiness ComputingOnly 34999 Shop Now Managed Print Services Save Millions Gain Visibility Take Control Shop Now Managed Print Services Save Millions Gain Visibility Take Control Shop Now Managed Print Services Save Millions Gain Visibility Take Control Shop Now Managed Print Services Save Millions Gain Visibility Take Control </v>
       </c>
       <c r="E7" t="str">
-        <v>,t){         var h=0;         $(t).find('.sub-group-name').each(function(i,s){             h=Math.max(h,$(s).height());         }).each(function(i,s){             $(s).height(h);         });     });     cont.hide(); });                            All Products     Mfg Part Number     PCM Part Number                                                      PCM.dropDown = (function($j) {  var init = function($id, $main, inputBar, elem) {   var dropDownDiv;   var textSpan;   var dropSpan;   var inputDiv;   var searchNow = $main.find('.searchInputBtn');      var SEARCH_TEXT = 'Search Products';   var PADDING_SELECT = 30;   var BORDER_WIDTH = 1;    var initEvent = function() {        placeHolder();    elem.selectBoxIt();    elem.change(function(){                 adjustSearchBox();             });    searchNow.click(function(){     checkInputBox();     return false;    });    inputBar.keypress(function(e){     if(e.which === 13){      checkInputBox();      return false;     }    });        adjustSearchBox();   };   var checkInputBox = function(){    var val = $j.trim(inputBar.val()).replace(/\\/g, "");             if(val.length === 0 || val === SEARCH_TEXT){                 alert('Please enter a search keyword');                 //PCM.modalBx('', {'width': 350}).modal().openModal('#error-search');             }else{                 var $type=elem,                 _val = encodeURIComponent(val),                 _q = $type.val().replace(/$0/g, _val),                 url = [$type.attr('href'), _val, _q?"&amp;":"", _q];                 window.location= url.join("");             }   };   var adjustSearchBox = function(){    textSpan = $main.find('.selectboxit-text');    dropSpan = $main.find('.selectboxit');    inputDiv = $main.find('.hm-srch-inpt');        dropSpan.width((textSpan.width() + PADDING_SELECT) + 'px');    inputDiv.width(($main.width() - dropSpan.parent().width() - BORDER_WIDTH ) + 'px');       };   var placeHolder = function(){        var textBox = $id + ' .searchInput';       $j(document).on('blur', textBox, function () {               placeText($j(this), SEARCH_TEXT);           });           $j(document).on('focus', textBox, function () {               clrText($j(this), SEARCH_TEXT);           });           $j(document).on('input', textBox, function () {               placeText($j(this), SEARCH_TEXT);               clrText($j(this), SEARCH_TEXT, true);           });            placeText($j(textBox), SEARCH_TEXT);   };    var placeText = function (base, txt) {           if ($j.trim(base.val()) === '') {               base.val(txt);               base.addClass('plcfont');                          } else if ($j.trim(base.val()) !== txt) {               base.removeClass('plcfont');           }        };       var clrText = function (base, txt, isAddStyle) {           if ($j.trim(base.val()) === txt) {               base.val('');               base.removeClass('plcfont');           }       };   initEvent();  };   return {   init : init  }; })(jQuery);        jQuery(function(j){     var $id='#search-menu-9', $main=j($id), $searchInput = $main.find('.searchInput'), $option = $main.find('[selectit="searchOptions"]');     PCM.dropDown.init($id, $main, $searchInput, $option);     PCM.typeAhead.init($main, $searchInput, "/ajaxCall/typeahead", $option); });   {{#category}} &lt;h3 class="first"&gt;Matching Keywords&lt;/h3&gt; &lt;ul class="first-lvl"&gt;  {{#suggestions}}     &lt;li&gt;&lt;a href="/s?rch&amp;includeImage=true&amp;q={{keyword}}&amp;ssrc=box"&gt;&lt;span class="txt"&gt;{{keyword}}&lt;/span&gt;&lt;span class="count"&gt;({{count}})&lt;/span&gt;&lt;/a&gt;         {{#firstSection}}         &lt;ul class="second-lvl"&gt;             {{#items}}             &lt;li&gt;&lt;a href="/s?rch&amp;includeImage=true&amp;q={{keyword}}&amp;stn={{name}}&amp;ssrc=box" data-keyword="{{keyword}}"&gt;in {{name}}&lt;/a&gt;&lt;/li&gt;             {{/items}}         &lt;/ul&gt;         {{/firstSection}}     &lt;/li&gt;     {{/suggestions}} &lt;/ul&gt; {{/category}} {{#brand}} &lt;h3&gt;Matching Brands&lt;/h3&gt; &lt;ul class="second-lvl"&gt;  {{#items}}  &lt;li&gt;&lt;a href="/s?rch&amp;includeImage=true&amp;q={{keyword}}&amp;man={{name}}&amp;ssrc=box" data-keyword="{{keyword}}"&gt;by {{name}}&lt;/a&gt;&lt;/li&gt;  {{/items}} &lt;/ul&gt; {{/brand}} {{#product}} &lt;h3&gt;Suggestions for {{keyword}}&lt;/h3&gt; &lt;ul class="suggest"&gt;  {{#items}}     &lt;li&gt;         &lt;a href="/p/{{edp}}" title="{{name}}" data-keyword="{{edp}}"&gt;             &lt;span class="tbl"&gt;                 &lt;span class="tr"&gt;                     &lt;span class="td col-img"&gt;&lt;img src="{{#imagePath}}{{imagePath}}{{/imagePath}}{{^imagePath}}/mall/widgetti/images/shared/noImageMed.jpg{{/imagePath}}" e_src="/mall/widgetti/images/shared/noImageMed.jpg" width="67"&gt;&lt;/span&gt;                     &lt;span class="td col-desc"&gt;                         &lt;span class="offer"&gt;{{manufacturer}}&lt;/span&gt;                         &lt;span class="prod-title"&gt;{{name}}&lt;/span&gt;                     &lt;/span&gt;                 &lt;/span&gt;             &lt;/span&gt;         &lt;/a&gt;     &lt;/li&gt;     {{/items}} &lt;/ul&gt; {{/product}}                                                              Menu                                            WELCOME TO PCM!                                                                                                                                                                                                                                     Thank You!                                                         Thank you for subscribing to our newsletter. Be sure to check your email for exclusive offers and discounts.                                   jQuery(document).ready(function() {      PCM.subscribeEmailValidate.init({formNewsLetterEle: '#email-subscribe',          allowPageReload : false});  });      1-800-700-1000    (function(c, h, a, t, _, i, d) {     c[_] = c[_] || function() {         (c[_].q = c[_].q || []).push(arguments)     }, c[_].l = 1 * new Date();     i = h.createElement(a), d = h.getElementsByTagName(a)[0];     i.async = 1;     i.src = t;     d.parentNode.insertBefore(i, d) })(window, document, 'script', 'https://chatidcdn.com/embed/pcm/latest.js', 'CID');            Follow     PCM Blog  Spiceworks  Facebook  LinkedIn  Twitter  YouTube            jQuery(document).ready(function(){  var pcm_tooltip_opts = {};   if('useContentID' == 'useContentID' &amp;&amp; '#follow-us-social' != ''){   pcm_tooltip_opts.customContentID = '#follow-us-social';  }else if('useContentID' == 'customContent' &amp;&amp; '' != ''){   pcm_tooltip_opts.customContent = ''  }   if('' != ''){   pcm_tooltip_opts.isThemeHeader = true;   pcm_tooltip_opts.headerTitle = '';   pcm_tooltip_opts.headerBg = '#1b5d9e';   pcm_tooltip_opts.headerColor = '#000';  }   if('1px' != '0' &amp;&amp; '1px' != '0px'){   pcm_tooltip_opts.tooltipBorderSize = '1px';   pcm_tooltip_opts.tooltipBorderColor = '#e6e6e6';  }    if('' != ''){ pcm_tooltip_opts.width = ''; }  if('25px' != ''){ pcm_tooltip_opts.customArrowPos = '25px'; }  if('bottom' != 'auto'){ pcm_tooltip_opts.tooltipShowDirection = 'bottom'; }  if('#fff' != ''){ pcm_tooltip_opts.contentBGcolor = '#fff'; }  if('10px' != ''){ pcm_tooltip_opts.contentPadding = '10px'; }  if('-4' != ''){ pcm_tooltip_opts.distanceFromBaseElement = '-4'; }  if('800' != ''){ pcm_tooltip_opts.zIndex = '800'; }    pcm_tooltip_opts.eventsArray = 'click'.split(',');    jQuery('#follow-link').pcm_tooltip(pcm_tooltip_opts); });            jQuery(document).ready(function(){  var pcm_tooltip_opts = {};   if('useHref' == 'useContentID' &amp;&amp; '' != ''){   pcm_tooltip_opts.customContentID = '';  }else if('useHref' == 'customContent' &amp;&amp; '' != ''){   pcm_tooltip_opts.customContent = ''  }   if('' != ''){   pcm_tooltip_opts.isThemeHeader = true;   pcm_tooltip_opts.headerTitle = '';   pcm_tooltip_opts.headerBg = '#1b5d9e';   pcm_tooltip_opts.headerColor = '#000';  }   if('1px' != '0' &amp;&amp; '1px' != '0px'){   pcm_tooltip_opts.tooltipBorderSize = '1px';   pcm_tooltip_opts.tooltipBorderColor = '#e6e6e6';  }    if('' != ''){ pcm_tooltip_opts.width = ''; }  if('19px' != ''){ pcm_tooltip_opts.customArrowPos = '19px'; }  if('bottom' != 'auto'){ pcm_tooltip_opts.tooltipShowDirection = 'bottom'; }  if('#fff' != ''){ pcm_tooltip_opts.contentBGcolor = '#fff'; }  if('0' != ''){ pcm_tooltip_opts.contentPadding = '0'; }  if('-4' != ''){ pcm_tooltip_opts.distanceFromBaseElement = '-4'; }  if('800' != ''){ pcm_tooltip_opts.zIndex = '800'; }    pcm_tooltip_opts.eventsArray = 'click'.split(',');    jQuery('.sslink.dropd.ttipdwn').pcm_tooltip(pcm_tooltip_opts); });       Sign in                                                     Order Status                                                Sign In                                   New account?  Register                                                     /* jQuery(function($){                 PCM.tooltipDown.init('#signin-btn-21');             }); */                     Cart ()   var PCM = PCM || {}; PCM.cart=(function($){     function update(){         $.ajax({             url:"/home?op=mall.web.misc.cartLink.cartLink",             type:'POST',             dataType:'json',             data:'false',             success:count         });     }     function count(data){         if(typeof data !== 'undefined'){             $('[data-bind="cart-count"]').text(data.count)         }     }     return {         update:update     }; })(jQuery); PCM.cart.update();                                                                                                                                                                    PCM (Home)                                              STARTUPS / ENTREPRENEURSMEDIUM / LARGE BUSINESSENTERPRISEHEALTHCARE                                                                                                                                              GOVERNMENT (Home)                                              FEDERALSTATE &amp; LOCALEDUCATIONHEALTHCARE                                                                                                                                              E-PROCUREMENT                                              PCM BUSINESS DIRECTPCM OPSTRACK                                                             jQuery(function($){     PCM.changeHomepage.init();     var lastClickedTab = 'last_clicked_tab';     var active = getCookie(lastClickedTab);     var widget=$("#drk-mmenu-13"), $greet=widget.find('.greetings-txt');     if('msc-515,msc-497,msc-428,msc-429,msc-426,msc-427,msc-home,msc-430,msc-425,'.indexOf('msc-home,') &gt; -1){   active = 'msc-home';  }     var txt=widget.find('[navpoint-id="' + active + '"]')     if(txt.length) {         var greetings = txt.attr('greetings');         if(greetings) {             $greet.text(greetings);         }         txt.addClass('actv');     }else{      widget.find('a[navpoint-id]').first().addClass('actv');     }     $greet.show();          var host = window.location.host;     var links= widget.find('a[navpoint-id]')     links.click(function(e){      var navId = $(this).attr('navpoint-id'), href=$(this).attr('href');      if(navId &amp;&amp; href &amp;&amp; (href.charAt(0)=='/' || host===href.split('/')[2])){       document.cookie = lastClickedTab + '=' + navId + '; expires=' + setExpirationDate(30) + '; path=/';      }     });     var setExpirationDate = function(days){      var date = new Date();         date.setTime(date.getTime()+(days*24*60*60*1000));         return date.toUTCString();     };      });  var getCookie = function(name){  var nameEQ = name + "=";     var ca = document.cookie.split(';');     for(var i=0;i &lt; ca.length;i++) {         var c = jQuery.trim(ca[i]);         if (c.indexOf(nameEQ) === 0) return c.substring(nameEQ.length,c.length);     }     return null; };                                        Solutions &amp; Services                Cloud    Products                                                                                               Cloud Partners                                             Shop Now                                                                                                        PCM Hybrid Cloud                                             Learn More                                                                                                                                                   Featured                                    Deal of the Week                  Top Searches                  Ultrabook Finder                  Memory Finder                  Ink/Toner Finder                                                                                               Hardware                                    Accessories                  Cables                  Computers                  Memory                  Monitors &amp; Projectors                  Networking                  Printers &amp; Supplies                  Racks, Power &amp; Cooling                  Scanners                  Servers                  Storage                                           All Categories                                                                              Software                                    Backup                  Business                  Database                  Desktop &amp; Web Publishing                  Management                  Operating Systems                  Security                  Unified Collaboration                  Virtualization                                           All Categories                                                                              Brands                                    Apple                  Cisco                  Dell                  Google                  HPI                  HPE                  Intel                  Lenovo                  Microsoft                  Samsung                  Symantec                  VMware                                           All Brands                                                       jQuery(function($){     PCM.mainNav.init();     var cont=$('.static-links-con,.menu-nav');     cont.show();     $('.menu-nav .static-links-con').each(function(i,t){         var h=0;         $(t).find('.sub-group-name').each(function(i,s){             h=Math.max(h,$(s).height());         }).each(function(i,s){             $(s).height(h);         });     });     cont.hide(); });                            All Products     Mfg Part Number     PCM Part Number                                                      PCM.dropDown = (function($j) {  var init = function($id, $main, inputBar, elem) {   var dropDownDiv;   var textSpan;   var dropSpan;   var inputDiv;   var searchNow = $main.find('.searchInputBtn');      var SEARCH_TEXT = 'Search Products';   var PADDING_SELECT = 30;   var BORDER_WIDTH = 1;    var initEvent = function() {        placeHolder();    elem.selectBoxIt();    elem.change(function(){                 adjustSearchBox();             });    searchNow.click(function(){     checkInputBox();     return false;    });    inputBar.keypress(function(e){     if(e.which === 13){      checkInputBox();      return false;     }    });        adjustSearchBox();   };   var checkInputBox = function(){    var val = $j.trim(inputBar.val()).replace(/\\/g, "");             if(val.length === 0 || val === SEARCH_TEXT){                 alert('Please enter a search keyword');                 //PCM.modalBx('', {'width': 350}).modal().openModal('#error-search');             }else{                 var $type=elem,                 _val = encodeURIComponent(val),                 _q = $type.val().replace(/$0/g, _val),                 url = [$type.attr('href'), _val, _q?"&amp;":"", _q];                 window.location= url.join("");             }   };   var adjustSearchBox = function(){    textSpan = $main.find('.selectboxit-text');    dropSpan = $main.find('.selectboxit');    inputDiv = $main.find('.hm-srch-inpt');        dropSpan.width((textSpan.width() + PADDING_SELECT) + 'px');    inputDiv.width(($main.width() - dropSpan.parent().width() - BORDER_WIDTH ) + 'px');       };   var placeHolder = function(){        var textBox = $id + ' .searchInput';       $j(document).on('blur', textBox, function () {               placeText($j(this), SEARCH_TEXT);           });           $j(document).on('focus', textBox, function () {               clrText($j(this), SEARCH_TEXT);           });           $j(document).on('input', textBox, function () {               placeText($j(this), SEARCH_TEXT);               clrText($j(this), SEARCH_TEXT, true);           });            placeText($j(textBox), SEARCH_TEXT);   };    var placeText = function (base, txt) {           if ($j.trim(base.val()) === '') {               base.val(txt);               base.addClass('plcfont');                          } else if ($j.trim(base.val()) !== txt) {               base.removeClass('plcfont');           }        };       var clrText = function (base, txt, isAddStyle) {           if ($j.trim(base.val()) === txt) {               base.val('');               base.removeClass('plcfont');           }       };   initEvent();  };   return {   init : init  }; })(jQuery);        jQuery(function(j){     var $id='#search-menu-9', $main=j($id), $searchInput = $main.find('.searchInput'), $option = $main.find('[selectit="searchOptions"]');     PCM.dropDown.init($id, $main, $searchInput, $option);     PCM.typeAhead.init($main, $searchInput, "/ajaxCall/typeahead", $option); });   {{#category}} &lt;h3 class="first"&gt;Matching Keywords&lt;/h3&gt; &lt;ul class="first-lvl"&gt;  {{#suggestions}}     &lt;li&gt;&lt;a href="/s?rch&amp;includeImage=true&amp;q={{keyword}}&amp;ssrc=box"&gt;&lt;span class="txt"&gt;{{keyword}}&lt;/span&gt;&lt;span class="count"&gt;({{count}})&lt;/span&gt;&lt;/a&gt;         {{#firstSection}}         &lt;ul class="second-lvl"&gt;             {{#items}}             &lt;li&gt;&lt;a href="/s?rch&amp;includeImage=true&amp;q={{keyword}}&amp;stn={{name}}&amp;ssrc=box" data-keyword="{{keyword}}"&gt;in {{name}}&lt;/a&gt;&lt;/li&gt;             {{/items}}         &lt;/ul&gt;         {{/firstSection}}     &lt;/li&gt;     {{/suggestions}} &lt;/ul&gt; {{/category}} {{#brand}} &lt;h3&gt;Matching Brands&lt;/h3&gt; &lt;ul class="second-lvl"&gt;  {{#items}}  &lt;li&gt;&lt;a href="/s?rch&amp;includeImage=true&amp;q={{keyword}}&amp;man={{name}}&amp;ssrc=box" data-keyword="{{keyword}}"&gt;by {{name}}&lt;/a&gt;&lt;/li&gt;  {{/items}} &lt;/ul&gt; {{/brand}} {{#product}} &lt;h3&gt;Suggestions for {{keyword}}&lt;/h3&gt; &lt;ul class="suggest"&gt;  {{#items}}     &lt;li&gt;         &lt;a href="/p/{{edp}}" title="{{name}}" data-keyword="{{edp}}"&gt;             &lt;span class="tbl"&gt;                 &lt;span class="tr"&gt;                     &lt;span class="td col-img"&gt;&lt;img src="{{#imagePath}}{{imagePath}}{{/imagePath}}{{^imagePath}}/mall/widgetti/images/shared/noImageMed.jpg{{/imagePath}}" e_src="/mall/widgetti/images/shared/noImageMed.jpg" width="67"&gt;&lt;/span&gt;                     &lt;span class="td col-desc"&gt;                         &lt;span class="offer"&gt;{{manufacturer}}&lt;/span&gt;                         &lt;span class="prod-title"&gt;{{name}}&lt;/span&gt;                     &lt;/span&gt;                 &lt;/span&gt;             &lt;/span&gt;         &lt;/a&gt;     &lt;/li&gt;     {{/items}} &lt;/ul&gt; {{/product}}                                                     Menu                                            WELCOME TO PCM!                                                                                                                                                                                                                                     Thank You!                                                         Thank you for subscribing to our newsletter. Be sure to check your email for exclusive offers and discounts.                                   jQuery(document).ready(function() {      PCM.subscribeEmailValidate.init({formNewsLetterEle: '#email-subscribe',          allowPageReload : false});  });      1-800-700-1000    (function(c, h, a, t, _, i, d) {     c[_] = c[_] || function() {         (c[_].q = c[_].q || []).push(arguments)     }, c[_].l = 1 * new Date();     i = h.createElement(a), d = h.getElementsByTagName(a)[0];     i.async = 1;     i.src = t;     d.parentNode.insertBefore(i, d) })(window, document, 'script', 'https://chatidcdn.com/embed/pcm/latest.js', 'CID');            Follow     PCM Blog  Spiceworks  Facebook  LinkedIn  Twitter  YouTube            jQuery(document).ready(function(){  var pcm_tooltip_opts = {};   if('useContentID' == 'useContentID' &amp;&amp; '#follow-us-social' != ''){   pcm_tooltip_opts.customContentID = '#follow-us-social';  }else if('useContentID' == 'customContent' &amp;&amp; '' != ''){   pcm_tooltip_opts.customContent = ''  }   if('' != ''){   pcm_tooltip_opts.isThemeHeader = true;   pcm_tooltip_opts.headerTitle = '';   pcm_tooltip_opts.headerBg = '#1b5d9e';   pcm_tooltip_opts.headerColor = '#000';  }   if('1px' != '0' &amp;&amp; '1px' != '0px'){   pcm_tooltip_opts.tooltipBorderSize = '1px';   pcm_tooltip_opts.tooltipBorderColor = '#e6e6e6';  }    if('' != ''){ pcm_tooltip_opts.width = ''; }  if('25px' != ''){ pcm_tooltip_opts.customArrowPos = '25px'; }  if('bottom' != 'auto'){ pcm_tooltip_opts.tooltipShowDirection = 'bottom'; }  if('#fff' != ''){ pcm_tooltip_opts.contentBGcolor = '#fff'; }  if('10px' != ''){ pcm_tooltip_opts.contentPadding = '10px'; }  if('-4' != ''){ pcm_tooltip_opts.distanceFromBaseElement = '-4'; }  if('800' != ''){ pcm_tooltip_opts.zIndex = '800'; }    pcm_tooltip_opts.eventsArray = 'click'.split(',');    jQuery('#follow-link').pcm_tooltip(pcm_tooltip_opts); });            jQuery(document).ready(function(){  var pcm_tooltip_opts = {};   if('useHref' == 'useContentID' &amp;&amp; '' != ''){   pcm_tooltip_opts.customContentID = '';  }else if('useHref' == 'customContent' &amp;&amp; '' != ''){   pcm_tooltip_opts.customContent = ''  }   if('' != ''){   pcm_tooltip_opts.isThemeHeader = true;   pcm_tooltip_opts.headerTitle = '';   pcm_tooltip_opts.headerBg = '#1b5d9e';   pcm_tooltip_opts.headerColor = '#000';  }   if('1px' != '0' &amp;&amp; '1px' != '0px'){   pcm_tooltip_opts.tooltipBorderSize = '1px';   pcm_tooltip_opts.tooltipBorderColor = '#e6e6e6';  }    if('' != ''){ pcm_tooltip_opts.width = ''; }  if('19px' != ''){ pcm_tooltip_opts.customArrowPos = '19px'; }  if('bottom' != 'auto'){ pcm_tooltip_opts.tooltipShowDirection = 'bottom'; }  if('#fff' != ''){ pcm_tooltip_opts.contentBGcolor = '#fff'; }  if('0' != ''){ pcm_tooltip_opts.contentPadding = '0'; }  if('-4' != ''){ pcm_tooltip_opts.distanceFromBaseElement = '-4'; }  if('800' != ''){ pcm_tooltip_opts.zIndex = '800'; }    pcm_tooltip_opts.eventsArray = 'click'.split(',');    jQuery('.sslink.dropd.ttipdwn').pcm_tooltip(pcm_tooltip_opts); });       Sign in                                                     Order Status                                                Sign In                                   New account?  Register                                                     /* jQuery(function($){                 PCM.tooltipDown.init('#signin-btn-21');             }); */                     Cart ()   var PCM = PCM || {}; PCM.cart=(function($){     function update(){         $.ajax({             url:"/home?op=mall.web.misc.cartLink.cartLink",             type:'POST',             dataType:'json',             data:'false',             success:count         });     }     function count(data){         if(typeof data !== 'undefined'){             $('[data-bind="cart-count"]').text(data.count)         }     }     return {         update:update     }; })(jQuery); PCM.cart.update();                                                                                                                                                                    PCM (Home)                                              STARTUPS / ENTREPRENEURSMEDIUM / LARGE BUSINESSENTERPRISEHEALTHCARE                                                                                                                                              GOVERNMENT (Home)                                              FEDERALSTATE &amp; LOCALEDUCATIONHEALTHCARE                                                                                                                                              E-PROCUREMENT                                              PCM BUSINESS DIRECTPCM OPSTRACK                                                             jQuery(function($){     PCM.changeHomepage.init();     var lastClickedTab = 'last_clicked_tab';     var active = getCookie(lastClickedTab);     var widget=$("#drk-mmenu-13"), $greet=widget.find('.greetings-txt');     if('msc-515,msc-497,msc-428,msc-429,msc-426,msc-427,msc-home,msc-430,msc-425,'.indexOf('msc-home,') &gt; -1){   active = 'msc-home';  }     var txt=widget.find('[navpoint-id="' + active + '"]')     if(txt.length) {         var greetings = txt.attr('greetings');         if(greetings) {             $greet.text(greetings);         }         txt.addClass('actv');     }else{      widget.find('a[navpoint-id]').first().addClass('actv');     }     $greet.show();          var host = window.location.host;     var links= widget.find('a[navpoint-id]')     links.click(function(e){      var navId = $(this).attr('navpoint-id'), href=$(this).attr('href');      if(navId &amp;&amp; href &amp;&amp; (href.charAt(0)=='/' || host===href.split('/')[2])){       document.cookie = lastClickedTab + '=' + navId + '; expires=' + setExpirationDate(30) + '; path=/';      }     });     var setExpirationDate = function(days){      var date = new Date();         date.setTime(date.getTime()+(days*24*60*60*1000));         return date.toUTCString();     };      });  var getCookie = function(name){  var nameEQ = name + "=";     var ca = document.cookie.split(';');     for(var i=0;i &lt; ca.length;i++) {         var c = jQuery.trim(ca[i]);         if (c.indexOf(nameEQ) === 0) return c.substring(nameEQ.length,c.length);     }     return null; };                                                                                                                                                                                                Thank You!                                                         Thank you for subscribing to our newsletter. Be sure to check your email for exclusive offers and discounts.                                   jQuery(document).ready(function() {      PCM.subscribeEmailValidate.init({formNewsLetterEle: '#email-subscribe',          allowPageReload : false});  });      1-800-700-1000    (function(c, h, a, t, _, i, d) {     c[_] = c[_] || function() {         (c[_].q = c[_].q || []).push(arguments)     }, c[_].l = 1 * new Date();     i = h.createElement(a), d = h.getElementsByTagName(a)[0];     i.async = 1;     i.src = t;     d.parentNode.insertBefore(i, d) })(window, document, 'script', 'https://chatidcdn.com/embed/pcm/latest.js', 'CID');            Follow     PCM Blog  Spiceworks  Facebook  LinkedIn  Twitter  YouTube            jQuery(document).ready(function(){  var pcm_tooltip_opts = {};   if('useContentID' == 'useContentID' &amp;&amp; '#follow-us-social' != ''){   pcm_tooltip_opts.customContentID = '#follow-us-social';  }else if('useContentID' == 'customContent' &amp;&amp; '' != ''){   pcm_tooltip_opts.customContent = ''  }   if('' != ''){   pcm_tooltip_opts.isThemeHeader = true;   pcm_tooltip_opts.headerTitle = '';   pcm_tooltip_opts.headerBg = '#1b5d9e';   pcm_tooltip_opts.headerColor = '#000';  }   if('1px' != '0' &amp;&amp; '1px' != '0px'){   pcm_tooltip_opts.tooltipBorderSize = '1px';   pcm_tooltip_opts.tooltipBorderColor = '#e6e6e6';  }    if('' != ''){ pcm_tooltip_opts.width = ''; }  if('25px' != ''){ pcm_tooltip_opts.customArrowPos = '25px'; }  if('bottom' != 'auto'){ pcm_tooltip_opts.tooltipShowDirection = 'bottom'; }  if('#fff' != ''){ pcm_tooltip_opts.contentBGcolor = '#fff'; }  if('10px' != ''){ pcm_tooltip_opts.contentPadding = '10px'; }  if('-4' != ''){ pcm_tooltip_opts.distanceFromBaseElement = '-4'; }  if('800' != ''){ pcm_tooltip_opts.zIndex = '800'; }    pcm_tooltip_opts.eventsArray = 'click'.split(',');    jQuery('#follow-link').pcm_tooltip(pcm_tooltip_opts); });            jQuery(document).ready(function(){  var pcm_tooltip_opts = {};   if('useHref' == 'useContentID' &amp;&amp; '' != ''){   pcm_tooltip_opts.customContentID = '';  }else if('useHref' == 'customContent' &amp;&amp; '' != ''){   pcm_tooltip_opts.customContent = ''  }   if('' != ''){   pcm_tooltip_opts.isThemeHeader = true;   pcm_tooltip_opts.headerTitle = '';   pcm_tooltip_opts.headerBg = '#1b5d9e';   pcm_tooltip_opts.headerColor = '#000';  }   if('1px' != '0' &amp;&amp; '1px' != '0px'){   pcm_tooltip_opts.tooltipBorderSize = '1px';   pcm_tooltip_opts.tooltipBorderColor = '#e6e6e6';  }    if('' != ''){ pcm_tooltip_opts.width = ''; }  if('19px' != ''){ pcm_tooltip_opts.customArrowPos = '19px'; }  if('bottom' != 'auto'){ pcm_tooltip_opts.tooltipShowDirection = 'bottom'; }  if('#fff' != ''){ pcm_tooltip_opts.contentBGcolor = '#fff'; }  if('0' != ''){ pcm_tooltip_opts.contentPadding = '0'; }  if('-4' != ''){ pcm_tooltip_opts.distanceFromBaseElement = '-4'; }  if('800' != ''){ pcm_tooltip_opts.zIndex = '800'; }    pcm_tooltip_opts.eventsArray = 'click'.split(',');    jQuery('.sslink.dropd.ttipdwn').pcm_tooltip(pcm_tooltip_opts); });       Sign in                                                     Order Status                                                Sign In                                   New account?  Register                                                     /* jQuery(function($){                 PCM.tooltipDown.init('#signin-btn-21');             }); */                     Cart ()   var PCM = PCM || {}; PCM.cart=(function($){     function update(){         $.ajax({             url:"/home?op=mall.web.misc.cartLink.cartLink",             type:'POST',             dataType:'json',             data:'false',             success:count         });     }     function count(data){         if(typeof data !== 'undefined'){             $('[data-bind="cart-count"]').text(data.count)         }     }     return {         update:update     }; })(jQuery); PCM.cart.update();                                                                                                                                                                                               Thank You!                                                         Thank you for subscribing to our newsletter. Be sure to check your email for exclusive offers and discounts.                                   jQuery(document).ready(function() {      PCM.subscribeEmailValidate.init({formNewsLetterEle: '#email-subscribe',          allowPageReload : false});  });    1-800-700-1000  (function(c, h, a, t, _, i, d) {     c[_] = c[_] || function() {         (c[_].q = c[_].q || []).push(arguments)     }, c[_].l = 1 * new Date();     i = h.createElement(a), d = h.getElementsByTagName(a)[0];     i.async = 1;     i.src = t;     d.parentNode.insertBefore(i, d) })(window, document, 'script', 'https://chatidcdn.com/embed/pcm/latest.js', 'CID');          Follow     PCM Blog  Spiceworks  Facebook  LinkedIn  Twitter  YouTube            jQuery(document).ready(function(){  var pcm_tooltip_opts = {};   if('useContentID' == 'useContentID' &amp;&amp; '#follow-us-social' != ''){   pcm_tooltip_opts.customContentID = '#follow-us-social';  }else if('useContentID' == 'customContent' &amp;&amp; '' != ''){   pcm_tooltip_opts.customContent = ''  }   if('' != ''){   pcm_tooltip_opts.isThemeHeader = true;   pcm_tooltip_opts.headerTitle = '';   pcm_tooltip_opts.headerBg = '#1b5d9e';   pcm_tooltip_opts.headerColor = '#000';  }   if('1px' != '0' &amp;&amp; '1px' != '0px'){   pcm_tooltip_opts.tooltipBorderSize = '1px';   pcm_tooltip_opts.tooltipBorderColor = '#e6e6e6';  }    if('' != ''){ pcm_tooltip_opts.width = ''; }  if('25px' != ''){ pcm_tooltip_opts.customArrowPos = '25px'; }  if('bottom' != 'auto'){ pcm_tooltip_opts.tooltipShowDirection = 'bottom'; }  if('#fff' != ''){ pcm_tooltip_opts.contentBGcolor = '#fff'; }  if('10px' != ''){ pcm_tooltip_opts.contentPadding = '10px'; }  if('-4' != ''){ pcm_tooltip_opts.distanceFromBaseElement = '-4'; }  if('800' != ''){ pcm_tooltip_opts.zIndex = '800'; }    pcm_tooltip_opts.eventsArray = 'click'.split(',');    jQuery('#follow-link').pcm_tooltip(pcm_tooltip_opts); });        Follow     PCM Blog  Spiceworks  Facebook  LinkedIn  Twitter  YouTube      jQuery(document).ready(function(){  var pcm_tooltip_opts = {};   if('useContentID' == 'useContentID' &amp;&amp; '#follow-us-social' != ''){   pcm_tooltip_opts.customContentID = '#follow-us-social';  }else if('useContentID' == 'customContent' &amp;&amp; '' != ''){   pcm_tooltip_opts.customContent = ''  }   if('' != ''){   pcm_tooltip_opts.isThemeHeader = true;   pcm_tooltip_opts.headerTitle = '';   pcm_tooltip_opts.headerBg = '#1b5d9e';   pcm_tooltip_opts.headerColor = '#000';  }   if('1px' != '0' &amp;&amp; '1px' != '0px'){   pcm_tooltip_opts.tooltipBorderSize = '1px';   pcm_tooltip_opts.tooltipBorderColor = '#e6e6e6';  }    if('' != ''){ pc</v>
-      </c>
-      <c r="F7" t="str">
-        <v xml:space="preserve">m_tooltip_opts.width = ''; }  if('25px' != ''){ pcm_tooltip_opts.customArrowPos = '25px'; }  if('bottom' != 'auto'){ pcm_tooltip_opts.tooltipShowDirection = 'bottom'; }  if('#fff' != ''){ pcm_tooltip_opts.contentBGcolor = '#fff'; }  if('10px' != ''){ pcm_tooltip_opts.contentPadding = '10px'; }  if('-4' != ''){ pcm_tooltip_opts.distanceFromBaseElement = '-4'; }  if('800' != ''){ pcm_tooltip_opts.zIndex = '800'; }    pcm_tooltip_opts.eventsArray = 'click'.split(',');    jQuery('#follow-link').pcm_tooltip(pcm_tooltip_opts); });      jQuery(document).ready(function(){  var pcm_tooltip_opts = {};   if('useHref' == 'useContentID' &amp;&amp; '' != ''){   pcm_tooltip_opts.customContentID = '';  }else if('useHref' == 'customContent' &amp;&amp; '' != ''){   pcm_tooltip_opts.customContent = ''  }   if('' != ''){   pcm_tooltip_opts.isThemeHeader = true;   pcm_tooltip_opts.headerTitle = '';   pcm_tooltip_opts.headerBg = '#1b5d9e';   pcm_tooltip_opts.headerColor = '#000';  }   if('1px' != '0' &amp;&amp; '1px' != '0px'){   pcm_tooltip_opts.tooltipBorderSize = '1px';   pcm_tooltip_opts.tooltipBorderColor = '#e6e6e6';  }    if('' != ''){ pcm_tooltip_opts.width = ''; }  if('19px' != ''){ pcm_tooltip_opts.customArrowPos = '19px'; }  if('bottom' != 'auto'){ pcm_tooltip_opts.tooltipShowDirection = 'bottom'; }  if('#fff' != ''){ pcm_tooltip_opts.contentBGcolor = '#fff'; }  if('0' != ''){ pcm_tooltip_opts.contentPadding = '0'; }  if('-4' != ''){ pcm_tooltip_opts.distanceFromBaseElement = '-4'; }  if('800' != ''){ pcm_tooltip_opts.zIndex = '800'; }    pcm_tooltip_opts.eventsArray = 'click'.split(',');    jQuery('.sslink.dropd.ttipdwn').pcm_tooltip(pcm_tooltip_opts); });     Sign in                                                     Order Status                                                Sign In                                   New account?  Register                                                     /* jQuery(function($){                 PCM.tooltipDown.init('#signin-btn-21');             }); */                   Cart ()   var PCM = PCM || {}; PCM.cart=(function($){     function update(){         $.ajax({             url:"/home?op=mall.web.misc.cartLink.cartLink",             type:'POST',             dataType:'json',             data:'false',             success:count         });     }     function count(data){         if(typeof data !== 'undefined'){             $('[data-bind="cart-count"]').text(data.count)         }     }     return {         update:update     }; })(jQuery); PCM.cart.update();                                  Solutions &amp; Services                Cloud    Products                                                                                               Cloud Partners                                             Shop Now                                                                                                        PCM Hybrid Cloud                                             Learn More                                                                                                                                                   Featured                                    Deal of the Week                  Top Searches                  Ultrabook Finder                  Memory Finder                  Ink/Toner Finder                                                                                               Hardware                                    Accessories                  Cables                  Computers                  Memory                  Monitors &amp; Projectors                  Networking                  Printers &amp; Supplies                  Racks, Power &amp; Cooling                  Scanners                  Servers                  Storage                                           All Categories                                                                              Software                                    Backup                  Business                  Database                  Desktop &amp; Web Publishing                  Management                  Operating Systems                  Security                  Unified Collaboration                  Virtualization                                           All Categories                                                                              Brands                                    Apple                  Cisco                  Dell                  Google                  HPI                  HPE                  Intel                  Lenovo                  Microsoft                  Samsung                  Symantec                  VMware                                           All Brands                                                       jQuery(function($){     PCM.mainNav.init();     var cont=$('.static-links-con,.menu-nav');     cont.show();     $('.menu-nav .static-links-con').each(function(i,t){         var h=0;         $(t).find('.sub-group-name').each(function(i,s){             h=Math.max(h,$(s).height());         }).each(function(i,s){             $(s).height(h);         });     });     cont.hide(); });                            All Products     Mfg Part Number     PCM Part Number                                                      PCM.dropDown = (function($j) {  var init = function($id, $main, inputBar, elem) {   var dropDownDiv;   var textSpan;   var dropSpan;   var inputDiv;   var searchNow = $main.find('.searchInputBtn');      var SEARCH_TEXT = 'Search Products';   var PADDING_SELECT = 30;   var BORDER_WIDTH = 1;    var initEvent = function() {        placeHolder();    elem.selectBoxIt();    elem.change(function(){                 adjustSearchBox();             });    searchNow.click(function(){     checkInputBox();     return false;    });    inputBar.keypress(function(e){     if(e.which === 13){      checkInputBox();      return false;     }    });        adjustSearchBox();   };   var checkInputBox = function(){    var val = $j.trim(inputBar.val()).replace(/\\/g, "");             if(val.length === 0 || val === SEARCH_TEXT){                 alert('Please enter a search keyword');                 //PCM.modalBx('', {'width': 350}).modal().openModal('#error-search');             }else{                 var $type=elem,                 _val = encodeURIComponent(val),                 _q = $type.val().replace(/$0/g, _val),                 url = [$type.attr('href'), _val, _q?"&amp;":"", _q];                 window.location= url.join("");             }   };   var adjustSearchBox = function(){    textSpan = $main.find('.selectboxit-text');    dropSpan = $main.find('.selectboxit');    inputDiv = $main.find('.hm-srch-inpt');        dropSpan.width((textSpan.width() + PADDING_SELECT) + 'px');    inputDiv.width(($main.width() - dropSpan.parent().width() - BORDER_WIDTH ) + 'px');       };   var placeHolder = function(){        var textBox = $id + ' .searchInput';       $j(document).on('blur', textBox, function () {               placeText($j(this), SEARCH_TEXT);           });           $j(document).on('focus', textBox, function () {               clrText($j(this), SEARCH_TEXT);           });           $j(document).on('input', textBox, function () {               placeText($j(this), SEARCH_TEXT);               clrText($j(this), SEARCH_TEXT, true);           });            placeText($j(textBox), SEARCH_TEXT);   };    var placeText = function (base, txt) {           if ($j.trim(base.val()) === '') {               base.val(txt);               base.addClass('plcfont');                          } else if ($j.trim(base.val()) !== txt) {               base.removeClass('plcfont');           }        };       var clrText = function (base, txt, isAddStyle) {           if ($j.trim(base.val()) === txt) {               base.val('');               base.removeClass('plcfont');           }       };   initEvent();  };   return {   init : init  }; })(jQuery);        jQuery(function(j){     var $id='#search-menu-9', $main=j($id), $searchInput = $main.find('.searchInput'), $option = $main.find('[selectit="searchOptions"]');     PCM.dropDown.init($id, $main, $searchInput, $option);     PCM.typeAhead.init($main, $searchInput, "/ajaxCall/typeahead", $option); });   {{#category}} &lt;h3 class="first"&gt;Matching Keywords&lt;/h3&gt; &lt;ul class="first-lvl"&gt;  {{#suggestions}}     &lt;li&gt;&lt;a href="/s?rch&amp;includeImage=true&amp;q={{keyword}}&amp;ssrc=box"&gt;&lt;span class="txt"&gt;{{keyword}}&lt;/span&gt;&lt;span class="count"&gt;({{count}})&lt;/span&gt;&lt;/a&gt;         {{#firstSection}}         &lt;ul class="second-lvl"&gt;             {{#items}}             &lt;li&gt;&lt;a href="/s?rch&amp;includeImage=true&amp;q={{keyword}}&amp;stn={{name}}&amp;ssrc=box" data-keyword="{{keyword}}"&gt;in {{name}}&lt;/a&gt;&lt;/li&gt;             {{/items}}         &lt;/ul&gt;         {{/firstSection}}     &lt;/li&gt;     {{/suggestions}} &lt;/ul&gt; {{/category}} {{#brand}} &lt;h3&gt;Matching Brands&lt;/h3&gt; &lt;ul class="second-lvl"&gt;  {{#items}}  &lt;li&gt;&lt;a href="/s?rch&amp;includeImage=true&amp;q={{keyword}}&amp;man={{name}}&amp;ssrc=box" data-keyword="{{keyword}}"&gt;by {{name}}&lt;/a&gt;&lt;/li&gt;  {{/items}} &lt;/ul&gt; {{/brand}} {{#product}} &lt;h3&gt;Suggestions for {{keyword}}&lt;/h3&gt; &lt;ul class="suggest"&gt;  {{#items}}     &lt;li&gt;         &lt;a href="/p/{{edp}}" title="{{name}}" data-keyword="{{edp}}"&gt;             &lt;span class="tbl"&gt;                 &lt;span class="tr"&gt;                     &lt;span class="td col-img"&gt;&lt;img src="{{#imagePath}}{{imagePath}}{{/imagePath}}{{^imagePath}}/mall/widgetti/images/shared/noImageMed.jpg{{/imagePath}}" e_src="/mall/widgetti/images/shared/noImageMed.jpg" width="67"&gt;&lt;/span&gt;                     &lt;span class="td col-desc"&gt;                         &lt;span class="offer"&gt;{{manufacturer}}&lt;/span&gt;                         &lt;span class="prod-title"&gt;{{name}}&lt;/span&gt;                     &lt;/span&gt;                 &lt;/span&gt;             &lt;/span&gt;         &lt;/a&gt;     &lt;/li&gt;     {{/items}} &lt;/ul&gt; {{/product}}                          Solutions &amp; Services     Solutions &amp; Services       Cloud    Products                                                                                               Cloud Partners                                             Shop Now                                                                                                        PCM Hybrid Cloud                                             Learn More                                                                                                                                                   Featured                                    Deal of the Week                  Top Searches                  Ultrabook Finder                  Memory Finder                  Ink/Toner Finder                                                                                               Hardware                                    Accessories                  Cables                  Computers                  Memory                  Monitors &amp; Projectors                  Networking                  Printers &amp; Supplies                  Racks, Power &amp; Cooling                  Scanners                  Servers                  Storage                                           All Categories                                                                              Software                                    Backup                  Business                  Database                  Desktop &amp; Web Publishing                  Management                  Operating Systems                  Security                  Unified Collaboration                  Virtualization                                           All Categories                                                                              Brands                                    Apple                  Cisco                  Dell                  Google                  HPI                  HPE                  Intel                  Lenovo                  Microsoft                  Samsung                  Symantec                  VMware                                           All Brands                                                       jQuery(function($){     PCM.mainNav.init();     var cont=$('.static-links-con,.menu-nav');     cont.show();     $('.menu-nav .static-links-con').each(function(i,t){         var h=0;         $(t).find('.sub-group-name').each(function(i,s){             h=Math.max(h,$(s).height());         }).each(function(i,s){             $(s).height(h);         });     });     cont.hide(); });                          All Products     Mfg Part Number     PCM Part Number                                                      PCM.dropDown = (function($j) {  var init = function($id, $main, inputBar, elem) {   var dropDownDiv;   var textSpan;   var dropSpan;   var inputDiv;   var searchNow = $main.find('.searchInputBtn');      var SEARCH_TEXT = 'Search Products';   var PADDING_SELECT = 30;   var BORDER_WIDTH = 1;    var initEvent = function() {        placeHolder();    elem.selectBoxIt();    elem.change(function(){                 adjustSearchBox();             });    searchNow.click(function(){     checkInputBox();     return false;    });    inputBar.keypress(function(e){     if(e.which === 13){      checkInputBox();      return false;     }    });        adjustSearchBox();   };   var checkInputBox = function(){    var val = $j.trim(inputBar.val()).replace(/\\/g, "");             if(val.length === 0 || val === SEARCH_TEXT){                 alert('Please enter a search keyword');                 //PCM.modalBx('', {'width': 350}).modal().openModal('#error-search');             }else{                 var $type=elem,                 _val = encodeURIComponent(val),                 _q = $type.val().replace(/$0/g, _val),                 url = [$type.attr('href'), _val, _q?"&amp;":"", _q];                 window.location= url.join("");             }   };   var adjustSearchBox = function(){    textSpan = $main.find('.selectboxit-text');    dropSpan = $main.find('.selectboxit');    inputDiv = $main.find('.hm-srch-inpt');        dropSpan.width((textSpan.width() + PADDING_SELECT) + 'px');    inputDiv.width(($main.width() - dropSpan.parent().width() - BORDER_WIDTH ) + 'px');       };   var placeHolder = function(){        var textBox = $id + ' .searchInput';       $j(document).on('blur', textBox, function () {               placeText($j(this), SEARCH_TEXT);           });           $j(document).on('focus', textBox, function () {               clrText($j(this), SEARCH_TEXT);           });           $j(document).on('input', textBox, function () {               placeText($j(this), SEARCH_TEXT);               clrText($j(this), SEARCH_TEXT, true);           });            placeText($j(textBox), SEARCH_TEXT);   };    var placeText = function (base, txt) {           if ($j.trim(base.val()) === '') {               base.val(txt);               base.addClass('plcfont');                          } else if ($j.trim(base.val()) !== txt) {               base.removeClass('plcfont');           }        };       var clrText = function (base, txt, isAddStyle) {           if ($j.trim(base.val()) === txt) {               base.val('');               base.removeClass('plcfont');           }       };   initEvent();  };   return {   init : init  }; })(jQuery);        jQuery(function(j){     var $id='#search-menu-9', $main=j($id), $searchInput = $main.find('.searchInput'), $option = $main.find('[selectit="searchOptions"]');     PCM.dropDown.init($id, $main, $searchInput, $option);     PCM.typeAhead.init($main, $searchInput, "/ajaxCall/typeahead", $option); });   {{#category}} &lt;h3 class="first"&gt;Matching Keywords&lt;/h3&gt; &lt;ul class="first-lvl"&gt;  {{#suggestions}}     &lt;li&gt;&lt;a href="/s?rch&amp;includeImage=true&amp;q={{keyword}}&amp;ssrc=box"&gt;&lt;span class="txt"&gt;{{keyword}}&lt;/span&gt;&lt;span class="count"&gt;({{count}})&lt;/span&gt;&lt;/a&gt;         {{#firstSection}}         &lt;ul class="second-lvl"&gt;             {{#items}}             &lt;li&gt;&lt;a href="/s?rch&amp;includeImage=true&amp;q={{keyword}}&amp;stn={{name}}&amp;ssrc=box" data-keyword="{{keyword}}"&gt;in {{name}}&lt;/a&gt;&lt;/li&gt;             {{/items}}         &lt;/ul&gt;         {{/firstSection}}     &lt;/li&gt;     {{/suggestions}} &lt;/ul&gt; {{/category}} {{#brand}} &lt;h3&gt;Matching Brands&lt;/h3&gt; &lt;ul class="second-lvl"&gt;  {{#items}}  &lt;li&gt;&lt;a href="/s?rch&amp;includeImage=true&amp;q={{keyword}}&amp;man={{name}}&amp;ssrc=box" data-keyword="{{keyword}}"&gt;by {{name}}&lt;/a&gt;&lt;/li&gt;  {{/items}} &lt;/ul&gt; {{/brand}} {{#product}} &lt;h3&gt;Suggestions for {{keyword}}&lt;/h3&gt; &lt;ul class="suggest"&gt;  {{#items}}     &lt;li&gt;         &lt;a href="/p/{{edp}}" title="{{name}}" data-keyword="{{edp}}"&gt;             &lt;span class="tbl"&gt;                 &lt;span class="tr"&gt;                     &lt;span class="td col-img"&gt;&lt;img src="{{#imagePath}}{{imagePath}}{{/imagePath}}{{^imagePath}}/mall/widgetti/images/shared/noImageMed.jpg{{/imagePath}}" e_src="/mall/widgetti/images/shared/noImageMed.jpg" width="67"&gt;&lt;/span&gt;                     &lt;span class="td col-desc"&gt;                         &lt;span class="offer"&gt;{{manufacturer}}&lt;/span&gt;                         &lt;span class="prod-title"&gt;{{name}}&lt;/span&gt;                     &lt;/span&gt;                 &lt;/span&gt;             &lt;/span&gt;         &lt;/a&gt;     &lt;/li&gt;     {{/items}} &lt;/ul&gt; {{/product}}                                                      document.getElementsByName = function(name){    return jQuery('[name="' + name + '"]');    }                                                          document.getElementsByName = function(name){    return jQuery('[name="' + name + '"]');    }        document.getElementsByName = function(name){    return jQuery('[name="' + name + '"]');    }                                                                                                                                                                                          jQuery(function($){     PCM.slideBanner.init($('#sldr-widget-10'), '/home?1453599977565&amp;op=mall.web.misc.layeredSlider.layeredSlider&amp;banners=msc-home-10#banners'); });                               Picking the Right Printer for your Office [INFOGRAPHIC]                     January 19, 2016                     Microsoft Announces Major Change to the Enterprise Agreement Program                     January 6, 2016                     How Christmas Gifts Could Impact BYOD                     January 4, 2016                     Enhance Your Creativity with Adobe Stock                     December 30, 2015                     HP Print Security Seminars: Is Your Network at Risk to Hackers?                     December 22, 2015                     Share Costs and Save Time with Hewlett Packard Enterprise Healthcare                     December 21, 2015                     Microsoft Announces that Windows Server 2016 will be Launching Next Quarter                     December 11, 2015                     Last Chance to Register for Vision Hollywood!                     December 10, 2015                     How Big of a Deal is the Apple-Cisco Partnership?                     December 9, 2015                     Webcast: ShoreTel Truly Unified Communications                     December 8, 2015                     Ergotron StyleView: Fit for Every Body                     December 7, 2015                     The Digital Pulse of Tomorrow’s Healthcare with Lenovo                     December 7, 2015                                                                               jQuery(function($){     PCM.newsFeed.init();     var t8=$('.pcm-nws .trunk8'),li=t8.closest('li');     li.css('display','block');     t8.trunk8().removeClass('trunk8');     li.css('display','');      //Reapply title to support html tags   var rcNws =  jQuery('.hm-nws').find('.rc-nws');   var title = jQuery('.hm-nws').find('.titleTempHolder').val();   rcNws.html(title);   jQuery('.hm-nws').find('.titleTempHolder').remove();    });                                                                                  Deal of the Week                     HP 14" G3 Quad-Core ChromebookOnly $179.99               Shop Now                                                                                    Lenovo B40-80 80F6 Notebook              Reach a New Height inBusiness ComputingOnly $349.99                Shop Now                                                                       Managed Print Services              Save Millions. Gain Visibility. Take Control.               Shop Now                                                                                   Featured Products                                                         Bestsellers                                                         New Arrivals                                                         Trending                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                      &lt;div class="prd-tbl-con rctb hide-avail"&gt;         &lt;div class="tr"&gt; {{#products}}     &lt;div class="tbl-cll itemlist {{first}} {{last}}" data-sku="{{dpno}}"&gt;         &lt;!--if secret sale         &lt;div class="icn-vio-ssp"&gt;&lt;/div&gt;         --&gt;         {{#lowestPrice}}         &lt;div class="icn-vio-gbp"&gt;&lt;/div&gt;         {{/lowestPrice}}         &lt;div class="item {{first}} {{last}}"&gt;             &lt;div class="itm-img"&gt;                 &lt;img class="img-load" src="/widgets/product-view/img/load.gif" /&gt;                 {{^notAvailable}}&lt;a class="prod-image" href="{{link}}" title="{{name}}"&gt;&lt;img class="pro-image" src="{{imgSrc}}"                     e_src="/widgets/product-view/img/noImage_150.jpg"/&gt;&lt;/a&gt;{{/notAvailable}}                 {{#notAvailable}}&lt;img class="pro-image" src="/mall/widgetti/images/shared/notAvailable_150.jpg"                     e_src="/widgets/product-view/img/noImage_150.jpg"/&gt;{{/notAvailable}}             &lt;/div&gt;             {{^savePrice}}             &lt;div class="item-cll npsve"&gt;&lt;/div&gt;             {{/savePrice}}             {{#savePrice}}             &lt;div class="itm-sve"&gt;                 &lt;span&gt;Save&lt;/span&gt; &lt;span class="svprc"&gt;{{savePrice}}&lt;/span&gt;{{#savePercent}} &lt;span class="nrm"&gt;(&lt;/span&gt;&lt;span                     class="sv-prcnt nrm"&gt;{{savePercent}}&lt;/span&gt;&lt;span class="nrm"&gt;)&lt;/span&gt;{{/savePercent}}             &lt;/div&gt;             {{/savePrice}}              &lt;div class="itm-ttl prod-name"&gt;                 &lt;h2&gt;                     {{^notAvailable}}&lt;a href="{{link}}" title="{{name}}"&gt;{{name}}&lt;/a&gt;{{/notAvailable}}                     {{#notAvailable}}&lt;span class="prodName"&gt;Product is No Longer Available&lt;/span&gt;{{/notAvailable}}                 &lt;/h2&gt;             &lt;/div&gt;             &lt;div class="itm-eval prod-avail"&gt;                 {{^notAvailable}}                 &lt;div class="avlb"&gt;                     &lt;span class="avlbs"&gt;Availability:&lt;/span&gt;                     &lt;span class="statavlb"&gt;{{availability}}&lt;/span&gt;                 &lt;/div&gt;                 {{#rateValue}}                 &lt;div class="istr"&gt;                     &lt;div class="str" style="width: {{rate}}%;"&gt;&lt;/div&gt;                 &lt;/div&gt;                 &lt;div class="rater"&gt;                     &lt;a href="{{link}}#pdppdpUserReview" title="Ratings"&gt; ({{rateValue}})&lt;/a&gt;                 &lt;/div&gt;                 {{/rateValue}}                 {{^rateValue}}                 &lt;div class="nstr rater"&gt;&lt;a href="https://www.pcm.com/o/Write-A-Review/msc-66?op=mall.web.zones.pdpRecentReviews.writeReview&amp;amp;dpno={{dpno}}" title="Be the first to write a review"&gt;Be the first to write a review&lt;/a&gt;&lt;/div&gt;                 {{/rateValue}}                 {{/notAvailable}}             &lt;/div&gt;             &lt;div class="itm-prc"&gt;                 &lt;div class="pprcd"&gt;                     &lt;!--if secretsale                     &lt;div class="rprice upp ssp"&gt;                         &lt;span class="ntce"&gt;Secret Sale Price&lt;/span&gt;                     &lt;/div&gt;                     --&gt;                     &lt;!--else--&gt;                      &lt;div class="prc lprc"&gt;                         &lt;p&gt;{{listPrice}}&lt;/p&gt;                     &lt;/div&gt;                     &lt;div class="prc tprc"&gt;                         &lt;p class="prod-price"&gt;{{totalPrice}}&lt;/p&gt;                     &lt;/div&gt;                     &lt;div class="clr"&gt;&lt;/div&gt;                     &lt;!--end--&gt;                 &lt;/div&gt;                 {{#enableCartBtn}}                 &lt;div class="crt-btn"&gt;                 {{#lowestPrice}}                     &lt;div class="crt upp"&gt;                         &lt;a data-action="Button:See Lowest Price" data-label="prod-{{dpno}}" href="{{link}}" class="ga" title="See Lowest Price"&gt;See Lowest Price&lt;/a&gt;                     &lt;/div&gt;                 {{/lowestPrice}}                 {{#callPrice}}                     &lt;div class="crt upp"&gt;                          &lt;a  href="{{link}}" class="upplinks ga" title="Call For Price"&gt;Call For Price&lt;/a&gt;                     &lt;/div&gt;                 {{/callPrice}}                 {{#addCart}}                     &lt;div class="qty"&gt;                         &lt;div class="bl"&gt;&lt;/div&gt;                         &lt;input type="text" id="addCartQty{{dpno}}" value="1" maxlength="3"&gt;                         &lt;div class="br"&gt;&lt;/div&gt;                         &lt;div class="clr"&gt;&lt;/div&gt;                     &lt;/div&gt;                     &lt;div class="crt"&gt;                         &lt;a href="#section=category&amp;amp;sku={{dpno}}" class="mbxlinks" metadata="{{metadata}}"                            title="Add to Cart"&gt;Add to Cart&lt;/a&gt;                     &lt;/div&gt;                 {{/addCart}}                 &lt;div class="clr"&gt;&lt;/div&gt;                 &lt;/div&gt;                 {{/enableCartBtn}}             &lt;/div&gt;         &lt;/div&gt;     &lt;/div&gt; {{/products}}     &lt;/div&gt; &lt;/div&gt;   &lt;div class="pge"&gt;     &lt;div class="num"&gt;         &lt;span class="crnt"&gt;{{startIndex}}&lt;/span&gt;&lt;span&gt;-&lt;/span&gt;&lt;span class="lmtpg"&gt;{{endIndex}}&lt;/span&gt;&lt;/span&gt;         &lt;span&gt;of&lt;/span&gt;&lt;span class="ttl"&gt;{{totalRecords}}&lt;/span&gt;     &lt;/div&gt;     &lt;div class="arw"&gt;         &lt;a href="#" class="lft {{left}}" data-page="{{previousPage}}"&gt;&lt;div class="aim {{left}}"&gt;&lt;/div&gt; &lt;/a&gt;         &lt;a href="#" class="rht {{right}}" data-page="{{nextPage}}"&gt;&lt;div class="aim {{right}}"&gt;&lt;/div&gt;&lt;/a&gt;         &lt;div class="clr"&gt;&lt;/div&gt;     &lt;/div&gt;     &lt;div class="clr"&gt;&lt;/div&gt; &lt;/div&gt;   &lt;div class="cnt bh-enabled"&gt;     &lt;h4&gt;You have no recently viewed items to display.&lt;/h4&gt;     &lt;p&gt;Can't find what you're searching for? Try one of these categories:&lt;/p&gt;     &lt;ul&gt;         {{#links}}&lt;li&gt;&lt;a title="{{label}}" href="{{link}}"{{#newTab}} target="_blank"{{/newTab}}&gt;{{label}}&lt;/a&gt;&lt;/li&gt;{{/links}}     &lt;/ul&gt; &lt;/div&gt; &lt;div class="cnt bh-disabled"&gt;     &lt;h4&gt;Your browsing history is disabled. &lt;a class="onbrowtrigger enable-browsing" href="#enable" url="/ajaxCall/recentlyviewed"&gt;Enable browsing history&lt;/a&gt;&lt;/h4&gt;     &lt;p&gt;Keep track of what you've viewed by turning on your browsing history. See items you've viewed, searches you've conducted and products you've visited.&lt;/p&gt; &lt;/div&gt;    jQuery(function($){     var $id = '#prod-view-tb-36';     PCM.productView.init($id);     PCM.gridRotate.init($($id).width(), $id, '.itemlist'); });                                  test                Preferred Partners                                                                                                                                                                                                                                jQuery(function($){     PCM.slideBanner.init($('#sldr-widget-10'), '/home?1453599977565&amp;op=mall.web.misc.layeredSlider.layeredSlider&amp;banners=msc-home-10#banners'); });                         Picking the Right Printer for your Office [INFOGRAPHIC]                     January 19, 2016                     Microsoft Announces Major Change to the Enterprise Agreement Program                     January 6, 2016                     How Christmas Gifts Could Impact BYOD                     January 4, 2016                     Enhance Your Creativity with Adobe Stock                     December 30, 2015                     HP Print Security Seminars: Is Your Network at Risk to Hackers?                     December 22, 2015                     Share Costs and Save Time with Hewlett Packard Enterprise Healthcare                     December 21, 2015                     Microsoft Announces that Windows Server 2016 will be Launching Next Quarter                     December 11, 2015                     Last Chance to Register for Vision Hollywood!                     December 10, 2015                     How Big of a Deal is the Apple-Cisco Partnership?                     December 9, 2015                     Webcast: ShoreTel Truly Unified Communications                     December 8, 2015                     Ergotron StyleView: Fit for Every Body                     December 7, 2015                     The Digital Pulse of Tomorrow’s Healthcare with Lenovo                     December 7, 2015                                                                               jQuery(function($){     PCM.newsFeed.init();     var t8=$('.pcm-nws .trunk8'),li=t8.closest('li');     li.css('display','block');     t8.trunk8().removeClass('trunk8');     li.css('display','');      //Reapply title to support html tags   var rcNws =  jQuery('.hm-nws').find('.rc-nws');   var title = jQuery('.hm-nws').find('.titleTempHolder').val();   rcNws.html(title);   jQuery('.hm-nws').find('.titleTempHolder').remove();    });                                                                     Deal of the Week                     HP 14" G3 Quad-Core ChromebookOnly $179.99               Shop Now                                                                                    Lenovo B40-80 80F6 Notebook              Reach a New Height inBusiness ComputingOnly $349.99                Shop Now                                                                       Managed Print Services              Save Millions. Gain Visibility. Take Control.               Shop Now                                                                                                  Deal of the Week                     HP 14" G3 Quad-Core ChromebookOnly $179.99               Shop Now                                                                                    Lenovo B40-80 80F6 Notebook              Reach a New Height inBusiness ComputingOnly $349.99                Shop Now                                                                       Managed Print Services              Save Millions. Gain Visibility. Take Control.               Shop Now                                                                      Deal of the Week                     HP 14" G3 Quad-Core ChromebookOnly $179.99               Shop Now                                                          Deal of the Week                     HP 14" G3 Quad-Core ChromebookOnly $179.99               Shop Now                           Deal of the Week                     HP 14" G3 Quad-Core ChromebookOnly $179.99               Shop Now     Deal of the Week HP 14" G3 Quad-Core ChromebookOnly $179.99  Shop Now                                      Lenovo B40-80 80F6 Notebook              Reach a New Height inBusiness ComputingOnly $349.99                Shop Now                                             Lenovo B40-80 80F6 Notebook              Reach a New Height inBusiness ComputingOnly $349.99                Shop Now              Lenovo B40-80 80F6 Notebook              Reach a New Height inBusiness ComputingOnly $349.99                Shop Now     Lenovo B40-80 80F6 Notebook Reach a New Height inBusiness ComputingOnly $349.99   Shop Now                                      Managed Print Services              Save Millions. Gain Visibility. Take Control.               Shop Now                                             Managed Print Services              Save Millions. Gain Visibility. Take Control.               Shop Now              Managed Print Services              Save Millions. Gain Visibility. Take Control.               Shop Now     Managed Print Services Save Millions. Gain Visibility. Take Control.  Shop Now                                  Featured Products                                                         Bestsellers                                                         New Arrivals                                                         Trending                                                                                                                                                                                      </v>
+        <v>Shop Now Featured Products Bestsellers New Arrivals Trending div classprdtblcon rctb hideavail div classtr products div classtblcll itemlist first last dataskudpno if secret sale div classicnviosspdiv lowestPrice div classicnviogbpdiv lowestPrice div classitem first last div classitmimg img classimgload srcwidgetsproductviewimgloadgif notAvailablea classprodimage hreflink titlenameimg classproimage srcimgSrc esrcwidgetsproductviewimgnoImage150jpganotAvailable notAvailableimg classproimage srcmallwidgettiimagessharednotAvailable150jpg esrcwidgetsproductviewimgnoImage150jpgnotAvailable div savePrice div classitemcll npsvediv savePrice savePrice div classitmsve spanSavespan span classsvprcsavePricespansavePercent span classnrmspanspan classsvprcnt nrmsavePercentspanspan classnrmspansavePercent div savePrice div classitmttl prodname h2 notAvailablea hreflink titlenamenameanotAvailable notAvailablespan classprodNameProduct is No Longer AvailablespannotAvailable h2 div div classitmeval prodavail notAvailable div classavlb span classavlbsAvailabilityspan span classstatavlbavailabilityspan div rateValue div classistr div classstr stylewidth ratediv div div classrater a hreflinkpdppdpUserReview titleRatings rateValuea div rateValue rateValue div classnstr ratera hrefhttpswwwpcmcomoWriteAReviewmsc66opmallwebzonespdpRecentReviewswriteReviewampdpnodpno titleBe the first to write a reviewBe the first to write a reviewadiv rateValue notAvailable div div classitmprc div classpprcd if secretsale div classrprice upp ssp span classntceSecret Sale Pricespan div else div classprc lprc plistPricep div div classprc tprc p classprodpricetotalPricep div div classclrdiv end div enableCartBtn div classcrtbtn lowestPrice div classcrt upp a dataactionButtonSee Lowest Price datalabelproddpno hreflink classga titleSee Lowest PriceSee Lowest Pricea div lowestPrice callPrice div classcrt upp a hreflink classupplinks ga titleCall For PriceCall For Pricea div callPrice addCart div classqty div classbldiv input typetext idaddCartQtydpno value1 maxlength3 div classbrdiv div classclrdiv div div classcrt a hrefsectioncategoryampskudpno classmbxlinks metadatametadata titleAdd to CartAdd to Carta div addCart div classclrdiv div enableCartBtn div div div products div div div classpge div classnum span classcrntstartIndexspanspanspanspan classlmtpgendIndexspanspan spanofspanspan classttltotalRecordsspan div div classarw a href classlft left datapagepreviousPagediv classaim leftdiv a a href classrht right datapagenextPagediv classaim rightdiva div classclrdiv div div classclrdiv div div classcnt bhenabled h4You have no recently viewed items to displayh4 pCant find what youre searching for Try one of these categoriesp ul linkslia titlelabel hreflinknewTab targetblanknewTablabelalilinks ul div div classcnt bhdisabled h4Your browsing history is disabled a classonbrowtrigger enablebrowsing hrefenable urlajaxCallrecentlyviewedEnable browsing historyah4 pKeep track of what youve viewed by turning on your browsing history See items youve viewed searches youve conducted and products youve visitedp div jQueryfunction var id prodviewtb36 PCMproductViewinitid PCMgridRotateinitidwidth id itemlist test Preferred Partners test Preferred Partners test Preferred Partners test Preferred Partners More than an IT Provider Were Your Technology Partner Since 1987 PCM has been a leading provider of IT products services solutions to businesses government agencies educational institutions and healthcare facilitiesWe provide access to over 300000 IT products like tablets slate notebooks desktops servers storage and networking from leading manufacturers like Cisco HP Apple Adobe Lenovo and Microsoft With powerful eProcurement tools comprehensive software licensing solutions and dedicated Account Executives its easy to get exactly what you need to tackle your technical challenges Our Company Support We Provide About Us Blog Brands Careers Certification Authorization Events Executives Investor Relations Locations Privacy Policy RSS Site Map Terms of Use and Sale Why PCM Catalog Subcriptions Contact Us Email Subscriptions Help Topics My Account Order Status Business Direct Employee Purchase Program Leasing Financing OpsTRACK Product Configurator Services Solutions Follow Us Spiceworks LinkedIn Facebook Twitter Youtube We proudly welcome American Express® Cards 1940 E Mariposa Ave El Segundo CA 90245 8007001000© 2016 PCM Sales Inc Entrust Tooltwist var gts gts gtspushid 235936 gtspushgooglebasesubaccountid 7846456 gtspushgooglebasecountry US gtspushgooglebaselanguage EN jQuerywindowload function var scheme https documentlocationprotocol https http var gts documentcreateElementscript gtstype textjavascript gtsasync true gtssrc scheme wwwgooglecommercecomtrustedstoresgtmpcompiledjs var s documentgetElementsByTagNamescript0 sparentNodeinsertBeforegts s More than an IT Provider Were Your Technology Partner Since 1987 PCM has been a leading provider of IT products services solutions to businesses government agencies educational institutions and healthcare facilitiesWe provide access to over 300000 IT products like tablets slate notebooks desktops servers storage and networking from leading manufacturers like Cisco HP Apple Adobe Lenovo and Microsoft With powerful eProcurement tools comprehensive software licensing solutions and dedicated Account Executives its easy to get exactly what you need to tackle your technical challenges Our Company Support We Provide About Us Blog Brands Careers Certification Authorization Events Executives Investor Relations Locations Privacy Policy RSS Site Map Terms of Use and Sale Why PCM Catalog Subcriptions Contact Us Email Subscriptions Help Topics My Account Order Status Business Direct Employee Purchase Program Leasing Financing OpsTRACK Product Configurator Services Solutions Follow Us Spiceworks LinkedIn Facebook Twitter Youtube We proudly welcome American Express® Cards 1940 E Mariposa Ave El Segundo CA 90245 8007001000© 2016 PCM Sales Inc Entrust Tooltwist More than an IT Provider Were Your Technology Partner Since 1987 PCM has been a leading provider of IT products services solutions to businesses government agencies educational institutions and healthcare facilitiesWe provide access to over 300000 IT products like tablets slate notebooks desktops servers storage and networking from leading manufacturers like Cisco HP Apple Adobe Lenovo and Microsoft With powerful eProcurement tools comprehensive software licensing solutions and dedicated Account Executives its easy to get exactly what you need to tackle your technical challenges Our Company Support We Provide About Us Blog Brands Careers Certification Authorization Events Executives Investor Relations Locations Privacy Policy RSS Site Map Terms of Use and Sale Why PCM Catalog Subcriptions Contact Us Email Subscriptions Help Topics My Account Order Status Business Direct Employee Purchase Program Leasing Financing OpsTRACK Product Configurator Services Solutions Our Company Support We Provide About Us Blog Brands Careers Certification Authorization Events Executives About Us Blog Brands Careers Certification Authorization Events Executives Investor Relations Locations Privacy Policy RSS Site Map Terms of Use and Sale Why PCM Investor Relations Locations Privacy Policy RSS Site Map Terms of Use and Sale Why PCM Catalog Subcriptions Contact Us Email Subscriptions Help Topics My Account Order Status Catalog Subcriptions Contact Us Email Subscriptions Help Topics My Account Order Status Business Direct Employee Purchase Program Leasing Financing OpsTRACK Product Configurator Services Solutions Business Direct Employee Purchase Program Leasing Financing OpsTRACK Product Configurator Services Solutions Follow Us Spiceworks LinkedIn Facebook Twitter Youtube We proudly welcome American Express® Cards Follow Us Spiceworks LinkedIn Facebook Twitter Youtube Follow Us Spiceworks LinkedIn Facebook Twitter Youtube We proudly welcome American Express® Cards We proudly welcome American Express® Cards 1940 E Mariposa Ave El Segundo CA 90245 8007001000© 2016 PCM Sales Inc Entrust Tooltwist 1940 E Mariposa Ave El Segundo CA 90245 8007001000© 2016 PCM Sales Inc Entrust Tooltwist Entrust Tooltwist var gts gts gtspushid 235936 gtspushgooglebasesubaccountid 7846456 gtspushgooglebasecountry US gtspushgooglebaselanguage EN jQuerywindowload function var scheme https documentlocationprotocol https http var gts documentcreateElementscript gtstype textjavascript gtsasync true gtssrc scheme wwwgooglecommercecomtrustedstoresgtmpcompiledjs var s documentgetElementsByTagNamescript0 sparentNodeinsertBeforegts s var gts gts gtspushid 235936 gtspushgooglebasesubaccountid 7846456 gtspushgooglebasecountry US gtspushgooglebaselanguage EN jQuerywindowload function var scheme https documentlocationprotocol https http var gts documentcreateElementscript gtstype textjavascript gtsasync true gtssrc scheme wwwgooglecommercecomtrustedstoresgtmpcompiledjs var s documentgetElementsByTagNamescript0 sparentNodeinsertBeforegts s WELCOME TO PCM Thank you for subscribing to our newsletter Be sure to check your email for exclusive offers and discounts 18007001000 HP 14 G3 QuadCore ChromebookOnly 17999 Shop Now Reach a New Height inBusiness ComputingOnly 34999 Shop Now Save Millions Gain Visibility Take Control Shop Now test Since 1987 PCM has been a leading provider of IT products services solutions to businesses government agencies educational institutions and healthcare facilitiesWe provide access to over 300000 IT products like tablets slate notebooks desktops servers storage and networking from leading manufacturers like Cisco HP Apple Adobe Lenovo and Microsoft With powerful eProcurement tools comprehensive software licensing solutions and dedicated Account Executives its easy to get exactly what you need to tackle your technical challenges Follow Us 1940 E Mariposa Ave El Segundo CA 90245 8007001000© 2016 PCM Sales Inc Menu Follow PCM Blog Spiceworks Facebook LinkedIn Twitter YouTube Sign in Order Status Sign In Register Cart PCM Home STARTUPS ENTREPRENEURS MEDIUM LARGE BUSINESS ENTERPRISE HEALTHCARE GOVERNMENT Home FEDERAL STATE LOCAL EDUCATION HEALTHCARE PCM BUSINESS DIRECT PCM OPSTRACK Solutions Services Cloud Products Cloud Partners Shop Now PCM Hybrid Cloud Learn More Deal of the Week Top Searches Ultrabook Finder Memory Finder InkToner Finder Accessories Cables Computers Memory Monitors Projectors Networking Printers Supplies Racks Power Cooling Scanners Servers Storage All Categories Backup Business Database Desktop Web Publishing Management Operating Systems Security Unified Collaboration Virtualization All Categories Apple Cisco Dell Google HPI HPE Intel Lenovo Microsoft Samsung Symantec VMware All Brands Picking the Right Printer for your Office INFOGRAPHIC January 19 2016 Microsoft Announces Major Change to the Enterprise Agreement Program January 6 2016 How Christmas Gifts Could Impact BYOD January 4 2016 Enhance Your Creativity with Adobe Stock December 30 2015 HP Print Security Seminars Is Your Network at Risk to Hackers December 22 2015 Share Costs and Save Time with Hewlett Packard Enterprise Healthcare December 21 2015 Microsoft Announces that Windows Server 2016 will be Launching Next Quarter December 11 2015 Last Chance to Register for Vision Hollywood December 10 2015 How Big of a Deal is the AppleCisco Partnership December 9 2015 Webcast ShoreTel Truly Unified Communications December 8 2015 Ergotron StyleView Fit for Every Body December 7 2015 The Digital Pulse of Tomorrow’s Healthcare with Lenovo December 7 2015 Deal of the Week Shop Now Lenovo B4080 80F6 Notebook Shop Now Managed Print Services Shop Now Featured Products Bestsellers New Arrivals Trending tablets slate notebooks desktops servers storage networking About Us Blog Brands Careers Certification Authorization Events Executives Investor Relations Locations Privacy Policy RSS Site Map Terms of Use and Sale Why PCM Catalog Subcriptions Contact Us Email Subscriptions Help Topics My Account Order Status Business Direct Employee Purchase Program Leasing Financing OpsTRACK Product Configurator Services Solutions Spiceworks LinkedIn Facebook Twitter Youtube Entrust Tooltwist 18007001000 PCM Blog Spiceworks Facebook LinkedIn Twitter YouTube New account Home Home Picking the Right Printer for your Office INFOGRAPHIC January 19 2016 Microsoft Announces Major Change to the Enterprise Agreement Program January 6 2016 How Christmas Gifts Could Impact BYOD January 4 2016 Enhance Your Creativity with Adobe Stock December 30 2015 HP Print Security Seminars Is Your Network at Risk to Hackers December 22 2015 Share Costs and Save Time with Hewlett Packard Enterprise Healthcare December 21 2015 Microsoft Announces that Windows Server 2016 will be Launching Next Quarter December 11 2015 Last Chance to Register for Vision Hollywood December 10 2015 How Big of a Deal is the AppleCisco Partnership December 9 2015 Webcast ShoreTel Truly Unified Communications December 8 2015 Ergotron StyleView Fit for Every Body December 7 2015 The Digital Pulse of Tomorrow’s Healthcare with Lenovo December 7 2015 Deal of the Week HP 14 G3 QuadCore ChromebookOnly 17999 Lenovo B4080 80F6 Notebook Reach a New Height inBusiness ComputingOnly 34999 Managed Print Services Featured Products Bestsellers New Arrivals Trending Follow Us Spiceworks LinkedIn Facebook Twitter Youtube We proudly welcome American Express® Cards ® 1940 E Mariposa Ave El Segundo CA 90245 8007001000© 2016 PCM Sales Inc 2016 Entrust Tooltwist</v>
       </c>
     </row>
     <row r="8">
@@ -513,16 +465,7 @@
         <v>reseller</v>
       </c>
       <c r="C8" t="str">
-        <v>Academic Superstore : Academic Software discounts for students, teachers and schools Academic edition software discounts for students, teachers and schools. Educational pricing available to college students, k12 students, homeschool students, faculty, universities, educational institutions and parents. Academic Superstore, academic software, academic, academic price, academic discount, academic edition, academic version, student software, student price, student discount, student edition, student version, discount software, educational software, educational price, educational discount, educational edition, teacher software, school software, adobe academic, adobe discounts, microsoft academic, microsoft discounts Shop by Category                  Office &amp; Productivity                               Microsoft Solutions                                            Business &amp; Productivity                                            Business Training                                           Graphics, Art &amp; Design                               Adobe Tools                                            Animation &amp; Modeling                                            Color Management                                            Desktop Publishing                                            Graphics &amp; Illustration                                            Graphics Tablets                                            Web Publishing                                            Design Training                                           Educational Tools                               Art &amp; Music Software                                            Critical Thinking Software                                            Graphing Software                                            Language Arts Software                                            Science Software                                            Social Studies Software                                            Typing Software                                            Classroom Electronics                                            Classroom Learning Aids                                           AntiVirus &amp; Security                               Anti-Virus                                            Content Filtering                                            Firewall &amp; Security                                           CAD &amp; Engineering                               3D Printers                                            Architectural Design                                            CAD &amp; Modeling                                            Map Making/GIS                                            Mechanical Design                                            CAD Training                                           Laptops &amp; Tablets                               Notebook Computers                                            Notebook Accessories                                            Tablets                                            Tablet Accessories                                            Laptop Carts                                            Bags                                           OS &amp; Utilities                               Operating Systems                                            Programming                                            Utilities                                           Music &amp; Video                               Audio Production                                            Digital Video Software                                            DJ Equipment                                            Headphones &amp; Earbuds                                            MIDI Devices                                            Music &amp; Video Training                                            Notation                                            Recording Products                                            Sheet Music &amp; Guitar Tab                                            Video Hardware                                           Electronic Accessories                               Cables                                            Expansion Cards                                            Headphones &amp; Headsets                                            Keyboards &amp; Mice                                            Monitors                                            MP3 &amp; Phone Accessories                                            Networking Products                                            Power Products                                            Printers &amp; Scanners                                            Security Cables                                            Speakers                                            Storage Devices                                            Web Cameras                                              Office &amp; Productivity                               Microsoft Solutions                                            Business &amp; Productivity                                            Business Training                                       Microsoft Solutions                        Business &amp; Productivity                        Business Training                   Graphics, Art &amp; Design                               Adobe Tools                                            Animation &amp; Modeling                                            Color Management                                            Desktop Publishing                                            Graphics &amp; Illustration                                            Graphics Tablets                                            Web Publishing                                            Design Training                                       Adobe Tools                        Animation &amp; Modeling                        Color Management                        Desktop Publishing                        Graphics &amp; Illustration                        Graphics Tablets                        Web Publishing                        Design Training                   Educational Tools                               Art &amp; Music Software                                            Critical Thinking Software                                            Graphing Software                                            Language Arts Software                                            Science Software                                            Social Studies Software                                            Typing Software                                            Classroom Electronics                                            Classroom Learning Aids                                       Art &amp; Music Software                        Critical Thinking Software                        Graphing Software                        Language Arts Software                        Science Software                        Social Studies Software                        Typing Software                        Classroom Electronics                        Classroom Learning Aids                   AntiVirus &amp; Security                               Anti-Virus                                            Content Filtering                                            Firewall &amp; Security                                       Anti-Virus                        Content Filtering                        Firewall &amp; Security                   CAD &amp; Engineering                               3D Printers                                            Architectural Design                                            CAD &amp; Modeling                                            Map Making/GIS                                            Mechanical Design                                            CAD Training                                       3D Printers                        Architectural Design                        CAD &amp; Modeling                        Map Making/GIS                        Mechanical Design                        CAD Training                   Laptops &amp; Tablets                               Notebook Computers                                            Notebook Accessories                                            Tablets                                            Tablet Accessories                                            Laptop Carts                                            Bags                                       Notebook Computers                        Notebook Accessories                        Tablets                        Tablet Accessories                        Laptop Carts                        Bags                   OS &amp; Utilities                               Operating Systems                                            Programming                                            Utilities                                       Operating Systems                        Programming                        Utilities                   Music &amp; Video                               Audio Production                                            Digital Video Software                                            DJ Equipment                                            Headphones &amp; Earbuds                                            MIDI Devices                                            Music &amp; Video Training                                            Notation                                            Recording Products                                            Sheet Music &amp; Guitar Tab                                            Video Hardware                                       Audio Production                        Digital Video Software                        DJ Equipment                        Headphones &amp; Earbuds                        MIDI Devices                        Music &amp; Video Training                        Notation                        Recording Products                        Sheet Music &amp; Guitar Tab                        Video Hardware                   Electronic Accessories                               Cables                                            Expansion Cards                                            Headphones &amp; Headsets                                            Keyboards &amp; Mice                                            Monitors                                            MP3 &amp; Phone Accessories                                            Networking Products                                            Power Products                                            Printers &amp; Scanners                                            Security Cables                                            Speakers                                            Storage Devices                                            Web Cameras                                       Cables                        Expansion Cards                        Headphones &amp; Headsets                        Keyboards &amp; Mice                        Monitors                        MP3 &amp; Phone Accessories                        Networking Products                        Power Products                        Printers &amp; Scanners                        Security Cables                        Speakers                        Storage Devices                        Web Cameras            Shop by Brand                       Adobe Creative CloudAcrobatPhotoshop Elements &amp; Premiere ElementsPhotoshopCaptivatePresenter          Autodesk AutoCAD3ds maxMayaInventorFusion 360RevitSketchBook Pro          Avid Technology Media Composer Pro ToolsSibeliusArtist SeriesPhotoScore and AudioScoreiLok          Corel PainterCorelDRAW Graphics SuiteWordPerfect OfficeCorelDRAW Technical SuitePaintShop ProDazzle VideoVideoStudioToastGame CaptureWinDVDEasy VHS to DVDEasy LP to MP3View all Titles          FileMaker FileMaker ProFileMaker Advanced          Microsoft OfficeOffice for MacintoshKeyboardsWindows ServerTablet Cases/CoversExcelTablet Docking StationsWordVisual StudioSurfaceBeats by Dr. DreIT AcademyView all Titles          Quark QuarkXPress          Sony PS Vita AccessoriesPS3 Accessories          Symantec Norton Hotspot PrivacyNorton Small BusinessNorton UtilitiesNorton Anti-TheftNorton Mobile Security          Toon Boom HarmonyStoryboard Pro    View all 450+ Brands               Adobe Creative CloudAcrobatPhotoshop Elements &amp; Premiere ElementsPhotoshopCaptivatePresenter  Creative Cloud Acrobat Photoshop Elements &amp; Premiere Elements Photoshop Captivate Presenter          Autodesk AutoCAD3ds maxMayaInventorFusion 360RevitSketchBook Pro  AutoCAD 3ds max Maya Inventor Fusion 360 Revit SketchBook Pro          Avid Technology Media Composer Pro ToolsSibeliusArtist SeriesPhotoScore and AudioScoreiLok  Media Composer  Pro Tools Sibelius Artist Series PhotoScore and AudioScore iLok          Corel PainterCorelDRAW Graphics SuiteWordPerfect OfficeCorelDRAW Technical SuitePaintShop ProDazzle VideoVideoStudioToastGame CaptureWinDVDEasy VHS to DVDEasy LP to MP3View all Titles  Painter CorelDRAW Graphics Suite WordPerfect Office CorelDRAW Technical Suite PaintShop Pro Dazzle Video VideoStudio Toast Game Capture WinDVD Easy VHS to DVD Easy LP to MP3 View all Titles          FileMaker FileMaker ProFileMaker Advanced  FileMaker Pro FileMaker Advanced          Microsoft OfficeOffice for MacintoshKeyboardsWindows ServerTablet Cases/CoversExcelTablet Docking StationsWordVisual StudioSurfaceBeats by Dr. DreIT AcademyView all Titles  Office Office for Macintosh Keyboards Windows Server Tablet Cases/Covers Excel Tablet Docking Stations Word Visual Studio Surface Beats by Dr. Dre IT Academy View all Titles          Quark QuarkXPress  QuarkXPress          Sony PS Vita AccessoriesPS3 Accessories  PS Vita Accessories PS3 Accessories          Symantec Norton Hotspot PrivacyNorton Small BusinessNorton UtilitiesNorton Anti-TheftNorton Mobile Security  Norton Hotspot Privacy Norton Small Business Norton Utilities Norton Anti-Theft Norton Mobile Security          Toon Boom HarmonyStoryboard Pro  Harmony Storyboard Pro View all 450+ Brands School Services                            School Services                         Get a Quote      School Services Get a Quote    Instant Online Verification          Dated Student ID from the current semester or school year          Course Schedule          Registration Receipt for this semester          Letter of Enrollment on school letterhead.          Report Card          Dated Student ID from the current semester or school year          Registration Receipt          Letter of Enrollment on school letterhead          Link to your faculty web page          Current Faculty ID          Letter of Employment on school letterhead          Pay Stub (cross out confidential information)          Membership in Home School Association          Receipt for Home School Curriculum          Letter of intent to home school from a state agency       Your Purchase Order    Copy of IRS 501(c)3 form          IRS letter stating that you are a 501(c)3        FAQ  Contact Us  800.876.3507 Privacy Policy Terms &amp; Conditions About Us                 Office &amp; Productivity Microsoft Solutions Business &amp; Productivity Business Training Graphics, Art &amp; Design Adobe Tools Animation &amp; Modeling Color Management Desktop Publishing Graphics &amp; Illustration Graphics Tablets Web Publishing Design Training Educational Tools Art &amp; Music Software Critical Thinking Software Graphing Software Language Arts Software Science Software Social Studies Software Typing Software Classroom Electronics Classroom Learning Aids AntiVirus &amp; Security Anti-Virus Content Filtering Firewall &amp; Security CAD &amp; Engineering 3D Printers Architectural Design CAD &amp; Modeling Map Making/GIS Mechanical Design CAD Training Laptops &amp; Tablets Notebook Computers Notebook Accessories Tablets Tablet Accessories Laptop Carts Bags OS &amp; Utilities Operating Systems Programming Utilities Music &amp; Video Audio Production Digital Video Software DJ Equipment Headphones &amp; Earbuds MIDI Devices Music &amp; Video Training Notation Recording Products Sheet Music &amp; Guitar Tab Video Hardware Electronic Accessories Cables Expansion Cards Headphones &amp; Headsets Keyboards &amp; Mice Monitors MP3 &amp; Phone Accessories Networking Products Power Products Printers &amp; Scanners Security Cables Speakers Storage Devices Web Cameras Adobe Creative Cloud Acrobat Photoshop Elements &amp; Premiere Elements Photoshop Captivate Presenter Autodesk AutoCAD 3ds max Maya Inventor Fusion 360 Revit SketchBook Pro Avid Technology Media Composer  Pro Tools Sibelius Artist Series PhotoScore and AudioScore iLok Corel Painter CorelDRAW Graphics Suite WordPerfect Office CorelDRAW Technical Suite PaintShop Pro Dazzle Video VideoStudio Toast Game Capture WinDVD Easy VHS to DVD Easy LP to MP3 View all Titles FileMaker FileMaker Pro FileMaker Advanced Microsoft Office Office for Macintosh Keyboards Windows Server Tablet Cases/Covers Excel Tablet Docking Stations Word Visual Studio Surface Beats by Dr. Dre IT Academy View all Titles Quark QuarkXPress Sony PS Vita Accessories PS3 Accessories Symantec Norton Hotspot Privacy Norton Small Business Norton Utilities Norton Anti-Theft Norton Mobile Security Toon Boom Harmony Storyboard Pro View all 450+ Brands School Services School Services Get a Quote My Account   Office &amp; Productivity Graphics, Art &amp; Design Educational Tools AntiVirus &amp; Security CAD &amp; Engineering Laptops &amp; Tablets OS &amp; Utilities Music &amp; Video Electronic Accessories  FAQ  Contact Us  800.876.3507 Privacy Policy Terms &amp; Conditions About Us     Sign Up For Special Offers    (cross out confidential information) Microsoft Office, Adobe Acrobat, SPSS... Creative Cloud, Photoshop, Wacom... Rosetta Stone, LeapFrog, Inspiration... Symantec, ESET, Kaspersky... Autodesk, SolidWorks, TurboCAD... Microsoft Surface, HP, Dell... Windows, TechSmith, WinZip... Pro Tools, After Effects, Sibelius... Displays, Graphics Tablets, Harddrives... find, follow &amp; friend us for exclusive deals &amp; discounts</v>
-      </c>
-      <c r="D8" t="str">
-        <v>Academic Superstore : Academic Software discounts for students, teachers and schools Academic edition software discounts for students, teachers and schools. Educational pricing available to college students, k12 students, homeschool students, faculty, universities, educational institutions and parents. Academic Superstore, academic software, academic, academic price, academic discount, academic edition, academic version, student software, student price, student discount, student edition, student version, discount software, educational software, educational price, educational discount, educational edition, teacher software, school software, adobe academic, adobe discounts, microsoft academic, microsoft discounts Shop by Category                  Office &amp; Productivity                               Microsoft Solutions                                            Business &amp; Productivity                                            Business Training                                           Graphics, Art &amp; Design                               Adobe Tools                                            Animation &amp; Modeling                                            Color Management                                            Desktop Publishing                                            Graphics &amp; Illustration                                            Graphics Tablets                                            Web Publishing                                            Design Training                                           Educational Tools                               Art &amp; Music Software                                            Critical Thinking Software                                            Graphing Software                                            Language Arts Software                                            Science Software                                            Social Studies Software                                            Typing Software                                            Classroom Electronics                                            Classroom Learning Aids                                           AntiVirus &amp; Security                               Anti-Virus                                            Content Filtering                                            Firewall &amp; Security                                           CAD &amp; Engineering                               3D Printers                                            Architectural Design                                            CAD &amp; Modeling                                            Map Making/GIS                                            Mechanical Design                                            CAD Training                                           Laptops &amp; Tablets                               Notebook Computers                                            Notebook Accessories                                            Tablets                                            Tablet Accessories                                            Laptop Carts                                            Bags                                           OS &amp; Utilities                               Operating Systems                                            Programming                                            Utilities                                           Music &amp; Video                               Audio Production                                            Digital Video Software                                            DJ Equipment                                            Headphones &amp; Earbuds                                            MIDI Devices                                            Music &amp; Video Training                                            Notation                                            Recording Products                                            Sheet Music &amp; Guitar Tab                                            Video Hardware                                           Electronic Accessories                               Cables                                            Expansion Cards                                            Headphones &amp; Headsets                                            Keyboards &amp; Mice                                            Monitors                                            MP3 &amp; Phone Accessories                                            Networking Products                                            Power Products                                            Printers &amp; Scanners                                            Security Cables                                            Speakers                                            Storage Devices                                            Web Cameras                                              Office &amp; Productivity                               Microsoft Solutions                                            Business &amp; Productivity                                            Business Training                                       Microsoft Solutions                        Business &amp; Productivity                        Business Training                   Graphics, Art &amp; Design                               Adobe Tools                                            Animation &amp; Modeling                                            Color Management                                            Desktop Publishing                                            Graphics &amp; Illustration                                            Graphics Tablets                                            Web Publishing                                            Design Training                                       Adobe Tools                        Animation &amp; Modeling                        Color Management                        Desktop Publishing                        Graphics &amp; Illustration                        Graphics Tablets                        Web Publishing                        Design Training                   Educational Tools                               Art &amp; Music Software                                            Critical Thinking Software                                            Graphing Software                                            Language Arts Software                                            Science Software                                            Social Studies Software                                            Typing Software                                            Classroom Electronics                                            Classroom Learning Aids                                       Art &amp; Music Software                        Critical Thinking Software                        Graphing Software                        Language Arts Software                        Science Software                        Social Studies Software                        Typing Software                        Classroom Electronics                        Classroom Learning Aids                   AntiVirus &amp; Security                               Anti-Virus                                            Content Filtering                                            Firewall &amp; Security                                       Anti-Virus                        Content Filtering                        Firewall &amp; Security                   CAD &amp; Engineering                               3D Printers                                            Architectural Design                                            CAD &amp; Modeling                                            Map Making/GIS                                            Mechanical Design                                            CAD Training                                       3D Printers                        Architectural Design                        CAD &amp; Modeling                        Map Making/GIS                        Mechanical Design                        CAD Training                   Laptops &amp; Tablets                               Notebook Computers                                            Notebook Accessories                                            Tablets                                            Tablet Accessories                                            Laptop Carts                                            Bags                                       Notebook Computers                        Notebook Accessories                        Tablets                        Tablet Accessories                        Laptop Carts                        Bags                   OS &amp; Utilities                               Operating Systems                                            Programming                                            Utilities                                       Operating Systems                        Programming                        Utilities                   Music &amp; Video                               Audio Production                                            Digital Video Software                                            DJ Equipment                                            Headphones &amp; Earbuds                                            MIDI Devices                                            Music &amp; Video Training                                            Notation                                            Recording Products                                            Sheet Music &amp; Guitar Tab                                            Video Hardware                                       Audio Production                        Digital Video Software                        DJ Equipment                        Headphones &amp; Earbuds                        MIDI Devices                        Music &amp; Video Training                        Notation                        Recording Products                        Sheet Music &amp; Guitar Tab                        Video Hardware                   Electronic Accessories                               Cables                                            Expansion Cards                                            Headphones &amp; Headsets                                            Keyboards &amp; Mice                                            Monitors                                            MP3 &amp; Phone Accessories                                            Networking Products                                            Power Products                                            Printers &amp; Scanners                                            Security Cables                                            Speakers                                            Storage Devices                                            Web Cameras                                       Cables                        Expansion Cards                        Headphones &amp; Headsets                        Keyboards &amp; Mice                        Monitors                        MP3 &amp; Phone Accessories                        Networking Products                        Power Products                        Printers &amp; Scanners                        Security Cables                        Speakers                        Storage Devices                        Web Cameras            Shop by Brand                       Adobe Creative CloudAcrobatPhotoshop Elements &amp; Premiere ElementsPhotoshopCaptivatePresenter          Autodesk AutoCAD3ds maxMayaInventorFusion 360RevitSketchBook Pro          Avid Technology Media Composer Pro ToolsSibeliusArtist SeriesPhotoScore and AudioScoreiLok          Corel PainterCorelDRAW Graphics SuiteWordPerfect OfficeCorelDRAW Technical SuitePaintShop ProDazzle VideoVideoStudioToastGame CaptureWinDVDEasy VHS to DVDEasy LP to MP3View all Titles          FileMaker FileMaker ProFileMaker Advanced          Microsoft OfficeOffice for MacintoshKeyboardsWindows ServerTablet Cases/CoversExcelTablet Docking StationsWordVisual StudioSurfaceBeats by Dr. DreIT AcademyView all Titles          Quark QuarkXPress          Sony PS Vita AccessoriesPS3 Accessories          Symantec Norton Hotspot PrivacyNorton Small BusinessNorton UtilitiesNorton Anti-TheftNorton Mobile Security          Toon Boom HarmonyStoryboard Pro    View all 450+ Brands               Adobe Creative CloudAcrobatPhotoshop Elements &amp; Premiere ElementsPhotoshopCaptivatePresenter  Creative Cloud Acrobat Photoshop Elements &amp; Premiere Elements Photoshop Captivate Presenter          Autodesk AutoCAD3ds maxMayaInventorFusion 360RevitSketchBook Pro  AutoCAD 3ds max Maya Inventor Fusion 360 Revit SketchBook Pro          Avid Technology Media Composer Pro ToolsSibeliusArtist SeriesPhotoScore and AudioScoreiLok  Media Composer  Pro Tools Sibelius Artist Series PhotoScore and AudioScore iLok          Corel PainterCorelDRAW Graphics SuiteWordPerfect OfficeCorelDRAW Technical SuitePaintShop ProDazzle VideoVideoStudioToastGame CaptureWinDVDEasy VHS to DVDEasy LP to MP3View all Titles  Painter CorelDRAW Graphics Suite WordPerfect Office CorelDRAW Technical Suite PaintShop Pro Dazzle Video VideoStudio Toast Game Capture WinDVD Easy VHS to DVD Easy LP to MP3 View all Titles          FileMaker FileMaker ProFileMaker Advanced  FileMaker Pro FileMaker Advanced          Microsoft OfficeOffice for MacintoshKeyboardsWindows ServerTablet Cases/CoversExcelTablet Docking StationsWordVisual StudioSurfaceBeats by Dr. DreIT AcademyView all Titles  Office Office for Macintosh Keyboards Windows Server Tablet Cases/Covers Excel Tablet Docking Stations Word Visual Studio Surface Beats by Dr. Dre IT Academy View all Titles          Quark QuarkXPress  QuarkXPress          Sony PS Vita AccessoriesPS3 Accessories  PS Vita Accessories PS3 Accessories          Symantec Norton Hotspot PrivacyNorton Small BusinessNorton UtilitiesNorton Anti-TheftNorton Mobile Security  Norton Hotspot Privacy Norton Small Business Norton Utilities Norton Anti-Theft Norton Mobile Security          Toon Boom HarmonyStoryboard Pro  Harmony Storyboard Pro View all 450+ Brands School Services                            School Services                         Get a Quote      School Services Get a Quote    Instant Online Verification          Dated Student ID from the current semester or school year          Course Schedule          Registration Receipt for this semester          Letter of Enrollment on school letterhead.          Report Card          Dated Student ID from the current semester or school year          Registration Receipt          Letter of Enrollment on school letterhead          Link to your faculty web page          Current Faculty ID          Letter of Employment on school letterhead          Pay Stub (cross out confidential information)          Membership in Home School Association          Receipt for Home School Curriculum          Letter of intent to home school from a state agency       Your Purchase Order    Copy of IRS 501(c)3 form          IRS letter stating that you are a 501(c)3        FAQ  Contact Us  800.876.3507 Privacy Policy Terms &amp; Conditions About Us                 Office &amp; Productivity Microsoft Solutions Business &amp; Productivity Business Training Graphics, Art &amp; Design Adobe Tools Animation &amp; Modeling Color Management Desktop Publishing Graphics &amp; Illustration Graphics Tablets Web Publishing Design Training Educational Tools Art &amp; Music Software Critical Thinking Software Graphing Software Language Arts Software Science Software Social Studies Software Typing Software Classroom Electronics Classroom Learning Aids AntiVirus &amp; Security Anti-Virus Content Filtering Firewall &amp; Security CAD &amp; Engineering 3D Printers Architectural Design CAD &amp; Modeling Map Making/GIS Mechanical Design CAD Training Laptops &amp; Tablets Notebook Computers Notebook Accessories Tablets Tablet Accessories Laptop Carts Bags OS &amp; Utilities Operating Systems Programming Utilities Music &amp; Video Audio Production Digital Video Software DJ Equipment Headphones &amp; Earbuds MIDI Devices Music &amp; Video Training Notation Recording Products Sheet Music &amp; Guitar Tab Video Hardware Electronic Accessories Cables Expansion Cards Headphones &amp; Headsets Keyboards &amp; Mice Monitors MP3 &amp; Phone Accessories Networking Products Power Products Printers &amp; Scanners Security Cables Speakers Storage Devices Web Cameras Adobe Creative Cloud Acrobat Photoshop Elements &amp; Premiere Elements Photoshop Captivate Presenter Autodesk AutoCAD 3ds max Maya Inventor Fusion 360 Revit SketchBook Pro Avid Technology Media Composer  Pro Tools Sibelius Artist Series PhotoScore and AudioScore iLok Corel Painter CorelDRAW Graphics Suite WordPerfect Office CorelDRAW Technical Suite PaintShop Pro Dazzle Video VideoStudio Toast Game Capture WinDVD Easy VHS to DVD Easy LP to MP3 View all Titles FileMaker FileMaker Pro FileMaker Advanced Microsoft Office Office for Macintosh Keyboards Windows Server Tablet Cases/Covers Excel Tablet Docking Stations Word Visual Studio Surface Beats by Dr. Dre IT Academy View all Titles Quark QuarkXPress Sony PS Vita Accessories PS3 Accessories Symantec Norton Hotspot Privacy Norton Small Business Norton Utilities Norton Anti-Theft Norton Mobile Security Toon Boom Harmony Storyboard Pro View all 450+ Brands School Services School Services Get a Quote My Account   Office &amp; Productivity Graphics, Art &amp; Design Educational Tools AntiVirus &amp; Security CAD &amp; Engineering Laptops &amp; Tablets OS &amp; Utilities Music &amp; Video Electronic Accessories  FAQ  Contact Us  800.876.3507 Privacy Policy Terms &amp; Conditions About Us     Sign Up For Special Offers    (cross out confidential information) Microsoft Office, Adobe Acrobat, SPSS... Creative Cloud, Photoshop, Wacom... Rosetta Stone, LeapFrog, Inspiration... Symantec, ESET, Kaspersky... Autodesk, SolidWorks, TurboCAD... Microsoft Surface, HP, Dell... Windows, TechSmith, WinZip... Pro Tools, After Effects, Sibelius... Displays, Graphics Tablets, Harddrives... find, follow &amp; friend us for exclusive deals &amp; discounts</v>
-      </c>
-      <c r="E8" t="str">
-        <v>Academic Superstore : Academic Software discounts for students, teachers and schools Academic edition software discounts for students, teachers and schools. Educational pricing available to college students, k12 students, homeschool students, faculty, universities, educational institutions and parents. Academic Superstore, academic software, academic, academic price, academic discount, academic edition, academic version, student software, student price, student discount, student edition, student version, discount software, educational software, educational price, educational discount, educational edition, teacher software, school software, adobe academic, adobe discounts, microsoft academic, microsoft discounts Shop by Category                  Office &amp; Productivity                               Microsoft Solutions                                            Business &amp; Productivity                                            Business Training                                           Graphics, Art &amp; Design                               Adobe Tools                                            Animation &amp; Modeling                                            Color Management                                            Desktop Publishing                                            Graphics &amp; Illustration                                            Graphics Tablets                                            Web Publishing                                            Design Training                                           Educational Tools                               Art &amp; Music Software                                            Critical Thinking Software                                            Graphing Software                                            Language Arts Software                                            Science Software                                            Social Studies Software                                            Typing Software                                            Classroom Electronics                                            Classroom Learning Aids                                           AntiVirus &amp; Security                               Anti-Virus                                            Content Filtering                                            Firewall &amp; Security                                           CAD &amp; Engineering                               3D Printers                                            Architectural Design                                            CAD &amp; Modeling                                            Map Making/GIS                                            Mechanical Design                                            CAD Training                                           Laptops &amp; Tablets                               Notebook Computers                                            Notebook Accessories                                            Tablets                                            Tablet Accessories                                            Laptop Carts                                            Bags                                           OS &amp; Utilities                               Operating Systems                                            Programming                                            Utilities                                           Music &amp; Video                               Audio Production                                            Digital Video Software                                            DJ Equipment                                            Headphones &amp; Earbuds                                            MIDI Devices                                            Music &amp; Video Training                                            Notation                                            Recording Products                                            Sheet Music &amp; Guitar Tab                                            Video Hardware                                           Electronic Accessories                               Cables                                            Expansion Cards                                            Headphones &amp; Headsets                                            Keyboards &amp; Mice                                            Monitors                                            MP3 &amp; Phone Accessories                                            Networking Products                                            Power Products                                            Printers &amp; Scanners                                            Security Cables                                            Speakers                                            Storage Devices                                            Web Cameras                                              Office &amp; Productivity                               Microsoft Solutions                                            Business &amp; Productivity                                            Business Training                                       Microsoft Solutions                        Business &amp; Productivity                        Business Training                   Graphics, Art &amp; Design                               Adobe Tools                                            Animation &amp; Modeling                                            Color Management                                            Desktop Publishing                                            Graphics &amp; Illustration                                            Graphics Tablets                                            Web Publishing                                            Design Training                                       Adobe Tools                        Animation &amp; Modeling                        Color Management                        Desktop Publishing                        Graphics &amp; Illustration                        Graphics Tablets                        Web Publishing                        Design Training                   Educational Tools                               Art &amp; Music Software                                            Critical Thinking Software                                            Graphing Software                                            Language Arts Software                                            Science Software                                            Social Studies Software                                            Typing Software                                            Classroom Electronics                                            Classroom Learning Aids                                       Art &amp; Music Software                        Critical Thinking Software                        Graphing Software                        Language Arts Software                        Science Software                        Social Studies Software                        Typing Software                        Classroom Electronics                        Classroom Learning Aids                   AntiVirus &amp; Security                               Anti-Virus                                            Content Filtering                                            Firewall &amp; Security                                       Anti-Virus                        Content Filtering                        Firewall &amp; Security                   CAD &amp; Engineering                               3D Printers                                            Architectural Design                                            CAD &amp; Modeling                                            Map Making/GIS                                            Mechanical Design                                            CAD Training                                       3D Printers                        Architectural Design                        CAD &amp; Modeling                        Map Making/GIS                        Mechanical Design                        CAD Training                   Laptops &amp; Tablets                               Notebook Computers                                            Notebook Accessories                                            Tablets                                            Tablet Accessories                                            Laptop Carts                                            Bags                                       Notebook Computers                        Notebook Accessories                        Tablets                        Tablet Accessories                        Laptop Carts                        Bags                   OS &amp; Utilities                               Operating Systems                                            Programming                                            Utilities                                       Operating Systems                        Programming                        Utilities                   Music &amp; Video                               Audio Production                                            Digital Video Software                                            DJ Equipment                                            Headphones &amp; Earbuds                                            MIDI Devices                                            Music &amp; Video Training                                            Notation                                            Recording Products                                            Sheet Music &amp; Guitar Tab                                            Video Hardware                                       Audio Production                        Digital Video Software                        DJ Equipment                        Headphones &amp; Earbuds                        MIDI Devices                        Music &amp; Video Training                        Notation                        Recording Products                        Sheet Music &amp; Guitar Tab                        Video Hardware                   Electronic Accessories                               Cables                                            Expansion Cards                                            Headphones &amp; Headsets                                            Keyboards &amp; Mice                                            Monitors                                            MP3 &amp; Phone Accessories                                            Networking Products                                            Power Products                                            Printers &amp; Scanners                                            Security Cables                                            Speakers                                            Storage Devices                                            Web Cameras                                       Cables                        Expansion Cards                        Headphones &amp; Headsets                        Keyboards &amp; Mice                        Monitors                        MP3 &amp; Phone Accessories                        Networking Products                        Power Products                        Printers &amp; Scanners                        Security Cables                        Speakers                        Storage Devices                        Web Cameras            Shop by Brand                       Adobe Creative CloudAcrobatPhotoshop Elements &amp; Premiere ElementsPhotoshopCaptivatePresenter          Autodesk AutoCAD3ds maxMayaInventorFusion 360RevitSketchBook Pro          Avid Technology Media Composer Pro ToolsSibeliusArtist SeriesPhotoScore and AudioScoreiLok          Corel PainterCorelDRAW Graphics SuiteWordPerfect OfficeCorelDRAW Technical SuitePaintShop ProDazzle VideoVideoStudioToastGame CaptureWinDVDEasy VHS to DVDEasy LP to MP3View all Titles          FileMaker FileMaker ProFileMaker Advanced          Microsoft OfficeOffice for MacintoshKeyboardsWindows ServerTablet Cases/CoversExcelTablet Docking StationsWordVisual StudioSurfaceBeats by Dr. DreIT AcademyView all Titles          Quark QuarkXPress          Sony PS Vita AccessoriesPS3 Accessories          Symantec Norton Hotspot PrivacyNorton Small BusinessNorton UtilitiesNorton Anti-TheftNorton Mobile Security          Toon Boom HarmonyStoryboard Pro    View all 450+ Brands               Adobe Creative CloudAcrobatPhotoshop Elements &amp; Premiere ElementsPhotoshopCaptivatePresenter  Creative Cloud Acrobat Photoshop Elements &amp; Premiere Elements Photoshop Captivate Presenter          Autodesk AutoCAD3ds maxMayaInventorFusion 360RevitSketchBook Pro  AutoCAD 3ds max Maya Inventor Fusion 360 Revit SketchBook Pro          Avid Technology Media Composer Pro ToolsSibeliusArtist SeriesPhotoScore and AudioScoreiLok  Media Composer  Pro Tools Sibelius Artist Series PhotoScore and AudioScore iLok          Corel PainterCorelDRAW Graphics SuiteWordPerfect OfficeCorelDRAW Technical SuitePaintShop ProDazzle VideoVideoStudioToastGame CaptureWinDVDEasy VHS to DVDEasy LP to MP3View all Titles  Painter CorelDRAW Graphics Suite WordPerfect Office CorelDRAW Technical Suite PaintShop Pro Dazzle Video VideoStudio Toast Game Capture WinDVD Easy VHS to DVD Easy LP to MP3 View all Titles          FileMaker FileMaker ProFileMaker Advanced  FileMaker Pro FileMaker Advanced          Microsoft OfficeOffice for MacintoshKeyboardsWindows ServerTablet Cases/CoversExcelTablet Docking StationsWordVisual StudioSurfaceBeats by Dr. DreIT AcademyView all Titles  Office Office for Macintosh Keyboards Windows Server Tablet Cases/Covers Excel Tablet Docking Stations Word Visual Studio Surface Beats by Dr. Dre IT Academy View all Titles          Quark QuarkXPress  QuarkXPress          Sony PS Vita AccessoriesPS3 Accessories  PS Vita Accessories PS3 Accessories          Symantec Norton Hotspot PrivacyNorton Small BusinessNorton UtilitiesNorton Anti-TheftNorton Mobile Security  Norton Hotspot Privacy Norton Small Business Norton Utilities Norton Anti-Theft Norton Mobile Security          Toon Boom HarmonyStoryboard Pro  Harmony Storyboard Pro View all 450+ Brands School Services                            School Services                         Get a Quote      School Services Get a Quote    Instant Online Verification          Dated Student ID from the current semester or school year          Course Schedule          Registration Receipt for this semester          Letter of Enrollment on school letterhead.          Report Card          Dated Student ID from the current semester or school year          Registration Receipt          Letter of Enrollment on school letterhead          Link to your faculty web page          Current Faculty ID          Letter of Employment on school letterhead          Pay Stub (cross out confidential information)          Membership in Home School Association          Receipt for Home School Curriculum          Letter of intent to home school from a state agency       Your Purchase Order    Copy of IRS 501(c)3 form          IRS letter stating that you are a 501(c)3        FAQ  Contact Us  800.876.3507 Privacy Policy Terms &amp; Conditions About Us                 Office &amp; Productivity Microsoft Solutions Business &amp; Productivity Business Training Graphics, Art &amp; Design Adobe Tools Animation &amp; Modeling Color Management Desktop Publishing Graphics &amp; Illustration Graphics Tablets Web Publishing Design Training Educational Tools Art &amp; Music Software Critical Thinking Software Graphing Software Language Arts Software Science Software Social Studies Software Typing Software Classroom Electronics Classroom Learning Aids AntiVirus &amp; Security Anti-Virus Content Filtering Firewall &amp; Security CAD &amp; Engineering 3D Printers Architectural Design CAD &amp; Modeling Map Making/GIS Mechanical Design CAD Training Laptops &amp; Tablets Notebook Computers Notebook Accessories Tablets Tablet Accessories Laptop Carts Bags OS &amp; Utilities Operating Systems Programming Utilities Music &amp; Video Audio Production Digital Video Software DJ Equipment Headphones &amp; Earbuds MIDI Devices Music &amp; Video Training Notation Recording Products Sheet Music &amp; Guitar Tab Video Hardware Electronic Accessories Cables Expansion Cards Headphones &amp; Headsets Keyboards &amp; Mice Monitors MP3 &amp; Phone Accessories Networking Products Power Products Printers &amp; Scanners Security Cables Speakers Storage Devices Web Cameras Adobe Creative Cloud Acrobat Photoshop Elements &amp; Premiere Elements Photoshop Captivate Presenter Autodesk AutoCAD 3ds max Maya Inventor Fusion 360 Revit SketchBook Pro Avid Technology Media Composer  Pro Tools Sibelius Artist Series PhotoScore and AudioScore iLok Corel Painter CorelDRAW Graphics Suite WordPerfect Office CorelDRAW Technical Suite PaintShop Pro Dazzle Video VideoStudio Toast Game Capture WinDVD Easy VHS to DVD Easy LP to MP3 View all Titles FileMaker FileMaker Pro FileMaker Advanced Microsoft Office Office for Macintosh Keyboards Windows Server Tablet Cases/Covers Excel Tablet Docking Stations Word Visual Studio Surface Beats by Dr. Dre IT Academy View all Titles Quark QuarkXPress Sony PS Vita Accessories PS3 Accessories Symantec Norton Hotspot Privacy Norton Small Business Norton Utilities Norton Anti-Theft Norton Mobile Security Toon Boom Harmony Storyboard Pro View all 450+ Brands School Services School Services Get a Quote My Account   Office &amp; Productivity Graphics, Art &amp; Design Educational Tools AntiVirus &amp; Security CAD &amp; Engineering Laptops &amp; Tablets OS &amp; Utilities Music &amp; Video Electronic Accessories  FAQ  Contact Us  800.876.3507 Privacy Policy Terms &amp; Conditions About Us     Sign Up For Special Offers    (cross out confidential information) Microsoft Office, Adobe Acrobat, SPSS... Creative Cloud, Photoshop, Wacom... Rosetta Stone, LeapFrog, Inspiration... Symantec, ESET, Kaspersky... Autodesk, SolidWorks, TurboCAD... Microsoft Surface, HP, Dell... Windows, TechSmith, WinZip... Pro Tools, After Effects, Sibelius... Displays, Graphics Tablets, Harddrives... find, follow &amp; friend us for exclusive deals &amp; discounts</v>
-      </c>
-      <c r="F8" t="str">
-        <v>Academic Superstore : Academic Software discounts for students, teachers and schools Academic edition software discounts for students, teachers and schools. Educational pricing available to college students, k12 students, homeschool students, faculty, universities, educational institutions and parents. Academic Superstore, academic software, academic, academic price, academic discount, academic edition, academic version, student software, student price, student discount, student edition, student version, discount software, educational software, educational price, educational discount, educational edition, teacher software, school software, adobe academic, adobe discounts, microsoft academic, microsoft discounts Shop by Category                  Office &amp; Productivity                               Microsoft Solutions                                            Business &amp; Productivity                                            Business Training                                           Graphics, Art &amp; Design                               Adobe Tools                                            Animation &amp; Modeling                                            Color Management                                            Desktop Publishing                                            Graphics &amp; Illustration                                            Graphics Tablets                                            Web Publishing                                            Design Training                                           Educational Tools                               Art &amp; Music Software                                            Critical Thinking Software                                            Graphing Software                                            Language Arts Software                                            Science Software                                            Social Studies Software                                            Typing Software                                            Classroom Electronics                                            Classroom Learning Aids                                           AntiVirus &amp; Security                               Anti-Virus                                            Content Filtering                                            Firewall &amp; Security                                           CAD &amp; Engineering                               3D Printers                                            Architectural Design                                            CAD &amp; Modeling                                            Map Making/GIS                                            Mechanical Design                                            CAD Training                                           Laptops &amp; Tablets                               Notebook Computers                                            Notebook Accessories                                            Tablets                                            Tablet Accessories                                            Laptop Carts                                            Bags                                           OS &amp; Utilities                               Operating Systems                                            Programming                                            Utilities                                           Music &amp; Video                               Audio Production                                            Digital Video Software                                            DJ Equipment                                            Headphones &amp; Earbuds                                            MIDI Devices                                            Music &amp; Video Training                                            Notation                                            Recording Products                                            Sheet Music &amp; Guitar Tab                                            Video Hardware                                           Electronic Accessories                               Cables                                            Expansion Cards                                            Headphones &amp; Headsets                                            Keyboards &amp; Mice                                            Monitors                                            MP3 &amp; Phone Accessories                                            Networking Products                                            Power Products                                            Printers &amp; Scanners                                            Security Cables                                            Speakers                                            Storage Devices                                            Web Cameras                                              Office &amp; Productivity                               Microsoft Solutions                                            Business &amp; Productivity                                            Business Training                                       Microsoft Solutions                        Business &amp; Productivity                        Business Training                   Graphics, Art &amp; Design                               Adobe Tools                                            Animation &amp; Modeling                                            Color Management                                            Desktop Publishing                                            Graphics &amp; Illustration                                            Graphics Tablets                                            Web Publishing                                            Design Training                                       Adobe Tools                        Animation &amp; Modeling                        Color Management                        Desktop Publishing                        Graphics &amp; Illustration                        Graphics Tablets                        Web Publishing                        Design Training                   Educational Tools                               Art &amp; Music Software                                            Critical Thinking Software                                            Graphing Software                                            Language Arts Software                                            Science Software                                            Social Studies Software                                            Typing Software                                            Classroom Electronics                                            Classroom Learning Aids                                       Art &amp; Music Software                        Critical Thinking Software                        Graphing Software                        Language Arts Software                        Science Software                        Social Studies Software                        Typing Software                        Classroom Electronics                        Classroom Learning Aids                   AntiVirus &amp; Security                               Anti-Virus                                            Content Filtering                                            Firewall &amp; Security                                       Anti-Virus                        Content Filtering                        Firewall &amp; Security                   CAD &amp; Engineering                               3D Printers                                            Architectural Design                                            CAD &amp; Modeling                                            Map Making/GIS                                            Mechanical Design                                            CAD Training                                       3D Printers                        Architectural Design                        CAD &amp; Modeling                        Map Making/GIS                        Mechanical Design                        CAD Training                   Laptops &amp; Tablets                               Notebook Computers                                            Notebook Accessories                                            Tablets                                            Tablet Accessories                                            Laptop Carts                                            Bags                                       Notebook Computers                        Notebook Accessories                        Tablets                        Tablet Accessories                        Laptop Carts                        Bags                   OS &amp; Utilities                               Operating Systems                                            Programming                                            Utilities                                       Operating Systems                        Programming                        Utilities                   Music &amp; Video                               Audio Production                                            Digital Video Software                                            DJ Equipment                                            Headphones &amp; Earbuds                                            MIDI Devices                                            Music &amp; Video Training                                            Notation                                            Recording Products                                            Sheet Music &amp; Guitar Tab                                            Video Hardware                                       Audio Production                        Digital Video Software                        DJ Equipment                        Headphones &amp; Earbuds                        MIDI Devices                        Music &amp; Video Training                        Notation                        Recording Products                        Sheet Music &amp; Guitar Tab                        Video Hardware                   Electronic Accessories                               Cables                                            Expansion Cards                                            Headphones &amp; Headsets                                            Keyboards &amp; Mice                                            Monitors                                            MP3 &amp; Phone Accessories                                            Networking Products                                            Power Products                                            Printers &amp; Scanners                                            Security Cables                                            Speakers                                            Storage Devices                                            Web Cameras                                       Cables                        Expansion Cards                        Headphones &amp; Headsets                        Keyboards &amp; Mice                        Monitors                        MP3 &amp; Phone Accessories                        Networking Products                        Power Products                        Printers &amp; Scanners                        Security Cables                        Speakers                        Storage Devices                        Web Cameras            Shop by Brand                       Adobe Creative CloudAcrobatPhotoshop Elements &amp; Premiere ElementsPhotoshopCaptivatePresenter          Autodesk AutoCAD3ds maxMayaInventorFusion 360RevitSketchBook Pro          Avid Technology Media Composer Pro ToolsSibeliusArtist SeriesPhotoScore and AudioScoreiLok          Corel PainterCorelDRAW Graphics SuiteWordPerfect OfficeCorelDRAW Technical SuitePaintShop ProDazzle VideoVideoStudioToastGame CaptureWinDVDEasy VHS to DVDEasy LP to MP3View all Titles          FileMaker FileMaker ProFileMaker Advanced          Microsoft OfficeOffice for MacintoshKeyboardsWindows ServerTablet Cases/CoversExcelTablet Docking StationsWordVisual StudioSurfaceBeats by Dr. DreIT AcademyView all Titles          Quark QuarkXPress          Sony PS Vita AccessoriesPS3 Accessories          Symantec Norton Hotspot PrivacyNorton Small BusinessNorton UtilitiesNorton Anti-TheftNorton Mobile Security          Toon Boom HarmonyStoryboard Pro    View all 450+ Brands               Adobe Creative CloudAcrobatPhotoshop Elements &amp; Premiere ElementsPhotoshopCaptivatePresenter  Creative Cloud Acrobat Photoshop Elements &amp; Premiere Elements Photoshop Captivate Presenter          Autodesk AutoCAD3ds maxMayaInventorFusion 360RevitSketchBook Pro  AutoCAD 3ds max Maya Inventor Fusion 360 Revit SketchBook Pro          Avid Technology Media Composer Pro ToolsSibeliusArtist SeriesPhotoScore and AudioScoreiLok  Media Composer  Pro Tools Sibelius Artist Series PhotoScore and AudioScore iLok          Corel PainterCorelDRAW Graphics SuiteWordPerfect OfficeCorelDRAW Technical SuitePaintShop ProDazzle VideoVideoStudioToastGame CaptureWinDVDEasy VHS to DVDEasy LP to MP3View all Titles  Painter CorelDRAW Graphics Suite WordPerfect Office CorelDRAW Technical Suite PaintShop Pro Dazzle Video VideoStudio Toast Game Capture WinDVD Easy VHS to DVD Easy LP to MP3 View all Titles          FileMaker FileMaker ProFileMaker Advanced  FileMaker Pro FileMaker Advanced          Microsoft OfficeOffice for MacintoshKeyboardsWindows ServerTablet Cases/CoversExcelTablet Docking StationsWordVisual StudioSurfaceBeats by Dr. DreIT AcademyView all Titles  Office Office for Macintosh Keyboards Windows Server Tablet Cases/Covers Excel Tablet Docking Stations Word Visual Studio Surface Beats by Dr. Dre IT Academy View all Titles          Quark QuarkXPress  QuarkXPress          Sony PS Vita AccessoriesPS3 Accessories  PS Vita Accessories PS3 Accessories          Symantec Norton Hotspot PrivacyNorton Small BusinessNorton UtilitiesNorton Anti-TheftNorton Mobile Security  Norton Hotspot Privacy Norton Small Business Norton Utilities Norton Anti-Theft Norton Mobile Security          Toon Boom HarmonyStoryboard Pro  Harmony Storyboard Pro View all 450+ Brands School Services                            School Services                         Get a Quote      School Services Get a Quote    Instant Online Verification          Dated Student ID from the current semester or school year          Course Schedule          Registration Receipt for this semester          Letter of Enrollment on school letterhead.          Report Card          Dated Student ID from the current semester or school year          Registration Receipt          Letter of Enrollment on school letterhead          Link to your faculty web page          Current Faculty ID          Letter of Employment on school letterhead          Pay Stub (cross out confidential information)          Membership in Home School Association          Receipt for Home School Curriculum          Letter of intent to home school from a state agency       Your Purchase Order    Copy of IRS 501(c)3 form          IRS letter stating that you are a 501(c)3        FAQ  Contact Us  800.876.3507 Privacy Policy Terms &amp; Conditions About Us                 Office &amp; Productivity Microsoft Solutions Business &amp; Productivity Business Training Graphics, Art &amp; Design Adobe Tools Animation &amp; Modeling Color Management Desktop Publishing Graphics &amp; Illustration Graphics Tablets Web Publishing Design Training Educational Tools Art &amp; Music Software Critical Thinking Software Graphing Software Language Arts Software Science Software Social Studies Software Typing Software Classroom Electronics Classroom Learning Aids AntiVirus &amp; Security Anti-Virus Content Filtering Firewall &amp; Security CAD &amp; Engineering 3D Printers Architectural Design CAD &amp; Modeling Map Making/GIS Mechanical Design CAD Training Laptops &amp; Tablets Notebook Computers Notebook Accessories Tablets Tablet Accessories Laptop Carts Bags OS &amp; Utilities Operating Systems Programming Utilities Music &amp; Video Audio Production Digital Video Software DJ Equipment Headphones &amp; Earbuds MIDI Devices Music &amp; Video Training Notation Recording Products Sheet Music &amp; Guitar Tab Video Hardware Electronic Accessories Cables Expansion Cards Headphones &amp; Headsets Keyboards &amp; Mice Monitors MP3 &amp; Phone Accessories Networking Products Power Products Printers &amp; Scanners Security Cables Speakers Storage Devices Web Cameras Adobe Creative Cloud Acrobat Photoshop Elements &amp; Premiere Elements Photoshop Captivate Presenter Autodesk AutoCAD 3ds max Maya Inventor Fusion 360 Revit SketchBook Pro Avid Technology Media Composer  Pro Tools Sibelius Artist Series PhotoScore and AudioScore iLok Corel Painter CorelDRAW Graphics Suite WordPerfect Office CorelDRAW Technical Suite PaintShop Pro Dazzle Video VideoStudio Toast Game Capture WinDVD Easy VHS to DVD Easy LP to MP3 View all Titles FileMaker FileMaker Pro FileMaker Advanced Microsoft Office Office for Macintosh Keyboards Windows Server Tablet Cases/Covers Excel Tablet Docking Stations Word Visual Studio Surface Beats by Dr. Dre IT Academy View all Titles Quark QuarkXPress Sony PS Vita Accessories PS3 Accessories Symantec Norton Hotspot Privacy Norton Small Business Norton Utilities Norton Anti-Theft Norton Mobile Security Toon Boom Harmony Storyboard Pro View all 450+ Brands School Services School Services Get a Quote My Account   Office &amp; Productivity Graphics, Art &amp; Design Educational Tools AntiVirus &amp; Security CAD &amp; Engineering Laptops &amp; Tablets OS &amp; Utilities Music &amp; Video Electronic Accessories  FAQ  Contact Us  800.876.3507 Privacy Policy Terms &amp; Conditions About Us     Sign Up For Special Offers    (cross out confidential information) Microsoft Office, Adobe Acrobat, SPSS... Creative Cloud, Photoshop, Wacom... Rosetta Stone, LeapFrog, Inspiration... Symantec, ESET, Kaspersky... Autodesk, SolidWorks, TurboCAD... Microsoft Surface, HP, Dell... Windows, TechSmith, WinZip... Pro Tools, After Effects, Sibelius... Displays, Graphics Tablets, Harddrives... find, follow &amp; friend us for exclusive deals &amp; discounts</v>
+        <v>Academic Superstore Academic Software discounts for students teachers and schools Academic edition software discounts for students teachers and schools Educational pricing available to college students k12 students homeschool students faculty universities educational institutions and parents Academic Superstore academic software academic academic price academic discount academic edition academic version student software student price student discount student edition student version discount software educational software educational price educational discount educational edition teacher software school software adobe academic adobe discounts microsoft academic microsoft discounts Shop by Category Office Productivity Microsoft Solutions Business Productivity Business Training Graphics Art Design Adobe Tools Animation Modeling Color Management Desktop Publishing Graphics Illustration Graphics Tablets Web Publishing Design Training Educational Tools Art Music Software Critical Thinking Software Graphing Software Language Arts Software Science Software Social Studies Software Typing Software Classroom Electronics Classroom Learning Aids AntiVirus Security AntiVirus Content Filtering Firewall Security CAD Engineering 3D Printers Architectural Design CAD Modeling Map MakingGIS Mechanical Design CAD Training Laptops Tablets Notebook Computers Notebook Accessories Tablets Tablet Accessories Laptop Carts Bags OS Utilities Operating Systems Programming Utilities Music Video Audio Production Digital Video Software DJ Equipment Headphones Earbuds MIDI Devices Music Video Training Notation Recording Products Sheet Music Guitar Tab Video Hardware Electronic Accessories Cables Expansion Cards Headphones Headsets Keyboards Mice Monitors MP3 Phone Accessories Networking Products Power Products Printers Scanners Security Cables Speakers Storage Devices Web Cameras Office Productivity Microsoft Solutions Business Productivity Business Training Microsoft Solutions Business Productivity Business Training Graphics Art Design Adobe Tools Animation Modeling Color Management Desktop Publishing Graphics Illustration Graphics Tablets Web Publishing Design Training Adobe Tools Animation Modeling Color Management Desktop Publishing Graphics Illustration Graphics Tablets Web Publishing Design Training Educational Tools Art Music Software Critical Thinking Software Graphing Software Language Arts Software Science Software Social Studies Software Typing Software Classroom Electronics Classroom Learning Aids Art Music Software Critical Thinking Software Graphing Software Language Arts Software Science Software Social Studies Software Typing Software Classroom Electronics Classroom Learning Aids AntiVirus Security AntiVirus Content Filtering Firewall Security AntiVirus Content Filtering Firewall Security CAD Engineering 3D Printers Architectural Design CAD Modeling Map MakingGIS Mechanical Design CAD Training 3D Printers Architectural Design CAD Modeling Map MakingGIS Mechanical Design CAD Training Laptops Tablets Notebook Computers Notebook Accessories Tablets Tablet Accessories Laptop Carts Bags Notebook Computers Notebook Accessories Tablets Tablet Accessories Laptop Carts Bags OS Utilities Operating Systems Programming Utilities Operating Systems Programming Utilities Music Video Audio Production Digital Video Software DJ Equipment Headphones Earbuds MIDI Devices Music Video Training Notation Recording Products Sheet Music Guitar Tab Video Hardware Audio Production Digital Video Software DJ Equipment Headphones Earbuds MIDI Devices Music Video Training Notation Recording Products Sheet Music Guitar Tab Video Hardware Electronic Accessories Cables Expansion Cards Headphones Headsets Keyboards Mice Monitors MP3 Phone Accessories Networking Products Power Products Printers Scanners Security Cables Speakers Storage Devices Web Cameras Cables Expansion Cards Headphones Headsets Keyboards Mice Monitors MP3 Phone Accessories Networking Products Power Products Printers Scanners Security Cables Speakers Storage Devices Web Cameras Shop by Brand Adobe Creative CloudAcrobatPhotoshop Elements Premiere ElementsPhotoshopCaptivatePresenter Autodesk AutoCAD3ds maxMayaInventorFusion 360RevitSketchBook Pro Avid Technology Media Composer Pro ToolsSibeliusArtist SeriesPhotoScore and AudioScoreiLok Corel PainterCorelDRAW Graphics SuiteWordPerfect OfficeCorelDRAW Technical SuitePaintShop ProDazzle VideoVideoStudioToastGame CaptureWinDVDEasy VHS to DVDEasy LP to MP3View all Titles FileMaker FileMaker ProFileMaker Advanced Microsoft OfficeOffice for MacintoshKeyboardsWindows ServerTablet CasesCoversExcelTablet Docking StationsWordVisual StudioSurfaceBeats by Dr DreIT AcademyView all Titles Quark QuarkXPress Sony PS Vita AccessoriesPS3 Accessories Symantec Norton Hotspot PrivacyNorton Small BusinessNorton UtilitiesNorton AntiTheftNorton Mobile Security Toon Boom HarmonyStoryboard Pro View all 450 Brands Adobe Creative CloudAcrobatPhotoshop Elements Premiere ElementsPhotoshopCaptivatePresenter Creative Cloud Acrobat Photoshop Elements Premiere Elements Photoshop Captivate Presenter Autodesk AutoCAD3ds maxMayaInventorFusion 360RevitSketchBook Pro AutoCAD 3ds max Maya Inventor Fusion 360 Revit SketchBook Pro Avid Technology Media Composer Pro ToolsSibeliusArtist SeriesPhotoScore and AudioScoreiLok Media Composer Pro Tools Sibelius Artist Series PhotoScore and AudioScore iLok Corel PainterCorelDRAW Graphics SuiteWordPerfect OfficeCorelDRAW Technical SuitePaintShop ProDazzle VideoVideoStudioToastGame CaptureWinDVDEasy VHS to DVDEasy LP to MP3View all Titles Painter CorelDRAW Graphics Suite WordPerfect Office CorelDRAW Technical Suite PaintShop Pro Dazzle Video VideoStudio Toast Game Capture WinDVD Easy VHS to DVD Easy LP to MP3 View all Titles FileMaker FileMaker ProFileMaker Advanced FileMaker Pro FileMaker Advanced Microsoft OfficeOffice for MacintoshKeyboardsWindows ServerTablet CasesCoversExcelTablet Docking StationsWordVisual StudioSurfaceBeats by Dr DreIT AcademyView all Titles Office Office for Macintosh Keyboards Windows Server Tablet CasesCovers Excel Tablet Docking Stations Word Visual Studio Surface Beats by Dr Dre IT Academy View all Titles Quark QuarkXPress QuarkXPress Sony PS Vita AccessoriesPS3 Accessories PS Vita Accessories PS3 Accessories Symantec Norton Hotspot PrivacyNorton Small BusinessNorton UtilitiesNorton AntiTheftNorton Mobile Security Norton Hotspot Privacy Norton Small Business Norton Utilities Norton AntiTheft Norton Mobile Security Toon Boom HarmonyStoryboard Pro Harmony Storyboard Pro View all 450 Brands School Services School Services Get a Quote School Services Get a Quote Instant Online Verification Dated Student ID from the current semester or school year Course Schedule Registration Receipt for this semester Letter of Enrollment on school letterhead Report Card Dated Student ID from the current semester or school year Registration Receipt Letter of Enrollment on school letterhead Link to your faculty web page Current Faculty ID Letter of Employment on school letterhead Pay Stub cross out confidential information Membership in Home School Association Receipt for Home School Curriculum Letter of intent to home school from a state agency Your Purchase Order Copy of IRS 501c3 form IRS letter stating that you are a 501c3 FAQ Contact Us 8008763507 Privacy Policy Terms Conditions About Us Office Productivity Microsoft Solutions Business Productivity Business Training Graphics Art Design Adobe Tools Animation Modeling Color Management Desktop Publishing Graphics Illustration Graphics Tablets Web Publishing Design Training Educational Tools Art Music Software Critical Thinking Software Graphing Software Language Arts Software Science Software Social Studies Software Typing Software Classroom Electronics Classroom Learning Aids AntiVirus Security AntiVirus Content Filtering Firewall Security CAD Engineering 3D Printers Architectural Design CAD Modeling Map MakingGIS Mechanical Design CAD Training Laptops Tablets Notebook Computers Notebook Accessories Tablets Tablet Accessories Laptop Carts Bags OS Utilities Operating Systems Programming Utilities Music Video Audio Production Digital Video Software DJ Equipment Headphones Earbuds MIDI Devices Music Video Training Notation Recording Products Sheet Music Guitar Tab Video Hardware Electronic Accessories Cables Expansion Cards Headphones Headsets Keyboards Mice Monitors MP3 Phone Accessories Networking Products Power Products Printers Scanners Security Cables Speakers Storage Devices Web Cameras Adobe Creative Cloud Acrobat Photoshop Elements Premiere Elements Photoshop Captivate Presenter Autodesk AutoCAD 3ds max Maya Inventor Fusion 360 Revit SketchBook Pro Avid Technology Media Composer Pro Tools Sibelius Artist Series PhotoScore and AudioScore iLok Corel Painter CorelDRAW Graphics Suite WordPerfect Office CorelDRAW Technical Suite PaintShop Pro Dazzle Video VideoStudio Toast Game Capture WinDVD Easy VHS to DVD Easy LP to MP3 View all Titles FileMaker FileMaker Pro FileMaker Advanced Microsoft Office Office for Macintosh Keyboards Windows Server Tablet CasesCovers Excel Tablet Docking Stations Word Visual Studio Surface Beats by Dr Dre IT Academy View all Titles Quark QuarkXPress Sony PS Vita Accessories PS3 Accessories Symantec Norton Hotspot Privacy Norton Small Business Norton Utilities Norton AntiTheft Norton Mobile Security Toon Boom Harmony Storyboard Pro View all 450 Brands School Services School Services Get a Quote My Account Office Productivity Graphics Art Design Educational Tools AntiVirus Security CAD Engineering Laptops Tablets OS Utilities Music Video Electronic Accessories FAQ Contact Us 8008763507 Privacy Policy Terms Conditions About Us Sign Up For Special Offers cross out confidential information Microsoft Office Adobe Acrobat SPSS Creative Cloud Photoshop Wacom Rosetta Stone LeapFrog Inspiration Symantec ESET Kaspersky Autodesk SolidWorks TurboCAD Microsoft Surface HP Dell Windows TechSmith WinZip Pro Tools After Effects Sibelius Displays Graphics Tablets Harddrives find follow friend us for exclusive deals discounts</v>
       </c>
     </row>
     <row r="9">
@@ -533,16 +476,7 @@
         <v>reseller</v>
       </c>
       <c r="C9" t="str">
-        <v>CDW -  Computers, Hardware, Software and IT Solutions for Business  The information technology products, expertise and service you need to make your business successful. Fast shipping, fast answers, the industry's largest in-stock inventories, custom configurations and more. anti-virus, business computers, business software, business technology, business laptop, cables, cdw, cdw.com, CDW@work, computer, computer accessories, computer configuration, computer hardware, computer memory, computer service, computer technical services, computer technology services, computers, corporate computing products, desktop, desktops, desktop pcs, desktop pc, digital flow, handheld computer, handhelds, hard drives, information technology, input devices, kvm, lan products, laptop, laptops, laser printers, lcd projector, lcd projectors, macwarehouse, memory upgrades, microwarehouse, modems, monitor, monitors, network security, networking computers, notebook computers, pc, pcs, pda, power protection, printer, printer supplies, printers, projectors, scanners, server, servers, software licensing, technology products, telephony, toner, voip, wan products, wireless, wireless computing, wireless networking, workstations, www.cdw.com Featured Products Solution Spotlight: Mobility Popular Products Our Experts Account Log On We're the people who get IT Discover how CDW and our partners can help you mobilize your business. AirWatch by VMware Enterprise Mobility Management AirWatch by VMware Enterprise Mobility Management Sandra                       Cloud Client Executive                      Talk to our experts about your business needs. We won't charge you a cent. Who We Are What We Do How We Do It How Can We Help Shop Mobile    Account Log On  or  Create Account                    Cart (0)                                                        Hardware                                                                                                                                  Software                                                                                                                                  Solutions                                                                                                                                  Cloud                                                                                                                                  Brands                                                                                                                                  Blog                                                                                                     Deals                                                                            Energy &amp; Utilities Financial Services Government / Education Healthcare International Nonprofit Retail Small Business Startups                                                                                                                                                                                                    New and Now                             Our latest products and freshest news                                                                                                                                                                                                                                                  CDW Digital                             All the IT resources you need, all in one app                                                                                                                                          Dell Latitude E5550                                           Keep your workforce productive on the go or at the desk                                          $1,029.99                                                                                                                                             Dell Wyse D10D                                          Resolve the challenges of provisioning, managing, maintaining and securing enterprise desktops                                           $359.99                                                                                                                                             Ricoh Aficio SP 3510SF                                          Operate more efficiently with fast 30 page-per-minute output speeds                                          $399.00                                                                                                                                           Polycom SoundStation IP 5000                                          Advanced audio performance designed for executive offices and smaller conference rooms                                          $366.00                                                                                                                                           Plantronics Voyager Legend Headset                                           Three precision-tuned microphones cancel noise and wind                                          $139.99                                       notebooks tablets printers desktops data storage Who We Are About Us Careers Community Involvement Diversity Investor Relations International Solutions Locations What We Do  CDW Blog  CDW Site Info  E-Procurement  Leasing  Solutions and Services How We Do It  Awards  Customer Reviews  Media Library  Newsroom  CDW Technoliner How Can We Help Customer Relations E-Waste Recycling FAQs                  Product Recalls Support Shop Account Center Best Deals Brands Catalog Request Outlet Product Finders Quick Order Status Subscription Center Mobile Android App iPhone App                                                                                                                                                             Remember my User Name. 800.800.4239                              Send E-mail                             Answer within 24 Hours                          When it comes to supporting your business, you're not alone. It's you and CDW. And our partners. And tech designed for today, tomorrow and beyond. Every Monday, we slash the price of one of our products. Get it before it sells out. With a 12.3" display, Surface Pro 4 is the tablet that performs like a notebook. See what else the Surface can do. We'll help you find the tech you need, from Apple to Zebra. I would recommend CDW to anyone." - Project CoordinatorJanuary 15, 2016 Keep your workforce productive on the go or at the desk Resolve the challenges of provisioning, managing, maintaining and securing enterprise desktops  Operate more efficiently with fast 30 page-per-minute output speeds Advanced audio performance designed for executive offices and smaller conference rooms Three precision-tuned microphones cancel noise and wind "CDW was a great partner in that they were able to hold our inventory and ship it out in whatever partials were needed when they got the call from each of our offices," says Susan Luu, JA's senior vice president for business improvement. "CDW was a great partner in that they were able to hold our inventory and ship it out in whatever partials were needed when they got the call from each of our offices," says Susan Luu, JA's senior vice president for business improvement. Learn how to build and deliver the right apps for on-the-go users.                               Provide your employees with access to corporate applications, data and resources from virtually anywhere on almost any device, while keeping corporate information secure.                                                       A mobility platform that provides the flexibility to manage multiple use cases, unified management of endpoints, end-to-end security and seamless integration across enterprise systems                                                        Designed for organizations of all sizes to run applications at high service levels and maximize hardware savings through higher capacity utilization and consolidation ratios                            Based in Chicago, Sandra has more than a decade of experience working with integrated IT solutions, from security services to application management. Our Cloud Client Executives work to customize a cloud solution that perfectly fits your unique needs.      Account Log On Create Account       Cart (0)                                     All Product Catalog CDW Outlet Catalog close Send E-mail                              Hardware                                                                                    Software                                                                                    Solutions                                                                                    Cloud                                                                                    Brands                                                                                    Blog                                                       Deals                                                       Energy &amp; Utilities Financial Services Government / Education Healthcare International Nonprofit Retail Small Business Startups See how we can help your team Get it before it sells out.  See what else the Surface can do. Contact us                                                                Our latest products and freshest news                                                               All the IT resources you need, all in one app See more reviews                                                                       Dell Latitude E5550                                                                                                       Dell Wyse D10D                                                                                                      Ricoh Aficio SP 3510SF                                                                                                    Polycom SoundStation IP 5000                                                                                                    Plantronics Voyager Legend Headset                       Read case study Read case study Get the guide Get more details Explore now Get more details Contact a mobility pro notebooks tablets printers desktops data storage                          Get to know Sandra                                           Get to know our process                  Forgot User Name? Forgot Password? Create an account                                About Us Careers Community Involvement Diversity Investor Relations International Solutions Locations CDW Blog CDW Site Info E-Procurement Leasing Solutions and Services Awards Customer Reviews Media Library Newsroom CDW Technoliner Customer Relations E-Waste Recycling FAQs Product Recalls Support Account Center Best Deals Brands Catalog Request Outlet Product Finders Quick Order Status Subscription Center Android App iPhone App                                                                                              Site Map Privacy Policy Terms and Conditions  or  0 800.800.4239  Mon-Fri 7am-7:30pm CT Forgot User Name? Forgot Password? Remember my User Name.</v>
-      </c>
-      <c r="D9" t="str">
-        <v>CDW -  Computers, Hardware, Software and IT Solutions for Business  The information technology products, expertise and service you need to make your business successful. Fast shipping, fast answers, the industry's largest in-stock inventories, custom configurations and more. anti-virus, business computers, business software, business technology, business laptop, cables, cdw, cdw.com, CDW@work, computer, computer accessories, computer configuration, computer hardware, computer memory, computer service, computer technical services, computer technology services, computers, corporate computing products, desktop, desktops, desktop pcs, desktop pc, digital flow, handheld computer, handhelds, hard drives, information technology, input devices, kvm, lan products, laptop, laptops, laser printers, lcd projector, lcd projectors, macwarehouse, memory upgrades, microwarehouse, modems, monitor, monitors, network security, networking computers, notebook computers, pc, pcs, pda, power protection, printer, printer supplies, printers, projectors, scanners, server, servers, software licensing, technology products, telephony, toner, voip, wan products, wireless, wireless computing, wireless networking, workstations, www.cdw.com Featured Products Solution Spotlight: Mobility Popular Products Our Experts Account Log On We're the people who get IT Discover how CDW and our partners can help you mobilize your business. AirWatch by VMware Enterprise Mobility Management AirWatch by VMware Enterprise Mobility Management Sandra                       Cloud Client Executive                      Talk to our experts about your business needs. We won't charge you a cent. Who We Are What We Do How We Do It How Can We Help Shop Mobile    Account Log On  or  Create Account                    Cart (0)                                                        Hardware                                                                                                                                  Software                                                                                                                                  Solutions                                                                                                                                  Cloud                                                                                                                                  Brands                                                                                                                                  Blog                                                                                                     Deals                                                                            Energy &amp; Utilities Financial Services Government / Education Healthcare International Nonprofit Retail Small Business Startups                                                                                                                                                                                                    New and Now                             Our latest products and freshest news                                                                                                                                                                                                                                                  CDW Digital                             All the IT resources you need, all in one app                                                                                                                                          Dell Latitude E5550                                           Keep your workforce productive on the go or at the desk                                          $1,029.99                                                                                                                                             Dell Wyse D10D                                          Resolve the challenges of provisioning, managing, maintaining and securing enterprise desktops                                           $359.99                                                                                                                                             Ricoh Aficio SP 3510SF                                          Operate more efficiently with fast 30 page-per-minute output speeds                                          $399.00                                                                                                                                           Polycom SoundStation IP 5000                                          Advanced audio performance designed for executive offices and smaller conference rooms                                          $366.00                                                                                                                                           Plantronics Voyager Legend Headset                                           Three precision-tuned microphones cancel noise and wind                                          $139.99                                       notebooks tablets printers desktops data storage Who We Are About Us Careers Community Involvement Diversity Investor Relations International Solutions Locations What We Do  CDW Blog  CDW Site Info  E-Procurement  Leasing  Solutions and Services How We Do It  Awards  Customer Reviews  Media Library  Newsroom  CDW Technoliner How Can We Help Customer Relations E-Waste Recycling FAQs                  Product Recalls Support Shop Account Center Best Deals Brands Catalog Request Outlet Product Finders Quick Order Status Subscription Center Mobile Android App iPhone App                                                                                                                                                             Remember my User Name. 800.800.4239                              Send E-mail                             Answer within 24 Hours                          When it comes to supporting your business, you're not alone. It's you and CDW. And our partners. And tech designed for today, tomorrow and beyond. Every Monday, we slash the price of one of our products. Get it before it sells out. With a 12.3" display, Surface Pro 4 is the tablet that performs like a notebook. See what else the Surface can do. We'll help you find the tech you need, from Apple to Zebra. I would recommend CDW to anyone." - Project CoordinatorJanuary 15, 2016 Keep your workforce productive on the go or at the desk Resolve the challenges of provisioning, managing, maintaining and securing enterprise desktops  Operate more efficiently with fast 30 page-per-minute output speeds Advanced audio performance designed for executive offices and smaller conference rooms Three precision-tuned microphones cancel noise and wind "CDW was a great partner in that they were able to hold our inventory and ship it out in whatever partials were needed when they got the call from each of our offices," says Susan Luu, JA's senior vice president for business improvement. "CDW was a great partner in that they were able to hold our inventory and ship it out in whatever partials were needed when they got the call from each of our offices," says Susan Luu, JA's senior vice president for business improvement. Learn how to build and deliver the right apps for on-the-go users.                               Provide your employees with access to corporate applications, data and resources from virtually anywhere on almost any device, while keeping corporate information secure.                                                       A mobility platform that provides the flexibility to manage multiple use cases, unified management of endpoints, end-to-end security and seamless integration across enterprise systems                                                        Designed for organizations of all sizes to run applications at high service levels and maximize hardware savings through higher capacity utilization and consolidation ratios                            Based in Chicago, Sandra has more than a decade of experience working with integrated IT solutions, from security services to application management. Our Cloud Client Executives work to customize a cloud solution that perfectly fits your unique needs.      Account Log On Create Account       Cart (0)                                     All Product Catalog CDW Outlet Catalog close Send E-mail                              Hardware                                                                                    Software                                                                                    Solutions                                                                                    Cloud                                                                                    Brands                                                                                    Blog                                                       Deals                                                       Energy &amp; Utilities Financial Services Government / Education Healthcare International Nonprofit Retail Small Business Startups See how we can help your team Get it before it sells out.  See what else the Surface can do. Contact us                                                                Our latest products and freshest news                                                               All the IT resources you need, all in one app See more reviews                                                                       Dell Latitude E5550                                                                                                       Dell Wyse D10D                                                                                                      Ricoh Aficio SP 3510SF                                                                                                    Polycom SoundStation IP 5000                                                                                                    Plantronics Voyager Legend Headset                       Read case study Read case study Get the guide Get more details Explore now Get more details Contact a mobility pro notebooks tablets printers desktops data storage                          Get to know Sandra                                           Get to know our process                  Forgot User Name? Forgot Password? Create an account                                About Us Careers Community Involvement Diversity Investor Relations International Solutions Locations CDW Blog CDW Site Info E-Procurement Leasing Solutions and Services Awards Customer Reviews Media Library Newsroom CDW Technoliner Customer Relations E-Waste Recycling FAQs Product Recalls Support Account Center Best Deals Brands Catalog Request Outlet Product Finders Quick Order Status Subscription Center Android App iPhone App                                                                                              Site Map Privacy Policy Terms and Conditions  or  0 800.800.4239  Mon-Fri 7am-7:30pm CT Forgot User Name? Forgot Password? Remember my User Name.</v>
-      </c>
-      <c r="E9" t="str">
-        <v>CDW -  Computers, Hardware, Software and IT Solutions for Business  The information technology products, expertise and service you need to make your business successful. Fast shipping, fast answers, the industry's largest in-stock inventories, custom configurations and more. anti-virus, business computers, business software, business technology, business laptop, cables, cdw, cdw.com, CDW@work, computer, computer accessories, computer configuration, computer hardware, computer memory, computer service, computer technical services, computer technology services, computers, corporate computing products, desktop, desktops, desktop pcs, desktop pc, digital flow, handheld computer, handhelds, hard drives, information technology, input devices, kvm, lan products, laptop, laptops, laser printers, lcd projector, lcd projectors, macwarehouse, memory upgrades, microwarehouse, modems, monitor, monitors, network security, networking computers, notebook computers, pc, pcs, pda, power protection, printer, printer supplies, printers, projectors, scanners, server, servers, software licensing, technology products, telephony, toner, voip, wan products, wireless, wireless computing, wireless networking, workstations, www.cdw.com Featured Products Solution Spotlight: Mobility Popular Products Our Experts Account Log On We're the people who get IT Discover how CDW and our partners can help you mobilize your business. AirWatch by VMware Enterprise Mobility Management AirWatch by VMware Enterprise Mobility Management Sandra                       Cloud Client Executive                      Talk to our experts about your business needs. We won't charge you a cent. Who We Are What We Do How We Do It How Can We Help Shop Mobile    Account Log On  or  Create Account                    Cart (0)                                                        Hardware                                                                                                                                  Software                                                                                                                                  Solutions                                                                                                                                  Cloud                                                                                                                                  Brands                                                                                                                                  Blog                                                                                                     Deals                                                                            Energy &amp; Utilities Financial Services Government / Education Healthcare International Nonprofit Retail Small Business Startups                                                                                                                                                                                                    New and Now                             Our latest products and freshest news                                                                                                                                                                                                                                                  CDW Digital                             All the IT resources you need, all in one app                                                                                                                                          Dell Latitude E5550                                           Keep your workforce productive on the go or at the desk                                          $1,029.99                                                                                                                                             Dell Wyse D10D                                          Resolve the challenges of provisioning, managing, maintaining and securing enterprise desktops                                           $359.99                                                                                                                                             Ricoh Aficio SP 3510SF                                          Operate more efficiently with fast 30 page-per-minute output speeds                                          $399.00                                                                                                                                           Polycom SoundStation IP 5000                                          Advanced audio performance designed for executive offices and smaller conference rooms                                          $366.00                                                                                                                                           Plantronics Voyager Legend Headset                                           Three precision-tuned microphones cancel noise and wind                                          $139.99                                       notebooks tablets printers desktops data storage Who We Are About Us Careers Community Involvement Diversity Investor Relations International Solutions Locations What We Do  CDW Blog  CDW Site Info  E-Procurement  Leasing  Solutions and Services How We Do It  Awards  Customer Reviews  Media Library  Newsroom  CDW Technoliner How Can We Help Customer Relations E-Waste Recycling FAQs                  Product Recalls Support Shop Account Center Best Deals Brands Catalog Request Outlet Product Finders Quick Order Status Subscription Center Mobile Android App iPhone App                                                                                                                                                             Remember my User Name. 800.800.4239                              Send E-mail                             Answer within 24 Hours                          When it comes to supporting your business, you're not alone. It's you and CDW. And our partners. And tech designed for today, tomorrow and beyond. Every Monday, we slash the price of one of our products. Get it before it sells out. With a 12.3" display, Surface Pro 4 is the tablet that performs like a notebook. See what else the Surface can do. We'll help you find the tech you need, from Apple to Zebra. I would recommend CDW to anyone." - Project CoordinatorJanuary 15, 2016 Keep your workforce productive on the go or at the desk Resolve the challenges of provisioning, managing, maintaining and securing enterprise desktops  Operate more efficiently with fast 30 page-per-minute output speeds Advanced audio performance designed for executive offices and smaller conference rooms Three precision-tuned microphones cancel noise and wind "CDW was a great partner in that they were able to hold our inventory and ship it out in whatever partials were needed when they got the call from each of our offices," says Susan Luu, JA's senior vice president for business improvement. "CDW was a great partner in that they were able to hold our inventory and ship it out in whatever partials were needed when they got the call from each of our offices," says Susan Luu, JA's senior vice president for business improvement. Learn how to build and deliver the right apps for on-the-go users.                               Provide your employees with access to corporate applications, data and resources from virtually anywhere on almost any device, while keeping corporate information secure.                                                       A mobility platform that provides the flexibility to manage multiple use cases, unified management of endpoints, end-to-end security and seamless integration across enterprise systems                                                        Designed for organizations of all sizes to run applications at high service levels and maximize hardware savings through higher capacity utilization and consolidation ratios                            Based in Chicago, Sandra has more than a decade of experience working with integrated IT solutions, from security services to application management. Our Cloud Client Executives work to customize a cloud solution that perfectly fits your unique needs.      Account Log On Create Account       Cart (0)                                     All Product Catalog CDW Outlet Catalog close Send E-mail                              Hardware                                                                                    Software                                                                                    Solutions                                                                                    Cloud                                                                                    Brands                                                                                    Blog                                                       Deals                                                       Energy &amp; Utilities Financial Services Government / Education Healthcare International Nonprofit Retail Small Business Startups See how we can help your team Get it before it sells out.  See what else the Surface can do. Contact us                                                                Our latest products and freshest news                                                               All the IT resources you need, all in one app See more reviews                                                                       Dell Latitude E5550                                                                                                       Dell Wyse D10D                                                                                                      Ricoh Aficio SP 3510SF                                                                                                    Polycom SoundStation IP 5000                                                                                                    Plantronics Voyager Legend Headset                       Read case study Read case study Get the guide Get more details Explore now Get more details Contact a mobility pro notebooks tablets printers desktops data storage                          Get to know Sandra                                           Get to know our process                  Forgot User Name? Forgot Password? Create an account                                About Us Careers Community Involvement Diversity Investor Relations International Solutions Locations CDW Blog CDW Site Info E-Procurement Leasing Solutions and Services Awards Customer Reviews Media Library Newsroom CDW Technoliner Customer Relations E-Waste Recycling FAQs Product Recalls Support Account Center Best Deals Brands Catalog Request Outlet Product Finders Quick Order Status Subscription Center Android App iPhone App                                                                                              Site Map Privacy Policy Terms and Conditions  or  0 800.800.4239  Mon-Fri 7am-7:30pm CT Forgot User Name? Forgot Password? Remember my User Name.</v>
-      </c>
-      <c r="F9" t="str">
-        <v>CDW -  Computers, Hardware, Software and IT Solutions for Business  The information technology products, expertise and service you need to make your business successful. Fast shipping, fast answers, the industry's largest in-stock inventories, custom configurations and more. anti-virus, business computers, business software, business technology, business laptop, cables, cdw, cdw.com, CDW@work, computer, computer accessories, computer configuration, computer hardware, computer memory, computer service, computer technical services, computer technology services, computers, corporate computing products, desktop, desktops, desktop pcs, desktop pc, digital flow, handheld computer, handhelds, hard drives, information technology, input devices, kvm, lan products, laptop, laptops, laser printers, lcd projector, lcd projectors, macwarehouse, memory upgrades, microwarehouse, modems, monitor, monitors, network security, networking computers, notebook computers, pc, pcs, pda, power protection, printer, printer supplies, printers, projectors, scanners, server, servers, software licensing, technology products, telephony, toner, voip, wan products, wireless, wireless computing, wireless networking, workstations, www.cdw.com Featured Products Solution Spotlight: Mobility Popular Products Our Experts Account Log On We're the people who get IT Discover how CDW and our partners can help you mobilize your business. AirWatch by VMware Enterprise Mobility Management AirWatch by VMware Enterprise Mobility Management Sandra                       Cloud Client Executive                      Talk to our experts about your business needs. We won't charge you a cent. Who We Are What We Do How We Do It How Can We Help Shop Mobile    Account Log On  or  Create Account                    Cart (0)                                                        Hardware                                                                                                                                  Software                                                                                                                                  Solutions                                                                                                                                  Cloud                                                                                                                                  Brands                                                                                                                                  Blog                                                                                                     Deals                                                                            Energy &amp; Utilities Financial Services Government / Education Healthcare International Nonprofit Retail Small Business Startups                                                                                                                                                                                                    New and Now                             Our latest products and freshest news                                                                                                                                                                                                                                                  CDW Digital                             All the IT resources you need, all in one app                                                                                                                                          Dell Latitude E5550                                           Keep your workforce productive on the go or at the desk                                          $1,029.99                                                                                                                                             Dell Wyse D10D                                          Resolve the challenges of provisioning, managing, maintaining and securing enterprise desktops                                           $359.99                                                                                                                                             Ricoh Aficio SP 3510SF                                          Operate more efficiently with fast 30 page-per-minute output speeds                                          $399.00                                                                                                                                           Polycom SoundStation IP 5000                                          Advanced audio performance designed for executive offices and smaller conference rooms                                          $366.00                                                                                                                                           Plantronics Voyager Legend Headset                                           Three precision-tuned microphones cancel noise and wind                                          $139.99                                       notebooks tablets printers desktops data storage Who We Are About Us Careers Community Involvement Diversity Investor Relations International Solutions Locations What We Do  CDW Blog  CDW Site Info  E-Procurement  Leasing  Solutions and Services How We Do It  Awards  Customer Reviews  Media Library  Newsroom  CDW Technoliner How Can We Help Customer Relations E-Waste Recycling FAQs                  Product Recalls Support Shop Account Center Best Deals Brands Catalog Request Outlet Product Finders Quick Order Status Subscription Center Mobile Android App iPhone App                                                                                                                                                             Remember my User Name. 800.800.4239                              Send E-mail                             Answer within 24 Hours                          When it comes to supporting your business, you're not alone. It's you and CDW. And our partners. And tech designed for today, tomorrow and beyond. Every Monday, we slash the price of one of our products. Get it before it sells out. With a 12.3" display, Surface Pro 4 is the tablet that performs like a notebook. See what else the Surface can do. We'll help you find the tech you need, from Apple to Zebra. I would recommend CDW to anyone." - Project CoordinatorJanuary 15, 2016 Keep your workforce productive on the go or at the desk Resolve the challenges of provisioning, managing, maintaining and securing enterprise desktops  Operate more efficiently with fast 30 page-per-minute output speeds Advanced audio performance designed for executive offices and smaller conference rooms Three precision-tuned microphones cancel noise and wind "CDW was a great partner in that they were able to hold our inventory and ship it out in whatever partials were needed when they got the call from each of our offices," says Susan Luu, JA's senior vice president for business improvement. "CDW was a great partner in that they were able to hold our inventory and ship it out in whatever partials were needed when they got the call from each of our offices," says Susan Luu, JA's senior vice president for business improvement. Learn how to build and deliver the right apps for on-the-go users.                               Provide your employees with access to corporate applications, data and resources from virtually anywhere on almost any device, while keeping corporate information secure.                                                       A mobility platform that provides the flexibility to manage multiple use cases, unified management of endpoints, end-to-end security and seamless integration across enterprise systems                                                        Designed for organizations of all sizes to run applications at high service levels and maximize hardware savings through higher capacity utilization and consolidation ratios                            Based in Chicago, Sandra has more than a decade of experience working with integrated IT solutions, from security services to application management. Our Cloud Client Executives work to customize a cloud solution that perfectly fits your unique needs.      Account Log On Create Account       Cart (0)                                     All Product Catalog CDW Outlet Catalog close Send E-mail                              Hardware                                                                                    Software                                                                                    Solutions                                                                                    Cloud                                                                                    Brands                                                                                    Blog                                                       Deals                                                       Energy &amp; Utilities Financial Services Government / Education Healthcare International Nonprofit Retail Small Business Startups See how we can help your team Get it before it sells out.  See what else the Surface can do. Contact us                                                                Our latest products and freshest news                                                               All the IT resources you need, all in one app See more reviews                                                                       Dell Latitude E5550                                                                                                       Dell Wyse D10D                                                                                                      Ricoh Aficio SP 3510SF                                                                                                    Polycom SoundStation IP 5000                                                                                                    Plantronics Voyager Legend Headset                       Read case study Read case study Get the guide Get more details Explore now Get more details Contact a mobility pro notebooks tablets printers desktops data storage                          Get to know Sandra                                           Get to know our process                  Forgot User Name? Forgot Password? Create an account                                About Us Careers Community Involvement Diversity Investor Relations International Solutions Locations CDW Blog CDW Site Info E-Procurement Leasing Solutions and Services Awards Customer Reviews Media Library Newsroom CDW Technoliner Customer Relations E-Waste Recycling FAQs Product Recalls Support Account Center Best Deals Brands Catalog Request Outlet Product Finders Quick Order Status Subscription Center Android App iPhone App                                                                                              Site Map Privacy Policy Terms and Conditions  or  0 800.800.4239  Mon-Fri 7am-7:30pm CT Forgot User Name? Forgot Password? Remember my User Name.</v>
+        <v>CDW Computers Hardware Software and IT Solutions for Business The information technology products expertise and service you need to make your business successful Fast shipping fast answers the industrys largest instock inventories custom configurations and more antivirus business computers business software business technology business laptop cables cdw cdwcom CDWwork computer computer accessories computer configuration computer hardware computer memory computer service computer technical services computer technology services computers corporate computing products desktop desktops desktop pcs desktop pc digital flow handheld computer handhelds hard drives information technology input devices kvm lan products laptop laptops laser printers lcd projector lcd projectors macwarehouse memory upgrades microwarehouse modems monitor monitors network security networking computers notebook computers pc pcs pda power protection printer printer supplies printers projectors scanners server servers software licensing technology products telephony toner voip wan products wireless wireless computing wireless networking workstations wwwcdwcom Featured Products Solution Spotlight Mobility Popular Products Our Experts Account Log On Were the people who get IT Discover how CDW and our partners can help you mobilize your business AirWatch by VMware Enterprise Mobility Management AirWatch by VMware Enterprise Mobility Management Sandra Cloud Client Executive Talk to our experts about your business needs We wont charge you a cent Who We Are What We Do How We Do It How Can We Help Shop Mobile Account Log On or Create Account Cart 0 Hardware Software Solutions Cloud Brands Blog Deals Energy Utilities Financial Services Government Education Healthcare International Nonprofit Retail Small Business Startups New and Now Our latest products and freshest news CDW Digital All the IT resources you need all in one app Dell Latitude E5550 Keep your workforce productive on the go or at the desk 102999 Dell Wyse D10D Resolve the challenges of provisioning managing maintaining and securing enterprise desktops 35999 Ricoh Aficio SP 3510SF Operate more efficiently with fast 30 pageperminute output speeds 39900 Polycom SoundStation IP 5000 Advanced audio performance designed for executive offices and smaller conference rooms 36600 Plantronics Voyager Legend Headset Three precisiontuned microphones cancel noise and wind 13999 notebooks tablets printers desktops data storage Who We Are About Us Careers Community Involvement Diversity Investor Relations International Solutions Locations What We Do CDW Blog CDW Site Info EProcurement Leasing Solutions and Services How We Do It Awards Customer Reviews Media Library Newsroom CDW Technoliner How Can We Help Customer Relations EWaste Recycling FAQs Product Recalls Support Shop Account Center Best Deals Brands Catalog Request Outlet Product Finders Quick Order Status Subscription Center Mobile Android App iPhone App Remember my User Name 8008004239 Send Email Answer within 24 Hours When it comes to supporting your business youre not alone Its you and CDW And our partners And tech designed for today tomorrow and beyond Every Monday we slash the price of one of our products Get it before it sells out With a 123 display Surface Pro 4 is the tablet that performs like a notebook See what else the Surface can do Well help you find the tech you need from Apple to Zebra I would recommend CDW to anyone Project CoordinatorJanuary 15 2016 Keep your workforce productive on the go or at the desk Resolve the challenges of provisioning managing maintaining and securing enterprise desktops Operate more efficiently with fast 30 pageperminute output speeds Advanced audio performance designed for executive offices and smaller conference rooms Three precisiontuned microphones cancel noise and wind CDW was a great partner in that they were able to hold our inventory and ship it out in whatever partials were needed when they got the call from each of our offices says Susan Luu JAs senior vice president for business improvement CDW was a great partner in that they were able to hold our inventory and ship it out in whatever partials were needed when they got the call from each of our offices says Susan Luu JAs senior vice president for business improvement Learn how to build and deliver the right apps for onthego users Provide your employees with access to corporate applications data and resources from virtually anywhere on almost any device while keeping corporate information secure A mobility platform that provides the flexibility to manage multiple use cases unified management of endpoints endtoend security and seamless integration across enterprise systems Designed for organizations of all sizes to run applications at high service levels and maximize hardware savings through higher capacity utilization and consolidation ratios Based in Chicago Sandra has more than a decade of experience working with integrated IT solutions from security services to application management Our Cloud Client Executives work to customize a cloud solution that perfectly fits your unique needs Account Log On Create Account Cart 0 All Product Catalog CDW Outlet Catalog close Send Email Hardware Software Solutions Cloud Brands Blog Deals Energy Utilities Financial Services Government Education Healthcare International Nonprofit Retail Small Business Startups See how we can help your team Get it before it sells out See what else the Surface can do Contact us Our latest products and freshest news All the IT resources you need all in one app See more reviews Dell Latitude E5550 Dell Wyse D10D Ricoh Aficio SP 3510SF Polycom SoundStation IP 5000 Plantronics Voyager Legend Headset Read case study Read case study Get the guide Get more details Explore now Get more details Contact a mobility pro notebooks tablets printers desktops data storage Get to know Sandra Get to know our process Forgot User Name Forgot Password Create an account About Us Careers Community Involvement Diversity Investor Relations International Solutions Locations CDW Blog CDW Site Info EProcurement Leasing Solutions and Services Awards Customer Reviews Media Library Newsroom CDW Technoliner Customer Relations EWaste Recycling FAQs Product Recalls Support Account Center Best Deals Brands Catalog Request Outlet Product Finders Quick Order Status Subscription Center Android App iPhone App Site Map Privacy Policy Terms and Conditions or 0 8008004239 MonFri 7am730pm CT Forgot User Name Forgot Password Remember my User Name</v>
       </c>
     </row>
     <row r="10">
@@ -553,16 +487,7 @@
         <v>reseller</v>
       </c>
       <c r="C10" t="str">
-        <v>Computer Hardware, Software &amp; IT Solutions | Insight Insight is a leading provider of hardware, software, cloud solutions and IT services to business, government, education and healthcare clients. Learn more. Learn Solve Buy Manage Intelligent Technology™ solutions that go beyond IT                                                                                                                                                                                                                                                                                                                                                                              Learn                                     about trending IT topics.                                                                                                                                                                                                                                                                       Solve                                     with our IT solutions.                                                                                                                                                                                                                                                                       Buy                                     products and services.                                                                                                                                                                                                                                                                       Manage                                     IT solutions with Insight.                                                                                                                                                                                                    Call now:1.800.INSIGHT                                                              Account Login Track Order                                                   United States                                                                                                                      Australia                                                               Canada: English                                                               Canada: French                                                               Austria                                                               Belgium                                                               China: English                                                               China: 中文简体                                                               Czech Republic                                                               Denmark                                                               Finland                                                               France                                                               Germany                                                               Hong Kong                                                               Hungary                                                               Ireland                                                               Italy                                                               Netherlands                                                               New Zealand                                                               Norway                                                               Poland                                                               Russia                                                               Singapore                                                               Spain                                                               Sweden                                                               Switzerland: Deutsch                                                               Switzerland: Français                                                                United Kingdom                                                               United States                                                                              Australia  Canada: English  Canada: French  Austria  Belgium  China: English  China: 中文简体  Czech Republic  Denmark  Finland  France  Germany  Hong Kong  Hungary  Ireland  Italy  Netherlands  New Zealand  Norway  Poland  Russia  Singapore  Spain  Sweden  Switzerland: Deutsch  Switzerland: Français   United Kingdom  United States SEWP Contract 1.800.INSIGHT 1.800.INSIGHT Chat Now Account Login Track Order                                           United States                                                                                                     Australia                                                       Canada: English                                                       Canada: French                                                       Austria                                                       Belgium                                                       China: English                                                       China: 中文简体                                                       Czech Republic                                                       Denmark                                                       Finland                                                       France                                                       Germany                                                       Hong Kong                                                       Hungary                                                       Ireland                                                       Italy                                                       Netherlands                                                       New Zealand                                                       Norway                                                       Poland                                                       Russia                                                       Singapore                                                       Spain                                                       Sweden                                                       Switzerland: Deutsch                                                       Switzerland: Français                                                        United Kingdom                                                       United States                                                                 Australia  Canada: English  Canada: French  Austria  Belgium  China: English  China: 中文简体  Czech Republic  Denmark  Finland  France  Germany  Hong Kong  Hungary  Ireland  Italy  Netherlands  New Zealand  Norway  Poland  Russia  Singapore  Spain  Sweden  Switzerland: Deutsch  Switzerland: Français   United Kingdom  United States 1.800.INSIGHT Chat Now Small to medium business Enterprise Federal government Education Service providers Healthcare State and local government More Mobility Security Cloud Networking Software Data center More Notebooks Office 365 Desktops Software Servers Warranties More E-commerce Procurement Supply chain More Our story   Awards Corporate responsibility Management team   Contact us Newsroom Careers Investor Relations Partnerships Spiceworks Linked In Facebook Twitter Youtube Google Plus Terms of Sale Terms of Sale (IPS) Return Policy Terms of Use Privacy Policy Safe Harbor Policy about trending topics. Stay informed on new and emerging technologies, and learn more about evolving industry trends. your challenges. Get help resolving your technology challenges with intelligent IT solutions tailored to your business. new products and services. Shop for hardware, software and cloud solutions, and services to help you throughout the IT lifecycle. your customized purchasing. Simplify all aspects of your organization’s purchasing, from selection to preparation and delivery.                                      Learn                                     about trending IT topics.                                                                       Solve                                     with our IT solutions.                                                                       Buy                                     products and services.                                                                       Manage                                     IT solutions with Insight.                                                                                               Call now:1.800.INSIGHT                                         Account Login Track Order   United States   Australia  Canada: English  Canada: French  Austria  Belgium  China: English  China: 中文简体  Czech Republic  Denmark  Finland  France  Germany  Hong Kong  Hungary  Ireland  Italy  Netherlands  New Zealand  Norway  Poland  Russia  Singapore  Spain  Sweden  Switzerland: Deutsch  Switzerland: Français   United Kingdom  United States SEWP Contract 1.800.INSIGHT 1.800.INSIGHT Chat Now Account Login Track Order   United States  Australia  Canada: English  Canada: French  Austria  Belgium  China: English  China: 中文简体  Czech Republic  Denmark  Finland  France  Germany  Hong Kong  Hungary  Ireland  Italy  Netherlands  New Zealand  Norway  Poland  Russia  Singapore  Spain  Sweden  Switzerland: Deutsch  Switzerland: Français   United Kingdom  United States 1.800.INSIGHT Chat Now                                                                                  Learn Browse our library Small to medium business Enterprise Federal government Education Service providers Healthcare State and local government More Solve Find a solution Mobility Security Cloud Networking Software Data center More Buy Start shopping Notebooks Office 365 Desktops Software Servers Warranties More Manage Save time &amp; money E-commerce Procurement Supply chain More 1-800-INSIGHT  Contact us  Chat  Frequently asked questions  Help topics Our story   Awards Corporate responsibility Management team   Contact us Newsroom Careers Investor Relations Partnerships Spiceworks Linked In Facebook Twitter Youtube Google Plus ​ Get the newsletter Terms of Sale Terms of Sale (IPS) Return Policy Terms of Use Privacy Policy Safe Harbor Policy Learn about trending IT topics. Solve with our IT solutions. Buy products and services. Manage IT solutions with Insight.                  Call now:1.800.INSIGHT                  1-800-INSIGHT   Contact us   Chat   Frequently asked questions   Help topics Spiceworks Spiceworks Linked In Linked In Facebook Facebook Twitter Twitter Youtube Youtube Google Plus Google Plus ​ Copyright © 2016 Insight</v>
-      </c>
-      <c r="D10" t="str">
-        <v>Computer Hardware, Software &amp; IT Solutions | Insight Insight is a leading provider of hardware, software, cloud solutions and IT services to business, government, education and healthcare clients. Learn more. Learn Solve Buy Manage Intelligent Technology™ solutions that go beyond IT                                                                                                                                                                                                                                                                                                                                                                              Learn                                     about trending IT topics.                                                                                                                                                                                                                                                                       Solve                                     with our IT solutions.                                                                                                                                                                                                                                                                       Buy                                     products and services.                                                                                                                                                                                                                                                                       Manage                                     IT solutions with Insight.                                                                                                                                                                                                    Call now:1.800.INSIGHT                                                              Account Login Track Order                                                   United States                                                                                                                      Australia                                                               Canada: English                                                               Canada: French                                                               Austria                                                               Belgium                                                               China: English                                                               China: 中文简体                                                               Czech Republic                                                               Denmark                                                               Finland                                                               France                                                               Germany                                                               Hong Kong                                                               Hungary                                                               Ireland                                                               Italy                                                               Netherlands                                                               New Zealand                                                               Norway                                                               Poland                                                               Russia                                                               Singapore                                                               Spain                                                               Sweden                                                               Switzerland: Deutsch                                                               Switzerland: Français                                                                United Kingdom                                                               United States                                                                              Australia  Canada: English  Canada: French  Austria  Belgium  China: English  China: 中文简体  Czech Republic  Denmark  Finland  France  Germany  Hong Kong  Hungary  Ireland  Italy  Netherlands  New Zealand  Norway  Poland  Russia  Singapore  Spain  Sweden  Switzerland: Deutsch  Switzerland: Français   United Kingdom  United States SEWP Contract 1.800.INSIGHT 1.800.INSIGHT Chat Now Account Login Track Order                                           United States                                                                                                     Australia                                                       Canada: English                                                       Canada: French                                                       Austria                                                       Belgium                                                       China: English                                                       China: 中文简体                                                       Czech Republic                                                       Denmark                                                       Finland                                                       France                                                       Germany                                                       Hong Kong                                                       Hungary                                                       Ireland                                                       Italy                                                       Netherlands                                                       New Zealand                                                       Norway                                                       Poland                                                       Russia                                                       Singapore                                                       Spain                                                       Sweden                                                       Switzerland: Deutsch                                                       Switzerland: Français                                                        United Kingdom                                                       United States                                                                 Australia  Canada: English  Canada: French  Austria  Belgium  China: English  China: 中文简体  Czech Republic  Denmark  Finland  France  Germany  Hong Kong  Hungary  Ireland  Italy  Netherlands  New Zealand  Norway  Poland  Russia  Singapore  Spain  Sweden  Switzerland: Deutsch  Switzerland: Français   United Kingdom  United States 1.800.INSIGHT Chat Now Small to medium business Enterprise Federal government Education Service providers Healthcare State and local government More Mobility Security Cloud Networking Software Data center More Notebooks Office 365 Desktops Software Servers Warranties More E-commerce Procurement Supply chain More Our story   Awards Corporate responsibility Management team   Contact us Newsroom Careers Investor Relations Partnerships Spiceworks Linked In Facebook Twitter Youtube Google Plus Terms of Sale Terms of Sale (IPS) Return Policy Terms of Use Privacy Policy Safe Harbor Policy about trending topics. Stay informed on new and emerging technologies, and learn more about evolving industry trends. your challenges. Get help resolving your technology challenges with intelligent IT solutions tailored to your business. new products and services. Shop for hardware, software and cloud solutions, and services to help you throughout the IT lifecycle. your customized purchasing. Simplify all aspects of your organization’s purchasing, from selection to preparation and delivery.                                      Learn                                     about trending IT topics.                                                                       Solve                                     with our IT solutions.                                                                       Buy                                     products and services.                                                                       Manage                                     IT solutions with Insight.                                                                                               Call now:1.800.INSIGHT                                         Account Login Track Order   United States   Australia  Canada: English  Canada: French  Austria  Belgium  China: English  China: 中文简体  Czech Republic  Denmark  Finland  France  Germany  Hong Kong  Hungary  Ireland  Italy  Netherlands  New Zealand  Norway  Poland  Russia  Singapore  Spain  Sweden  Switzerland: Deutsch  Switzerland: Français   United Kingdom  United States SEWP Contract 1.800.INSIGHT 1.800.INSIGHT Chat Now Account Login Track Order   United States  Australia  Canada: English  Canada: French  Austria  Belgium  China: English  China: 中文简体  Czech Republic  Denmark  Finland  France  Germany  Hong Kong  Hungary  Ireland  Italy  Netherlands  New Zealand  Norway  Poland  Russia  Singapore  Spain  Sweden  Switzerland: Deutsch  Switzerland: Français   United Kingdom  United States 1.800.INSIGHT Chat Now                                                                                  Learn Browse our library Small to medium business Enterprise Federal government Education Service providers Healthcare State and local government More Solve Find a solution Mobility Security Cloud Networking Software Data center More Buy Start shopping Notebooks Office 365 Desktops Software Servers Warranties More Manage Save time &amp; money E-commerce Procurement Supply chain More 1-800-INSIGHT  Contact us  Chat  Frequently asked questions  Help topics Our story   Awards Corporate responsibility Management team   Contact us Newsroom Careers Investor Relations Partnerships Spiceworks Linked In Facebook Twitter Youtube Google Plus ​ Get the newsletter Terms of Sale Terms of Sale (IPS) Return Policy Terms of Use Privacy Policy Safe Harbor Policy Learn about trending IT topics. Solve with our IT solutions. Buy products and services. Manage IT solutions with Insight.                  Call now:1.800.INSIGHT                  1-800-INSIGHT   Contact us   Chat   Frequently asked questions   Help topics Spiceworks Spiceworks Linked In Linked In Facebook Facebook Twitter Twitter Youtube Youtube Google Plus Google Plus ​ Copyright © 2016 Insight</v>
-      </c>
-      <c r="E10" t="str">
-        <v>Computer Hardware, Software &amp; IT Solutions | Insight Insight is a leading provider of hardware, software, cloud solutions and IT services to business, government, education and healthcare clients. Learn more. Learn Solve Buy Manage Intelligent Technology™ solutions that go beyond IT                                                                                                                                                                                                                                                                                                                                                                              Learn                                     about trending IT topics.                                                                                                                                                                                                                                                                       Solve                                     with our IT solutions.                                                                                                                                                                                                                                                                       Buy                                     products and services.                                                                                                                                                                                                                                                                       Manage                                     IT solutions with Insight.                                                                                                                                                                                                    Call now:1.800.INSIGHT                                                              Account Login Track Order                                                   United States                                                                                                                      Australia                                                               Canada: English                                                               Canada: French                                                               Austria                                                               Belgium                                                               China: English                                                               China: 中文简体                                                               Czech Republic                                                               Denmark                                                               Finland                                                               France                                                               Germany                                                               Hong Kong                                                               Hungary                                                               Ireland                                                               Italy                                                               Netherlands                                                               New Zealand                                                               Norway                                                               Poland                                                               Russia                                                               Singapore                                                               Spain                                                               Sweden                                                               Switzerland: Deutsch                                                               Switzerland: Français                                                                United Kingdom                                                               United States                                                                              Australia  Canada: English  Canada: French  Austria  Belgium  China: English  China: 中文简体  Czech Republic  Denmark  Finland  France  Germany  Hong Kong  Hungary  Ireland  Italy  Netherlands  New Zealand  Norway  Poland  Russia  Singapore  Spain  Sweden  Switzerland: Deutsch  Switzerland: Français   United Kingdom  United States SEWP Contract 1.800.INSIGHT 1.800.INSIGHT Chat Now Account Login Track Order                                           United States                                                                                                     Australia                                                       Canada: English                                                       Canada: French                                                       Austria                                                       Belgium                                                       China: English                                                       China: 中文简体                                                       Czech Republic                                                       Denmark                                                       Finland                                                       France                                                       Germany                                                       Hong Kong                                                       Hungary                                                       Ireland                                                       Italy                                                       Netherlands                                                       New Zealand                                                       Norway                                                       Poland                                                       Russia                                                       Singapore                                                       Spain                                                       Sweden                                                       Switzerland: Deutsch                                                       Switzerland: Français                                                        United Kingdom                                                       United States                                                                 Australia  Canada: English  Canada: French  Austria  Belgium  China: English  China: 中文简体  Czech Republic  Denmark  Finland  France  Germany  Hong Kong  Hungary  Ireland  Italy  Netherlands  New Zealand  Norway  Poland  Russia  Singapore  Spain  Sweden  Switzerland: Deutsch  Switzerland: Français   United Kingdom  United States 1.800.INSIGHT Chat Now Small to medium business Enterprise Federal government Education Service providers Healthcare State and local government More Mobility Security Cloud Networking Software Data center More Notebooks Office 365 Desktops Software Servers Warranties More E-commerce Procurement Supply chain More Our story   Awards Corporate responsibility Management team   Contact us Newsroom Careers Investor Relations Partnerships Spiceworks Linked In Facebook Twitter Youtube Google Plus Terms of Sale Terms of Sale (IPS) Return Policy Terms of Use Privacy Policy Safe Harbor Policy about trending topics. Stay informed on new and emerging technologies, and learn more about evolving industry trends. your challenges. Get help resolving your technology challenges with intelligent IT solutions tailored to your business. new products and services. Shop for hardware, software and cloud solutions, and services to help you throughout the IT lifecycle. your customized purchasing. Simplify all aspects of your organization’s purchasing, from selection to preparation and delivery.                                      Learn                                     about trending IT topics.                                                                       Solve                                     with our IT solutions.                                                                       Buy                                     products and services.                                                                       Manage                                     IT solutions with Insight.                                                                                               Call now:1.800.INSIGHT                                         Account Login Track Order   United States   Australia  Canada: English  Canada: French  Austria  Belgium  China: English  China: 中文简体  Czech Republic  Denmark  Finland  France  Germany  Hong Kong  Hungary  Ireland  Italy  Netherlands  New Zealand  Norway  Poland  Russia  Singapore  Spain  Sweden  Switzerland: Deutsch  Switzerland: Français   United Kingdom  United States SEWP Contract 1.800.INSIGHT 1.800.INSIGHT Chat Now Account Login Track Order   United States  Australia  Canada: English  Canada: French  Austria  Belgium  China: English  China: 中文简体  Czech Republic  Denmark  Finland  France  Germany  Hong Kong  Hungary  Ireland  Italy  Netherlands  New Zealand  Norway  Poland  Russia  Singapore  Spain  Sweden  Switzerland: Deutsch  Switzerland: Français   United Kingdom  United States 1.800.INSIGHT Chat Now                                                                                  Learn Browse our library Small to medium business Enterprise Federal government Education Service providers Healthcare State and local government More Solve Find a solution Mobility Security Cloud Networking Software Data center More Buy Start shopping Notebooks Office 365 Desktops Software Servers Warranties More Manage Save time &amp; money E-commerce Procurement Supply chain More 1-800-INSIGHT  Contact us  Chat  Frequently asked questions  Help topics Our story   Awards Corporate responsibility Management team   Contact us Newsroom Careers Investor Relations Partnerships Spiceworks Linked In Facebook Twitter Youtube Google Plus ​ Get the newsletter Terms of Sale Terms of Sale (IPS) Return Policy Terms of Use Privacy Policy Safe Harbor Policy Learn about trending IT topics. Solve with our IT solutions. Buy products and services. Manage IT solutions with Insight.                  Call now:1.800.INSIGHT                  1-800-INSIGHT   Contact us   Chat   Frequently asked questions   Help topics Spiceworks Spiceworks Linked In Linked In Facebook Facebook Twitter Twitter Youtube Youtube Google Plus Google Plus ​ Copyright © 2016 Insight</v>
-      </c>
-      <c r="F10" t="str">
-        <v>Computer Hardware, Software &amp; IT Solutions | Insight Insight is a leading provider of hardware, software, cloud solutions and IT services to business, government, education and healthcare clients. Learn more. Learn Solve Buy Manage Intelligent Technology™ solutions that go beyond IT                                                                                                                                                                                                                                                                                                                                                                              Learn                                     about trending IT topics.                                                                                                                                                                                                                                                                       Solve                                     with our IT solutions.                                                                                                                                                                                                                                                                       Buy                                     products and services.                                                                                                                                                                                                                                                                       Manage                                     IT solutions with Insight.                                                                                                                                                                                                    Call now:1.800.INSIGHT                                                              Account Login Track Order                                                   United States                                                                                                                      Australia                                                               Canada: English                                                               Canada: French                                                               Austria                                                               Belgium                                                               China: English                                                               China: 中文简体                                                               Czech Republic                                                               Denmark                                                               Finland                                                               France                                                               Germany                                                               Hong Kong                                                               Hungary                                                               Ireland                                                               Italy                                                               Netherlands                                                               New Zealand                                                               Norway                                                               Poland                                                               Russia                                                               Singapore                                                               Spain                                                               Sweden                                                               Switzerland: Deutsch                                                               Switzerland: Français                                                                United Kingdom                                                               United States                                                                              Australia  Canada: English  Canada: French  Austria  Belgium  China: English  China: 中文简体  Czech Republic  Denmark  Finland  France  Germany  Hong Kong  Hungary  Ireland  Italy  Netherlands  New Zealand  Norway  Poland  Russia  Singapore  Spain  Sweden  Switzerland: Deutsch  Switzerland: Français   United Kingdom  United States SEWP Contract 1.800.INSIGHT 1.800.INSIGHT Chat Now Account Login Track Order                                           United States                                                                                                     Australia                                                       Canada: English                                                       Canada: French                                                       Austria                                                       Belgium                                                       China: English                                                       China: 中文简体                                                       Czech Republic                                                       Denmark                                                       Finland                                                       France                                                       Germany                                                       Hong Kong                                                       Hungary                                                       Ireland                                                       Italy                                                       Netherlands                                                       New Zealand                                                       Norway                                                       Poland                                                       Russia                                                       Singapore                                                       Spain                                                       Sweden                                                       Switzerland: Deutsch                                                       Switzerland: Français                                                        United Kingdom                                                       United States                                                                 Australia  Canada: English  Canada: French  Austria  Belgium  China: English  China: 中文简体  Czech Republic  Denmark  Finland  France  Germany  Hong Kong  Hungary  Ireland  Italy  Netherlands  New Zealand  Norway  Poland  Russia  Singapore  Spain  Sweden  Switzerland: Deutsch  Switzerland: Français   United Kingdom  United States 1.800.INSIGHT Chat Now Small to medium business Enterprise Federal government Education Service providers Healthcare State and local government More Mobility Security Cloud Networking Software Data center More Notebooks Office 365 Desktops Software Servers Warranties More E-commerce Procurement Supply chain More Our story   Awards Corporate responsibility Management team   Contact us Newsroom Careers Investor Relations Partnerships Spiceworks Linked In Facebook Twitter Youtube Google Plus Terms of Sale Terms of Sale (IPS) Return Policy Terms of Use Privacy Policy Safe Harbor Policy about trending topics. Stay informed on new and emerging technologies, and learn more about evolving industry trends. your challenges. Get help resolving your technology challenges with intelligent IT solutions tailored to your business. new products and services. Shop for hardware, software and cloud solutions, and services to help you throughout the IT lifecycle. your customized purchasing. Simplify all aspects of your organization’s purchasing, from selection to preparation and delivery.                                      Learn                                     about trending IT topics.                                                                       Solve                                     with our IT solutions.                                                                       Buy                                     products and services.                                                                       Manage                                     IT solutions with Insight.                                                                                               Call now:1.800.INSIGHT                                         Account Login Track Order   United States   Australia  Canada: English  Canada: French  Austria  Belgium  China: English  China: 中文简体  Czech Republic  Denmark  Finland  France  Germany  Hong Kong  Hungary  Ireland  Italy  Netherlands  New Zealand  Norway  Poland  Russia  Singapore  Spain  Sweden  Switzerland: Deutsch  Switzerland: Français   United Kingdom  United States SEWP Contract 1.800.INSIGHT 1.800.INSIGHT Chat Now Account Login Track Order   United States  Australia  Canada: English  Canada: French  Austria  Belgium  China: English  China: 中文简体  Czech Republic  Denmark  Finland  France  Germany  Hong Kong  Hungary  Ireland  Italy  Netherlands  New Zealand  Norway  Poland  Russia  Singapore  Spain  Sweden  Switzerland: Deutsch  Switzerland: Français   United Kingdom  United States 1.800.INSIGHT Chat Now                                                                                  Learn Browse our library Small to medium business Enterprise Federal government Education Service providers Healthcare State and local government More Solve Find a solution Mobility Security Cloud Networking Software Data center More Buy Start shopping Notebooks Office 365 Desktops Software Servers Warranties More Manage Save time &amp; money E-commerce Procurement Supply chain More 1-800-INSIGHT  Contact us  Chat  Frequently asked questions  Help topics Our story   Awards Corporate responsibility Management team   Contact us Newsroom Careers Investor Relations Partnerships Spiceworks Linked In Facebook Twitter Youtube Google Plus ​ Get the newsletter Terms of Sale Terms of Sale (IPS) Return Policy Terms of Use Privacy Policy Safe Harbor Policy Learn about trending IT topics. Solve with our IT solutions. Buy products and services. Manage IT solutions with Insight.                  Call now:1.800.INSIGHT                  1-800-INSIGHT   Contact us   Chat   Frequently asked questions   Help topics Spiceworks Spiceworks Linked In Linked In Facebook Facebook Twitter Twitter Youtube Youtube Google Plus Google Plus ​ Copyright © 2016 Insight</v>
+        <v>Computer Hardware Software IT Solutions Insight Insight is a leading provider of hardware software cloud solutions and IT services to business government education and healthcare clients Learn more Learn Solve Buy Manage Intelligent Technology™ solutions that go beyond IT Learn about trending IT topics Solve with our IT solutions Buy products and services Manage IT solutions with Insight Call now1800INSIGHT Account Login Track Order United States Australia Canada English Canada French Austria Belgium China English China 中文简体 Czech Republic Denmark Finland France Germany Hong Kong Hungary Ireland Italy Netherlands New Zealand Norway Poland Russia Singapore Spain Sweden Switzerland Deutsch Switzerland Français United Kingdom United States Australia Canada English Canada French Austria Belgium China English China 中文简体 Czech Republic Denmark Finland France Germany Hong Kong Hungary Ireland Italy Netherlands New Zealand Norway Poland Russia Singapore Spain Sweden Switzerland Deutsch Switzerland Français United Kingdom United States SEWP Contract 1800INSIGHT 1800INSIGHT Chat Now Account Login Track Order United States Australia Canada English Canada French Austria Belgium China English China 中文简体 Czech Republic Denmark Finland France Germany Hong Kong Hungary Ireland Italy Netherlands New Zealand Norway Poland Russia Singapore Spain Sweden Switzerland Deutsch Switzerland Français United Kingdom United States Australia Canada English Canada French Austria Belgium China English China 中文简体 Czech Republic Denmark Finland France Germany Hong Kong Hungary Ireland Italy Netherlands New Zealand Norway Poland Russia Singapore Spain Sweden Switzerland Deutsch Switzerland Français United Kingdom United States 1800INSIGHT Chat Now Small to medium business Enterprise Federal government Education Service providers Healthcare State and local government More Mobility Security Cloud Networking Software Data center More Notebooks Office 365 Desktops Software Servers Warranties More Ecommerce Procurement Supply chain More Our story Awards Corporate responsibility Management team Contact us Newsroom Careers Investor Relations Partnerships Spiceworks Linked In Facebook Twitter Youtube Google Plus Terms of Sale Terms of Sale IPS Return Policy Terms of Use Privacy Policy Safe Harbor Policy about trending topics Stay informed on new and emerging technologies and learn more about evolving industry trends your challenges Get help resolving your technology challenges with intelligent IT solutions tailored to your business new products and services Shop for hardware software and cloud solutions and services to help you throughout the IT lifecycle your customized purchasing Simplify all aspects of your organization’s purchasing from selection to preparation and delivery Learn about trending IT topics Solve with our IT solutions Buy products and services Manage IT solutions with Insight Call now1800INSIGHT Account Login Track Order United States Australia Canada English Canada French Austria Belgium China English China 中文简体 Czech Republic Denmark Finland France Germany Hong Kong Hungary Ireland Italy Netherlands New Zealand Norway Poland Russia Singapore Spain Sweden Switzerland Deutsch Switzerland Français United Kingdom United States SEWP Contract 1800INSIGHT 1800INSIGHT Chat Now Account Login Track Order United States Australia Canada English Canada French Austria Belgium China English China 中文简体 Czech Republic Denmark Finland France Germany Hong Kong Hungary Ireland Italy Netherlands New Zealand Norway Poland Russia Singapore Spain Sweden Switzerland Deutsch Switzerland Français United Kingdom United States 1800INSIGHT Chat Now Learn Browse our library Small to medium business Enterprise Federal government Education Service providers Healthcare State and local government More Solve Find a solution Mobility Security Cloud Networking Software Data center More Buy Start shopping Notebooks Office 365 Desktops Software Servers Warranties More Manage Save time money Ecommerce Procurement Supply chain More 1800INSIGHT Contact us Chat Frequently asked questions Help topics Our story Awards Corporate responsibility Management team Contact us Newsroom Careers Investor Relations Partnerships Spiceworks Linked In Facebook Twitter Youtube Google Plus ​ Get the newsletter Terms of Sale Terms of Sale IPS Return Policy Terms of Use Privacy Policy Safe Harbor Policy Learn about trending IT topics Solve with our IT solutions Buy products and services Manage IT solutions with Insight Call now1800INSIGHT 1800INSIGHT Contact us Chat Frequently asked questions Help topics Spiceworks Spiceworks Linked In Linked In Facebook Facebook Twitter Twitter Youtube Youtube Google Plus Google Plus ​ Copyright © 2016 Insight</v>
       </c>
     </row>
     <row r="11">
@@ -573,16 +498,7 @@
         <v>developers</v>
       </c>
       <c r="C11" t="str">
-        <v>Web Development, Mobile Apps and Cloud Consulting Company | Promatics Technologies India Promatics is an ISO certified, award winning web and mobile apps development company. We develop and deliver websites and mobile apps for startups, SMEs and enterprise. Web Development India, Mobile Apps Development Company, Web Development Company, App Developers India, Outsourcing to India, Software Development India Company Web Development Mobile Apps Development eCommerce Development CMS Cloud Solutions Validation and Testing IT Consulting Design Hire Dedicated Resources Product Development Processes Work Careers Talk To Us What We Do Our Work Testimonials Awards and Accreditations Blog Our Clients Web Development Mobile App Development Ecommerce Development Cloud Consulting User Experience Design CMS Development Web Development Mobile App Development Ecommerce Development Cloud Consulting User Experience Design CMS Development Auto Kuća Peter Jackson Zolace Jimmbo JumpStart Africa Zupa! Auto Kuća Peter Jackson Zolace Jimmbo JumpStart Africa Zupa! 5 Features that Makes Magento 2 an Irresistible Platform What CES 2016 Brought this Year? 5 Reasons for Getting Excited About Design In 2016 Like What You See? Let’s Work Together Company Services Processes Tweets Watch Movement JJ Threads Poulsbo RV Dr. Ian McColl Follow us on Facebook Follow us on Google Follow us on Twitter Follow us on Linkedin        Home            Company              Main Menu      About Us        Mission and Core Values        Investor Relations        Certifications and Accreditations        Partners        Why Promatics                       Services             Main Menu             Web Development                 All Services        Web Development             PHP          Ruby on Rails          Python          HTML5          Java          Node Js                                   Mobile Apps Development                 All Services        Mobile Apps Development          iPhone Apps Development          iPad Apps Development          Android Development          Cross Platform Frameworks          Wearables                                 eCommerce Development                 All Services        eCommerce Development          Magento Solutions          Custom eCommerce Development          Other eCommerce Development                                 CMS                 All Services        CMS          Drupal          Wordpress          Joomla          Custom Development                                Design                 All Services        Design         User Experience          Responsive Web Design         Analysis and Optimization                                 Cloud Solutions                 All Services        Cloud Solutions          AWS           Google App Engine         SaaS Development          Salesforce                                Validation and Testing                  All Services        Validation and Testing           Security Testing           Performance Testing           QA and Maintenance                               IT Consulting                  All Services        IT Consulting          Web Strategy Consulting           Digital Media Consulting                               Hire Dedicated Resources                        Product Development                         Processes              Main Menu           IT Outsourcing to Promatics         Agile Development        Promatics Engagement Models        Technologies        Project Management        Quality Assurance                          Work               Main Menu       Portfolio        Our Clients        Case Studies        Testimonials                          Blog              Careers             Main Menu       Why Join Us?        Life @ Promatics         Current Openings        Resume Application Form                       Talk to us                Main Menu       Request A Quote        Contact Us                   Home         Company              Main Menu      About Us        Mission and Core Values        Investor Relations        Certifications and Accreditations        Partners        Why Promatics              Main Menu About Us   Mission and Core Values   Investor Relations   Certifications and Accreditations   Partners   Why Promatics          Services             Main Menu             Web Development                 All Services        Web Development             PHP          Ruby on Rails          Python          HTML5          Java          Node Js                                   Mobile Apps Development                 All Services        Mobile Apps Development          iPhone Apps Development          iPad Apps Development          Android Development          Cross Platform Frameworks          Wearables                                 eCommerce Development                 All Services        eCommerce Development          Magento Solutions          Custom eCommerce Development          Other eCommerce Development                                 CMS                 All Services        CMS          Drupal          Wordpress          Joomla          Custom Development                                Design                 All Services        Design         User Experience          Responsive Web Design         Analysis and Optimization                                 Cloud Solutions                 All Services        Cloud Solutions          AWS           Google App Engine         SaaS Development          Salesforce                                Validation and Testing                  All Services        Validation and Testing           Security Testing           Performance Testing           QA and Maintenance                               IT Consulting                  All Services        IT Consulting          Web Strategy Consulting           Digital Media Consulting                               Hire Dedicated Resources                        Product Development                  Main Menu        Web Development                 All Services        Web Development             PHP          Ruby on Rails          Python          HTML5          Java          Node Js                 All Services Web Development   PHP   Ruby on Rails   Python   HTML5   Java   Node Js           Mobile Apps Development                 All Services        Mobile Apps Development          iPhone Apps Development          iPad Apps Development          Android Development          Cross Platform Frameworks          Wearables                 All Services Mobile Apps Development   iPhone Apps Development   iPad Apps Development   Android Development   Cross Platform Frameworks   Wearables           eCommerce Development                 All Services        eCommerce Development          Magento Solutions          Custom eCommerce Development          Other eCommerce Development                 All Services eCommerce Development   Magento Solutions   Custom eCommerce Development   Other eCommerce Development           CMS                 All Services        CMS          Drupal          Wordpress          Joomla          Custom Development                 All Services CMS   Drupal   Wordpress   Joomla   Custom Development           Design                 All Services        Design         User Experience          Responsive Web Design         Analysis and Optimization                 All Services Design  User Experience   Responsive Web Design  Analysis and Optimization           Cloud Solutions                 All Services        Cloud Solutions          AWS           Google App Engine         SaaS Development          Salesforce                 All Services Cloud Solutions   AWS    Google App Engine  SaaS Development   Salesforce           Validation and Testing                  All Services        Validation and Testing           Security Testing           Performance Testing           QA and Maintenance                 All Services Validation and Testing    Security Testing    Performance Testing    QA and Maintenance          IT Consulting                  All Services        IT Consulting          Web Strategy Consulting           Digital Media Consulting                 All Services IT Consulting   Web Strategy Consulting    Digital Media Consulting          Hire Dedicated Resources                Product Development             Processes              Main Menu           IT Outsourcing to Promatics         Agile Development        Promatics Engagement Models        Technologies        Project Management        Quality Assurance                  Main Menu  IT Outsourcing to Promatics    Agile Development   Promatics Engagement Models   Technologies   Project Management   Quality Assurance          Work               Main Menu       Portfolio        Our Clients        Case Studies        Testimonials                  Main Menu  Portfolio   Our Clients   Case Studies   Testimonials          Blog           Careers             Main Menu       Why Join Us?        Life @ Promatics         Current Openings        Resume Application Form                 Main Menu  Why Join Us?   Life @ Promatics    Current Openings   Resume Application Form       Talk to us                Main Menu       Request A Quote        Contact Us                Main Menu  Request A Quote   Contact Us  Home  Company                                             Company            About Us             Mission and Core Values             Investor Relations             Certifications and Accreditations             Partners             Why Promatics                                           About Us   Mission and Core Values   Investor Relations   Certifications and Accreditations   Partners   Why Promatics  Services                                                                             Web Development              PHP               Ruby on Rails               Python               HTML5               Java               Node Js                                      Mobile Apps Development               iPhone Apps Development                iPad Apps Development                Android Development                 Cross Platform Frameworks               Wearables                                      eCommerce Development              Magento Solutions               Custom eCommerce Development               Other eCommerce Development                                      CMS              Drupal               Wordpress               Joomla               Custom Development                                                                    Cloud Solutions             AWS              Google App Engine              SaaS Development              Salesforce                                   Validation and Testing             Security Testing              Performance Testing              QA and Maintenance                                   IT Consulting             Web Strategy Consulting              Digital Media Consulting                                   Design             User Experience              Responsive Web Design              Analysis and Optimization                                                       Hire Dedicated Resources                                  Product Development                                                      PHP   Ruby on Rails   Python   HTML5   Java   Node Js    iPhone Apps Development    iPad Apps Development    Android Development     Cross Platform Frameworks   Wearables   Magento Solutions   Custom eCommerce Development   Other eCommerce Development   Drupal   Wordpress   Joomla   Custom Development   AWS   Google App Engine   SaaS Development   Salesforce   Security Testing   Performance Testing   QA and Maintenance   Web Strategy Consulting   Digital Media Consulting   User Experience   Responsive Web Design   Analysis and Optimization   Processes                                             Processes            IT Outsourcing to Promatics             Agile Development             Promatics Engagement Models             Technologies             Project Management             Quality Assurance                                           IT Outsourcing to Promatics   Agile Development   Promatics Engagement Models   Technologies   Project Management   Quality Assurance   Work                                             Work            Portfolio            Our Clients            Case Studies            Testimonials                                           Portfolio  Our Clients  Case Studies  Testimonials  Blog  Careers                                             Careers            Why Join Us?            Life @ Promatics             Current Openings             Resume Application Form                                           Why Join Us?  Life @ Promatics   Current Openings   Resume Application Form   Talk to us                                             Talk To Us            Request A Quote            Contact Us                                           Request A Quote  Contact Us                                                                  Watch Movement         The story behind watch movement becoming the favorite app of the luxury watches enthusiasts all over the world.         View case study                                                                                                           JJ Threads         How a custom clothing designer module built by Promatics helped J.J Threads break sales records?         View case study                                                                                                               Poulsbo RV         How did we exceed America's Top RV dealer’s expectations?         View case study                                     About Us    Core Values and Vision    Investor Relations    Certifications and Accreditations    Partners    Why Promatics   Web Development  Mobile Apps Development  eCommerce Development  CMS  Cloud Solutions  Validation &amp; Testing   IT Outsourcing to Promatics    Agile Development    Promatics Engagement Models    Technologies    Project Management    Quality Assurance  Careers Sitemap Case Studies Portfolio Blog                 We develop and deliver award-winning, functional, and beautiful web sites that are both technically compliant and aesthetically perfect.                                We bring to life, high performance Mobile Apps which are functionally excellent and carry immersive user experience.                                We help our clients create user-centered Ecommerce solutions for an omni channel world; never losing sight of the fact that effective                                Cloud and SaaS came a long way from being just a cool term. We can identify your requirements precisely; layout optimal cloud solutions                                Promatics’ strives to create unique experiences between the customer and product. We challenge ourselves to achieve functional beauty                                The architecture of the content and presentation should be adapted to the custom requirements and individual needs.                            We develop and deliver award-winning, functional, and beautiful web sites that are both technically compliant and aesthetically perfect.                        We bring to life, high performance Mobile Apps which are functionally excellent and carry immersive user experience.                        We help our clients create user-centered Ecommerce solutions for an omni channel world; never losing sight of the fact that effective                        Cloud and SaaS came a long way from being just a cool term. We can identify your requirements precisely; layout optimal cloud solutions                        Promatics’ strives to create unique experiences between the customer and product. We challenge ourselves to achieve functional beauty                        The architecture of the content and presentation should be adapted to the custom requirements and individual needs.            Autokuca is one of the world’s leading company that sells new and used cars online and deals.. The Peter Jackson Group is the Victorian behemoth in men’s tailored fashion industry. The Group.. Zolace the online Shopping store was brought into reality by two individuals in 2014 who had big dreams.. An online marketplace for commission-free property. A super easy and safe way to list your rooms, apartments.. JumpStart Africa is a crowdfunding platform developed by Promatics for creative projects. Users can list.. Discover a delightful new way to buy &amp; sell all your awesome things.. Autokuca is one of the world’s leading company that sells new and used cars online and deals.. The Peter Jackson Group is the Victorian behemoth in men’s tailored fashion industry. The Group.. Zolace the online Shopping store was brought into reality by two individuals in 2014 who had big dreams.. An online marketplace for commission-free property. A super easy and safe way to list your rooms, apartments.. JumpStart Africa is a crowdfunding platform developed by Promatics for creative projects. Users can list.. Discover a delightful new way to buy &amp; sell all your awesome things..                                 Dr. Ian McColl            Consultant Dermatologist            John Flynn Hospital, Tugun, Gold Coast, Australia                                      I have been involved in online education for some years and recently I needed to a website developed to present examinations to candidates.            Read More            What makes Magento 2 the ultimate ecommerce platform? https://t.co/edOQMWzzxH   #magento2  #magentodevelopment  #magentoshop Copyright © 2016 by Promatics Technologies Pvt Ltd. All Rights Reserved. Home  Company   Main Menu About Us  Mission and Core Values  Investor Relations  Certifications and Accreditations  Partners  Why Promatics  Services   Main Menu Web Development   All Services Web Development  PHP  Ruby on Rails  Python  HTML5  Java  Node Js  Mobile Apps Development   All Services Mobile Apps Development  iPhone Apps Development  iPad Apps Development  Android Development  Cross Platform Frameworks  Wearables  eCommerce Development   All Services eCommerce Development  Magento Solutions  Custom eCommerce Development  Other eCommerce Development  CMS   All Services CMS  Drupal  Wordpress  Joomla  Custom Development  Design   All Services Design User Experience  Responsive Web Design  Analysis and Optimization  Cloud Solutions   All Services Cloud Solutions  AWS   Google App Engine  SaaS Development  Salesforce  Validation and Testing   All Services Validation and Testing  Security Testing  Performance Testing  QA and Maintenance  IT Consulting   All Services IT Consulting  Web Strategy Consulting  Digital Media Consulting  Hire Dedicated Resources  Product Development  Processes  Main Menu IT Outsourcing to Promatics  Agile Development  Promatics Engagement Models  Technologies  Project Management  Quality Assurance  Work  Main Menu Portfolio  Our Clients  Case Studies  Testimonials  Blog  Careers  Main Menu Why Join Us?  Life @ Promatics  Current Openings  Resume Application Form  Talk to us  Main Menu Request A Quote  Contact Us  Contact Us Home  Company About Us Mission and Core Values Investor Relations Certifications and Accreditations Partners Why Promatics Services Web Development PHP Ruby on Rails Python HTML5 Java Node Js Mobile Apps Development  iPhone Apps Development  iPad Apps Development  Android Development   Cross Platform Frameworks Wearables eCommerce Development Magento Solutions Custom eCommerce Development Other eCommerce Development CMS Drupal Wordpress Joomla Custom Development  Cloud Solutions AWS Google App Engine SaaS Development Salesforce Validation and Testing Security Testing Performance Testing QA and Maintenance IT Consulting Web Strategy Consulting Digital Media Consulting Design User Experience Responsive Web Design Analysis and Optimization Hire Dedicated Resources Product Development  Processes IT Outsourcing to Promatics Agile Development Promatics Engagement Models Technologies Project Management Quality Assurance  Work Portfolio Our Clients Case Studies Testimonials Blog  Careers Why Join Us? Life @ Promatics Current Openings Resume Application Form  Talk to us Request A Quote Contact Us View case study View case study View case study Web Development                                                               Mobile App Development                                                               Ecommerce Development                                                               Cloud Consulting                                                               User Experience Design                                                               CMS Development                                                               Web Development                                               Mobile App Development                                               Ecommerce Development                                               Cloud Consulting                                               User Experience Design                                               CMS Development                                               Previous Next                                     Auto Kuća             Autokuca is one of the world’s leading company that sells new and used cars online and deals..                                                                      Peter Jackson             The Peter Jackson Group is the Victorian behemoth in men’s tailored fashion industry. The Group..                                                                      Zolace             Zolace the online Shopping store was brought into reality by two individuals in 2014 who had big dreams..                                                                      Jimmbo             An online marketplace for commission-free property. A super easy and safe way to list your rooms, apartments..                                                                      JumpStart Africa             JumpStart Africa is a crowdfunding platform developed by Promatics for creative projects. Users can list..                                                                      Zupa!             Discover a delightful new way to buy &amp; sell all your awesome things..                                                                Auto Kuća           Autokuca is one of the world’s leading company that sells new and used cars online and deals..                                                          Peter Jackson           The Peter Jackson Group is the Victorian behemoth in men’s tailored fashion industry. The Group..                                                          Zolace           Zolace the online Shopping store was brought into reality by two individuals in 2014 who had big dreams..                                                          Jimmbo           An online marketplace for commission-free property. A super easy and safe way to list your rooms, apartments..                                                          JumpStart Africa           JumpStart Africa is a crowdfunding platform developed by Promatics for creative projects. Users can list..                                                          Zupa!           Discover a delightful new way to buy &amp; sell all your awesome things..                            Previous Next Dr. Ian McColl Read More           5 Features that Makes Magento 2 an Irresistible Platform                   What CES 2016 Brought this Year?                   5 Reasons for Getting Excited About Design In 2016         Request for quote  About Us  Core Values and Vision  Investor Relations  Certifications and Accreditations  Partners  Why Promatics  Web Development  Mobile Apps Development  eCommerce Development  CMS  Cloud Solutions  Validation &amp; Testing  IT Outsourcing to Promatics  Agile Development  Promatics Engagement Models  Technologies  Project Management  Quality Assurance Promatics https://t.co/edOQMWzzxH #magento2 #magentodevelopment #magentoshop Careers Sitemap Case Studies Portfolio Blog Follow us on Facebook Follow us on Google Follow us on Twitter Follow us on Linkedin Consultant Dermatologist John Flynn Hospital, Tugun, Gold Coast, Australia</v>
-      </c>
-      <c r="D11" t="str">
-        <v>Web Development, Mobile Apps and Cloud Consulting Company | Promatics Technologies India Promatics is an ISO certified, award winning web and mobile apps development company. We develop and deliver websites and mobile apps for startups, SMEs and enterprise. Web Development India, Mobile Apps Development Company, Web Development Company, App Developers India, Outsourcing to India, Software Development India Company Web Development Mobile Apps Development eCommerce Development CMS Cloud Solutions Validation and Testing IT Consulting Design Hire Dedicated Resources Product Development Processes Work Careers Talk To Us What We Do Our Work Testimonials Awards and Accreditations Blog Our Clients Web Development Mobile App Development Ecommerce Development Cloud Consulting User Experience Design CMS Development Web Development Mobile App Development Ecommerce Development Cloud Consulting User Experience Design CMS Development Auto Kuća Peter Jackson Zolace Jimmbo JumpStart Africa Zupa! Auto Kuća Peter Jackson Zolace Jimmbo JumpStart Africa Zupa! 5 Features that Makes Magento 2 an Irresistible Platform What CES 2016 Brought this Year? 5 Reasons for Getting Excited About Design In 2016 Like What You See? Let’s Work Together Company Services Processes Tweets Watch Movement JJ Threads Poulsbo RV Dr. Ian McColl Follow us on Facebook Follow us on Google Follow us on Twitter Follow us on Linkedin        Home            Company              Main Menu      About Us        Mission and Core Values        Investor Relations        Certifications and Accreditations        Partners        Why Promatics                       Services             Main Menu             Web Development                 All Services        Web Development             PHP          Ruby on Rails          Python          HTML5          Java          Node Js                                   Mobile Apps Development                 All Services        Mobile Apps Development          iPhone Apps Development          iPad Apps Development          Android Development          Cross Platform Frameworks          Wearables                                 eCommerce Development                 All Services        eCommerce Development          Magento Solutions          Custom eCommerce Development          Other eCommerce Development                                 CMS                 All Services        CMS          Drupal          Wordpress          Joomla          Custom Development                                Design                 All Services        Design         User Experience          Responsive Web Design         Analysis and Optimization                                 Cloud Solutions                 All Services        Cloud Solutions          AWS           Google App Engine         SaaS Development          Salesforce                                Validation and Testing                  All Services        Validation and Testing           Security Testing           Performance Testing           QA and Maintenance                               IT Consulting                  All Services        IT Consulting          Web Strategy Consulting           Digital Media Consulting                               Hire Dedicated Resources                        Product Development                         Processes              Main Menu           IT Outsourcing to Promatics         Agile Development        Promatics Engagement Models        Technologies        Project Management        Quality Assurance                          Work               Main Menu       Portfolio        Our Clients        Case Studies        Testimonials                          Blog              Careers             Main Menu       Why Join Us?        Life @ Promatics         Current Openings        Resume Application Form                       Talk to us                Main Menu       Request A Quote        Contact Us                   Home         Company              Main Menu      About Us        Mission and Core Values        Investor Relations        Certifications and Accreditations        Partners        Why Promatics              Main Menu About Us   Mission and Core Values   Investor Relations   Certifications and Accreditations   Partners   Why Promatics          Services             Main Menu             Web Development                 All Services        Web Development             PHP          Ruby on Rails          Python          HTML5          Java          Node Js                                   Mobile Apps Development                 All Services        Mobile Apps Development          iPhone Apps Development          iPad Apps Development          Android Development          Cross Platform Frameworks          Wearables                                 eCommerce Development                 All Services        eCommerce Development          Magento Solutions          Custom eCommerce Development          Other eCommerce Development                                 CMS                 All Services        CMS          Drupal          Wordpress          Joomla          Custom Development                                Design                 All Services        Design         User Experience          Responsive Web Design         Analysis and Optimization                                 Cloud Solutions                 All Services        Cloud Solutions          AWS           Google App Engine         SaaS Development          Salesforce                                Validation and Testing                  All Services        Validation and Testing           Security Testing           Performance Testing           QA and Maintenance                               IT Consulting                  All Services        IT Consulting          Web Strategy Consulting           Digital Media Consulting                               Hire Dedicated Resources                        Product Development                  Main Menu        Web Development                 All Services        Web Development             PHP          Ruby on Rails          Python          HTML5          Java          Node Js                 All Services Web Development   PHP   Ruby on Rails   Python   HTML5   Java   Node Js           Mobile Apps Development                 All Services        Mobile Apps Development          iPhone Apps Development          iPad Apps Development          Android Development          Cross Platform Frameworks          Wearables                 All Services Mobile Apps Development   iPhone Apps Development   iPad Apps Development   Android Development   Cross Platform Frameworks   Wearables           eCommerce Development                 All Services        eCommerce Development          Magento Solutions          Custom eCommerce Development          Other eCommerce Development                 All Services eCommerce Development   Magento Solutions   Custom eCommerce Development   Other eCommerce Development           CMS                 All Services        CMS          Drupal          Wordpress          Joomla          Custom Development                 All Services CMS   Drupal   Wordpress   Joomla   Custom Development           Design                 All Services        Design         User Experience          Responsive Web Design         Analysis and Optimization                 All Services Design  User Experience   Responsive Web Design  Analysis and Optimization           Cloud Solutions                 All Services        Cloud Solutions          AWS           Google App Engine         SaaS Development          Salesforce                 All Services Cloud Solutions   AWS    Google App Engine  SaaS Development   Salesforce           Validation and Testing                  All Services        Validation and Testing           Security Testing           Performance Testing           QA and Maintenance                 All Services Validation and Testing    Security Testing    Performance Testing    QA and Maintenance          IT Consulting                  All Services        IT Consulting          Web Strategy Consulting           Digital Media Consulting                 All Services IT Consulting   Web Strategy Consulting    Digital Media Consulting          Hire Dedicated Resources                Product Development             Processes              Main Menu           IT Outsourcing to Promatics         Agile Development        Promatics Engagement Models        Technologies        Project Management        Quality Assurance                  Main Menu  IT Outsourcing to Promatics    Agile Development   Promatics Engagement Models   Technologies   Project Management   Quality Assurance          Work               Main Menu       Portfolio        Our Clients        Case Studies        Testimonials                  Main Menu  Portfolio   Our Clients   Case Studies   Testimonials          Blog           Careers             Main Menu       Why Join Us?        Life @ Promatics         Current Openings        Resume Application Form                 Main Menu  Why Join Us?   Life @ Promatics    Current Openings   Resume Application Form       Talk to us                Main Menu       Request A Quote        Contact Us                Main Menu  Request A Quote   Contact Us  Home  Company                                             Company            About Us             Mission and Core Values             Investor Relations             Certifications and Accreditations             Partners             Why Promatics                                           About Us   Mission and Core Values   Investor Relations   Certifications and Accreditations   Partners   Why Promatics  Services                                                                             Web Development              PHP               Ruby on Rails               Python               HTML5               Java               Node Js                                      Mobile Apps Development               iPhone Apps Development                iPad Apps Development                Android Development                 Cross Platform Frameworks               Wearables                                      eCommerce Development              Magento Solutions               Custom eCommerce Development               Other eCommerce Development                                      CMS              Drupal               Wordpress               Joomla               Custom Development                                                                    Cloud Solutions             AWS              Google App Engine              SaaS Development              Salesforce                                   Validation and Testing             Security Testing              Performance Testing              QA and Maintenance                                   IT Consulting             Web Strategy Consulting              Digital Media Consulting                                   Design             User Experience              Responsive Web Design              Analysis and Optimization                                                       Hire Dedicated Resources                                  Product Development                                                      PHP   Ruby on Rails   Python   HTML5   Java   Node Js    iPhone Apps Development    iPad Apps Development    Android Development     Cross Platform Frameworks   Wearables   Magento Solutions   Custom eCommerce Development   Other eCommerce Development   Drupal   Wordpress   Joomla   Custom Development   AWS   Google App Engine   SaaS Development   Salesforce   Security Testing   Performance Testing   QA and Maintenance   Web Strategy Consulting   Digital Media Consulting   User Experience   Responsive Web Design   Analysis and Optimization   Processes                                             Processes            IT Outsourcing to Promatics             Agile Development             Promatics Engagement Models             Technologies             Project Management             Quality Assurance                                           IT Outsourcing to Promatics   Agile Development   Promatics Engagement Models   Technologies   Project Management   Quality Assurance   Work                                             Work            Portfolio            Our Clients            Case Studies            Testimonials                                           Portfolio  Our Clients  Case Studies  Testimonials  Blog  Careers                                             Careers            Why Join Us?            Life @ Promatics             Current Openings             Resume Application Form                                           Why Join Us?  Life @ Promatics   Current Openings   Resume Application Form   Talk to us                                             Talk To Us            Request A Quote            Contact Us                                           Request A Quote  Contact Us                                                                  Watch Movement         The story behind watch movement becoming the favorite app of the luxury watches enthusiasts all over the world.         View case study                                                                                                           JJ Threads         How a custom clothing designer module built by Promatics helped J.J Threads break sales records?         View case study                                                                                                               Poulsbo RV         How did we exceed America's Top RV dealer’s expectations?         View case study                                     About Us    Core Values and Vision    Investor Relations    Certifications and Accreditations    Partners    Why Promatics   Web Development  Mobile Apps Development  eCommerce Development  CMS  Cloud Solutions  Validation &amp; Testing   IT Outsourcing to Promatics    Agile Development    Promatics Engagement Models    Technologies    Project Management    Quality Assurance  Careers Sitemap Case Studies Portfolio Blog                 We develop and deliver award-winning, functional, and beautiful web sites that are both technically compliant and aesthetically perfect.                                We bring to life, high performance Mobile Apps which are functionally excellent and carry immersive user experience.                                We help our clients create user-centered Ecommerce solutions for an omni channel world; never losing sight of the fact that effective                                Cloud and SaaS came a long way from being just a cool term. We can identify your requirements precisely; layout optimal cloud solutions                                Promatics’ strives to create unique experiences between the customer and product. We challenge ourselves to achieve functional beauty                                The architecture of the content and presentation should be adapted to the custom requirements and individual needs.                            We develop and deliver award-winning, functional, and beautiful web sites that are both technically compliant and aesthetically perfect.                        We bring to life, high performance Mobile Apps which are functionally excellent and carry immersive user experience.                        We help our clients create user-centered Ecommerce solutions for an omni channel world; never losing sight of the fact that effective                        Cloud and SaaS came a long way from being just a cool term. We can identify your requirements precisely; layout optimal cloud solutions                        Promatics’ strives to create unique experiences between the customer and product. We challenge ourselves to achieve functional beauty                        The architecture of the content and presentation should be adapted to the custom requirements and individual needs.            Autokuca is one of the world’s leading company that sells new and used cars online and deals.. The Peter Jackson Group is the Victorian behemoth in men’s tailored fashion industry. The Group.. Zolace the online Shopping store was brought into reality by two individuals in 2014 who had big dreams.. An online marketplace for commission-free property. A super easy and safe way to list your rooms, apartments.. JumpStart Africa is a crowdfunding platform developed by Promatics for creative projects. Users can list.. Discover a delightful new way to buy &amp; sell all your awesome things.. Autokuca is one of the world’s leading company that sells new and used cars online and deals.. The Peter Jackson Group is the Victorian behemoth in men’s tailored fashion industry. The Group.. Zolace the online Shopping store was brought into reality by two individuals in 2014 who had big dreams.. An online marketplace for commission-free property. A super easy and safe way to list your rooms, apartments.. JumpStart Africa is a crowdfunding platform developed by Promatics for creative projects. Users can list.. Discover a delightful new way to buy &amp; sell all your awesome things..                                 Dr. Ian McColl            Consultant Dermatologist            John Flynn Hospital, Tugun, Gold Coast, Australia                                      I have been involved in online education for some years and recently I needed to a website developed to present examinations to candidates.            Read More            What makes Magento 2 the ultimate ecommerce platform? https://t.co/edOQMWzzxH   #magento2  #magentodevelopment  #magentoshop Copyright © 2016 by Promatics Technologies Pvt Ltd. All Rights Reserved. Home  Company   Main Menu About Us  Mission and Core Values  Investor Relations  Certifications and Accreditations  Partners  Why Promatics  Services   Main Menu Web Development   All Services Web Development  PHP  Ruby on Rails  Python  HTML5  Java  Node Js  Mobile Apps Development   All Services Mobile Apps Development  iPhone Apps Development  iPad Apps Development  Android Development  Cross Platform Frameworks  Wearables  eCommerce Development   All Services eCommerce Development  Magento Solutions  Custom eCommerce Development  Other eCommerce Development  CMS   All Services CMS  Drupal  Wordpress  Joomla  Custom Development  Design   All Services Design User Experience  Responsive Web Design  Analysis and Optimization  Cloud Solutions   All Services Cloud Solutions  AWS   Google App Engine  SaaS Development  Salesforce  Validation and Testing   All Services Validation and Testing  Security Testing  Performance Testing  QA and Maintenance  IT Consulting   All Services IT Consulting  Web Strategy Consulting  Digital Media Consulting  Hire Dedicated Resources  Product Development  Processes  Main Menu IT Outsourcing to Promatics  Agile Development  Promatics Engagement Models  Technologies  Project Management  Quality Assurance  Work  Main Menu Portfolio  Our Clients  Case Studies  Testimonials  Blog  Careers  Main Menu Why Join Us?  Life @ Promatics  Current Openings  Resume Application Form  Talk to us  Main Menu Request A Quote  Contact Us  Contact Us Home  Company About Us Mission and Core Values Investor Relations Certifications and Accreditations Partners Why Promatics Services Web Development PHP Ruby on Rails Python HTML5 Java Node Js Mobile Apps Development  iPhone Apps Development  iPad Apps Development  Android Development   Cross Platform Frameworks Wearables eCommerce Development Magento Solutions Custom eCommerce Development Other eCommerce Development CMS Drupal Wordpress Joomla Custom Development  Cloud Solutions AWS Google App Engine SaaS Development Salesforce Validation and Testing Security Testing Performance Testing QA and Maintenance IT Consulting Web Strategy Consulting Digital Media Consulting Design User Experience Responsive Web Design Analysis and Optimization Hire Dedicated Resources Product Development  Processes IT Outsourcing to Promatics Agile Development Promatics Engagement Models Technologies Project Management Quality Assurance  Work Portfolio Our Clients Case Studies Testimonials Blog  Careers Why Join Us? Life @ Promatics Current Openings Resume Application Form  Talk to us Request A Quote Contact Us View case study View case study View case study Web Development                                                               Mobile App Development                                                               Ecommerce Development                                                               Cloud Consulting                                                               User Experience Design                                                               CMS Development                                                               Web Development                                               Mobile App Development                                               Ecommerce Development                                               Cloud Consulting                                               User Experience Design                                               CMS Development                                               Previous Next                                     Auto Kuća             Autokuca is one of the world’s leading company that sells new and used cars online and deals..                                                                      Peter Jackson             The Peter Jackson Group is the Victorian behemoth in men’s tailored fashion industry. The Group..                                                                      Zolace             Zolace the online Shopping store was brought into reality by two individuals in 2014 who had big dreams..                                                                      Jimmbo             An online marketplace for commission-free property. A super easy and safe way to list your rooms, apartments..                                                                      JumpStart Africa             JumpStart Africa is a crowdfunding platform developed by Promatics for creative projects. Users can list..                                                                      Zupa!             Discover a delightful new way to buy &amp; sell all your awesome things..                                                                Auto Kuća           Autokuca is one of the world’s leading company that sells new and used cars online and deals..                                                          Peter Jackson           The Peter Jackson Group is the Victorian behemoth in men’s tailored fashion industry. The Group..                                                          Zolace           Zolace the online Shopping store was brought into reality by two individuals in 2014 who had big dreams..                                                          Jimmbo           An online marketplace for commission-free property. A super easy and safe way to list your rooms, apartments..                                                          JumpStart Africa           JumpStart Africa is a crowdfunding platform developed by Promatics for creative projects. Users can list..                                                          Zupa!           Discover a delightful new way to buy &amp; sell all your awesome things..                            Previous Next Dr. Ian McColl Read More           5 Features that Makes Magento 2 an Irresistible Platform                   What CES 2016 Brought this Year?                   5 Reasons for Getting Excited About Design In 2016         Request for quote  About Us  Core Values and Vision  Investor Relations  Certifications and Accreditations  Partners  Why Promatics  Web Development  Mobile Apps Development  eCommerce Development  CMS  Cloud Solutions  Validation &amp; Testing  IT Outsourcing to Promatics  Agile Development  Promatics Engagement Models  Technologies  Project Management  Quality Assurance Promatics https://t.co/edOQMWzzxH #magento2 #magentodevelopment #magentoshop Careers Sitemap Case Studies Portfolio Blog Follow us on Facebook Follow us on Google Follow us on Twitter Follow us on Linkedin Consultant Dermatologist John Flynn Hospital, Tugun, Gold Coast, Australia</v>
-      </c>
-      <c r="E11" t="str">
-        <v>Web Development, Mobile Apps and Cloud Consulting Company | Promatics Technologies India Promatics is an ISO certified, award winning web and mobile apps development company. We develop and deliver websites and mobile apps for startups, SMEs and enterprise. Web Development India, Mobile Apps Development Company, Web Development Company, App Developers India, Outsourcing to India, Software Development India Company Web Development Mobile Apps Development eCommerce Development CMS Cloud Solutions Validation and Testing IT Consulting Design Hire Dedicated Resources Product Development Processes Work Careers Talk To Us What We Do Our Work Testimonials Awards and Accreditations Blog Our Clients Web Development Mobile App Development Ecommerce Development Cloud Consulting User Experience Design CMS Development Web Development Mobile App Development Ecommerce Development Cloud Consulting User Experience Design CMS Development Auto Kuća Peter Jackson Zolace Jimmbo JumpStart Africa Zupa! Auto Kuća Peter Jackson Zolace Jimmbo JumpStart Africa Zupa! 5 Features that Makes Magento 2 an Irresistible Platform What CES 2016 Brought this Year? 5 Reasons for Getting Excited About Design In 2016 Like What You See? Let’s Work Together Company Services Processes Tweets Watch Movement JJ Threads Poulsbo RV Dr. Ian McColl Follow us on Facebook Follow us on Google Follow us on Twitter Follow us on Linkedin        Home            Company              Main Menu      About Us        Mission and Core Values        Investor Relations        Certifications and Accreditations        Partners        Why Promatics                       Services             Main Menu             Web Development                 All Services        Web Development             PHP          Ruby on Rails          Python          HTML5          Java          Node Js                                   Mobile Apps Development                 All Services        Mobile Apps Development          iPhone Apps Development          iPad Apps Development          Android Development          Cross Platform Frameworks          Wearables                                 eCommerce Development                 All Services        eCommerce Development          Magento Solutions          Custom eCommerce Development          Other eCommerce Development                                 CMS                 All Services        CMS          Drupal          Wordpress          Joomla          Custom Development                                Design                 All Services        Design         User Experience          Responsive Web Design         Analysis and Optimization                                 Cloud Solutions                 All Services        Cloud Solutions          AWS           Google App Engine         SaaS Development          Salesforce                                Validation and Testing                  All Services        Validation and Testing           Security Testing           Performance Testing           QA and Maintenance                               IT Consulting                  All Services        IT Consulting          Web Strategy Consulting           Digital Media Consulting                               Hire Dedicated Resources                        Product Development                         Processes              Main Menu           IT Outsourcing to Promatics         Agile Development        Promatics Engagement Models        Technologies        Project Management        Quality Assurance                          Work               Main Menu       Portfolio        Our Clients        Case Studies        Testimonials                          Blog              Careers             Main Menu       Why Join Us?        Life @ Promatics         Current Openings        Resume Application Form                       Talk to us                Main Menu       Request A Quote        Contact Us                   Home         Company              Main Menu      About Us        Mission and Core Values        Investor Relations        Certifications and Accreditations        Partners        Why Promatics              Main Menu About Us   Mission and Core Values   Investor Relations   Certifications and Accreditations   Partners   Why Promatics          Services             Main Menu             Web Development                 All Services        Web Development             PHP          Ruby on Rails          Python          HTML5          Java          Node Js                                   Mobile Apps Development                 All Services        Mobile Apps Development          iPhone Apps Development          iPad Apps Development          Android Development          Cross Platform Frameworks          Wearables                                 eCommerce Development                 All Services        eCommerce Development          Magento Solutions          Custom eCommerce Development          Other eCommerce Development                                 CMS                 All Services        CMS          Drupal          Wordpress          Joomla          Custom Development                                Design                 All Services        Design         User Experience          Responsive Web Design         Analysis and Optimization                                 Cloud Solutions                 All Services        Cloud Solutions          AWS           Google App Engine         SaaS Development          Salesforce                                Validation and Testing                  All Services        Validation and Testing           Security Testing           Performance Testing           QA and Maintenance                               IT Consulting                  All Services        IT Consulting          Web Strategy Consulting           Digital Media Consulting                               Hire Dedicated Resources                        Product Development                  Main Menu        Web Development                 All Services        Web Development             PHP          Ruby on Rails          Python          HTML5          Java          Node Js                 All Services Web Development   PHP   Ruby on Rails   Python   HTML5   Java   Node Js           Mobile Apps Development                 All Services        Mobile Apps Development          iPhone Apps Development          iPad Apps Development          Android Development          Cross Platform Frameworks          Wearables                 All Services Mobile Apps Development   iPhone Apps Development   iPad Apps Development   Android Development   Cross Platform Frameworks   Wearables           eCommerce Development                 All Services        eCommerce Development          Magento Solutions          Custom eCommerce Development          Other eCommerce Development                 All Services eCommerce Development   Magento Solutions   Custom eCommerce Development   Other eCommerce Development           CMS                 All Services        CMS          Drupal          Wordpress          Joomla          Custom Development                 All Services CMS   Drupal   Wordpress   Joomla   Custom Development           Design                 All Services        Design         User Experience          Responsive Web Design         Analysis and Optimization                 All Services Design  User Experience   Responsive Web Design  Analysis and Optimization           Cloud Solutions                 All Services        Cloud Solutions          AWS           Google App Engine         SaaS Development          Salesforce                 All Services Cloud Solutions   AWS    Google App Engine  SaaS Development   Salesforce           Validation and Testing                  All Services        Validation and Testing           Security Testing           Performance Testing           QA and Maintenance                 All Services Validation and Testing    Security Testing    Performance Testing    QA and Maintenance          IT Consulting                  All Services        IT Consulting          Web Strategy Consulting           Digital Media Consulting                 All Services IT Consulting   Web Strategy Consulting    Digital Media Consulting          Hire Dedicated Resources                Product Development             Processes              Main Menu           IT Outsourcing to Promatics         Agile Development        Promatics Engagement Models        Technologies        Project Management        Quality Assurance                  Main Menu  IT Outsourcing to Promatics    Agile Development   Promatics Engagement Models   Technologies   Project Management   Quality Assurance          Work               Main Menu       Portfolio        Our Clients        Case Studies        Testimonials                  Main Menu  Portfolio   Our Clients   Case Studies   Testimonials          Blog           Careers             Main Menu       Why Join Us?        Life @ Promatics         Current Openings        Resume Application Form                 Main Menu  Why Join Us?   Life @ Promatics    Current Openings   Resume Application Form       Talk to us                Main Menu       Request A Quote        Contact Us                Main Menu  Request A Quote   Contact Us  Home  Company                                             Company            About Us             Mission and Core Values             Investor Relations             Certifications and Accreditations             Partners             Why Promatics                                           About Us   Mission and Core Values   Investor Relations   Certifications and Accreditations   Partners   Why Promatics  Services                                                                             Web Development              PHP               Ruby on Rails               Python               HTML5               Java               Node Js                                      Mobile Apps Development               iPhone Apps Development                iPad Apps Development                Android Development                 Cross Platform Frameworks               Wearables                                      eCommerce Development              Magento Solutions               Custom eCommerce Development               Other eCommerce Development                                      CMS              Drupal               Wordpress               Joomla               Custom Development                                                                    Cloud Solutions             AWS              Google App Engine              SaaS Development              Salesforce                                   Validation and Testing             Security Testing              Performance Testing              QA and Maintenance                                   IT Consulting             Web Strategy Consulting              Digital Media Consulting                                   Design             User Experience              Responsive Web Design              Analysis and Optimization                                                       Hire Dedicated Resources                                  Product Development                                                      PHP   Ruby on Rails   Python   HTML5   Java   Node Js    iPhone Apps Development    iPad Apps Development    Android Development     Cross Platform Frameworks   Wearables   Magento Solutions   Custom eCommerce Development   Other eCommerce Development   Drupal   Wordpress   Joomla   Custom Development   AWS   Google App Engine   SaaS Development   Salesforce   Security Testing   Performance Testing   QA and Maintenance   Web Strategy Consulting   Digital Media Consulting   User Experience   Responsive Web Design   Analysis and Optimization   Processes                                             Processes            IT Outsourcing to Promatics             Agile Development             Promatics Engagement Models             Technologies             Project Management             Quality Assurance                                           IT Outsourcing to Promatics   Agile Development   Promatics Engagement Models   Technologies   Project Management   Quality Assurance   Work                                             Work            Portfolio            Our Clients            Case Studies            Testimonials                                           Portfolio  Our Clients  Case Studies  Testimonials  Blog  Careers                                             Careers            Why Join Us?            Life @ Promatics             Current Openings             Resume Application Form                                           Why Join Us?  Life @ Promatics   Current Openings   Resume Application Form   Talk to us                                             Talk To Us            Request A Quote            Contact Us                                           Request A Quote  Contact Us                                                                  Watch Movement         The story behind watch movement becoming the favorite app of the luxury watches enthusiasts all over the world.         View case study                                                                                                           JJ Threads         How a custom clothing designer module built by Promatics helped J.J Threads break sales records?         View case study                                                                                                               Poulsbo RV         How did we exceed America's Top RV dealer’s expectations?         View case study                                     About Us    Core Values and Vision    Investor Relations    Certifications and Accreditations    Partners    Why Promatics   Web Development  Mobile Apps Development  eCommerce Development  CMS  Cloud Solutions  Validation &amp; Testing   IT Outsourcing to Promatics    Agile Development    Promatics Engagement Models    Technologies    Project Management    Quality Assurance  Careers Sitemap Case Studies Portfolio Blog                 We develop and deliver award-winning, functional, and beautiful web sites that are both technically compliant and aesthetically perfect.                                We bring to life, high performance Mobile Apps which are functionally excellent and carry immersive user experience.                                We help our clients create user-centered Ecommerce solutions for an omni channel world; never losing sight of the fact that effective                                Cloud and SaaS came a long way from being just a cool term. We can identify your requirements precisely; layout optimal cloud solutions                                Promatics’ strives to create unique experiences between the customer and product. We challenge ourselves to achieve functional beauty                                The architecture of the content and presentation should be adapted to the custom requirements and individual needs.                            We develop and deliver award-winning, functional, and beautiful web sites that are both technically compliant and aesthetically perfect.                        We bring to life, high performance Mobile Apps which are functionally excellent and carry immersive user experience.                        We help our clients create user-centered Ecommerce solutions for an omni channel world; never losing sight of the fact that effective                        Cloud and SaaS came a long way from being just a cool term. We can identify your requirements precisely; layout optimal cloud solutions                        Promatics’ strives to create unique experiences between the customer and product. We challenge ourselves to achieve functional beauty                        The architecture of the content and presentation should be adapted to the custom requirements and individual needs.            Autokuca is one of the world’s leading company that sells new and used cars online and deals.. The Peter Jackson Group is the Victorian behemoth in men’s tailored fashion industry. The Group.. Zolace the online Shopping store was brought into reality by two individuals in 2014 who had big dreams.. An online marketplace for commission-free property. A super easy and safe way to list your rooms, apartments.. JumpStart Africa is a crowdfunding platform developed by Promatics for creative projects. Users can list.. Discover a delightful new way to buy &amp; sell all your awesome things.. Autokuca is one of the world’s leading company that sells new and used cars online and deals.. The Peter Jackson Group is the Victorian behemoth in men’s tailored fashion industry. The Group.. Zolace the online Shopping store was brought into reality by two individuals in 2014 who had big dreams.. An online marketplace for commission-free property. A super easy and safe way to list your rooms, apartments.. JumpStart Africa is a crowdfunding platform developed by Promatics for creative projects. Users can list.. Discover a delightful new way to buy &amp; sell all your awesome things..                                 Dr. Ian McColl            Consultant Dermatologist            John Flynn Hospital, Tugun, Gold Coast, Australia                                      I have been involved in online education for some years and recently I needed to a website developed to present examinations to candidates.            Read More            What makes Magento 2 the ultimate ecommerce platform? https://t.co/edOQMWzzxH   #magento2  #magentodevelopment  #magentoshop Copyright © 2016 by Promatics Technologies Pvt Ltd. All Rights Reserved. Home  Company   Main Menu About Us  Mission and Core Values  Investor Relations  Certifications and Accreditations  Partners  Why Promatics  Services   Main Menu Web Development   All Services Web Development  PHP  Ruby on Rails  Python  HTML5  Java  Node Js  Mobile Apps Development   All Services Mobile Apps Development  iPhone Apps Development  iPad Apps Development  Android Development  Cross Platform Frameworks  Wearables  eCommerce Development   All Services eCommerce Development  Magento Solutions  Custom eCommerce Development  Other eCommerce Development  CMS   All Services CMS  Drupal  Wordpress  Joomla  Custom Development  Design   All Services Design User Experience  Responsive Web Design  Analysis and Optimization  Cloud Solutions   All Services Cloud Solutions  AWS   Google App Engine  SaaS Development  Salesforce  Validation and Testing   All Services Validation and Testing  Security Testing  Performance Testing  QA and Maintenance  IT Consulting   All Services IT Consulting  Web Strategy Consulting  Digital Media Consulting  Hire Dedicated Resources  Product Development  Processes  Main Menu IT Outsourcing to Promatics  Agile Development  Promatics Engagement Models  Technologies  Project Management  Quality Assurance  Work  Main Menu Portfolio  Our Clients  Case Studies  Testimonials  Blog  Careers  Main Menu Why Join Us?  Life @ Promatics  Current Openings  Resume Application Form  Talk to us  Main Menu Request A Quote  Contact Us  Contact Us Home  Company About Us Mission and Core Values Investor Relations Certifications and Accreditations Partners Why Promatics Services Web Development PHP Ruby on Rails Python HTML5 Java Node Js Mobile Apps Development  iPhone Apps Development  iPad Apps Development  Android Development   Cross Platform Frameworks Wearables eCommerce Development Magento Solutions Custom eCommerce Development Other eCommerce Development CMS Drupal Wordpress Joomla Custom Development  Cloud Solutions AWS Google App Engine SaaS Development Salesforce Validation and Testing Security Testing Performance Testing QA and Maintenance IT Consulting Web Strategy Consulting Digital Media Consulting Design User Experience Responsive Web Design Analysis and Optimization Hire Dedicated Resources Product Development  Processes IT Outsourcing to Promatics Agile Development Promatics Engagement Models Technologies Project Management Quality Assurance  Work Portfolio Our Clients Case Studies Testimonials Blog  Careers Why Join Us? Life @ Promatics Current Openings Resume Application Form  Talk to us Request A Quote Contact Us View case study View case study View case study Web Development                                                               Mobile App Development                                                               Ecommerce Development                                                               Cloud Consulting                                                               User Experience Design                                                               CMS Development                                                               Web Development                                               Mobile App Development                                               Ecommerce Development                                               Cloud Consulting                                               User Experience Design                                               CMS Development                                               Previous Next                                     Auto Kuća             Autokuca is one of the world’s leading company that sells new and used cars online and deals..                                                                      Peter Jackson             The Peter Jackson Group is the Victorian behemoth in men’s tailored fashion industry. The Group..                                                                      Zolace             Zolace the online Shopping store was brought into reality by two individuals in 2014 who had big dreams..                                                                      Jimmbo             An online marketplace for commission-free property. A super easy and safe way to list your rooms, apartments..                                                                      JumpStart Africa             JumpStart Africa is a crowdfunding platform developed by Promatics for creative projects. Users can list..                                                                      Zupa!             Discover a delightful new way to buy &amp; sell all your awesome things..                                                                Auto Kuća           Autokuca is one of the world’s leading company that sells new and used cars online and deals..                                                          Peter Jackson           The Peter Jackson Group is the Victorian behemoth in men’s tailored fashion industry. The Group..                                                          Zolace           Zolace the online Shopping store was brought into reality by two individuals in 2014 who had big dreams..                                                          Jimmbo           An online marketplace for commission-free property. A super easy and safe way to list your rooms, apartments..                                                          JumpStart Africa           JumpStart Africa is a crowdfunding platform developed by Promatics for creative projects. Users can list..                                                          Zupa!           Discover a delightful new way to buy &amp; sell all your awesome things..                            Previous Next Dr. Ian McColl Read More           5 Features that Makes Magento 2 an Irresistible Platform                   What CES 2016 Brought this Year?                   5 Reasons for Getting Excited About Design In 2016         Request for quote  About Us  Core Values and Vision  Investor Relations  Certifications and Accreditations  Partners  Why Promatics  Web Development  Mobile Apps Development  eCommerce Development  CMS  Cloud Solutions  Validation &amp; Testing  IT Outsourcing to Promatics  Agile Development  Promatics Engagement Models  Technologies  Project Management  Quality Assurance Promatics https://t.co/edOQMWzzxH #magento2 #magentodevelopment #magentoshop Careers Sitemap Case Studies Portfolio Blog Follow us on Facebook Follow us on Google Follow us on Twitter Follow us on Linkedin Consultant Dermatologist John Flynn Hospital, Tugun, Gold Coast, Australia</v>
-      </c>
-      <c r="F11" t="str">
-        <v>Web Development, Mobile Apps and Cloud Consulting Company | Promatics Technologies India Promatics is an ISO certified, award winning web and mobile apps development company. We develop and deliver websites and mobile apps for startups, SMEs and enterprise. Web Development India, Mobile Apps Development Company, Web Development Company, App Developers India, Outsourcing to India, Software Development India Company Web Development Mobile Apps Development eCommerce Development CMS Cloud Solutions Validation and Testing IT Consulting Design Hire Dedicated Resources Product Development Processes Work Careers Talk To Us What We Do Our Work Testimonials Awards and Accreditations Blog Our Clients Web Development Mobile App Development Ecommerce Development Cloud Consulting User Experience Design CMS Development Web Development Mobile App Development Ecommerce Development Cloud Consulting User Experience Design CMS Development Auto Kuća Peter Jackson Zolace Jimmbo JumpStart Africa Zupa! Auto Kuća Peter Jackson Zolace Jimmbo JumpStart Africa Zupa! 5 Features that Makes Magento 2 an Irresistible Platform What CES 2016 Brought this Year? 5 Reasons for Getting Excited About Design In 2016 Like What You See? Let’s Work Together Company Services Processes Tweets Watch Movement JJ Threads Poulsbo RV Dr. Ian McColl Follow us on Facebook Follow us on Google Follow us on Twitter Follow us on Linkedin        Home            Company              Main Menu      About Us        Mission and Core Values        Investor Relations        Certifications and Accreditations        Partners        Why Promatics                       Services             Main Menu             Web Development                 All Services        Web Development             PHP          Ruby on Rails          Python          HTML5          Java          Node Js                                   Mobile Apps Development                 All Services        Mobile Apps Development          iPhone Apps Development          iPad Apps Development          Android Development          Cross Platform Frameworks          Wearables                                 eCommerce Development                 All Services        eCommerce Development          Magento Solutions          Custom eCommerce Development          Other eCommerce Development                                 CMS                 All Services        CMS          Drupal          Wordpress          Joomla          Custom Development                                Design                 All Services        Design         User Experience          Responsive Web Design         Analysis and Optimization                                 Cloud Solutions                 All Services        Cloud Solutions          AWS           Google App Engine         SaaS Development          Salesforce                                Validation and Testing                  All Services        Validation and Testing           Security Testing           Performance Testing           QA and Maintenance                               IT Consulting                  All Services        IT Consulting          Web Strategy Consulting           Digital Media Consulting                               Hire Dedicated Resources                        Product Development                         Processes              Main Menu           IT Outsourcing to Promatics         Agile Development        Promatics Engagement Models        Technologies        Project Management        Quality Assurance                          Work               Main Menu       Portfolio        Our Clients        Case Studies        Testimonials                          Blog              Careers             Main Menu       Why Join Us?        Life @ Promatics         Current Openings        Resume Application Form                       Talk to us                Main Menu       Request A Quote        Contact Us                   Home         Company              Main Menu      About Us        Mission and Core Values        Investor Relations        Certifications and Accreditations        Partners        Why Promatics              Main Menu About Us   Mission and Core Values   Investor Relations   Certifications and Accreditations   Partners   Why Promatics          Services             Main Menu             Web Development                 All Services        Web Development             PHP          Ruby on Rails          Python          HTML5          Java          Node Js                                   Mobile Apps Development                 All Services        Mobile Apps Development          iPhone Apps Development          iPad Apps Development          Android Development          Cross Platform Frameworks          Wearables                                 eCommerce Development                 All Services        eCommerce Development          Magento Solutions          Custom eCommerce Development          Other eCommerce Development                                 CMS                 All Services        CMS          Drupal          Wordpress          Joomla          Custom Development                                Design                 All Services        Design         User Experience          Responsive Web Design         Analysis and Optimization                                 Cloud Solutions                 All Services        Cloud Solutions          AWS           Google App Engine         SaaS Development          Salesforce                                Validation and Testing                  All Services        Validation and Testing           Security Testing           Performance Testing           QA and Maintenance                               IT Consulting                  All Services        IT Consulting          Web Strategy Consulting           Digital Media Consulting                               Hire Dedicated Resources                        Product Development                  Main Menu        Web Development                 All Services        Web Development             PHP          Ruby on Rails          Python          HTML5          Java          Node Js                 All Services Web Development   PHP   Ruby on Rails   Python   HTML5   Java   Node Js           Mobile Apps Development                 All Services        Mobile Apps Development          iPhone Apps Development          iPad Apps Development          Android Development          Cross Platform Frameworks          Wearables                 All Services Mobile Apps Development   iPhone Apps Development   iPad Apps Development   Android Development   Cross Platform Frameworks   Wearables           eCommerce Development                 All Services        eCommerce Development          Magento Solutions          Custom eCommerce Development          Other eCommerce Development                 All Services eCommerce Development   Magento Solutions   Custom eCommerce Development   Other eCommerce Development           CMS                 All Services        CMS          Drupal          Wordpress          Joomla          Custom Development                 All Services CMS   Drupal   Wordpress   Joomla   Custom Development           Design                 All Services        Design         User Experience          Responsive Web Design         Analysis and Optimization                 All Services Design  User Experience   Responsive Web Design  Analysis and Optimization           Cloud Solutions                 All Services        Cloud Solutions          AWS           Google App Engine         SaaS Development          Salesforce                 All Services Cloud Solutions   AWS    Google App Engine  SaaS Development   Salesforce           Validation and Testing                  All Services        Validation and Testing           Security Testing           Performance Testing           QA and Maintenance                 All Services Validation and Testing    Security Testing    Performance Testing    QA and Maintenance          IT Consulting                  All Services        IT Consulting          Web Strategy Consulting           Digital Media Consulting                 All Services IT Consulting   Web Strategy Consulting    Digital Media Consulting          Hire Dedicated Resources                Product Development             Processes              Main Menu           IT Outsourcing to Promatics         Agile Development        Promatics Engagement Models        Technologies        Project Management        Quality Assurance                  Main Menu  IT Outsourcing to Promatics    Agile Development   Promatics Engagement Models   Technologies   Project Management   Quality Assurance          Work               Main Menu       Portfolio        Our Clients        Case Studies        Testimonials                  Main Menu  Portfolio   Our Clients   Case Studies   Testimonials          Blog           Careers             Main Menu       Why Join Us?        Life @ Promatics         Current Openings        Resume Application Form                 Main Menu  Why Join Us?   Life @ Promatics    Current Openings   Resume Application Form       Talk to us                Main Menu       Request A Quote        Contact Us                Main Menu  Request A Quote   Contact Us  Home  Company                                             Company            About Us             Mission and Core Values             Investor Relations             Certifications and Accreditations             Partners             Why Promatics                                           About Us   Mission and Core Values   Investor Relations   Certifications and Accreditations   Partners   Why Promatics  Services                                                                             Web Development              PHP               Ruby on Rails               Python               HTML5               Java               Node Js                                      Mobile Apps Development               iPhone Apps Development                iPad Apps Development                Android Development                 Cross Platform Frameworks               Wearables                                      eCommerce Development              Magento Solutions               Custom eCommerce Development               Other eCommerce Development                                      CMS              Drupal               Wordpress               Joomla               Custom Development                                                                    Cloud Solutions             AWS              Google App Engine              SaaS Development              Salesforce                                   Validation and Testing             Security Testing              Performance Testing              QA and Maintenance                                   IT Consulting             Web Strategy Consulting              Digital Media Consulting                                   Design             User Experience              Responsive Web Design              Analysis and Optimization                                                       Hire Dedicated Resources                                  Product Development                                                      PHP   Ruby on Rails   Python   HTML5   Java   Node Js    iPhone Apps Development    iPad Apps Development    Android Development     Cross Platform Frameworks   Wearables   Magento Solutions   Custom eCommerce Development   Other eCommerce Development   Drupal   Wordpress   Joomla   Custom Development   AWS   Google App Engine   SaaS Development   Salesforce   Security Testing   Performance Testing   QA and Maintenance   Web Strategy Consulting   Digital Media Consulting   User Experience   Responsive Web Design   Analysis and Optimization   Processes                                             Processes            IT Outsourcing to Promatics             Agile Development             Promatics Engagement Models             Technologies             Project Management             Quality Assurance                                           IT Outsourcing to Promatics   Agile Development   Promatics Engagement Models   Technologies   Project Management   Quality Assurance   Work                                             Work            Portfolio            Our Clients            Case Studies            Testimonials                                           Portfolio  Our Clients  Case Studies  Testimonials  Blog  Careers                                             Careers            Why Join Us?            Life @ Promatics             Current Openings             Resume Application Form                                           Why Join Us?  Life @ Promatics   Current Openings   Resume Application Form   Talk to us                                             Talk To Us            Request A Quote            Contact Us                                           Request A Quote  Contact Us                                                                  Watch Movement         The story behind watch movement becoming the favorite app of the luxury watches enthusiasts all over the world.         View case study                                                                                                           JJ Threads         How a custom clothing designer module built by Promatics helped J.J Threads break sales records?         View case study                                                                                                               Poulsbo RV         How did we exceed America's Top RV dealer’s expectations?         View case study                                     About Us    Core Values and Vision    Investor Relations    Certifications and Accreditations    Partners    Why Promatics   Web Development  Mobile Apps Development  eCommerce Development  CMS  Cloud Solutions  Validation &amp; Testing   IT Outsourcing to Promatics    Agile Development    Promatics Engagement Models    Technologies    Project Management    Quality Assurance  Careers Sitemap Case Studies Portfolio Blog                 We develop and deliver award-winning, functional, and beautiful web sites that are both technically compliant and aesthetically perfect.                                We bring to life, high performance Mobile Apps which are functionally excellent and carry immersive user experience.                                We help our clients create user-centered Ecommerce solutions for an omni channel world; never losing sight of the fact that effective                                Cloud and SaaS came a long way from being just a cool term. We can identify your requirements precisely; layout optimal cloud solutions                                Promatics’ strives to create unique experiences between the customer and product. We challenge ourselves to achieve functional beauty                                The architecture of the content and presentation should be adapted to the custom requirements and individual needs.                            We develop and deliver award-winning, functional, and beautiful web sites that are both technically compliant and aesthetically perfect.                        We bring to life, high performance Mobile Apps which are functionally excellent and carry immersive user experience.                        We help our clients create user-centered Ecommerce solutions for an omni channel world; never losing sight of the fact that effective                        Cloud and SaaS came a long way from being just a cool term. We can identify your requirements precisely; layout optimal cloud solutions                        Promatics’ strives to create unique experiences between the customer and product. We challenge ourselves to achieve functional beauty                        The architecture of the content and presentation should be adapted to the custom requirements and individual needs.            Autokuca is one of the world’s leading company that sells new and used cars online and deals.. The Peter Jackson Group is the Victorian behemoth in men’s tailored fashion industry. The Group.. Zolace the online Shopping store was brought into reality by two individuals in 2014 who had big dreams.. An online marketplace for commission-free property. A super easy and safe way to list your rooms, apartments.. JumpStart Africa is a crowdfunding platform developed by Promatics for creative projects. Users can list.. Discover a delightful new way to buy &amp; sell all your awesome things.. Autokuca is one of the world’s leading company that sells new and used cars online and deals.. The Peter Jackson Group is the Victorian behemoth in men’s tailored fashion industry. The Group.. Zolace the online Shopping store was brought into reality by two individuals in 2014 who had big dreams.. An online marketplace for commission-free property. A super easy and safe way to list your rooms, apartments.. JumpStart Africa is a crowdfunding platform developed by Promatics for creative projects. Users can list.. Discover a delightful new way to buy &amp; sell all your awesome things..                                 Dr. Ian McColl            Consultant Dermatologist            John Flynn Hospital, Tugun, Gold Coast, Australia                                      I have been involved in online education for some years and recently I needed to a website developed to present examinations to candidates.            Read More            What makes Magento 2 the ultimate ecommerce platform? https://t.co/edOQMWzzxH   #magento2  #magentodevelopment  #magentoshop Copyright © 2016 by Promatics Technologies Pvt Ltd. All Rights Reserved. Home  Company   Main Menu About Us  Mission and Core Values  Investor Relations  Certifications and Accreditations  Partners  Why Promatics  Services   Main Menu Web Development   All Services Web Development  PHP  Ruby on Rails  Python  HTML5  Java  Node Js  Mobile Apps Development   All Services Mobile Apps Development  iPhone Apps Development  iPad Apps Development  Android Development  Cross Platform Frameworks  Wearables  eCommerce Development   All Services eCommerce Development  Magento Solutions  Custom eCommerce Development  Other eCommerce Development  CMS   All Services CMS  Drupal  Wordpress  Joomla  Custom Development  Design   All Services Design User Experience  Responsive Web Design  Analysis and Optimization  Cloud Solutions   All Services Cloud Solutions  AWS   Google App Engine  SaaS Development  Salesforce  Validation and Testing   All Services Validation and Testing  Security Testing  Performance Testing  QA and Maintenance  IT Consulting   All Services IT Consulting  Web Strategy Consulting  Digital Media Consulting  Hire Dedicated Resources  Product Development  Processes  Main Menu IT Outsourcing to Promatics  Agile Development  Promatics Engagement Models  Technologies  Project Management  Quality Assurance  Work  Main Menu Portfolio  Our Clients  Case Studies  Testimonials  Blog  Careers  Main Menu Why Join Us?  Life @ Promatics  Current Openings  Resume Application Form  Talk to us  Main Menu Request A Quote  Contact Us  Contact Us Home  Company About Us Mission and Core Values Investor Relations Certifications and Accreditations Partners Why Promatics Services Web Development PHP Ruby on Rails Python HTML5 Java Node Js Mobile Apps Development  iPhone Apps Development  iPad Apps Development  Android Development   Cross Platform Frameworks Wearables eCommerce Development Magento Solutions Custom eCommerce Development Other eCommerce Development CMS Drupal Wordpress Joomla Custom Development  Cloud Solutions AWS Google App Engine SaaS Development Salesforce Validation and Testing Security Testing Performance Testing QA and Maintenance IT Consulting Web Strategy Consulting Digital Media Consulting Design User Experience Responsive Web Design Analysis and Optimization Hire Dedicated Resources Product Development  Processes IT Outsourcing to Promatics Agile Development Promatics Engagement Models Technologies Project Management Quality Assurance  Work Portfolio Our Clients Case Studies Testimonials Blog  Careers Why Join Us? Life @ Promatics Current Openings Resume Application Form  Talk to us Request A Quote Contact Us View case study View case study View case study Web Development                                                               Mobile App Development                                                               Ecommerce Development                                                               Cloud Consulting                                                               User Experience Design                                                               CMS Development                                                               Web Development                                               Mobile App Development                                               Ecommerce Development                                               Cloud Consulting                                               User Experience Design                                               CMS Development                                               Previous Next                                     Auto Kuća             Autokuca is one of the world’s leading company that sells new and used cars online and deals..                                                                      Peter Jackson             The Peter Jackson Group is the Victorian behemoth in men’s tailored fashion industry. The Group..                                                                      Zolace             Zolace the online Shopping store was brought into reality by two individuals in 2014 who had big dreams..                                                                      Jimmbo             An online marketplace for commission-free property. A super easy and safe way to list your rooms, apartments..                                                                      JumpStart Africa             JumpStart Africa is a crowdfunding platform developed by Promatics for creative projects. Users can list..                                                                      Zupa!             Discover a delightful new way to buy &amp; sell all your awesome things..                                                                Auto Kuća           Autokuca is one of the world’s leading company that sells new and used cars online and deals..                                                          Peter Jackson           The Peter Jackson Group is the Victorian behemoth in men’s tailored fashion industry. The Group..                                                          Zolace           Zolace the online Shopping store was brought into reality by two individuals in 2014 who had big dreams..                                                          Jimmbo           An online marketplace for commission-free property. A super easy and safe way to list your rooms, apartments..                                                          JumpStart Africa           JumpStart Africa is a crowdfunding platform developed by Promatics for creative projects. Users can list..                                                          Zupa!           Discover a delightful new way to buy &amp; sell all your awesome things..                            Previous Next Dr. Ian McColl Read More           5 Features that Makes Magento 2 an Irresistible Platform                   What CES 2016 Brought this Year?                   5 Reasons for Getting Excited About Design In 2016         Request for quote  About Us  Core Values and Vision  Investor Relations  Certifications and Accreditations  Partners  Why Promatics  Web Development  Mobile Apps Development  eCommerce Development  CMS  Cloud Solutions  Validation &amp; Testing  IT Outsourcing to Promatics  Agile Development  Promatics Engagement Models  Technologies  Project Management  Quality Assurance Promatics https://t.co/edOQMWzzxH #magento2 #magentodevelopment #magentoshop Careers Sitemap Case Studies Portfolio Blog Follow us on Facebook Follow us on Google Follow us on Twitter Follow us on Linkedin Consultant Dermatologist John Flynn Hospital, Tugun, Gold Coast, Australia</v>
+        <v>Web Development Mobile Apps and Cloud Consulting Company Promatics Technologies India Promatics is an ISO certified award winning web and mobile apps development company We develop and deliver websites and mobile apps for startups SMEs and enterprise Web Development India Mobile Apps Development Company Web Development Company App Developers India Outsourcing to India Software Development India Company Web Development Mobile Apps Development eCommerce Development CMS Cloud Solutions Validation and Testing IT Consulting Design Hire Dedicated Resources Product Development Processes Work Careers Talk To Us What We Do Our Work Testimonials Awards and Accreditations Blog Our Clients Web Development Mobile App Development Ecommerce Development Cloud Consulting User Experience Design CMS Development Web Development Mobile App Development Ecommerce Development Cloud Consulting User Experience Design CMS Development Auto Kuća Peter Jackson Zolace Jimmbo JumpStart Africa Zupa Auto Kuća Peter Jackson Zolace Jimmbo JumpStart Africa Zupa 5 Features that Makes Magento 2 an Irresistible Platform What CES 2016 Brought this Year 5 Reasons for Getting Excited About Design In 2016 Like What You See Let’s Work Together Company Services Processes Tweets Watch Movement JJ Threads Poulsbo RV Dr Ian McColl Follow us on Facebook Follow us on Google Follow us on Twitter Follow us on Linkedin Home Company Main Menu About Us Mission and Core Values Investor Relations Certifications and Accreditations Partners Why Promatics Services Main Menu Web Development All Services Web Development PHP Ruby on Rails Python HTML5 Java Node Js Mobile Apps Development All Services Mobile Apps Development iPhone Apps Development iPad Apps Development Android Development Cross Platform Frameworks Wearables eCommerce Development All Services eCommerce Development Magento Solutions Custom eCommerce Development Other eCommerce Development CMS All Services CMS Drupal Wordpress Joomla Custom Development Design All Services Design User Experience Responsive Web Design Analysis and Optimization Cloud Solutions All Services Cloud Solutions AWS Google App Engine SaaS Development Salesforce Validation and Testing All Services Validation and Testing Security Testing Performance Testing QA and Maintenance IT Consulting All Services IT Consulting Web Strategy Consulting Digital Media Consulting Hire Dedicated Resources Product Development Processes Main Menu IT Outsourcing to Promatics Agile Development Promatics Engagement Models Technologies Project Management Quality Assurance Work Main Menu Portfolio Our Clients Case Studies Testimonials Blog Careers Main Menu Why Join Us Life Promatics Current Openings Resume Application Form Talk to us Main Menu Request A Quote Contact Us Home Company Main Menu About Us Mission and Core Values Investor Relations Certifications and Accreditations Partners Why Promatics Main Menu About Us Mission and Core Values Investor Relations Certifications and Accreditations Partners Why Promatics Services Main Menu Web Development All Services Web Development PHP Ruby on Rails Python HTML5 Java Node Js Mobile Apps Development All Services Mobile Apps Development iPhone Apps Development iPad Apps Development Android Development Cross Platform Frameworks Wearables eCommerce Development All Services eCommerce Development Magento Solutions Custom eCommerce Development Other eCommerce Development CMS All Services CMS Drupal Wordpress Joomla Custom Development Design All Services Design User Experience Responsive Web Design Analysis and Optimization Cloud Solutions All Services Cloud Solutions AWS Google App Engine SaaS Development Salesforce Validation and Testing All Services Validation and Testing Security Testing Performance Testing QA and Maintenance IT Consulting All Services IT Consulting Web Strategy Consulting Digital Media Consulting Hire Dedicated Resources Product Development Main Menu Web Development All Services Web Development PHP Ruby on Rails Python HTML5 Java Node Js All Services Web Development PHP Ruby on Rails Python HTML5 Java Node Js Mobile Apps Development All Services Mobile Apps Development iPhone Apps Development iPad Apps Development Android Development Cross Platform Frameworks Wearables All Services Mobile Apps Development iPhone Apps Development iPad Apps Development Android Development Cross Platform Frameworks Wearables eCommerce Development All Services eCommerce Development Magento Solutions Custom eCommerce Development Other eCommerce Development All Services eCommerce Development Magento Solutions Custom eCommerce Development Other eCommerce Development CMS All Services CMS Drupal Wordpress Joomla Custom Development All Services CMS Drupal Wordpress Joomla Custom Development Design All Services Design User Experience Responsive Web Design Analysis and Optimization All Services Design User Experience Responsive Web Design Analysis and Optimization Cloud Solutions All Services Cloud Solutions AWS Google App Engine SaaS Development Salesforce All Services Cloud Solutions AWS Google App Engine SaaS Development Salesforce Validation and Testing All Services Validation and Testing Security Testing Performance Testing QA and Maintenance All Services Validation and Testing Security Testing Performance Testing QA and Maintenance IT Consulting All Services IT Consulting Web Strategy Consulting Digital Media Consulting All Services IT Consulting Web Strategy Consulting Digital Media Consulting Hire Dedicated Resources Product Development Processes Main Menu IT Outsourcing to Promatics Agile Development Promatics Engagement Models Technologies Project Management Quality Assurance Main Menu IT Outsourcing to Promatics Agile Development Promatics Engagement Models Technologies Project Management Quality Assurance Work Main Menu Portfolio Our Clients Case Studies Testimonials Main Menu Portfolio Our Clients Case Studies Testimonials Blog Careers Main Menu Why Join Us Life Promatics Current Openings Resume Application Form Main Menu Why Join Us Life Promatics Current Openings Resume Application Form Talk to us Main Menu Request A Quote Contact Us Main Menu Request A Quote Contact Us Home Company Company About Us Mission and Core Values Investor Relations Certifications and Accreditations Partners Why Promatics About Us Mission and Core Values Investor Relations Certifications and Accreditations Partners Why Promatics Services Web Development PHP Ruby on Rails Python HTML5 Java Node Js Mobile Apps Development iPhone Apps Development iPad Apps Development Android Development Cross Platform Frameworks Wearables eCommerce Development Magento Solutions Custom eCommerce Development Other eCommerce Development CMS Drupal Wordpress Joomla Custom Development Cloud Solutions AWS Google App Engine SaaS Development Salesforce Validation and Testing Security Testing Performance Testing QA and Maintenance IT Consulting Web Strategy Consulting Digital Media Consulting Design User Experience Responsive Web Design Analysis and Optimization Hire Dedicated Resources Product Development PHP Ruby on Rails Python HTML5 Java Node Js iPhone Apps Development iPad Apps Development Android Development Cross Platform Frameworks Wearables Magento Solutions Custom eCommerce Development Other eCommerce Development Drupal Wordpress Joomla Custom Development AWS Google App Engine SaaS Development Salesforce Security Testing Performance Testing QA and Maintenance Web Strategy Consulting Digital Media Consulting User Experience Responsive Web Design Analysis and Optimization Processes Processes IT Outsourcing to Promatics Agile Development Promatics Engagement Models Technologies Project Management Quality Assurance IT Outsourcing to Promatics Agile Development Promatics Engagement Models Technologies Project Management Quality Assurance Work Work Portfolio Our Clients Case Studies Testimonials Portfolio Our Clients Case Studies Testimonials Blog Careers Careers Why Join Us Life Promatics Current Openings Resume Application Form Why Join Us Life Promatics Current Openings Resume Application Form Talk to us Talk To Us Request A Quote Contact Us Request A Quote Contact Us Watch Movement The story behind watch movement becoming the favorite app of the luxury watches enthusiasts all over the world View case study JJ Threads How a custom clothing designer module built by Promatics helped JJ Threads break sales records View case study Poulsbo RV How did we exceed Americas Top RV dealer’s expectations View case study About Us Core Values and Vision Investor Relations Certifications and Accreditations Partners Why Promatics Web Development Mobile Apps Development eCommerce Development CMS Cloud Solutions Validation Testing IT Outsourcing to Promatics Agile Development Promatics Engagement Models Technologies Project Management Quality Assurance Careers Sitemap Case Studies Portfolio Blog We develop and deliver awardwinning functional and beautiful web sites that are both technically compliant and aesthetically perfect We bring to life high performance Mobile Apps which are functionally excellent and carry immersive user experience We help our clients create usercentered Ecommerce solutions for an omni channel world never losing sight of the fact that effective Cloud and SaaS came a long way from being just a cool term We can identify your requirements precisely layout optimal cloud solutions Promatics’ strives to create unique experiences between the customer and product We challenge ourselves to achieve functional beauty The architecture of the content and presentation should be adapted to the custom requirements and individual needs We develop and deliver awardwinning functional and beautiful web sites that are both technically compliant and aesthetically perfect We bring to life high performance Mobile Apps which are functionally excellent and carry immersive user experience We help our clients create usercentered Ecommerce solutions for an omni channel world never losing sight of the fact that effective Cloud and SaaS came a long way from being just a cool term We can identify your requirements precisely layout optimal cloud solutions Promatics’ strives to create unique experiences between the customer and product We challenge ourselves to achieve functional beauty The architecture of the content and presentation should be adapted to the custom requirements and individual needs Autokuca is one of the world’s leading company that sells new and used cars online and deals The Peter Jackson Group is the Victorian behemoth in men’s tailored fashion industry The Group Zolace the online Shopping store was brought into reality by two individuals in 2014 who had big dreams An online marketplace for commissionfree property A super easy and safe way to list your rooms apartments JumpStart Africa is a crowdfunding platform developed by Promatics for creative projects Users can list Discover a delightful new way to buy sell all your awesome things Autokuca is one of the world’s leading company that sells new and used cars online and deals The Peter Jackson Group is the Victorian behemoth in men’s tailored fashion industry The Group Zolace the online Shopping store was brought into reality by two individuals in 2014 who had big dreams An online marketplace for commissionfree property A super easy and safe way to list your rooms apartments JumpStart Africa is a crowdfunding platform developed by Promatics for creative projects Users can list Discover a delightful new way to buy sell all your awesome things Dr Ian McColl Consultant Dermatologist John Flynn Hospital Tugun Gold Coast Australia I have been involved in online education for some years and recently I needed to a website developed to present examinations to candidates Read More What makes Magento 2 the ultimate ecommerce platform httpstcoedOQMWzzxH magento2 magentodevelopment magentoshop Copyright © 2016 by Promatics Technologies Pvt Ltd All Rights Reserved Home Company Main Menu About Us Mission and Core Values Investor Relations Certifications and Accreditations Partners Why Promatics Services Main Menu Web Development All Services Web Development PHP Ruby on Rails Python HTML5 Java Node Js Mobile Apps Development All Services Mobile Apps Development iPhone Apps Development iPad Apps Development Android Development Cross Platform Frameworks Wearables eCommerce Development All Services eCommerce Development Magento Solutions Custom eCommerce Development Other eCommerce Development CMS All Services CMS Drupal Wordpress Joomla Custom Development Design All Services Design User Experience Responsive Web Design Analysis and Optimization Cloud Solutions All Services Cloud Solutions AWS Google App Engine SaaS Development Salesforce Validation and Testing All Services Validation and Testing Security Testing Performance Testing QA and Maintenance IT Consulting All Services IT Consulting Web Strategy Consulting Digital Media Consulting Hire Dedicated Resources Product Development Processes Main Menu IT Outsourcing to Promatics Agile Development Promatics Engagement Models Technologies Project Management Quality Assurance Work Main Menu Portfolio Our Clients Case Studies Testimonials Blog Careers Main Menu Why Join Us Life Promatics Current Openings Resume Application Form Talk to us Main Menu Request A Quote Contact Us Contact Us Home Company About Us Mission and Core Values Investor Relations Certifications and Accreditations Partners Why Promatics Services Web Development PHP Ruby on Rails Python HTML5 Java Node Js Mobile Apps Development iPhone Apps Development iPad Apps Development Android Development Cross Platform Frameworks Wearables eCommerce Development Magento Solutions Custom eCommerce Development Other eCommerce Development CMS Drupal Wordpress Joomla Custom Development Cloud Solutions AWS Google App Engine SaaS Development Salesforce Validation and Testing Security Testing Performance Testing QA and Maintenance IT Consulting Web Strategy Consulting Digital Media Consulting Design User Experience Responsive Web Design Analysis and Optimization Hire Dedicated Resources Product Development Processes IT Outsourcing to Promatics Agile Development Promatics Engagement Models Technologies Project Management Quality Assurance Work Portfolio Our Clients Case Studies Testimonials Blog Careers Why Join Us Life Promatics Current Openings Resume Application Form Talk to us Request A Quote Contact Us View case study View case study View case study Web Development Mobile App Development Ecommerce Development Cloud Consulting User Experience Design CMS Development Web Development Mobile App Development Ecommerce Development Cloud Consulting User Experience Design CMS Development Previous Next Auto Kuća Autokuca is one of the world’s leading company that sells new and used cars online and deals Peter Jackson The Peter Jackson Group is the Victorian behemoth in men’s tailored fashion industry The Group Zolace Zolace the online Shopping store was brought into reality by two individuals in 2014 who had big dreams Jimmbo An online marketplace for commissionfree property A super easy and safe way to list your rooms apartments JumpStart Africa JumpStart Africa is a crowdfunding platform developed by Promatics for creative projects Users can list Zupa Discover a delightful new way to buy sell all your awesome things Auto Kuća Autokuca is one of the world’s leading company that sells new and used cars online and deals Peter Jackson The Peter Jackson Group is the Victorian behemoth in men’s tailored fashion industry The Group Zolace Zolace the online Shopping store was brought into reality by two individuals in 2014 who had big dreams Jimmbo An online marketplace for commissionfree property A super easy and safe way to list your rooms apartments JumpStart Africa JumpStart Africa is a crowdfunding platform developed by Promatics for creative projects Users can list Zupa Discover a delightful new way to buy sell all your awesome things Previous Next Dr Ian McColl Read More 5 Features that Makes Magento 2 an Irresistible Platform What CES 2016 Brought this Year 5 Reasons for Getting Excited About Design In 2016 Request for quote About Us Core Values and Vision Investor Relations Certifications and Accreditations Partners Why Promatics Web Development Mobile Apps Development eCommerce Development CMS Cloud Solutions Validation Testing IT Outsourcing to Promatics Agile Development Promatics Engagement Models Technologies Project Management Quality Assurance Promatics httpstcoedOQMWzzxH magento2 magentodevelopment magentoshop Careers Sitemap Case Studies Portfolio Blog Follow us on Facebook Follow us on Google Follow us on Twitter Follow us on Linkedin Consultant Dermatologist John Flynn Hospital Tugun Gold Coast Australia</v>
       </c>
     </row>
     <row r="12">
@@ -593,16 +509,7 @@
         <v>developers</v>
       </c>
       <c r="C12" t="str">
-        <v>Bilberrry - Digital Agency | Application Design and Development Bilberrry – The Internet Agency WE HELP OUR CLIENTS ACHIEVE THEIR ONLINE GOALS. Services We Offer Companies We’ve Worked With Applications We’ve Built Technologies We Use Our team.From Seattle to Kyiv DESIGN STRATEGY DEVELOPMENT MARKETING home team projects careers contact us Web Application Design Mobile Application Design Responsive Website Design Ecommerce Website Design Logo Design Product Roadmap Strategy Content Marketing Strategy SEO Content Strategy Social Media Advertising Strategy Email Marketing Strategy Custom Web App Development Custom Mobile App Development Website Development Ecommerce Website Development Dedicated or Part-Time Full Stack Development Team Social Media Marketing and Management Services Blog Content Writing Services SEO Copywriting Services Adwords Management Services Paid Social Media Marketing and Manage Email Marketing Services                                                                              Scripting Languages: PHP, Python, Go Frameworks: Yii2, Laravel Tools: Composer, Bower Architecture: REST, Microservices View: HTML5, CSS3 built with Less, Sass, Jade Scripting Languages/Libs: JavaScript, TypeScript, JQuery Frameworks: AngularJS 1 and 2, ReactJS, BackboneJS Cloud Hosting: Amazon AWS, DigitalOcean, others Web Server: Nginx Database: MySQL, PgSQL, Mongodb Caching Servers/Tools: Varnish, Memcached Versioning Control: Git, Svn Deployment Tools: Docker, Vagrant, Ansible, Chef The internet is amazingly beautiful and tremendously powerful. It is also complex, constantly evolving and often misunderstood. Enter Bilberrry, an Internet Agency that knows the web and is here to help. Whether you are launching a new website, building a new web/mobile application, or pursuing new online marketing strategies, Bilberrry has you covered. The internet is part of our identity, and we are here to make it part of yours as well.                        home team projects careers contact us CONTACT US FOR A FREE QUOTE Meet our team CONTACT US FOR A FREE QUOTE UX &amp; UI DESIGN, FRONT-END DEVELOPMENT, BACK-END DEVELOPMENT, BRANDING Trackolade.com UX &amp; UI DESIGN, FRONT-END DEVELOPMENT, BACK-END DEVELOPMENT, BRANDING MyOGSM.com UX &amp; UI DESIGN, FRONT-END DEVELOPMENT, BACK-END DEVELOPMENT, BRANDING Ardentservices.com UX &amp; UI DESIGN, FRONT-END DEVELOPMENT, BACK-END DEVELOPMENT, BRANDING Perflux.com             BACKEND             FRONTEND             INFRASTRUCTURE</v>
-      </c>
-      <c r="D12" t="str">
-        <v>Bilberrry - Digital Agency | Application Design and Development Bilberrry – The Internet Agency WE HELP OUR CLIENTS ACHIEVE THEIR ONLINE GOALS. Services We Offer Companies We’ve Worked With Applications We’ve Built Technologies We Use Our team.From Seattle to Kyiv DESIGN STRATEGY DEVELOPMENT MARKETING home team projects careers contact us Web Application Design Mobile Application Design Responsive Website Design Ecommerce Website Design Logo Design Product Roadmap Strategy Content Marketing Strategy SEO Content Strategy Social Media Advertising Strategy Email Marketing Strategy Custom Web App Development Custom Mobile App Development Website Development Ecommerce Website Development Dedicated or Part-Time Full Stack Development Team Social Media Marketing and Management Services Blog Content Writing Services SEO Copywriting Services Adwords Management Services Paid Social Media Marketing and Manage Email Marketing Services                                                                              Scripting Languages: PHP, Python, Go Frameworks: Yii2, Laravel Tools: Composer, Bower Architecture: REST, Microservices View: HTML5, CSS3 built with Less, Sass, Jade Scripting Languages/Libs: JavaScript, TypeScript, JQuery Frameworks: AngularJS 1 and 2, ReactJS, BackboneJS Cloud Hosting: Amazon AWS, DigitalOcean, others Web Server: Nginx Database: MySQL, PgSQL, Mongodb Caching Servers/Tools: Varnish, Memcached Versioning Control: Git, Svn Deployment Tools: Docker, Vagrant, Ansible, Chef The internet is amazingly beautiful and tremendously powerful. It is also complex, constantly evolving and often misunderstood. Enter Bilberrry, an Internet Agency that knows the web and is here to help. Whether you are launching a new website, building a new web/mobile application, or pursuing new online marketing strategies, Bilberrry has you covered. The internet is part of our identity, and we are here to make it part of yours as well.                        home team projects careers contact us CONTACT US FOR A FREE QUOTE Meet our team CONTACT US FOR A FREE QUOTE UX &amp; UI DESIGN, FRONT-END DEVELOPMENT, BACK-END DEVELOPMENT, BRANDING Trackolade.com UX &amp; UI DESIGN, FRONT-END DEVELOPMENT, BACK-END DEVELOPMENT, BRANDING MyOGSM.com UX &amp; UI DESIGN, FRONT-END DEVELOPMENT, BACK-END DEVELOPMENT, BRANDING Ardentservices.com UX &amp; UI DESIGN, FRONT-END DEVELOPMENT, BACK-END DEVELOPMENT, BRANDING Perflux.com             BACKEND             FRONTEND             INFRASTRUCTURE</v>
-      </c>
-      <c r="E12" t="str">
-        <v>Bilberrry - Digital Agency | Application Design and Development Bilberrry – The Internet Agency WE HELP OUR CLIENTS ACHIEVE THEIR ONLINE GOALS. Services We Offer Companies We’ve Worked With Applications We’ve Built Technologies We Use Our team.From Seattle to Kyiv DESIGN STRATEGY DEVELOPMENT MARKETING home team projects careers contact us Web Application Design Mobile Application Design Responsive Website Design Ecommerce Website Design Logo Design Product Roadmap Strategy Content Marketing Strategy SEO Content Strategy Social Media Advertising Strategy Email Marketing Strategy Custom Web App Development Custom Mobile App Development Website Development Ecommerce Website Development Dedicated or Part-Time Full Stack Development Team Social Media Marketing and Management Services Blog Content Writing Services SEO Copywriting Services Adwords Management Services Paid Social Media Marketing and Manage Email Marketing Services                                                                              Scripting Languages: PHP, Python, Go Frameworks: Yii2, Laravel Tools: Composer, Bower Architecture: REST, Microservices View: HTML5, CSS3 built with Less, Sass, Jade Scripting Languages/Libs: JavaScript, TypeScript, JQuery Frameworks: AngularJS 1 and 2, ReactJS, BackboneJS Cloud Hosting: Amazon AWS, DigitalOcean, others Web Server: Nginx Database: MySQL, PgSQL, Mongodb Caching Servers/Tools: Varnish, Memcached Versioning Control: Git, Svn Deployment Tools: Docker, Vagrant, Ansible, Chef The internet is amazingly beautiful and tremendously powerful. It is also complex, constantly evolving and often misunderstood. Enter Bilberrry, an Internet Agency that knows the web and is here to help. Whether you are launching a new website, building a new web/mobile application, or pursuing new online marketing strategies, Bilberrry has you covered. The internet is part of our identity, and we are here to make it part of yours as well.                        home team projects careers contact us CONTACT US FOR A FREE QUOTE Meet our team CONTACT US FOR A FREE QUOTE UX &amp; UI DESIGN, FRONT-END DEVELOPMENT, BACK-END DEVELOPMENT, BRANDING Trackolade.com UX &amp; UI DESIGN, FRONT-END DEVELOPMENT, BACK-END DEVELOPMENT, BRANDING MyOGSM.com UX &amp; UI DESIGN, FRONT-END DEVELOPMENT, BACK-END DEVELOPMENT, BRANDING Ardentservices.com UX &amp; UI DESIGN, FRONT-END DEVELOPMENT, BACK-END DEVELOPMENT, BRANDING Perflux.com             BACKEND             FRONTEND             INFRASTRUCTURE</v>
-      </c>
-      <c r="F12" t="str">
-        <v>Bilberrry - Digital Agency | Application Design and Development Bilberrry – The Internet Agency WE HELP OUR CLIENTS ACHIEVE THEIR ONLINE GOALS. Services We Offer Companies We’ve Worked With Applications We’ve Built Technologies We Use Our team.From Seattle to Kyiv DESIGN STRATEGY DEVELOPMENT MARKETING home team projects careers contact us Web Application Design Mobile Application Design Responsive Website Design Ecommerce Website Design Logo Design Product Roadmap Strategy Content Marketing Strategy SEO Content Strategy Social Media Advertising Strategy Email Marketing Strategy Custom Web App Development Custom Mobile App Development Website Development Ecommerce Website Development Dedicated or Part-Time Full Stack Development Team Social Media Marketing and Management Services Blog Content Writing Services SEO Copywriting Services Adwords Management Services Paid Social Media Marketing and Manage Email Marketing Services                                                                              Scripting Languages: PHP, Python, Go Frameworks: Yii2, Laravel Tools: Composer, Bower Architecture: REST, Microservices View: HTML5, CSS3 built with Less, Sass, Jade Scripting Languages/Libs: JavaScript, TypeScript, JQuery Frameworks: AngularJS 1 and 2, ReactJS, BackboneJS Cloud Hosting: Amazon AWS, DigitalOcean, others Web Server: Nginx Database: MySQL, PgSQL, Mongodb Caching Servers/Tools: Varnish, Memcached Versioning Control: Git, Svn Deployment Tools: Docker, Vagrant, Ansible, Chef The internet is amazingly beautiful and tremendously powerful. It is also complex, constantly evolving and often misunderstood. Enter Bilberrry, an Internet Agency that knows the web and is here to help. Whether you are launching a new website, building a new web/mobile application, or pursuing new online marketing strategies, Bilberrry has you covered. The internet is part of our identity, and we are here to make it part of yours as well.                        home team projects careers contact us CONTACT US FOR A FREE QUOTE Meet our team CONTACT US FOR A FREE QUOTE UX &amp; UI DESIGN, FRONT-END DEVELOPMENT, BACK-END DEVELOPMENT, BRANDING Trackolade.com UX &amp; UI DESIGN, FRONT-END DEVELOPMENT, BACK-END DEVELOPMENT, BRANDING MyOGSM.com UX &amp; UI DESIGN, FRONT-END DEVELOPMENT, BACK-END DEVELOPMENT, BRANDING Ardentservices.com UX &amp; UI DESIGN, FRONT-END DEVELOPMENT, BACK-END DEVELOPMENT, BRANDING Perflux.com             BACKEND             FRONTEND             INFRASTRUCTURE</v>
+        <v>Bilberrry Digital Agency Application Design and Development Bilberrry The Internet Agency WE HELP OUR CLIENTS ACHIEVE THEIR ONLINE GOALS Services We Offer Companies We’ve Worked With Applications We’ve Built Technologies We Use Our teamFrom Seattle to Kyiv DESIGN STRATEGY DEVELOPMENT MARKETING home team projects careers contact us Web Application Design Mobile Application Design Responsive Website Design Ecommerce Website Design Logo Design Product Roadmap Strategy Content Marketing Strategy SEO Content Strategy Social Media Advertising Strategy Email Marketing Strategy Custom Web App Development Custom Mobile App Development Website Development Ecommerce Website Development Dedicated or PartTime Full Stack Development Team Social Media Marketing and Management Services Blog Content Writing Services SEO Copywriting Services Adwords Management Services Paid Social Media Marketing and Manage Email Marketing Services Scripting Languages PHP Python Go Frameworks Yii2 Laravel Tools Composer Bower Architecture REST Microservices View HTML5 CSS3 built with Less Sass Jade Scripting LanguagesLibs JavaScript TypeScript JQuery Frameworks AngularJS 1 and 2 ReactJS BackboneJS Cloud Hosting Amazon AWS DigitalOcean others Web Server Nginx Database MySQL PgSQL Mongodb Caching ServersTools Varnish Memcached Versioning Control Git Svn Deployment Tools Docker Vagrant Ansible Chef The internet is amazingly beautiful and tremendously powerful It is also complex constantly evolving and often misunderstood Enter Bilberrry an Internet Agency that knows the web and is here to help Whether you are launching a new website building a new webmobile application or pursuing new online marketing strategies Bilberrry has you covered The internet is part of our identity and we are here to make it part of yours as well home team projects careers contact us CONTACT US FOR A FREE QUOTE Meet our team CONTACT US FOR A FREE QUOTE UX UI DESIGN FRONTEND DEVELOPMENT BACKEND DEVELOPMENT BRANDING Trackoladecom UX UI DESIGN FRONTEND DEVELOPMENT BACKEND DEVELOPMENT BRANDING MyOGSMcom UX UI DESIGN FRONTEND DEVELOPMENT BACKEND DEVELOPMENT BRANDING Ardentservicescom UX UI DESIGN FRONTEND DEVELOPMENT BACKEND DEVELOPMENT BRANDING Perfluxcom BACKEND FRONTEND INFRASTRUCTURE</v>
       </c>
     </row>
     <row r="13">
@@ -613,16 +520,7 @@
         <v>developers</v>
       </c>
       <c r="C13" t="str">
-        <v>Software Development Company - Application Development Outsourcing - ScienceSoft ScienceSoft is a custom software development company with 26 years' experience, 450 experts and operations in Texas, USA and Europe. software development company, application development outsourcing, application development company, custom software development Professional Software Development              Custom Software Development                          Enterprise Mobile Apps                          Websites and Portals                          SharePoint                          Dynamics CRM                          Business Intelligence           26+ years in IT business 450+ employees 1200+ completed projects Testimonials Partners Our locations Home About Company Team Management Team Our Specialists How We Work Development Process Agile development Quality Management System Delivery Models Intellectual Property Protection Free White Papers Milestones Strategic Relations Testimonials Corporate Social Responsibility Photo Gallery Blog  Company  Team Management Team Our Specialists  Management Team  Our Specialists  How We Work Development Process Agile development Quality Management System Delivery Models Intellectual Property Protection Free White Papers  Development Process Agile development  Agile development  Quality Management System  Delivery Models  Intellectual Property Protection  Free White Papers  Milestones  Strategic Relations  Testimonials  Corporate Social Responsibility  Photo Gallery  Blog  Services Custom Software Development Healthcare Life Sciences Patient Engagement Telecom Banking and Finance Retail Marketing Data Analysis Outsourced Product Development Desktop application development Mobile Application Development Enterprise Mobile Application Development Mobile Technology Consulting Mobile Medical Application Development Cross-Platform Mobile Development Xamarin Development Website Design and Development Corporate Web Portal Development Website Redesign Medical Website Design E-commerce Website Development Outsourced Development Center Software QA and Testing Functional Testing Performance Testing Automated Testing Data Warehouse / Business Intelligence Testing Mobile Device Testing Cloud and Network Services Cloud Infrastructure Management Application Maintenance and Support Enterprise System Management Services Networking Management Services Microsoft Office 365 Migration IT Service Management  Custom Software Development Healthcare Life Sciences Patient Engagement Telecom Banking and Finance Retail Marketing Data Analysis  Healthcare  Life Sciences  Patient Engagement  Telecom  Banking and Finance  Retail  Marketing  Data Analysis  Outsourced Product Development Desktop application development  Desktop application development  Mobile Application Development Enterprise Mobile Application Development Mobile Technology Consulting Mobile Medical Application Development Cross-Platform Mobile Development Xamarin Development  Enterprise Mobile Application Development  Mobile Technology Consulting  Mobile Medical Application Development  Cross-Platform Mobile Development  Xamarin Development  Website Design and Development Corporate Web Portal Development Website Redesign Medical Website Design E-commerce Website Development  Corporate Web Portal Development  Website Redesign  Medical Website Design  E-commerce Website Development  Outsourced Development Center  Software QA and Testing Functional Testing Performance Testing Automated Testing Data Warehouse / Business Intelligence Testing Mobile Device Testing  Functional Testing  Performance Testing  Automated Testing  Data Warehouse / Business Intelligence Testing  Mobile Device Testing  Cloud and Network Services Cloud Infrastructure Management Application Maintenance and Support Enterprise System Management Services Networking Management Services Microsoft Office 365 Migration IT Service Management  Cloud Infrastructure Management  Application Maintenance and Support  Enterprise System Management Services  Networking Management Services  Microsoft Office 365 Migration  IT Service Management  Solutions CRM &amp; Loyalty Microsoft Dynamics CRM Consulting and Customization  Charts/BI Solution for MS Dynamics CRM CRM for Retail Loyalty for Retail EmailScoop N to N Grid SharePoint SharePoint Competence Center Corporate Portals and Intranets Customer Portals SharePoint Migration SharePoint Maintenance and Support SharePoint Health Check Service SharePoint add-ins InOffice Cakes&amp;Candles  Weather Vibes Images Uploader News Trap Workflows Manager  Office Compass Map Contacts Rates Description Business Intelligence Advanced Data Analysis Data Integration &amp; Reporting BI Infrastructure  Security Intelligence SIEM Services Identity and Access Management Services  Fraud Protection for Banks SIEM Case Studies SIEM Materials to Download Health Check Framework for IBM QRadar SIEM Enterprise Content Management (ECM)  CRM &amp; Loyalty Microsoft Dynamics CRM Consulting and Customization  Charts/BI Solution for MS Dynamics CRM CRM for Retail Loyalty for Retail EmailScoop N to N Grid  Microsoft Dynamics CRM Consulting and Customization  Charts/BI Solution for MS Dynamics CRM  Charts/BI Solution for MS Dynamics CRM  CRM for Retail  Loyalty for Retail  EmailScoop  N to N Grid  SharePoint SharePoint Competence Center Corporate Portals and Intranets Customer Portals SharePoint Migration SharePoint Maintenance and Support SharePoint Health Check Service SharePoint add-ins InOffice Cakes&amp;Candles  Weather Vibes Images Uploader News Trap Workflows Manager  Office Compass Map Contacts Rates Description  SharePoint Competence Center  Corporate Portals and Intranets  Customer Portals  SharePoint Migration  SharePoint Maintenance and Support  SharePoint Health Check Service  SharePoint add-ins InOffice Cakes&amp;Candles  Weather Vibes Images Uploader News Trap Workflows Manager  Office Compass Map Contacts Rates Description  InOffice Cakes&amp;Candles   Weather Vibes  Images Uploader  News Trap  Workflows Manager   Office Compass  Map Contacts  Rates Description  Business Intelligence Advanced Data Analysis Data Integration &amp; Reporting BI Infrastructure   Advanced Data Analysis  Data Integration &amp; Reporting  BI Infrastructure   Security Intelligence SIEM Services Identity and Access Management Services  Fraud Protection for Banks SIEM Case Studies SIEM Materials to Download Health Check Framework for IBM QRadar SIEM  SIEM Services  Identity and Access Management Services   Fraud Protection for Banks  SIEM Case Studies  SIEM Materials to Download  Health Check Framework for IBM QRadar SIEM  Enterprise Content Management (ECM)  Technologies C++ Qt .NET .NET Framework Java PHP Frontend Mobile Database Development Databases  C++ Qt  Qt  .NET .NET Framework  .NET Framework  Java  PHP  Frontend  Mobile  Database Development Databases  Databases  Case Studies Healthcare Telecommunications Retail Banking Entertainment Education Travel and Hospitality Logistics and Transportation Manufacturing Oil and Gas   Healthcare  Telecommunications  Retail  Banking  Entertainment  Education  Travel and Hospitality  Logistics and Transportation  Manufacturing  Oil and Gas   Press Room Press Releases Media Coverage  Press Releases  Media Coverage  Careers Vacancies Working for ScienceSoft  Vacancies  Working for ScienceSoft  Contact Us Request a Quote Become ScienceSoft’s Partner  Request a Quote  Become ScienceSoft’s Partner  Home About Services Solutions Case Studies Press Room Careers Contact Us Site Map We offer full-cycle development services for web, mobile and desktop that have already brought value to Walmart, eBay and Viber 75 experts, 300+ projects. We develop iOS, Android, WP, Cordova and Xamarin apps, mobile back-ends, provide integration and maintenance All-round website development services from design to maintenance with 180 web experts and a record of 250 delivered websites   We create corporate web portals and intranets to help established enterprises benefit from collaboration and document management Industry-focused consulting, customizing and loyalty solutions for B2B and B2C enterprises, featuring a retail bank CRM with 7 mln clients Bringing in Data Science and BI expertise since 1989, we cover our clients’ needs with data warehouses, OLAP cubes, reports and dashboards …exciting journey from the dawn of articficial intelligence systems to the connected world of outsourcing nurturing relationships with Microsoft, IBM, Oracle and other leaders. …and still growing - in 2014 ScienceSoft won the Fastest Growing Company Award from Ernst &amp; Young. …for happy customers from over 25 countries including giants such as IBM, Tieto, PerkinElmer and Leo Burnett as well as SMEs and startups such as would-be Viber.  ScienceSoft has proved itself to be a trusted partner for proceeding with long-term relationship. We are delighted to have found such a highly professional, reliable and committed technology partner in ScienceSoft.  I have been very satisfied with the quality of their product and have been pleasantly surprised by their level of service. here                                  Svenska                                                               Français                                                               Deutsch                                                               Suomi                                                               Русский                              Home About Company Team Management Team Our Specialists How We Work Development Process Agile development Quality Management System Delivery Models Intellectual Property Protection Free White Papers Milestones Strategic Relations Testimonials Corporate Social Responsibility Photo Gallery Blog Services Custom Software Development Healthcare Life Sciences Patient Engagement Telecom Banking and Finance Retail Marketing Data Analysis Outsourced Product Development Desktop application development Mobile Application Development Enterprise Mobile Application Development Mobile Technology Consulting Mobile Medical Application Development Cross-Platform Mobile Development Xamarin Development Website Design and Development Corporate Web Portal Development Website Redesign Medical Website Design E-commerce Website Development Outsourced Development Center Software QA and Testing Functional Testing Performance Testing Automated Testing Data Warehouse / Business Intelligence Testing Mobile Device Testing Cloud and Network Services Cloud Infrastructure Management Application Maintenance and Support Enterprise System Management Services Networking Management Services Microsoft Office 365 Migration IT Service Management Solutions CRM &amp; Loyalty Microsoft Dynamics CRM Consulting and Customization  Charts/BI Solution for MS Dynamics CRM CRM for Retail Loyalty for Retail EmailScoop N to N Grid SharePoint SharePoint Competence Center Corporate Portals and Intranets Customer Portals SharePoint Migration SharePoint Maintenance and Support SharePoint Health Check Service SharePoint add-ins InOffice Cakes&amp;Candles  Weather Vibes Images Uploader News Trap Workflows Manager  Office Compass Map Contacts Rates Description Business Intelligence Advanced Data Analysis Data Integration &amp; Reporting BI Infrastructure  Security Intelligence SIEM Services Identity and Access Management Services  Fraud Protection for Banks SIEM Case Studies SIEM Materials to Download Health Check Framework for IBM QRadar SIEM Enterprise Content Management (ECM) Technologies C++ Qt .NET .NET Framework Java PHP Frontend Mobile Database Development Databases Case Studies Healthcare Telecommunications Retail Banking Entertainment Education Travel and Hospitality Logistics and Transportation Manufacturing Oil and Gas  Press Room Press Releases Media Coverage Careers Vacancies Working for ScienceSoft Contact Us Request a Quote Become ScienceSoft’s Partner                                                                                 Custom Software Development                                 See more                                                                                               Enterprise Mobile Apps                                 See more                                                                                               Websites and Portals                                 See more                                                                                               SharePoint                                 See more                                                                                               Dynamics CRM                                 See more                                                                                               Business Intelligence                                 See more                    James Bowerman ,              IBM             Director Compliance Product Development                       Marc O'Dwyer,              Big Red Book             Managing Director                       Ryan O'Grady,              Fotaflo              CEO          Home About Services Solutions Case Studies Press Room Careers Contact Us Site Map                                        Services Custom Software Development Outsourced Product Development Mobile Application Development Website Design and Development Outsourced Development Center Software QA and Testing Cloud and Network Services About Company Team Delivery Models IP Protection Development Process Quality Management System Contact us Contact Information Become ScienceSoft's Partner Request for Quote contact@scnsoft.com +1 214 306 68 37 contact@scnsoft.com English Svenska Français Deutsch Suomi Русский Menu Home 26+ 450+ 1200+ IBM Director Compliance Product Development Big Red Book Managing Director Fotaflo  CEO © 1989–2015 ScienceSoft Inc. Phone: +1 214 306 68 37 Email: contact@scnsoft.com                  © 1989–2015 ScienceSoft Inc.                 Phone: +1 214 306 68 37                 Email: contact@scnsoft.com              © 1989–2015 ScienceSoft Inc. Phone: +1 214 306 68 37 Email: contact@scnsoft.com</v>
-      </c>
-      <c r="D13" t="str">
-        <v>Software Development Company - Application Development Outsourcing - ScienceSoft ScienceSoft is a custom software development company with 26 years' experience, 450 experts and operations in Texas, USA and Europe. software development company, application development outsourcing, application development company, custom software development Professional Software Development              Custom Software Development                          Enterprise Mobile Apps                          Websites and Portals                          SharePoint                          Dynamics CRM                          Business Intelligence           26+ years in IT business 450+ employees 1200+ completed projects Testimonials Partners Our locations Home About Company Team Management Team Our Specialists How We Work Development Process Agile development Quality Management System Delivery Models Intellectual Property Protection Free White Papers Milestones Strategic Relations Testimonials Corporate Social Responsibility Photo Gallery Blog  Company  Team Management Team Our Specialists  Management Team  Our Specialists  How We Work Development Process Agile development Quality Management System Delivery Models Intellectual Property Protection Free White Papers  Development Process Agile development  Agile development  Quality Management System  Delivery Models  Intellectual Property Protection  Free White Papers  Milestones  Strategic Relations  Testimonials  Corporate Social Responsibility  Photo Gallery  Blog  Services Custom Software Development Healthcare Life Sciences Patient Engagement Telecom Banking and Finance Retail Marketing Data Analysis Outsourced Product Development Desktop application development Mobile Application Development Enterprise Mobile Application Development Mobile Technology Consulting Mobile Medical Application Development Cross-Platform Mobile Development Xamarin Development Website Design and Development Corporate Web Portal Development Website Redesign Medical Website Design E-commerce Website Development Outsourced Development Center Software QA and Testing Functional Testing Performance Testing Automated Testing Data Warehouse / Business Intelligence Testing Mobile Device Testing Cloud and Network Services Cloud Infrastructure Management Application Maintenance and Support Enterprise System Management Services Networking Management Services Microsoft Office 365 Migration IT Service Management  Custom Software Development Healthcare Life Sciences Patient Engagement Telecom Banking and Finance Retail Marketing Data Analysis  Healthcare  Life Sciences  Patient Engagement  Telecom  Banking and Finance  Retail  Marketing  Data Analysis  Outsourced Product Development Desktop application development  Desktop application development  Mobile Application Development Enterprise Mobile Application Development Mobile Technology Consulting Mobile Medical Application Development Cross-Platform Mobile Development Xamarin Development  Enterprise Mobile Application Development  Mobile Technology Consulting  Mobile Medical Application Development  Cross-Platform Mobile Development  Xamarin Development  Website Design and Development Corporate Web Portal Development Website Redesign Medical Website Design E-commerce Website Development  Corporate Web Portal Development  Website Redesign  Medical Website Design  E-commerce Website Development  Outsourced Development Center  Software QA and Testing Functional Testing Performance Testing Automated Testing Data Warehouse / Business Intelligence Testing Mobile Device Testing  Functional Testing  Performance Testing  Automated Testing  Data Warehouse / Business Intelligence Testing  Mobile Device Testing  Cloud and Network Services Cloud Infrastructure Management Application Maintenance and Support Enterprise System Management Services Networking Management Services Microsoft Office 365 Migration IT Service Management  Cloud Infrastructure Management  Application Maintenance and Support  Enterprise System Management Services  Networking Management Services  Microsoft Office 365 Migration  IT Service Management  Solutions CRM &amp; Loyalty Microsoft Dynamics CRM Consulting and Customization  Charts/BI Solution for MS Dynamics CRM CRM for Retail Loyalty for Retail EmailScoop N to N Grid SharePoint SharePoint Competence Center Corporate Portals and Intranets Customer Portals SharePoint Migration SharePoint Maintenance and Support SharePoint Health Check Service SharePoint add-ins InOffice Cakes&amp;Candles  Weather Vibes Images Uploader News Trap Workflows Manager  Office Compass Map Contacts Rates Description Business Intelligence Advanced Data Analysis Data Integration &amp; Reporting BI Infrastructure  Security Intelligence SIEM Services Identity and Access Management Services  Fraud Protection for Banks SIEM Case Studies SIEM Materials to Download Health Check Framework for IBM QRadar SIEM Enterprise Content Management (ECM)  CRM &amp; Loyalty Microsoft Dynamics CRM Consulting and Customization  Charts/BI Solution for MS Dynamics CRM CRM for Retail Loyalty for Retail EmailScoop N to N Grid  Microsoft Dynamics CRM Consulting and Customization  Charts/BI Solution for MS Dynamics CRM  Charts/BI Solution for MS Dynamics CRM  CRM for Retail  Loyalty for Retail  EmailScoop  N to N Grid  SharePoint SharePoint Competence Center Corporate Portals and Intranets Customer Portals SharePoint Migration SharePoint Maintenance and Support SharePoint Health Check Service SharePoint add-ins InOffice Cakes&amp;Candles  Weather Vibes Images Uploader News Trap Workflows Manager  Office Compass Map Contacts Rates Description  SharePoint Competence Center  Corporate Portals and Intranets  Customer Portals  SharePoint Migration  SharePoint Maintenance and Support  SharePoint Health Check Service  SharePoint add-ins InOffice Cakes&amp;Candles  Weather Vibes Images Uploader News Trap Workflows Manager  Office Compass Map Contacts Rates Description  InOffice Cakes&amp;Candles   Weather Vibes  Images Uploader  News Trap  Workflows Manager   Office Compass  Map Contacts  Rates Description  Business Intelligence Advanced Data Analysis Data Integration &amp; Reporting BI Infrastructure   Advanced Data Analysis  Data Integration &amp; Reporting  BI Infrastructure   Security Intelligence SIEM Services Identity and Access Management Services  Fraud Protection for Banks SIEM Case Studies SIEM Materials to Download Health Check Framework for IBM QRadar SIEM  SIEM Services  Identity and Access Management Services   Fraud Protection for Banks  SIEM Case Studies  SIEM Materials to Download  Health Check Framework for IBM QRadar SIEM  Enterprise Content Management (ECM)  Technologies C++ Qt .NET .NET Framework Java PHP Frontend Mobile Database Development Databases  C++ Qt  Qt  .NET .NET Framework  .NET Framework  Java  PHP  Frontend  Mobile  Database Development Databases  Databases  Case Studies Healthcare Telecommunications Retail Banking Entertainment Education Travel and Hospitality Logistics and Transportation Manufacturing Oil and Gas   Healthcare  Telecommunications  Retail  Banking  Entertainment  Education  Travel and Hospitality  Logistics and Transportation  Manufacturing  Oil and Gas   Press Room Press Releases Media Coverage  Press Releases  Media Coverage  Careers Vacancies Working for ScienceSoft  Vacancies  Working for ScienceSoft  Contact Us Request a Quote Become ScienceSoft’s Partner  Request a Quote  Become ScienceSoft’s Partner  Home About Services Solutions Case Studies Press Room Careers Contact Us Site Map We offer full-cycle development services for web, mobile and desktop that have already brought value to Walmart, eBay and Viber 75 experts, 300+ projects. We develop iOS, Android, WP, Cordova and Xamarin apps, mobile back-ends, provide integration and maintenance All-round website development services from design to maintenance with 180 web experts and a record of 250 delivered websites   We create corporate web portals and intranets to help established enterprises benefit from collaboration and document management Industry-focused consulting, customizing and loyalty solutions for B2B and B2C enterprises, featuring a retail bank CRM with 7 mln clients Bringing in Data Science and BI expertise since 1989, we cover our clients’ needs with data warehouses, OLAP cubes, reports and dashboards …exciting journey from the dawn of articficial intelligence systems to the connected world of outsourcing nurturing relationships with Microsoft, IBM, Oracle and other leaders. …and still growing - in 2014 ScienceSoft won the Fastest Growing Company Award from Ernst &amp; Young. …for happy customers from over 25 countries including giants such as IBM, Tieto, PerkinElmer and Leo Burnett as well as SMEs and startups such as would-be Viber.  ScienceSoft has proved itself to be a trusted partner for proceeding with long-term relationship. We are delighted to have found such a highly professional, reliable and committed technology partner in ScienceSoft.  I have been very satisfied with the quality of their product and have been pleasantly surprised by their level of service. here                                  Svenska                                                               Français                                                               Deutsch                                                               Suomi                                                               Русский                              Home About Company Team Management Team Our Specialists How We Work Development Process Agile development Quality Management System Delivery Models Intellectual Property Protection Free White Papers Milestones Strategic Relations Testimonials Corporate Social Responsibility Photo Gallery Blog Services Custom Software Development Healthcare Life Sciences Patient Engagement Telecom Banking and Finance Retail Marketing Data Analysis Outsourced Product Development Desktop application development Mobile Application Development Enterprise Mobile Application Development Mobile Technology Consulting Mobile Medical Application Development Cross-Platform Mobile Development Xamarin Development Website Design and Development Corporate Web Portal Development Website Redesign Medical Website Design E-commerce Website Development Outsourced Development Center Software QA and Testing Functional Testing Performance Testing Automated Testing Data Warehouse / Business Intelligence Testing Mobile Device Testing Cloud and Network Services Cloud Infrastructure Management Application Maintenance and Support Enterprise System Management Services Networking Management Services Microsoft Office 365 Migration IT Service Management Solutions CRM &amp; Loyalty Microsoft Dynamics CRM Consulting and Customization  Charts/BI Solution for MS Dynamics CRM CRM for Retail Loyalty for Retail EmailScoop N to N Grid SharePoint SharePoint Competence Center Corporate Portals and Intranets Customer Portals SharePoint Migration SharePoint Maintenance and Support SharePoint Health Check Service SharePoint add-ins InOffice Cakes&amp;Candles  Weather Vibes Images Uploader News Trap Workflows Manager  Office Compass Map Contacts Rates Description Business Intelligence Advanced Data Analysis Data Integration &amp; Reporting BI Infrastructure  Security Intelligence SIEM Services Identity and Access Management Services  Fraud Protection for Banks SIEM Case Studies SIEM Materials to Download Health Check Framework for IBM QRadar SIEM Enterprise Content Management (ECM) Technologies C++ Qt .NET .NET Framework Java PHP Frontend Mobile Database Development Databases Case Studies Healthcare Telecommunications Retail Banking Entertainment Education Travel and Hospitality Logistics and Transportation Manufacturing Oil and Gas  Press Room Press Releases Media Coverage Careers Vacancies Working for ScienceSoft Contact Us Request a Quote Become ScienceSoft’s Partner                                                                                 Custom Software Development                                 See more                                                                                               Enterprise Mobile Apps                                 See more                                                                                               Websites and Portals                                 See more                                                                                               SharePoint                                 See more                                                                                               Dynamics CRM                                 See more                                                                                               Business Intelligence                                 See more                    James Bowerman ,              IBM             Director Compliance Product Development                       Marc O'Dwyer,              Big Red Book             Managing Director                       Ryan O'Grady,              Fotaflo              CEO          Home About Services Solutions Case Studies Press Room Careers Contact Us Site Map                                        Services Custom Software Development Outsourced Product Development Mobile Application Development Website Design and Development Outsourced Development Center Software QA and Testing Cloud and Network Services About Company Team Delivery Models IP Protection Development Process Quality Management System Contact us Contact Information Become ScienceSoft's Partner Request for Quote contact@scnsoft.com +1 214 306 68 37 contact@scnsoft.com English Svenska Français Deutsch Suomi Русский Menu Home 26+ 450+ 1200+ IBM Director Compliance Product Development Big Red Book Managing Director Fotaflo  CEO © 1989–2015 ScienceSoft Inc. Phone: +1 214 306 68 37 Email: contact@scnsoft.com                  © 1989–2015 ScienceSoft Inc.                 Phone: +1 214 306 68 37                 Email: contact@scnsoft.com              © 1989–2015 ScienceSoft Inc. Phone: +1 214 306 68 37 Email: contact@scnsoft.com</v>
-      </c>
-      <c r="E13" t="str">
-        <v>Software Development Company - Application Development Outsourcing - ScienceSoft ScienceSoft is a custom software development company with 26 years' experience, 450 experts and operations in Texas, USA and Europe. software development company, application development outsourcing, application development company, custom software development Professional Software Development              Custom Software Development                          Enterprise Mobile Apps                          Websites and Portals                          SharePoint                          Dynamics CRM                          Business Intelligence           26+ years in IT business 450+ employees 1200+ completed projects Testimonials Partners Our locations Home About Company Team Management Team Our Specialists How We Work Development Process Agile development Quality Management System Delivery Models Intellectual Property Protection Free White Papers Milestones Strategic Relations Testimonials Corporate Social Responsibility Photo Gallery Blog  Company  Team Management Team Our Specialists  Management Team  Our Specialists  How We Work Development Process Agile development Quality Management System Delivery Models Intellectual Property Protection Free White Papers  Development Process Agile development  Agile development  Quality Management System  Delivery Models  Intellectual Property Protection  Free White Papers  Milestones  Strategic Relations  Testimonials  Corporate Social Responsibility  Photo Gallery  Blog  Services Custom Software Development Healthcare Life Sciences Patient Engagement Telecom Banking and Finance Retail Marketing Data Analysis Outsourced Product Development Desktop application development Mobile Application Development Enterprise Mobile Application Development Mobile Technology Consulting Mobile Medical Application Development Cross-Platform Mobile Development Xamarin Development Website Design and Development Corporate Web Portal Development Website Redesign Medical Website Design E-commerce Website Development Outsourced Development Center Software QA and Testing Functional Testing Performance Testing Automated Testing Data Warehouse / Business Intelligence Testing Mobile Device Testing Cloud and Network Services Cloud Infrastructure Management Application Maintenance and Support Enterprise System Management Services Networking Management Services Microsoft Office 365 Migration IT Service Management  Custom Software Development Healthcare Life Sciences Patient Engagement Telecom Banking and Finance Retail Marketing Data Analysis  Healthcare  Life Sciences  Patient Engagement  Telecom  Banking and Finance  Retail  Marketing  Data Analysis  Outsourced Product Development Desktop application development  Desktop application development  Mobile Application Development Enterprise Mobile Application Development Mobile Technology Consulting Mobile Medical Application Development Cross-Platform Mobile Development Xamarin Development  Enterprise Mobile Application Development  Mobile Technology Consulting  Mobile Medical Application Development  Cross-Platform Mobile Development  Xamarin Development  Website Design and Development Corporate Web Portal Development Website Redesign Medical Website Design E-commerce Website Development  Corporate Web Portal Development  Website Redesign  Medical Website Design  E-commerce Website Development  Outsourced Development Center  Software QA and Testing Functional Testing Performance Testing Automated Testing Data Warehouse / Business Intelligence Testing Mobile Device Testing  Functional Testing  Performance Testing  Automated Testing  Data Warehouse / Business Intelligence Testing  Mobile Device Testing  Cloud and Network Services Cloud Infrastructure Management Application Maintenance and Support Enterprise System Management Services Networking Management Services Microsoft Office 365 Migration IT Service Management  Cloud Infrastructure Management  Application Maintenance and Support  Enterprise System Management Services  Networking Management Services  Microsoft Office 365 Migration  IT Service Management  Solutions CRM &amp; Loyalty Microsoft Dynamics CRM Consulting and Customization  Charts/BI Solution for MS Dynamics CRM CRM for Retail Loyalty for Retail EmailScoop N to N Grid SharePoint SharePoint Competence Center Corporate Portals and Intranets Customer Portals SharePoint Migration SharePoint Maintenance and Support SharePoint Health Check Service SharePoint add-ins InOffice Cakes&amp;Candles  Weather Vibes Images Uploader News Trap Workflows Manager  Office Compass Map Contacts Rates Description Business Intelligence Advanced Data Analysis Data Integration &amp; Reporting BI Infrastructure  Security Intelligence SIEM Services Identity and Access Management Services  Fraud Protection for Banks SIEM Case Studies SIEM Materials to Download Health Check Framework for IBM QRadar SIEM Enterprise Content Management (ECM)  CRM &amp; Loyalty Microsoft Dynamics CRM Consulting and Customization  Charts/BI Solution for MS Dynamics CRM CRM for Retail Loyalty for Retail EmailScoop N to N Grid  Microsoft Dynamics CRM Consulting and Customization  Charts/BI Solution for MS Dynamics CRM  Charts/BI Solution for MS Dynamics CRM  CRM for Retail  Loyalty for Retail  EmailScoop  N to N Grid  SharePoint SharePoint Competence Center Corporate Portals and Intranets Customer Portals SharePoint Migration SharePoint Maintenance and Support SharePoint Health Check Service SharePoint add-ins InOffice Cakes&amp;Candles  Weather Vibes Images Uploader News Trap Workflows Manager  Office Compass Map Contacts Rates Description  SharePoint Competence Center  Corporate Portals and Intranets  Customer Portals  SharePoint Migration  SharePoint Maintenance and Support  SharePoint Health Check Service  SharePoint add-ins InOffice Cakes&amp;Candles  Weather Vibes Images Uploader News Trap Workflows Manager  Office Compass Map Contacts Rates Description  InOffice Cakes&amp;Candles   Weather Vibes  Images Uploader  News Trap  Workflows Manager   Office Compass  Map Contacts  Rates Description  Business Intelligence Advanced Data Analysis Data Integration &amp; Reporting BI Infrastructure   Advanced Data Analysis  Data Integration &amp; Reporting  BI Infrastructure   Security Intelligence SIEM Services Identity and Access Management Services  Fraud Protection for Banks SIEM Case Studies SIEM Materials to Download Health Check Framework for IBM QRadar SIEM  SIEM Services  Identity and Access Management Services   Fraud Protection for Banks  SIEM Case Studies  SIEM Materials to Download  Health Check Framework for IBM QRadar SIEM  Enterprise Content Management (ECM)  Technologies C++ Qt .NET .NET Framework Java PHP Frontend Mobile Database Development Databases  C++ Qt  Qt  .NET .NET Framework  .NET Framework  Java  PHP  Frontend  Mobile  Database Development Databases  Databases  Case Studies Healthcare Telecommunications Retail Banking Entertainment Education Travel and Hospitality Logistics and Transportation Manufacturing Oil and Gas   Healthcare  Telecommunications  Retail  Banking  Entertainment  Education  Travel and Hospitality  Logistics and Transportation  Manufacturing  Oil and Gas   Press Room Press Releases Media Coverage  Press Releases  Media Coverage  Careers Vacancies Working for ScienceSoft  Vacancies  Working for ScienceSoft  Contact Us Request a Quote Become ScienceSoft’s Partner  Request a Quote  Become ScienceSoft’s Partner  Home About Services Solutions Case Studies Press Room Careers Contact Us Site Map We offer full-cycle development services for web, mobile and desktop that have already brought value to Walmart, eBay and Viber 75 experts, 300+ projects. We develop iOS, Android, WP, Cordova and Xamarin apps, mobile back-ends, provide integration and maintenance All-round website development services from design to maintenance with 180 web experts and a record of 250 delivered websites   We create corporate web portals and intranets to help established enterprises benefit from collaboration and document management Industry-focused consulting, customizing and loyalty solutions for B2B and B2C enterprises, featuring a retail bank CRM with 7 mln clients Bringing in Data Science and BI expertise since 1989, we cover our clients’ needs with data warehouses, OLAP cubes, reports and dashboards …exciting journey from the dawn of articficial intelligence systems to the connected world of outsourcing nurturing relationships with Microsoft, IBM, Oracle and other leaders. …and still growing - in 2014 ScienceSoft won the Fastest Growing Company Award from Ernst &amp; Young. …for happy customers from over 25 countries including giants such as IBM, Tieto, PerkinElmer and Leo Burnett as well as SMEs and startups such as would-be Viber.  ScienceSoft has proved itself to be a trusted partner for proceeding with long-term relationship. We are delighted to have found such a highly professional, reliable and committed technology partner in ScienceSoft.  I have been very satisfied with the quality of their product and have been pleasantly surprised by their level of service. here                                  Svenska                                                               Français                                                               Deutsch                                                               Suomi                                                               Русский                              Home About Company Team Management Team Our Specialists How We Work Development Process Agile development Quality Management System Delivery Models Intellectual Property Protection Free White Papers Milestones Strategic Relations Testimonials Corporate Social Responsibility Photo Gallery Blog Services Custom Software Development Healthcare Life Sciences Patient Engagement Telecom Banking and Finance Retail Marketing Data Analysis Outsourced Product Development Desktop application development Mobile Application Development Enterprise Mobile Application Development Mobile Technology Consulting Mobile Medical Application Development Cross-Platform Mobile Development Xamarin Development Website Design and Development Corporate Web Portal Development Website Redesign Medical Website Design E-commerce Website Development Outsourced Development Center Software QA and Testing Functional Testing Performance Testing Automated Testing Data Warehouse / Business Intelligence Testing Mobile Device Testing Cloud and Network Services Cloud Infrastructure Management Application Maintenance and Support Enterprise System Management Services Networking Management Services Microsoft Office 365 Migration IT Service Management Solutions CRM &amp; Loyalty Microsoft Dynamics CRM Consulting and Customization  Charts/BI Solution for MS Dynamics CRM CRM for Retail Loyalty for Retail EmailScoop N to N Grid SharePoint SharePoint Competence Center Corporate Portals and Intranets Customer Portals SharePoint Migration SharePoint Maintenance and Support SharePoint Health Check Service SharePoint add-ins InOffice Cakes&amp;Candles  Weather Vibes Images Uploader News Trap Workflows Manager  Office Compass Map Contacts Rates Description Business Intelligence Advanced Data Analysis Data Integration &amp; Reporting BI Infrastructure  Security Intelligence SIEM Services Identity and Access Management Services  Fraud Protection for Banks SIEM Case Studies SIEM Materials to Download Health Check Framework for IBM QRadar SIEM Enterprise Content Management (ECM) Technologies C++ Qt .NET .NET Framework Java PHP Frontend Mobile Database Development Databases Case Studies Healthcare Telecommunications Retail Banking Entertainment Education Travel and Hospitality Logistics and Transportation Manufacturing Oil and Gas  Press Room Press Releases Media Coverage Careers Vacancies Working for ScienceSoft Contact Us Request a Quote Become ScienceSoft’s Partner                                                                                 Custom Software Development                                 See more                                                                                               Enterprise Mobile Apps                                 See more                                                                                               Websites and Portals                                 See more                                                                                               SharePoint                                 See more                                                                                               Dynamics CRM                                 See more                                                                                               Business Intelligence                                 See more                    James Bowerman ,              IBM             Director Compliance Product Development                       Marc O'Dwyer,              Big Red Book             Managing Director                       Ryan O'Grady,              Fotaflo              CEO          Home About Services Solutions Case Studies Press Room Careers Contact Us Site Map                                        Services Custom Software Development Outsourced Product Development Mobile Application Development Website Design and Development Outsourced Development Center Software QA and Testing Cloud and Network Services About Company Team Delivery Models IP Protection Development Process Quality Management System Contact us Contact Information Become ScienceSoft's Partner Request for Quote contact@scnsoft.com +1 214 306 68 37 contact@scnsoft.com English Svenska Français Deutsch Suomi Русский Menu Home 26+ 450+ 1200+ IBM Director Compliance Product Development Big Red Book Managing Director Fotaflo  CEO © 1989–2015 ScienceSoft Inc. Phone: +1 214 306 68 37 Email: contact@scnsoft.com                  © 1989–2015 ScienceSoft Inc.                 Phone: +1 214 306 68 37                 Email: contact@scnsoft.com              © 1989–2015 ScienceSoft Inc. Phone: +1 214 306 68 37 Email: contact@scnsoft.com</v>
-      </c>
-      <c r="F13" t="str">
-        <v>Software Development Company - Application Development Outsourcing - ScienceSoft ScienceSoft is a custom software development company with 26 years' experience, 450 experts and operations in Texas, USA and Europe. software development company, application development outsourcing, application development company, custom software development Professional Software Development              Custom Software Development                          Enterprise Mobile Apps                          Websites and Portals                          SharePoint                          Dynamics CRM                          Business Intelligence           26+ years in IT business 450+ employees 1200+ completed projects Testimonials Partners Our locations Home About Company Team Management Team Our Specialists How We Work Development Process Agile development Quality Management System Delivery Models Intellectual Property Protection Free White Papers Milestones Strategic Relations Testimonials Corporate Social Responsibility Photo Gallery Blog  Company  Team Management Team Our Specialists  Management Team  Our Specialists  How We Work Development Process Agile development Quality Management System Delivery Models Intellectual Property Protection Free White Papers  Development Process Agile development  Agile development  Quality Management System  Delivery Models  Intellectual Property Protection  Free White Papers  Milestones  Strategic Relations  Testimonials  Corporate Social Responsibility  Photo Gallery  Blog  Services Custom Software Development Healthcare Life Sciences Patient Engagement Telecom Banking and Finance Retail Marketing Data Analysis Outsourced Product Development Desktop application development Mobile Application Development Enterprise Mobile Application Development Mobile Technology Consulting Mobile Medical Application Development Cross-Platform Mobile Development Xamarin Development Website Design and Development Corporate Web Portal Development Website Redesign Medical Website Design E-commerce Website Development Outsourced Development Center Software QA and Testing Functional Testing Performance Testing Automated Testing Data Warehouse / Business Intelligence Testing Mobile Device Testing Cloud and Network Services Cloud Infrastructure Management Application Maintenance and Support Enterprise System Management Services Networking Management Services Microsoft Office 365 Migration IT Service Management  Custom Software Development Healthcare Life Sciences Patient Engagement Telecom Banking and Finance Retail Marketing Data Analysis  Healthcare  Life Sciences  Patient Engagement  Telecom  Banking and Finance  Retail  Marketing  Data Analysis  Outsourced Product Development Desktop application development  Desktop application development  Mobile Application Development Enterprise Mobile Application Development Mobile Technology Consulting Mobile Medical Application Development Cross-Platform Mobile Development Xamarin Development  Enterprise Mobile Application Development  Mobile Technology Consulting  Mobile Medical Application Development  Cross-Platform Mobile Development  Xamarin Development  Website Design and Development Corporate Web Portal Development Website Redesign Medical Website Design E-commerce Website Development  Corporate Web Portal Development  Website Redesign  Medical Website Design  E-commerce Website Development  Outsourced Development Center  Software QA and Testing Functional Testing Performance Testing Automated Testing Data Warehouse / Business Intelligence Testing Mobile Device Testing  Functional Testing  Performance Testing  Automated Testing  Data Warehouse / Business Intelligence Testing  Mobile Device Testing  Cloud and Network Services Cloud Infrastructure Management Application Maintenance and Support Enterprise System Management Services Networking Management Services Microsoft Office 365 Migration IT Service Management  Cloud Infrastructure Management  Application Maintenance and Support  Enterprise System Management Services  Networking Management Services  Microsoft Office 365 Migration  IT Service Management  Solutions CRM &amp; Loyalty Microsoft Dynamics CRM Consulting and Customization  Charts/BI Solution for MS Dynamics CRM CRM for Retail Loyalty for Retail EmailScoop N to N Grid SharePoint SharePoint Competence Center Corporate Portals and Intranets Customer Portals SharePoint Migration SharePoint Maintenance and Support SharePoint Health Check Service SharePoint add-ins InOffice Cakes&amp;Candles  Weather Vibes Images Uploader News Trap Workflows Manager  Office Compass Map Contacts Rates Description Business Intelligence Advanced Data Analysis Data Integration &amp; Reporting BI Infrastructure  Security Intelligence SIEM Services Identity and Access Management Services  Fraud Protection for Banks SIEM Case Studies SIEM Materials to Download Health Check Framework for IBM QRadar SIEM Enterprise Content Management (ECM)  CRM &amp; Loyalty Microsoft Dynamics CRM Consulting and Customization  Charts/BI Solution for MS Dynamics CRM CRM for Retail Loyalty for Retail EmailScoop N to N Grid  Microsoft Dynamics CRM Consulting and Customization  Charts/BI Solution for MS Dynamics CRM  Charts/BI Solution for MS Dynamics CRM  CRM for Retail  Loyalty for Retail  EmailScoop  N to N Grid  SharePoint SharePoint Competence Center Corporate Portals and Intranets Customer Portals SharePoint Migration SharePoint Maintenance and Support SharePoint Health Check Service SharePoint add-ins InOffice Cakes&amp;Candles  Weather Vibes Images Uploader News Trap Workflows Manager  Office Compass Map Contacts Rates Description  SharePoint Competence Center  Corporate Portals and Intranets  Customer Portals  SharePoint Migration  SharePoint Maintenance and Support  SharePoint Health Check Service  SharePoint add-ins InOffice Cakes&amp;Candles  Weather Vibes Images Uploader News Trap Workflows Manager  Office Compass Map Contacts Rates Description  InOffice Cakes&amp;Candles   Weather Vibes  Images Uploader  News Trap  Workflows Manager   Office Compass  Map Contacts  Rates Description  Business Intelligence Advanced Data Analysis Data Integration &amp; Reporting BI Infrastructure   Advanced Data Analysis  Data Integration &amp; Reporting  BI Infrastructure   Security Intelligence SIEM Services Identity and Access Management Services  Fraud Protection for Banks SIEM Case Studies SIEM Materials to Download Health Check Framework for IBM QRadar SIEM  SIEM Services  Identity and Access Management Services   Fraud Protection for Banks  SIEM Case Studies  SIEM Materials to Download  Health Check Framework for IBM QRadar SIEM  Enterprise Content Management (ECM)  Technologies C++ Qt .NET .NET Framework Java PHP Frontend Mobile Database Development Databases  C++ Qt  Qt  .NET .NET Framework  .NET Framework  Java  PHP  Frontend  Mobile  Database Development Databases  Databases  Case Studies Healthcare Telecommunications Retail Banking Entertainment Education Travel and Hospitality Logistics and Transportation Manufacturing Oil and Gas   Healthcare  Telecommunications  Retail  Banking  Entertainment  Education  Travel and Hospitality  Logistics and Transportation  Manufacturing  Oil and Gas   Press Room Press Releases Media Coverage  Press Releases  Media Coverage  Careers Vacancies Working for ScienceSoft  Vacancies  Working for ScienceSoft  Contact Us Request a Quote Become ScienceSoft’s Partner  Request a Quote  Become ScienceSoft’s Partner  Home About Services Solutions Case Studies Press Room Careers Contact Us Site Map We offer full-cycle development services for web, mobile and desktop that have already brought value to Walmart, eBay and Viber 75 experts, 300+ projects. We develop iOS, Android, WP, Cordova and Xamarin apps, mobile back-ends, provide integration and maintenance All-round website development services from design to maintenance with 180 web experts and a record of 250 delivered websites   We create corporate web portals and intranets to help established enterprises benefit from collaboration and document management Industry-focused consulting, customizing and loyalty solutions for B2B and B2C enterprises, featuring a retail bank CRM with 7 mln clients Bringing in Data Science and BI expertise since 1989, we cover our clients’ needs with data warehouses, OLAP cubes, reports and dashboards …exciting journey from the dawn of articficial intelligence systems to the connected world of outsourcing nurturing relationships with Microsoft, IBM, Oracle and other leaders. …and still growing - in 2014 ScienceSoft won the Fastest Growing Company Award from Ernst &amp; Young. …for happy customers from over 25 countries including giants such as IBM, Tieto, PerkinElmer and Leo Burnett as well as SMEs and startups such as would-be Viber.  ScienceSoft has proved itself to be a trusted partner for proceeding with long-term relationship. We are delighted to have found such a highly professional, reliable and committed technology partner in ScienceSoft.  I have been very satisfied with the quality of their product and have been pleasantly surprised by their level of service. here                                  Svenska                                                               Français                                                               Deutsch                                                               Suomi                                                               Русский                              Home About Company Team Management Team Our Specialists How We Work Development Process Agile development Quality Management System Delivery Models Intellectual Property Protection Free White Papers Milestones Strategic Relations Testimonials Corporate Social Responsibility Photo Gallery Blog Services Custom Software Development Healthcare Life Sciences Patient Engagement Telecom Banking and Finance Retail Marketing Data Analysis Outsourced Product Development Desktop application development Mobile Application Development Enterprise Mobile Application Development Mobile Technology Consulting Mobile Medical Application Development Cross-Platform Mobile Development Xamarin Development Website Design and Development Corporate Web Portal Development Website Redesign Medical Website Design E-commerce Website Development Outsourced Development Center Software QA and Testing Functional Testing Performance Testing Automated Testing Data Warehouse / Business Intelligence Testing Mobile Device Testing Cloud and Network Services Cloud Infrastructure Management Application Maintenance and Support Enterprise System Management Services Networking Management Services Microsoft Office 365 Migration IT Service Management Solutions CRM &amp; Loyalty Microsoft Dynamics CRM Consulting and Customization  Charts/BI Solution for MS Dynamics CRM CRM for Retail Loyalty for Retail EmailScoop N to N Grid SharePoint SharePoint Competence Center Corporate Portals and Intranets Customer Portals SharePoint Migration SharePoint Maintenance and Support SharePoint Health Check Service SharePoint add-ins InOffice Cakes&amp;Candles  Weather Vibes Images Uploader News Trap Workflows Manager  Office Compass Map Contacts Rates Description Business Intelligence Advanced Data Analysis Data Integration &amp; Reporting BI Infrastructure  Security Intelligence SIEM Services Identity and Access Management Services  Fraud Protection for Banks SIEM Case Studies SIEM Materials to Download Health Check Framework for IBM QRadar SIEM Enterprise Content Management (ECM) Technologies C++ Qt .NET .NET Framework Java PHP Frontend Mobile Database Development Databases Case Studies Healthcare Telecommunications Retail Banking Entertainment Education Travel and Hospitality Logistics and Transportation Manufacturing Oil and Gas  Press Room Press Releases Media Coverage Careers Vacancies Working for ScienceSoft Contact Us Request a Quote Become ScienceSoft’s Partner                                                                                 Custom Software Development                                 See more                                                                                               Enterprise Mobile Apps                                 See more                                                                                               Websites and Portals                                 See more                                                                                               SharePoint                                 See more                                                                                               Dynamics CRM                                 See more                                                                                               Business Intelligence                                 See more                    James Bowerman ,              IBM             Director Compliance Product Development                       Marc O'Dwyer,              Big Red Book             Managing Director                       Ryan O'Grady,              Fotaflo              CEO          Home About Services Solutions Case Studies Press Room Careers Contact Us Site Map                                        Services Custom Software Development Outsourced Product Development Mobile Application Development Website Design and Development Outsourced Development Center Software QA and Testing Cloud and Network Services About Company Team Delivery Models IP Protection Development Process Quality Management System Contact us Contact Information Become ScienceSoft's Partner Request for Quote contact@scnsoft.com +1 214 306 68 37 contact@scnsoft.com English Svenska Français Deutsch Suomi Русский Menu Home 26+ 450+ 1200+ IBM Director Compliance Product Development Big Red Book Managing Director Fotaflo  CEO © 1989–2015 ScienceSoft Inc. Phone: +1 214 306 68 37 Email: contact@scnsoft.com                  © 1989–2015 ScienceSoft Inc.                 Phone: +1 214 306 68 37                 Email: contact@scnsoft.com              © 1989–2015 ScienceSoft Inc. Phone: +1 214 306 68 37 Email: contact@scnsoft.com</v>
+        <v>Software Development Company Application Development Outsourcing ScienceSoft ScienceSoft is a custom software development company with 26 years experience 450 experts and operations in Texas USA and Europe software development company application development outsourcing application development company custom software development Professional Software Development Custom Software Development Enterprise Mobile Apps Websites and Portals SharePoint Dynamics CRM Business Intelligence 26 years in IT business 450 employees 1200 completed projects Testimonials Partners Our locations Home About Company Team Management Team Our Specialists How We Work Development Process Agile development Quality Management System Delivery Models Intellectual Property Protection Free White Papers Milestones Strategic Relations Testimonials Corporate Social Responsibility Photo Gallery Blog Company Team Management Team Our Specialists Management Team Our Specialists How We Work Development Process Agile development Quality Management System Delivery Models Intellectual Property Protection Free White Papers Development Process Agile development Agile development Quality Management System Delivery Models Intellectual Property Protection Free White Papers Milestones Strategic Relations Testimonials Corporate Social Responsibility Photo Gallery Blog Services Custom Software Development Healthcare Life Sciences Patient Engagement Telecom Banking and Finance Retail Marketing Data Analysis Outsourced Product Development Desktop application development Mobile Application Development Enterprise Mobile Application Development Mobile Technology Consulting Mobile Medical Application Development CrossPlatform Mobile Development Xamarin Development Website Design and Development Corporate Web Portal Development Website Redesign Medical Website Design Ecommerce Website Development Outsourced Development Center Software QA and Testing Functional Testing Performance Testing Automated Testing Data Warehouse Business Intelligence Testing Mobile Device Testing Cloud and Network Services Cloud Infrastructure Management Application Maintenance and Support Enterprise System Management Services Networking Management Services Microsoft Office 365 Migration IT Service Management Custom Software Development Healthcare Life Sciences Patient Engagement Telecom Banking and Finance Retail Marketing Data Analysis Healthcare Life Sciences Patient Engagement Telecom Banking and Finance Retail Marketing Data Analysis Outsourced Product Development Desktop application development Desktop application development Mobile Application Development Enterprise Mobile Application Development Mobile Technology Consulting Mobile Medical Application Development CrossPlatform Mobile Development Xamarin Development Enterprise Mobile Application Development Mobile Technology Consulting Mobile Medical Application Development CrossPlatform Mobile Development Xamarin Development Website Design and Development Corporate Web Portal Development Website Redesign Medical Website Design Ecommerce Website Development Corporate Web Portal Development Website Redesign Medical Website Design Ecommerce Website Development Outsourced Development Center Software QA and Testing Functional Testing Performance Testing Automated Testing Data Warehouse Business Intelligence Testing Mobile Device Testing Functional Testing Performance Testing Automated Testing Data Warehouse Business Intelligence Testing Mobile Device Testing Cloud and Network Services Cloud Infrastructure Management Application Maintenance and Support Enterprise System Management Services Networking Management Services Microsoft Office 365 Migration IT Service Management Cloud Infrastructure Management Application Maintenance and Support Enterprise System Management Services Networking Management Services Microsoft Office 365 Migration IT Service Management Solutions CRM Loyalty Microsoft Dynamics CRM Consulting and Customization ChartsBI Solution for MS Dynamics CRM CRM for Retail Loyalty for Retail EmailScoop N to N Grid SharePoint SharePoint Competence Center Corporate Portals and Intranets Customer Portals SharePoint Migration SharePoint Maintenance and Support SharePoint Health Check Service SharePoint addins InOffice CakesCandles Weather Vibes Images Uploader News Trap Workflows Manager Office Compass Map Contacts Rates Description Business Intelligence Advanced Data Analysis Data Integration Reporting BI Infrastructure Security Intelligence SIEM Services Identity and Access Management Services Fraud Protection for Banks SIEM Case Studies SIEM Materials to Download Health Check Framework for IBM QRadar SIEM Enterprise Content Management ECM CRM Loyalty Microsoft Dynamics CRM Consulting and Customization ChartsBI Solution for MS Dynamics CRM CRM for Retail Loyalty for Retail EmailScoop N to N Grid Microsoft Dynamics CRM Consulting and Customization ChartsBI Solution for MS Dynamics CRM ChartsBI Solution for MS Dynamics CRM CRM for Retail Loyalty for Retail EmailScoop N to N Grid SharePoint SharePoint Competence Center Corporate Portals and Intranets Customer Portals SharePoint Migration SharePoint Maintenance and Support SharePoint Health Check Service SharePoint addins InOffice CakesCandles Weather Vibes Images Uploader News Trap Workflows Manager Office Compass Map Contacts Rates Description SharePoint Competence Center Corporate Portals and Intranets Customer Portals SharePoint Migration SharePoint Maintenance and Support SharePoint Health Check Service SharePoint addins InOffice CakesCandles Weather Vibes Images Uploader News Trap Workflows Manager Office Compass Map Contacts Rates Description InOffice CakesCandles Weather Vibes Images Uploader News Trap Workflows Manager Office Compass Map Contacts Rates Description Business Intelligence Advanced Data Analysis Data Integration Reporting BI Infrastructure Advanced Data Analysis Data Integration Reporting BI Infrastructure Security Intelligence SIEM Services Identity and Access Management Services Fraud Protection for Banks SIEM Case Studies SIEM Materials to Download Health Check Framework for IBM QRadar SIEM SIEM Services Identity and Access Management Services Fraud Protection for Banks SIEM Case Studies SIEM Materials to Download Health Check Framework for IBM QRadar SIEM Enterprise Content Management ECM Technologies C Qt NET NET Framework Java PHP Frontend Mobile Database Development Databases C Qt Qt NET NET Framework NET Framework Java PHP Frontend Mobile Database Development Databases Databases Case Studies Healthcare Telecommunications Retail Banking Entertainment Education Travel and Hospitality Logistics and Transportation Manufacturing Oil and Gas Healthcare Telecommunications Retail Banking Entertainment Education Travel and Hospitality Logistics and Transportation Manufacturing Oil and Gas Press Room Press Releases Media Coverage Press Releases Media Coverage Careers Vacancies Working for ScienceSoft Vacancies Working for ScienceSoft Contact Us Request a Quote Become ScienceSoft’s Partner Request a Quote Become ScienceSoft’s Partner Home About Services Solutions Case Studies Press Room Careers Contact Us Site Map We offer fullcycle development services for web mobile and desktop that have already brought value to Walmart eBay and Viber 75 experts 300 projects We develop iOS Android WP Cordova and Xamarin apps mobile backends provide integration and maintenance Allround website development services from design to maintenance with 180 web experts and a record of 250 delivered websites We create corporate web portals and intranets to help established enterprises benefit from collaboration and document management Industryfocused consulting customizing and loyalty solutions for B2B and B2C enterprises featuring a retail bank CRM with 7 mln clients Bringing in Data Science and BI expertise since 1989 we cover our clients’ needs with data warehouses OLAP cubes reports and dashboards …exciting journey from the dawn of articficial intelligence systems to the connected world of outsourcing nurturing relationships with Microsoft IBM Oracle and other leaders …and still growing in 2014 ScienceSoft won the Fastest Growing Company Award from Ernst Young …for happy customers from over 25 countries including giants such as IBM Tieto PerkinElmer and Leo Burnett as well as SMEs and startups such as wouldbe Viber ScienceSoft has proved itself to be a trusted partner for proceeding with longterm relationship We are delighted to have found such a highly professional reliable and committed technology partner in ScienceSoft I have been very satisfied with the quality of their product and have been pleasantly surprised by their level of service here Svenska Français Deutsch Suomi Русский Home About Company Team Management Team Our Specialists How We Work Development Process Agile development Quality Management System Delivery Models Intellectual Property Protection Free White Papers Milestones Strategic Relations Testimonials Corporate Social Responsibility Photo Gallery Blog Services Custom Software Development Healthcare Life Sciences Patient Engagement Telecom Banking and Finance Retail Marketing Data Analysis Outsourced Product Development Desktop application development Mobile Application Development Enterprise Mobile Application Development Mobile Technology Consulting Mobile Medical Application Development CrossPlatform Mobile Development Xamarin Development Website Design and Development Corporate Web Portal Development Website Redesign Medical Website Design Ecommerce Website Development Outsourced Development Center Software QA and Testing Functional Testing Performance Testing Automated Testing Data Warehouse Business Intelligence Testing Mobile Device Testing Cloud and Network Services Cloud Infrastructure Management Application Maintenance and Support Enterprise System Management Services Networking Management Services Microsoft Office 365 Migration IT Service Management Solutions CRM Loyalty Microsoft Dynamics CRM Consulting and Customization ChartsBI Solution for MS Dynamics CRM CRM for Retail Loyalty for Retail EmailScoop N to N Grid SharePoint SharePoint Competence Center Corporate Portals and Intranets Customer Portals SharePoint Migration SharePoint Maintenance and Support SharePoint Health Check Service SharePoint addins InOffice CakesCandles Weather Vibes Images Uploader News Trap Workflows Manager Office Compass Map Contacts Rates Description Business Intelligence Advanced Data Analysis Data Integration Reporting BI Infrastructure Security Intelligence SIEM Services Identity and Access Management Services Fraud Protection for Banks SIEM Case Studies SIEM Materials to Download Health Check Framework for IBM QRadar SIEM Enterprise Content Management ECM Technologies C Qt NET NET Framework Java PHP Frontend Mobile Database Development Databases Case Studies Healthcare Telecommunications Retail Banking Entertainment Education Travel and Hospitality Logistics and Transportation Manufacturing Oil and Gas Press Room Press Releases Media Coverage Careers Vacancies Working for ScienceSoft Contact Us Request a Quote Become ScienceSoft’s Partner Custom Software Development See more Enterprise Mobile Apps See more Websites and Portals See more SharePoint See more Dynamics CRM See more Business Intelligence See more James Bowerman IBM Director Compliance Product Development Marc ODwyer Big Red Book Managing Director Ryan OGrady Fotaflo CEO Home About Services Solutions Case Studies Press Room Careers Contact Us Site Map Services Custom Software Development Outsourced Product Development Mobile Application Development Website Design and Development Outsourced Development Center Software QA and Testing Cloud and Network Services About Company Team Delivery Models IP Protection Development Process Quality Management System Contact us Contact Information Become ScienceSofts Partner Request for Quote contactscnsoftcom 1 214 306 68 37 contactscnsoftcom English Svenska Français Deutsch Suomi Русский Menu Home 26 450 1200 IBM Director Compliance Product Development Big Red Book Managing Director Fotaflo CEO © 19892015 ScienceSoft Inc Phone 1 214 306 68 37 Email contactscnsoftcom © 19892015 ScienceSoft Inc Phone 1 214 306 68 37 Email contactscnsoftcom © 19892015 ScienceSoft Inc Phone 1 214 306 68 37 Email contactscnsoftcom</v>
       </c>
     </row>
     <row r="14">
@@ -633,16 +531,10 @@
         <v>developers</v>
       </c>
       <c r="C14" t="str">
-        <v>Itransition Software Development Company. Custom Software Programming Services Itransition Software Company with 16 years in software development and pool of 1200 software developers offers custom software development, web and mobile development, QA services. Headquartered in Austin, Texas and offshore software development centers in Eastern Europe. Expanding Your Software Horizons Technology Consulting Software Prototyping Custom Software Development Software Product Development Enterprise Application Integration Application Security Virtualization Management Software QA and Testing Dedicated Development Centers Customer Service Devops-as-a-Service B2B and B2C Web Portals Enterprise Extranets and Intranets Document Management Business Intelligence Enterprise Resource Planning Enterprise Content Management Customer Relationship Management Billing and Payments Enterprise Mobility .NET Java PHP Python Ruby on Rails C/C++ SAP Mobile About Advantages Awards and Recognition Approach Partnership Executive Blog Corporate News Career ENTERPRISE SOFTWARE. ADVANCED WEB. MOBILE APPS. Our customers About SELECTED CASES About HighLights HighLights Quick Start Contact Us Result-Driven Software Services  Value-Added Solutions &amp; Domains Expertise Enterprise Portals &amp; Intranets    B2B and B2C Web Portals    Enterprise Content/Document Management    Content Management and Distribution    Enterprise Resource Planning    Business Intelligence    Billing and Payments    Customer Relationship Management    Enterprise Portals &amp; Intranets    B2B and B2C Web Portals    Enterprise Content/Document Management    Content Management and Distribution    Enterprise Resource Planning    Business Intelligence    Billing and Payments    Customer Relationship Management  Technology Excellence and Maturity  Dedicated Development Center Services Result-Driven Software Services  Solutions Value-Added Solutions &amp; Domains Expertise   Enterprise Portals &amp; Intranets    B2B and B2C Web Portals    Enterprise Content/Document Management    Content Management and Distribution    Enterprise Resource Planning    Business Intelligence    Billing and Payments    Customer Relationship Management    Enterprise Portals &amp; Intranets    B2B and B2C Web Portals    Enterprise Content/Document Management    Content Management and Distribution    Enterprise Resource Planning    Business Intelligence    Billing and Payments    Customer Relationship Management  2015 IAOP research Sales Knowledge Choosing the App Format How to Work With Partners 2015 IAOP research Sales Knowledge Choosing the App Format How to Work With Partners Contact Analysis Proposal Agile and Responsive Mature and Flexible  Complex Solutions Made Easy Our Technology Centers  Reliable Partner, Not Just a Vendor  Collaboration Matters Engage Build Trust Operate Agile and Responsive Mature and Flexible  Complex Solutions Made Easy Services   Technology ConsultingFrom resolving specific IT-related issues to strategic business transformation fueled by IT, we deliver full-featured technology consulting services:  IT Infrastructure Audit IT Strategy Development Software Architecture Review Application Security Consulting Project Requirements Design Business Process Analysis Software PrototypingPrototyping is a perfect choice for refining functionality, detecting potential issues and setting right priorities. We deliver:  Specification Sketches Clickable Wireframes Designed Interface Working Prototype  Custom Software DevelopmentFrom smart customization of the pre-developed platforms to full-cycle custom software development along with your vision, Itransition is here to deliver custom software solutions that match your unique requirements.  Enterprise Solutions Web Applications (incl.SaaS) Mobile Applications Software Product DevelopmentAs a full-cycle Software Product Development service vendor, we are here to support you at any stage of your product evolution:  Feasibility Study Prototyping &amp; Design Development Customization &amp; Deployment Support &amp; Maintenance Enterprise Application IntegrationWe provide a full range of integration services to help our customers streamline their operations across multiple systems, data sources and/or locations:  Analysis &amp; Consulting Enterprise Service Bus Implementation  Hub-and-spoke Integration Point-to-point Integration &amp; Ad Hoc Solutions Application SecurityWe offer expertise along with our value-added services across all three major blocks to ensure your all round security:  Operational Security (processes, policies, regulations) Infrastructure Security (network &amp; OS-level Application Security (security development lifecycle framework) Virtualization ManagementWe are ready to help you with all the aspects of virtualization:  IT Infrastructure Assessment &amp; Gap Analysis Virtual Infrastructure Design &amp; Planning Financial Analysis (Licensing) Implementation &amp; Migration Ongoing Management &amp; Maintenance  Software QA and TestingWe deliver both stand-alone and integrated testing services, offering supreme quality assurance through deep understanding of your business goals and applications:  QA Consulting Full-Cycle QA Software Testing Test Automation  Compliance Testing &amp; Pre-Certification  Dedicated Development CentersWe offer you a time-proven, individually adjusted cooperation strategy for a win-win result/ Launching your Dedicated Team with Itransition you will surely get:  Full Control Scalability &amp; Flexibility Established Processes Exclusive Engagement  Customer ServiceWith Itransition, you can fully rely on our team to take care of your customer needs. We ensure all-round, top-notch user experience for you and your clients via:  Customer Issue Management Back Office Services Technical Support  Devops-as-a-ServiceItransition provides DevOps-as-a-Service, automating end-to-end delivery processes and ensuring the scalability and security of large enterprises and newborn startups' infrastructure. We bring your development and operations together by addressing key pain-points in your DevOps spectrum, enabling your business to produce innovative capabilities faster and in an efficient manner. We offer:  DevOps Assessment DevOps Automation DevOps Management   Technology ConsultingSoftware PrototypingCustom Software DevelopmentSoftware Product DevelopmentEnterprise Application IntegrationApplication SecurityVirtualization ManagementSoftware QA and TestingDedicated Development CentersCustomer ServiceDevops-as-a-Service  IT Infrastructure Audit IT Strategy Development Software Architecture Review Application Security Consulting Project Requirements Design Business Process Analysis Specification Sketches Clickable Wireframes Designed Interface Working Prototype Enterprise Solutions Web Applications (incl.SaaS) Mobile Applications Feasibility Study Prototyping &amp; Design Development Customization &amp; Deployment Support &amp; Maintenance Analysis &amp; Consulting Enterprise Service Bus Implementation  Hub-and-spoke Integration Point-to-point Integration &amp; Ad Hoc Solutions Operational Security (processes, policies, regulations) Infrastructure Security (network &amp; OS-level Application Security (security development lifecycle framework) IT Infrastructure Assessment &amp; Gap Analysis Virtual Infrastructure Design &amp; Planning Financial Analysis (Licensing) Implementation &amp; Migration Ongoing Management &amp; Maintenance QA Consulting Full-Cycle QA Software Testing Test Automation  Compliance Testing &amp; Pre-Certification Full Control Scalability &amp; Flexibility Established Processes Exclusive Engagement Customer Issue Management Back Office Services Technical Support DevOps Assessment DevOps Automation DevOps Management  Technology Consulting Software Prototyping Custom Software Development Software Product Development Enterprise Application Integration Application Security Virtualization Management Software QA and Testing Dedicated Development Centers Customer Service Devops-as-a-Service Solutions  B2B and B2C Web PortalsFrom compact vertical solutions to complex cloud portals, we deliver rich online experience for:  Ecommerce Media &amp; Entertainment Social Networks &amp; Communities And more Enterprise Extranets and IntranetsWe build a complete portal infrastructure that allows for people-centric integration of all types of enterprise information assets to enhance:  Internal &amp; External Collaboration Data Visualization Employee &amp; Knowledge Management  Document ManagementWe deliver full-cycle and industry-specific DMS solutions to enterprises operating in:  Retail Oil&amp;Gas Telecom And more Business IntelligenceSeeking to derive actionable insights from the avalanche of data? Itransition delivers Business Intelligence and Analytics solutions to enable access to, analysis and visual representation of data at its peak value. We deliver:  Tailored BI Components  Full-fledged BI Solutions  Enterprise Resource PlanningFocused on delivering efficient ERP solutions that match your business needs and IT development strategy, we utilize three main ERP tech stacks:  SAP Product Family Microsoft Solutions Open Source Platforms Enterprise Content ManagementOur experience allows us to leverage ECM capabilities to help you consolidate heterogeneous content of the following types into a single centrally managed repository:  Documents &amp; Records Media Assets Web Content Customer Relationship ManagementStriving to make the most valuable CRM features work for your business, we offer:  Custom CRM Solutions &amp; Add-ons Development Microsoft Dynamics Implementation SalesForce Integration Billing and PaymentsFor financial institutions and companies with specific industry needs we offer expertise in developing and implementing service-oriented solutions fully covering the following areas:  Invoicing &amp; Billing Payment  Management Enterprise MobilityEnterprise mobility projects of different scale and complexity for companies striving to:  Empower their field personnel, mobile and travelling employees Connect with mobile customers Enrich business with new services and mobile commerce B2B and B2C Web PortalsEnterprise Extranets and IntranetsDocument ManagementBusiness IntelligenceEnterprise Resource PlanningEnterprise Content ManagementCustomer Relationship ManagementBilling and PaymentsEnterprise Mobility  Ecommerce Media &amp; Entertainment Social Networks &amp; Communities And more Internal &amp; External Collaboration Data Visualization Employee &amp; Knowledge Management Retail Oil&amp;Gas Telecom And more Tailored BI Components  Full-fledged BI Solutions  SAP Product Family Microsoft Solutions Open Source Platforms Documents &amp; Records Media Assets Web Content Custom CRM Solutions &amp; Add-ons Development Microsoft Dynamics Implementation SalesForce Integration Invoicing &amp; Billing Payment  Customer Management Empower their field personnel, mobile and travelling employees Connect with mobile customers Enrich business with new services and mobile commerce B2B and B2C Web Portals Enterprise Extranets and Intranets Document Management Business Intelligence Enterprise Resource Planning Enterprise Content Management Customer Relationship Management Billing and Payments Enterprise Mobility Technologies  .NETWe've been investing in .Net development from the very first day of the framework introduction. As a Microsoft Gold Certified Partner with a pool of 400+ technology experts, we deliver:   Enterprise solutions  Desktop applications  Web applications JavaInitially established as a Java development company, we've evolved into a global IT services provider with a diversified portfolio of technologies, still preserving pristine passion for coding in Java, delivering:  Enterprise-level systems End-to-end web applications High-reliability solutions PHPWith over 12 years of experience in building reliable and scalable applications, our PHP development team have extensive knowledge of:  Custom web apps development Legacy apps enhancement  Database-driven websites And many more PythonOur Python engineers craft fast, effective and highly productive software across numerous application domains including:  Database-driven web applications Desktop GUIs  Corporate networking And many more Ruby on RailsPassionate Ruby evangelists and Ruby Masters, Itransition's RoR teams deliver  Database-driven web applications Robust online services and backends for mobile solutions Scalable e-commerce platforms and SaaS solutions C/C++From requirements management to delivery, product upgrades and support, we deliver full-cycle development of high-performance applications:  C/ C++ Native/Cross-Platform Apps C/ C++ Frameworks System-Level Software SAPWe've been a SAP Partner since 2008 delivering the following services:  SAP consulting SAP implementation &amp; rollouts SAP solution enhancement MobileWe offer extensive hands-on experience in development of incredibly feature-laden mobile applications:  iOS, Android, Windows Mobile web Cross-platform Legacy .NETJavaPHPPythonRuby on RailsC/C++SAPMobile   Enterprise solutions  Desktop applications  Web applications Enterprise-level systems End-to-end web applications High-reliability solutions Custom web apps development Legacy apps enhancement  Database-driven websites And many more Database-driven web applications Desktop GUIs  Corporate networking And many more Database-driven web applications Robust online services and backends for mobile solutions Scalable e-commerce platforms and SaaS solutions C/ C++ Native/Cross-Platform Apps C/ C++ Frameworks System-Level Software SAP consulting SAP implementation &amp; rollouts SAP solution enhancement iOS, Android, Windows Mobile web Cross-platform Legacy .NET Java PHP Python Ruby on Rails C/C++ SAP Mobile Portfolio Company  AboutItransition is expert in development, customization and integration of complex enterprise-level solutions offering a well-balanced blend of technology skills, domain knowledge, hands-on experience, effective methodology, and passion for IT.  Quick Facts Selected Customers Operating Principles Core Values AdvantagesThere are valid reasons why our clients make their choice in favor of Itransition:  Comprehensive Solutions Best Practices Qualified Expertise Reasonable Cost Seamless Communication Awards and RecognitionIndependently recognized by industry thought leaders, Itransition has been repeatedly included into the following lists:  Global Outsourcing 100  Software 500  Global Services 100 And more ApproachBeing a customer-oriented company, we do our best to make our processes as clear and transparent for you as possible.  Development Methodology Quality Management Project Organization Engagement Models PartnershipItransiton Channel Partnership Program provides partners around the world with the highest quality and greatest variety of IT services to maximize their business growth. Our Partnership Program comes in two levels:  Authorized Partner Preferred Partner Executive BlogOur corporate blog aims to offer a unique insight into the backstage of the outsourcing industry. We hope it helps to let you know more about what is going on in the industry we're working in, the solutions we're working on, and the processes we're applying while working. Stay tuned!Corporate NewsGet our corporate news &amp; all latest updates directly from Itransition - all our most recent achievements, freshly launched initiatives, updates on our service lines, solution offerings, news on partnerships, and many more. Stay tuned!CareerToday Itransition is the team of enthusiastic and forward-thinking managers, IT consultants, business analysts, software architects and developers, QA and maintenance engineers. Together they build a great company to work with. Join us!AboutAdvantagesAwards and RecognitionApproachPartnershipExecutive BlogCorporate NewsCareer  Quick Facts Selected Customers Operating Principles Core Values Comprehensive Solutions Best Practices Qualified Expertise Reasonable Cost Seamless Communication Global Outsourcing 100  Software 500  Global Services 100 And more Development Methodology Quality Management Project Organization Engagement Models Authorized Partner Preferred Partner About Advantages Awards and Recognition Approach Partnership Executive Blog Corporate News Career Contact Us Technology Consulting Software Prototyping Custom Software Development Software Product Development Enterprise Application Integration Application Security Virtualization Management Software QA and Testing Maintenance and Support Dedicated Development Centers    Enterprise Portals &amp; Intranets  Accelerated business processes through more efficient utilization of corporate information resources     B2B and B2C Web Portals  Advanced solutions for customer communication and service, supply chain management, sales automation and other business      Enterprise Content/Document Management  Facilitated document-related operations - document capturing, routing, life cycle management, search, etc     Content Management and Distribution  Heterogeneous content from diverse sources consolidated into a single centrally managed repository with accurate data      Enterprise Resource Planning  Rich functionality – from finance and human resources management to procurement and order  to boost      Business Intelligence  Enterprise-wide reporting, online analytical  data mining, benchmarking and business performance management      Billing and Payments  Service-oriented systems for financial institutions, payment service providers and companies with specific industry needs     Customer Relationship Management  Accelerated business processes − from account management &amp; marketing campaigns to sales automation &amp; customer service      Enterprise Portals &amp; Intranets  Accelerated business processes through more efficient utilization of corporate information resources     B2B and B2C Web Portals  Advanced solutions for customer communication and service, supply chain management, sales automation and other business      Enterprise Content/Document Management  Facilitated document-related operations - document capturing, routing, life cycle management, search, etc     Content Management and Distribution  Heterogeneous content from diverse sources consolidated into a single centrally managed repository with accurate data      Enterprise Resource Planning  Rich functionality – from finance and human resources management to procurement and order  to boost      Business Intelligence  Enterprise-wide reporting, online analytical  data mining, benchmarking and business performance management      Billing and Payments  Service-oriented systems for financial institutions, payment service providers and companies with specific industry needs     Customer Relationship Management  Accelerated business processes − from account management &amp; marketing campaigns to sales automation &amp; customer service    .NET   PHP   C++   JAVA   Ruby on Rails    Mobile   Core team setup   Organization of required infrastructure   Initial knowledge transfer   Setup and implementation of processes   Full-scale team ramp-up with required expertise and qualifications   Knowledge accumulation by the team   Methodology &amp; processes adjustment   Team performance optimization   Scaling up and down the team in line with your needs   Involving specific domain and technology experts on an ad hoc basis   Integrating with in-house and multi-site teams  Technology Consulting Software Prototyping Custom Software Development Software Product Development Enterprise Application Integration Application Security Virtualization Management Software QA and Testing Maintenance and Support Dedicated Development Centers    Enterprise Portals &amp; Intranets  Accelerated business processes through more efficient utilization of corporate information resources     B2B and B2C Web Portals  Advanced solutions for customer communication and service, supply chain management, sales automation and other business      Enterprise Content/Document Management  Facilitated document-related operations - document capturing, routing, life cycle management, search, etc     Content Management and Distribution  Heterogeneous content from diverse sources consolidated into a single centrally managed repository with accurate data      Enterprise Resource Planning  Rich functionality – from finance and human resources management to procurement and order  to boost      Business Intelligence  Enterprise-wide reporting, online analytical  data mining, benchmarking and business performance management      Billing and Payments  Service-oriented systems for financial institutions, payment service providers and companies with specific industry needs     Customer Relationship Management  Accelerated business processes − from account management &amp; marketing campaigns to sales automation &amp; customer service      Enterprise Portals &amp; Intranets  Accelerated business processes through more efficient utilization of corporate information resources     B2B and B2C Web Portals  Advanced solutions for customer communication and service, supply chain management, sales automation and other business      Enterprise Content/Document Management  Facilitated document-related operations - document capturing, routing, life cycle management, search, etc     Content Management and Distribution  Heterogeneous content from diverse sources consolidated into a single centrally managed repository with accurate data      Enterprise Resource Planning  Rich functionality – from finance and human resources management to procurement and order  to boost      Business Intelligence  Enterprise-wide reporting, online analytical  data mining, benchmarking and business performance management      Billing and Payments  Service-oriented systems for financial institutions, payment service providers and companies with specific industry needs     Customer Relationship Management  Accelerated business processes − from account management &amp; marketing campaigns to sales automation &amp; customer service                                                     Jose Brotons COO Product Madness                  Simon Aloyts CTO Liquid Generation                  Dan Zalta CEO Fee Technology                  John Liptak President UBERbase and Oakwood    .NET ISVs Banking &amp; Finance Billing &amp; Payments Collaboration Tools PHP Banking &amp; Finance Portals eLearning &amp; Online Training C/C++ Manufacturing Mobility Java ISVs Media Content Distribution Business Intelligence Portals Customer Relationship Management .NET Telecom Business Intelligence Enterprise Resource Management Ruby Legal Portals Collaboration Tools Java ISVs Banking &amp; Finance Billing &amp; Payments Public Sector Portals .NET ISVs .NET HTML5 eLearning &amp; Online Training Python Portals Media Content Distribution C/C++ Python Portals Media Content Distribution Manufacturing Collaboration Tools Mobility Customer Relationship Management Oil &amp; Gas Business Intelligence PHP Oil &amp; Gas Business Intelligence .NET Telecom .NET Telecom Collaboration Tools .NET ISVs Media &amp; Entertainment Business Intelligence Java Telecom .NET HTML5 Oil &amp; Gas Portals Collaboration Tools Portals Collaboration Tools Ruby Media Content Distribution Billing &amp; Payments Gaming .NET Social Networking Billing &amp; Payments Mobility .NET ISVs eCommerce eCommerce Social Networking Business Intelligence Java Banking &amp; Finance Enterprise Resource Management Java HTML5 Travel &amp; Hospitality Portals Ruby C/C++ ISVs Manufacturing Retail Portals Media Content Distribution Mobility   2015 IAOP research  We proudly announce that according to the 2015 Global Outsourcing 100 research Itransition scored best in the Customer Reference and Company Certification categories.     Sales Knowledge  Any business struggles with knowledge accumulation and making it transparent to all employees. Especially this is critical for sales departments in service companies.     Choosing the App Format  The choice of the best mobile delivery format is very important for any business nowadays. Which mobile delivery format suits you best?     How to Work With Partners  Here is the list of our 10 tips, which may help you build a strong foundation for your business partnership for many years to come.      2015 IAOP research  We proudly announce that according to the 2015 Global Outsourcing 100 research Itransition scored best in the Customer Reference and Company Certification categories.       Sales Knowledge  Any business struggles with knowledge accumulation and making it transparent to all employees. Especially this is critical for sales departments in service companies.       Choosing the App Format  The choice of the best mobile delivery format is very important for any business nowadays. Which mobile delivery format suits you best?       How to Work With Partners  Here is the list of our 10 tips, which may help you build a strong foundation for your business partnership for many years to come.      1 Contact Submit your project request (be it a detailed specification or just an idea) using our contact form.    Analysis We will contact you shortly to clarify your project requirements.   Proposal We will provide our free non-binding bid or proposal for your review.  About Advantages Awards &amp; Recognition Approach Partnership Executive Blog Corporate News Career Technology Consulting  Software Prototyping Custom Software Development  Software Product Development  Enterprise Application Integration Application Security Virtualization Management Software QA and Testing  Dedicated Development Centers Customer Service Devops-as-a-Service B2B and B2C Web Portals  Enterprise Extranets and Intranets  Document Management  Business Intelligence  Enterprise Resource Planning  Enterprise Content Management Customer Relationship Management Billing and Payments Enterprise Mobility .NET Java PHP Python Ruby on Rails C/C++ SAP Mobile              Jump to navigation  Delivering software projects worldwide to customers from startups &amp; SMBs to Fortune 500 companies. Balanced blend of technology skills and domain knowledge of 1,300 seasoned IT professionals, powered by passion for IT.  News Itransition Scored Best in the Customer Reference and Company Certification   News Itransition Enters the World’s Top Java Developers List   Blog Multiple Projects in the Services Sector – How to Juggle It All   News Itransition is 2015 Global Outsourcing 100® company   Blog The Three Most Destructive Outsourcing Stereotypes Debunked   Blog Gaining Competitive Advantage with Data-Driven Decision Making   Blog Some Risks And Challenges Of Outsourcing   Blog 10 Ways to Manage Professional Teams Effectively   Blog 10 Tips on How to Work With Business Partners  Our software outsourcing services range from technology consulting and business analysis to QA, application maintenance and solution integration. Our integrated service lines have been shaped by nearly two decades of delivering value to our customers, and are built on a deep understanding of business needs and market trends, along with the technology expertise and software industry best practices.  We are fully equipped to deliver first-class services that result in improved business efficiency, increased ROI cost-effectiveness, risk mitigation for our clients, not to speak of transparency and predictability that are guaranteed by default. We rely on our time-proven processes, tools and techniques to bring the highest level of quality to our growing range of services. At the same time we are highly flexible to meet the needs of various customers – from startups and SMBs to Fortune 500 companies.  From advanced Portals and eCommerce solutions to ERP &amp; BI, we are dedicated to build easy-to-use solutions (no matter how complex they could be) either from scratch or as a combination of out-of-the-box modules for you to reach your business goals the shortest way.  Accelerated business processes through more efficient utilization of corporate information resources Advanced solutions for customer communication and service, supply chain management, sales automation and other business  Facilitated document-related operations - document capturing, routing, life cycle management, search, etc Heterogeneous content from diverse sources consolidated into a single centrally managed repository with accurate data  Rich functionality – from finance and human resources management to procurement and order  to boost  Enterprise-wide reporting, online analytical  data mining, benchmarking and business performance management  Service-oriented systems for financial institutions, payment service providers and companies with specific industry needs Accelerated business processes − from account management &amp; marketing campaigns to sales automation &amp; customer service  Accelerated business processes through more efficient utilization of corporate information resources Advanced solutions for customer communication and service, supply chain management, sales automation and other business  Facilitated document-related operations - document capturing, routing, life cycle management, search, etc Heterogeneous content from diverse sources consolidated into a single centrally managed repository with accurate data  Rich functionality – from finance and human resources management to procurement and order  to boost  Enterprise-wide reporting, online analytical  data mining, benchmarking and business performance management  Service-oriented systems for financial institutions, payment service providers and companies with specific industry needs Accelerated business processes − from account management &amp; marketing campaigns to sales automation &amp; customer service  Since 1998, we’ve been maintaining a comprehensive technology stack for we know how to efficiently combine legacy and innovation to address your business challenges with the right technology. Our software developers know how to adopt and ramp up emerging programming technologies quickly to execute the most ambitious projects and deliver the right results in terms of efficiency, performance, interoperability, and user experience.  We will guide you through all the technologies and platforms available on the market to find your ideal solution. At the same time we always encourage you to share with us all your technology requirements, wishes and concerns. While our experience and expertise are fully at your service, we do believe that only close collaboration with our customers all the way a project goes can bring tangible results. A Dedicated Development Center at Itransition is an efficient way to boost your business with top-quality resources fully attuned to your requirements and business objectives. Your Dedicated Center run by Itransition is literally your doorway to hi-end software developers, infrastructure and advanced methodologies to ensure scalability and flexibility, while maintaining full control and transparency. Our software outsourcing services range from technology consulting and business analysis to QA, application maintenance and solution integration. Our integrated service lines have been shaped by nearly two decades of delivering value to our customers, and are built on a deep understanding of business needs and market trends, along with the technology expertise and software industry best practices.  We are fully equipped to deliver first-class services that result in improved business efficiency, increased ROI cost-effectiveness, risk mitigation for our clients, not to speak of transparency and predictability that are guaranteed by default. We rely on our time-proven processes, tools and techniques to bring the highest level of quality to our growing range of services. At the same time we are highly flexible to meet the needs of various customers – from startups and SMBs to Fortune 500 companies.  From advanced Portals and eCommerce solutions to ERP &amp; BI, we are dedicated to build easy-to-use solutions (no matter how complex they could be) either from scratch or as a combination of out-of-the-box modules for you to reach your business goals the shortest way.  Accelerated business processes through more efficient utilization of corporate information resources Advanced solutions for customer communication and service, supply chain management, sales automation and other business  Facilitated document-related operations - document capturing, routing, life cycle management, search, etc Heterogeneous content from diverse sources consolidated into a single centrally managed repository with accurate data  Rich functionality – from financ</v>
+        <v>Itransition Software Development Company Custom Software Programming Services Itransition Software Company with 16 years in software development and pool of 1200 software developers offers custom software development web and mobile development QA services Headquartered in Austin Texas and offshore software development centers in Eastern Europe Expanding Your Software Horizons Technology Consulting Software Prototyping Custom Software Development Software Product Development Enterprise Application Integration Application Security Virtualization Management Software QA and Testing Dedicated Development Centers Customer Service DevopsasaService B2B and B2C Web Portals Enterprise Extranets and Intranets Document Management Business Intelligence Enterprise Resource Planning Enterprise Content Management Customer Relationship Management Billing and Payments Enterprise Mobility NET Java PHP Python Ruby on Rails CC SAP Mobile About Advantages Awards and Recognition Approach Partnership Executive Blog Corporate News Career ENTERPRISE SOFTWARE ADVANCED WEB MOBILE APPS Our customers About SELECTED CASES About HighLights HighLights Quick Start Contact Us ResultDriven Software Services ValueAdded Solutions Domains Expertise Enterprise Portals Intranets B2B and B2C Web Portals Enterprise ContentDocument Management Content Management and Distribution Enterprise Resource Planning Business Intelligence Billing and Payments Customer Relationship Management Enterprise Portals Intranets B2B and B2C Web Portals Enterprise ContentDocument Management Content Management and Distribution Enterprise Resource Planning Business Intelligence Billing and Payments Customer Relationship Management Technology Excellence and Maturity Dedicated Development Center Services ResultDriven Software Services Solutions ValueAdded Solutions Domains Expertise Enterprise Portals Intranets B2B and B2C Web Portals Enterprise ContentDocument Management Content Management and Distribution Enterprise Resource Planning Business Intelligence Billing and Payments Customer Relationship Management Enterprise Portals Intranets B2B and B2C Web Portals Enterprise ContentDocument Management Content Management and Distribution Enterprise Resource Planning Business Intelligence Billing and Payments Customer Relationship Management 2015 IAOP research Sales Knowledge Choosing the App Format How to Work With Partners 2015 IAOP research Sales Knowledge Choosing the App Format How to Work With Partners Contact Analysis Proposal Agile and Responsive Mature and Flexible Complex Solutions Made Easy Our Technology Centers Reliable Partner Not Just a Vendor Collaboration Matters Engage Build Trust Operate Agile and Responsive Mature and Flexible Complex Solutions Made Easy Services Technology ConsultingFrom resolving specific ITrelated issues to strategic business transformation fueled by IT we deliver fullfeatured technology consulting services IT Infrastructure Audit IT Strategy Development Software Architecture Review Application Security Consulting Project Requirements Design Business Process Analysis Software PrototypingPrototyping is a perfect choice for refining functionality detecting potential issues and setting right priorities We deliver Specification Sketches Clickable Wireframes Designed Interface Working Prototype Custom Software DevelopmentFrom smart customization of the predeveloped platforms to fullcycle custom software development along with your vision Itransition is here to deliver custom software solutions that match your unique requirements Enterprise Solutions Web Applications inclSaaS Mobile Applications Software Product DevelopmentAs a fullcycle Software Product Development service vendor we are here to support you at any stage of your product evolution Feasibility Study Prototyping Design Development Customization Deployment Support Maintenance Enterprise Application IntegrationWe provide a full range of integration services to help our customers streamline their operations across multiple systems data sources andor locations Analysis Consulting Enterprise Service Bus Implementation Hubandspoke Integration Pointtopoint Integration Ad Hoc Solutions Application SecurityWe offer expertise along with our valueadded services across all three major blocks to ensure your all round security Operational Security processes policies regulations Infrastructure Security network OSlevel Application Security security development lifecycle framework Virtualization ManagementWe are ready to help you with all the aspects of virtualization IT Infrastructure Assessment Gap Analysis Virtual Infrastructure Design Planning Financial Analysis Licensing Implementation Migration Ongoing Management Maintenance Software QA and TestingWe deliver both standalone and integrated testing services offering supreme quality assurance through deep understanding of your business goals and applications QA Consulting FullCycle QA Software Testing Test Automation Compliance Testing PreCertification Dedicated Development CentersWe offer you a timeproven individually adjusted cooperation strategy for a winwin result Launching your Dedicated Team with Itransition you will surely get Full Control Scalability Flexibility Established Processes Exclusive Engagement Customer ServiceWith Itransition you can fully rely on our team to take care of your customer needs We ensure allround topnotch user experience for you and your clients via Customer Issue Management Back Office Services Technical Support DevopsasaServiceItransition provides DevOpsasaService automating endtoend delivery processes and ensuring the scalability and security of large enterprises and newborn startups infrastructure We bring your development and operations together by addressing key painpoints in your DevOps spectrum enabling your business to produce innovative capabilities faster and in an efficient manner We offer DevOps Assessment DevOps Automation DevOps Management Technology ConsultingSoftware PrototypingCustom Software DevelopmentSoftware Product DevelopmentEnterprise Application IntegrationApplication SecurityVirtualization ManagementSoftware QA and TestingDedicated Development CentersCustomer ServiceDevopsasaService IT Infrastructure Audit IT Strategy Development Software Architecture Review Application Security Consulting Project Requirements Design Business Process Analysis Specification Sketches Clickable Wireframes Designed Interface Working Prototype Enterprise Solutions Web Applications inclSaaS Mobile Applications Feasibility Study Prototyping Design Development Customization Deployment Support Maintenance Analysis Consulting Enterprise Service Bus Implementation Hubandspoke Integration Pointtopoint Integration Ad Hoc Solutions Operational Security processes policies regulations Infrastructure Security network OSlevel Application Security security development lifecycle framework IT Infrastructure Assessment Gap Analysis Virtual Infrastructure Design Planning Financial Analysis Licensing Implementation Migration Ongoing Management Maintenance QA Consulting FullCycle QA Software Testing Test Automation Compliance Testing PreCertification Full Control Scalability Flexibility Established Processes Exclusive Engagement Customer Issue Management Back Office Services Technical Support DevOps Assessment DevOps Automation DevOps Management Technology Consulting Software Prototyping Custom Software Development Software Product Development Enterprise Application Integration Application Security Virtualization Management Software QA and Testing Dedicated Development Centers Customer Service DevopsasaService Solutions B2B and B2C Web PortalsFrom compact vertical solutions to complex cloud portals we deliver rich online experience for Ecommerce Media Entertainment Social Networks Communities And more Enterprise Extranets and IntranetsWe build a complete portal infrastructure that allows for peoplecentric integration of all types of enterprise information assets to enhance Internal External Collaboration Data Visualization Employee Knowledge Management Document ManagementWe deliver fullcycle and industryspecific DMS solutions to enterprises operating in Retail OilGas Telecom And more Business IntelligenceSeeking to derive actionable insights from the avalanche of data Itransition delivers Business Intelligence and Analytics solutions to enable access to analysis and visual representation of data at its peak value We deliver Tailored BI Components Fullfledged BI Solutions Enterprise Resource PlanningFocused on delivering efficient ERP solutions that match your business needs and IT development strategy we utilize three main ERP tech stacks SAP Product Family Microsoft Solutions Open Source Platforms Enterprise Content ManagementOur experience allows us to leverage ECM capabilities to help you consolidate heterogeneous content of the following types into a single centrally managed repository Documents Records Media Assets Web Content Customer Relationship ManagementStriving to make the most valuable CRM features work for your business we offer Custom CRM Solutions Addons Development Microsoft Dynamics Implementation SalesForce Integration Billing and PaymentsFor financial institutions and companies with specific industry needs we offer expertise in developing and implementing serviceoriented solutions fully covering the following areas Invoicing Billing Payment Management Enterprise MobilityEnterprise mobility projects of different scale and complexity for companies striving to Empower their field personnel mobile and travelling employees Connect with mobile customers Enrich business with new services and mobile commerce B2B and B2C Web PortalsEnterprise Extranets and IntranetsDocument ManagementBusiness IntelligenceEnterprise Resource PlanningEnterprise Content ManagementCustomer Relationship ManagementBilling and PaymentsEnterprise Mobility Ecommerce Media Entertainment Social Networks Communities And more Internal External Collaboration Data Visualization Employee Knowledge Management Retail OilGas Telecom And more Tailored BI Components Fullfledged BI Solutions SAP Product Family Microsoft Solutions Open Source Platforms Documents Records Media Assets Web Content Custom CRM Solutions Addons Development Microsoft Dynamics Implementation SalesForce Integration Invoicing Billing Payment Customer Management Empower their field personnel mobile and travelling employees Connect with mobile customers Enrich business with new services and mobile commerce B2B and B2C Web Portals Enterprise Extranets and Intranets Document Management Business Intelligence Enterprise Resource Planning Enterprise Content Management Customer Relationship Management Billing and Payments Enterprise Mobility Technologies NETWeve been investing in Net development from the very first day of the framework introduction As a Microsoft Gold Certified Partner with a pool of 400 technology experts we deliver Enterprise solutions Desktop applications Web applications JavaInitially established as a Java development company weve evolved into a global IT services provider with a diversified portfolio of technologies still preserving pristine passion for coding in Java delivering Enterpriselevel systems Endtoend web applications Highreliability solutions PHPWith over 12 years of experience in building reliable and scalable applications our PHP development team have extensive knowledge of Custom web apps development Legacy apps enhancement Databasedriven websites And many more PythonOur Python engineers craft fast effective and highly productive software across numerous application domains including Databasedriven web applications Desktop GUIs Corporate networking And many more Ruby on RailsPassionate Ruby evangelists and Ruby Masters Itransitions RoR teams deliver Databasedriven web applications Robust online services and backends for mobile solutions Scalable ecommerce platforms and SaaS solutions CCFrom requirements management to delivery product upgrades and support we deliver fullcycle development of highperformance applications C C NativeCrossPlatform Apps C C Frameworks SystemLevel Software SAPWeve been a SAP Partner since 2008 delivering the following services SAP consulting SAP implementation rollouts SAP solution enhancement MobileWe offer extensive handson experience in development of incredibly featureladen mobile applications iOS Android Windows Mobile web Crossplatform Legacy NETJavaPHPPythonRuby on RailsCCSAPMobile Enterprise solutions Desktop applications Web applications Enterpriselevel systems Endtoend web applications Highreliability solutions Custom web apps development Legacy apps enhancement Databasedriven websites And many more Databasedriven web applications Desktop GUIs Corporate networking And many more Databasedriven web applications Robust online services and backends for mobile solutions Scalable ecommerce platforms and SaaS solutions C C NativeCrossPlatform Apps C C Frameworks SystemLevel Software SAP consulting SAP implementation rollouts SAP solution enhancement iOS Android Windows Mobile web Crossplatform Legacy NET Java PHP Python Ruby on Rails CC SAP Mobile Portfolio Company AboutItransition is expert in development customization and integration of complex enterpriselevel solutions offering a wellbalanced blend of technology skills domain knowledge handson experience effective methodology and passion for IT Quick Facts Selected Customers Operating Principles Core Values AdvantagesThere are valid reasons why our clients make their choice in favor of Itransition Comprehensive Solutions Best Practices Qualified Expertise Reasonable Cost Seamless Communication Awards and RecognitionIndependently recognized by industry thought leaders Itransition has been repeatedly included into the following lists Global Outsourcing 100 Software 500 Global Services 100 And more ApproachBeing a customeroriented company we do our best to make our processes as clear and transparent for you as possible Development Methodology Quality Management Project Organization Engagement Models PartnershipItransiton Channel Partnership Program provides partners around the world with the highest quality and greatest variety of IT services to maximize their business growth Our Partnership Program comes in two levels Authorized Partner Preferred Partner Executive BlogOur corporate blog aims to offer a unique insight into the backstage of the outsourcing industry We hope it helps to let you know more about what is going on in the industry were working in the solutions were working on and the processes were applying while working Stay tunedCorporate NewsGet our corporate news all latest updates directly from Itransition all our most recent achievements freshly launched initiatives updates on our service lines solution offerings news on partnerships and many more Stay tunedCareerToday Itransition is the team of enthusiastic and forwardthinking managers IT consultants business analysts software architects and developers QA and maintenance engineers Together they build a great company to work with Join usAboutAdvantagesAwards and RecognitionApproachPartnershipExecutive BlogCorporate NewsCareer Quick Facts Selected Customers Operating Principles Core Values Comprehensive Solutions Best Practices Qualified Expertise Reasonable Cost Seamless Communication Global Outsourcing 100 Software 500 Global Services 100 And more Development Methodology Quality Management Project Organization Engagement Models Authorized Partner Preferred Partner About Advantages Awards and Recognition Approach Partnership Executive Blog Corporate News Career Contact Us Technology Consulting Software Prototyping Custom Software Development Software Product Development Enterprise Application Integration Application Security Virtualization Management Software QA and Testing Maintenance and Support Dedicated Development Centers Enterprise Portals Intranets Accelerated business processes through more efficient utilization of corporate information resources B2B and B2C Web Portals Advanced solutions for customer communication and service supply chain management sales automation and other business Enterprise ContentDocument Management Facilitated documentrelated operations document capturing routing life cycle management search etc Content Management and Distribution Heterogeneous content from diverse sources consolidated into a single centrally managed repository with accurate data Enterprise Resource Planning Rich functionality from finance and human resources management to procurement and order to boost Business Intelligence Enterprisewide reporting online analytical data mining benchmarking and business performance management Billing and Payments Serviceoriented systems for financial institutions payment service providers and companies with specific industry needs Customer Relationship Management Accelerated business processes − from account management marketing campaigns to sales automation customer service Enterprise Portals Intranets Accelerated business processes through more efficient utilization of corporate information resources B2B and B2C Web Portals Advanced solutions for customer communication and service supply chain management sales automation and other business Enterprise ContentDocument Management Facilitated documentrelated operations document capturing routing life cycle management search etc Content Management and Distribution Heterogeneous content from diverse sources consolidated into a single centrally managed repository with accurate data Enterprise Resource Planning Rich functionality from finance and human resources management to procurement and order to boost Business Intelligence Enterprisewide reporting online analytical data mining benchmarking and business performance management Billing and Payments Serviceoriented systems for financial institutions payment service providers and companies with specific industry needs Customer Relationship Management Accelerated business processes − from account management marketing campaigns to sales automation customer service NET PHP C JAVA Ruby on Rails Mobile Core team setup Organization of required infrastructure Initial knowledge transfer Setup and implementation of processes Fullscale team rampup with required expertise and qualifications Knowledge accumulation by the team Methodology processes adjustment Team performance optimization Scaling up and down the team in line with your needs Involving specific domain and technology experts on an ad hoc basis Integrating with inhouse and multisite teams Technology Consulting Software Prototyping Custom Software Development Software Product Development Enterprise Application Integration Application Security Virtualization Management Software QA and Testing Maintenance and Support Dedicated Development Centers Enterprise Portals Intranets Accelerated business processes through more efficient utilization of corporate information resources B2B and B2C Web Portals Advanced solutions for customer communication and service supply chain management sales automation and other business Enterprise ContentDocument Management Facilitated documentrelated operations document capturing routing life cycle management search etc Content Management and Distribution Heterogeneous content from diverse sources consolidated into a single centrally managed repository with accurate data Enterprise Resource Planning Rich functionality from finance and human resources management to procurement and order to boost Business Intelligence Enterprisewide reporting online analytical data mining benchmarking and business performance management Billing and Payments Serviceoriented systems for financial institutions payment service providers and companies with specific industry needs Customer Relationship Management Accelerated business processes − from account management marketing campaigns to sales automation customer service Enterprise Portals Intranets Accelerated business processes through more efficient utilization of corporate information resources B2B and B2C Web Portals Advanced solutions for customer communication and service supply chain management sales automation and other business Enterprise ContentDocument Management Facilitated documentrelated operations document capturing routing life cycle management search etc Content Management and Distribution Heterogeneous content from diverse sources consolidated into a single centrally managed repository with accurate data Enterprise Resource Planning Rich functionality from finance and human resources management to procurement and order to boost Business Intelligence Enterprisewide reporting online analytical data mining benchmarking and business performance management Billing and Payments Serviceoriented systems for financial institutions payment service providers and companies with specific industry needs Customer Relationship Management Accelerated business processes − from account management marketing campaigns to sales automation customer service Jose Brotons COO Product Madness Simon Aloyts CTO Liquid Generation Dan Zalta CEO Fee Technology John Liptak President UBERbase and Oakwood NET ISVs Banking Finance Billing Payments Collaboration Tools PHP Banking Finance Portals eLearning Online Training CC Manufacturing Mobility Java ISVs Media Content Distribution Business Intelligence Portals Customer Relationship Management NET Telecom Business Intelligence Enterprise Resource Management Ruby Legal Portals Collaboration Tools Java ISVs Banking Finance Billing Payments Public Sector Portals NET ISVs NET HTML5 eLearning Online Training Python Portals Media Content Distribution CC Python Portals Media Content Distribution Manufacturing Collaboration Tools Mobility Customer Relationship Management Oil Gas Business Intelligence PHP Oil Gas Business Intelligence NET Telecom NET Telecom Collaboration Tools NET ISVs Media Entertainment Business Intelligence Java Telecom NET HTML5 Oil Gas Portals Collaboration Tools Portals Collaboration Tools Ruby Media Content Distribution Billing Payments Gaming NET Social Networking Billing Payments Mobility NET ISVs eCommerce eCommerce Social Networking Business Intelligence Java Banking Finance Enterprise Resource Management Java HTML5 Travel Hospitality Portals Ruby CC ISVs Manufacturing Retail Portals Media Content Distribution Mobility 2015 IAOP research We proudly announce that according to the 2015 Global Outsourcing 100 research Itransition scored best in the Customer Reference and Company Certification categories Sales Knowledge Any business struggles with knowledge accumulation and making it transparent to all employees Especially this is critical for sales departments in service companies Choosing the App Format The choice of the best mobile delivery format is very important for any business nowadays Which mobile delivery format suits you best How to Work With Partners Here is the list of our 10 tips which may help you build a strong foundation for your business partnership for many years to come 2015 IAOP research We proudly announce that according to the 2015 Global Outsourcing 100 research Itransition scored best in the Customer Reference and Company Certification categories Sales Knowledge Any business struggles with knowledge accumulation and making it transparent to all employees Especially this is critical for sales departments in service companies Choosing the App Format The choice of the best mobile delivery format is very important for any business nowadays Which mobile delivery format suits you best How to Work With Partners Here is the list of our 10 tips which may help you build a strong foundation for your business partnership for many years to come 1 Contact Submit your project request be it a detailed specification or just an idea using our contact form Analysis We will contact you shortly to clarify your project requirements Proposal We will provide our free nonbinding bid or proposal for your review About Advantages Awards Recognition Approach Partnership Executive Blog Corporate News Career Technology Consulting Software Prototyping Custom Software Development Software Product Development Enterprise Application Integration Application Security Virtualization Management Software QA and Testing Dedicated Development Centers Customer Service DevopsasaService B2B and B2C Web Portals Enterprise Extranets and Intranets Document Management Business Intelligence Enterprise Resource Planning Enterprise Content Management Customer Relationship Management Billing and Payments Enterprise Mobility NET Java PHP Python Ruby on Rails CC SAP Mobile Jump to navigation Delivering software projects worldwide to customers from startups SMBs to Fortune 500 companies Balanced blend of technology skills and domain knowledge of 1300 seasoned IT professionals powered by passion for IT News Itransition Scored Best in the Customer Reference and Company Certification News Itransition Enters the World’s Top Java Developers List Blog Multiple Projects in the Services Sector How to Juggle It All News Itransition is 2015 Global Outsourcing 100® company Blog The Three Most Destructive Outsourcing Stereotypes Debunked Blog Gaining Competitive Advantage with DataDriven Decision Making Blog Some Risks And Challenges Of Outsourcing Blog 10 Ways to Manage Professional Teams Effectively Blog 10 Tips on How to Work With Business Partners Our software outsourcing services range from technology consulting and business analysis to QA application maintenance and solution integration Our integrated service lines have been shaped by nearly two decades of delivering value to our customers and are built on a deep understanding of business needs and market trends along with the technology expertise and software industry best practices We are fully equipped to deliver firstclass services that result in improved business efficiency increased ROI costeffectiveness risk mitigation for our clients not to speak of transparency and predictability that are guaranteed by default We rely on our timeproven processes tools and techniques to bring the highest level of quality to our growing range of services At the same time we are highly flexible to meet the needs of various customers from startups and SMBs to Fortune 500 companies From advanced Portals and eCommerce solutions to ERP BI we are dedicated to build easytouse solutions no matter how complex they could be either from scratch or as a combination of outofthebox modules for you to reach your business goals the shortest way Accelerated business processes through more efficient utilization of corporate information resources Advanced solutions for customer communication and service supply chain management sales automation and other business Facilitated documentrelated operations document capturing routing life cycle management search etc Heterogeneous content from diverse sources consolidated into a single centrally managed repository with accurate data Rich functionality from finance and human resources management to procurement and order to boost Enterprisewide reporting online analytical data mining benchmarking and business performance management Serviceoriented systems for financial institutions payment service providers and companies with specific industry needs Accelerated business processes − from account management marketing campaigns to sales automation customer service Accelerated business processes through more efficient utilization of corporate information resources Advanced solutions for customer communication and service supply chain management sales automation and other business Facilitated documentrelated operations document capturing routing life cycle management search etc Heterogeneous content from diverse sources consolidated into a single centrally managed repository with accurate data Rich functionality from finance and human resources management to procurement and order to boost Enterprisewide reporting online analytical data mining benchmarking and business performance management Serviceoriented systems for financial institutions payment service providers and companies with specific industry needs Accelerated business processes − from account management marketing campaigns to sales automation customer service Since 1998 we’ve been maintaining a comprehensive technology stack for we know how to efficiently combine legacy and innovation to address your business challenges with the right technology Our software developers know how to adopt and ramp up emerging programming technologies quickly to execute the most ambitious projects and deliver the right results in terms of efficiency performance interoperability and user experience We will guide you through all the technologies and platforms available on the market to find your ideal solution At the same time we always encourage you to share with us all your technology requirements wishes and concerns While our experience and expertise are fully at your service we do believe that only close collaboration with our customers all the way a project goes can bring tangible results A Dedicated Development Center at Itransition is an efficient way to boost your business with topquality resources fully attuned to your requirements and business objectives Your Dedicated Center run by Itransition is literally your doorway to hiend software developers infrastructure and advanced methodologies to ensure scalability and flexibility while maintaining full control and transparency Our software outsourcing services range from technology consulting and business analysis to QA application maintenance and solution integration Our integrated service lines have been shaped by nearly two decades of delivering value to our customers and are built on a deep understanding of business needs and market trends along with the technology expertise and software industry best practices We are fully equipped to deliver firstclass services that result in improved business efficiency increased ROI costeffectiveness risk mitigation for our clients not to speak of transparency and predictability that are guaranteed by default We rely on our timeproven processes tools and techniques to bring the highest level of quality to our growing range of services At the same time we are highly flexible to meet the needs of various customers from startups and SMBs to Fortune 500 companies From advanced Portals and eCommerce solutions to ERP BI we are dedicated to build easytouse solutions no matter how complex they could be either from scratch or as a combination of outofthebox modules for you to reach your business goals the shortest way Accelerated business processes through more efficient utilization of corporate information resources Advanced solutions for customer communication and service supply chain management sales automation and other business Facilitated documentrelated operations document capturing routing life cycle management search etc Heterogeneous content from diverse sources consolidated into a single centrally managed repository with accurate data Rich functionality from finance and human resources management to procurement and order to boost Enterprisewide reporting online analytical data mining benchmarking and business performance management Serviceoriented systems for financial institutions payment service providers and companies with specific industry needs Accelerated business processes − from account management marketing campaigns to sales automation customer service Accelerated business processes through more efficient utilization of corporate information resources Advanced solutions for customer communication and service supply chain management sales automation and other business Facilitated documentrelated operations document capturing routing life cycle management search etc Heterogeneous content from diverse sources consolidated into a single centrally managed repository with accurate data Rich functionality from finance and human resources management to procurement and order to boost Enterprisewide reporting online analytical data mining benchmarking and business performance management Serviceoriented systems for financial institutions payment service providers and companies with specific industry needs Accelerated business processes − from account management marketing campaigns to sales automation customer service “McLaren Software h</v>
       </c>
       <c r="D14" t="str">
-        <v>e and human resources management to procurement and order  to boost  Enterprise-wide reporting, online analytical  data mining, benchmarking and business performance management  Service-oriented systems for financial institutions, payment service providers and companies with specific industry needs Accelerated business processes − from account management &amp; marketing campaigns to sales automation &amp; customer service  Accelerated business processes through more efficient utilization of corporate information resources Advanced solutions for customer communication and service, supply chain management, sales automation and other business  Facilitated document-related operations - document capturing, routing, life cycle management, search, etc Heterogeneous content from diverse sources consolidated into a single centrally managed repository with accurate data  Rich functionality – from finance and human resources management to procurement and order  to boost  Enterprise-wide reporting, online analytical  data mining, benchmarking and business performance management  Service-oriented systems for financial institutions, payment service providers and companies with specific industry needs Accelerated business processes − from account management &amp; marketing campaigns to sales automation &amp; customer service  “McLaren Software has been partnering with Itransition since 2004, previously as part of Sword Group, and currently as an Idox Company. Throughout the long company’s history Itransition stayed a reliable technology partner for us, demonstrating solid expertise in a number of technology stacks, as well as process maturity, including project management, business analysis and customer support. Along with software development, we have extended the use of Itransition into other areas including performance improvement and QA, and this is not the limit.”   Andy Hamlyn, Head of Development, McLaren Software   Jose Brotons  COO Product Madness  Simon Aloyts  CTO Liquid Generation  Dan Zalta  CEO Fee Technology  John Liptak  President UBERbase and Oakwood HowWe Work  Our mission is to help our customers create innovative services and solutions and grow their businesses. For that purpose we provide rich technology competencies, domain expertise, and passion for quality of our software professionals. With more than 1,300 diverse IT professionals on board, we can effectively handle software projects of any scale and complexity.  Read more  Since our inception in 1998, we have been focused on delivering the best while maintaining an open-minded, dynamic, and customer-centric approach. That is why we have succeeded in becoming a one-stop software partner for our global clients ranging from SMBs to Fortune 500 enterprises.   We have been continuously recognized among the world’s best outsourcing providers by independent industry experts in such ratings as The Global Outsourcing 100 by IOAP, The Software 500 by Software Magazine, and others.   Accounts Payable Automation   Flexible and transparent SaaS solution fully automating accounts payable workflow serving hundreds of thousands of payees with millions of bills processed daily.   Corporate Learning Portal   Proactive management of offline trainings and Moodle-based online courses to help the company's tech personnel reduce the learning curve and minimize time to commencing active contribution to the company’s operations.   Mobile Gadget Family   adidas miCoach product family includes gadgets that collect various activity statistics such as speed, number of steps, calories burnt, workout time, distance, and heart rate, along with the web-based backend.   Online Recruitment Platform   SaaS for employers, recruiters and job seekers with full cycle recruiting process support, secure candidate profiles management system, video interviews and online tests modules, and time tracking and reporting.   Partner Portal   For a leading provider of office solutions Itransition delivered a web portal enabling the Customer’s geographically dispersed resellers to harness the functionality of the company’s customer relationship management software.   Network Resource Management   Life:) automates its data-driven operations centered around mobile network resource management with a high scalability web-based solution delivered by Itransition.   Online Patent Handling   Marker tools and evidence templates for evidence discovery, online editing and export of patent infringement reports, integration into a comprehensive patent monetization platform.   Insurance Management Platform   The solution processes heavy volumes of personal financial data related to health insurance, its functionality including full-cycle refunds management.   SaaS for Public Housing   A USA based company automating implementation of Public Housing programs teams up with Itransition for full-cycle development of a set of ASP.NET cloud-based apps united in a single solution.   Archive Migration Solution   Next-gen e-mail archive migration software with versatile platform support and near-zero risk of data loss or tampering for both premium and mid-segment clients.   Satellite Operation Platform   A governmental aerospace organization aimed at developing an interactive e-learning platform which would ensure that the trainees acquire the necessary operational skills while eliminating the risks and costs related to live satellite manipulation.   Digital Marketing Solution   Seeking to expand its market presence, a UK-based company turned to Itransition for co-development, maintenance and support of their core marketing tool - automated social network referral platform allowing companies to promote their products online.   Video Streaming   Itransition delivered an advanced platform allowing security personnel of all-kind organizations to connect to the networks of surveillance cameras installed, view live streaming with zero downtime, record the footage and save the content as video files.   Mobile Order  Solution   Itransition takes over mobile solution architecture optimization and code refactoring to deliver a fully operating system.   Automated KPI Tool   One of the oil &amp; gas industry leaders turned to Itransition with a request of developing a solution for report generation to improve the process of company’s performance analysis.   Network Management System   Reliable and flexible network infrastructure monitoring system with real-time network diagnostics and event notification, unmatched connectivity and comprehensive reports and live monitoring capabilities.   Full IT Services Coverage   Itransition takes over the mobile operator’s software QA, maintenance and functionality development project to help life:) grow subscriber base and remarkably strengthen its positions on the market.   Debt Collection   A leading telecommunications company turns to Itransition with a request to develop an application that would automate  a large amount of subscribers’ debts and payments.   Elastic Quality Assessment   A globally operating company turned to Itransition requesting development of a multi-tenant translation quality assessment solution dynamically adjusting consumed cloud resources to the amount of files processed at any point in time.   ESB for LTE Carrier   A comprehensive ESB solution capable of working with both external and internal systems that utilize multiple communication protocols in a distributed and heterogeneous infrastructure.   Key Document Management   A leading oil &amp; gas company turned to Itransition as a trusted vendor with a request to develop a corporate portal that would help them save up to 900 000$ a year.   Project Control &amp; Assurance   A leading oil &amp; gas company turned to Itransition as a trusted vendor with a request to develop a system that would help automate the process of collaborating on project documentation.   Series of Facebook Games   Scalable, high load-resistant solution able to handle tens of thousands of users simultaneously playing games on Facebook (100m users for one installation, 450,000 active users daily, 2.2 million users monthly, 40,000 requests per minute).   Crowd-Funding Network   Online platform featuring rich social media functionality to enable full-featured crowd-funding: any visitor is welcome to register and create a personal profile, launch a fundraising campaign, or browse projects and pledge to fundraising.   Online Ordering Platform   Online ordering system to control objects like menu items, products, pages, etc., and featuring integration with POS, Kiosk, and payment gateway, support of different locations, extensive reports for all restaurants, etc.   Organic Food Community Portal   Powerful online BI-driven sales and marketing tool, comprehensive suite of community-focused services and solutions, integrated proprietary Quality Assurance system for partner evaluation and relationship mapping.   Expense Management System   Expense management system redevelopment for CarlaBella entailed a sustainable 12-year cooperation regarding Expense Management System technical support and functionality enhancement.   Affiliate Partner Network   The world’s largest online travel company hires Itransition to revamp its global 10,000 private label-strong Affiliate Network to further maintain the market leading position and boost revenues generated by the EAN line of business.   Unlimited Range Baby Monitor   With Evoz baby Monitor parents can listen to their baby anytime, anywhere, right from their iPhone or any web browser. The solution tracks and analyzes real-time data, and lets them learn more about the health and activity of their children.   MORE   View FUll Portfolio  HowWe Work  Our mission is to help our customers create innovative services and solutions and grow their businesses. For that purpose we provide rich technology competencies, domain expertise, and passion for quality of our software professionals. With more than 1,300 diverse IT professionals on board, we can effectively handle software projects of any scale and complexity.  Read more  Since our inception in 1998, we have been focused on delivering the best while maintaining an open-minded, dynamic, and customer-centric approach. That is why we have succeeded in becoming a one-stop software partner for our global clients ranging from SMBs to Fortune 500 enterprises.   We have been continuously recognized among the world’s best outsourcing providers by independent industry experts in such ratings as The Global Outsourcing 100 by IOAP, The Software 500 by Software Magazine, and others.  We proudly announce that according to the 2015 Global Outsourcing 100 research Itransition scored best in the Customer Reference and Company Certification categories. Any business struggles with knowledge accumulation and making it transparent to all employees. Especially this is critical for sales departments in service companies. The choice of the best mobile delivery format is very important for any business nowadays. Which mobile delivery format suits you best? Here is the list of our 10 tips, which may help you build a strong foundation for your business partnership for many years to come. We proudly announce that according to the 2015 Global Outsourcing 100 research Itransition scored best in the Customer Reference and Company Certification categories. Any business struggles with knowledge accumulation and making it transparent to all employees. Especially this is critical for sales departments in service companies. The choice of the best mobile delivery format is very important for any business nowadays. Which mobile delivery format suits you best? Here is the list of our 10 tips, which may help you build a strong foundation for your business partnership for many years to come. Submit your project request (be it a detailed specification or just an idea) using our contact form. We will contact you shortly to clarify your project requirements. We will provide our free non-binding bid or proposal for your review. Submitting Submitted Company Services Solutions Technologies US: 512 501 3620 UK: 161 408 1560 info@itransition.com 1999 — 2016 © Itransition. All rights reserved. here Jump to navigation Services  Technology Consulting Software Prototyping Custom Software Development Software Product Development Enterprise Application Integration Application Security Virtualization Management Software QA and Testing Dedicated Development Centers Customer Service Devops-as-a-Service Solutions B2B and B2C Web Portals Enterprise Extranets and Intranets Document Management Business Intelligence Enterprise Resource Planning Enterprise Content Management Customer Relationship Management Billing and Payments Enterprise Mobility Technologies .NET Java PHP Python Ruby on Rails C/C++ SAP Mobile Portfolio Company About Advantages Awards and Recognition Approach Partnership Executive Blog Corporate News Career Contact Us Itransition Scored Best in the Customer Reference and Company Certification Itransition Enters the World’s Top Java Developers List Multiple Projects in the Services Sector – How to Juggle It All Itransition is 2015 Global Outsourcing 100® company The Three Most Destructive Outsourcing Stereotypes Debunked Gaining Competitive Advantage with Data-Driven Decision Making Some Risks And Challenges Of Outsourcing 10 Ways to Manage Professional Teams Effectively 10 Tips on How to Work With Business Partners Technology Consulting Software Prototyping Custom Software Development Software Product Development Enterprise Application Integration Application Security Virtualization Management Software QA and Testing Maintenance and Support Dedicated Development Centers Enterprise Portals &amp; Intranets B2B and B2C Web Portals Enterprise Content/Document Management Content Management and Distribution Enterprise Resource Planning Business Intelligence Billing and Payments Customer Relationship Management Enterprise Portals &amp; Intranets B2B and B2C Web Portals Enterprise Content/Document Management Content Management and Distribution Enterprise Resource Planning Business Intelligence Billing and Payments Customer Relationship Management .NET PHP C++ JAVA Ruby on Rails Mobile Read More Technology Consulting Software Prototyping Custom Software Development Software Product Development Enterprise Application Integration Application Security Virtualization Management Software QA and Testing Maintenance and Support Dedicated Development Centers Enterprise Portals &amp; Intranets B2B and B2C Web Portals Enterprise Content/Document Management Content Management and Distribution Enterprise Resource Planning Business Intelligence Billing and Payments Customer Relationship Management Enterprise Portals &amp; Intranets B2B and B2C Web Portals Enterprise Content/Document Management Content Management and Distribution Enterprise Resource Planning Business Intelligence Billing and Payments Customer Relationship Management Play ► Read more      Accounts Payable Automation   .NET ISVs Banking &amp; Finance Billing &amp; Payments Collaboration Tools   Flexible and transparent SaaS solution fully automating accounts payable workflow serving hundreds of thousands of payees with millions of bills processed daily.          Corporate Learning Portal   PHP Banking &amp; Finance Portals eLearning &amp; Online Training   Proactive management of offline trainings and Moodle-based online courses to help the company's tech personnel reduce the learning curve and minimize time to commencing active contribution to the company’s operations.          Mobile Gadget Family   C/C++ Manufacturing Mobility   adidas miCoach product family includes gadgets that collect various activity statistics such as speed, number of steps, calories burnt, workout time, distance, and heart rate, along with the web-based backend.          Online Recruitment Platform   Java ISVs Media Content Distribution Business Intelligence   SaaS for employers, recruiters and job seekers with full cycle recruiting process support, secure candidate profiles management system, video interviews and online tests modules, and time tracking and reporting.          Partner Portal   Portals Customer Relationship Management   For a leading provider of office solutions Itransition delivered a web portal enabling the Customer’s geographically dispersed resellers to harness the functionality of the company’s customer relationship management software.          Network Resource Management   .NET Telecom Business Intelligence Enterprise Resource Management   Life:) automates its data-driven operations centered around mobile network resource management with a high scalability web-based solution delivered by Itransition.          Online Patent Handling   Ruby Legal Portals Collaboration Tools   Marker tools and evidence templates for evidence discovery, online editing and export of patent infringement reports, integration into a comprehensive patent monetization platform.          Insurance Management Platform   Java ISVs Banking &amp; Finance Billing &amp; Payments   The solution processes heavy volumes of personal financial data related to health insurance, its functionality including full-cycle refunds management.          SaaS for Public Housing   Public Sector Portals   A USA based company automating implementation of Public Housing programs teams up with Itransition for full-cycle development of a set of ASP.NET cloud-based apps united in a single solution.          Archive Migration Solution   .NET ISVs   Next-gen e-mail archive migration software with versatile platform support and near-zero risk of data loss or tampering for both premium and mid-segment clients.          Satellite Operation Platform   .NET HTML5 eLearning &amp; Online Training   A governmental aerospace organization aimed at developing an interactive e-learning platform which would ensure that the trainees acquire the necessary operational skills while eliminating the risks and costs related to live satellite manipulation.          Digital Marketing Solution   Python Portals Media Content Distribution   Seeking to expand its market presence, a UK-based company turned to Itransition for co-development, maintenance and support of their core marketing tool - automated social network referral platform allowing companies to promote their products online.          Video Streaming   C/C++ Python Portals Media Content Distribution   Itransition delivered an advanced platform allowing security personnel of all-kind organizations to connect to the networks of surveillance cameras installed, view live streaming with zero downtime, record the footage and save the content as video files.          Mobile Order  Solution   Manufacturing Collaboration Tools Mobility Customer Relationship Management   Itransition takes over mobile solution architecture optimization and code refactoring to deliver a fully operating system.          Automated KPI Tool   Oil &amp; Gas Business Intelligence   One of the oil &amp; gas industry leaders turned to Itransition with a request of developing a solution for report generation to improve the process of company’s performance analysis.          Network Management System   PHP Oil &amp; Gas Business Intelligence   Reliable and flexible network infrastructure monitoring system with real-time network diagnostics and event notification, unmatched connectivity and comprehensive reports and live monitoring capabilities.          Full IT Services Coverage   .NET Telecom   Itransition takes over the mobile operator’s software QA, maintenance and functionality development project to help life:) grow subscriber base and remarkably strengthen its positions on the market.          Debt Collection   .NET Telecom Collaboration Tools   A leading telecommunications company turns to Itransition with a request to develop an application that would automate  a large amount of subscribers’ debts and payments.          Elastic Quality Assessment   .NET ISVs Media &amp; Entertainment Business Intelligence   A globally operating company turned to Itransition requesting development of a multi-tenant translation quality assessment solution dynamically adjusting consumed cloud resources to the amount of files processed at any point in time.          ESB for LTE Carrier   Java Telecom   A comprehensive ESB solution capable of working with both external and internal systems that utilize multiple communication protocols in a distributed and heterogeneous infrastructure.          Key Document Management   .NET HTML5 Oil &amp; Gas Portals Collaboration Tools   A leading oil &amp; gas company turned to Itransition as a trusted vendor with a request to develop a corporate portal that would help them save up to 900 000$ a year.          Project Control &amp; Assurance   Portals Collaboration Tools   A leading oil &amp; gas company turned to Itransition as a trusted vendor with a request to develop a system that would help automate the process of collaborating on project documentation.          Series of Facebook Games   Ruby Media Content Distribution Billing &amp; Payments Gaming   Scalable, high load-resistant solution able to handle tens of thousands of users simultaneously playing games on Facebook (100m users for one installation, 450,000 active users daily, 2.2 million users monthly, 40,000 requests per minute).          Crowd-Funding Network   .NET Social Networking Billing &amp; Payments Mobility   Online platform featuring rich social media functionality to enable full-featured crowd-funding: any visitor is welcome to register and create a personal profile, launch a fundraising campaign, or browse projects and pledge to fundraising.          Online Ordering Platform   .NET ISVs eCommerce   Online ordering system to control objects like menu items, products, pages, etc., and featuring integration with POS, Kiosk, and payment gateway, support of different locations, extensive reports for all restaurants, etc.          Organic Food Community Portal   eCommerce Social Networking Business Intelligence   Powerful online BI-driven sales and marketing tool, comprehensive suite of community-focused services and solutions, integrated proprietary Quality Assurance system for partner evaluation and relationship mapping.          Expense Management System   Java Banking &amp; Finance Enterprise Resource Management   Expense management system redevelopment for CarlaBella entailed a sustainable 12-year cooperation regarding Expense Management System technical support and functionality enhancement.          Affiliate Partner Network   Java HTML5 Travel &amp; Hospitality Portals   The world’s largest online travel company hires Itransition to revamp its global 10,000 private label-strong Affiliate Network to further maintain the market leading position and boost revenues generated by the EAN line of business.          Unlimited Range Baby Monitor   Ruby C/C++ ISVs Manufacturing Retail Portals Media Content Distribution Mobility   With Evoz baby Monitor parents can listen to their baby anytime, anywhere, right from their iPhone or any web browser. The solution tracks and analyzes real-time data, and lets them learn more about the health and activity of their children.     MORE View FUll Portfolio Play ► Read more  2015 IAOP research  We proudly announce that according to the 2015 Global Outsourcing 100 research Itransition scored best in the Customer Reference and Company Certification categories.   Sales Knowledge  Any business struggles with knowledge accumulation and making it transparent to all employees. Especially this is critical for sales departments in service companies.   Choosing the App Format  The choice of the best mobile delivery format is very important for any business nowadays. Which mobile delivery format suits you best?   How to Work With Partners  Here is the list of our 10 tips, which may help you build a strong foundation for your business partnership for many years to come.  John Henderson  2015 IAOP research  We proudly announce that according to the 2015 Global Outsourcing 100 research Itransition scored best in the Customer Reference and Company Certification categories.   Sales Knowledge  Any business struggles with knowledge accumulation and making it transparent to all employees. Especially this is critical for sales departments in service companies.   Choosing the App Format  The choice of the best mobile delivery format is very important for any business nowadays. Which mobile delivery format suits you best?   How to Work With Partners  Here is the list of our 10 tips, which may help you build a strong foundation for your business partnership for many years to come.  John Henderson  1 Contact Submit your project request (be it a detailed specification or just an idea) using our contact form.  About Advantages Awards &amp; Recognition Approach Partnership Executive Blog Corporate News Career Technology Consulting  Software Prototyping Custom Software Development  Software Product Development  Enterprise Application Integration Application Security Virtualization Management Software QA and Testing  Dedicated Development Centers Customer Service Devops-as-a-Service B2B and B2C Web Portals  Enterprise Extranets and Intranets  Document Management  Business Intelligence  Enterprise Resource Planning  Enterprise Content Management Customer Relationship Management Billing and Payments Enterprise Mobility .NET Java PHP Python Ruby on Rails C/C++ SAP Mobile info@itransition.com Privacy Policy           News News Blog News Blog Blog Blog Blog Blog  Andy Hamlyn Jose Brotons Simon Aloyts Dan Zalta John Liptak ► ► 1 Means mandatory field US: UK:</v>
-      </c>
-      <c r="E14" t="str">
-        <v>e and human resources management to procurement and order  to boost  Enterprise-wide reporting, online analytical  data mining, benchmarking and business performance management  Service-oriented systems for financial institutions, payment service providers and companies with specific industry needs Accelerated business processes − from account management &amp; marketing campaigns to sales automation &amp; customer service  Accelerated business processes through more efficient utilization of corporate information resources Advanced solutions for customer communication and service, supply chain management, sales automation and other business  Facilitated document-related operations - document capturing, routing, life cycle management, search, etc Heterogeneous content from diverse sources consolidated into a single centrally managed repository with accurate data  Rich functionality – from finance and human resources management to procurement and order  to boost  Enterprise-wide reporting, online analytical  data mining, benchmarking and business performance management  Service-oriented systems for financial institutions, payment service providers and companies with specific industry needs Accelerated business processes − from account management &amp; marketing campaigns to sales automation &amp; customer service  “McLaren Software has been partnering with Itransition since 2004, previously as part of Sword Group, and currently as an Idox Company. Throughout the long company’s history Itransition stayed a reliable technology partner for us, demonstrating solid expertise in a number of technology stacks, as well as process maturity, including project management, business analysis and customer support. Along with software development, we have extended the use of Itransition into other areas including performance improvement and QA, and this is not the limit.”   Andy Hamlyn, Head of Development, McLaren Software   Jose Brotons  COO Product Madness  Simon Aloyts  CTO Liquid Generation  Dan Zalta  CEO Fee Technology  John Liptak  President UBERbase and Oakwood HowWe Work  Our mission is to help our customers create innovative services and solutions and grow their businesses. For that purpose we provide rich technology competencies, domain expertise, and passion for quality of our software professionals. With more than 1,300 diverse IT professionals on board, we can effectively handle software projects of any scale and complexity.  Read more  Since our inception in 1998, we have been focused on delivering the best while maintaining an open-minded, dynamic, and customer-centric approach. That is why we have succeeded in becoming a one-stop software partner for our global clients ranging from SMBs to Fortune 500 enterprises.   We have been continuously recognized among the world’s best outsourcing providers by independent industry experts in such ratings as The Global Outsourcing 100 by IOAP, The Software 500 by Software Magazine, and others.   Accounts Payable Automation   Flexible and transparent SaaS solution fully automating accounts payable workflow serving hundreds of thousands of payees with millions of bills processed daily.   Corporate Learning Portal   Proactive management of offline trainings and Moodle-based online courses to help the company's tech personnel reduce the learning curve and minimize time to commencing active contribution to the company’s operations.   Mobile Gadget Family   adidas miCoach product family includes gadgets that collect various activity statistics such as speed, number of steps, calories burnt, workout time, distance, and heart rate, along with the web-based backend.   Online Recruitment Platform   SaaS for employers, recruiters and job seekers with full cycle recruiting process support, secure candidate profiles management system, video interviews and online tests modules, and time tracking and reporting.   Partner Portal   For a leading provider of office solutions Itransition delivered a web portal enabling the Customer’s geographically dispersed resellers to harness the functionality of the company’s customer relationship management software.   Network Resource Management   Life:) automates its data-driven operations centered around mobile network resource management with a high scalability web-based solution delivered by Itransition.   Online Patent Handling   Marker tools and evidence templates for evidence discovery, online editing and export of patent infringement reports, integration into a comprehensive patent monetization platform.   Insurance Management Platform   The solution processes heavy volumes of personal financial data related to health insurance, its functionality including full-cycle refunds management.   SaaS for Public Housing   A USA based company automating implementation of Public Housing programs teams up with Itransition for full-cycle development of a set of ASP.NET cloud-based apps united in a single solution.   Archive Migration Solution   Next-gen e-mail archive migration software with versatile platform support and near-zero risk of data loss or tampering for both premium and mid-segment clients.   Satellite Operation Platform   A governmental aerospace organization aimed at developing an interactive e-learning platform which would ensure that the trainees acquire the necessary operational skills while eliminating the risks and costs related to live satellite manipulation.   Digital Marketing Solution   Seeking to expand its market presence, a UK-based company turned to Itransition for co-development, maintenance and support of their core marketing tool - automated social network referral platform allowing companies to promote their products online.   Video Streaming   Itransition delivered an advanced platform allowing security personnel of all-kind organizations to connect to the networks of surveillance cameras installed, view live streaming with zero downtime, record the footage and save the content as video files.   Mobile Order  Solution   Itransition takes over mobile solution architecture optimization and code refactoring to deliver a fully operating system.   Automated KPI Tool   One of the oil &amp; gas industry leaders turned to Itransition with a request of developing a solution for report generation to improve the process of company’s performance analysis.   Network Management System   Reliable and flexible network infrastructure monitoring system with real-time network diagnostics and event notification, unmatched connectivity and comprehensive reports and live monitoring capabilities.   Full IT Services Coverage   Itransition takes over the mobile operator’s software QA, maintenance and functionality development project to help life:) grow subscriber base and remarkably strengthen its positions on the market.   Debt Collection   A leading telecommunications company turns to Itransition with a request to develop an application that would automate  a large amount of subscribers’ debts and payments.   Elastic Quality Assessment   A globally operating company turned to Itransition requesting development of a multi-tenant translation quality assessment solution dynamically adjusting consumed cloud resources to the amount of files processed at any point in time.   ESB for LTE Carrier   A comprehensive ESB solution capable of working with both external and internal systems that utilize multiple communication protocols in a distributed and heterogeneous infrastructure.   Key Document Management   A leading oil &amp; gas company turned to Itransition as a trusted vendor with a request to develop a corporate portal that would help them save up to 900 000$ a year.   Project Control &amp; Assurance   A leading oil &amp; gas company turned to Itransition as a trusted vendor with a request to develop a system that would help automate the process of collaborating on project documentation.   Series of Facebook Games   Scalable, high load-resistant solution able to handle tens of thousands of users simultaneously playing games on Facebook (100m users for one installation, 450,000 active users daily, 2.2 million users monthly, 40,000 requests per minute).   Crowd-Funding Network   Online platform featuring rich social media functionality to enable full-featured crowd-funding: any visitor is welcome to register and create a personal profile, launch a fundraising campaign, or browse projects and pledge to fundraising.   Online Ordering Platform   Online ordering system to control objects like menu items, products, pages, etc., and featuring integration with POS, Kiosk, and payment gateway, support of different locations, extensive reports for all restaurants, etc.   Organic Food Community Portal   Powerful online BI-driven sales and marketing tool, comprehensive suite of community-focused services and solutions, integrated proprietary Quality Assurance system for partner evaluation and relationship mapping.   Expense Management System   Expense management system redevelopment for CarlaBella entailed a sustainable 12-year cooperation regarding Expense Management System technical support and functionality enhancement.   Affiliate Partner Network   The world’s largest online travel company hires Itransition to revamp its global 10,000 private label-strong Affiliate Network to further maintain the market leading position and boost revenues generated by the EAN line of business.   Unlimited Range Baby Monitor   With Evoz baby Monitor parents can listen to their baby anytime, anywhere, right from their iPhone or any web browser. The solution tracks and analyzes real-time data, and lets them learn more about the health and activity of their children.   MORE   View FUll Portfolio  HowWe Work  Our mission is to help our customers create innovative services and solutions and grow their businesses. For that purpose we provide rich technology competencies, domain expertise, and passion for quality of our software professionals. With more than 1,300 diverse IT professionals on board, we can effectively handle software projects of any scale and complexity.  Read more  Since our inception in 1998, we have been focused on delivering the best while maintaining an open-minded, dynamic, and customer-centric approach. That is why we have succeeded in becoming a one-stop software partner for our global clients ranging from SMBs to Fortune 500 enterprises.   We have been continuously recognized among the world’s best outsourcing providers by independent industry experts in such ratings as The Global Outsourcing 100 by IOAP, The Software 500 by Software Magazine, and others.  We proudly announce that according to the 2015 Global Outsourcing 100 research Itransition scored best in the Customer Reference and Company Certification categories. Any business struggles with knowledge accumulation and making it transparent to all employees. Especially this is critical for sales departments in service companies. The choice of the best mobile delivery format is very important for any business nowadays. Which mobile delivery format suits you best? Here is the list of our 10 tips, which may help you build a strong foundation for your business partnership for many years to come. We proudly announce that according to the 2015 Global Outsourcing 100 research Itransition scored best in the Customer Reference and Company Certification categories. Any business struggles with knowledge accumulation and making it transparent to all employees. Especially this is critical for sales departments in service companies. The choice of the best mobile delivery format is very important for any business nowadays. Which mobile delivery format suits you best? Here is the list of our 10 tips, which may help you build a strong foundation for your business partnership for many years to come. Submit your project request (be it a detailed specification or just an idea) using our contact form. We will contact you shortly to clarify your project requirements. We will provide our free non-binding bid or proposal for your review. Submitting Submitted Company Services Solutions Technologies US: 512 501 3620 UK: 161 408 1560 info@itransition.com 1999 — 2016 © Itransition. All rights reserved. here Jump to navigation Services  Technology Consulting Software Prototyping Custom Software Development Software Product Development Enterprise Application Integration Application Security Virtualization Management Software QA and Testing Dedicated Development Centers Customer Service Devops-as-a-Service Solutions B2B and B2C Web Portals Enterprise Extranets and Intranets Document Management Business Intelligence Enterprise Resource Planning Enterprise Content Management Customer Relationship Management Billing and Payments Enterprise Mobility Technologies .NET Java PHP Python Ruby on Rails C/C++ SAP Mobile Portfolio Company About Advantages Awards and Recognition Approach Partnership Executive Blog Corporate News Career Contact Us Itransition Scored Best in the Customer Reference and Company Certification Itransition Enters the World’s Top Java Developers List Multiple Projects in the Services Sector – How to Juggle It All Itransition is 2015 Global Outsourcing 100® company The Three Most Destructive Outsourcing Stereotypes Debunked Gaining Competitive Advantage with Data-Driven Decision Making Some Risks And Challenges Of Outsourcing 10 Ways to Manage Professional Teams Effectively 10 Tips on How to Work With Business Partners Technology Consulting Software Prototyping Custom Software Development Software Product Development Enterprise Application Integration Application Security Virtualization Management Software QA and Testing Maintenance and Support Dedicated Development Centers Enterprise Portals &amp; Intranets B2B and B2C Web Portals Enterprise Content/Document Management Content Management and Distribution Enterprise Resource Planning Business Intelligence Billing and Payments Customer Relationship Management Enterprise Portals &amp; Intranets B2B and B2C Web Portals Enterprise Content/Document Management Content Management and Distribution Enterprise Resource Planning Business Intelligence Billing and Payments Customer Relationship Management .NET PHP C++ JAVA Ruby on Rails Mobile Read More Technology Consulting Software Prototyping Custom Software Development Software Product Development Enterprise Application Integration Application Security Virtualization Management Software QA and Testing Maintenance and Support Dedicated Development Centers Enterprise Portals &amp; Intranets B2B and B2C Web Portals Enterprise Content/Document Management Content Management and Distribution Enterprise Resource Planning Business Intelligence Billing and Payments Customer Relationship Management Enterprise Portals &amp; Intranets B2B and B2C Web Portals Enterprise Content/Document Management Content Management and Distribution Enterprise Resource Planning Business Intelligence Billing and Payments Customer Relationship Management Play ► Read more      Accounts Payable Automation   .NET ISVs Banking &amp; Finance Billing &amp; Payments Collaboration Tools   Flexible and transparent SaaS solution fully automating accounts payable workflow serving hundreds of thousands of payees with millions of bills processed daily.          Corporate Learning Portal   PHP Banking &amp; Finance Portals eLearning &amp; Online Training   Proactive management of offline trainings and Moodle-based online courses to help the company's tech personnel reduce the learning curve and minimize time to commencing active contribution to the company’s operations.          Mobile Gadget Family   C/C++ Manufacturing Mobility   adidas miCoach product family includes gadgets that collect various activity statistics such as speed, number of steps, calories burnt, workout time, distance, and heart rate, along with the web-based backend.          Online Recruitment Platform   Java ISVs Media Content Distribution Business Intelligence   SaaS for employers, recruiters and job seekers with full cycle recruiting process support, secure candidate profiles management system, video interviews and online tests modules, and time tracking and reporting.          Partner Portal   Portals Customer Relationship Management   For a leading provider of office solutions Itransition delivered a web portal enabling the Customer’s geographically dispersed resellers to harness the functionality of the company’s customer relationship management software.          Network Resource Management   .NET Telecom Business Intelligence Enterprise Resource Management   Life:) automates its data-driven operations centered around mobile network resource management with a high scalability web-based solution delivered by Itransition.          Online Patent Handling   Ruby Legal Portals Collaboration Tools   Marker tools and evidence templates for evidence discovery, online editing and export of patent infringement reports, integration into a comprehensive patent monetization platform.          Insurance Management Platform   Java ISVs Banking &amp; Finance Billing &amp; Payments   The solution processes heavy volumes of personal financial data related to health insurance, its functionality including full-cycle refunds management.          SaaS for Public Housing   Public Sector Portals   A USA based company automating implementation of Public Housing programs teams up with Itransition for full-cycle development of a set of ASP.NET cloud-based apps united in a single solution.          Archive Migration Solution   .NET ISVs   Next-gen e-mail archive migration software with versatile platform support and near-zero risk of data loss or tampering for both premium and mid-segment clients.          Satellite Operation Platform   .NET HTML5 eLearning &amp; Online Training   A governmental aerospace organization aimed at developing an interactive e-learning platform which would ensure that the trainees acquire the necessary operational skills while eliminating the risks and costs related to live satellite manipulation.          Digital Marketing Solution   Python Portals Media Content Distribution   Seeking to expand its market presence, a UK-based company turned to Itransition for co-development, maintenance and support of their core marketing tool - automated social network referral platform allowing companies to promote their products online.          Video Streaming   C/C++ Python Portals Media Content Distribution   Itransition delivered an advanced platform allowing security personnel of all-kind organizations to connect to the networks of surveillance cameras installed, view live streaming with zero downtime, record the footage and save the content as video files.          Mobile Order  Solution   Manufacturing Collaboration Tools Mobility Customer Relationship Management   Itransition takes over mobile solution architecture optimization and code refactoring to deliver a fully operating system.          Automated KPI Tool   Oil &amp; Gas Business Intelligence   One of the oil &amp; gas industry leaders turned to Itransition with a request of developing a solution for report generation to improve the process of company’s performance analysis.          Network Management System   PHP Oil &amp; Gas Business Intelligence   Reliable and flexible network infrastructure monitoring system with real-time network diagnostics and event notification, unmatched connectivity and comprehensive reports and live monitoring capabilities.          Full IT Services Coverage   .NET Telecom   Itransition takes over the mobile operator’s software QA, maintenance and functionality development project to help life:) grow subscriber base and remarkably strengthen its positions on the market.          Debt Collection   .NET Telecom Collaboration Tools   A leading telecommunications company turns to Itransition with a request to develop an application that would automate  a large amount of subscribers’ debts and payments.          Elastic Quality Assessment   .NET ISVs Media &amp; Entertainment Business Intelligence   A globally operating company turned to Itransition requesting development of a multi-tenant translation quality assessment solution dynamically adjusting consumed cloud resources to the amount of files processed at any point in time.          ESB for LTE Carrier   Java Telecom   A comprehensive ESB solution capable of working with both external and internal systems that utilize multiple communication protocols in a distributed and heterogeneous infrastructure.          Key Document Management   .NET HTML5 Oil &amp; Gas Portals Collaboration Tools   A leading oil &amp; gas company turned to Itransition as a trusted vendor with a request to develop a corporate portal that would help them save up to 900 000$ a year.          Project Control &amp; Assurance   Portals Collaboration Tools   A leading oil &amp; gas company turned to Itransition as a trusted vendor with a request to develop a system that would help automate the process of collaborating on project documentation.          Series of Facebook Games   Ruby Media Content Distribution Billing &amp; Payments Gaming   Scalable, high load-resistant solution able to handle tens of thousands of users simultaneously playing games on Facebook (100m users for one installation, 450,000 active users daily, 2.2 million users monthly, 40,000 requests per minute).          Crowd-Funding Network   .NET Social Networking Billing &amp; Payments Mobility   Online platform featuring rich social media functionality to enable full-featured crowd-funding: any visitor is welcome to register and create a personal profile, launch a fundraising campaign, or browse projects and pledge to fundraising.          Online Ordering Platform   .NET ISVs eCommerce   Online ordering system to control objects like menu items, products, pages, etc., and featuring integration with POS, Kiosk, and payment gateway, support of different locations, extensive reports for all restaurants, etc.          Organic Food Community Portal   eCommerce Social Networking Business Intelligence   Powerful online BI-driven sales and marketing tool, comprehensive suite of community-focused services and solutions, integrated proprietary Quality Assurance system for partner evaluation and relationship mapping.          Expense Management System   Java Banking &amp; Finance Enterprise Resource Management   Expense management system redevelopment for CarlaBella entailed a sustainable 12-year cooperation regarding Expense Management System technical support and functionality enhancement.          Affiliate Partner Network   Java HTML5 Travel &amp; Hospitality Portals   The world’s largest online travel company hires Itransition to revamp its global 10,000 private label-strong Affiliate Network to further maintain the market leading position and boost revenues generated by the EAN line of business.          Unlimited Range Baby Monitor   Ruby C/C++ ISVs Manufacturing Retail Portals Media Content Distribution Mobility   With Evoz baby Monitor parents can listen to their baby anytime, anywhere, right from their iPhone or any web browser. The solution tracks and analyzes real-time data, and lets them learn more about the health and activity of their children.     MORE View FUll Portfolio Play ► Read more  2015 IAOP research  We proudly announce that according to the 2015 Global Outsourcing 100 research Itransition scored best in the Customer Reference and Company Certification categories.   Sales Knowledge  Any business struggles with knowledge accumulation and making it transparent to all employees. Especially this is critical for sales departments in service companies.   Choosing the App Format  The choice of the best mobile delivery format is very important for any business nowadays. Which mobile delivery format suits you best?   How to Work With Partners  Here is the list of our 10 tips, which may help you build a strong foundation for your business partnership for many years to come.  John Henderson  2015 IAOP research  We proudly announce that according to the 2015 Global Outsourcing 100 research Itransition scored best in the Customer Reference and Company Certification categories.   Sales Knowledge  Any business struggles with knowledge accumulation and making it transparent to all employees. Especially this is critical for sales departments in service companies.   Choosing the App Format  The choice of the best mobile delivery format is very important for any business nowadays. Which mobile delivery format suits you best?   How to Work With Partners  Here is the list of our 10 tips, which may help you build a strong foundation for your business partnership for many years to come.  John Henderson  1 Contact Submit your project request (be it a detailed specification or just an idea) using our contact form.  About Advantages Awards &amp; Recognition Approach Partnership Executive Blog Corporate News Career Technology Consulting  Software Prototyping Custom Software Development  Software Product Development  Enterprise Application Integration Application Security Virtualization Management Software QA and Testing  Dedicated Development Centers Customer Service Devops-as-a-Service B2B and B2C Web Portals  Enterprise Extranets and Intranets  Document Management  Business Intelligence  Enterprise Resource Planning  Enterprise Content Management Customer Relationship Management Billing and Payments Enterprise Mobility .NET Java PHP Python Ruby on Rails C/C++ SAP Mobile info@itransition.com Privacy Policy           News News Blog News Blog Blog Blog Blog Blog  Andy Hamlyn Jose Brotons Simon Aloyts Dan Zalta John Liptak ► ► 1 Means mandatory field US: UK:</v>
-      </c>
-      <c r="F14" t="str">
-        <v>e and human resources management to procurement and order  to boost  Enterprise-wide reporting, online analytical  data mining, benchmarking and business performance management  Service-oriented systems for financial institutions, payment service providers and companies with specific industry needs Accelerated business processes − from account management &amp; marketing campaigns to sales automation &amp; customer service  Accelerated business processes through more efficient utilization of corporate information resources Advanced solutions for customer communication and service, supply chain management, sales automation and other business  Facilitated document-related operations - document capturing, routing, life cycle management, search, etc Heterogeneous content from diverse sources consolidated into a single centrally managed repository with accurate data  Rich functionality – from finance and human resources management to procurement and order  to boost  Enterprise-wide reporting, online analytical  data mining, benchmarking and business performance management  Service-oriented systems for financial institutions, payment service providers and companies with specific industry needs Accelerated business processes − from account management &amp; marketing campaigns to sales automation &amp; customer service  “McLaren Software has been partnering with Itransition since 2004, previously as part of Sword Group, and currently as an Idox Company. Throughout the long company’s history Itransition stayed a reliable technology partner for us, demonstrating solid expertise in a number of technology stacks, as well as process maturity, including project management, business analysis and customer support. Along with software development, we have extended the use of Itransition into other areas including performance improvement and QA, and this is not the limit.”   Andy Hamlyn, Head of Development, McLaren Software   Jose Brotons  COO Product Madness  Simon Aloyts  CTO Liquid Generation  Dan Zalta  CEO Fee Technology  John Liptak  President UBERbase and Oakwood HowWe Work  Our mission is to help our customers create innovative services and solutions and grow their businesses. For that purpose we provide rich technology competencies, domain expertise, and passion for quality of our software professionals. With more than 1,300 diverse IT professionals on board, we can effectively handle software projects of any scale and complexity.  Read more  Since our inception in 1998, we have been focused on delivering the best while maintaining an open-minded, dynamic, and customer-centric approach. That is why we have succeeded in becoming a one-stop software partner for our global clients ranging from SMBs to Fortune 500 enterprises.   We have been continuously recognized among the world’s best outsourcing providers by independent industry experts in such ratings as The Global Outsourcing 100 by IOAP, The Software 500 by Software Magazine, and others.   Accounts Payable Automation   Flexible and transparent SaaS solution fully automating accounts payable workflow serving hundreds of thousands of payees with millions of bills processed daily.   Corporate Learning Portal   Proactive management of offline trainings and Moodle-based online courses to help the company's tech personnel reduce the learning curve and minimize time to commencing active contribution to the company’s operations.   Mobile Gadget Family   adidas miCoach product family includes gadgets that collect various activity statistics such as speed, number of steps, calories burnt, workout time, distance, and heart rate, along with the web-based backend.   Online Recruitment Platform   SaaS for employers, recruiters and job seekers with full cycle recruiting process support, secure candidate profiles management system, video interviews and online tests modules, and time tracking and reporting.   Partner Portal   For a leading provider of office solutions Itransition delivered a web portal enabling the Customer’s geographically dispersed resellers to harness the functionality of the company’s customer relationship management software.   Network Resource Management   Life:) automates its data-driven operations centered around mobile network resource management with a high scalability web-based solution delivered by Itransition.   Online Patent Handling   Marker tools and evidence templates for evidence discovery, online editing and export of patent infringement reports, integration into a comprehensive patent monetization platform.   Insurance Management Platform   The solution processes heavy volumes of personal financial data related to health insurance, its functionality including full-cycle refunds management.   SaaS for Public Housing   A USA based company automating implementation of Public Housing programs teams up with Itransition for full-cycle development of a set of ASP.NET cloud-based apps united in a single solution.   Archive Migration Solution   Next-gen e-mail archive migration software with versatile platform support and near-zero risk of data loss or tampering for both premium and mid-segment clients.   Satellite Operation Platform   A governmental aerospace organization aimed at developing an interactive e-learning platform which would ensure that the trainees acquire the necessary operational skills while eliminating the risks and costs related to live satellite manipulation.   Digital Marketing Solution   Seeking to expand its market presence, a UK-based company turned to Itransition for co-development, maintenance and support of their core marketing tool - automated social network referral platform allowing companies to promote their products online.   Video Streaming   Itransition delivered an advanced platform allowing security personnel of all-kind organizations to connect to the networks of surveillance cameras installed, view live streaming with zero downtime, record the footage and save the content as video files.   Mobile Order  Solution   Itransition takes over mobile solution architecture optimization and code refactoring to deliver a fully operating system.   Automated KPI Tool   One of the oil &amp; gas industry leaders turned to Itransition with a request of developing a solution for report generation to improve the process of company’s performance analysis.   Network Management System   Reliable and flexible network infrastructure monitoring system with real-time network diagnostics and event notification, unmatched connectivity and comprehensive reports and live monitoring capabilities.   Full IT Services Coverage   Itransition takes over the mobile operator’s software QA, maintenance and functionality development project to help life:) grow subscriber base and remarkably strengthen its positions on the market.   Debt Collection   A leading telecommunications company turns to Itransition with a request to develop an application that would automate  a large amount of subscribers’ debts and payments.   Elastic Quality Assessment   A globally operating company turned to Itransition requesting development of a multi-tenant translation quality assessment solution dynamically adjusting consumed cloud resources to the amount of files processed at any point in time.   ESB for LTE Carrier   A comprehensive ESB solution capable of working with both external and internal systems that utilize multiple communication protocols in a distributed and heterogeneous infrastructure.   Key Document Management   A leading oil &amp; gas company turned to Itransition as a trusted vendor with a request to develop a corporate portal that would help them save up to 900 000$ a year.   Project Control &amp; Assurance   A leading oil &amp; gas company turned to Itransition as a trusted vendor with a request to develop a system that would help automate the process of collaborating on project documentation.   Series of Facebook Games   Scalable, high load-resistant solution able to handle tens of thousands of users simultaneously playing games on Facebook (100m users for one installation, 450,000 active users daily, 2.2 million users monthly, 40,000 requests per minute).   Crowd-Funding Network   Online platform featuring rich social media functionality to enable full-featured crowd-funding: any visitor is welcome to register and create a personal profile, launch a fundraising campaign, or browse projects and pledge to fundraising.   Online Ordering Platform   Online ordering system to control objects like menu items, products, pages, etc., and featuring integration with POS, Kiosk, and payment gateway, support of different locations, extensive reports for all restaurants, etc.   Organic Food Community Portal   Powerful online BI-driven sales and marketing tool, comprehensive suite of community-focused services and solutions, integrated proprietary Quality Assurance system for partner evaluation and relationship mapping.   Expense Management System   Expense management system redevelopment for CarlaBella entailed a sustainable 12-year cooperation regarding Expense Management System technical support and functionality enhancement.   Affiliate Partner Network   The world’s largest online travel company hires Itransition to revamp its global 10,000 private label-strong Affiliate Network to further maintain the market leading position and boost revenues generated by the EAN line of business.   Unlimited Range Baby Monitor   With Evoz baby Monitor parents can listen to their baby anytime, anywhere, right from their iPhone or any web browser. The solution tracks and analyzes real-time data, and lets them learn more about the health and activity of their children.   MORE   View FUll Portfolio  HowWe Work  Our mission is to help our customers create innovative services and solutions and grow their businesses. For that purpose we provide rich technology competencies, domain expertise, and passion for quality of our software professionals. With more than 1,300 diverse IT professionals on board, we can effectively handle software projects of any scale and complexity.  Read more  Since our inception in 1998, we have been focused on delivering the best while maintaining an open-minded, dynamic, and customer-centric approach. That is why we have succeeded in becoming a one-stop software partner for our global clients ranging from SMBs to Fortune 500 enterprises.   We have been continuously recognized among the world’s best outsourcing providers by independent industry experts in such ratings as The Global Outsourcing 100 by IOAP, The Software 500 by Software Magazine, and others.  We proudly announce that according to the 2015 Global Outsourcing 100 research Itransition scored best in the Customer Reference and Company Certification categories. Any business struggles with knowledge accumulation and making it transparent to all employees. Especially this is critical for sales departments in service companies. The choice of the best mobile delivery format is very important for any business nowadays. Which mobile delivery format suits you best? Here is the list of our 10 tips, which may help you build a strong foundation for your business partnership for many years to come. We proudly announce that according to the 2015 Global Outsourcing 100 research Itransition scored best in the Customer Reference and Company Certification categories. Any business struggles with knowledge accumulation and making it transparent to all employees. Especially this is critical for sales departments in service companies. The choice of the best mobile delivery format is very important for any business nowadays. Which mobile delivery format suits you best? Here is the list of our 10 tips, which may help you build a strong foundation for your business partnership for many years to come. Submit your project request (be it a detailed specification or just an idea) using our contact form. We will contact you shortly to clarify your project requirements. We will provide our free non-binding bid or proposal for your review. Submitting Submitted Company Services Solutions Technologies US: 512 501 3620 UK: 161 408 1560 info@itransition.com 1999 — 2016 © Itransition. All rights reserved. here Jump to navigation Services  Technology Consulting Software Prototyping Custom Software Development Software Product Development Enterprise Application Integration Application Security Virtualization Management Software QA and Testing Dedicated Development Centers Customer Service Devops-as-a-Service Solutions B2B and B2C Web Portals Enterprise Extranets and Intranets Document Management Business Intelligence Enterprise Resource Planning Enterprise Content Management Customer Relationship Management Billing and Payments Enterprise Mobility Technologies .NET Java PHP Python Ruby on Rails C/C++ SAP Mobile Portfolio Company About Advantages Awards and Recognition Approach Partnership Executive Blog Corporate News Career Contact Us Itransition Scored Best in the Customer Reference and Company Certification Itransition Enters the World’s Top Java Developers List Multiple Projects in the Services Sector – How to Juggle It All Itransition is 2015 Global Outsourcing 100® company The Three Most Destructive Outsourcing Stereotypes Debunked Gaining Competitive Advantage with Data-Driven Decision Making Some Risks And Challenges Of Outsourcing 10 Ways to Manage Professional Teams Effectively 10 Tips on How to Work With Business Partners Technology Consulting Software Prototyping Custom Software Development Software Product Development Enterprise Application Integration Application Security Virtualization Management Software QA and Testing Maintenance and Support Dedicated Development Centers Enterprise Portals &amp; Intranets B2B and B2C Web Portals Enterprise Content/Document Management Content Management and Distribution Enterprise Resource Planning Business Intelligence Billing and Payments Customer Relationship Management Enterprise Portals &amp; Intranets B2B and B2C Web Portals Enterprise Content/Document Management Content Management and Distribution Enterprise Resource Planning Business Intelligence Billing and Payments Customer Relationship Management .NET PHP C++ JAVA Ruby on Rails Mobile Read More Technology Consulting Software Prototyping Custom Software Development Software Product Development Enterprise Application Integration Application Security Virtualization Management Software QA and Testing Maintenance and Support Dedicated Development Centers Enterprise Portals &amp; Intranets B2B and B2C Web Portals Enterprise Content/Document Management Content Management and Distribution Enterprise Resource Planning Business Intelligence Billing and Payments Customer Relationship Management Enterprise Portals &amp; Intranets B2B and B2C Web Portals Enterprise Content/Document Management Content Management and Distribution Enterprise Resource Planning Business Intelligence Billing and Payments Customer Relationship Management Play ► Read more      Accounts Payable Automation   .NET ISVs Banking &amp; Finance Billing &amp; Payments Collaboration Tools   Flexible and transparent SaaS solution fully automating accounts payable workflow serving hundreds of thousands of payees with millions of bills processed daily.          Corporate Learning Portal   PHP Banking &amp; Finance Portals eLearning &amp; Online Training   Proactive management of offline trainings and Moodle-based online courses to help the company's tech personnel reduce the learning curve and minimize time to commencing active contribution to the company’s operations.          Mobile Gadget Family   C/C++ Manufacturing Mobility   adidas miCoach product family includes gadgets that collect various activity statistics such as speed, number of steps, calories burnt, workout time, distance, and heart rate, along with the web-based backend.          Online Recruitment Platform   Java ISVs Media Content Distribution Business Intelligence   SaaS for employers, recruiters and job seekers with full cycle recruiting process support, secure candidate profiles management system, video interviews and online tests modules, and time tracking and reporting.          Partner Portal   Portals Customer Relationship Management   For a leading provider of office solutions Itransition delivered a web portal enabling the Customer’s geographically dispersed resellers to harness the functionality of the company’s customer relationship management software.          Network Resource Management   .NET Telecom Business Intelligence Enterprise Resource Management   Life:) automates its data-driven operations centered around mobile network resource management with a high scalability web-based solution delivered by Itransition.          Online Patent Handling   Ruby Legal Portals Collaboration Tools   Marker tools and evidence templates for evidence discovery, online editing and export of patent infringement reports, integration into a comprehensive patent monetization platform.          Insurance Management Platform   Java ISVs Banking &amp; Finance Billing &amp; Payments   The solution processes heavy volumes of personal financial data related to health insurance, its functionality including full-cycle refunds management.          SaaS for Public Housing   Public Sector Portals   A USA based company automating implementation of Public Housing programs teams up with Itransition for full-cycle development of a set of ASP.NET cloud-based apps united in a single solution.          Archive Migration Solution   .NET ISVs   Next-gen e-mail archive migration software with versatile platform support and near-zero risk of data loss or tampering for both premium and mid-segment clients.          Satellite Operation Platform   .NET HTML5 eLearning &amp; Online Training   A governmental aerospace organization aimed at developing an interactive e-learning platform which would ensure that the trainees acquire the necessary operational skills while eliminating the risks and costs related to live satellite manipulation.          Digital Marketing Solution   Python Portals Media Content Distribution   Seeking to expand its market presence, a UK-based company turned to Itransition for co-development, maintenance and support of their core marketing tool - automated social network referral platform allowing companies to promote their products online.          Video Streaming   C/C++ Python Portals Media Content Distribution   Itransition delivered an advanced platform allowing security personnel of all-kind organizations to connect to the networks of surveillance cameras installed, view live streaming with zero downtime, record the footage and save the content as video files.          Mobile Order  Solution   Manufacturing Collaboration Tools Mobility Customer Relationship Management   Itransition takes over mobile solution architecture optimization and code refactoring to deliver a fully operating system.          Automated KPI Tool   Oil &amp; Gas Business Intelligence   One of the oil &amp; gas industry leaders turned to Itransition with a request of developing a solution for report generation to improve the process of company’s performance analysis.          Network Management System   PHP Oil &amp; Gas Business Intelligence   Reliable and flexible network infrastructure monitoring system with real-time network diagnostics and event notification, unmatched connectivity and comprehensive reports and live monitoring capabilities.          Full IT Services Coverage   .NET Telecom   Itransition takes over the mobile operator’s software QA, maintenance and functionality development project to help life:) grow subscriber base and remarkably strengthen its positions on the market.          Debt Collection   .NET Telecom Collaboration Tools   A leading telecommunications company turns to Itransition with a request to develop an application that would automate  a large amount of subscribers’ debts and payments.          Elastic Quality Assessment   .NET ISVs Media &amp; Entertainment Business Intelligence   A globally operating company turned to Itransition requesting development of a multi-tenant translation quality assessment solution dynamically adjusting consumed cloud resources to the amount of files processed at any point in time.          ESB for LTE Carrier   Java Telecom   A comprehensive ESB solution capable of working with both external and internal systems that utilize multiple communication protocols in a distributed and heterogeneous infrastructure.          Key Document Management   .NET HTML5 Oil &amp; Gas Portals Collaboration Tools   A leading oil &amp; gas company turned to Itransition as a trusted vendor with a request to develop a corporate portal that would help them save up to 900 000$ a year.          Project Control &amp; Assurance   Portals Collaboration Tools   A leading oil &amp; gas company turned to Itransition as a trusted vendor with a request to develop a system that would help automate the process of collaborating on project documentation.          Series of Facebook Games   Ruby Media Content Distribution Billing &amp; Payments Gaming   Scalable, high load-resistant solution able to handle tens of thousands of users simultaneously playing games on Facebook (100m users for one installation, 450,000 active users daily, 2.2 million users monthly, 40,000 requests per minute).          Crowd-Funding Network   .NET Social Networking Billing &amp; Payments Mobility   Online platform featuring rich social media functionality to enable full-featured crowd-funding: any visitor is welcome to register and create a personal profile, launch a fundraising campaign, or browse projects and pledge to fundraising.          Online Ordering Platform   .NET ISVs eCommerce   Online ordering system to control objects like menu items, products, pages, etc., and featuring integration with POS, Kiosk, and payment gateway, support of different locations, extensive reports for all restaurants, etc.          Organic Food Community Portal   eCommerce Social Networking Business Intelligence   Powerful online BI-driven sales and marketing tool, comprehensive suite of community-focused services and solutions, integrated proprietary Quality Assurance system for partner evaluation and relationship mapping.          Expense Management System   Java Banking &amp; Finance Enterprise Resource Management   Expense management system redevelopment for CarlaBella entailed a sustainable 12-year cooperation regarding Expense Management System technical support and functionality enhancement.          Affiliate Partner Network   Java HTML5 Travel &amp; Hospitality Portals   The world’s largest online travel company hires Itransition to revamp its global 10,000 private label-strong Affiliate Network to further maintain the market leading position and boost revenues generated by the EAN line of business.          Unlimited Range Baby Monitor   Ruby C/C++ ISVs Manufacturing Retail Portals Media Content Distribution Mobility   With Evoz baby Monitor parents can listen to their baby anytime, anywhere, right from their iPhone or any web browser. The solution tracks and analyzes real-time data, and lets them learn more about the health and activity of their children.     MORE View FUll Portfolio Play ► Read more  2015 IAOP research  We proudly announce that according to the 2015 Global Outsourcing 100 research Itransition scored best in the Customer Reference and Company Certification categories.   Sales Knowledge  Any business struggles with knowledge accumulation and making it transparent to all employees. Especially this is critical for sales departments in service companies.   Choosing the App Format  The choice of the best mobile delivery format is very important for any business nowadays. Which mobile delivery format suits you best?   How to Work With Partners  Here is the list of our 10 tips, which may help you build a strong foundation for your business partnership for many years to come.  John Henderson  2015 IAOP research  We proudly announce that according to the 2015 Global Outsourcing 100 research Itransition scored best in the Customer Reference and Company Certification categories.   Sales Knowledge  Any business struggles with knowledge accumulation and making it transparent to all employees. Especially this is critical for sales departments in service companies.   Choosing the App Format  The choice of the best mobile delivery format is very important for any business nowadays. Which mobile delivery format suits you best?   How to Work With Partners  Here is the list of our 10 tips, which may help you build a strong foundation for your business partnership for many years to come.  John Henderson  1 Contact Submit your project request (be it a detailed specification or just an idea) using our contact form.  About Advantages Awards &amp; Recognition Approach Partnership Executive Blog Corporate News Career Technology Consulting  Software Prototyping Custom Software Development  Software Product Development  Enterprise Application Integration Application Security Virtualization Management Software QA and Testing  Dedicated Development Centers Customer Service Devops-as-a-Service B2B and B2C Web Portals  Enterprise Extranets and Intranets  Document Management  Business Intelligence  Enterprise Resource Planning  Enterprise Content Management Customer Relationship Management Billing and Payments Enterprise Mobility .NET Java PHP Python Ruby on Rails C/C++ SAP Mobile info@itransition.com Privacy Policy           News News Blog News Blog Blog Blog Blog Blog  Andy Hamlyn Jose Brotons Simon Aloyts Dan Zalta John Liptak ► ► 1 Means mandatory field US: UK:</v>
+        <v>as been partnering with Itransition since 2004 previously as part of Sword Group and currently as an Idox Company Throughout the long company’s history Itransition stayed a reliable technology partner for us demonstrating solid expertise in a number of technology stacks as well as process maturity including project management business analysis and customer support Along with software development we have extended the use of Itransition into other areas including performance improvement and QA and this is not the limit” Andy Hamlyn Head of Development McLaren Software Jose Brotons COO Product Madness Simon Aloyts CTO Liquid Generation Dan Zalta CEO Fee Technology John Liptak President UBERbase and Oakwood HowWe Work Our mission is to help our customers create innovative services and solutions and grow their businesses For that purpose we provide rich technology competencies domain expertise and passion for quality of our software professionals With more than 1300 diverse IT professionals on board we can effectively handle software projects of any scale and complexity Read more Since our inception in 1998 we have been focused on delivering the best while maintaining an openminded dynamic and customercentric approach That is why we have succeeded in becoming a onestop software partner for our global clients ranging from SMBs to Fortune 500 enterprises We have been continuously recognized among the world’s best outsourcing providers by independent industry experts in such ratings as The Global Outsourcing 100 by IOAP The Software 500 by Software Magazine and others Accounts Payable Automation Flexible and transparent SaaS solution fully automating accounts payable workflow serving hundreds of thousands of payees with millions of bills processed daily Corporate Learning Portal Proactive management of offline trainings and Moodlebased online courses to help the companys tech personnel reduce the learning curve and minimize time to commencing active contribution to the company’s operations Mobile Gadget Family adidas miCoach product family includes gadgets that collect various activity statistics such as speed number of steps calories burnt workout time distance and heart rate along with the webbased backend Online Recruitment Platform SaaS for employers recruiters and job seekers with full cycle recruiting process support secure candidate profiles management system video interviews and online tests modules and time tracking and reporting Partner Portal For a leading provider of office solutions Itransition delivered a web portal enabling the Customer’s geographically dispersed resellers to harness the functionality of the company’s customer relationship management software Network Resource Management Life automates its datadriven operations centered around mobile network resource management with a high scalability webbased solution delivered by Itransition Online Patent Handling Marker tools and evidence templates for evidence discovery online editing and export of patent infringement reports integration into a comprehensive patent monetization platform Insurance Management Platform The solution processes heavy volumes of personal financial data related to health insurance its functionality including fullcycle refunds management SaaS for Public Housing A USA based company automating implementation of Public Housing programs teams up with Itransition for fullcycle development of a set of ASPNET cloudbased apps united in a single solution Archive Migration Solution Nextgen email archive migration software with versatile platform support and nearzero risk of data loss or tampering for both premium and midsegment clients Satellite Operation Platform A governmental aerospace organization aimed at developing an interactive elearning platform which would ensure that the trainees acquire the necessary operational skills while eliminating the risks and costs related to live satellite manipulation Digital Marketing Solution Seeking to expand its market presence a UKbased company turned to Itransition for codevelopment maintenance and support of their core marketing tool automated social network referral platform allowing companies to promote their products online Video Streaming Itransition delivered an advanced platform allowing security personnel of allkind organizations to connect to the networks of surveillance cameras installed view live streaming with zero downtime record the footage and save the content as video files Mobile Order Solution Itransition takes over mobile solution architecture optimization and code refactoring to deliver a fully operating system Automated KPI Tool One of the oil gas industry leaders turned to Itransition with a request of developing a solution for report generation to improve the process of company’s performance analysis Network Management System Reliable and flexible network infrastructure monitoring system with realtime network diagnostics and event notification unmatched connectivity and comprehensive reports and live monitoring capabilities Full IT Services Coverage Itransition takes over the mobile operator’s software QA maintenance and functionality development project to help life grow subscriber base and remarkably strengthen its positions on the market Debt Collection A leading telecommunications company turns to Itransition with a request to develop an application that would automate a large amount of subscribers’ debts and payments Elastic Quality Assessment A globally operating company turned to Itransition requesting development of a multitenant translation quality assessment solution dynamically adjusting consumed cloud resources to the amount of files processed at any point in time ESB for LTE Carrier A comprehensive ESB solution capable of working with both external and internal systems that utilize multiple communication protocols in a distributed and heterogeneous infrastructure Key Document Management A leading oil gas company turned to Itransition as a trusted vendor with a request to develop a corporate portal that would help them save up to 900 000 a year Project Control Assurance A leading oil gas company turned to Itransition as a trusted vendor with a request to develop a system that would help automate the process of collaborating on project documentation Series of Facebook Games Scalable high loadresistant solution able to handle tens of thousands of users simultaneously playing games on Facebook 100m users for one installation 450000 active users daily 22 million users monthly 40000 requests per minute CrowdFunding Network Online platform featuring rich social media functionality to enable fullfeatured crowdfunding any visitor is welcome to register and create a personal profile launch a fundraising campaign or browse projects and pledge to fundraising Online Ordering Platform Online ordering system to control objects like menu items products pages etc and featuring integration with POS Kiosk and payment gateway support of different locations extensive reports for all restaurants etc Organic Food Community Portal Powerful online BIdriven sales and marketing tool comprehensive suite of communityfocused services and solutions integrated proprietary Quality Assurance system for partner evaluation and relationship mapping Expense Management System Expense management system redevelopment for CarlaBella entailed a sustainable 12year cooperation regarding Expense Management System technical support and functionality enhancement Affiliate Partner Network The world’s largest online travel company hires Itransition to revamp its global 10000 private labelstrong Affiliate Network to further maintain the market leading position and boost revenues generated by the EAN line of business Unlimited Range Baby Monitor With Evoz baby Monitor parents can listen to their baby anytime anywhere right from their iPhone or any web browser The solution tracks and analyzes realtime data and lets them learn more about the health and activity of their children MORE View FUll Portfolio HowWe Work Our mission is to help our customers create innovative services and solutions and grow their businesses For that purpose we provide rich technology competencies domain expertise and passion for quality of our software professionals With more than 1300 diverse IT professionals on board we can effectively handle software projects of any scale and complexity Read more Since our inception in 1998 we have been focused on delivering the best while maintaining an openminded dynamic and customercentric approach That is why we have succeeded in becoming a onestop software partner for our global clients ranging from SMBs to Fortune 500 enterprises We have been continuously recognized among the world’s best outsourcing providers by independent industry experts in such ratings as The Global Outsourcing 100 by IOAP The Software 500 by Software Magazine and others We proudly announce that according to the 2015 Global Outsourcing 100 research Itransition scored best in the Customer Reference and Company Certification categories Any business struggles with knowledge accumulation and making it transparent to all employees Especially this is critical for sales departments in service companies The choice of the best mobile delivery format is very important for any business nowadays Which mobile delivery format suits you best Here is the list of our 10 tips which may help you build a strong foundation for your business partnership for many years to come We proudly announce that according to the 2015 Global Outsourcing 100 research Itransition scored best in the Customer Reference and Company Certification categories Any business struggles with knowledge accumulation and making it transparent to all employees Especially this is critical for sales departments in service companies The choice of the best mobile delivery format is very important for any business nowadays Which mobile delivery format suits you best Here is the list of our 10 tips which may help you build a strong foundation for your business partnership for many years to come Submit your project request be it a detailed specification or just an idea using our contact form We will contact you shortly to clarify your project requirements We will provide our free nonbinding bid or proposal for your review Submitting Submitted Company Services Solutions Technologies US 512 501 3620 UK 161 408 1560 infoitransitioncom 1999 2016 © Itransition All rights reserved here Jump to navigation Services Technology Consulting Software Prototyping Custom Software Development Software Product Development Enterprise Application Integration Application Security Virtualization Management Software QA and Testing Dedicated Development Centers Customer Service DevopsasaService Solutions B2B and B2C Web Portals Enterprise Extranets and Intranets Document Management Business Intelligence Enterprise Resource Planning Enterprise Content Management Customer Relationship Management Billing and Payments Enterprise Mobility Technologies NET Java PHP Python Ruby on Rails CC SAP Mobile Portfolio Company About Advantages Awards and Recognition Approach Partnership Executive Blog Corporate News Career Contact Us Itransition Scored Best in the Customer Reference and Company Certification Itransition Enters the World’s Top Java Developers List Multiple Projects in the Services Sector How to Juggle It All Itransition is 2015 Global Outsourcing 100® company The Three Most Destructive Outsourcing Stereotypes Debunked Gaining Competitive Advantage with DataDriven Decision Making Some Risks And Challenges Of Outsourcing 10 Ways to Manage Professional Teams Effectively 10 Tips on How to Work With Business Partners Technology Consulting Software Prototyping Custom Software Development Software Product Development Enterprise Application Integration Application Security Virtualization Management Software QA and Testing Maintenance and Support Dedicated Development Centers Enterprise Portals Intranets B2B and B2C Web Portals Enterprise ContentDocument Management Content Management and Distribution Enterprise Resource Planning Business Intelligence Billing and Payments Customer Relationship Management Enterprise Portals Intranets B2B and B2C Web Portals Enterprise ContentDocument Management Content Management and Distribution Enterprise Resource Planning Business Intelligence Billing and Payments Customer Relationship Management NET PHP C JAVA Ruby on Rails Mobile Read More Technology Consulting Software Prototyping Custom Software Development Software Product Development Enterprise Application Integration Application Security Virtualization Management Software QA and Testing Maintenance and Support Dedicated Development Centers Enterprise Portals Intranets B2B and B2C Web Portals Enterprise ContentDocument Management Content Management and Distribution Enterprise Resource Planning Business Intelligence Billing and Payments Customer Relationship Management Enterprise Portals Intranets B2B and B2C Web Portals Enterprise ContentDocument Management Content Management and Distribution Enterprise Resource Planning Business Intelligence Billing and Payments Customer Relationship Management Play ► Read more Accounts Payable Automation NET ISVs Banking Finance Billing Payments Collaboration Tools Flexible and transparent SaaS solution fully automating accounts payable workflow serving hundreds of thousands of payees with millions of bills processed daily Corporate Learning Portal PHP Banking Finance Portals eLearning Online Training Proactive management of offline trainings and Moodlebased online courses to help the companys tech personnel reduce the learning curve and minimize time to commencing active contribution to the company’s operations Mobile Gadget Family CC Manufacturing Mobility adidas miCoach product family includes gadgets that collect various activity statistics such as speed number of steps calories burnt workout time distance and heart rate along with the webbased backend Online Recruitment Platform Java ISVs Media Content Distribution Business Intelligence SaaS for employers recruiters and job seekers with full cycle recruiting process support secure candidate profiles management system video interviews and online tests modules and time tracking and reporting Partner Portal Portals Customer Relationship Management For a leading provider of office solutions Itransition delivered a web portal enabling the Customer’s geographically dispersed resellers to harness the functionality of the company’s customer relationship management software Network Resource Management NET Telecom Business Intelligence Enterprise Resource Management Life automates its datadriven operations centered around mobile network resource management with a high scalability webbased solution delivered by Itransition Online Patent Handling Ruby Legal Portals Collaboration Tools Marker tools and evidence templates for evidence discovery online editing and export of patent infringement reports integration into a comprehensive patent monetization platform Insurance Management Platform Java ISVs Banking Finance Billing Payments The solution processes heavy volumes of personal financial data related to health insurance its functionality including fullcycle refunds management SaaS for Public Housing Public Sector Portals A USA based company automating implementation of Public Housing programs teams up with Itransition for fullcycle development of a set of ASPNET cloudbased apps united in a single solution Archive Migration Solution NET ISVs Nextgen email archive migration software with versatile platform support and nearzero risk of data loss or tampering for both premium and midsegment clients Satellite Operation Platform NET HTML5 eLearning Online Training A governmental aerospace organization aimed at developing an interactive elearning platform which would ensure that the trainees acquire the necessary operational skills while eliminating the risks and costs related to live satellite manipulation Digital Marketing Solution Python Portals Media Content Distribution Seeking to expand its market presence a UKbased company turned to Itransition for codevelopment maintenance and support of their core marketing tool automated social network referral platform allowing companies to promote their products online Video Streaming CC Python Portals Media Content Distribution Itransition delivered an advanced platform allowing security personnel of allkind organizations to connect to the networks of surveillance cameras installed view live streaming with zero downtime record the footage and save the content as video files Mobile Order Solution Manufacturing Collaboration Tools Mobility Customer Relationship Management Itransition takes over mobile solution architecture optimization and code refactoring to deliver a fully operating system Automated KPI Tool Oil Gas Business Intelligence One of the oil gas industry leaders turned to Itransition with a request of developing a solution for report generation to improve the process of company’s performance analysis Network Management System PHP Oil Gas Business Intelligence Reliable and flexible network infrastructure monitoring system with realtime network diagnostics and event notification unmatched connectivity and comprehensive reports and live monitoring capabilities Full IT Services Coverage NET Telecom Itransition takes over the mobile operator’s software QA maintenance and functionality development project to help life grow subscriber base and remarkably strengthen its positions on the market Debt Collection NET Telecom Collaboration Tools A leading telecommunications company turns to Itransition with a request to develop an application that would automate a large amount of subscribers’ debts and payments Elastic Quality Assessment NET ISVs Media Entertainment Business Intelligence A globally operating company turned to Itransition requesting development of a multitenant translation quality assessment solution dynamically adjusting consumed cloud resources to the amount of files processed at any point in time ESB for LTE Carrier Java Telecom A comprehensive ESB solution capable of working with both external and internal systems that utilize multiple communication protocols in a distributed and heterogeneous infrastructure Key Document Management NET HTML5 Oil Gas Portals Collaboration Tools A leading oil gas company turned to Itransition as a trusted vendor with a request to develop a corporate portal that would help them save up to 900 000 a year Project Control Assurance Portals Collaboration Tools A leading oil gas company turned to Itransition as a trusted vendor with a request to develop a system that would help automate the process of collaborating on project documentation Series of Facebook Games Ruby Media Content Distribution Billing Payments Gaming Scalable high loadresistant solution able to handle tens of thousands of users simultaneously playing games on Facebook 100m users for one installation 450000 active users daily 22 million users monthly 40000 requests per minute CrowdFunding Network NET Social Networking Billing Payments Mobility Online platform featuring rich social media functionality to enable fullfeatured crowdfunding any visitor is welcome to register and create a personal profile launch a fundraising campaign or browse projects and pledge to fundraising Online Ordering Platform NET ISVs eCommerce Online ordering system to control objects like menu items products pages etc and featuring integration with POS Kiosk and payment gateway support of different locations extensive reports for all restaurants etc Organic Food Community Portal eCommerce Social Networking Business Intelligence Powerful online BIdriven sales and marketing tool comprehensive suite of communityfocused services and solutions integrated proprietary Quality Assurance system for partner evaluation and relationship mapping Expense Management System Java Banking Finance Enterprise Resource Management Expense management system redevelopment for CarlaBella entailed a sustainable 12year cooperation regarding Expense Management System technical support and functionality enhancement Affiliate Partner Network Java HTML5 Travel Hospitality Portals The world’s largest online travel company hires Itransition to revamp its global 10000 private labelstrong Affiliate Network to further maintain the market leading position and boost revenues generated by the EAN line of business Unlimited Range Baby Monitor Ruby CC ISVs Manufacturing Retail Portals Media Content Distribution Mobility With Evoz baby Monitor parents can listen to their baby anytime anywhere right from their iPhone or any web browser The solution tracks and analyzes realtime data and lets them learn more about the health and activity of their children MORE View FUll Portfolio Play ► Read more 2015 IAOP research We proudly announce that according to the 2015 Global Outsourcing 100 research Itransition scored best in the Customer Reference and Company Certification categories Sales Knowledge Any business struggles with knowledge accumulation and making it transparent to all employees Especially this is critical for sales departments in service companies Choosing the App Format The choice of the best mobile delivery format is very important for any business nowadays Which mobile delivery format suits you best How to Work With Partners Here is the list of our 10 tips which may help you build a strong foundation for your business partnership for many years to come John Henderson 2015 IAOP research We proudly announce that according to the 2015 Global Outsourcing 100 research Itransition scored best in the Customer Reference and Company Certification categories Sales Knowledge Any business struggles with knowledge accumulation and making it transparent to all employees Especially this is critical for sales departments in service companies Choosing the App Format The choice of the best mobile delivery format is very important for any business nowadays Which mobile delivery format suits you best How to Work With Partners Here is the list of our 10 tips which may help you build a strong foundation for your business partnership for many years to come John Henderson 1 Contact Submit your project request be it a detailed specification or just an idea using our contact form About Advantages Awards Recognition Approach Partnership Executive Blog Corporate News Career Technology Consulting Software Prototyping Custom Software Development Software Product Development Enterprise Application Integration Application Security Virtualization Management Software QA and Testing Dedicated Development Centers Customer Service DevopsasaService B2B and B2C Web Portals Enterprise Extranets and Intranets Document Management Business Intelligence Enterprise Resource Planning Enterprise Content Management Customer Relationship Management Billing and Payments Enterprise Mobility NET Java PHP Python Ruby on Rails CC SAP Mobile infoitransitioncom Privacy Policy News News Blog News Blog Blog Blog Blog Blog Andy Hamlyn Jose Brotons Simon Aloyts Dan Zalta John Liptak ► ► 1 Means mandatory field US UK</v>
       </c>
     </row>
     <row r="15">
@@ -653,16 +545,7 @@
         <v>developers</v>
       </c>
       <c r="C15" t="str">
-        <v>PHP, Symfony 2, Ruby On Rails, Mobile - The Software House Over 50 expert web and mobile developer with an exceptional track record and extremely satisfied customers. If you need a solid dev team, drop us a line! About us We build great products for startups Need more development power for your existing business? Our clients about us: We have worked with  these amazing companies Meet the people  behind our success We're a partner of: Write to us: GET YOUR PROJECT PROPERLY DONE Call us You can reach us also at: What we bring to the table: You can count on our help in every stage of the development process. We have teams of great developers ready to help you grow your business. They are: These companies have trusted us with building the key pieces of their businesses.                            Portfolio                                                       Career                                                       PL                                                       EN                          About us Our offer Our clients People Contact us                              Portfolio                                                       Career                                                       PL                                                       EN                          PawełPHP Developer ZofiaRuby Developer Mateusz KubiczekCEO TomaszNew Business Manager PatrycjuszGraphic Designer KrzysztofPHP Developer GrzegorzRuby Developer TomaszRuby Developer WiktorPHP Developer ŁukaszRuby Developer MaciejPHP Developer SzymonPHP Developer AleksanderFrontend Developer DamianPHP Developer AdamPHP Developer Join us PiotrPHP Developer PiotrPHP Developer LidiaHR Manager WojciechPHP Developer WojtekRuby Developer PiotrMobile Developer Marcin MazurekChief Marketing Officer MateuszPHP Developer TomaszPHP Developer AleksanderMobile Developer Marek GajdaCTO TomaszProject Manager MarcinPHP Developer MarcinFrontend Developer JerzyPHP Developer JacekPHP Developer KrystianFrontend Developer PawełPHP Developer ŁukaszRuby Developer BartłomiejPHP Developer AgnieszkaGraphic Designer TomaszPHP Developer AndrzejFrontend Developer MichałPHP Developer MaciejPHP Developer DanielRuby Developer DariuszPHP Developer PiotrPHP Developer MariuszPHP Developer BartoszPHP Developer MichałMobile Developer AnnaQA Specialist DamianFrontend Developer KamilFrontend Developer MVP Development in Scrum Mobile applications Dedicated web development in Ruby and PHP based on Scrum Other services Ready to share your idea with us We have over 40 developers working in: hire your skilled team                              Portfolio                                                       Career                                                       PL                                                       EN                          About us Our offer Our clients People Contact us                              Portfolio                                                       Career                                                       PL                                                       EN                          Start building your app Hire us! Join us [email protected] /* &lt;![CDATA[ */!function(){try{var t="currentScript"in document?document.currentScript:function(){for(var t=document.getElementsByTagName("script"),e=t.length;e--;)if(t[e].getAttribute("data-cfhash"))return t[e]}();if(t&amp;&amp;t.previousSibling){var e,r,n,i,c=t.previousSibling,a=c.getAttribute("data-cfemail");if(a){for(e="",r=parseInt(a.substr(0,2),16),n=2;a.length-n;n+=2)i=parseInt(a.substr(n,2),16)^r,e+=String.fromCharCode(i);e=document.createTextNode(e),c.parentNode.replaceChild(e,c)}t.parentNode.removeChild(t);}}catch(u){}}()/* ]]&gt; */ [email protected] /* &lt;![CDATA[ */!function(){try{var t="currentScript"in document?document.currentScript:function(){for(var t=document.getElementsByTagName("script"),e=t.length;e--;)if(t[e].getAttribute("data-cfhash"))return t[e]}();if(t&amp;&amp;t.previousSibling){var e,r,n,i,c=t.previousSibling,a=c.getAttribute("data-cfemail");if(a){for(e="",r=parseInt(a.substr(0,2),16),n=2;a.length-n;n+=2)i=parseInt(a.substr(n,2),16)^r,e+=String.fromCharCode(i);e=document.createTextNode(e),c.parentNode.replaceChild(e,c)}t.parentNode.removeChild(t);}}catch(u){}}()/* ]]&gt; */ Our privacy policy Terms of service privacy policy  Toggle navigation John Max Miller, CEO  | Matthew Criticos, Partner  | James F. Ruffer III, co-founder  | Michael Fussenegger, CTO   | Magdalena Dąbrowska, Marketing Specialist  | Tapio Nurminen, CEO |  | Paweł PHP Developer Zofia Ruby Developer Mateusz Kubiczek CEO Tomasz New Business Manager Patrycjusz Graphic Designer Krzysztof PHP Developer Grzegorz Ruby Developer Tomasz Ruby Developer Wiktor PHP Developer Łukasz Ruby Developer Maciej PHP Developer Szymon PHP Developer Aleksander Frontend Developer Damian PHP Developer Adam PHP Developer Join us Piotr PHP Developer Piotr PHP Developer Lidia HR Manager Wojciech PHP Developer Wojtek Ruby Developer Piotr Mobile Developer Marcin Mazurek Chief Marketing Officer Mateusz PHP Developer Tomasz PHP Developer Aleksander Mobile Developer Marek Gajda CTO Tomasz Project Manager Marcin PHP Developer Marcin Frontend Developer Jerzy PHP Developer Jacek PHP Developer Krystian Frontend Developer Paweł PHP Developer Łukasz Ruby Developer Bartłomiej PHP Developer Agnieszka Graphic Designer Tomasz PHP Developer Andrzej Frontend Developer Michał PHP Developer Maciej PHP Developer Daniel Ruby Developer Dariusz PHP Developer Piotr PHP Developer Mariusz PHP Developer Bartosz PHP Developer Michał Mobile Developer Anna QA Specialist Damian Frontend Developer Kamil Frontend Developer [email protected] Send your message Send [email protected] 44-100  Gliwice 31-036  Kraków MVP Development in Scrum Mobile applications Dedicated web development in Ruby and PHP based on Scrum Other services</v>
-      </c>
-      <c r="D15" t="str">
-        <v>PHP, Symfony 2, Ruby On Rails, Mobile - The Software House Over 50 expert web and mobile developer with an exceptional track record and extremely satisfied customers. If you need a solid dev team, drop us a line! About us We build great products for startups Need more development power for your existing business? Our clients about us: We have worked with  these amazing companies Meet the people  behind our success We're a partner of: Write to us: GET YOUR PROJECT PROPERLY DONE Call us You can reach us also at: What we bring to the table: You can count on our help in every stage of the development process. We have teams of great developers ready to help you grow your business. They are: These companies have trusted us with building the key pieces of their businesses.                            Portfolio                                                       Career                                                       PL                                                       EN                          About us Our offer Our clients People Contact us                              Portfolio                                                       Career                                                       PL                                                       EN                          PawełPHP Developer ZofiaRuby Developer Mateusz KubiczekCEO TomaszNew Business Manager PatrycjuszGraphic Designer KrzysztofPHP Developer GrzegorzRuby Developer TomaszRuby Developer WiktorPHP Developer ŁukaszRuby Developer MaciejPHP Developer SzymonPHP Developer AleksanderFrontend Developer DamianPHP Developer AdamPHP Developer Join us PiotrPHP Developer PiotrPHP Developer LidiaHR Manager WojciechPHP Developer WojtekRuby Developer PiotrMobile Developer Marcin MazurekChief Marketing Officer MateuszPHP Developer TomaszPHP Developer AleksanderMobile Developer Marek GajdaCTO TomaszProject Manager MarcinPHP Developer MarcinFrontend Developer JerzyPHP Developer JacekPHP Developer KrystianFrontend Developer PawełPHP Developer ŁukaszRuby Developer BartłomiejPHP Developer AgnieszkaGraphic Designer TomaszPHP Developer AndrzejFrontend Developer MichałPHP Developer MaciejPHP Developer DanielRuby Developer DariuszPHP Developer PiotrPHP Developer MariuszPHP Developer BartoszPHP Developer MichałMobile Developer AnnaQA Specialist DamianFrontend Developer KamilFrontend Developer MVP Development in Scrum Mobile applications Dedicated web development in Ruby and PHP based on Scrum Other services Ready to share your idea with us We have over 40 developers working in: hire your skilled team                              Portfolio                                                       Career                                                       PL                                                       EN                          About us Our offer Our clients People Contact us                              Portfolio                                                       Career                                                       PL                                                       EN                          Start building your app Hire us! Join us [email protected] /* &lt;![CDATA[ */!function(){try{var t="currentScript"in document?document.currentScript:function(){for(var t=document.getElementsByTagName("script"),e=t.length;e--;)if(t[e].getAttribute("data-cfhash"))return t[e]}();if(t&amp;&amp;t.previousSibling){var e,r,n,i,c=t.previousSibling,a=c.getAttribute("data-cfemail");if(a){for(e="",r=parseInt(a.substr(0,2),16),n=2;a.length-n;n+=2)i=parseInt(a.substr(n,2),16)^r,e+=String.fromCharCode(i);e=document.createTextNode(e),c.parentNode.replaceChild(e,c)}t.parentNode.removeChild(t);}}catch(u){}}()/* ]]&gt; */ [email protected] /* &lt;![CDATA[ */!function(){try{var t="currentScript"in document?document.currentScript:function(){for(var t=document.getElementsByTagName("script"),e=t.length;e--;)if(t[e].getAttribute("data-cfhash"))return t[e]}();if(t&amp;&amp;t.previousSibling){var e,r,n,i,c=t.previousSibling,a=c.getAttribute("data-cfemail");if(a){for(e="",r=parseInt(a.substr(0,2),16),n=2;a.length-n;n+=2)i=parseInt(a.substr(n,2),16)^r,e+=String.fromCharCode(i);e=document.createTextNode(e),c.parentNode.replaceChild(e,c)}t.parentNode.removeChild(t);}}catch(u){}}()/* ]]&gt; */ Our privacy policy Terms of service privacy policy  Toggle navigation John Max Miller, CEO  | Matthew Criticos, Partner  | James F. Ruffer III, co-founder  | Michael Fussenegger, CTO   | Magdalena Dąbrowska, Marketing Specialist  | Tapio Nurminen, CEO |  | Paweł PHP Developer Zofia Ruby Developer Mateusz Kubiczek CEO Tomasz New Business Manager Patrycjusz Graphic Designer Krzysztof PHP Developer Grzegorz Ruby Developer Tomasz Ruby Developer Wiktor PHP Developer Łukasz Ruby Developer Maciej PHP Developer Szymon PHP Developer Aleksander Frontend Developer Damian PHP Developer Adam PHP Developer Join us Piotr PHP Developer Piotr PHP Developer Lidia HR Manager Wojciech PHP Developer Wojtek Ruby Developer Piotr Mobile Developer Marcin Mazurek Chief Marketing Officer Mateusz PHP Developer Tomasz PHP Developer Aleksander Mobile Developer Marek Gajda CTO Tomasz Project Manager Marcin PHP Developer Marcin Frontend Developer Jerzy PHP Developer Jacek PHP Developer Krystian Frontend Developer Paweł PHP Developer Łukasz Ruby Developer Bartłomiej PHP Developer Agnieszka Graphic Designer Tomasz PHP Developer Andrzej Frontend Developer Michał PHP Developer Maciej PHP Developer Daniel Ruby Developer Dariusz PHP Developer Piotr PHP Developer Mariusz PHP Developer Bartosz PHP Developer Michał Mobile Developer Anna QA Specialist Damian Frontend Developer Kamil Frontend Developer [email protected] Send your message Send [email protected] 44-100  Gliwice 31-036  Kraków MVP Development in Scrum Mobile applications Dedicated web development in Ruby and PHP based on Scrum Other services</v>
-      </c>
-      <c r="E15" t="str">
-        <v>PHP, Symfony 2, Ruby On Rails, Mobile - The Software House Over 50 expert web and mobile developer with an exceptional track record and extremely satisfied customers. If you need a solid dev team, drop us a line! About us We build great products for startups Need more development power for your existing business? Our clients about us: We have worked with  these amazing companies Meet the people  behind our success We're a partner of: Write to us: GET YOUR PROJECT PROPERLY DONE Call us You can reach us also at: What we bring to the table: You can count on our help in every stage of the development process. We have teams of great developers ready to help you grow your business. They are: These companies have trusted us with building the key pieces of their businesses.                            Portfolio                                                       Career                                                       PL                                                       EN                          About us Our offer Our clients People Contact us                              Portfolio                                                       Career                                                       PL                                                       EN                          PawełPHP Developer ZofiaRuby Developer Mateusz KubiczekCEO TomaszNew Business Manager PatrycjuszGraphic Designer KrzysztofPHP Developer GrzegorzRuby Developer TomaszRuby Developer WiktorPHP Developer ŁukaszRuby Developer MaciejPHP Developer SzymonPHP Developer AleksanderFrontend Developer DamianPHP Developer AdamPHP Developer Join us PiotrPHP Developer PiotrPHP Developer LidiaHR Manager WojciechPHP Developer WojtekRuby Developer PiotrMobile Developer Marcin MazurekChief Marketing Officer MateuszPHP Developer TomaszPHP Developer AleksanderMobile Developer Marek GajdaCTO TomaszProject Manager MarcinPHP Developer MarcinFrontend Developer JerzyPHP Developer JacekPHP Developer KrystianFrontend Developer PawełPHP Developer ŁukaszRuby Developer BartłomiejPHP Developer AgnieszkaGraphic Designer TomaszPHP Developer AndrzejFrontend Developer MichałPHP Developer MaciejPHP Developer DanielRuby Developer DariuszPHP Developer PiotrPHP Developer MariuszPHP Developer BartoszPHP Developer MichałMobile Developer AnnaQA Specialist DamianFrontend Developer KamilFrontend Developer MVP Development in Scrum Mobile applications Dedicated web development in Ruby and PHP based on Scrum Other services Ready to share your idea with us We have over 40 developers working in: hire your skilled team                              Portfolio                                                       Career                                                       PL                                                       EN                          About us Our offer Our clients People Contact us                              Portfolio                                                       Career                                                       PL                                                       EN                          Start building your app Hire us! Join us [email protected] /* &lt;![CDATA[ */!function(){try{var t="currentScript"in document?document.currentScript:function(){for(var t=document.getElementsByTagName("script"),e=t.length;e--;)if(t[e].getAttribute("data-cfhash"))return t[e]}();if(t&amp;&amp;t.previousSibling){var e,r,n,i,c=t.previousSibling,a=c.getAttribute("data-cfemail");if(a){for(e="",r=parseInt(a.substr(0,2),16),n=2;a.length-n;n+=2)i=parseInt(a.substr(n,2),16)^r,e+=String.fromCharCode(i);e=document.createTextNode(e),c.parentNode.replaceChild(e,c)}t.parentNode.removeChild(t);}}catch(u){}}()/* ]]&gt; */ [email protected] /* &lt;![CDATA[ */!function(){try{var t="currentScript"in document?document.currentScript:function(){for(var t=document.getElementsByTagName("script"),e=t.length;e--;)if(t[e].getAttribute("data-cfhash"))return t[e]}();if(t&amp;&amp;t.previousSibling){var e,r,n,i,c=t.previousSibling,a=c.getAttribute("data-cfemail");if(a){for(e="",r=parseInt(a.substr(0,2),16),n=2;a.length-n;n+=2)i=parseInt(a.substr(n,2),16)^r,e+=String.fromCharCode(i);e=document.createTextNode(e),c.parentNode.replaceChild(e,c)}t.parentNode.removeChild(t);}}catch(u){}}()/* ]]&gt; */ Our privacy policy Terms of service privacy policy  Toggle navigation John Max Miller, CEO  | Matthew Criticos, Partner  | James F. Ruffer III, co-founder  | Michael Fussenegger, CTO   | Magdalena Dąbrowska, Marketing Specialist  | Tapio Nurminen, CEO |  | Paweł PHP Developer Zofia Ruby Developer Mateusz Kubiczek CEO Tomasz New Business Manager Patrycjusz Graphic Designer Krzysztof PHP Developer Grzegorz Ruby Developer Tomasz Ruby Developer Wiktor PHP Developer Łukasz Ruby Developer Maciej PHP Developer Szymon PHP Developer Aleksander Frontend Developer Damian PHP Developer Adam PHP Developer Join us Piotr PHP Developer Piotr PHP Developer Lidia HR Manager Wojciech PHP Developer Wojtek Ruby Developer Piotr Mobile Developer Marcin Mazurek Chief Marketing Officer Mateusz PHP Developer Tomasz PHP Developer Aleksander Mobile Developer Marek Gajda CTO Tomasz Project Manager Marcin PHP Developer Marcin Frontend Developer Jerzy PHP Developer Jacek PHP Developer Krystian Frontend Developer Paweł PHP Developer Łukasz Ruby Developer Bartłomiej PHP Developer Agnieszka Graphic Designer Tomasz PHP Developer Andrzej Frontend Developer Michał PHP Developer Maciej PHP Developer Daniel Ruby Developer Dariusz PHP Developer Piotr PHP Developer Mariusz PHP Developer Bartosz PHP Developer Michał Mobile Developer Anna QA Specialist Damian Frontend Developer Kamil Frontend Developer [email protected] Send your message Send [email protected] 44-100  Gliwice 31-036  Kraków MVP Development in Scrum Mobile applications Dedicated web development in Ruby and PHP based on Scrum Other services</v>
-      </c>
-      <c r="F15" t="str">
-        <v>PHP, Symfony 2, Ruby On Rails, Mobile - The Software House Over 50 expert web and mobile developer with an exceptional track record and extremely satisfied customers. If you need a solid dev team, drop us a line! About us We build great products for startups Need more development power for your existing business? Our clients about us: We have worked with  these amazing companies Meet the people  behind our success We're a partner of: Write to us: GET YOUR PROJECT PROPERLY DONE Call us You can reach us also at: What we bring to the table: You can count on our help in every stage of the development process. We have teams of great developers ready to help you grow your business. They are: These companies have trusted us with building the key pieces of their businesses.                            Portfolio                                                       Career                                                       PL                                                       EN                          About us Our offer Our clients People Contact us                              Portfolio                                                       Career                                                       PL                                                       EN                          PawełPHP Developer ZofiaRuby Developer Mateusz KubiczekCEO TomaszNew Business Manager PatrycjuszGraphic Designer KrzysztofPHP Developer GrzegorzRuby Developer TomaszRuby Developer WiktorPHP Developer ŁukaszRuby Developer MaciejPHP Developer SzymonPHP Developer AleksanderFrontend Developer DamianPHP Developer AdamPHP Developer Join us PiotrPHP Developer PiotrPHP Developer LidiaHR Manager WojciechPHP Developer WojtekRuby Developer PiotrMobile Developer Marcin MazurekChief Marketing Officer MateuszPHP Developer TomaszPHP Developer AleksanderMobile Developer Marek GajdaCTO TomaszProject Manager MarcinPHP Developer MarcinFrontend Developer JerzyPHP Developer JacekPHP Developer KrystianFrontend Developer PawełPHP Developer ŁukaszRuby Developer BartłomiejPHP Developer AgnieszkaGraphic Designer TomaszPHP Developer AndrzejFrontend Developer MichałPHP Developer MaciejPHP Developer DanielRuby Developer DariuszPHP Developer PiotrPHP Developer MariuszPHP Developer BartoszPHP Developer MichałMobile Developer AnnaQA Specialist DamianFrontend Developer KamilFrontend Developer MVP Development in Scrum Mobile applications Dedicated web development in Ruby and PHP based on Scrum Other services Ready to share your idea with us We have over 40 developers working in: hire your skilled team                              Portfolio                                                       Career                                                       PL                                                       EN                          About us Our offer Our clients People Contact us                              Portfolio                                                       Career                                                       PL                                                       EN                          Start building your app Hire us! Join us [email protected] /* &lt;![CDATA[ */!function(){try{var t="currentScript"in document?document.currentScript:function(){for(var t=document.getElementsByTagName("script"),e=t.length;e--;)if(t[e].getAttribute("data-cfhash"))return t[e]}();if(t&amp;&amp;t.previousSibling){var e,r,n,i,c=t.previousSibling,a=c.getAttribute("data-cfemail");if(a){for(e="",r=parseInt(a.substr(0,2),16),n=2;a.length-n;n+=2)i=parseInt(a.substr(n,2),16)^r,e+=String.fromCharCode(i);e=document.createTextNode(e),c.parentNode.replaceChild(e,c)}t.parentNode.removeChild(t);}}catch(u){}}()/* ]]&gt; */ [email protected] /* &lt;![CDATA[ */!function(){try{var t="currentScript"in document?document.currentScript:function(){for(var t=document.getElementsByTagName("script"),e=t.length;e--;)if(t[e].getAttribute("data-cfhash"))return t[e]}();if(t&amp;&amp;t.previousSibling){var e,r,n,i,c=t.previousSibling,a=c.getAttribute("data-cfemail");if(a){for(e="",r=parseInt(a.substr(0,2),16),n=2;a.length-n;n+=2)i=parseInt(a.substr(n,2),16)^r,e+=String.fromCharCode(i);e=document.createTextNode(e),c.parentNode.replaceChild(e,c)}t.parentNode.removeChild(t);}}catch(u){}}()/* ]]&gt; */ Our privacy policy Terms of service privacy policy  Toggle navigation John Max Miller, CEO  | Matthew Criticos, Partner  | James F. Ruffer III, co-founder  | Michael Fussenegger, CTO   | Magdalena Dąbrowska, Marketing Specialist  | Tapio Nurminen, CEO |  | Paweł PHP Developer Zofia Ruby Developer Mateusz Kubiczek CEO Tomasz New Business Manager Patrycjusz Graphic Designer Krzysztof PHP Developer Grzegorz Ruby Developer Tomasz Ruby Developer Wiktor PHP Developer Łukasz Ruby Developer Maciej PHP Developer Szymon PHP Developer Aleksander Frontend Developer Damian PHP Developer Adam PHP Developer Join us Piotr PHP Developer Piotr PHP Developer Lidia HR Manager Wojciech PHP Developer Wojtek Ruby Developer Piotr Mobile Developer Marcin Mazurek Chief Marketing Officer Mateusz PHP Developer Tomasz PHP Developer Aleksander Mobile Developer Marek Gajda CTO Tomasz Project Manager Marcin PHP Developer Marcin Frontend Developer Jerzy PHP Developer Jacek PHP Developer Krystian Frontend Developer Paweł PHP Developer Łukasz Ruby Developer Bartłomiej PHP Developer Agnieszka Graphic Designer Tomasz PHP Developer Andrzej Frontend Developer Michał PHP Developer Maciej PHP Developer Daniel Ruby Developer Dariusz PHP Developer Piotr PHP Developer Mariusz PHP Developer Bartosz PHP Developer Michał Mobile Developer Anna QA Specialist Damian Frontend Developer Kamil Frontend Developer [email protected] Send your message Send [email protected] 44-100  Gliwice 31-036  Kraków MVP Development in Scrum Mobile applications Dedicated web development in Ruby and PHP based on Scrum Other services</v>
+        <v>PHP Symfony 2 Ruby On Rails Mobile The Software House Over 50 expert web and mobile developer with an exceptional track record and extremely satisfied customers If you need a solid dev team drop us a line About us We build great products for startups Need more development power for your existing business Our clients about us We have worked with these amazing companies Meet the people behind our success Were a partner of Write to us GET YOUR PROJECT PROPERLY DONE Call us You can reach us also at What we bring to the table You can count on our help in every stage of the development process We have teams of great developers ready to help you grow your business They are These companies have trusted us with building the key pieces of their businesses Portfolio Career PL EN About us Our offer Our clients People Contact us Portfolio Career PL EN PawełPHP Developer ZofiaRuby Developer Mateusz KubiczekCEO TomaszNew Business Manager PatrycjuszGraphic Designer KrzysztofPHP Developer GrzegorzRuby Developer TomaszRuby Developer WiktorPHP Developer ŁukaszRuby Developer MaciejPHP Developer SzymonPHP Developer AleksanderFrontend Developer DamianPHP Developer AdamPHP Developer Join us PiotrPHP Developer PiotrPHP Developer LidiaHR Manager WojciechPHP Developer WojtekRuby Developer PiotrMobile Developer Marcin MazurekChief Marketing Officer MateuszPHP Developer TomaszPHP Developer AleksanderMobile Developer Marek GajdaCTO TomaszProject Manager MarcinPHP Developer MarcinFrontend Developer JerzyPHP Developer JacekPHP Developer KrystianFrontend Developer PawełPHP Developer ŁukaszRuby Developer BartłomiejPHP Developer AgnieszkaGraphic Designer TomaszPHP Developer AndrzejFrontend Developer MichałPHP Developer MaciejPHP Developer DanielRuby Developer DariuszPHP Developer PiotrPHP Developer MariuszPHP Developer BartoszPHP Developer MichałMobile Developer AnnaQA Specialist DamianFrontend Developer KamilFrontend Developer MVP Development in Scrum Mobile applications Dedicated web development in Ruby and PHP based on Scrum Other services Ready to share your idea with us We have over 40 developers working in hire your skilled team Portfolio Career PL EN About us Our offer Our clients People Contact us Portfolio Career PL EN Start building your app Hire us Join us email protected CDATA functiontryvar tcurrentScriptin documentdocumentcurrentScriptfunctionforvar tdocumentgetElementsByTagNamescriptetlengtheiftegetAttributedatacfhashreturn teifttpreviousSiblingvar ernictpreviousSiblingacgetAttributedatacfemailifaforerparseIntasubstr0216n2alengthnn2iparseIntasubstrn216reStringfromCharCodeiedocumentcreateTextNodeecparentNodereplaceChildectparentNoderemoveChildtcatchu email protected CDATA functiontryvar tcurrentScriptin documentdocumentcurrentScriptfunctionforvar tdocumentgetElementsByTagNamescriptetlengtheiftegetAttributedatacfhashreturn teifttpreviousSiblingvar ernictpreviousSiblingacgetAttributedatacfemailifaforerparseIntasubstr0216n2alengthnn2iparseIntasubstrn216reStringfromCharCodeiedocumentcreateTextNodeecparentNodereplaceChildectparentNoderemoveChildtcatchu Our privacy policy Terms of service privacy policy Toggle navigation John Max Miller CEO Matthew Criticos Partner James F Ruffer III cofounder Michael Fussenegger CTO Magdalena Dąbrowska Marketing Specialist Tapio Nurminen CEO Paweł PHP Developer Zofia Ruby Developer Mateusz Kubiczek CEO Tomasz New Business Manager Patrycjusz Graphic Designer Krzysztof PHP Developer Grzegorz Ruby Developer Tomasz Ruby Developer Wiktor PHP Developer Łukasz Ruby Developer Maciej PHP Developer Szymon PHP Developer Aleksander Frontend Developer Damian PHP Developer Adam PHP Developer Join us Piotr PHP Developer Piotr PHP Developer Lidia HR Manager Wojciech PHP Developer Wojtek Ruby Developer Piotr Mobile Developer Marcin Mazurek Chief Marketing Officer Mateusz PHP Developer Tomasz PHP Developer Aleksander Mobile Developer Marek Gajda CTO Tomasz Project Manager Marcin PHP Developer Marcin Frontend Developer Jerzy PHP Developer Jacek PHP Developer Krystian Frontend Developer Paweł PHP Developer Łukasz Ruby Developer Bartłomiej PHP Developer Agnieszka Graphic Designer Tomasz PHP Developer Andrzej Frontend Developer Michał PHP Developer Maciej PHP Developer Daniel Ruby Developer Dariusz PHP Developer Piotr PHP Developer Mariusz PHP Developer Bartosz PHP Developer Michał Mobile Developer Anna QA Specialist Damian Frontend Developer Kamil Frontend Developer email protected Send your message Send email protected 44100 Gliwice 31036 Kraków MVP Development in Scrum Mobile applications Dedicated web development in Ruby and PHP based on Scrum Other services</v>
       </c>
     </row>
     <row r="16">
@@ -673,16 +556,7 @@
         <v>developers</v>
       </c>
       <c r="C16" t="str">
-        <v>OK GROW! — Web and mobile app development in Toronto Expert web and mobile app development in Toronto. We build software that solves problems and creates opportunities for our clients. Expert web and mobile app development We build software that solves problems and creates opportunities for our clients. Good Software Starts With Strategic UX Launch a better product sooner with Meteor Safe At Home Vet Practice Report Card Find out more Stay updated Get in touch 70% of IT products are a failure because they do not get adopted. 80% of IT budgets are spent fixing these products.  This article talks about the power of strategic UX and the ROI of building products right the first time. Read More About Strategic UX → Already a well-known brand offline, Kidde Canada wanted to venture into the mobile app world. But they wanted to provide real value to their present and future customers rather than simply moving old media to a new format. There was a key problem to solve: how do we make sure the app stays installed after the first few uses? CONTINUE READING → As software developers we’re used to having detailed analytics available to understand and fine-tune our business and interactions with customers. But offline businesses like veterinary practices haven’t, until now, had the same tools available. We’re big fans of making data-driven product and business decisions so we jumped at the chance to help solve this problem.  CONTINUE READING → Meteor.js is a toolkit for building modern web apps and cross-platform mobile apps in a fraction of the time. Learn More About Meteor → “Very easy to work with, and always exceeded my expectations.” — Brandon Budz, Yellow Pages Group “For entrepreneurs and startups, you should consider the OK GROW! team the technical team that you are unable to recruit. They recognize the importance of building your own internal team, and due to their active presence in the local tech community, will help you in cultivating that team. Most of all, they're a group of great people that are interested in seeing your company thrive as much as their own.” — Adam Epstein, HUDDLERS Contact / Services Methodology / Work Team / Blog Join us Twitter Facebook Google+ GitHub Hire Us +1-855-747-9930 hello@okgrow.com 298 Dundas St. West, Unit BToronto, OntarioM5T 1G2, Canada Services  Methodology Work   Team   Blog   Contact  Read More About Strategic UX → CONTINUE READING →  CONTINUE READING → Learn More About Meteor → See More of Our Work → Contact Services Methodology Work Team Blog Join us Twitter Facebook Google+ GitHub Hire Us +1-855-747-9930 hello@okgrow.com 298 Dundas St. West, Unit BToronto, OntarioM5T 1G2, Canada Meteor.js is a toolkit for building   web apps and cross-platform mobile apps in a fraction of the time. Get tips and info in your inbox occasionally Thanks for signing up, and please do give us some feedback!  /   /   /  298 Dundas St. West, Unit B Toronto, Ontario M5T 1G2, Canada</v>
-      </c>
-      <c r="D16" t="str">
-        <v>OK GROW! — Web and mobile app development in Toronto Expert web and mobile app development in Toronto. We build software that solves problems and creates opportunities for our clients. Expert web and mobile app development We build software that solves problems and creates opportunities for our clients. Good Software Starts With Strategic UX Launch a better product sooner with Meteor Safe At Home Vet Practice Report Card Find out more Stay updated Get in touch 70% of IT products are a failure because they do not get adopted. 80% of IT budgets are spent fixing these products.  This article talks about the power of strategic UX and the ROI of building products right the first time. Read More About Strategic UX → Already a well-known brand offline, Kidde Canada wanted to venture into the mobile app world. But they wanted to provide real value to their present and future customers rather than simply moving old media to a new format. There was a key problem to solve: how do we make sure the app stays installed after the first few uses? CONTINUE READING → As software developers we’re used to having detailed analytics available to understand and fine-tune our business and interactions with customers. But offline businesses like veterinary practices haven’t, until now, had the same tools available. We’re big fans of making data-driven product and business decisions so we jumped at the chance to help solve this problem.  CONTINUE READING → Meteor.js is a toolkit for building modern web apps and cross-platform mobile apps in a fraction of the time. Learn More About Meteor → “Very easy to work with, and always exceeded my expectations.” — Brandon Budz, Yellow Pages Group “For entrepreneurs and startups, you should consider the OK GROW! team the technical team that you are unable to recruit. They recognize the importance of building your own internal team, and due to their active presence in the local tech community, will help you in cultivating that team. Most of all, they're a group of great people that are interested in seeing your company thrive as much as their own.” — Adam Epstein, HUDDLERS Contact / Services Methodology / Work Team / Blog Join us Twitter Facebook Google+ GitHub Hire Us +1-855-747-9930 hello@okgrow.com 298 Dundas St. West, Unit BToronto, OntarioM5T 1G2, Canada Services  Methodology Work   Team   Blog   Contact  Read More About Strategic UX → CONTINUE READING →  CONTINUE READING → Learn More About Meteor → See More of Our Work → Contact Services Methodology Work Team Blog Join us Twitter Facebook Google+ GitHub Hire Us +1-855-747-9930 hello@okgrow.com 298 Dundas St. West, Unit BToronto, OntarioM5T 1G2, Canada Meteor.js is a toolkit for building   web apps and cross-platform mobile apps in a fraction of the time. Get tips and info in your inbox occasionally Thanks for signing up, and please do give us some feedback!  /   /   /  298 Dundas St. West, Unit B Toronto, Ontario M5T 1G2, Canada</v>
-      </c>
-      <c r="E16" t="str">
-        <v>OK GROW! — Web and mobile app development in Toronto Expert web and mobile app development in Toronto. We build software that solves problems and creates opportunities for our clients. Expert web and mobile app development We build software that solves problems and creates opportunities for our clients. Good Software Starts With Strategic UX Launch a better product sooner with Meteor Safe At Home Vet Practice Report Card Find out more Stay updated Get in touch 70% of IT products are a failure because they do not get adopted. 80% of IT budgets are spent fixing these products.  This article talks about the power of strategic UX and the ROI of building products right the first time. Read More About Strategic UX → Already a well-known brand offline, Kidde Canada wanted to venture into the mobile app world. But they wanted to provide real value to their present and future customers rather than simply moving old media to a new format. There was a key problem to solve: how do we make sure the app stays installed after the first few uses? CONTINUE READING → As software developers we’re used to having detailed analytics available to understand and fine-tune our business and interactions with customers. But offline businesses like veterinary practices haven’t, until now, had the same tools available. We’re big fans of making data-driven product and business decisions so we jumped at the chance to help solve this problem.  CONTINUE READING → Meteor.js is a toolkit for building modern web apps and cross-platform mobile apps in a fraction of the time. Learn More About Meteor → “Very easy to work with, and always exceeded my expectations.” — Brandon Budz, Yellow Pages Group “For entrepreneurs and startups, you should consider the OK GROW! team the technical team that you are unable to recruit. They recognize the importance of building your own internal team, and due to their active presence in the local tech community, will help you in cultivating that team. Most of all, they're a group of great people that are interested in seeing your company thrive as much as their own.” — Adam Epstein, HUDDLERS Contact / Services Methodology / Work Team / Blog Join us Twitter Facebook Google+ GitHub Hire Us +1-855-747-9930 hello@okgrow.com 298 Dundas St. West, Unit BToronto, OntarioM5T 1G2, Canada Services  Methodology Work   Team   Blog   Contact  Read More About Strategic UX → CONTINUE READING →  CONTINUE READING → Learn More About Meteor → See More of Our Work → Contact Services Methodology Work Team Blog Join us Twitter Facebook Google+ GitHub Hire Us +1-855-747-9930 hello@okgrow.com 298 Dundas St. West, Unit BToronto, OntarioM5T 1G2, Canada Meteor.js is a toolkit for building   web apps and cross-platform mobile apps in a fraction of the time. Get tips and info in your inbox occasionally Thanks for signing up, and please do give us some feedback!  /   /   /  298 Dundas St. West, Unit B Toronto, Ontario M5T 1G2, Canada</v>
-      </c>
-      <c r="F16" t="str">
-        <v>OK GROW! — Web and mobile app development in Toronto Expert web and mobile app development in Toronto. We build software that solves problems and creates opportunities for our clients. Expert web and mobile app development We build software that solves problems and creates opportunities for our clients. Good Software Starts With Strategic UX Launch a better product sooner with Meteor Safe At Home Vet Practice Report Card Find out more Stay updated Get in touch 70% of IT products are a failure because they do not get adopted. 80% of IT budgets are spent fixing these products.  This article talks about the power of strategic UX and the ROI of building products right the first time. Read More About Strategic UX → Already a well-known brand offline, Kidde Canada wanted to venture into the mobile app world. But they wanted to provide real value to their present and future customers rather than simply moving old media to a new format. There was a key problem to solve: how do we make sure the app stays installed after the first few uses? CONTINUE READING → As software developers we’re used to having detailed analytics available to understand and fine-tune our business and interactions with customers. But offline businesses like veterinary practices haven’t, until now, had the same tools available. We’re big fans of making data-driven product and business decisions so we jumped at the chance to help solve this problem.  CONTINUE READING → Meteor.js is a toolkit for building modern web apps and cross-platform mobile apps in a fraction of the time. Learn More About Meteor → “Very easy to work with, and always exceeded my expectations.” — Brandon Budz, Yellow Pages Group “For entrepreneurs and startups, you should consider the OK GROW! team the technical team that you are unable to recruit. They recognize the importance of building your own internal team, and due to their active presence in the local tech community, will help you in cultivating that team. Most of all, they're a group of great people that are interested in seeing your company thrive as much as their own.” — Adam Epstein, HUDDLERS Contact / Services Methodology / Work Team / Blog Join us Twitter Facebook Google+ GitHub Hire Us +1-855-747-9930 hello@okgrow.com 298 Dundas St. West, Unit BToronto, OntarioM5T 1G2, Canada Services  Methodology Work   Team   Blog   Contact  Read More About Strategic UX → CONTINUE READING →  CONTINUE READING → Learn More About Meteor → See More of Our Work → Contact Services Methodology Work Team Blog Join us Twitter Facebook Google+ GitHub Hire Us +1-855-747-9930 hello@okgrow.com 298 Dundas St. West, Unit BToronto, OntarioM5T 1G2, Canada Meteor.js is a toolkit for building   web apps and cross-platform mobile apps in a fraction of the time. Get tips and info in your inbox occasionally Thanks for signing up, and please do give us some feedback!  /   /   /  298 Dundas St. West, Unit B Toronto, Ontario M5T 1G2, Canada</v>
+        <v>OK GROW Web and mobile app development in Toronto Expert web and mobile app development in Toronto We build software that solves problems and creates opportunities for our clients Expert web and mobile app development We build software that solves problems and creates opportunities for our clients Good Software Starts With Strategic UX Launch a better product sooner with Meteor Safe At Home Vet Practice Report Card Find out more Stay updated Get in touch 70 of IT products are a failure because they do not get adopted 80 of IT budgets are spent fixing these products This article talks about the power of strategic UX and the ROI of building products right the first time Read More About Strategic UX → Already a wellknown brand offline Kidde Canada wanted to venture into the mobile app world But they wanted to provide real value to their present and future customers rather than simply moving old media to a new format There was a key problem to solve how do we make sure the app stays installed after the first few uses CONTINUE READING → As software developers we’re used to having detailed analytics available to understand and finetune our business and interactions with customers But offline businesses like veterinary practices haven’t until now had the same tools available We’re big fans of making datadriven product and business decisions so we jumped at the chance to help solve this problem CONTINUE READING → Meteorjs is a toolkit for building modern web apps and crossplatform mobile apps in a fraction of the time Learn More About Meteor → “Very easy to work with and always exceeded my expectations” Brandon Budz Yellow Pages Group “For entrepreneurs and startups you should consider the OK GROW team the technical team that you are unable to recruit They recognize the importance of building your own internal team and due to their active presence in the local tech community will help you in cultivating that team Most of all theyre a group of great people that are interested in seeing your company thrive as much as their own” Adam Epstein HUDDLERS Contact Services Methodology Work Team Blog Join us Twitter Facebook Google GitHub Hire Us 18557479930 hellookgrowcom 298 Dundas St West Unit BToronto OntarioM5T 1G2 Canada Services Methodology Work Team Blog Contact Read More About Strategic UX → CONTINUE READING → CONTINUE READING → Learn More About Meteor → See More of Our Work → Contact Services Methodology Work Team Blog Join us Twitter Facebook Google GitHub Hire Us 18557479930 hellookgrowcom 298 Dundas St West Unit BToronto OntarioM5T 1G2 Canada Meteorjs is a toolkit for building web apps and crossplatform mobile apps in a fraction of the time Get tips and info in your inbox occasionally Thanks for signing up and please do give us some feedback 298 Dundas St West Unit B Toronto Ontario M5T 1G2 Canada</v>
       </c>
     </row>
     <row r="17">
@@ -693,16 +567,7 @@
         <v>Training and dev</v>
       </c>
       <c r="C17" t="str">
-        <v>Vancouver Digital Marketing, Web Design &amp; Development Courses RED Academy is a unique Vancouver-based technology academy created for the designers, creators, developers and digital marketers of tomorrow. BC’s Leading Tech Academy Taught by the Industry, for the Industry. Professional Programs Evening Foundation Programs Evening Essentials Programs Meet Some of Our Instructors Real Projects, Real Learning. Interested in finding out more? Katie Jeanes Mandi Wise Lindsay Henwood Robert MacKie Lyndon Mayer David Kohler Some of Our Partners Contact Form Courses Full-Time Professional Programs  – Digital Marketing &amp; Strategy  – Web Developer  – User Experience Designer  Part-Time Foundation Programs  – Digital Marketing Foundation  – Web Developer Foundation  – User Experience Design Foundation  Part-Time Essentials Programs  – AngularJS  – Design Essentials   Full-Time Professional Programs – Digital Marketing &amp; Strategy – Web Developer – User Experience Designer Part-Time Foundation Programs – Digital Marketing Foundation – Web Developer Foundation – User Experience Design Foundation Part-Time Essentials Programs – AngularJS – Design Essentials About   Meet The Team  Become an Instructor  Careers  Submit A Student Project  Hiring Partner Program  Community Programs   Meet The Team Become an Instructor Careers Submit A Student Project Hiring Partner Program Community Programs Blog Events Contact ​ 604​ ​674​ ​8332 Full-Time Professional Part-Time Foundation Part-Time Essentials                                                                                                                             Professional Programs                                     Full Time Programs, 12 weeks immersive.                                     View                                         Courses                                                                                                                                                Course Name Dates                                                                                                                                      UX Designer Professional                                                                                                     11 Apr - 30 Jun                                                                                                                                                                                   Web Developer Professional                                                                                                     11 Apr - 30 Jun                                                                                                                                                                                   Digital Marketing Professional                                                                                                     11 Apr - 30 Jun                                                                                                                                                                                                                                                                                                                                                                   Evening Foundation Programs                                     Part Time Programs, two evenings per week for 10 weeks.                                     View                                         Courses                                                                                                                                                Course Name Dates                                                                                                                                      UX Designer Foundation                                                                                                     25 Jan - 1 Apr                                                                                                                                                                                   Web Developer Foundation                                                                                                     25 Jan - 1 Apr                                                                                                                                                                                   Digital Marketing Foundation                                                                                                     26 Jan - 1 Apr                                                                                                                                                                                                                                                                                                                                                                               Evening Essentials Programs                                     Part Time Programs, one evening per week for 5 weeks.                                         View Courses                                                                                                                                                                Course Name Dates                                                                                                                                                  AngularJS in Production                                                                                                             2 Feb - 11 Feb                                                                                                                                                                                                   Visual Designer Essentials                                                                                                             1 Feb - 25 Feb                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                          Katie Jeanes                                                 Instructor, Digital Marketing                                                 With over 8 years of experience in Analytics, User Acquisition and Social Media, Katie joins the team as an instructor of Digital Marketing. She has also previously founded two startups in digital media and fashion technology. Inspired by creative entrepreneurs and innovative startups, Katie is excited to demystify digital marketing and helping students launch a career they love. She also happens to be a darn good baker!                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                          Mandi Wise                                                 Lead Instructor, Head of Curriculum                                                 Mandi is one of the lead instructors for our immersive programs. Web developer by day (and usually at night too), Mandi specializes in custom WordPress plugin and theme development. Her background in content strategy and web writing has helped her develop a well-rounded approach to her current skill set. When she’s not creating structurally sound websites that work like a well-oiled machine, you can find her making use of a fleet of vintage cameras. In fact, nothing makes her quite as excited as the sound of a Polaroid SX-70 camera the moment it ejects a new photo.                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                          Lindsay Henwood                                                 Lead Instructor, UX Designer                                                 Lindsay Henwood loves UX design. She has a diverse background – from University of Victoria to surf instruction and all points in between – but her empathetic nature and passion for design thinking led her to the field of UX over the last several years. A graduate of General Assembly’s UX Design Immersive program in Seattle, she has worked with companies like Shopify, Sitka, and Navicet to refine their products and presence. Her design sensibilities translate into her teaching, offering students clear insights into the practice of UX thinking and application. She gets excited about user research, affinity diagrams and usability testing, and she’ll jump at the chance to chat about UX – so feel free to reach out to her about it or swing by to meet in person. She also wouldn’t mind if you brought snacks along too.                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                          Robert MacKie                                                 Instructor, UX Designer                                                 Robert is a people person and a person of the arts. From tiny start ups, to digital agencies to massive corporations, Robert brings 10 years design experience from a wide range of industries. Woven into those years is a wealth of experience and love of new media, visual and performance arts. Immensely social and outgoing, he has an equal love of working with people – be it helping, mentoring, teaching them or just having a good old conversation. But what puts him over the moon? Bringing those worlds together. Seeing the positive impact that comes of bringing art, design and people together is what Robert considers pure bliss.                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                          Lyndon Mayer                                                 Instructor, UX Designer                                                 Lyndon is a highly experienced UX Designer originally from Melbourne, Australia. Over the past 7 years he’s worked with small and large scale clients across both hemispheres on projects ranging from websites, native apps and service based products. Currently working at Electronic Arts in Burnaby, he’s tasked with designing the next generation of web connected game experiences for EA and EA Sports titles. Lyndon is a huge advocate for applying good user centred design principles to every problem and is especially interested in natural interfaces and contextual application design.                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                          David Kohler                                                 Academic Director                                                 As Academic Director of RED Academy, David has found a natural element for his passion of empowering people. He is making it his mission to ensure that students benefit from a dynamic, authentic and productive environment at RED by way of providing instructors with the tools to create engaging learning activities. Following over a decade of university-level teaching experience, David took on to develop himself as a trainer and as a coach. David holds a Ph.D. in theoretical mathematics, makes a different soup (almost) every Monday. He is originally from Switzerland and as a result, has a funny accent.                                                                                                                                                                                                                   Name* Email*                                                       Phone Message*                                         View                                 Courses                             Attend Intro Session                          RED Academy is a leading-edge technology school for the designers, creators, developers and digital marketers of tomorrow. We were born out of some of Western Canada’s leading digital agencies, and work closely with a network of industry partners to design highly engaging, immersive learning programs that give our students the right technical skills and knowledge to succeed in today’s rapidly evolving workplace. Learn to become a web developer - FT and PT programs. Learn to design user interfaces  - FT and PT programs. Engage, drive and measure traffic - FT and PT programs. Full Time Programs, 12 weeks immersive.                                                  UX Designer Professional                                                                                                     11 Apr - 30 Jun                                                                                               Web Developer Professional                                                                                                     11 Apr - 30 Jun                                                                                               Digital Marketing Professional                                                                                                     11 Apr - 30 Jun                                              Part Time Programs, two evenings per week for 10 weeks.                                                  UX Designer Foundation                                                                                                     25 Jan - 1 Apr                                                                                               Web Developer Foundation                                                                                                     25 Jan - 1 Apr                                                                                               Digital Marketing Foundation                                                                                                     26 Jan - 1 Apr                                              Part Time Programs, one evening per week for 5 weeks.                                                      AngularJS in Production                                                                                                             2 Feb - 11 Feb                                                                                                       Visual Designer Essentials                                                                                                             1 Feb - 25 Feb                                                  Instructor, Digital Marketing With over 8 years of experience in Analytics, User Acquisition and Social Media, Katie joins the team as an instructor of Digital Marketing. She has also previously founded two startups in digital media and fashion technology. Inspired by creative entrepreneurs and innovative startups, Katie is excited to demystify digital marketing and helping students launch a career they love. She also happens to be a darn good baker! Lead Instructor, Head of Curriculum Mandi is one of the lead instructors for our immersive programs. Web developer by day (and usually at night too), Mandi specializes in custom WordPress plugin and theme development. Her background in content strategy and web writing has helped her develop a well-rounded approach to her current skill set. When she’s not creating structurally sound websites that work like a well-oiled machine, you can find her making use of a fleet of vintage cameras. In fact, nothing makes her quite as excited as the sound of a Polaroid SX-70 camera the moment it ejects a new photo. Lead Instructor, UX Designer Lindsay Henwood loves UX design. She has a diverse background – from University of Victoria to surf instruction and all points in between – but her empathetic nature and passion for design thinking led her to the field of UX over the last several years. A graduate of General Assembly’s UX Design Immersive program in Seattle, she has worked with companies like Shopify, Sitka, and Navicet to refine their products and presence. Her design sensibilities translate into her teaching, offering students clear insights into the practice of UX thinking and application. She gets excited about user research, affinity diagrams and usability testing, and she’ll jump at the chance to chat about UX – so feel free to reach out to her about it or swing by to meet in person. She also wouldn’t mind if you brought snacks along too. Instructor, UX Designer Robert is a people person and a person of the arts. From tiny start ups, to digital agencies to massive corporations, Robert brings 10 years design experience from a wide range of industries. Woven into those years is a wealth of experience and love of new media, visual and performance arts. Immensely social and outgoing, he has an equal love of working with people – be it helping, mentoring, teaching them or just having a good old conversation. But what puts him over the moon? Bringing those worlds together. Seeing the positive impact that comes of bringing art, design and people together is what Robert considers pure bliss. Instructor, UX Designer Lyndon is a highly experienced UX Designer originally from Melbourne, Australia. Over the past 7 years he’s worked with small and large scale clients across both hemispheres on projects ranging from websites, native apps and service based products. Currently working at Electronic Arts in Burnaby, he’s tasked with designing the next generation of web connected game experiences for EA and EA Sports titles. Lyndon is a huge advocate for applying good user centred design principles to every problem and is especially interested in natural interfaces and contextual application design. Academic Director As Academic Director of RED Academy, David has found a natural element for his passion of empowering people. He is making it his mission to ensure that students benefit from a dynamic, authentic and productive environment at RED by way of providing instructors with the tools to create engaging learning activities. Following over a decade of university-level teaching experience, David took on to develop himself as a trainer and as a coach. David holds a Ph.D. in theoretical mathematics, makes a different soup (almost) every Monday. He is originally from Switzerland and as a result, has a funny accent. Our unique learning programs have been developed by today’s industry professionals—many of whom work with Canada’s largest creative agencies and brands—all taught in small classes of no more than six students per instructor. Our students work on real-world projects that provide them with the tools and experience to succeed in today’s fast-paced digital environment. Our instructors work closely with a diverse group of hiring and community program partners to develop programs that challenge and excite our students. Each day they’re asked to create high-value digital work, not grind through monotonous text book exercises. It’s the kind of practical experience that sets our students apart and allows them to gain an edge in the competitive tech marketplace. We just hired one of your grads .. So thanks for that; also still in discussions with a second one for a slightly different role; so it may end up as two hires.  While we had a large turn out; the RED grads were definitely a cut above – so you can take that as a feather in your cap. Get in touch and we'll walk you through the rest.                              Powered By Drive Digital RED Academy Courses Full-Time Professional Programs – Digital Marketing &amp; Strategy – Web Developer – User Experience Designer Part-Time Foundation Programs – Digital Marketing Foundation – Web Developer Foundation – User Experience Design Foundation Part-Time Essentials Programs – AngularJS – Design Essentials About Meet The Team Become an Instructor Careers Submit A Student Project Hiring Partner Program Community Programs Blog Events Contact ​ 604​ ​674​ ​8332 View                                 Courses Attend Intro Session Full-Time Professional Part-Time Foundation Part-Time Essentials View                                         Courses UX Designer Professional                                                     Web Developer Professional                                                     Digital Marketing Professional                                                     View                                         Courses UX Designer Foundation                                                     Web Developer Foundation                                                     Digital Marketing Foundation                                                     View Courses AngularJS in Production                                                         Visual Designer Essentials                                                         Drive Digital Toggle navigation Dates 11 Apr - 30 Jun 11 Apr - 30 Jun 11 Apr - 30 Jun Dates 25 Jan - 1 Apr 25 Jan - 1 Apr 26 Jan - 1 Apr Dates 2 Feb - 11 Feb 1 Feb - 25 Feb Robert Robert Robert * * * Powered By Drive Digital</v>
-      </c>
-      <c r="D17" t="str">
-        <v>Vancouver Digital Marketing, Web Design &amp; Development Courses RED Academy is a unique Vancouver-based technology academy created for the designers, creators, developers and digital marketers of tomorrow. BC’s Leading Tech Academy Taught by the Industry, for the Industry. Professional Programs Evening Foundation Programs Evening Essentials Programs Meet Some of Our Instructors Real Projects, Real Learning. Interested in finding out more? Katie Jeanes Mandi Wise Lindsay Henwood Robert MacKie Lyndon Mayer David Kohler Some of Our Partners Contact Form Courses Full-Time Professional Programs  – Digital Marketing &amp; Strategy  – Web Developer  – User Experience Designer  Part-Time Foundation Programs  – Digital Marketing Foundation  – Web Developer Foundation  – User Experience Design Foundation  Part-Time Essentials Programs  – AngularJS  – Design Essentials   Full-Time Professional Programs – Digital Marketing &amp; Strategy – Web Developer – User Experience Designer Part-Time Foundation Programs – Digital Marketing Foundation – Web Developer Foundation – User Experience Design Foundation Part-Time Essentials Programs – AngularJS – Design Essentials About   Meet The Team  Become an Instructor  Careers  Submit A Student Project  Hiring Partner Program  Community Programs   Meet The Team Become an Instructor Careers Submit A Student Project Hiring Partner Program Community Programs Blog Events Contact ​ 604​ ​674​ ​8332 Full-Time Professional Part-Time Foundation Part-Time Essentials                                                                                                                             Professional Programs                                     Full Time Programs, 12 weeks immersive.                                     View                                         Courses                                                                                                                                                Course Name Dates                                                                                                                                      UX Designer Professional                                                                                                     11 Apr - 30 Jun                                                                                                                                                                                   Web Developer Professional                                                                                                     11 Apr - 30 Jun                                                                                                                                                                                   Digital Marketing Professional                                                                                                     11 Apr - 30 Jun                                                                                                                                                                                                                                                                                                                                                                   Evening Foundation Programs                                     Part Time Programs, two evenings per week for 10 weeks.                                     View                                         Courses                                                                                                                                                Course Name Dates                                                                                                                                      UX Designer Foundation                                                                                                     25 Jan - 1 Apr                                                                                                                                                                                   Web Developer Foundation                                                                                                     25 Jan - 1 Apr                                                                                                                                                                                   Digital Marketing Foundation                                                                                                     26 Jan - 1 Apr                                                                                                                                                                                                                                                                                                                                                                               Evening Essentials Programs                                     Part Time Programs, one evening per week for 5 weeks.                                         View Courses                                                                                                                                                                Course Name Dates                                                                                                                                                  AngularJS in Production                                                                                                             2 Feb - 11 Feb                                                                                                                                                                                                   Visual Designer Essentials                                                                                                             1 Feb - 25 Feb                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                          Katie Jeanes                                                 Instructor, Digital Marketing                                                 With over 8 years of experience in Analytics, User Acquisition and Social Media, Katie joins the team as an instructor of Digital Marketing. She has also previously founded two startups in digital media and fashion technology. Inspired by creative entrepreneurs and innovative startups, Katie is excited to demystify digital marketing and helping students launch a career they love. She also happens to be a darn good baker!                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                          Mandi Wise                                                 Lead Instructor, Head of Curriculum                                                 Mandi is one of the lead instructors for our immersive programs. Web developer by day (and usually at night too), Mandi specializes in custom WordPress plugin and theme development. Her background in content strategy and web writing has helped her develop a well-rounded approach to her current skill set. When she’s not creating structurally sound websites that work like a well-oiled machine, you can find her making use of a fleet of vintage cameras. In fact, nothing makes her quite as excited as the sound of a Polaroid SX-70 camera the moment it ejects a new photo.                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                          Lindsay Henwood                                                 Lead Instructor, UX Designer                                                 Lindsay Henwood loves UX design. She has a diverse background – from University of Victoria to surf instruction and all points in between – but her empathetic nature and passion for design thinking led her to the field of UX over the last several years. A graduate of General Assembly’s UX Design Immersive program in Seattle, she has worked with companies like Shopify, Sitka, and Navicet to refine their products and presence. Her design sensibilities translate into her teaching, offering students clear insights into the practice of UX thinking and application. She gets excited about user research, affinity diagrams and usability testing, and she’ll jump at the chance to chat about UX – so feel free to reach out to her about it or swing by to meet in person. She also wouldn’t mind if you brought snacks along too.                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                          Robert MacKie                                                 Instructor, UX Designer                                                 Robert is a people person and a person of the arts. From tiny start ups, to digital agencies to massive corporations, Robert brings 10 years design experience from a wide range of industries. Woven into those years is a wealth of experience and love of new media, visual and performance arts. Immensely social and outgoing, he has an equal love of working with people – be it helping, mentoring, teaching them or just having a good old conversation. But what puts him over the moon? Bringing those worlds together. Seeing the positive impact that comes of bringing art, design and people together is what Robert considers pure bliss.                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                          Lyndon Mayer                                                 Instructor, UX Designer                                                 Lyndon is a highly experienced UX Designer originally from Melbourne, Australia. Over the past 7 years he’s worked with small and large scale clients across both hemispheres on projects ranging from websites, native apps and service based products. Currently working at Electronic Arts in Burnaby, he’s tasked with designing the next generation of web connected game experiences for EA and EA Sports titles. Lyndon is a huge advocate for applying good user centred design principles to every problem and is especially interested in natural interfaces and contextual application design.                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                          David Kohler                                                 Academic Director                                                 As Academic Director of RED Academy, David has found a natural element for his passion of empowering people. He is making it his mission to ensure that students benefit from a dynamic, authentic and productive environment at RED by way of providing instructors with the tools to create engaging learning activities. Following over a decade of university-level teaching experience, David took on to develop himself as a trainer and as a coach. David holds a Ph.D. in theoretical mathematics, makes a different soup (almost) every Monday. He is originally from Switzerland and as a result, has a funny accent.                                                                                                                                                                                                                   Name* Email*                                                       Phone Message*                                         View                                 Courses                             Attend Intro Session                          RED Academy is a leading-edge technology school for the designers, creators, developers and digital marketers of tomorrow. We were born out of some of Western Canada’s leading digital agencies, and work closely with a network of industry partners to design highly engaging, immersive learning programs that give our students the right technical skills and knowledge to succeed in today’s rapidly evolving workplace. Learn to become a web developer - FT and PT programs. Learn to design user interfaces  - FT and PT programs. Engage, drive and measure traffic - FT and PT programs. Full Time Programs, 12 weeks immersive.                                                  UX Designer Professional                                                                                                     11 Apr - 30 Jun                                                                                               Web Developer Professional                                                                                                     11 Apr - 30 Jun                                                                                               Digital Marketing Professional                                                                                                     11 Apr - 30 Jun                                              Part Time Programs, two evenings per week for 10 weeks.                                                  UX Designer Foundation                                                                                                     25 Jan - 1 Apr                                                                                               Web Developer Foundation                                                                                                     25 Jan - 1 Apr                                                                                               Digital Marketing Foundation                                                                                                     26 Jan - 1 Apr                                              Part Time Programs, one evening per week for 5 weeks.                                                      AngularJS in Production                                                                                                             2 Feb - 11 Feb                                                                                                       Visual Designer Essentials                                                                                                             1 Feb - 25 Feb                                                  Instructor, Digital Marketing With over 8 years of experience in Analytics, User Acquisition and Social Media, Katie joins the team as an instructor of Digital Marketing. She has also previously founded two startups in digital media and fashion technology. Inspired by creative entrepreneurs and innovative startups, Katie is excited to demystify digital marketing and helping students launch a career they love. She also happens to be a darn good baker! Lead Instructor, Head of Curriculum Mandi is one of the lead instructors for our immersive programs. Web developer by day (and usually at night too), Mandi specializes in custom WordPress plugin and theme development. Her background in content strategy and web writing has helped her develop a well-rounded approach to her current skill set. When she’s not creating structurally sound websites that work like a well-oiled machine, you can find her making use of a fleet of vintage cameras. In fact, nothing makes her quite as excited as the sound of a Polaroid SX-70 camera the moment it ejects a new photo. Lead Instructor, UX Designer Lindsay Henwood loves UX design. She has a diverse background – from University of Victoria to surf instruction and all points in between – but her empathetic nature and passion for design thinking led her to the field of UX over the last several years. A graduate of General Assembly’s UX Design Immersive program in Seattle, she has worked with companies like Shopify, Sitka, and Navicet to refine their products and presence. Her design sensibilities translate into her teaching, offering students clear insights into the practice of UX thinking and application. She gets excited about user research, affinity diagrams and usability testing, and she’ll jump at the chance to chat about UX – so feel free to reach out to her about it or swing by to meet in person. She also wouldn’t mind if you brought snacks along too. Instructor, UX Designer Robert is a people person and a person of the arts. From tiny start ups, to digital agencies to massive corporations, Robert brings 10 years design experience from a wide range of industries. Woven into those years is a wealth of experience and love of new media, visual and performance arts. Immensely social and outgoing, he has an equal love of working with people – be it helping, mentoring, teaching them or just having a good old conversation. But what puts him over the moon? Bringing those worlds together. Seeing the positive impact that comes of bringing art, design and people together is what Robert considers pure bliss. Instructor, UX Designer Lyndon is a highly experienced UX Designer originally from Melbourne, Australia. Over the past 7 years he’s worked with small and large scale clients across both hemispheres on projects ranging from websites, native apps and service based products. Currently working at Electronic Arts in Burnaby, he’s tasked with designing the next generation of web connected game experiences for EA and EA Sports titles. Lyndon is a huge advocate for applying good user centred design principles to every problem and is especially interested in natural interfaces and contextual application design. Academic Director As Academic Director of RED Academy, David has found a natural element for his passion of empowering people. He is making it his mission to ensure that students benefit from a dynamic, authentic and productive environment at RED by way of providing instructors with the tools to create engaging learning activities. Following over a decade of university-level teaching experience, David took on to develop himself as a trainer and as a coach. David holds a Ph.D. in theoretical mathematics, makes a different soup (almost) every Monday. He is originally from Switzerland and as a result, has a funny accent. Our unique learning programs have been developed by today’s industry professionals—many of whom work with Canada’s largest creative agencies and brands—all taught in small classes of no more than six students per instructor. Our students work on real-world projects that provide them with the tools and experience to succeed in today’s fast-paced digital environment. Our instructors work closely with a diverse group of hiring and community program partners to develop programs that challenge and excite our students. Each day they’re asked to create high-value digital work, not grind through monotonous text book exercises. It’s the kind of practical experience that sets our students apart and allows them to gain an edge in the competitive tech marketplace. We just hired one of your grads .. So thanks for that; also still in discussions with a second one for a slightly different role; so it may end up as two hires.  While we had a large turn out; the RED grads were definitely a cut above – so you can take that as a feather in your cap. Get in touch and we'll walk you through the rest.                              Powered By Drive Digital RED Academy Courses Full-Time Professional Programs – Digital Marketing &amp; Strategy – Web Developer – User Experience Designer Part-Time Foundation Programs – Digital Marketing Foundation – Web Developer Foundation – User Experience Design Foundation Part-Time Essentials Programs – AngularJS – Design Essentials About Meet The Team Become an Instructor Careers Submit A Student Project Hiring Partner Program Community Programs Blog Events Contact ​ 604​ ​674​ ​8332 View                                 Courses Attend Intro Session Full-Time Professional Part-Time Foundation Part-Time Essentials View                                         Courses UX Designer Professional                                                     Web Developer Professional                                                     Digital Marketing Professional                                                     View                                         Courses UX Designer Foundation                                                     Web Developer Foundation                                                     Digital Marketing Foundation                                                     View Courses AngularJS in Production                                                         Visual Designer Essentials                                                         Drive Digital Toggle navigation Dates 11 Apr - 30 Jun 11 Apr - 30 Jun 11 Apr - 30 Jun Dates 25 Jan - 1 Apr 25 Jan - 1 Apr 26 Jan - 1 Apr Dates 2 Feb - 11 Feb 1 Feb - 25 Feb Robert Robert Robert * * * Powered By Drive Digital</v>
-      </c>
-      <c r="E17" t="str">
-        <v>Vancouver Digital Marketing, Web Design &amp; Development Courses RED Academy is a unique Vancouver-based technology academy created for the designers, creators, developers and digital marketers of tomorrow. BC’s Leading Tech Academy Taught by the Industry, for the Industry. Professional Programs Evening Foundation Programs Evening Essentials Programs Meet Some of Our Instructors Real Projects, Real Learning. Interested in finding out more? Katie Jeanes Mandi Wise Lindsay Henwood Robert MacKie Lyndon Mayer David Kohler Some of Our Partners Contact Form Courses Full-Time Professional Programs  – Digital Marketing &amp; Strategy  – Web Developer  – User Experience Designer  Part-Time Foundation Programs  – Digital Marketing Foundation  – Web Developer Foundation  – User Experience Design Foundation  Part-Time Essentials Programs  – AngularJS  – Design Essentials   Full-Time Professional Programs – Digital Marketing &amp; Strategy – Web Developer – User Experience Designer Part-Time Foundation Programs – Digital Marketing Foundation – Web Developer Foundation – User Experience Design Foundation Part-Time Essentials Programs – AngularJS – Design Essentials About   Meet The Team  Become an Instructor  Careers  Submit A Student Project  Hiring Partner Program  Community Programs   Meet The Team Become an Instructor Careers Submit A Student Project Hiring Partner Program Community Programs Blog Events Contact ​ 604​ ​674​ ​8332 Full-Time Professional Part-Time Foundation Part-Time Essentials                                                                                                                             Professional Programs                                     Full Time Programs, 12 weeks immersive.                                     View                                         Courses                                                                                                                                                Course Name Dates                                                                                                                                      UX Designer Professional                                                                                                     11 Apr - 30 Jun                                                                                                                                                                                   Web Developer Professional                                                                                                     11 Apr - 30 Jun                                                                                                                                                                                   Digital Marketing Professional                                                                                                     11 Apr - 30 Jun                                                                                                                                                                                                                                                                                                                                                                   Evening Foundation Programs                                     Part Time Programs, two evenings per week for 10 weeks.                                     View                                         Courses                                                                                                                                                Course Name Dates                                                                                                                                      UX Designer Foundation                                                                                                     25 Jan - 1 Apr                                                                                                                                                                                   Web Developer Foundation                                                                                                     25 Jan - 1 Apr                                                                                                                                                                                   Digital Marketing Foundation                                                                                                     26 Jan - 1 Apr                                                                                                                                                                                                                                                                                                                                                                               Evening Essentials Programs                                     Part Time Programs, one evening per week for 5 weeks.                                         View Courses                                                                                                                                                                Course Name Dates                                                                                                                                                  AngularJS in Production                                                                                                             2 Feb - 11 Feb                                                                                                                                                                                                   Visual Designer Essentials                                                                                                             1 Feb - 25 Feb                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                          Katie Jeanes                                                 Instructor, Digital Marketing                                                 With over 8 years of experience in Analytics, User Acquisition and Social Media, Katie joins the team as an instructor of Digital Marketing. She has also previously founded two startups in digital media and fashion technology. Inspired by creative entrepreneurs and innovative startups, Katie is excited to demystify digital marketing and helping students launch a career they love. She also happens to be a darn good baker!                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                          Mandi Wise                                                 Lead Instructor, Head of Curriculum                                                 Mandi is one of the lead instructors for our immersive programs. Web developer by day (and usually at night too), Mandi specializes in custom WordPress plugin and theme development. Her background in content strategy and web writing has helped her develop a well-rounded approach to her current skill set. When she’s not creating structurally sound websites that work like a well-oiled machine, you can find her making use of a fleet of vintage cameras. In fact, nothing makes her quite as excited as the sound of a Polaroid SX-70 camera the moment it ejects a new photo.                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                          Lindsay Henwood                                                 Lead Instructor, UX Designer                                                 Lindsay Henwood loves UX design. She has a diverse background – from University of Victoria to surf instruction and all points in between – but her empathetic nature and passion for design thinking led her to the field of UX over the last several years. A graduate of General Assembly’s UX Design Immersive program in Seattle, she has worked with companies like Shopify, Sitka, and Navicet to refine their products and presence. Her design sensibilities translate into her teaching, offering students clear insights into the practice of UX thinking and application. She gets excited about user research, affinity diagrams and usability testing, and she’ll jump at the chance to chat about UX – so feel free to reach out to her about it or swing by to meet in person. She also wouldn’t mind if you brought snacks along too.                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                          Robert MacKie                                                 Instructor, UX Designer                                                 Robert is a people person and a person of the arts. From tiny start ups, to digital agencies to massive corporations, Robert brings 10 years design experience from a wide range of industries. Woven into those years is a wealth of experience and love of new media, visual and performance arts. Immensely social and outgoing, he has an equal love of working with people – be it helping, mentoring, teaching them or just having a good old conversation. But what puts him over the moon? Bringing those worlds together. Seeing the positive impact that comes of bringing art, design and people together is what Robert considers pure bliss.                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                          Lyndon Mayer                                                 Instructor, UX Designer                                                 Lyndon is a highly experienced UX Designer originally from Melbourne, Australia. Over the past 7 years he’s worked with small and large scale clients across both hemispheres on projects ranging from websites, native apps and service based products. Currently working at Electronic Arts in Burnaby, he’s tasked with designing the next generation of web connected game experiences for EA and EA Sports titles. Lyndon is a huge advocate for applying good user centred design principles to every problem and is especially interested in natural interfaces and contextual application design.                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                          David Kohler                                                 Academic Director                                                 As Academic Director of RED Academy, David has found a natural element for his passion of empowering people. He is making it his mission to ensure that students benefit from a dynamic, authentic and productive environment at RED by way of providing instructors with the tools to create engaging learning activities. Following over a decade of university-level teaching experience, David took on to develop himself as a trainer and as a coach. David holds a Ph.D. in theoretical mathematics, makes a different soup (almost) every Monday. He is originally from Switzerland and as a result, has a funny accent.                                                                                                                                                                                                                   Name* Email*                                                       Phone Message*                                         View                                 Courses                             Attend Intro Session                          RED Academy is a leading-edge technology school for the designers, creators, developers and digital marketers of tomorrow. We were born out of some of Western Canada’s leading digital agencies, and work closely with a network of industry partners to design highly engaging, immersive learning programs that give our students the right technical skills and knowledge to succeed in today’s rapidly evolving workplace. Learn to become a web developer - FT and PT programs. Learn to design user interfaces  - FT and PT programs. Engage, drive and measure traffic - FT and PT programs. Full Time Programs, 12 weeks immersive.                                                  UX Designer Professional                                                                                                     11 Apr - 30 Jun                                                                                               Web Developer Professional                                                                                                     11 Apr - 30 Jun                                                                                               Digital Marketing Professional                                                                                                     11 Apr - 30 Jun                                              Part Time Programs, two evenings per week for 10 weeks.                                                  UX Designer Foundation                                                                                                     25 Jan - 1 Apr                                                                                               Web Developer Foundation                                                                                                     25 Jan - 1 Apr                                                                                               Digital Marketing Foundation                                                                                                     26 Jan - 1 Apr                                              Part Time Programs, one evening per week for 5 weeks.                                                      AngularJS in Production                                                                                                             2 Feb - 11 Feb                                                                                                       Visual Designer Essentials                                                                                                             1 Feb - 25 Feb                                                  Instructor, Digital Marketing With over 8 years of experience in Analytics, User Acquisition and Social Media, Katie joins the team as an instructor of Digital Marketing. She has also previously founded two startups in digital media and fashion technology. Inspired by creative entrepreneurs and innovative startups, Katie is excited to demystify digital marketing and helping students launch a career they love. She also happens to be a darn good baker! Lead Instructor, Head of Curriculum Mandi is one of the lead instructors for our immersive programs. Web developer by day (and usually at night too), Mandi specializes in custom WordPress plugin and theme development. Her background in content strategy and web writing has helped her develop a well-rounded approach to her current skill set. When she’s not creating structurally sound websites that work like a well-oiled machine, you can find her making use of a fleet of vintage cameras. In fact, nothing makes her quite as excited as the sound of a Polaroid SX-70 camera the moment it ejects a new photo. Lead Instructor, UX Designer Lindsay Henwood loves UX design. She has a diverse background – from University of Victoria to surf instruction and all points in between – but her empathetic nature and passion for design thinking led her to the field of UX over the last several years. A graduate of General Assembly’s UX Design Immersive program in Seattle, she has worked with companies like Shopify, Sitka, and Navicet to refine their products and presence. Her design sensibilities translate into her teaching, offering students clear insights into the practice of UX thinking and application. She gets excited about user research, affinity diagrams and usability testing, and she’ll jump at the chance to chat about UX – so feel free to reach out to her about it or swing by to meet in person. She also wouldn’t mind if you brought snacks along too. Instructor, UX Designer Robert is a people person and a person of the arts. From tiny start ups, to digital agencies to massive corporations, Robert brings 10 years design experience from a wide range of industries. Woven into those years is a wealth of experience and love of new media, visual and performance arts. Immensely social and outgoing, he has an equal love of working with people – be it helping, mentoring, teaching them or just having a good old conversation. But what puts him over the moon? Bringing those worlds together. Seeing the positive impact that comes of bringing art, design and people together is what Robert considers pure bliss. Instructor, UX Designer Lyndon is a highly experienced UX Designer originally from Melbourne, Australia. Over the past 7 years he’s worked with small and large scale clients across both hemispheres on projects ranging from websites, native apps and service based products. Currently working at Electronic Arts in Burnaby, he’s tasked with designing the next generation of web connected game experiences for EA and EA Sports titles. Lyndon is a huge advocate for applying good user centred design principles to every problem and is especially interested in natural interfaces and contextual application design. Academic Director As Academic Director of RED Academy, David has found a natural element for his passion of empowering people. He is making it his mission to ensure that students benefit from a dynamic, authentic and productive environment at RED by way of providing instructors with the tools to create engaging learning activities. Following over a decade of university-level teaching experience, David took on to develop himself as a trainer and as a coach. David holds a Ph.D. in theoretical mathematics, makes a different soup (almost) every Monday. He is originally from Switzerland and as a result, has a funny accent. Our unique learning programs have been developed by today’s industry professionals—many of whom work with Canada’s largest creative agencies and brands—all taught in small classes of no more than six students per instructor. Our students work on real-world projects that provide them with the tools and experience to succeed in today’s fast-paced digital environment. Our instructors work closely with a diverse group of hiring and community program partners to develop programs that challenge and excite our students. Each day they’re asked to create high-value digital work, not grind through monotonous text book exercises. It’s the kind of practical experience that sets our students apart and allows them to gain an edge in the competitive tech marketplace. We just hired one of your grads .. So thanks for that; also still in discussions with a second one for a slightly different role; so it may end up as two hires.  While we had a large turn out; the RED grads were definitely a cut above – so you can take that as a feather in your cap. Get in touch and we'll walk you through the rest.                              Powered By Drive Digital RED Academy Courses Full-Time Professional Programs – Digital Marketing &amp; Strategy – Web Developer – User Experience Designer Part-Time Foundation Programs – Digital Marketing Foundation – Web Developer Foundation – User Experience Design Foundation Part-Time Essentials Programs – AngularJS – Design Essentials About Meet The Team Become an Instructor Careers Submit A Student Project Hiring Partner Program Community Programs Blog Events Contact ​ 604​ ​674​ ​8332 View                                 Courses Attend Intro Session Full-Time Professional Part-Time Foundation Part-Time Essentials View                                         Courses UX Designer Professional                                                     Web Developer Professional                                                     Digital Marketing Professional                                                     View                                         Courses UX Designer Foundation                                                     Web Developer Foundation                                                     Digital Marketing Foundation                                                     View Courses AngularJS in Production                                                         Visual Designer Essentials                                                         Drive Digital Toggle navigation Dates 11 Apr - 30 Jun 11 Apr - 30 Jun 11 Apr - 30 Jun Dates 25 Jan - 1 Apr 25 Jan - 1 Apr 26 Jan - 1 Apr Dates 2 Feb - 11 Feb 1 Feb - 25 Feb Robert Robert Robert * * * Powered By Drive Digital</v>
-      </c>
-      <c r="F17" t="str">
-        <v>Vancouver Digital Marketing, Web Design &amp; Development Courses RED Academy is a unique Vancouver-based technology academy created for the designers, creators, developers and digital marketers of tomorrow. BC’s Leading Tech Academy Taught by the Industry, for the Industry. Professional Programs Evening Foundation Programs Evening Essentials Programs Meet Some of Our Instructors Real Projects, Real Learning. Interested in finding out more? Katie Jeanes Mandi Wise Lindsay Henwood Robert MacKie Lyndon Mayer David Kohler Some of Our Partners Contact Form Courses Full-Time Professional Programs  – Digital Marketing &amp; Strategy  – Web Developer  – User Experience Designer  Part-Time Foundation Programs  – Digital Marketing Foundation  – Web Developer Foundation  – User Experience Design Foundation  Part-Time Essentials Programs  – AngularJS  – Design Essentials   Full-Time Professional Programs – Digital Marketing &amp; Strategy – Web Developer – User Experience Designer Part-Time Foundation Programs – Digital Marketing Foundation – Web Developer Foundation – User Experience Design Foundation Part-Time Essentials Programs – AngularJS – Design Essentials About   Meet The Team  Become an Instructor  Careers  Submit A Student Project  Hiring Partner Program  Community Programs   Meet The Team Become an Instructor Careers Submit A Student Project Hiring Partner Program Community Programs Blog Events Contact ​ 604​ ​674​ ​8332 Full-Time Professional Part-Time Foundation Part-Time Essentials                                                                                                                             Professional Programs                                     Full Time Programs, 12 weeks immersive.                                     View                                         Courses                                                                                                                                                Course Name Dates                                                                                                                                      UX Designer Professional                                                                                                     11 Apr - 30 Jun                                                                                                                                                                                   Web Developer Professional                                                                                                     11 Apr - 30 Jun                                                                                                                                                                                   Digital Marketing Professional                                                                                                     11 Apr - 30 Jun                                                                                                                                                                                                                                                                                                                                                                   Evening Foundation Programs                                     Part Time Programs, two evenings per week for 10 weeks.                                     View                                         Courses                                                                                                                                                Course Name Dates                                                                                                                                      UX Designer Foundation                                                                                                     25 Jan - 1 Apr                                                                                                                                                                                   Web Developer Foundation                                                                                                     25 Jan - 1 Apr                                                                                                                                                                                   Digital Marketing Foundation                                                                                                     26 Jan - 1 Apr                                                                                                                                                                                                                                                                                                                                                                               Evening Essentials Programs                                     Part Time Programs, one evening per week for 5 weeks.                                         View Courses                                                                                                                                                                Course Name Dates                                                                                                                                                  AngularJS in Production                                                                                                             2 Feb - 11 Feb                                                                                                                                                                                                   Visual Designer Essentials                                                                                                             1 Feb - 25 Feb                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                          Katie Jeanes                                                 Instructor, Digital Marketing                                                 With over 8 years of experience in Analytics, User Acquisition and Social Media, Katie joins the team as an instructor of Digital Marketing. She has also previously founded two startups in digital media and fashion technology. Inspired by creative entrepreneurs and innovative startups, Katie is excited to demystify digital marketing and helping students launch a career they love. She also happens to be a darn good baker!                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                          Mandi Wise                                                 Lead Instructor, Head of Curriculum                                                 Mandi is one of the lead instructors for our immersive programs. Web developer by day (and usually at night too), Mandi specializes in custom WordPress plugin and theme development. Her background in content strategy and web writing has helped her develop a well-rounded approach to her current skill set. When she’s not creating structurally sound websites that work like a well-oiled machine, you can find her making use of a fleet of vintage cameras. In fact, nothing makes her quite as excited as the sound of a Polaroid SX-70 camera the moment it ejects a new photo.                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                          Lindsay Henwood                                                 Lead Instructor, UX Designer                                                 Lindsay Henwood loves UX design. She has a diverse background – from University of Victoria to surf instruction and all points in between – but her empathetic nature and passion for design thinking led her to the field of UX over the last several years. A graduate of General Assembly’s UX Design Immersive program in Seattle, she has worked with companies like Shopify, Sitka, and Navicet to refine their products and presence. Her design sensibilities translate into her teaching, offering students clear insights into the practice of UX thinking and application. She gets excited about user research, affinity diagrams and usability testing, and she’ll jump at the chance to chat about UX – so feel free to reach out to her about it or swing by to meet in person. She also wouldn’t mind if you brought snacks along too.                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                          Robert MacKie                                                 Instructor, UX Designer                                                 Robert is a people person and a person of the arts. From tiny start ups, to digital agencies to massive corporations, Robert brings 10 years design experience from a wide range of industries. Woven into those years is a wealth of experience and love of new media, visual and performance arts. Immensely social and outgoing, he has an equal love of working with people – be it helping, mentoring, teaching them or just having a good old conversation. But what puts him over the moon? Bringing those worlds together. Seeing the positive impact that comes of bringing art, design and people together is what Robert considers pure bliss.                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                          Lyndon Mayer                                                 Instructor, UX Designer                                                 Lyndon is a highly experienced UX Designer originally from Melbourne, Australia. Over the past 7 years he’s worked with small and large scale clients across both hemispheres on projects ranging from websites, native apps and service based products. Currently working at Electronic Arts in Burnaby, he’s tasked with designing the next generation of web connected game experiences for EA and EA Sports titles. Lyndon is a huge advocate for applying good user centred design principles to every problem and is especially interested in natural interfaces and contextual application design.                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                          David Kohler                                                 Academic Director                                                 As Academic Director of RED Academy, David has found a natural element for his passion of empowering people. He is making it his mission to ensure that students benefit from a dynamic, authentic and productive environment at RED by way of providing instructors with the tools to create engaging learning activities. Following over a decade of university-level teaching experience, David took on to develop himself as a trainer and as a coach. David holds a Ph.D. in theoretical mathematics, makes a different soup (almost) every Monday. He is originally from Switzerland and as a result, has a funny accent.                                                                                                                                                                                                                   Name* Email*                                                       Phone Message*                                         View                                 Courses                             Attend Intro Session                          RED Academy is a leading-edge technology school for the designers, creators, developers and digital marketers of tomorrow. We were born out of some of Western Canada’s leading digital agencies, and work closely with a network of industry partners to design highly engaging, immersive learning programs that give our students the right technical skills and knowledge to succeed in today’s rapidly evolving workplace. Learn to become a web developer - FT and PT programs. Learn to design user interfaces  - FT and PT programs. Engage, drive and measure traffic - FT and PT programs. Full Time Programs, 12 weeks immersive.                                                  UX Designer Professional                                                                                                     11 Apr - 30 Jun                                                                                               Web Developer Professional                                                                                                     11 Apr - 30 Jun                                                                                               Digital Marketing Professional                                                                                                     11 Apr - 30 Jun                                              Part Time Programs, two evenings per week for 10 weeks.                                                  UX Designer Foundation                                                                                                     25 Jan - 1 Apr                                                                                               Web Developer Foundation                                                                                                     25 Jan - 1 Apr                                                                                               Digital Marketing Foundation                                                                                                     26 Jan - 1 Apr                                              Part Time Programs, one evening per week for 5 weeks.                                                      AngularJS in Production                                                                                                             2 Feb - 11 Feb                                                                                                       Visual Designer Essentials                                                                                                             1 Feb - 25 Feb                                                  Instructor, Digital Marketing With over 8 years of experience in Analytics, User Acquisition and Social Media, Katie joins the team as an instructor of Digital Marketing. She has also previously founded two startups in digital media and fashion technology. Inspired by creative entrepreneurs and innovative startups, Katie is excited to demystify digital marketing and helping students launch a career they love. She also happens to be a darn good baker! Lead Instructor, Head of Curriculum Mandi is one of the lead instructors for our immersive programs. Web developer by day (and usually at night too), Mandi specializes in custom WordPress plugin and theme development. Her background in content strategy and web writing has helped her develop a well-rounded approach to her current skill set. When she’s not creating structurally sound websites that work like a well-oiled machine, you can find her making use of a fleet of vintage cameras. In fact, nothing makes her quite as excited as the sound of a Polaroid SX-70 camera the moment it ejects a new photo. Lead Instructor, UX Designer Lindsay Henwood loves UX design. She has a diverse background – from University of Victoria to surf instruction and all points in between – but her empathetic nature and passion for design thinking led her to the field of UX over the last several years. A graduate of General Assembly’s UX Design Immersive program in Seattle, she has worked with companies like Shopify, Sitka, and Navicet to refine their products and presence. Her design sensibilities translate into her teaching, offering students clear insights into the practice of UX thinking and application. She gets excited about user research, affinity diagrams and usability testing, and she’ll jump at the chance to chat about UX – so feel free to reach out to her about it or swing by to meet in person. She also wouldn’t mind if you brought snacks along too. Instructor, UX Designer Robert is a people person and a person of the arts. From tiny start ups, to digital agencies to massive corporations, Robert brings 10 years design experience from a wide range of industries. Woven into those years is a wealth of experience and love of new media, visual and performance arts. Immensely social and outgoing, he has an equal love of working with people – be it helping, mentoring, teaching them or just having a good old conversation. But what puts him over the moon? Bringing those worlds together. Seeing the positive impact that comes of bringing art, design and people together is what Robert considers pure bliss. Instructor, UX Designer Lyndon is a highly experienced UX Designer originally from Melbourne, Australia. Over the past 7 years he’s worked with small and large scale clients across both hemispheres on projects ranging from websites, native apps and service based products. Currently working at Electronic Arts in Burnaby, he’s tasked with designing the next generation of web connected game experiences for EA and EA Sports titles. Lyndon is a huge advocate for applying good user centred design principles to every problem and is especially interested in natural interfaces and contextual application design. Academic Director As Academic Director of RED Academy, David has found a natural element for his passion of empowering people. He is making it his mission to ensure that students benefit from a dynamic, authentic and productive environment at RED by way of providing instructors with the tools to create engaging learning activities. Following over a decade of university-level teaching experience, David took on to develop himself as a trainer and as a coach. David holds a Ph.D. in theoretical mathematics, makes a different soup (almost) every Monday. He is originally from Switzerland and as a result, has a funny accent. Our unique learning programs have been developed by today’s industry professionals—many of whom work with Canada’s largest creative agencies and brands—all taught in small classes of no more than six students per instructor. Our students work on real-world projects that provide them with the tools and experience to succeed in today’s fast-paced digital environment. Our instructors work closely with a diverse group of hiring and community program partners to develop programs that challenge and excite our students. Each day they’re asked to create high-value digital work, not grind through monotonous text book exercises. It’s the kind of practical experience that sets our students apart and allows them to gain an edge in the competitive tech marketplace. We just hired one of your grads .. So thanks for that; also still in discussions with a second one for a slightly different role; so it may end up as two hires.  While we had a large turn out; the RED grads were definitely a cut above – so you can take that as a feather in your cap. Get in touch and we'll walk you through the rest.                              Powered By Drive Digital RED Academy Courses Full-Time Professional Programs – Digital Marketing &amp; Strategy – Web Developer – User Experience Designer Part-Time Foundation Programs – Digital Marketing Foundation – Web Developer Foundation – User Experience Design Foundation Part-Time Essentials Programs – AngularJS – Design Essentials About Meet The Team Become an Instructor Careers Submit A Student Project Hiring Partner Program Community Programs Blog Events Contact ​ 604​ ​674​ ​8332 View                                 Courses Attend Intro Session Full-Time Professional Part-Time Foundation Part-Time Essentials View                                         Courses UX Designer Professional                                                     Web Developer Professional                                                     Digital Marketing Professional                                                     View                                         Courses UX Designer Foundation                                                     Web Developer Foundation                                                     Digital Marketing Foundation                                                     View Courses AngularJS in Production                                                         Visual Designer Essentials                                                         Drive Digital Toggle navigation Dates 11 Apr - 30 Jun 11 Apr - 30 Jun 11 Apr - 30 Jun Dates 25 Jan - 1 Apr 25 Jan - 1 Apr 26 Jan - 1 Apr Dates 2 Feb - 11 Feb 1 Feb - 25 Feb Robert Robert Robert * * * Powered By Drive Digital</v>
+        <v>Vancouver Digital Marketing Web Design Development Courses RED Academy is a unique Vancouverbased technology academy created for the designers creators developers and digital marketers of tomorrow BC’s Leading Tech Academy Taught by the Industry for the Industry Professional Programs Evening Foundation Programs Evening Essentials Programs Meet Some of Our Instructors Real Projects Real Learning Interested in finding out more Katie Jeanes Mandi Wise Lindsay Henwood Robert MacKie Lyndon Mayer David Kohler Some of Our Partners Contact Form Courses FullTime Professional Programs Digital Marketing Strategy Web Developer User Experience Designer PartTime Foundation Programs Digital Marketing Foundation Web Developer Foundation User Experience Design Foundation PartTime Essentials Programs AngularJS Design Essentials FullTime Professional Programs Digital Marketing Strategy Web Developer User Experience Designer PartTime Foundation Programs Digital Marketing Foundation Web Developer Foundation User Experience Design Foundation PartTime Essentials Programs AngularJS Design Essentials About Meet The Team Become an Instructor Careers Submit A Student Project Hiring Partner Program Community Programs Meet The Team Become an Instructor Careers Submit A Student Project Hiring Partner Program Community Programs Blog Events Contact ​ 604​ ​674​ ​8332 FullTime Professional PartTime Foundation PartTime Essentials Professional Programs Full Time Programs 12 weeks immersive View Courses Course Name Dates UX Designer Professional 11 Apr 30 Jun Web Developer Professional 11 Apr 30 Jun Digital Marketing Professional 11 Apr 30 Jun Evening Foundation Programs Part Time Programs two evenings per week for 10 weeks View Courses Course Name Dates UX Designer Foundation 25 Jan 1 Apr Web Developer Foundation 25 Jan 1 Apr Digital Marketing Foundation 26 Jan 1 Apr Evening Essentials Programs Part Time Programs one evening per week for 5 weeks View Courses Course Name Dates AngularJS in Production 2 Feb 11 Feb Visual Designer Essentials 1 Feb 25 Feb Katie Jeanes Instructor Digital Marketing With over 8 years of experience in Analytics User Acquisition and Social Media Katie joins the team as an instructor of Digital Marketing She has also previously founded two startups in digital media and fashion technology Inspired by creative entrepreneurs and innovative startups Katie is excited to demystify digital marketing and helping students launch a career they love She also happens to be a darn good baker Mandi Wise Lead Instructor Head of Curriculum Mandi is one of the lead instructors for our immersive programs Web developer by day and usually at night too Mandi specializes in custom WordPress plugin and theme development Her background in content strategy and web writing has helped her develop a wellrounded approach to her current skill set When she’s not creating structurally sound websites that work like a welloiled machine you can find her making use of a fleet of vintage cameras In fact nothing makes her quite as excited as the sound of a Polaroid SX70 camera the moment it ejects a new photo Lindsay Henwood Lead Instructor UX Designer Lindsay Henwood loves UX design She has a diverse background from University of Victoria to surf instruction and all points in between but her empathetic nature and passion for design thinking led her to the field of UX over the last several years A graduate of General Assembly’s UX Design Immersive program in Seattle she has worked with companies like Shopify Sitka and Navicet to refine their products and presence Her design sensibilities translate into her teaching offering students clear insights into the practice of UX thinking and application She gets excited about user research affinity diagrams and usability testing and she’ll jump at the chance to chat about UX so feel free to reach out to her about it or swing by to meet in person She also wouldn’t mind if you brought snacks along too Robert MacKie Instructor UX Designer Robert is a people person and a person of the arts From tiny start ups to digital agencies to massive corporations Robert brings 10 years design experience from a wide range of industries Woven into those years is a wealth of experience and love of new media visual and performance arts Immensely social and outgoing he has an equal love of working with people be it helping mentoring teaching them or just having a good old conversation But what puts him over the moon Bringing those worlds together Seeing the positive impact that comes of bringing art design and people together is what Robert considers pure bliss Lyndon Mayer Instructor UX Designer Lyndon is a highly experienced UX Designer originally from Melbourne Australia Over the past 7 years he’s worked with small and large scale clients across both hemispheres on projects ranging from websites native apps and service based products Currently working at Electronic Arts in Burnaby he’s tasked with designing the next generation of web connected game experiences for EA and EA Sports titles Lyndon is a huge advocate for applying good user centred design principles to every problem and is especially interested in natural interfaces and contextual application design David Kohler Academic Director As Academic Director of RED Academy David has found a natural element for his passion of empowering people He is making it his mission to ensure that students benefit from a dynamic authentic and productive environment at RED by way of providing instructors with the tools to create engaging learning activities Following over a decade of universitylevel teaching experience David took on to develop himself as a trainer and as a coach David holds a PhD in theoretical mathematics makes a different soup almost every Monday He is originally from Switzerland and as a result has a funny accent Name Email Phone Message View Courses Attend Intro Session RED Academy is a leadingedge technology school for the designers creators developers and digital marketers of tomorrow We were born out of some of Western Canada’s leading digital agencies and work closely with a network of industry partners to design highly engaging immersive learning programs that give our students the right technical skills and knowledge to succeed in today’s rapidly evolving workplace Learn to become a web developer FT and PT programs Learn to design user interfaces FT and PT programs Engage drive and measure traffic FT and PT programs Full Time Programs 12 weeks immersive UX Designer Professional 11 Apr 30 Jun Web Developer Professional 11 Apr 30 Jun Digital Marketing Professional 11 Apr 30 Jun Part Time Programs two evenings per week for 10 weeks UX Designer Foundation 25 Jan 1 Apr Web Developer Foundation 25 Jan 1 Apr Digital Marketing Foundation 26 Jan 1 Apr Part Time Programs one evening per week for 5 weeks AngularJS in Production 2 Feb 11 Feb Visual Designer Essentials 1 Feb 25 Feb Instructor Digital Marketing With over 8 years of experience in Analytics User Acquisition and Social Media Katie joins the team as an instructor of Digital Marketing She has also previously founded two startups in digital media and fashion technology Inspired by creative entrepreneurs and innovative startups Katie is excited to demystify digital marketing and helping students launch a career they love She also happens to be a darn good baker Lead Instructor Head of Curriculum Mandi is one of the lead instructors for our immersive programs Web developer by day and usually at night too Mandi specializes in custom WordPress plugin and theme development Her background in content strategy and web writing has helped her develop a wellrounded approach to her current skill set When she’s not creating structurally sound websites that work like a welloiled machine you can find her making use of a fleet of vintage cameras In fact nothing makes her quite as excited as the sound of a Polaroid SX70 camera the moment it ejects a new photo Lead Instructor UX Designer Lindsay Henwood loves UX design She has a diverse background from University of Victoria to surf instruction and all points in between but her empathetic nature and passion for design thinking led her to the field of UX over the last several years A graduate of General Assembly’s UX Design Immersive program in Seattle she has worked with companies like Shopify Sitka and Navicet to refine their products and presence Her design sensibilities translate into her teaching offering students clear insights into the practice of UX thinking and application She gets excited about user research affinity diagrams and usability testing and she’ll jump at the chance to chat about UX so feel free to reach out to her about it or swing by to meet in person She also wouldn’t mind if you brought snacks along too Instructor UX Designer Robert is a people person and a person of the arts From tiny start ups to digital agencies to massive corporations Robert brings 10 years design experience from a wide range of industries Woven into those years is a wealth of experience and love of new media visual and performance arts Immensely social and outgoing he has an equal love of working with people be it helping mentoring teaching them or just having a good old conversation But what puts him over the moon Bringing those worlds together Seeing the positive impact that comes of bringing art design and people together is what Robert considers pure bliss Instructor UX Designer Lyndon is a highly experienced UX Designer originally from Melbourne Australia Over the past 7 years he’s worked with small and large scale clients across both hemispheres on projects ranging from websites native apps and service based products Currently working at Electronic Arts in Burnaby he’s tasked with designing the next generation of web connected game experiences for EA and EA Sports titles Lyndon is a huge advocate for applying good user centred design principles to every problem and is especially interested in natural interfaces and contextual application design Academic Director As Academic Director of RED Academy David has found a natural element for his passion of empowering people He is making it his mission to ensure that students benefit from a dynamic authentic and productive environment at RED by way of providing instructors with the tools to create engaging learning activities Following over a decade of universitylevel teaching experience David took on to develop himself as a trainer and as a coach David holds a PhD in theoretical mathematics makes a different soup almost every Monday He is originally from Switzerland and as a result has a funny accent Our unique learning programs have been developed by today’s industry professionalsmany of whom work with Canada’s largest creative agencies and brandsall taught in small classes of no more than six students per instructor Our students work on realworld projects that provide them with the tools and experience to succeed in today’s fastpaced digital environment Our instructors work closely with a diverse group of hiring and community program partners to develop programs that challenge and excite our students Each day they’re asked to create highvalue digital work not grind through monotonous text book exercises It’s the kind of practical experience that sets our students apart and allows them to gain an edge in the competitive tech marketplace We just hired one of your grads So thanks for that also still in discussions with a second one for a slightly different role so it may end up as two hires While we had a large turn out the RED grads were definitely a cut above so you can take that as a feather in your cap Get in touch and well walk you through the rest Powered By Drive Digital RED Academy Courses FullTime Professional Programs Digital Marketing Strategy Web Developer User Experience Designer PartTime Foundation Programs Digital Marketing Foundation Web Developer Foundation User Experience Design Foundation PartTime Essentials Programs AngularJS Design Essentials About Meet The Team Become an Instructor Careers Submit A Student Project Hiring Partner Program Community Programs Blog Events Contact ​ 604​ ​674​ ​8332 View Courses Attend Intro Session FullTime Professional PartTime Foundation PartTime Essentials View Courses UX Designer Professional Web Developer Professional Digital Marketing Professional View Courses UX Designer Foundation Web Developer Foundation Digital Marketing Foundation View Courses AngularJS in Production Visual Designer Essentials Drive Digital Toggle navigation Dates 11 Apr 30 Jun 11 Apr 30 Jun 11 Apr 30 Jun Dates 25 Jan 1 Apr 25 Jan 1 Apr 26 Jan 1 Apr Dates 2 Feb 11 Feb 1 Feb 25 Feb Robert Robert Robert Powered By Drive Digital</v>
       </c>
     </row>
     <row r="18">
@@ -713,16 +578,7 @@
         <v>Training and dev</v>
       </c>
       <c r="C18" t="str">
-        <v>Online Video Tutorials &amp; Training at Lynda.com Learn software, creative, and business skills to achieve your personal and professional goals. Join today to get access to thousands of courses. New skills. Improved skills. Now. Learn technology, creative and business skills you can use today. All memberships include Watch. Listen. Practice. Learn. Learn web development from a pro. A trusted source for knowledge. Training solutions for businesses, schools, government, and more Desktop, mobile, and tablet access Ready to learn? About Us Products Support Apps Connect                    Library                                                     Featured                                                                      Authors                                  Documentaries                                  Playlists                                  Software                                                       Authors                        Documentaries                        Playlists                        Software                    Log in                Sign Up                Start A Free Trial                Reactivate                           Business                                                                                  Small Business                                  Mid Market                                  Fortune 1000                                  Non Profit                                                             Small Business                        Mid Market                        Fortune 1000                        Non Profit                               Academic                                                                                  Higher Ed                                  K-12                                                             Higher Ed                        K-12                               Government                                                                                  State &amp; Local                                  Federal                                  Library                                                             State &amp; Local                        Federal                        Library                                 Developer                              439 Courses        17,947 Video Tutorials                                                               Design                              656 Courses        30,031 Video Tutorials                                                               Web                              1,256 Courses        50,450 Video Tutorials                                                               Photography                              604 Courses        27,088 Video Tutorials                                                               Business                              1,426 Courses        55,466 Video Tutorials                                                               Education                              175 Courses        7,324 Video Tutorials                                                               3D + Animation                              315 Courses        13,146 Video Tutorials                                                               Video                              566 Courses        21,923 Video Tutorials                                                               Audio + Music                              202 Courses        7,085 Video Tutorials                                                       Become a member       Try it free                      Unlimited access     Learn what you want, when you want, from our entire course library.               4,255 video courses     Find what you need in our growing library. New courses added weekly.               Expert teachers     Watch and learn from top experts who are passionate about teaching.               Variety of instruction     Courses for all levels cover technical skills, creative techniques, business strategies, and more.               On-the-go learning     Watch from your computer, tablet, or mobile device. Switch back and forth as you choose.               Custom playlists     Create and save lists of courses you want to watch, and share them with friends or colleagues.     Design Developer Web Business Photography Video Audio 3D Adobe Full Sail University NBC University of Southern California U.S. Office of Government Ethics patagonia Microsoft Mobile site and free apps for iPhone, iPad, and Android devices Switch devices without ever losing your place Offline viewing option for Annual Premium members About Us Careers Press Center Call for Trainers Video2Brain Our Plans Free Trial Academic Solutions Business Solutions Government Solutions Support Contact Us System Requirements Register Activation Key Site Feedback iPhone &amp; iPad Android Windows 8 Desktop App             new course releases newsletter general communications special notices new course releases newsletter general communications special notices                                    We have been unable to process your payment with the details provided.Please update your payment information.                                                                      We have been unable to process your payment with the details provided.Please update your payment information.                                More information Unlimited access Learn what you want, when you want, from our entire course library. 4,255 video courses Find what you need in our growing library. New courses added weekly. Expert teachers Watch and learn from top experts who are passionate about teaching. Variety of instruction Courses for all levels cover technical skills, creative techniques, business strategies, and more. On-the-go learning Watch from your computer, tablet, or mobile device. Switch back and forth as you choose. Custom playlists Create and save lists of courses you want to watch, and share them with friends or colleagues. You set the pace with online learning. Learn what you want, when you want, and practice with the instructor's files while you watch and listen. @lynda Just discovered you today - Thank You! For making learning easy &amp; enjoyable!@dawnmcfresh Our teachers are effective, passionate educators, who are also respected authorities in software, creative, and business fields. They're here to share their expertise in dozens of topics with you, with courses organized into these eight subject areas. We provide training to more than 4 million people, and  our members tell us that lynda.com helps them stay ahead of software updates, pick up brand-new skills,switch careers, land promotions, and explore new hobbies. What can we help you do? lynda.com excels at helping busy professionals keep their software skills razor sharp.—Jill Duffy, PCMag.com I really love your site. I have learned so much and, thanks to you, I have just released my first app for iPhone. —Stephanie J. Despite knowing about @lynda for years, this week I jumped on board and I don’t know how I lived without them. #FF —Justin D.  Read more from our members » In addition to          individual plans, we also offercost-effective group memberships that maketop-quality video training available to everyone inyour organization. Learn more » Some of our clients Lynda.comへようこそ！ 各分野の一流のエキスパートによるビデオトレーニングコースをお探しですか？日々増え続けているLynda.comの日本語によるビデオライブラリをぜひご覧ください。そして広がり続けているlynda.comコミュニティーにあなたもぜひご参加ください。 各分野の一流のエキスパートによるビデオトレーニングコースをお探しですか？日々増え続けているlynda.comの日本語によるビデオライブラリをぜひご覧ください。そして広がり続けているlynda.comコミュニティーにあなたもぜひご参加ください。 Thanks for signing up. We’ll send you a confirmation email shortly. Sign up and receive emails about lynda.com and our online training library: Here’s our privacy policy with more details about how we handle your information. Keep up with news, tips, and latest courses with emails from lynda.com. Sign up and receive emails about lynda.com and our online training library: Here’s our privacy policy with more details about how we handle your information. We've updated our terms and conditions (now called terms of service).Go Review and accept our updated terms of service. We have been unable to process your payment with the details provided.Please update your payment information Skip navigation             Lynda.com | a linkedin company      Library                  Featured Authors Documentaries Playlists Software Log in Sign Up Start A Free Trial Reactivate Business Small Business Mid Market Fortune 1000 Non Profit Academic Higher Ed K-12 Government State &amp; Local Federal Library                Developer                              439 Courses        17,947 Video Tutorials                                                    Design                              656 Courses        30,031 Video Tutorials                                                    Web                              1,256 Courses        50,450 Video Tutorials                                                    Photography                              604 Courses        27,088 Video Tutorials                                                    Business                              1,426 Courses        55,466 Video Tutorials                                                    Education                              175 Courses        7,324 Video Tutorials                                                    3D + Animation                              315 Courses        13,146 Video Tutorials                                                    Video                              566 Courses        21,923 Video Tutorials                                                    Audio + Music                              202 Courses        7,085 Video Tutorials                                     Try it free More information @dawnmcfresh Design Developer Web Business Photography Video Audio 3D  our members tell us —Jill Duffy, PCMag.com Read more from our members » individual plans group memberships Learn more » Try it free 日本版へ行く 日本版へ行く Don't show this message again About Us Careers Press Center Call for Trainers Video2Brain Our Plans Free Trial Academic Solutions Business Solutions Government Solutions Support Contact Us System Requirements Register Activation Key Site Feedback iPhone &amp; iPad Android Windows 8 Desktop App             Site Map Partner Program Privacy Policy Website Use Policy                               lynda.com | a linkedin company              privacy policy privacy policy submit Lightbox submit clicked Go Lynda.com | a linkedin company                Library                                 Featured                Solutions for:           Business                              Academic                              Government                            Developer        Developer                 439 Courses        17,947 Video Tutorials                439 Courses Courses 17,947 Video Tutorials Video Tutorials         Design        Design                 656 Courses        30,031 Video Tutorials                656 Courses Courses 30,031 Video Tutorials Video Tutorials         Web        Web                 1,256 Courses        50,450 Video Tutorials                1,256 Courses Courses 50,450 Video Tutorials Video Tutorials         Photography        Photography                 604 Courses        27,088 Video Tutorials                604 Courses Courses 27,088 Video Tutorials Video Tutorials         Business        Business                 1,426 Courses        55,466 Video Tutorials                1,426 Courses Courses 55,466 Video Tutorials Video Tutorials         Education        Education                 175 Courses        7,324 Video Tutorials                175 Courses Courses 7,324 Video Tutorials Video Tutorials         3D + Animation        3D + Animation                 315 Courses        13,146 Video Tutorials                315 Courses Courses 13,146 Video Tutorials Video Tutorials         Video        Video                 566 Courses        21,923 Video Tutorials                566 Courses Courses 21,923 Video Tutorials Video Tutorials         Audio + Music        Audio + Music                 202 Courses        7,085 Video Tutorials                202 Courses Courses 7,085 Video Tutorials Video Tutorials        Become a member       Try it free       Become a member web development 4 PEOPLE —Stephanie J. —Justin D.  © 2016 lynda.com, Inc. lynda.com | a linkedin company     submit Terms and conditions of use</v>
-      </c>
-      <c r="D18" t="str">
-        <v>Online Video Tutorials &amp; Training at Lynda.com Learn software, creative, and business skills to achieve your personal and professional goals. Join today to get access to thousands of courses. New skills. Improved skills. Now. Learn technology, creative and business skills you can use today. All memberships include Watch. Listen. Practice. Learn. Learn web development from a pro. A trusted source for knowledge. Training solutions for businesses, schools, government, and more Desktop, mobile, and tablet access Ready to learn? About Us Products Support Apps Connect                    Library                                                     Featured                                                                      Authors                                  Documentaries                                  Playlists                                  Software                                                       Authors                        Documentaries                        Playlists                        Software                    Log in                Sign Up                Start A Free Trial                Reactivate                           Business                                                                                  Small Business                                  Mid Market                                  Fortune 1000                                  Non Profit                                                             Small Business                        Mid Market                        Fortune 1000                        Non Profit                               Academic                                                                                  Higher Ed                                  K-12                                                             Higher Ed                        K-12                               Government                                                                                  State &amp; Local                                  Federal                                  Library                                                             State &amp; Local                        Federal                        Library                                 Developer                              439 Courses        17,947 Video Tutorials                                                               Design                              656 Courses        30,031 Video Tutorials                                                               Web                              1,256 Courses        50,450 Video Tutorials                                                               Photography                              604 Courses        27,088 Video Tutorials                                                               Business                              1,426 Courses        55,466 Video Tutorials                                                               Education                              175 Courses        7,324 Video Tutorials                                                               3D + Animation                              315 Courses        13,146 Video Tutorials                                                               Video                              566 Courses        21,923 Video Tutorials                                                               Audio + Music                              202 Courses        7,085 Video Tutorials                                                       Become a member       Try it free                      Unlimited access     Learn what you want, when you want, from our entire course library.               4,255 video courses     Find what you need in our growing library. New courses added weekly.               Expert teachers     Watch and learn from top experts who are passionate about teaching.               Variety of instruction     Courses for all levels cover technical skills, creative techniques, business strategies, and more.               On-the-go learning     Watch from your computer, tablet, or mobile device. Switch back and forth as you choose.               Custom playlists     Create and save lists of courses you want to watch, and share them with friends or colleagues.     Design Developer Web Business Photography Video Audio 3D Adobe Full Sail University NBC University of Southern California U.S. Office of Government Ethics patagonia Microsoft Mobile site and free apps for iPhone, iPad, and Android devices Switch devices without ever losing your place Offline viewing option for Annual Premium members About Us Careers Press Center Call for Trainers Video2Brain Our Plans Free Trial Academic Solutions Business Solutions Government Solutions Support Contact Us System Requirements Register Activation Key Site Feedback iPhone &amp; iPad Android Windows 8 Desktop App             new course releases newsletter general communications special notices new course releases newsletter general communications special notices                                    We have been unable to process your payment with the details provided.Please update your payment information.                                                                      We have been unable to process your payment with the details provided.Please update your payment information.                                More information Unlimited access Learn what you want, when you want, from our entire course library. 4,255 video courses Find what you need in our growing library. New courses added weekly. Expert teachers Watch and learn from top experts who are passionate about teaching. Variety of instruction Courses for all levels cover technical skills, creative techniques, business strategies, and more. On-the-go learning Watch from your computer, tablet, or mobile device. Switch back and forth as you choose. Custom playlists Create and save lists of courses you want to watch, and share them with friends or colleagues. You set the pace with online learning. Learn what you want, when you want, and practice with the instructor's files while you watch and listen. @lynda Just discovered you today - Thank You! For making learning easy &amp; enjoyable!@dawnmcfresh Our teachers are effective, passionate educators, who are also respected authorities in software, creative, and business fields. They're here to share their expertise in dozens of topics with you, with courses organized into these eight subject areas. We provide training to more than 4 million people, and  our members tell us that lynda.com helps them stay ahead of software updates, pick up brand-new skills,switch careers, land promotions, and explore new hobbies. What can we help you do? lynda.com excels at helping busy professionals keep their software skills razor sharp.—Jill Duffy, PCMag.com I really love your site. I have learned so much and, thanks to you, I have just released my first app for iPhone. —Stephanie J. Despite knowing about @lynda for years, this week I jumped on board and I don’t know how I lived without them. #FF —Justin D.  Read more from our members » In addition to          individual plans, we also offercost-effective group memberships that maketop-quality video training available to everyone inyour organization. Learn more » Some of our clients Lynda.comへようこそ！ 各分野の一流のエキスパートによるビデオトレーニングコースをお探しですか？日々増え続けているLynda.comの日本語によるビデオライブラリをぜひご覧ください。そして広がり続けているlynda.comコミュニティーにあなたもぜひご参加ください。 各分野の一流のエキスパートによるビデオトレーニングコースをお探しですか？日々増え続けているlynda.comの日本語によるビデオライブラリをぜひご覧ください。そして広がり続けているlynda.comコミュニティーにあなたもぜひご参加ください。 Thanks for signing up. We’ll send you a confirmation email shortly. Sign up and receive emails about lynda.com and our online training library: Here’s our privacy policy with more details about how we handle your information. Keep up with news, tips, and latest courses with emails from lynda.com. Sign up and receive emails about lynda.com and our online training library: Here’s our privacy policy with more details about how we handle your information. We've updated our terms and conditions (now called terms of service).Go Review and accept our updated terms of service. We have been unable to process your payment with the details provided.Please update your payment information Skip navigation             Lynda.com | a linkedin company      Library                  Featured Authors Documentaries Playlists Software Log in Sign Up Start A Free Trial Reactivate Business Small Business Mid Market Fortune 1000 Non Profit Academic Higher Ed K-12 Government State &amp; Local Federal Library                Developer                              439 Courses        17,947 Video Tutorials                                                    Design                              656 Courses        30,031 Video Tutorials                                                    Web                              1,256 Courses        50,450 Video Tutorials                                                    Photography                              604 Courses        27,088 Video Tutorials                                                    Business                              1,426 Courses        55,466 Video Tutorials                                                    Education                              175 Courses        7,324 Video Tutorials                                                    3D + Animation                              315 Courses        13,146 Video Tutorials                                                    Video                              566 Courses        21,923 Video Tutorials                                                    Audio + Music                              202 Courses        7,085 Video Tutorials                                     Try it free More information @dawnmcfresh Design Developer Web Business Photography Video Audio 3D  our members tell us —Jill Duffy, PCMag.com Read more from our members » individual plans group memberships Learn more » Try it free 日本版へ行く 日本版へ行く Don't show this message again About Us Careers Press Center Call for Trainers Video2Brain Our Plans Free Trial Academic Solutions Business Solutions Government Solutions Support Contact Us System Requirements Register Activation Key Site Feedback iPhone &amp; iPad Android Windows 8 Desktop App             Site Map Partner Program Privacy Policy Website Use Policy                               lynda.com | a linkedin company              privacy policy privacy policy submit Lightbox submit clicked Go Lynda.com | a linkedin company                Library                                 Featured                Solutions for:           Business                              Academic                              Government                            Developer        Developer                 439 Courses        17,947 Video Tutorials                439 Courses Courses 17,947 Video Tutorials Video Tutorials         Design        Design                 656 Courses        30,031 Video Tutorials                656 Courses Courses 30,031 Video Tutorials Video Tutorials         Web        Web                 1,256 Courses        50,450 Video Tutorials                1,256 Courses Courses 50,450 Video Tutorials Video Tutorials         Photography        Photography                 604 Courses        27,088 Video Tutorials                604 Courses Courses 27,088 Video Tutorials Video Tutorials         Business        Business                 1,426 Courses        55,466 Video Tutorials                1,426 Courses Courses 55,466 Video Tutorials Video Tutorials         Education        Education                 175 Courses        7,324 Video Tutorials                175 Courses Courses 7,324 Video Tutorials Video Tutorials         3D + Animation        3D + Animation                 315 Courses        13,146 Video Tutorials                315 Courses Courses 13,146 Video Tutorials Video Tutorials         Video        Video                 566 Courses        21,923 Video Tutorials                566 Courses Courses 21,923 Video Tutorials Video Tutorials         Audio + Music        Audio + Music                 202 Courses        7,085 Video Tutorials                202 Courses Courses 7,085 Video Tutorials Video Tutorials        Become a member       Try it free       Become a member web development 4 PEOPLE —Stephanie J. —Justin D.  © 2016 lynda.com, Inc. lynda.com | a linkedin company     submit Terms and conditions of use</v>
-      </c>
-      <c r="E18" t="str">
-        <v>Online Video Tutorials &amp; Training at Lynda.com Learn software, creative, and business skills to achieve your personal and professional goals. Join today to get access to thousands of courses. New skills. Improved skills. Now. Learn technology, creative and business skills you can use today. All memberships include Watch. Listen. Practice. Learn. Learn web development from a pro. A trusted source for knowledge. Training solutions for businesses, schools, government, and more Desktop, mobile, and tablet access Ready to learn? About Us Products Support Apps Connect                    Library                                                     Featured                                                                      Authors                                  Documentaries                                  Playlists                                  Software                                                       Authors                        Documentaries                        Playlists                        Software                    Log in                Sign Up                Start A Free Trial                Reactivate                           Business                                                                                  Small Business                                  Mid Market                                  Fortune 1000                                  Non Profit                                                             Small Business                        Mid Market                        Fortune 1000                        Non Profit                               Academic                                                                                  Higher Ed                                  K-12                                                             Higher Ed                        K-12                               Government                                                                                  State &amp; Local                                  Federal                                  Library                                                             State &amp; Local                        Federal                        Library                                 Developer                              439 Courses        17,947 Video Tutorials                                                               Design                              656 Courses        30,031 Video Tutorials                                                               Web                              1,256 Courses        50,450 Video Tutorials                                                               Photography                              604 Courses        27,088 Video Tutorials                                                               Business                              1,426 Courses        55,466 Video Tutorials                                                               Education                              175 Courses        7,324 Video Tutorials                                                               3D + Animation                              315 Courses        13,146 Video Tutorials                                                               Video                              566 Courses        21,923 Video Tutorials                                                               Audio + Music                              202 Courses        7,085 Video Tutorials                                                       Become a member       Try it free                      Unlimited access     Learn what you want, when you want, from our entire course library.               4,255 video courses     Find what you need in our growing library. New courses added weekly.               Expert teachers     Watch and learn from top experts who are passionate about teaching.               Variety of instruction     Courses for all levels cover technical skills, creative techniques, business strategies, and more.               On-the-go learning     Watch from your computer, tablet, or mobile device. Switch back and forth as you choose.               Custom playlists     Create and save lists of courses you want to watch, and share them with friends or colleagues.     Design Developer Web Business Photography Video Audio 3D Adobe Full Sail University NBC University of Southern California U.S. Office of Government Ethics patagonia Microsoft Mobile site and free apps for iPhone, iPad, and Android devices Switch devices without ever losing your place Offline viewing option for Annual Premium members About Us Careers Press Center Call for Trainers Video2Brain Our Plans Free Trial Academic Solutions Business Solutions Government Solutions Support Contact Us System Requirements Register Activation Key Site Feedback iPhone &amp; iPad Android Windows 8 Desktop App             new course releases newsletter general communications special notices new course releases newsletter general communications special notices                                    We have been unable to process your payment with the details provided.Please update your payment information.                                                                      We have been unable to process your payment with the details provided.Please update your payment information.                                More information Unlimited access Learn what you want, when you want, from our entire course library. 4,255 video courses Find what you need in our growing library. New courses added weekly. Expert teachers Watch and learn from top experts who are passionate about teaching. Variety of instruction Courses for all levels cover technical skills, creative techniques, business strategies, and more. On-the-go learning Watch from your computer, tablet, or mobile device. Switch back and forth as you choose. Custom playlists Create and save lists of courses you want to watch, and share them with friends or colleagues. You set the pace with online learning. Learn what you want, when you want, and practice with the instructor's files while you watch and listen. @lynda Just discovered you today - Thank You! For making learning easy &amp; enjoyable!@dawnmcfresh Our teachers are effective, passionate educators, who are also respected authorities in software, creative, and business fields. They're here to share their expertise in dozens of topics with you, with courses organized into these eight subject areas. We provide training to more than 4 million people, and  our members tell us that lynda.com helps them stay ahead of software updates, pick up brand-new skills,switch careers, land promotions, and explore new hobbies. What can we help you do? lynda.com excels at helping busy professionals keep their software skills razor sharp.—Jill Duffy, PCMag.com I really love your site. I have learned so much and, thanks to you, I have just released my first app for iPhone. —Stephanie J. Despite knowing about @lynda for years, this week I jumped on board and I don’t know how I lived without them. #FF —Justin D.  Read more from our members » In addition to          individual plans, we also offercost-effective group memberships that maketop-quality video training available to everyone inyour organization. Learn more » Some of our clients Lynda.comへようこそ！ 各分野の一流のエキスパートによるビデオトレーニングコースをお探しですか？日々増え続けているLynda.comの日本語によるビデオライブラリをぜひご覧ください。そして広がり続けているlynda.comコミュニティーにあなたもぜひご参加ください。 各分野の一流のエキスパートによるビデオトレーニングコースをお探しですか？日々増え続けているlynda.comの日本語によるビデオライブラリをぜひご覧ください。そして広がり続けているlynda.comコミュニティーにあなたもぜひご参加ください。 Thanks for signing up. We’ll send you a confirmation email shortly. Sign up and receive emails about lynda.com and our online training library: Here’s our privacy policy with more details about how we handle your information. Keep up with news, tips, and latest courses with emails from lynda.com. Sign up and receive emails about lynda.com and our online training library: Here’s our privacy policy with more details about how we handle your information. We've updated our terms and conditions (now called terms of service).Go Review and accept our updated terms of service. We have been unable to process your payment with the details provided.Please update your payment information Skip navigation             Lynda.com | a linkedin company      Library                  Featured Authors Documentaries Playlists Software Log in Sign Up Start A Free Trial Reactivate Business Small Business Mid Market Fortune 1000 Non Profit Academic Higher Ed K-12 Government State &amp; Local Federal Library                Developer                              439 Courses        17,947 Video Tutorials                                                    Design                              656 Courses        30,031 Video Tutorials                                                    Web                              1,256 Courses        50,450 Video Tutorials                                                    Photography                              604 Courses        27,088 Video Tutorials                                                    Business                              1,426 Courses        55,466 Video Tutorials                                                    Education                              175 Courses        7,324 Video Tutorials                                                    3D + Animation                              315 Courses        13,146 Video Tutorials                                                    Video                              566 Courses        21,923 Video Tutorials                                                    Audio + Music                              202 Courses        7,085 Video Tutorials                                     Try it free More information @dawnmcfresh Design Developer Web Business Photography Video Audio 3D  our members tell us —Jill Duffy, PCMag.com Read more from our members » individual plans group memberships Learn more » Try it free 日本版へ行く 日本版へ行く Don't show this message again About Us Careers Press Center Call for Trainers Video2Brain Our Plans Free Trial Academic Solutions Business Solutions Government Solutions Support Contact Us System Requirements Register Activation Key Site Feedback iPhone &amp; iPad Android Windows 8 Desktop App             Site Map Partner Program Privacy Policy Website Use Policy                               lynda.com | a linkedin company              privacy policy privacy policy submit Lightbox submit clicked Go Lynda.com | a linkedin company                Library                                 Featured                Solutions for:           Business                              Academic                              Government                            Developer        Developer                 439 Courses        17,947 Video Tutorials                439 Courses Courses 17,947 Video Tutorials Video Tutorials         Design        Design                 656 Courses        30,031 Video Tutorials                656 Courses Courses 30,031 Video Tutorials Video Tutorials         Web        Web                 1,256 Courses        50,450 Video Tutorials                1,256 Courses Courses 50,450 Video Tutorials Video Tutorials         Photography        Photography                 604 Courses        27,088 Video Tutorials                604 Courses Courses 27,088 Video Tutorials Video Tutorials         Business        Business                 1,426 Courses        55,466 Video Tutorials                1,426 Courses Courses 55,466 Video Tutorials Video Tutorials         Education        Education                 175 Courses        7,324 Video Tutorials                175 Courses Courses 7,324 Video Tutorials Video Tutorials         3D + Animation        3D + Animation                 315 Courses        13,146 Video Tutorials                315 Courses Courses 13,146 Video Tutorials Video Tutorials         Video        Video                 566 Courses        21,923 Video Tutorials                566 Courses Courses 21,923 Video Tutorials Video Tutorials         Audio + Music        Audio + Music                 202 Courses        7,085 Video Tutorials                202 Courses Courses 7,085 Video Tutorials Video Tutorials        Become a member       Try it free       Become a member web development 4 PEOPLE —Stephanie J. —Justin D.  © 2016 lynda.com, Inc. lynda.com | a linkedin company     submit Terms and conditions of use</v>
-      </c>
-      <c r="F18" t="str">
-        <v>Online Video Tutorials &amp; Training at Lynda.com Learn software, creative, and business skills to achieve your personal and professional goals. Join today to get access to thousands of courses. New skills. Improved skills. Now. Learn technology, creative and business skills you can use today. All memberships include Watch. Listen. Practice. Learn. Learn web development from a pro. A trusted source for knowledge. Training solutions for businesses, schools, government, and more Desktop, mobile, and tablet access Ready to learn? About Us Products Support Apps Connect                    Library                                                     Featured                                                                      Authors                                  Documentaries                                  Playlists                                  Software                                                       Authors                        Documentaries                        Playlists                        Software                    Log in                Sign Up                Start A Free Trial                Reactivate                           Business                                                                                  Small Business                                  Mid Market                                  Fortune 1000                                  Non Profit                                                             Small Business                        Mid Market                        Fortune 1000                        Non Profit                               Academic                                                                                  Higher Ed                                  K-12                                                             Higher Ed                        K-12                               Government                                                                                  State &amp; Local                                  Federal                                  Library                                                             State &amp; Local                        Federal                        Library                                 Developer                              439 Courses        17,947 Video Tutorials                                                               Design                              656 Courses        30,031 Video Tutorials                                                               Web                              1,256 Courses        50,450 Video Tutorials                                                               Photography                              604 Courses        27,088 Video Tutorials                                                               Business                              1,426 Courses        55,466 Video Tutorials                                                               Education                              175 Courses        7,324 Video Tutorials                                                               3D + Animation                              315 Courses        13,146 Video Tutorials                                                               Video                              566 Courses        21,923 Video Tutorials                                                               Audio + Music                              202 Courses        7,085 Video Tutorials                                                       Become a member       Try it free                      Unlimited access     Learn what you want, when you want, from our entire course library.               4,255 video courses     Find what you need in our growing library. New courses added weekly.               Expert teachers     Watch and learn from top experts who are passionate about teaching.               Variety of instruction     Courses for all levels cover technical skills, creative techniques, business strategies, and more.               On-the-go learning     Watch from your computer, tablet, or mobile device. Switch back and forth as you choose.               Custom playlists     Create and save lists of courses you want to watch, and share them with friends or colleagues.     Design Developer Web Business Photography Video Audio 3D Adobe Full Sail University NBC University of Southern California U.S. Office of Government Ethics patagonia Microsoft Mobile site and free apps for iPhone, iPad, and Android devices Switch devices without ever losing your place Offline viewing option for Annual Premium members About Us Careers Press Center Call for Trainers Video2Brain Our Plans Free Trial Academic Solutions Business Solutions Government Solutions Support Contact Us System Requirements Register Activation Key Site Feedback iPhone &amp; iPad Android Windows 8 Desktop App             new course releases newsletter general communications special notices new course releases newsletter general communications special notices                                    We have been unable to process your payment with the details provided.Please update your payment information.                                                                      We have been unable to process your payment with the details provided.Please update your payment information.                                More information Unlimited access Learn what you want, when you want, from our entire course library. 4,255 video courses Find what you need in our growing library. New courses added weekly. Expert teachers Watch and learn from top experts who are passionate about teaching. Variety of instruction Courses for all levels cover technical skills, creative techniques, business strategies, and more. On-the-go learning Watch from your computer, tablet, or mobile device. Switch back and forth as you choose. Custom playlists Create and save lists of courses you want to watch, and share them with friends or colleagues. You set the pace with online learning. Learn what you want, when you want, and practice with the instructor's files while you watch and listen. @lynda Just discovered you today - Thank You! For making learning easy &amp; enjoyable!@dawnmcfresh Our teachers are effective, passionate educators, who are also respected authorities in software, creative, and business fields. They're here to share their expertise in dozens of topics with you, with courses organized into these eight subject areas. We provide training to more than 4 million people, and  our members tell us that lynda.com helps them stay ahead of software updates, pick up brand-new skills,switch careers, land promotions, and explore new hobbies. What can we help you do? lynda.com excels at helping busy professionals keep their software skills razor sharp.—Jill Duffy, PCMag.com I really love your site. I have learned so much and, thanks to you, I have just released my first app for iPhone. —Stephanie J. Despite knowing about @lynda for years, this week I jumped on board and I don’t know how I lived without them. #FF —Justin D.  Read more from our members » In addition to          individual plans, we also offercost-effective group memberships that maketop-quality video training available to everyone inyour organization. Learn more » Some of our clients Lynda.comへようこそ！ 各分野の一流のエキスパートによるビデオトレーニングコースをお探しですか？日々増え続けているLynda.comの日本語によるビデオライブラリをぜひご覧ください。そして広がり続けているlynda.comコミュニティーにあなたもぜひご参加ください。 各分野の一流のエキスパートによるビデオトレーニングコースをお探しですか？日々増え続けているlynda.comの日本語によるビデオライブラリをぜひご覧ください。そして広がり続けているlynda.comコミュニティーにあなたもぜひご参加ください。 Thanks for signing up. We’ll send you a confirmation email shortly. Sign up and receive emails about lynda.com and our online training library: Here’s our privacy policy with more details about how we handle your information. Keep up with news, tips, and latest courses with emails from lynda.com. Sign up and receive emails about lynda.com and our online training library: Here’s our privacy policy with more details about how we handle your information. We've updated our terms and conditions (now called terms of service).Go Review and accept our updated terms of service. We have been unable to process your payment with the details provided.Please update your payment information Skip navigation             Lynda.com | a linkedin company      Library                  Featured Authors Documentaries Playlists Software Log in Sign Up Start A Free Trial Reactivate Business Small Business Mid Market Fortune 1000 Non Profit Academic Higher Ed K-12 Government State &amp; Local Federal Library                Developer                              439 Courses        17,947 Video Tutorials                                                    Design                              656 Courses        30,031 Video Tutorials                                                    Web                              1,256 Courses        50,450 Video Tutorials                                                    Photography                              604 Courses        27,088 Video Tutorials                                                    Business                              1,426 Courses        55,466 Video Tutorials                                                    Education                              175 Courses        7,324 Video Tutorials                                                    3D + Animation                              315 Courses        13,146 Video Tutorials                                                    Video                              566 Courses        21,923 Video Tutorials                                                    Audio + Music                              202 Courses        7,085 Video Tutorials                                     Try it free More information @dawnmcfresh Design Developer Web Business Photography Video Audio 3D  our members tell us —Jill Duffy, PCMag.com Read more from our members » individual plans group memberships Learn more » Try it free 日本版へ行く 日本版へ行く Don't show this message again About Us Careers Press Center Call for Trainers Video2Brain Our Plans Free Trial Academic Solutions Business Solutions Government Solutions Support Contact Us System Requirements Register Activation Key Site Feedback iPhone &amp; iPad Android Windows 8 Desktop App             Site Map Partner Program Privacy Policy Website Use Policy                               lynda.com | a linkedin company              privacy policy privacy policy submit Lightbox submit clicked Go Lynda.com | a linkedin company                Library                                 Featured                Solutions for:           Business                              Academic                              Government                            Developer        Developer                 439 Courses        17,947 Video Tutorials                439 Courses Courses 17,947 Video Tutorials Video Tutorials         Design        Design                 656 Courses        30,031 Video Tutorials                656 Courses Courses 30,031 Video Tutorials Video Tutorials         Web        Web                 1,256 Courses        50,450 Video Tutorials                1,256 Courses Courses 50,450 Video Tutorials Video Tutorials         Photography        Photography                 604 Courses        27,088 Video Tutorials                604 Courses Courses 27,088 Video Tutorials Video Tutorials         Business        Business                 1,426 Courses        55,466 Video Tutorials                1,426 Courses Courses 55,466 Video Tutorials Video Tutorials         Education        Education                 175 Courses        7,324 Video Tutorials                175 Courses Courses 7,324 Video Tutorials Video Tutorials         3D + Animation        3D + Animation                 315 Courses        13,146 Video Tutorials                315 Courses Courses 13,146 Video Tutorials Video Tutorials         Video        Video                 566 Courses        21,923 Video Tutorials                566 Courses Courses 21,923 Video Tutorials Video Tutorials         Audio + Music        Audio + Music                 202 Courses        7,085 Video Tutorials                202 Courses Courses 7,085 Video Tutorials Video Tutorials        Become a member       Try it free       Become a member web development 4 PEOPLE —Stephanie J. —Justin D.  © 2016 lynda.com, Inc. lynda.com | a linkedin company     submit Terms and conditions of use</v>
+        <v>Online Video Tutorials Training at Lyndacom Learn software creative and business skills to achieve your personal and professional goals Join today to get access to thousands of courses New skills Improved skills Now Learn technology creative and business skills you can use today All memberships include Watch Listen Practice Learn Learn web development from a pro A trusted source for knowledge Training solutions for businesses schools government and more Desktop mobile and tablet access Ready to learn About Us Products Support Apps Connect Library Featured Authors Documentaries Playlists Software Authors Documentaries Playlists Software Log in Sign Up Start A Free Trial Reactivate Business Small Business Mid Market Fortune 1000 Non Profit Small Business Mid Market Fortune 1000 Non Profit Academic Higher Ed K12 Higher Ed K12 Government State Local Federal Library State Local Federal Library Developer 439 Courses 17947 Video Tutorials Design 656 Courses 30031 Video Tutorials Web 1256 Courses 50450 Video Tutorials Photography 604 Courses 27088 Video Tutorials Business 1426 Courses 55466 Video Tutorials Education 175 Courses 7324 Video Tutorials 3D Animation 315 Courses 13146 Video Tutorials Video 566 Courses 21923 Video Tutorials Audio Music 202 Courses 7085 Video Tutorials Become a member Try it free Unlimited access Learn what you want when you want from our entire course library 4255 video courses Find what you need in our growing library New courses added weekly Expert teachers Watch and learn from top experts who are passionate about teaching Variety of instruction Courses for all levels cover technical skills creative techniques business strategies and more Onthego learning Watch from your computer tablet or mobile device Switch back and forth as you choose Custom playlists Create and save lists of courses you want to watch and share them with friends or colleagues Design Developer Web Business Photography Video Audio 3D Adobe Full Sail University NBC University of Southern California US Office of Government Ethics patagonia Microsoft Mobile site and free apps for iPhone iPad and Android devices Switch devices without ever losing your place Offline viewing option for Annual Premium members About Us Careers Press Center Call for Trainers Video2Brain Our Plans Free Trial Academic Solutions Business Solutions Government Solutions Support Contact Us System Requirements Register Activation Key Site Feedback iPhone iPad Android Windows 8 Desktop App new course releases newsletter general communications special notices new course releases newsletter general communications special notices We have been unable to process your payment with the details providedPlease update your payment information We have been unable to process your payment with the details providedPlease update your payment information More information Unlimited access Learn what you want when you want from our entire course library 4255 video courses Find what you need in our growing library New courses added weekly Expert teachers Watch and learn from top experts who are passionate about teaching Variety of instruction Courses for all levels cover technical skills creative techniques business strategies and more Onthego learning Watch from your computer tablet or mobile device Switch back and forth as you choose Custom playlists Create and save lists of courses you want to watch and share them with friends or colleagues You set the pace with online learning Learn what you want when you want and practice with the instructors files while you watch and listen lynda Just discovered you today Thank You For making learning easy enjoyabledawnmcfresh Our teachers are effective passionate educators who are also respected authorities in software creative and business fields Theyre here to share their expertise in dozens of topics with you with courses organized into these eight subject areas We provide training to more than 4 million people and our members tell us that lyndacom helps them stay ahead of software updates pick up brandnew skillsswitch careers land promotions and explore new hobbies What can we help you do lyndacom excels at helping busy professionals keep their software skills razor sharpJill Duffy PCMagcom I really love your site I have learned so much and thanks to you I have just released my first app for iPhone Stephanie J Despite knowing about lynda for years this week I jumped on board and I don’t know how I lived without them FF Justin D Read more from our members » In addition to individual plans we also offercosteffective group memberships that maketopquality video training available to everyone inyour organization Learn more » Some of our clients Lyndacomへようこそ！ 各分野の一流のエキスパートによるビデオトレーニングコースをお探しですか？日々増え続けているLyndacomの日本語によるビデオライブラリをぜひご覧ください。そして広がり続けているlyndacomコミュニティーにあなたもぜひご参加ください。 各分野の一流のエキスパートによるビデオトレーニングコースをお探しですか？日々増え続けているlyndacomの日本語によるビデオライブラリをぜひご覧ください。そして広がり続けているlyndacomコミュニティーにあなたもぜひご参加ください。 Thanks for signing up We’ll send you a confirmation email shortly Sign up and receive emails about lyndacom and our online training library Here’s our privacy policy with more details about how we handle your information Keep up with news tips and latest courses with emails from lyndacom Sign up and receive emails about lyndacom and our online training library Here’s our privacy policy with more details about how we handle your information Weve updated our terms and conditions now called terms of serviceGo Review and accept our updated terms of service We have been unable to process your payment with the details providedPlease update your payment information Skip navigation Lyndacom a linkedin company Library Featured Authors Documentaries Playlists Software Log in Sign Up Start A Free Trial Reactivate Business Small Business Mid Market Fortune 1000 Non Profit Academic Higher Ed K12 Government State Local Federal Library Developer 439 Courses 17947 Video Tutorials Design 656 Courses 30031 Video Tutorials Web 1256 Courses 50450 Video Tutorials Photography 604 Courses 27088 Video Tutorials Business 1426 Courses 55466 Video Tutorials Education 175 Courses 7324 Video Tutorials 3D Animation 315 Courses 13146 Video Tutorials Video 566 Courses 21923 Video Tutorials Audio Music 202 Courses 7085 Video Tutorials Try it free More information dawnmcfresh Design Developer Web Business Photography Video Audio 3D our members tell us Jill Duffy PCMagcom Read more from our members » individual plans group memberships Learn more » Try it free 日本版へ行く 日本版へ行く Dont show this message again About Us Careers Press Center Call for Trainers Video2Brain Our Plans Free Trial Academic Solutions Business Solutions Government Solutions Support Contact Us System Requirements Register Activation Key Site Feedback iPhone iPad Android Windows 8 Desktop App Site Map Partner Program Privacy Policy Website Use Policy lyndacom a linkedin company privacy policy privacy policy submit Lightbox submit clicked Go Lyndacom a linkedin company Library Featured Solutions for Business Academic Government Developer Developer 439 Courses 17947 Video Tutorials 439 Courses Courses 17947 Video Tutorials Video Tutorials Design Design 656 Courses 30031 Video Tutorials 656 Courses Courses 30031 Video Tutorials Video Tutorials Web Web 1256 Courses 50450 Video Tutorials 1256 Courses Courses 50450 Video Tutorials Video Tutorials Photography Photography 604 Courses 27088 Video Tutorials 604 Courses Courses 27088 Video Tutorials Video Tutorials Business Business 1426 Courses 55466 Video Tutorials 1426 Courses Courses 55466 Video Tutorials Video Tutorials Education Education 175 Courses 7324 Video Tutorials 175 Courses Courses 7324 Video Tutorials Video Tutorials 3D Animation 3D Animation 315 Courses 13146 Video Tutorials 315 Courses Courses 13146 Video Tutorials Video Tutorials Video Video 566 Courses 21923 Video Tutorials 566 Courses Courses 21923 Video Tutorials Video Tutorials Audio Music Audio Music 202 Courses 7085 Video Tutorials 202 Courses Courses 7085 Video Tutorials Video Tutorials Become a member Try it free Become a member web development 4 PEOPLE Stephanie J Justin D © 2016 lyndacom Inc lyndacom a linkedin company submit Terms and conditions of use</v>
       </c>
     </row>
     <row r="19">
@@ -733,16 +589,7 @@
         <v>Training and dev</v>
       </c>
       <c r="C19" t="str">
-        <v>Udemy: Online Courses Anytime, Anywhere                       Udemy is an online education marketplace with limitless variety: over 7 million students enrolled in more than 30,000 courses,taught by 19,000 instructors (and counting). What course will your life take? Ready to master some skills? Take your career to the next level! Development Business IT &amp; Software Office Productivity Personal Development Design Marketing Lifestyle Photography Health &amp; Fitness Teacher Training Music Academics Language Test Prep                                               Development                                                                        Development                                                                                                   Web Development                                                                                             Mobile Apps                                                                                             Programming Languages                                                                                             Game Development                                                                                             Databases                                                                                             Software Testing                                                                                             Software Engineering                                                                                             Development Tools                                                                                             E-Commerce                                                                                                     Web Development                                                    Mobile Apps                                                    Programming Languages                                                    Game Development                                                    Databases                                                    Software Testing                                                    Software Engineering                                                    Development Tools                                                    E-Commerce                                                     Business                                                                        Business                                                                                                   Finance                                                                                             Entrepreneurship                                                                                             Communications                                                                                             Management                                                                                             Sales                                                                                             Strategy                                                                                             Operations                                                                                             Project Management                                                                                             Business Law                                                                                             Data &amp; Analytics                                                                                             Home Business                                                                                             Human Resources                                                                                             Industry                                                                                             Media                                                                                             Real Estate                                                                                             Other                                                                                                     Finance                                                    Entrepreneurship                                                    Communications                                                    Management                                                    Sales                                                    Strategy                                                    Operations                                                    Project Management                                                    Business Law                                                    Data &amp; Analytics                                                    Home Business                                                    Human Resources                                                    Industry                                                    Media                                                    Real Estate                                                    Other                                                     IT &amp; Software                                                                        IT &amp; Software                                                                                                   IT Certification                                                                                             Network &amp; Security                                                                                             Hardware                                                                                             Operating Systems                                                                                             Other                                                                                                     IT Certification                                                    Network &amp; Security                                                    Hardware                                                    Operating Systems                                                    Other                                                     Office Productivity                                                                        Office Productivity                                                                                                   Microsoft                                                                                             Apple                                                                                             Google                                                                                             SAP                                                                                             Intuit                                                                                             Salesforce                                                                                             Oracle                                                                                             Other                                                                                                     Microsoft                                                    Apple                                                    Google                                                    SAP                                                    Intuit                                                    Salesforce                                                    Oracle                                                    Other                                                     Personal Development                                                                        Personal Development                                                                                                   Personal Transformation                                                                                             Productivity                                                                                             Leadership                                                                                             Personal Finance                                                                                             Career Development                                                                                             Parenting &amp; Relationships                                                                                             Happiness                                                                                             Religion &amp; Spirituality                                                                                             Personal Brand Building                                                                                             Creativity                                                                                             Influence                                                                                             Self Esteem                                                                                             Stress Management                                                                                             Memory &amp; Study Skills                                                                                             Motivation                                                                                             Other                                                                                                     Personal Transformation                                                    Productivity                                                    Leadership                                                    Personal Finance                                                    Career Development                                                    Parenting &amp; Relationships                                                    Happiness                                                    Religion &amp; Spirituality                                                    Personal Brand Building                                                    Creativity                                                    Influence                                                    Self Esteem                                                    Stress Management                                                    Memory &amp; Study Skills                                                    Motivation                                                    Other                                                     Design                                                                        Design                                                                                                   Web Design                                                                                             Graphic Design                                                                                             Design Tools                                                                                             User Experience                                                                                             Game Design                                                                                             Design Thinking                                                                                             3D &amp; Animation                                                                                             Fashion                                                                                             Architectural Design                                                                                             Interior Design                                                                                             Other                                                                                                     Web Design                                                    Graphic Design                                                    Design Tools                                                    User Experience                                                    Game Design                                                    Design Thinking                                                    3D &amp; Animation                                                    Fashion                                                    Architectural Design                                                    Interior Design                                                    Other                                                     Marketing                                                                        Marketing                                                                                                   Digital Marketing                                                                                             Search Engine Optimization                                                                                             Social Media Marketing                                                                                             Branding                                                                                             Marketing Fundamentals                                                                                             Analytics &amp; Automation                                                                                             Public Relations                                                                                             Advertising                                                                                             Video &amp; Mobile Marketing                                                                                             Content Marketing                                                                                             Non-Digital Marketing                                                                                             Growth Hacking                                                                                             Affiliate Marketing                                                                                             Product Marketing                                                                                             Other                                                                                                     Digital Marketing                                                    Search Engine Optimization                                                    Social Media Marketing                                                    Branding                                                    Marketing Fundamentals                                                    Analytics &amp; Automation                                                    Public Relations                                                    Advertising                                                    Video &amp; Mobile Marketing                                                    Content Marketing                                                    Non-Digital Marketing                                                    Growth Hacking                                                    Affiliate Marketing                                                    Product Marketing                                                    Other                                                     Lifestyle                                                                        Lifestyle                                                                                                   Arts &amp; Crafts                                                                                             Food &amp; Beverage                                                                                             Beauty &amp; Makeup                                                                                             Travel                                                                                             Gaming                                                                                             Home Improvement                                                                                             Pet Care &amp; Training                                                                                             Other                                                                                                     Arts &amp; Crafts                                                    Food &amp; Beverage                                                    Beauty &amp; Makeup                                                    Travel                                                    Gaming                                                    Home Improvement                                                    Pet Care &amp; Training                                                    Other                                                     Photography                                                                        Photography                                                                                                   Digital Photography                                                                                             Photography Fundamentals                                                                                             Portraits                                                                                             Landscape                                                                                             Black &amp; White                                                                                             Photography Tools                                                                                             Mobile Photography                                                                                             Travel Photography                                                                                             Commercial Photography                                                                                             Wedding Photography                                                                                             Wildlife Photography                                                                                             Video Design                                                                                             Other                                                                                                     Digital Photography                                                    Photography Fundamentals                                                    Portraits                                                    Landscape                                                    Black &amp; White                                                    Photography Tools                                                    Mobile Photography                                                    Travel Photography                                                    Commercial Photography                                                    Wedding Photography                                                    Wildlife Photography                                                    Video Design                                                    Other                                                     Health &amp; Fitness                                                                        Health &amp; Fitness                                                                                                   Fitness                                                                                             General Health                                                                                             Sports                                                                                             Nutrition                                                                                             Yoga                                                                                             Mental Health                                                                                             Dieting                                                                                             Self Defense                                                                                             Safety &amp; First Aid                                                                                             Dance                                                                                             Meditation                                                                                             Other                                                                                                     Fitness                                                    General Health                                                    Sports                                                    Nutrition                                                    Yoga                                                    Mental Health                                                    Dieting                                                    Self Defense                                                    Safety &amp; First Aid                                                    Dance                                                    Meditation                                                    Other                                                     Teacher Training                                                                        Teacher Training                                                                                                   Instructional Design                                                                                             Educational Development                                                                                             Teaching Tools                                                                                             Other                                                                                                     Instructional Design                                                    Educational Development                                                    Teaching Tools                                                    Other                                                     Music                                                                        Music                                                                                                   Instruments                                                                                             Production                                                                                             Music Fundamentals                                                                                             Vocal                                                                                             Music Techniques                                                                                             Music Software                                                                                             Other                                                                                                     Instruments                                                    Production                                                    Music Fundamentals                                                    Vocal                                                    Music Techniques                                                    Music Software                                                    Other                                                     Academics                                                                        Academics                                                                                                   Social Science                                                                                             Math &amp; Science                                                                                             Humanities                                                                                                     Social Science                                                    Math &amp; Science                                                    Humanities                                                     Language                                                                        Language                                                                                                   English                                                                                             Spanish                                                                                             German                                                                                             French                                                                                             Japanese                                                                                             Portuguese                                                                                             Chinese                                                                                             Russian                                                                                             Latin                                                                                             Arabic                                                                                             Hebrew                                                                                             Italian                                                                                             Other                                                                                                     English                                                    Spanish                                                    German                                                    French                                                    Japanese                                                    Portuguese                                                    Chinese                                                    Russian                                                    Latin                                                    Arabic                                                    Hebrew                                                    Italian                                                    Other                                                     Test Prep                                                                        Test Prep                                                                                                   Grad Entry Exam                                                                                             International High School                                                                                             College Entry Exam                                                                                             Test Taking Skills                                                                                             Other                                                                                                     Grad Entry Exam                                                    International High School                                                    College Entry Exam                                                    Test Taking Skills                                                    Other                                         Over 9 million students                                                More than 35,000 courses                                                Learn at your pace on any device                                                                                                    Top Python Courses                                                                                                                                    The Top Java Tutorials                                                                                                                                    Excel                                                                                                                                                                                  AWS Certified Solutions Architect - Associate 2016                                                         By Ryan Kroonenburg                                                     Want to pass the AWS Solutions Architect - Associate Exam? Want to become Amazon Web Services Certified? Do this course!                                                                                       26.6K Enrolled                                                             $79                                                                                                                                                                                                                          ITIL Foundation Course                                                         By ITSM Zone                                                     This course will prepare you for the ITIL Foundation exam                                                                                       5.2K Enrolled                                                             $229                                                                                                                                                                                                                          3D Animation: Basics To Full Body and Creature Mechanics                                                         By Charlie Grubel                                                     Learn to animate a ball bounce, bounce with a tail, standard walk and a zombie crawl! After, get a personal critique!                                                                                       163 Enrolled                                                             $49                                                                                                                                                                                                                          The Complete iOS 9 Developer Course - Build 18 Apps                                                         By Rob Percival                                                     Use Xcode 7 &amp; Swift 2 to make real apps like Uber, Instagram &amp; Flappy Bird. Includes free web hosting, assets &amp; ebook.                                                                                       70.6K Enrolled                                                             $199                                                                                                                                                                                                                          Photography Masterclass: Your Complete Guide to Photography                                                         By Phil Ebiner and 1 other                                                     The Best Selling Online Professional Photography Class: How to Take &amp; Sell Photos                                                                                       22.4K Enrolled                                                             $297                                                                                                                                                                                                                          Learn SAP Course - Online Beginner Training                                                         By Peter Moxon                                                     Learn SAP with Peter Moxon - Ideal</v>
-      </c>
-      <c r="D19" t="str">
-        <v xml:space="preserve"> Beginner SAP Training Course! Unlimited Life Time Access &amp; Fully Downloadable!                                                                                       2.5K Enrolled                                                             $109                                                                                                                                                                                                                          Effective Project Management With Trello                                                         By Uri Soglowek                                                     Effective Project Management: Manage Tasks and Projects, Increase Team Collaboration, and Boost Your Productivity                                                                                       767 Enrolled                                                             $47                                                                                                                                                                                                                          The Ultimate Python Programming Tutorial                                                          By Infinite Skills                                                     Python Programming tutorial for beginners. This Python Training Course Comes with Certification of Completion                                                                                       19.2K Enrolled                                                             $99                                                                                                                                                                                                                          The Java Spring Tutorial: Learn Java's Popular Web Framework                                                         By John Purcell                                                     Learn the hottest, most in-demand Java web framework, including web programming with Spring MVC and Hibernate. Lifetime access with no subscription on Udemy.                                                                                       15K Enrolled                                                             $39                                                                                                                                                                                                                          Microsoft Excel 2010: Advanced Training                                                         By Infinite Skills                                                     Master Advanced Excel 2010 Features. Become A Expert And Learn To Use Excel Like A Pro With This Advanced Excel Training                                                                                       70.4K Enrolled                                                             $99                                                                                                                                                                                                                          Become a Hadoop Developer |Training|Tutorial                                                          By Nitesh Jain                                                     Learn Hadoop and get certified &amp; bag one of the highest paying IT jobs in current times.                                                                                         12.9K Enrolled                                                             $198                                                                                                                                                                                                                          AWS Certified Solutions Architect (2013)                                                         By Linux Academy                                                     This Amazon Web Services course will focus on the concepts covered in AWS Certified Solutions Architect certifications.                                                                                       2.2K Enrolled                                                             $59                                                                                                                                                                                                                          Learn HTML5 Programming From Scratch                                                             By Eduonix Learning Solutions                                                     A Complete HTML5 Programming Course for Beginners                                                                                       198.6K Enrolled                                                             Free                                                                                                                                                                                                                          Java Tutorial for Complete Beginners                                                         By John Purcell                                                     Learn to program using the Java programming language                                                                                       492K Enrolled                                                             Free                                                                                                                                                                                                                          PLC Programming From Scratch                                                         By Paul Lynn                                                     This course will give a person with no prior experience the basic tools necessary to create  a PLC program from scratch.                                                                                       4.7K Enrolled                                                             $229                                                                                                                   About Us                                                       Udemy for Business                                                       Become an Instructor                                                       Affiliates                                                       Blog                                                       Topics                                                       Mobile Apps                                                       Support                                                       Careers                                                                                                                          English                                                                                                                                     English                                                                                                        Deutsch                                                                                                        Español                                                                                                        Français                                                                                                        Italiano                                                                                                        日本語                                                                                                        한국어                                                                                                        Português                                                                                                        Русский                                                                                                        Türkçe                                                                                                        中文(简体)                                                                                                        中文(繁體)                                                                                                                English                                                                     Deutsch                                                                     Español                                                                     Français                                                                     Italiano                                                                     日本語                                                                     한국어                                                                     Português                                                                     Русский                                                                     Türkçe                                                                     中文(简体)                                                                     中文(繁體)                                                                             Copyright © 2016 Udemy, Inc.                                                                                     Terms of Use                                                                                     Privacy Policy                                                                                     Copyright                                                         Browse Courses                                               Development                                                                              Web Development                                              Mobile Apps                                              Programming Languages                                              Game Development                                              Databases                                              Software Testing                                              Software Engineering                                              Development Tools                                              E-Commerce                                               Business                                                                              Finance                                              Entrepreneurship                                              Communications                                              Management                                              Sales                                              Strategy                                              Operations                                              Project Management                                              Business Law                                              Data &amp; Analytics                                              Home Business                                              Human Resources                                              Industry                                              Media                                              Real Estate                                              Other                                               IT &amp; Software                                                                              IT Certification                                              Network &amp; Security                                              Hardware                                              Operating Systems                                              Other                                               Office Productivity                                                                              Microsoft                                              Apple                                              Google                                              SAP                                              Intuit                                              Salesforce                                              Oracle                                              Other                                               Personal Development                                                                              Personal Transformation                                              Productivity                                              Leadership                                              Personal Finance                                              Career Development                                              Parenting &amp; Relationships                                              Happiness                                              Religion &amp; Spirituality                                              Personal Brand Building                                              Creativity                                              Influence                                              Self Esteem                                              Stress Management                                              Memory &amp; Study Skills                                              Motivation                                              Other                                               Design                                                                              Web Design                                              Graphic Design                                              Design Tools                                              User Experience                                              Game Design                                              Design Thinking                                              3D &amp; Animation                                              Fashion                                              Architectural Design                                              Interior Design                                              Other                                               Marketing                                                                              Digital Marketing                                              Search Engine Optimization                                              Social Media Marketing                                              Branding                                              Marketing Fundamentals                                              Analytics &amp; Automation                                              Public Relations                                              Advertising                                              Video &amp; Mobile Marketing                                              Content Marketing                                              Non-Digital Marketing                                              Growth Hacking                                              Affiliate Marketing                                              Product Marketing                                              Other                                               Lifestyle                                                                              Arts &amp; Crafts                                              Food &amp; Beverage                                              Beauty &amp; Makeup                                              Travel                                              Gaming                                              Home Improvement                                              Pet Care &amp; Training                                              Other                                               Photography                                                                              Digital Photography                                              Photography Fundamentals                                              Portraits                                              Landscape                                              Black &amp; White                                              Photography Tools                                              Mobile Photography                                              Travel Photography                                              Commercial Photography                                              Wedding Photography                                              Wildlife Photography                                              Video Design                                              Other                                               Health &amp; Fitness                                                                              Fitness                                              General Health                                              Sports                                              Nutrition                                              Yoga                                              Mental Health                                              Dieting                                              Self Defense                                              Safety &amp; First Aid                                              Dance                                              Meditation                                              Other                                               Teacher Training                                                                              Instructional Design                                              Educational Development                                              Teaching Tools                                              Other                                               Music                                                                              Instruments                                              Production                                              Music Fundamentals                                              Vocal                                              Music Techniques                                              Music Software                                              Other                                               Academics                                                                              Social Science                                              Math &amp; Science                                              Humanities                                               Language                                                                              English                                              Spanish                                              German                                              French                                              Japanese                                              Portuguese                                              Chinese                                              Russian                                              Latin                                              Arabic                                              Hebrew                                              Italian                                              Other                                               Test Prep                                                                              Grad Entry Exam                                              International High School                                              College Entry Exam                                              Test Taking Skills                                              Other                      Become an Instructor           Login       Sign Up                                                                                   Top Python Courses                                                                                                                              The Top Java Tutorials                                                                                                                              Excel                                                                                                                                                                    AWS Certified Solutions Architect - Associate 2016                                                         By Ryan Kroonenburg                                                     Want to pass the AWS Solutions Architect - Associate Exam? Want to become Amazon Web Services Certified? Do this course!                                                                                       26.6K Enrolled                                                             $79                                                                                                                                                                                                    ITIL Foundation Course                                                         By ITSM Zone                                                     This course will prepare you for the ITIL Foundation exam                                                                                       5.2K Enrolled                                                             $229                                                                                                                                                                                                    3D Animation: Basics To Full Body and Creature Mechanics                                                         By Charlie Grubel                                                     Learn to animate a ball bounce, bounce with a tail, standard walk and a zombie crawl! After, get a personal critique!                                                                                       163 Enrolled                                                             $49                                                                                                                                                                                                    The Complete iOS 9 Developer Course - Build 18 Apps                                                         By Rob Percival                                                     Use Xcode 7 &amp; Swift 2 to make real apps like Uber, Instagram &amp; Flappy Bird. Includes free web hosting, assets &amp; ebook.                                                                                       70.6K Enrolled                                                             $199                                                                                                                                                                                                    Photography Masterclass: Your Complete Guide to Photography                                                         By Phil Ebiner and 1 other                                                     The Best Selling Online Professional Photography Class: How to Take &amp; Sell Photos                                                                                       22.4K Enrolled                                                             $297                                                                                                                                                                                                    Learn SAP Course - Online Beginner Training                                                         By Peter Moxon                                                     Learn SAP with Peter Moxon - Ideal Beginner SAP Training Course! Unlimited Life Time Access &amp; Fully Downloadable!                                                                                       2.5K Enrolled                                                             $109                                                                                                                                                                                                    Effective Project Management With Trello                                                         By Uri Soglowek                                                     Effective Project Management: Manage Tasks and Projects, Increase Team Collaboration, and Boost Your Productivity                                                                                       767 Enrolled                                                             $47                                                                                                                                                                                                    The Ultimate Python Programming Tutorial                                                          By Infinite Skills                                                     Python Programming tutorial for beginners. This Python Training Course Comes with Certification of Completion                                                                                       19.2K Enrolled                                                             $99                                                                                                                                                                                                    The Java Spring Tutorial: Learn Java's Popular Web Framework                                                         By John Purcell                                                     Learn the hottest, most in-demand Java web framework, including web programming with Spring MVC and Hibernate. Lifetime access with no subscription on Udemy.                                                                                       15K Enrolled                                                             $39                                                                                                                                                                                                    Microsoft Excel 2010: Advanced Training                                                         By Infinite Skills                                                     Master Advanced Excel 2010 Features. Become A Expert And Learn To Use Excel Like A Pro With This Advanced Excel Training                                                                                       70.4K Enrolled                                                             $99                                                                                                                                                                                                    Become a Hadoop Developer |Training|Tutorial                                                          By Nitesh Jain                                                     Learn Hadoop and get certified &amp; bag one of the highest paying IT jobs in current times.                                                                                         12.9K Enrolled                                                             $198                                                                                                                                                                                                    AWS Certified Solutions Architect (2013)                                                         By Linux Academy                                                     This Amazon Web Services course will focus on the concepts covered in AWS Certified Solutions Architect certifications.                                                                                       2.2K Enrolled                                                             $59                                                                                                                                                                                                    Learn HTML5 Programming From Scratch                                                             By Eduonix Learning Solutions                                                     A Complete HTML5 Programming Course for Beginners                                                                                       198.6K Enrolled                                                             Free                                                                                                                                                                                                    Java Tutorial for Complete Beginners                                                         By John Purcell                                                     Learn to program using the Java programming language                                                                                       492K Enrolled                                                             Free                                                                                                                                                                                                    PLC Programming From Scratch                                                         By Paul Lynn                                                     This course will give a person with no prior experience the basic tools necessary to create  a PLC program from scratch.                                                                                       4.7K Enrolled                                                             $229                                                                                          Browse courses          Sign Up About Us Udemy for Business Become an Instructor Affiliates Blog Topics Mobile Apps Support Careers                                                               English                                             English                                       Deutsch                                       Español                                       Français                                       Italiano                                       日本語                                       한국어                                       Português                                       Русский                                       Türkçe                                       中文(简体)                                       中文(繁體)                                           Terms of Use                                               Privacy Policy                                               Copyright                       Development  Web Development Mobile Apps Programming Languages Game Development Databases Software Testing Software Engineering Development Tools E-Commerce  Business  Finance Entrepreneurship Communications Management Sales Strategy Operations Project Management Business Law Data &amp; Analytics Home Business Human Resources Industry Media Real Estate Other  IT &amp; Software  IT Certification Network &amp; Security Hardware Operating Systems Other  Office Productivity  Microsoft Apple Google SAP Intuit Salesforce Oracle Other  Personal Development  Personal Transformation Productivity Leadership Personal Finance Career Development Parenting &amp; Relationships Happiness Religion &amp; Spirituality Personal Brand Building Creativity Influence Self Esteem Stress Management Memory &amp; Study Skills Motivation Other  Design  Web Design Graphic Design Design Tools User Experience Game Design Design Thinking 3D &amp; Animation Fashion Architectural Design Interior Design Other  Marketing  Digital Marketing Search Engine Optimization Social Media Marketing Branding Marketing Fundamentals Analytics &amp; Automation Public Relations Advertising Video &amp; Mobile Marketing Content Marketing Non-Digital Marketing Growth Hacking Affiliate Marketing Product Marketing Other  Lifestyle  Arts &amp; Crafts Food &amp; Beverage Beauty &amp; Makeup Travel Gaming Home Improvement Pet Care &amp; Training Other  Photography  Digital Photography Photography Fundamentals Portraits Landscape Black &amp; White Photography Tools Mobile Photography Travel Photography Commercial Photography Wedding Photography Wildlife Photography Video Design Other  Health &amp; Fitness  Fitness General Health Sports Nutrition Yoga Mental Health Dieting Self Defense Safety &amp; First Aid Dance Meditation Other  Teacher Training  Instructional Design Educational Development Teaching Tools Other  Music  Instruments Production Music Fundamentals Vocal Music Techniques Music Software Other  Academics  Social Science Math &amp; Science Humanities  Language  English Spanish German French Japanese Portu</v>
-      </c>
-      <c r="E19" t="str">
-        <v>guese Chinese Russian Latin Arabic Hebrew Italian Other  Test Prep  Grad Entry Exam International High School College Entry Exam Test Taking Skills Other Over 9 million students More than 35,000 courses Learn at your pace on any device                                                            Top Python Courses                                                                         Top Python Courses                  Top Python Courses                                                            The Top Java Tutorials                                                                         The Top Java Tutorials                  The Top Java Tutorials                                                            Excel                                                                         Excel                  Excel                                                                                      AWS Certified Solutions Architect - Associate 2016                                                         By Ryan Kroonenburg                                                     Want to pass the AWS Solutions Architect - Associate Exam? Want to become Amazon Web Services Certified? Do this course!                                                                                       26.6K Enrolled                                                             $79                                                                                         AWS Certified Solutions Architect - Associate 2016                               By Ryan Kroonenburg                               Want to pass the AWS Solutions Architect - Associate Exam? Want to become Amazon Web Services Certified? Do this course!                                                                   26.6K Enrolled                                                             $79                                                        26.6K Enrolled                                   $79                                                                                                               ITIL Foundation Course                                                         By ITSM Zone                                                     This course will prepare you for the ITIL Foundation exam                                                                                       5.2K Enrolled                                                             $229                                                                                         ITIL Foundation Course                               By ITSM Zone                               This course will prepare you for the ITIL Foundation exam                                                                   5.2K Enrolled                                                             $229                                                        5.2K Enrolled                                   $229                                                                                                               3D Animation: Basics To Full Body and Creature Mechanics                                                         By Charlie Grubel                                                     Learn to animate a ball bounce, bounce with a tail, standard walk and a zombie crawl! After, get a personal critique!                                                                                       163 Enrolled                                                             $49                                                                                         3D Animation: Basics To Full Body and Creature Mechanics                               By Charlie Grubel                               Learn to animate a ball bounce, bounce with a tail, standard walk and a zombie crawl! After, get a personal critique!                                                                   163 Enrolled                                                             $49                                                        163 Enrolled                                   $49                                                                                                               The Complete iOS 9 Developer Course - Build 18 Apps                                                         By Rob Percival                                                     Use Xcode 7 &amp; Swift 2 to make real apps like Uber, Instagram &amp; Flappy Bird. Includes free web hosting, assets &amp; ebook.                                                                                       70.6K Enrolled                                                             $199                                                                                         The Complete iOS 9 Developer Course - Build 18 Apps                               By Rob Percival                               Use Xcode 7 &amp; Swift 2 to make real apps like Uber, Instagram &amp; Flappy Bird. Includes free web hosting, assets &amp; ebook.                                                                   70.6K Enrolled                                                             $199                                                        70.6K Enrolled                                   $199                                                                                                               Photography Masterclass: Your Complete Guide to Photography                                                         By Phil Ebiner and 1 other                                                     The Best Selling Online Professional Photography Class: How to Take &amp; Sell Photos                                                                                       22.4K Enrolled                                                             $297                                                                                         Photography Masterclass: Your Complete Guide to Photography                               By Phil Ebiner and 1 other                               The Best Selling Online Professional Photography Class: How to Take &amp; Sell Photos                                                                   22.4K Enrolled                                                             $297                                                        22.4K Enrolled                                   $297                                                                                                               Learn SAP Course - Online Beginner Training                                                         By Peter Moxon                                                     Learn SAP with Peter Moxon - Ideal Beginner SAP Training Course! Unlimited Life Time Access &amp; Fully Downloadable!                                                                                       2.5K Enrolled                                                             $109                                                                                         Learn SAP Course - Online Beginner Training                               By Peter Moxon                               Learn SAP with Peter Moxon - Ideal Beginner SAP Training Course! Unlimited Life Time Access &amp; Fully Downloadable!                                                                   2.5K Enrolled                                                             $109                                                        2.5K Enrolled                                   $109                                                                                                               Effective Project Management With Trello                                                         By Uri Soglowek                                                     Effective Project Management: Manage Tasks and Projects, Increase Team Collaboration, and Boost Your Productivity                                                                                       767 Enrolled                                                             $47                                                                                         Effective Project Management With Trello                               By Uri Soglowek                               Effective Project Management: Manage Tasks and Projects, Increase Team Collaboration, and Boost Your Productivity                                                                   767 Enrolled                                                             $47                                                        767 Enrolled                                   $47                                                                                                               The Ultimate Python Programming Tutorial                                                          By Infinite Skills                                                     Python Programming tutorial for beginners. This Python Training Course Comes with Certification of Completion                                                                                       19.2K Enrolled                                                             $99                                                                                         The Ultimate Python Programming Tutorial                                By Infinite Skills                               Python Programming tutorial for beginners. This Python Training Course Comes with Certification of Completion                                                                   19.2K Enrolled                                                             $99                                                        19.2K Enrolled                                   $99                                                                                                               The Java Spring Tutorial: Learn Java's Popular Web Framework                                                         By John Purcell                                                     Learn the hottest, most in-demand Java web framework, including web programming with Spring MVC and Hibernate. Lifetime access with no subscription on Udemy.                                                                                       15K Enrolled                                                             $39                                                                                         The Java Spring Tutorial: Learn Java's Popular Web Framework                               By John Purcell                               Learn the hottest, most in-demand Java web framework, including web programming with Spring MVC and Hibernate. Lifetime access with no subscription on Udemy.                                                                   15K Enrolled                                                             $39                                                        15K Enrolled                                   $39                                                                                                               Microsoft Excel 2010: Advanced Training                                                         By Infinite Skills                                                     Master Advanced Excel 2010 Features. Become A Expert And Learn To Use Excel Like A Pro With This Advanced Excel Training                                                                                       70.4K Enrolled                                                             $99                                                                                         Microsoft Excel 2010: Advanced Training                               By Infinite Skills                               Master Advanced Excel 2010 Features. Become A Expert And Learn To Use Excel Like A Pro With This Advanced Excel Training                                                                   70.4K Enrolled                                                             $99                                                        70.4K Enrolled                                   $99                                                                                                               Become a Hadoop Developer |Training|Tutorial                                                          By Nitesh Jain                                                     Learn Hadoop and get certified &amp; bag one of the highest paying IT jobs in current times.                                                                                         12.9K Enrolled                                                             $198                                                                                         Become a Hadoop Developer |Training|Tutorial                                By Nitesh Jain                               Learn Hadoop and get certified &amp; bag one of the highest paying IT jobs in current times.                                                                     12.9K Enrolled                                                             $198                                                        12.9K Enrolled                                   $198                                                                                                               AWS Certified Solutions Architect (2013)                                                         By Linux Academy                                                     This Amazon Web Services course will focus on the concepts covered in AWS Certified Solutions Architect certifications.                                                                                       2.2K Enrolled                                                             $59                                                                                         AWS Certified Solutions Architect (2013)                               By Linux Academy                               This Amazon Web Services course will focus on the concepts covered in AWS Certified Solutions Architect certifications.                                                                   2.2K Enrolled                                                             $59                                                        2.2K Enrolled                                   $59                                                                                                               Learn HTML5 Programming From Scratch                                                             By Eduonix Learning Solutions                                                     A Complete HTML5 Programming Course for Beginners                                                                                       198.6K Enrolled                                                             Free                                                                                         Learn HTML5 Programming From Scratch                                   By Eduonix Learning Solutions                               A Complete HTML5 Programming Course for Beginners                                                                   198.6K Enrolled                                                             Free                                                        198.6K Enrolled                                   Free                                                                                                               Java Tutorial for Complete Beginners                                                         By John Purcell                                                     Learn to program using the Java programming language                                                                                       492K Enrolled                                                             Free                                                                                         Java Tutorial for Complete Beginners                               By John Purcell                               Learn to program using the Java programming language                                                                   492K Enrolled                                                             Free                                                        492K Enrolled                                   Free                                                                                                               PLC Programming From Scratch                                                         By Paul Lynn                                                     This course will give a person with no prior experience the basic tools necessary to create  a PLC program from scratch.                                                                                       4.7K Enrolled                                                             $229                                                                                         PLC Programming From Scratch                               By Paul Lynn                               This course will give a person with no prior experience the basic tools necessary to create  a PLC program from scratch.                                                                   4.7K Enrolled                                                             $229                                                        4.7K Enrolled                                   $229                                                   Copyright © 2016 Udemy, Inc.</v>
-      </c>
-      <c r="F19" t="str">
-        <v>guese Chinese Russian Latin Arabic Hebrew Italian Other  Test Prep  Grad Entry Exam International High School College Entry Exam Test Taking Skills Other Over 9 million students More than 35,000 courses Learn at your pace on any device                                                            Top Python Courses                                                                         Top Python Courses                  Top Python Courses                                                            The Top Java Tutorials                                                                         The Top Java Tutorials                  The Top Java Tutorials                                                            Excel                                                                         Excel                  Excel                                                                                      AWS Certified Solutions Architect - Associate 2016                                                         By Ryan Kroonenburg                                                     Want to pass the AWS Solutions Architect - Associate Exam? Want to become Amazon Web Services Certified? Do this course!                                                                                       26.6K Enrolled                                                             $79                                                                                         AWS Certified Solutions Architect - Associate 2016                               By Ryan Kroonenburg                               Want to pass the AWS Solutions Architect - Associate Exam? Want to become Amazon Web Services Certified? Do this course!                                                                   26.6K Enrolled                                                             $79                                                        26.6K Enrolled                                   $79                                                                                                               ITIL Foundation Course                                                         By ITSM Zone                                                     This course will prepare you for the ITIL Foundation exam                                                                                       5.2K Enrolled                                                             $229                                                                                         ITIL Foundation Course                               By ITSM Zone                               This course will prepare you for the ITIL Foundation exam                                                                   5.2K Enrolled                                                             $229                                                        5.2K Enrolled                                   $229                                                                                                               3D Animation: Basics To Full Body and Creature Mechanics                                                         By Charlie Grubel                                                     Learn to animate a ball bounce, bounce with a tail, standard walk and a zombie crawl! After, get a personal critique!                                                                                       163 Enrolled                                                             $49                                                                                         3D Animation: Basics To Full Body and Creature Mechanics                               By Charlie Grubel                               Learn to animate a ball bounce, bounce with a tail, standard walk and a zombie crawl! After, get a personal critique!                                                                   163 Enrolled                                                             $49                                                        163 Enrolled                                   $49                                                                                                               The Complete iOS 9 Developer Course - Build 18 Apps                                                         By Rob Percival                                                     Use Xcode 7 &amp; Swift 2 to make real apps like Uber, Instagram &amp; Flappy Bird. Includes free web hosting, assets &amp; ebook.                                                                                       70.6K Enrolled                                                             $199                                                                                         The Complete iOS 9 Developer Course - Build 18 Apps                               By Rob Percival                               Use Xcode 7 &amp; Swift 2 to make real apps like Uber, Instagram &amp; Flappy Bird. Includes free web hosting, assets &amp; ebook.                                                                   70.6K Enrolled                                                             $199                                                        70.6K Enrolled                                   $199                                                                                                               Photography Masterclass: Your Complete Guide to Photography                                                         By Phil Ebiner and 1 other                                                     The Best Selling Online Professional Photography Class: How to Take &amp; Sell Photos                                                                                       22.4K Enrolled                                                             $297                                                                                         Photography Masterclass: Your Complete Guide to Photography                               By Phil Ebiner and 1 other                               The Best Selling Online Professional Photography Class: How to Take &amp; Sell Photos                                                                   22.4K Enrolled                                                             $297                                                        22.4K Enrolled                                   $297                                                                                                               Learn SAP Course - Online Beginner Training                                                         By Peter Moxon                                                     Learn SAP with Peter Moxon - Ideal Beginner SAP Training Course! Unlimited Life Time Access &amp; Fully Downloadable!                                                                                       2.5K Enrolled                                                             $109                                                                                         Learn SAP Course - Online Beginner Training                               By Peter Moxon                               Learn SAP with Peter Moxon - Ideal Beginner SAP Training Course! Unlimited Life Time Access &amp; Fully Downloadable!                                                                   2.5K Enrolled                                                             $109                                                        2.5K Enrolled                                   $109                                                                                                               Effective Project Management With Trello                                                         By Uri Soglowek                                                     Effective Project Management: Manage Tasks and Projects, Increase Team Collaboration, and Boost Your Productivity                                                                                       767 Enrolled                                                             $47                                                                                         Effective Project Management With Trello                               By Uri Soglowek                               Effective Project Management: Manage Tasks and Projects, Increase Team Collaboration, and Boost Your Productivity                                                                   767 Enrolled                                                             $47                                                        767 Enrolled                                   $47                                                                                                               The Ultimate Python Programming Tutorial                                                          By Infinite Skills                                                     Python Programming tutorial for beginners. This Python Training Course Comes with Certification of Completion                                                                                       19.2K Enrolled                                                             $99                                                                                         The Ultimate Python Programming Tutorial                                By Infinite Skills                               Python Programming tutorial for beginners. This Python Training Course Comes with Certification of Completion                                                                   19.2K Enrolled                                                             $99                                                        19.2K Enrolled                                   $99                                                                                                               The Java Spring Tutorial: Learn Java's Popular Web Framework                                                         By John Purcell                                                     Learn the hottest, most in-demand Java web framework, including web programming with Spring MVC and Hibernate. Lifetime access with no subscription on Udemy.                                                                                       15K Enrolled                                                             $39                                                                                         The Java Spring Tutorial: Learn Java's Popular Web Framework                               By John Purcell                               Learn the hottest, most in-demand Java web framework, including web programming with Spring MVC and Hibernate. Lifetime access with no subscription on Udemy.                                                                   15K Enrolled                                                             $39                                                        15K Enrolled                                   $39                                                                                                               Microsoft Excel 2010: Advanced Training                                                         By Infinite Skills                                                     Master Advanced Excel 2010 Features. Become A Expert And Learn To Use Excel Like A Pro With This Advanced Excel Training                                                                                       70.4K Enrolled                                                             $99                                                                                         Microsoft Excel 2010: Advanced Training                               By Infinite Skills                               Master Advanced Excel 2010 Features. Become A Expert And Learn To Use Excel Like A Pro With This Advanced Excel Training                                                                   70.4K Enrolled                                                             $99                                                        70.4K Enrolled                                   $99                                                                                                               Become a Hadoop Developer |Training|Tutorial                                                          By Nitesh Jain                                                     Learn Hadoop and get certified &amp; bag one of the highest paying IT jobs in current times.                                                                                         12.9K Enrolled                                                             $198                                                                                         Become a Hadoop Developer |Training|Tutorial                                By Nitesh Jain                               Learn Hadoop and get certified &amp; bag one of the highest paying IT jobs in current times.                                                                     12.9K Enrolled                                                             $198                                                        12.9K Enrolled                                   $198                                                                                                               AWS Certified Solutions Architect (2013)                                                         By Linux Academy                                                     This Amazon Web Services course will focus on the concepts covered in AWS Certified Solutions Architect certifications.                                                                                       2.2K Enrolled                                                             $59                                                                                         AWS Certified Solutions Architect (2013)                               By Linux Academy                               This Amazon Web Services course will focus on the concepts covered in AWS Certified Solutions Architect certifications.                                                                   2.2K Enrolled                                                             $59                                                        2.2K Enrolled                                   $59                                                                                                               Learn HTML5 Programming From Scratch                                                             By Eduonix Learning Solutions                                                     A Complete HTML5 Programming Course for Beginners                                                                                       198.6K Enrolled                                                             Free                                                                                         Learn HTML5 Programming From Scratch                                   By Eduonix Learning Solutions                               A Complete HTML5 Programming Course for Beginners                                                                   198.6K Enrolled                                                             Free                                                        198.6K Enrolled                                   Free                                                                                                               Java Tutorial for Complete Beginners                                                         By John Purcell                                                     Learn to program using the Java programming language                                                                                       492K Enrolled                                                             Free                                                                                         Java Tutorial for Complete Beginners                               By John Purcell                               Learn to program using the Java programming language                                                                   492K Enrolled                                                             Free                                                        492K Enrolled                                   Free                                                                                                               PLC Programming From Scratch                                                         By Paul Lynn                                                     This course will give a person with no prior experience the basic tools necessary to create  a PLC program from scratch.                                                                                       4.7K Enrolled                                                             $229                                                                                         PLC Programming From Scratch                               By Paul Lynn                               This course will give a person with no prior experience the basic tools necessary to create  a PLC program from scratch.                                                                   4.7K Enrolled                                                             $229                                                        4.7K Enrolled                                   $229                                                   Copyright © 2016 Udemy, Inc.</v>
+        <v>Udemy Online Courses Anytime Anywhere Udemy is an online education marketplace with limitless variety over 7 million students enrolled in more than 30000 coursestaught by 19000 instructors and counting What course will your life take Ready to master some skills Take your career to the next level Development Business IT Software Office Productivity Personal Development Design Marketing Lifestyle Photography Health Fitness Teacher Training Music Academics Language Test Prep Development Development Web Development Mobile Apps Programming Languages Game Development Databases Software Testing Software Engineering Development Tools ECommerce Web Development Mobile Apps Programming Languages Game Development Databases Software Testing Software Engineering Development Tools ECommerce Business Business Finance Entrepreneurship Communications Management Sales Strategy Operations Project Management Business Law Data Analytics Home Business Human Resources Industry Media Real Estate Other Finance Entrepreneurship Communications Management Sales Strategy Operations Project Management Business Law Data Analytics Home Business Human Resources Industry Media Real Estate Other IT Software IT Software IT Certification Network Security Hardware Operating Systems Other IT Certification Network Security Hardware Operating Systems Other Office Productivity Office Productivity Microsoft Apple Google SAP Intuit Salesforce Oracle Other Microsoft Apple Google SAP Intuit Salesforce Oracle Other Personal Development Personal Development Personal Transformation Productivity Leadership Personal Finance Career Development Parenting Relationships Happiness Religion Spirituality Personal Brand Building Creativity Influence Self Esteem Stress Management Memory Study Skills Motivation Other Personal Transformation Productivity Leadership Personal Finance Career Development Parenting Relationships Happiness Religion Spirituality Personal Brand Building Creativity Influence Self Esteem Stress Management Memory Study Skills Motivation Other Design Design Web Design Graphic Design Design Tools User Experience Game Design Design Thinking 3D Animation Fashion Architectural Design Interior Design Other Web Design Graphic Design Design Tools User Experience Game Design Design Thinking 3D Animation Fashion Architectural Design Interior Design Other Marketing Marketing Digital Marketing Search Engine Optimization Social Media Marketing Branding Marketing Fundamentals Analytics Automation Public Relations Advertising Video Mobile Marketing Content Marketing NonDigital Marketing Growth Hacking Affiliate Marketing Product Marketing Other Digital Marketing Search Engine Optimization Social Media Marketing Branding Marketing Fundamentals Analytics Automation Public Relations Advertising Video Mobile Marketing Content Marketing NonDigital Marketing Growth Hacking Affiliate Marketing Product Marketing Other Lifestyle Lifestyle Arts Crafts Food Beverage Beauty Makeup Travel Gaming Home Improvement Pet Care Training Other Arts Crafts Food Beverage Beauty Makeup Travel Gaming Home Improvement Pet Care Training Other Photography Photography Digital Photography Photography Fundamentals Portraits Landscape Black White Photography Tools Mobile Photography Travel Photography Commercial Photography Wedding Photography Wildlife Photography Video Design Other Digital Photography Photography Fundamentals Portraits Landscape Black White Photography Tools Mobile Photography Travel Photography Commercial Photography Wedding Photography Wildlife Photography Video Design Other Health Fitness Health Fitness Fitness General Health Sports Nutrition Yoga Mental Health Dieting Self Defense Safety First Aid Dance Meditation Other Fitness General Health Sports Nutrition Yoga Mental Health Dieting Self Defense Safety First Aid Dance Meditation Other Teacher Training Teacher Training Instructional Design Educational Development Teaching Tools Other Instructional Design Educational Development Teaching Tools Other Music Music Instruments Production Music Fundamentals Vocal Music Techniques Music Software Other Instruments Production Music Fundamentals Vocal Music Techniques Music Software Other Academics Academics Social Science Math Science Humanities Social Science Math Science Humanities Language Language English Spanish German French Japanese Portuguese Chinese Russian Latin Arabic Hebrew Italian Other English Spanish German French Japanese Portuguese Chinese Russian Latin Arabic Hebrew Italian Other Test Prep Test Prep Grad Entry Exam International High School College Entry Exam Test Taking Skills Other Grad Entry Exam International High School College Entry Exam Test Taking Skills Other Over 9 million students More than 35000 courses Learn at your pace on any device Top Python Courses The Top Java Tutorials Excel AWS Certified Solutions Architect Associate 2016 By Ryan Kroonenburg Want to pass the AWS Solutions Architect Associate Exam Want to become Amazon Web Services Certified Do this course 267K Enrolled 79 ITIL Foundation Course By ITSM Zone This course will prepare you for the ITIL Foundation exam 52K Enrolled 229 3D Animation Basics To Full Body and Creature Mechanics By Charlie Grubel Learn to animate a ball bounce bounce with a tail standard walk and a zombie crawl After get a personal critique 163 Enrolled 49 The Complete iOS 9 Developer Course Build 18 Apps By Rob Percival Use Xcode 7 Swift 2 to make real apps like Uber Instagram Flappy Bird Includes free web hosting assets ebook 707K Enrolled 199 Photography Masterclass Your Complete Guide to Photography By Phil Ebiner and 1 other The Best Selling Online Professional Photography Class How to Take Sell Photos 224K Enrolled 297 Learn SAP Course Online Beginner Training By Peter Moxon Learn SAP with Peter Moxon Ideal Beginner SAP Training Course Unlimited Life Time Access Fully Downloadable 25K Enrolled 109 Effective Project Management With Trello By Uri Soglowek Effective Project Management Manage Tasks and Projects Increase Team Collaboration and Boost Your Productivity 767 Enrolled 47 The Ultimate Python Programming Tutorial By Infinite Skills Python Programming tutorial for beginners This Python Training Course Comes with Certification of Completion 192K Enrolled 99 The Java Spring Tutorial Learn Javas Popular Web Framework By John Purcell Learn the hottest most indemand Java web framework including web programming with Spring MVC and Hibernate Lifetime access with no subscription on Udemy 15K Enrolled 39 Microsoft Excel 2010 Advanced Training By Infinite Skills Master Advanced Excel 2010 Features Become A Expert And Learn To Use Excel Like A Pro With This Advanced Excel Training 704K Enrolled 99 Become a Hadoop Developer TrainingTutorial By Nitesh Jain Learn Hadoop and get certified bag one of the highest paying IT jobs in current times 129K Enrolled 198 AWS Certified Solutions Architect 2013 By Linux Academy This Amazon Web Services course will focus on the concepts covered in AWS Certified Solutions Architect certifications 22K Enrolled 59 Learn HTML5 Programming From Scratch By Eduonix Learning Solutions A Complete HTML5 Programming Course for Beginners 1987K Enrolled Free Java Tutorial for Complete Beginners By John Purcell Learn to program using the Java programming language 4922K Enrolled Free PLC Programming From Scratch By Paul Lynn This course will give a person with no prior experience the basic tools necessary to create a PLC program from scratch 47K Enrolled 229 About Us Udemy for Business Become an Instructor Affiliates Blog Topics Mobile Apps Support Careers English English Deutsch Español Français Italiano 日本語 한국어 Português Русский Türkçe 中文简体 中文繁體 English Deutsch Español Français Italiano 日本語 한국어 Português Русский Türkçe 中文简体 中文繁體 Copyright © 2016 Udemy Inc Terms of Use Privacy Policy Copyright Browse Courses Development Web Development Mobile Apps Programming Languages Game Development Databases Software Testing Software Engineering Development Tools ECommerce Business Finance Entrepreneurship Communications Management Sales Strategy Operations Project Management Business Law Data Analytics Home Business Human Resources Industry Media Real Estate Other IT Software IT Certification Network Security Hardware Operating Systems Other Office Productivity Microsoft Apple Google SAP Intuit Salesforce Oracle Other Personal Development Personal Transformation Productivity Leadership Personal Finance Career Development Parenting Relationships Happiness Religion Spirituality Personal Brand Building Creativity Influence Self Esteem Stress Management Memory Study Skills Motivation Other Design Web Design Graphic Design Design Tools User Experience Game Design Design Thinking 3D Animation Fashion Architectural Design Interior Design Other Marketing Digital Marketing Search Engine Optimization Social Media Marketing Branding Marketing Fundamentals Analytics Automation Public Relations Advertising Video Mobile Marketing Content Marketing NonDigital Marketing Growth Hacking Affiliate Marketing Product Marketing Other Lifestyle Arts Crafts Food Beverage Beauty Makeup Travel Gaming Home Improvement Pet Care Training Other Photography Digital Photography Photography Fundamentals Portraits Landscape Black White Photography Tools Mobile Photography Travel Photography Commercial Photography Wedding Photography Wildlife Photography Video Design Other Health Fitness Fitness General Health Sports Nutrition Yoga Mental Health Dieting Self Defense Safety First Aid Dance Meditation Other Teacher Training Instructional Design Educational Development Teaching Tools Other Music Instruments Production Music Fundamentals Vocal Music Techniques Music Software Other Academics Social Science Math Science Humanities Language English Spanish German French Japanese Portuguese Chinese Russian Latin Arabic Hebrew Italian Other Test Prep Grad Entry Exam International High School College Entry Exam Test Taking Skills Other Become an Instructor Login Sign Up Top Python Courses The Top Java Tutorials Excel AWS Certified Solutions Architect Associate 2016 By Ryan Kroonenburg Want to pass the AWS Solutions Architect Associate Exam Want to become Amazon Web Services Certified Do this course 267K Enrolled 79 ITIL Foundation Course By ITSM Zone This course will prepare you for the ITIL Foundation exam 52K Enrolled 229 3D Animation Basics To Full Body and Creature Mechanics By Charlie Grubel Learn to animate a ball bounce bounce with a tail standard walk and a zombie crawl After get a personal critique 163 Enrolled 49 The Complete iOS 9 Developer Course Build 18 Apps By Rob Percival Use Xcode 7 Swift 2 to make real apps like Uber Instagram Flappy Bird Includes free web hosting assets ebook 707K Enrolled 199 Photography Masterclass Your Complete Guide to Photography By Phil Ebiner and 1 other The Best Selling Online Professional Photography Class How to Take Sell Photos 224K Enrolled 297 Learn SAP Course Online Beginner Training By Peter Moxon Learn SAP with Peter Moxon Ideal Beginner SAP Training Course Unlimited Life Time Access Fully Downloadable 25K Enrolled 109 Effective Project Management With Trello By Uri Soglowek Effective Project Management Manage Tasks and Projects Increase Team Collaboration and Boost Your Productivity 767 Enrolled 47 The Ultimate Python Programming Tutorial By Infinite Skills Python Programming tutorial for beginners This Python Training Course Comes with Certification of Completion 192K Enrolled 99 The Java Spring Tutorial Learn Javas Popular Web Framework By John Purcell Learn the hottest most indemand Java web framework including web programming with Spring MVC and Hibernate Lifetime access with no subscription on Udemy 15K Enrolled 39 Microsoft Excel 2010 Advanced Training By Infinite Skills Master Advanced Excel 2010 Features Become A Expert And Learn To Use Excel Like A Pro With This Advanced Excel Training 704K Enrolled 99 Become a Hadoop Developer TrainingTutorial By Nitesh Jain Learn Hadoop and get certified bag one of the highest paying IT jobs in current times 129K Enrolled 198 AWS Certified Solutions Architect 2013 By Linux Academy This Amazon Web Services course will focus on the concepts covered in AWS Certified Solutions Architect certifications 22K Enrolled 59 Learn HTML5 Programming From Scratch By Eduonix Learning Solutions A Complete HTML5 Programming Course for Beginners 1987K Enrolled Free Java Tutorial for Complete Beginners By John Purcell Learn to program using the Java programming language 4922K Enrolled Free PLC Programming From Scratch By Paul Lynn This course will give a person with no prior experience the basic tools necessary to create a PLC program from scratch 47K Enrolled 229 Browse courses Sign Up About Us Udemy for Business Become an Instructor Affiliates Blog Topics Mobile Apps Support Careers English English Deutsch Español Français Italiano 日本語 한국어 Português Русский Türkçe 中文简体 中文繁體 Terms of Use Privacy Policy Copyright Development Web Development Mobile Apps Programming Languages Game Development Databases Software Testing Software Engineering Development Tools ECommerce Business Finance Entrepreneurship Communications Management Sales Strategy Operations Project Management Business Law Data Analytics Home Business Human Resources Industry Media Real Estate Other IT Software IT Certification Network Security Hardware Operating Systems Other Office Productivity Microsoft Apple Google SAP Intuit Salesforce Oracle Other Personal Development Personal Transformation Productivity Leadership Personal Finance Career Development Parenting Relationships Happiness Religion Spirituality Personal Brand Building Creativity Influence Self Esteem Stress Management Memory Study Skills Motivation Other Design Web Design Graphic Design Design Tools User Experience Game Design Design Thinking 3D Animation Fashion Architectural Design Interior Design Other Marketing Digital Marketing Search Engine Optimization Social Media Marketing Branding Marketing Fundamentals Analytics Automation Public Relations Advertising Video Mobile Marketing Content Marketing NonDigital Marketing Growth Hacking Affiliate Marketing Product Marketing Other Lifestyle Arts Crafts Food Beverage Beauty Makeup Travel Gaming Home Improvement Pet Care Training Other Photography Digital Photography Photography Fundamentals Portraits Landscape Black White Photography Tools Mobile Photography Travel Photography Commercial Photography Wedding Photography Wildlife Photography Video Design Other Health Fitness Fitness General Health Sports Nutrition Yoga Mental Health Dieting Self Defense Safety First Aid Dance Meditation Other Teacher Training Instructional Design Educational Development Teaching Tools Other Music Instruments Production Music Fundamentals Vocal Music Techniques Music Software Other Academics Social Science Math Science Humanities Language English Spanish German French Japanese Portuguese Chinese Russian Latin Arabic Hebrew Italian Other Test Prep Grad Entry Exam International High School College Entry Exam Test Taking Skills Other Over 9 million students More than 35000 courses Learn at your pace on any device Top Python Courses Top Python Courses Top Python Courses The Top Java Tutorials The Top Java Tutorials The Top Java Tutorials Excel Excel Excel AWS Certified Solutions Architect Associate 2016 By Ryan Kroonenburg Want to pass the AWS Solutions Architect Associate Exam Want to become Amazon Web Services Certified Do this course 267K Enrolled 79 AWS Certified Solutions Architect Associate 2016 By Ryan Kroonenburg Want to pass the AWS Solutions Architect Associate Exam Want to become Amazon Web Services Certified Do this course 267K Enrolled 79 267K Enrolled 79 ITIL Foundation Course By ITSM Zone This course will prepare you for the ITIL Foundation exam 52K Enrolled 229 ITIL Foundation Course By ITSM Zone This course will prepare you for the ITIL Foundation exam 52K Enrolled 229 52K Enrolled 229 3D Animation Basics To Full Body and Creature Mechanics By Charlie Grubel Learn to animate a ball bounce bounce with a tail standard walk and a zombie crawl After get a personal critique 163 Enrolled 49 3D Animation Basics To Full Body and Creature Mechanics By Charlie Grubel Learn to animate a ball bounce bounce with a tail standard walk and a zombie crawl After get a personal critique 163 Enrolled 49 163 Enrolled 49 The Complete iOS 9 Developer Course Build 18 Apps By Rob Percival Use Xcode 7 Swift 2 to make real apps like Uber Instagram Flappy Bird Includes free web hosting assets ebook 707K Enrolled 199 The Complete iOS 9 Developer Course Build 18 Apps By Rob Percival Use Xcode 7 Swift 2 to make real apps like Uber Instagram Flappy Bird Includes free web hosting assets ebook 707K Enrolled 199 707K Enrolled 199 Photography Masterclass Your Complete Guide to Photography By Phil Ebiner and 1 other The Best Selling Online Professional Photography Class How to Take Sell Photos 224K Enrolled 297 Photography Masterclass Your Complete Guide to Photography By Phil Ebiner and 1 other The Best Selling Online Professional Photography Class How to Take Sell Photos 224K Enrolled 297 224K Enrolled 297 Learn SAP Course Online Beginner Training By Peter Moxon Learn SAP with Peter Moxon Ideal Beginner SAP Training Course Unlimited Life Time Access Fully Downloadable 25K Enrolled 109 Learn SAP Course Online Beginner Training By Peter Moxon Learn SAP with Peter Moxon Ideal Beginner SAP Training Course Unlimited Life Time Access Fully Downloadable 25K Enrolled 109 25K Enrolled 109 Effective Project Management With Trello By Uri Soglowek Effective Project Management Manage Tasks and Projects Increase Team Collaboration and Boost Your Productivity 767 Enrolled 47 Effective Project Management With Trello By Uri Soglowek Effective Project Management Manage Tasks and Projects Increase Team Collaboration and Boost Your Productivity 767 Enrolled 47 767 Enrolled 47 The Ultimate Python Programming Tutorial By Infinite Skills Python Programming tutorial for beginners This Python Training Course Comes with Certification of Completion 192K Enrolled 99 The Ultimate Python Programming Tutorial By Infinite Skills Python Programming tutorial for beginners This Python Training Course Comes with Certification of Completion 192K Enrolled 99 192K Enrolled 99 The Java Spring Tutorial Learn Javas Popular Web Framework By John Purcell Learn the hottest most indemand Java web framework including web programming with Spring MVC and Hibernate Lifetime access with no subscription on Udemy 15K Enrolled 39 The Java Spring Tutorial Learn Javas Popular Web Framework By John Purcell Learn the hottest most indemand Java web framework including web programming with Spring MVC and Hibernate Lifetime access with no subscription on Udemy 15K Enrolled 39 15K Enrolled 39 Microsoft Excel 2010 Advanced Training By Infinite Skills Master Advanced Excel 2010 Features Become A Expert And Learn To Use Excel Like A Pro With This Advanced Excel Training 704K Enrolled 99 Microsoft Excel 2010 Advanced Training By Infinite Skills Master Advanced Excel 2010 Features Become A Expert And Learn To Use Excel Like A Pro With This Advanced Excel Training 704K Enrolled 99 704K Enrolled 99 Become a Hadoop Developer TrainingTutorial By Nitesh Jain Learn Hadoop and get certified bag one of the highest paying IT jobs in current times 129K Enrolled 198 Become a Hadoop Developer TrainingTutorial By Nitesh Jain Learn Hadoop and get certified bag one of the highest paying IT jobs in current times 129K Enrolled 198 129K Enrolled 198 AWS Certified Solutions Architect 2013 By Linux Academy This Amazon Web Services course will focus on the concepts covered in AWS Certified Solutions Architect certifications 22K Enrolled 59 AWS Certified Solutions Architect 2013 By Linux Academy This Amazon Web Services course will focus on the concepts covered in AWS Certified Solutions Architect certifications 22K Enrolled 59 22K Enrolled 59 Learn HTML5 Programming From Scratch By Eduonix Learning Solutions A Complete HTML5 Programming Course for Beginners 1987K Enrolled Free Learn HTML5 Programming From Scratch By Eduonix Learning Solutions A Complete HTML5 Programming Course for Beginners 1987K Enrolled Free 1987K Enrolled Free Java Tutorial for Complete Beginners By John Purcell Learn to program using the Java programming language 4922K Enrolled Free Java Tutorial for Complete Beginners By John Purcell Learn to program using the Java programming language 4922K Enrolled Free 4922K Enrolled Free PLC Programming From Scratch By Paul Lynn This course will give a person with no prior experience the basic tools necessary to create a PLC program from scratch 47K Enrolled 229 PLC Programming From Scratch By Paul Lynn This course will give a person with no prior experience the basic tools necessary to create a PLC program from scratch 47K Enrolled 229 47K Enrolled 229 Copyright © 2016 Udemy Inc</v>
       </c>
     </row>
     <row r="20">
@@ -753,16 +600,7 @@
         <v>Training and dev</v>
       </c>
       <c r="C20" t="str">
-        <v>Online software tutorials, training CDs, Photoshop Tutorials, Dreamweaver Tutorials, Apple Tutorials from vtc.com vtc.com provides the latest Apple Tutorials, Adobe Tutorials, Cakewalk Tutorials, Corel Tutorials, Dreamweaver Tutorials, Macromedia Tutorials, Microsoft Tutorials, Oracle Tutorials, Photoshop Tutorials and Sony Tutorials as high quality quicktime videos Affordable software training Individuals and students Businesses and corporations Colleges and universities Easy-to-understand video tutorials Learn anywhere, at your own pace Train your staff easily and affordably Educate groups of students easily Popular courses New releases Categories Software or Publisher Recent Releases Resources Community VTC Terms and Conditions ONLINE DOWNLOAD USB FAST PORTABLE CERTIFICATES FLEXIBLE PRACTICAL COMPATIBLE LDAP / LCMS TRACKING EASY ADMIN COURSE LIST ONLINE ACCESS Business Applications Programming Certification Certification Programming Audio Home     About Us              Affiliates             Information         Register       Login                  Send Feedback           Customer Suggestions      Technical Problems             Support             Contact      About Us Affiliates             Information         Register       Login            Information Register Login Send Feedback           Customer Suggestions      Technical Problems          Customer Suggestions Technical Problems Support          Contact All Courses Categories Recent Releases Popular Courses In Development Animation &amp; 3D Audio Bundles Business Applications CAD  Certification Databases Game Design &amp; Development Graphics &amp; Page Layout Internet &amp; Web Design MasterClass! Multimedia &amp; Video Networking &amp; Security Operating Systems Programming Project Management QuickStart! Professional Podcasting Quickbooks Online Quickstart! Dropbox Corel Painter 2016 Zencart Service Oriented Architecture Part 2 Cubase 8 College Preparation Course Getting Started with Office 365 for Business QuickStart! - Adobe Flash Professional CC QuickStart! - Adobe Dreamweaver CC Installing and Configuring Windows Server 2012 (Exam 70-410) QuickStart! - Adobe Illustrator CC QuickStart! - Adobe Audition CC Advanced Java Programming (Java SE 7) QuickStart! - Adobe Premiere CC Microsoft Project 2013 CompTIA Linux+ (Exam LX0-101) Moodle Avid Media Composer 6 Advanced Ethical Hacking QuickStart! - 3D Printing Wireless Hacking and Security Prince2� - 2013 Foundation and Practitioner Exam Prep iOS 7 Microsoft Windows 7 Configuration (Exam 70-680) Configuring Microsoft Windows 8 (Exam 70-687) Pricing Help                                                                                                                                                                                            function ssLoadMovie(movieNum) {         // Bring in user agent detection result from PHP        var mobileDevice = 0;         if (ssMovieLoaded01 == false) {         jwplayer('movie-'+movieNum).setup({          width: 719,          height: 272,          duration: 223,          screencolor: '#0b2a37',          image: 'http://www.vtc.com/templates/country/en_free/images/jwplayer-bg.png',          stretching: 'fill',          autostart: true,          bufferlength: '10',          skin: 'http://www.vtc.com/templates/country/en_free/images/learnMore/skins/vtcwebbanner/vtcwebbanner.zip',          wmode: 'transparent',          'controlbar.idlehide': true,          modes: [           { type: 'html5' },           { type: 'flash', src: 'http://www.vtc.com/templates/country/en_free/images/learnMore/player.swf?file=http://www.vtc.com/templates/country/en_free/images/learnMore/media/movie-'+movieNum+'c.mp4&amp;image=http://www.vtc.com/templates/country/en_free/images/jwplayer-bg.png&amp;autostart=true' },           { type: 'download' }          ],          levels: [           { file: 'http://www.vtc.com/templates/country/en_free/images/learnMore/media/movie-'+movieNum+'c.mp4' }          ]         });         ssMovieLoaded01 = true;         //console.log('Movie loaded.');         jwplayer().onPause(function() {          ssMoviePlaying = false;         });         jwplayer().onPlay(function() {          ssMoviePlaying = true;         });         if (mobileDevice == 0) {          ssEnableOverlay();          jwplayer().getPlugin("controlbar").onHide(function() {           $('.movie-overlay-wrapper').fadeOut(100);          });          jwplayer().getPlugin("controlbar").onShow(function() {           $('.movie-overlay-wrapper').fadeIn(100);          });         }        }       }                            Affordable software training        Easy-to-understand video tutorials                                                                ONLINE                                  Get full access to our entire library!                                                                                                                                  DOWNLOAD                                  Save to your own drive or device                                                                                                                  USB                                  Portable training on the move                                                                                   Thanks VTC! I've learned more stuff in here and much faster than if I had bought a book or slept through a class. Keep up the good work and keep on...        Arellano Torres        more              LEARN MORE                                   ONLINE                                  Get full access to our entire library!                                                         DOWNLOAD                                  Save to your own drive or device                                                                    USB                                  Portable training on the move                                                                   Individuals and students        Learn anywhere, at your own pace                                                                FAST                                  No time consuming class schedules                                                                 PORTABLE                                  Train anywhere,whenever you want                                                                 CERTIFICATES                                  Certificates uponcourse completion                                                                                                      FileMaker Pro 12: Beginner, Intermediate &amp; Advanced Bundle                       FileMaker Pro 12: Beginner                       Microsoft Project 2013                       Quickstart! Dropbox                       Advanced Solutions of Microsoft SharePoint Server 2013 (Exam 70-332)                       Microsoft Office 2013 Bundle                       MCTS: Microsoft SharePoint 2010 Bundle                       QuickStart! - WampServer                                  LEARN MORE                                   FAST                                  No time consuming class schedules                                                        PORTABLE                                  Train anywhere,whenever you want                                                        CERTIFICATES                                  Certificates uponcourse completion                                 FileMaker Pro 12: Beginner, Intermediate &amp; Advanced Bundle FileMaker Pro 12: Beginner Microsoft Project 2013 Quickstart! Dropbox Advanced Solutions of Microsoft SharePoint Server 2013 (Exam 70-332) Microsoft Office 2013 Bundle MCTS: Microsoft SharePoint 2010 Bundle QuickStart! - WampServer                                   Businesses and corporations        Train your staff easily and affordably                                                                FLEXIBLE                                  Staff can sharemulti user accounts                                                                 PRACTICAL                                  Reduce supportcalls and costs                                                                 COMPATIBLE                                  Works with Windows, Mac and Linux                                                                                                      QuickStart! - Adobe Bridge CS6                   Adobe Encore CS6                   Microsoft SQL Server 2012 Development (Exam 70-464)                   Planning a Successful Website                   QuickStart! - VTC Help Movies                   Java Mobile Android Advanced Apps                   Apple Motion 2014                   Intermediate Oracle 11g                              LEARN MORE                                   FLEXIBLE                                  Staff can sharemulti user accounts                                                        PRACTICAL                                  Reduce supportcalls and costs                                                        COMPATIBLE                                  Works with Windows, Mac and Linux                                 QuickStart! - Adobe Bridge CS6 Adobe Encore CS6 Microsoft SQL Server 2012 Development (Exam 70-464) Planning a Successful Website QuickStart! - VTC Help Movies Java Mobile Android Advanced Apps Apple Motion 2014 Intermediate Oracle 11g                                   Colleges and universities        Educate groups of students easily                                                                LDAP / LCMS                                  Integrate with existing systems                                                                 TRACKING                                  Quickly monitor student progress                                                                 EASY ADMIN                                  Full per-user account control                                                                                                      Photoshop CC for Photographers                   JavaScript (1.8.5)                   QuickStart! - Responsive Dreamweaver CS6 Websites                   FileMaker Pro 13: Beginner                   MCSE: SharePoint Solutions Expert Bundle                   QuickStart! - Adobe Premiere Elements 11                   Data Structures and Algorithms in C++                   HTML5 + CSS3 Responsive Web Design                              LEARN MORE                                   LDAP / LCMS                                  Integrate with existing systems                                                        TRACKING                                  Quickly monitor student progress                                                        EASY ADMIN                                  Full per-user account control                                 Photoshop CC for Photographers JavaScript (1.8.5) QuickStart! - Responsive Dreamweaver CS6 Websites FileMaker Pro 13: Beginner MCSE: SharePoint Solutions Expert Bundle QuickStart! - Adobe Premiere Elements 11 Data Structures and Algorithms in C++ HTML5 + CSS3 Responsive Web Design              TRAINING TYPES                         FOR INDIVIDUALS                         FOR BUSINESS                         FOR COLLEGES                                                                      Business Applications Quickstart Office 365                                                                Programming Moodle                                                                Certification Red Hat Certified Engineer (RHCE) - Exam EX300                                                                Certification Oracle: Introduction to Oracle SQL and PL/SQL                                                                Programming  Service Oriented Architecture Part 2                                                                       Audio  Cubase 8             Feedback Become an Author Suggest a Course Verify Certificate Access Cards Authors Animation &amp; 3D Audio Bundles Business Applications CAD Certification Databases Game Design &amp; Development Graphics &amp; Page Layout Internet &amp; Web Design MasterClass! Multimedia &amp; Video Networking &amp; Security Operating Systems Programming Project Management QuickStart! Ableton Tutorials Adobe Tutorials Apache Tutorials Apple Tutorials Autodesk Tutorials Avid Tutorials Cakewalk Tutorials CompTIA Tutorials Corel Tutorials Dreamweaver Tutorials FileMaker Tutorials Java Tutorials Linux Tutorials Flash Tutorials Microsoft Tutorials MySQL Tutorials Oracle Tutorials Photoshop Tutorials PHP Tutorials Sony Tutorials Professional Podcasting Quickbooks Online Quickstart! Dropbox Corel Painter 2016 Zencart Service Oriented Architecture  Cubase 8 College Preparation Course Getting Started with Office 36 VTC Player VTC iPad App Access Card Verify Certificate Become a VTC Author! Site Map About Us Support FAQ Contact Terms and Conditions Facebook Twitter LinkedIn Blog                   Sign up |                   |                                   Username                                                                                                 Password                                                                                                                                   Remember me                                  After Login                                 Go to my home page                                                                    Stay on current page                                                                                                             Forgot password?                                                             Thanks VTC! I've learned more stuff in here and much faster than if I had bought a book or slept through a class. Keep up the good work and keep on... Arellano Torres more Client and visitor information gathered by VTC is used ONLY by VTC, our lists are never rented or sold. For more information, view our privacy policy. TERMS        &amp; CONDITIONS OF USE  BY SUBSCRIBING TO THIS SERVICE, YOU ARE CONSENTING             TO BE BOUND BY AND ARE BECOMING A PARTY TO THIS AGREEMENT, THE TERMS             AND CONDITIONS OF WHICH SHALL PREVAIL IN GOVERNING YOUR RIGHTS OF             USE. BY CLICKING THE "BECOME A MEMBER" BUTTON, THE INDIVIDUAL             OR ENTITY LICENSING THE PRODUCT ("YOU") IS CONSENTING TO             BE BOUND BY AND IS BECOMING A PARTY TO THIS AGREEMENT. IF LICENSEE             DOES NOT AGREE TO ALL OF THE TERMS OF THIS AGREEMENT, THE BUTTON             INDICATING "BECOME A MEMBER" MUST NOT BE SELECTED, AND             LICENSEE MUST NOT INSTALL OR USE THE SOFTWARE. 1. DEFINITIONS   "VTC" refers to Virtual Training Company,           Inc.         "You" refers to the user or subscriber.          "Software" refers to the VTC training content and software.  2. LICENSE: VTC hereby grants to You a worldwide,           non-royalty bearing, non-exclusive license to use the Software according           to the provisions contained herein and subject to payment of the applicable           subscription fees.  3. RESTRICTIONS: You may not do any of the following:  Save the Software to Your hard disk or other storage           medium; permit others to use the Software except as specified by addendum;           modify, reverse engineer, decompile, or disassemble the Software; make           derivative works based on the Software; publish or otherwise disseminate           the Software. VTC, Inc., VTC Online University, and the Virtual Training           Company site is owned and operated by VTC, Inc. as a corporation of           record.         All materials on this site are the property of VTC unless otherwise specified.         No material from these pages may be copied, reproduced, republished,         downloaded, uploaded, posted, transmitted, or distributed in any way.         Modification of the materials or use of the materials for any other purpose         is a violation of U.S. copyright law and other proprietary rights. For         purposes of this Agreement, the use of any such material on any other         web site or networked computer environment is prohibited.  4. FEES: The rights granted under this Agreement           are effective only upon payment of the subscription fees, which are           strictly non-refundable other than as expressly provided herein. The           term "monthly subscription" is defined as any 30 day period.           The term "yearly subscription" is defined as one 365 day           period. A yearly subscription ends on the same numerical date as it           began (example July 28, 2004 to July 28, 2005).                                      The VTC Online University is access to every VTC training tutorial in         our library. You pay a flat fee for access         to these titles. You are billed according to your renewal selection below,         and can renew monthly, yearly, or in any other increment offered. If         you choose to be billed monthly, you will be billed every 30 days for         the subscription until you request the subscription be cancelled. Our terms of service state that you must cancel a monthly subscription at least two business days before your renewal date. These two days give us enough time to ensure that you will not be charged again.  5. LIMITED WARRANTY: VTC warrants that the Software,           if operated as directed, will substantially achieve the functionality           described. VTC does not warrant, however, that Your use of the Software           will be uninterrupted or that the operation of the Software will be           error-free or secure. In addition, the security mechanisms implemented           by the Software have inherent limitations, and You must determine that           the Software sufficiently meets Your requirements. VTC also warrants           that the media containing the Software, if provided by VTC, is free           from defects in material from the date You acquired the Software. VTC's           sole liability for any breach of this warranty shall be, in VTC's sole           discretion: (i) to replace Your defective media or Software; or (ii)           to advise You how to achieve substantially the same functionality with           the Software as described; or (iii) if the above remedies are impracticable,           to refund the subscription fee You paid for the Software. Only if You           inform VTC of Your problem with the Software during the applicable           subscription period will VTC be obligated to honor this warranty. VTC           will use reasonable commercial efforts to repair, replace, advise,           or refund pursuant to the foregoing warranty within thirty (30) days           of being so notified. If any modifications are made to the Software           by You during the warranty period; if the medium is subjected to accident,           abuse, or improper use; or if You violate the terms of this Agreement,           then this warranty shall immediately terminate. This warranty shall           not apply if the Software is used on or in conjunction with hardware           or software other than the unmodified version of hardware and software           with which the Software was designed to be used as described.  THIS IS A LIMITED WARRANTY, AND IT IS THE ONLY           WARRANTY MADE BY VTC OR ITS SUPPLIERS. VTC MAKES NO OTHER WARRANTIES,           EXPRESS OR IMPLIED, INCLUDING BUT NOT LIMITED TO WARRANTIES OF MERCHANTABILITY,           FITNESS FOR A PARTICULAR PURPOSE, AND NONINFRINGEMENT OF THIRD PARTIES'           RIGHTS. YOU MAY HAVE OTHER STATUTORY RIGHTS. HOWEVER, TO THE FULL EXTENT           PERMITTED BY LAW, THE DURATION OF STATUTORILY REQUIRED WARRANTIES,           IF ANY, SHALL BE LIMITED TO THE ABOVE LIMITED WARRANTY PERIOD. MOREOVER,           IN NO EVENT WILL WARRANTIES PROVIDED BY LAW, IF ANY, APPLY UNLESS THEY           ARE REQUIRED TO APPLY BY STATUTE NOTWITHSTANDING THEIR EXCLUSION BY           CONTRACT. NO DEALER, AGENT, OR EMPLOYEE OF VTC IS AUTHORIZED TO MAKE           ANY MODIFICATIONS, EXTENSIONS, OR ADDITIONS TO THIS LIMITED WARRANTY.  6. PROPRIETARY RIGHTS: VTC reserves all proprietary           rights in and to the Software, is protected by copyright and other           intellectual property laws and by international treaties. VTC, Inc.  Trademark Notice: VTC, Virtual Training Company,           Inc., The VTC Logo, and VTC Online University, are trademarks of VTC,           Inc. All other company and product names may be trademarks of their           respective owners.         The information contained herein is subject to change without notice.         Copyright © 1995 - 2005 VTC, Inc. All rights reserved.  7. TERMINATION: This Agreement shall automatically           terminate if You fail to comply with the restrictions described herein.           Your obligations to pay outstanding subscription fees shall survive           any termination of this Agreement.  8. LIMITATION OF LIABILITY: UNDER NO CIRCUMSTANCES           AND UNDER NO LEGAL THEORY, TORT, CONTRACT, OR OTHERWISE, SHALL VTC           OR ITS SUPPLIERS OR RESELLERS BE LIABLE TO YOU OR ANY OTHER PERSON           FOR ANY INDIRECT, SPECIAL, INCIDENTAL, OR CONSEQUENTIAL DAMAGES OF           ANY CHARACTER, INCLUDING WITHOUT LIMITATION, DAMAGES FOR LOSS OF GOODWILL,           WORK STOPPAGE, COMPUTER FAILURE OR MALFUNCTION, OR ANY AND ALL OTHER           COMMERCIAL DAMAGES OR LOSSES. IN NO EVENT WILL VTC BE LIABLE FOR ANY           DAMAGES IN EXCESS OF THE AMOUNT VTC RECEIVED FROM YOU FOR A LICENSE           TO THE SOFTWARE, EVEN IF VTC SHALL HAVE BEEN INFORMED OF THE POSSIBILITY           OF SUCH         DAMAGES, OR FOR ANY CLAIM BY ANY OTHER PARTY. THIS LIMITATION OF LIABILITY         SHALL NOT APPLY TO LIABILITY FOR DEATH OR PERSONAL INJURY RESULTING FROM         VTC'S NEGLIGENCE TO THE EXTENT APPLICABLE LAW PROHIBITS SUCH LIMITATION.         SOME JURISDICTIONS DO NOT ALLOW THE EXCLUSION OR LIMITATION OF INCIDENTAL         OR CONSEQUENTIAL DAMAGES, SO THIS EXCLUSION AND LIMITATION MAY NOT APPLY         TO YOU.  9. Links To Other Materials: Linked sites found           at the VTC site are not under the control of VTC, and we are not responsible           for the content of any linked site or any link contained in a linked           site. VTC may change links based solely on our discretion, and we reserve           the right to terminate any link or linking program at any time. VTC           does not, by linking to sites, endorse companies or products to which           it links and reserves the right to note as such on its web pages. If           you decide to access any of the third party sites linked to this site,           you do this entirely at your own risk.  Forums, and Chat are not always screened by VTC,           and we are not responsible for the content of any public or open forum           content at the site. VTC may change these public forums based solely           on our discretion, and we reserve the right to terminate any forum           at any time. VTC does not, by allowing these forums, endorse companies           or products which may be mentioned in these forums, and reserves the           right to note as such on its web pages. If you decide to access any           of the public forums in this site, or linked to this site, you do this           entirely at your own risk.  9. GOVERNING LAW &amp; DISPUTE RESOLUTION: This           Agreement is governed by Virginia law. All disputes between You and           VTC shall be finally resolved through arbitration in Winchester, Virginia.           This site is controlled by VTC from its offices within the United States           of America. VTC makes no representation that materials in the site           are appropriate or available for use in other locations, and access           to them from territories where their content is illegal is prohibited.           Those who choose to access this site from other locations do so on           their own initiative and are responsible for compliance with applicable           local laws. You may not use or export the Materials in violation of           U.S. export laws and regulations. Any claim relating to the Materials           shall be governed by the internal substantive laws of the Commonwealth           of Virginia, USA.  VTC may revise these Terms at any time by updating           this posting. You should visit this page from time to time to review           the then-current Terms because they are binding on you. Certain provisions           of these Terms may be superseded by expressly designated legal notices           or terms located on particular pages at this Site.  If you have any questions regarding this policy,           or your information specifically, you may email us at:admin@vtc.com. Sign up Login Forgot password?  Home About Us Affiliates Information Register Login Send Feedback Customer Suggestions Technical Problems Support Contact Courses All Courses Categories Recent Releases Popular Courses In Development Animation &amp; 3D Audio Bundles Business Applications CAD Certification Databases Game Design &amp; Development Graphics &amp; Page Layout Internet &amp; Web Design MasterClass! Multimedia &amp; Video Networking &amp; Security Operating Systems Programming Project Management QuickStart! Professional Podcasting Quickbooks Online Quickstart! Dropbox Corel Painter 2016 Zencart Service Oriented Architecture Part 2 Cubase 8 College Preparation Course Getting Started with Office 365 for Business QuickStart! - Adobe Flash Professional CC QuickStart! - Adobe Dreamweaver CC Installing and Configuring Windows Server 2012 (Exam 70-410) QuickStart! - Adobe Illustrator CC QuickStart! - Adobe Audition CC Advanced Java Programming (Java SE 7) QuickStart! - Adobe Premiere CC Microsoft Project 2013 CompTIA Linux+ (Exam LX0-101) Moodle Avid Media Composer 6 Advanced Ethical Hacking QuickStart! - 3D Printing Wireless Hacking and Security Prince2� - 2013 Foundation and Practitioner Exam Prep iOS 7 Microsoft Windows 7 Configuration (Exam 70-680) Configuring Microsoft Windows 8 (Exam 70-687) Pricing Help                                     more LEARN MORE FileMaker Pro 12: Beginner, Intermediate &amp; Advanced Bundle FileMaker Pro 12: Beginner Microsoft Project 2013 Quickstart! Dropbox Advanced Solutions of Microsoft SharePoint Server 2013 (Exam 70-332) Microsoft Office 2013 Bundle MCTS: Microsoft SharePoint 2010 Bundle QuickStart! - WampServer LEARN MORE QuickStart! - Adobe Bridge CS6 Adobe Encore CS6 Microsoft SQL Server 2012 Development (Exam 70-464) Planning a Successful Website QuickStart! - VTC Help Movies Java Mobile Android Advanced Apps Apple Motion 2014 Intermediate Oracle 11g LEARN MORE Photoshop CC for Photographers JavaScript (1.8.5) QuickStart! - Responsive Dreamweaver CS6 Websites FileMaker Pro 13: Beginner MCSE: SharePoint Solutions Expert Bundle QuickStart! - Adobe Premiere Elements 11 Data Structures and Algorithms in C++ HTML5 + CSS3 Responsive Web Design LEARN MORE TRAINING TYPES FOR INDIVIDUALS FOR BUSINESS FOR COLLEGES View All Courses                           Business Applications Quickstart Office 365                           Programming Moodle                           Certification Red Hat Certified Engineer (RHCE) - Exam EX300                           Certification Oracle: Introduction to Oracle SQL and PL/SQL                           Programming Service Oriented Architecture Part 2                           Audio Cubase 8 Feedback Become an Author Suggest a Course Verify Certificate Access Cards Authors Animation &amp; 3D Audio Bundles Business Applications CAD Certification Databases Game Design &amp; Development Graphics &amp; Page Layout Internet &amp; Web Design MasterClass! Multimedia &amp; Video Networking &amp; Security Operating Systems Programming Project Management QuickStart! Ableton Tutorials Adobe Tutorials Apache Tutorials Apple Tutorials Autodesk Tutorials Avid Tutorials Cakewalk Tutorials CompTIA Tutorials Corel Tutorials Dreamweaver Tutorials FileMaker Tutorials Java Tutorials Linux Tutorials Flash Tutorials Microsoft Tutorials MySQL Tutorials Oracle Tutorials Photoshop Tutorials PHP Tutorials Sony Tutorials Professional Podcasting Quickbooks Online Quickstart! Dropbox Corel Painter 2016 Zencart Service Oriented Architecture  Cubase 8 College Preparation Course Getting Started with Office 36 VTC Player VTC iPad App Access Card Verify Certificate Become a VTC Author! Site Map About Us Support FAQ Contact Terms and Conditions Facebook Twitter LinkedIn Blog privacy policy       VTC Terms and Conditions      TERMS        &amp; CONDITIONS OF USE          BY SUBSCRIBING TO THIS SERVICE, YOU ARE CONSENTING             TO BE BOUND BY AND ARE BECOMING A PARTY TO THIS AGREEMENT, THE TERMS             AND CONDITIONS OF WHICH SHALL PREVAIL IN GOVERNING YOUR RIGHTS OF             USE. BY CLICKING THE "BECOME A MEMBER" BUTTON, THE INDIVIDUAL             OR ENTITY LICENSING THE PRODUCT ("YOU") IS CONSENTING TO             BE BOUND BY AND IS BECOMING A PARTY TO THIS AGREEMENT. IF LICENSEE             DOES NOT AGREE TO ALL OF THE TERMS OF THIS AGREEMENT, THE BUTTON             INDICATING "BECOME A MEMBER" MUST NOT BE SELECTED, AND             LICENSEE MUST NOT INSTALL OR USE THE SOFTWARE.       1. DEFINITIONS         "VTC" refers to Virtual Training Company,           Inc.         "You" refers to the user or subscriber.          "Software" refers to the VTC training content and software.        2. LICENSE: VTC hereby grants to You a worldwide,           non-royalty bearing, non-exclusive license to use the Software according           to the provisions contained herein and subject to payment of the applicable           subscription fees.        3. RESTRICTIONS: You may not do any of the following:        Save the Software to Your hard disk or other storage           medium; permit others to use the Software except as specified by addendum;           modify, reverse engineer, decompile, or disassemble the Software; make           derivative works based on the Software; publish or otherwise disseminate           the Software. VTC, Inc., VTC Online University, and the Virtual Training           Company site is owned and operated by VTC, Inc. as a corporation of           record.         All materials on this site are the property of VTC unless otherwise specified.         No material from these pages may be copied, reproduced, republished,         downloaded, uploaded, posted, transmitted, or distributed in any way.         Modification of the materials or use of the materials for any other purpose         is a violation of U.S. copyright law and other proprietary rights. For         purposes of this Agreement, the use of any such material on any other         web site or networked computer environment is prohibited.        4. FEES: The rights granted under this Agreement           are effective only upon payment of the subscription fees, which are           strictly non-refundable other than as expressly provided herein. The           term "monthly subscription" is defined as any 30 day period.           The term "yearly subscription" is defined as one 365 day           period. A yearly subscription ends on the same numerical date as it           began (example July 28, 2004 to July 28, 2005).                                      The VTC Online University is access to every VTC training tutorial in         our library. You pay a flat fee for access         to these titles. You are billed according to your renewal selection below,         and can renew monthly, yearly, or in any other increment offered. If         you choose to be billed monthly, you will be billed every 30 days for         the subscription until you request the subscription be cancelled. Our terms of service state that you must cancel a monthly subscription at least two business days before your renewal date. These two days give us enough time to ensure that you will not be charged again.        5. LIMITED WARRANTY: VTC warrants that the Software,           if operated as directed, will substantially achieve the functionality           described. VTC does not warrant, however, that Your use of the Software           will be uninterrupted or that the operation of the Software will be           error-free or secure. In addition, the security mechanisms implemented           by the Software have inherent limitations, and You must</v>
-      </c>
-      <c r="D20" t="str">
-        <v xml:space="preserve"> determine that           the Software sufficiently meets Your requirements. VTC also warrants           that the media containing the Software, if provided by VTC, is free           from defects in material from the date You acquired the Software. VTC's           sole liability for any breach of this warranty shall be, in VTC's sole           discretion: (i) to replace Your defective media or Software; or (ii)           to advise You how to achieve substantially the same functionality with           the Software as described; or (iii) if the above remedies are impracticable,           to refund the subscription fee You paid for the Software. Only if You           inform VTC of Your problem with the Software during the applicable           subscription period will VTC be obligated to honor this warranty. VTC           will use reasonable commercial efforts to repair, replace, advise,           or refund pursuant to the foregoing warranty within thirty (30) days           of being so notified. If any modifications are made to the Software           by You during the warranty period; if the medium is subjected to accident,           abuse, or improper use; or if You violate the terms of this Agreement,           then this warranty shall immediately terminate. This warranty shall           not apply if the Software is used on or in conjunction with hardware           or software other than the unmodified version of hardware and software           with which the Software was designed to be used as described.        THIS IS A LIMITED WARRANTY, AND IT IS THE ONLY           WARRANTY MADE BY VTC OR ITS SUPPLIERS. VTC MAKES NO OTHER WARRANTIES,           EXPRESS OR IMPLIED, INCLUDING BUT NOT LIMITED TO WARRANTIES OF MERCHANTABILITY,           FITNESS FOR A PARTICULAR PURPOSE, AND NONINFRINGEMENT OF THIRD PARTIES'           RIGHTS. YOU MAY HAVE OTHER STATUTORY RIGHTS. HOWEVER, TO THE FULL EXTENT           PERMITTED BY LAW, THE DURATION OF STATUTORILY REQUIRED WARRANTIES,           IF ANY, SHALL BE LIMITED TO THE ABOVE LIMITED WARRANTY PERIOD. MOREOVER,           IN NO EVENT WILL WARRANTIES PROVIDED BY LAW, IF ANY, APPLY UNLESS THEY           ARE REQUIRED TO APPLY BY STATUTE NOTWITHSTANDING THEIR EXCLUSION BY           CONTRACT. NO DEALER, AGENT, OR EMPLOYEE OF VTC IS AUTHORIZED TO MAKE           ANY MODIFICATIONS, EXTENSIONS, OR ADDITIONS TO THIS LIMITED WARRANTY.        6. PROPRIETARY RIGHTS: VTC reserves all proprietary           rights in and to the Software, is protected by copyright and other           intellectual property laws and by international treaties. VTC, Inc.        Trademark Notice: VTC, Virtual Training Company,           Inc., The VTC Logo, and VTC Online University, are trademarks of VTC,           Inc. All other company and product names may be trademarks of their           respective owners.         The information contained herein is subject to change without notice.         Copyright © 1995 - 2005 VTC, Inc. All rights reserved.        7. TERMINATION: This Agreement shall automatically           terminate if You fail to comply with the restrictions described herein.           Your obligations to pay outstanding subscription fees shall survive           any termination of this Agreement.        8. LIMITATION OF LIABILITY: UNDER NO CIRCUMSTANCES           AND UNDER NO LEGAL THEORY, TORT, CONTRACT, OR OTHERWISE, SHALL VTC           OR ITS SUPPLIERS OR RESELLERS BE LIABLE TO YOU OR ANY OTHER PERSON           FOR ANY INDIRECT, SPECIAL, INCIDENTAL, OR CONSEQUENTIAL DAMAGES OF           ANY CHARACTER, INCLUDING WITHOUT LIMITATION, DAMAGES FOR LOSS OF GOODWILL,           WORK STOPPAGE, COMPUTER FAILURE OR MALFUNCTION, OR ANY AND ALL OTHER           COMMERCIAL DAMAGES OR LOSSES. IN NO EVENT WILL VTC BE LIABLE FOR ANY           DAMAGES IN EXCESS OF THE AMOUNT VTC RECEIVED FROM YOU FOR A LICENSE           TO THE SOFTWARE, EVEN IF VTC SHALL HAVE BEEN INFORMED OF THE POSSIBILITY           OF SUCH         DAMAGES, OR FOR ANY CLAIM BY ANY OTHER PARTY. THIS LIMITATION OF LIABILITY         SHALL NOT APPLY TO LIABILITY FOR DEATH OR PERSONAL INJURY RESULTING FROM         VTC'S NEGLIGENCE TO THE EXTENT APPLICABLE LAW PROHIBITS SUCH LIMITATION.         SOME JURISDICTIONS DO NOT ALLOW THE EXCLUSION OR LIMITATION OF INCIDENTAL         OR CONSEQUENTIAL DAMAGES, SO THIS EXCLUSION AND LIMITATION MAY NOT APPLY         TO YOU.        9. Links To Other Materials: Linked sites found           at the VTC site are not under the control of VTC, and we are not responsible           for the content of any linked site or any link contained in a linked           site. VTC may change links based solely on our discretion, and we reserve           the right to terminate any link or linking program at any time. VTC           does not, by linking to sites, endorse companies or products to which           it links and reserves the right to note as such on its web pages. If           you decide to access any of the third party sites linked to this site,           you do this entirely at your own risk.        Forums, and Chat are not always screened by VTC,           and we are not responsible for the content of any public or open forum           content at the site. VTC may change these public forums based solely           on our discretion, and we reserve the right to terminate any forum           at any time. VTC does not, by allowing these forums, endorse companies           or products which may be mentioned in these forums, and reserves the           right to note as such on its web pages. If you decide to access any           of the public forums in this site, or linked to this site, you do this           entirely at your own risk.        9. GOVERNING LAW &amp; DISPUTE RESOLUTION: This           Agreement is governed by Virginia law. All disputes between You and           VTC shall be finally resolved through arbitration in Winchester, Virginia.           This site is controlled by VTC from its offices within the United States           of America. VTC makes no representation that materials in the site           are appropriate or available for use in other locations, and access           to them from territories where their content is illegal is prohibited.           Those who choose to access this site from other locations do so on           their own initiative and are responsible for compliance with applicable           local laws. You may not use or export the Materials in violation of           U.S. export laws and regulations. Any claim relating to the Materials           shall be governed by the internal substantive laws of the Commonwealth           of Virginia, USA.        VTC may revise these Terms at any time by updating           this posting. You should visit this page from time to time to review           the then-current Terms because they are binding on you. Certain provisions           of these Terms may be superseded by expressly designated legal notices           or terms located on particular pages at this Site.        If you have any questions regarding this policy,           or your information specifically, you may email us at:admin@vtc.com.            admin@vtc.com. Courses FOR FOR FOR Facebook Twitter LinkedIn Blog</v>
-      </c>
-      <c r="E20" t="str">
-        <v xml:space="preserve"> determine that           the Software sufficiently meets Your requirements. VTC also warrants           that the media containing the Software, if provided by VTC, is free           from defects in material from the date You acquired the Software. VTC's           sole liability for any breach of this warranty shall be, in VTC's sole           discretion: (i) to replace Your defective media or Software; or (ii)           to advise You how to achieve substantially the same functionality with           the Software as described; or (iii) if the above remedies are impracticable,           to refund the subscription fee You paid for the Software. Only if You           inform VTC of Your problem with the Software during the applicable           subscription period will VTC be obligated to honor this warranty. VTC           will use reasonable commercial efforts to repair, replace, advise,           or refund pursuant to the foregoing warranty within thirty (30) days           of being so notified. If any modifications are made to the Software           by You during the warranty period; if the medium is subjected to accident,           abuse, or improper use; or if You violate the terms of this Agreement,           then this warranty shall immediately terminate. This warranty shall           not apply if the Software is used on or in conjunction with hardware           or software other than the unmodified version of hardware and software           with which the Software was designed to be used as described.        THIS IS A LIMITED WARRANTY, AND IT IS THE ONLY           WARRANTY MADE BY VTC OR ITS SUPPLIERS. VTC MAKES NO OTHER WARRANTIES,           EXPRESS OR IMPLIED, INCLUDING BUT NOT LIMITED TO WARRANTIES OF MERCHANTABILITY,           FITNESS FOR A PARTICULAR PURPOSE, AND NONINFRINGEMENT OF THIRD PARTIES'           RIGHTS. YOU MAY HAVE OTHER STATUTORY RIGHTS. HOWEVER, TO THE FULL EXTENT           PERMITTED BY LAW, THE DURATION OF STATUTORILY REQUIRED WARRANTIES,           IF ANY, SHALL BE LIMITED TO THE ABOVE LIMITED WARRANTY PERIOD. MOREOVER,           IN NO EVENT WILL WARRANTIES PROVIDED BY LAW, IF ANY, APPLY UNLESS THEY           ARE REQUIRED TO APPLY BY STATUTE NOTWITHSTANDING THEIR EXCLUSION BY           CONTRACT. NO DEALER, AGENT, OR EMPLOYEE OF VTC IS AUTHORIZED TO MAKE           ANY MODIFICATIONS, EXTENSIONS, OR ADDITIONS TO THIS LIMITED WARRANTY.        6. PROPRIETARY RIGHTS: VTC reserves all proprietary           rights in and to the Software, is protected by copyright and other           intellectual property laws and by international treaties. VTC, Inc.        Trademark Notice: VTC, Virtual Training Company,           Inc., The VTC Logo, and VTC Online University, are trademarks of VTC,           Inc. All other company and product names may be trademarks of their           respective owners.         The information contained herein is subject to change without notice.         Copyright © 1995 - 2005 VTC, Inc. All rights reserved.        7. TERMINATION: This Agreement shall automatically           terminate if You fail to comply with the restrictions described herein.           Your obligations to pay outstanding subscription fees shall survive           any termination of this Agreement.        8. LIMITATION OF LIABILITY: UNDER NO CIRCUMSTANCES           AND UNDER NO LEGAL THEORY, TORT, CONTRACT, OR OTHERWISE, SHALL VTC           OR ITS SUPPLIERS OR RESELLERS BE LIABLE TO YOU OR ANY OTHER PERSON           FOR ANY INDIRECT, SPECIAL, INCIDENTAL, OR CONSEQUENTIAL DAMAGES OF           ANY CHARACTER, INCLUDING WITHOUT LIMITATION, DAMAGES FOR LOSS OF GOODWILL,           WORK STOPPAGE, COMPUTER FAILURE OR MALFUNCTION, OR ANY AND ALL OTHER           COMMERCIAL DAMAGES OR LOSSES. IN NO EVENT WILL VTC BE LIABLE FOR ANY           DAMAGES IN EXCESS OF THE AMOUNT VTC RECEIVED FROM YOU FOR A LICENSE           TO THE SOFTWARE, EVEN IF VTC SHALL HAVE BEEN INFORMED OF THE POSSIBILITY           OF SUCH         DAMAGES, OR FOR ANY CLAIM BY ANY OTHER PARTY. THIS LIMITATION OF LIABILITY         SHALL NOT APPLY TO LIABILITY FOR DEATH OR PERSONAL INJURY RESULTING FROM         VTC'S NEGLIGENCE TO THE EXTENT APPLICABLE LAW PROHIBITS SUCH LIMITATION.         SOME JURISDICTIONS DO NOT ALLOW THE EXCLUSION OR LIMITATION OF INCIDENTAL         OR CONSEQUENTIAL DAMAGES, SO THIS EXCLUSION AND LIMITATION MAY NOT APPLY         TO YOU.        9. Links To Other Materials: Linked sites found           at the VTC site are not under the control of VTC, and we are not responsible           for the content of any linked site or any link contained in a linked           site. VTC may change links based solely on our discretion, and we reserve           the right to terminate any link or linking program at any time. VTC           does not, by linking to sites, endorse companies or products to which           it links and reserves the right to note as such on its web pages. If           you decide to access any of the third party sites linked to this site,           you do this entirely at your own risk.        Forums, and Chat are not always screened by VTC,           and we are not responsible for the content of any public or open forum           content at the site. VTC may change these public forums based solely           on our discretion, and we reserve the right to terminate any forum           at any time. VTC does not, by allowing these forums, endorse companies           or products which may be mentioned in these forums, and reserves the           right to note as such on its web pages. If you decide to access any           of the public forums in this site, or linked to this site, you do this           entirely at your own risk.        9. GOVERNING LAW &amp; DISPUTE RESOLUTION: This           Agreement is governed by Virginia law. All disputes between You and           VTC shall be finally resolved through arbitration in Winchester, Virginia.           This site is controlled by VTC from its offices within the United States           of America. VTC makes no representation that materials in the site           are appropriate or available for use in other locations, and access           to them from territories where their content is illegal is prohibited.           Those who choose to access this site from other locations do so on           their own initiative and are responsible for compliance with applicable           local laws. You may not use or export the Materials in violation of           U.S. export laws and regulations. Any claim relating to the Materials           shall be governed by the internal substantive laws of the Commonwealth           of Virginia, USA.        VTC may revise these Terms at any time by updating           this posting. You should visit this page from time to time to review           the then-current Terms because they are binding on you. Certain provisions           of these Terms may be superseded by expressly designated legal notices           or terms located on particular pages at this Site.        If you have any questions regarding this policy,           or your information specifically, you may email us at:admin@vtc.com.            admin@vtc.com. Courses FOR FOR FOR Facebook Twitter LinkedIn Blog</v>
-      </c>
-      <c r="F20" t="str">
-        <v xml:space="preserve"> determine that           the Software sufficiently meets Your requirements. VTC also warrants           that the media containing the Software, if provided by VTC, is free           from defects in material from the date You acquired the Software. VTC's           sole liability for any breach of this warranty shall be, in VTC's sole           discretion: (i) to replace Your defective media or Software; or (ii)           to advise You how to achieve substantially the same functionality with           the Software as described; or (iii) if the above remedies are impracticable,           to refund the subscription fee You paid for the Software. Only if You           inform VTC of Your problem with the Software during the applicable           subscription period will VTC be obligated to honor this warranty. VTC           will use reasonable commercial efforts to repair, replace, advise,           or refund pursuant to the foregoing warranty within thirty (30) days           of being so notified. If any modifications are made to the Software           by You during the warranty period; if the medium is subjected to accident,           abuse, or improper use; or if You violate the terms of this Agreement,           then this warranty shall immediately terminate. This warranty shall           not apply if the Software is used on or in conjunction with hardware           or software other than the unmodified version of hardware and software           with which the Software was designed to be used as described.        THIS IS A LIMITED WARRANTY, AND IT IS THE ONLY           WARRANTY MADE BY VTC OR ITS SUPPLIERS. VTC MAKES NO OTHER WARRANTIES,           EXPRESS OR IMPLIED, INCLUDING BUT NOT LIMITED TO WARRANTIES OF MERCHANTABILITY,           FITNESS FOR A PARTICULAR PURPOSE, AND NONINFRINGEMENT OF THIRD PARTIES'           RIGHTS. YOU MAY HAVE OTHER STATUTORY RIGHTS. HOWEVER, TO THE FULL EXTENT           PERMITTED BY LAW, THE DURATION OF STATUTORILY REQUIRED WARRANTIES,           IF ANY, SHALL BE LIMITED TO THE ABOVE LIMITED WARRANTY PERIOD. MOREOVER,           IN NO EVENT WILL WARRANTIES PROVIDED BY LAW, IF ANY, APPLY UNLESS THEY           ARE REQUIRED TO APPLY BY STATUTE NOTWITHSTANDING THEIR EXCLUSION BY           CONTRACT. NO DEALER, AGENT, OR EMPLOYEE OF VTC IS AUTHORIZED TO MAKE           ANY MODIFICATIONS, EXTENSIONS, OR ADDITIONS TO THIS LIMITED WARRANTY.        6. PROPRIETARY RIGHTS: VTC reserves all proprietary           rights in and to the Software, is protected by copyright and other           intellectual property laws and by international treaties. VTC, Inc.        Trademark Notice: VTC, Virtual Training Company,           Inc., The VTC Logo, and VTC Online University, are trademarks of VTC,           Inc. All other company and product names may be trademarks of their           respective owners.         The information contained herein is subject to change without notice.         Copyright © 1995 - 2005 VTC, Inc. All rights reserved.        7. TERMINATION: This Agreement shall automatically           terminate if You fail to comply with the restrictions described herein.           Your obligations to pay outstanding subscription fees shall survive           any termination of this Agreement.        8. LIMITATION OF LIABILITY: UNDER NO CIRCUMSTANCES           AND UNDER NO LEGAL THEORY, TORT, CONTRACT, OR OTHERWISE, SHALL VTC           OR ITS SUPPLIERS OR RESELLERS BE LIABLE TO YOU OR ANY OTHER PERSON           FOR ANY INDIRECT, SPECIAL, INCIDENTAL, OR CONSEQUENTIAL DAMAGES OF           ANY CHARACTER, INCLUDING WITHOUT LIMITATION, DAMAGES FOR LOSS OF GOODWILL,           WORK STOPPAGE, COMPUTER FAILURE OR MALFUNCTION, OR ANY AND ALL OTHER           COMMERCIAL DAMAGES OR LOSSES. IN NO EVENT WILL VTC BE LIABLE FOR ANY           DAMAGES IN EXCESS OF THE AMOUNT VTC RECEIVED FROM YOU FOR A LICENSE           TO THE SOFTWARE, EVEN IF VTC SHALL HAVE BEEN INFORMED OF THE POSSIBILITY           OF SUCH         DAMAGES, OR FOR ANY CLAIM BY ANY OTHER PARTY. THIS LIMITATION OF LIABILITY         SHALL NOT APPLY TO LIABILITY FOR DEATH OR PERSONAL INJURY RESULTING FROM         VTC'S NEGLIGENCE TO THE EXTENT APPLICABLE LAW PROHIBITS SUCH LIMITATION.         SOME JURISDICTIONS DO NOT ALLOW THE EXCLUSION OR LIMITATION OF INCIDENTAL         OR CONSEQUENTIAL DAMAGES, SO THIS EXCLUSION AND LIMITATION MAY NOT APPLY         TO YOU.        9. Links To Other Materials: Linked sites found           at the VTC site are not under the control of VTC, and we are not responsible           for the content of any linked site or any link contained in a linked           site. VTC may change links based solely on our discretion, and we reserve           the right to terminate any link or linking program at any time. VTC           does not, by linking to sites, endorse companies or products to which           it links and reserves the right to note as such on its web pages. If           you decide to access any of the third party sites linked to this site,           you do this entirely at your own risk.        Forums, and Chat are not always screened by VTC,           and we are not responsible for the content of any public or open forum           content at the site. VTC may change these public forums based solely           on our discretion, and we reserve the right to terminate any forum           at any time. VTC does not, by allowing these forums, endorse companies           or products which may be mentioned in these forums, and reserves the           right to note as such on its web pages. If you decide to access any           of the public forums in this site, or linked to this site, you do this           entirely at your own risk.        9. GOVERNING LAW &amp; DISPUTE RESOLUTION: This           Agreement is governed by Virginia law. All disputes between You and           VTC shall be finally resolved through arbitration in Winchester, Virginia.           This site is controlled by VTC from its offices within the United States           of America. VTC makes no representation that materials in the site           are appropriate or available for use in other locations, and access           to them from territories where their content is illegal is prohibited.           Those who choose to access this site from other locations do so on           their own initiative and are responsible for compliance with applicable           local laws. You may not use or export the Materials in violation of           U.S. export laws and regulations. Any claim relating to the Materials           shall be governed by the internal substantive laws of the Commonwealth           of Virginia, USA.        VTC may revise these Terms at any time by updating           this posting. You should visit this page from time to time to review           the then-current Terms because they are binding on you. Certain provisions           of these Terms may be superseded by expressly designated legal notices           or terms located on particular pages at this Site.        If you have any questions regarding this policy,           or your information specifically, you may email us at:admin@vtc.com.            admin@vtc.com. Courses FOR FOR FOR Facebook Twitter LinkedIn Blog</v>
+        <v>Online software tutorials training CDs Photoshop Tutorials Dreamweaver Tutorials Apple Tutorials from vtccom vtccom provides the latest Apple Tutorials Adobe Tutorials Cakewalk Tutorials Corel Tutorials Dreamweaver Tutorials Macromedia Tutorials Microsoft Tutorials Oracle Tutorials Photoshop Tutorials and Sony Tutorials as high quality quicktime videos Affordable software training Individuals and students Businesses and corporations Colleges and universities Easytounderstand video tutorials Learn anywhere at your own pace Train your staff easily and affordably Educate groups of students easily Popular courses New releases Categories Software or Publisher Recent Releases Resources Community VTC Terms and Conditions ONLINE DOWNLOAD USB FAST PORTABLE CERTIFICATES FLEXIBLE PRACTICAL COMPATIBLE LDAP LCMS TRACKING EASY ADMIN COURSE LIST ONLINE ACCESS Business Applications Programming Certification Certification Programming Audio Home About Us Affiliates Information Register Login Send Feedback Customer Suggestions Technical Problems Support Contact About Us Affiliates Information Register Login Information Register Login Send Feedback Customer Suggestions Technical Problems Customer Suggestions Technical Problems Support Contact All Courses Categories Recent Releases Popular Courses In Development Animation 3D Audio Bundles Business Applications CAD Certification Databases Game Design Development Graphics Page Layout Internet Web Design MasterClass Multimedia Video Networking Security Operating Systems Programming Project Management QuickStart Professional Podcasting Quickbooks Online Quickstart Dropbox Corel Painter 2016 Zencart Service Oriented Architecture Part 2 Cubase 8 College Preparation Course Getting Started with Office 365 for Business QuickStart Adobe Flash Professional CC QuickStart Adobe Dreamweaver CC Installing and Configuring Windows Server 2012 Exam 70410 QuickStart Adobe Illustrator CC QuickStart Adobe Audition CC Advanced Java Programming Java SE 7 QuickStart Adobe Premiere CC Microsoft Project 2013 CompTIA Linux Exam LX0101 Moodle Avid Media Composer 6 Advanced Ethical Hacking QuickStart 3D Printing Wireless Hacking and Security Prince2� 2013 Foundation and Practitioner Exam Prep iOS 7 Microsoft Windows 7 Configuration Exam 70680 Configuring Microsoft Windows 8 Exam 70687 Pricing Help function ssLoadMoviemovieNum Bring in user agent detection result from PHP var mobileDevice 0 if ssMovieLoaded01 false jwplayermoviemovieNumsetup width 719 height 272 duration 223 screencolor 0b2a37 image httpwwwvtccomtemplatescountryenfreeimagesjwplayerbgpng stretching fill autostart true bufferlength 10 skin httpwwwvtccomtemplatescountryenfreeimageslearnMoreskinsvtcwebbannervtcwebbannerzip wmode transparent controlbaridlehide true modes type html5 type flash src httpwwwvtccomtemplatescountryenfreeimageslearnMoreplayerswffilehttpwwwvtccomtemplatescountryenfreeimageslearnMoremediamoviemovieNumcmp4imagehttpwwwvtccomtemplatescountryenfreeimagesjwplayerbgpngautostarttrue type download levels file httpwwwvtccomtemplatescountryenfreeimageslearnMoremediamoviemovieNumcmp4 ssMovieLoaded01 true consolelogMovie loaded jwplayeronPausefunction ssMoviePlaying false jwplayeronPlayfunction ssMoviePlaying true if mobileDevice 0 ssEnableOverlay jwplayergetPlugincontrolbaronHidefunction movieoverlaywrapperfadeOut100 jwplayergetPlugincontrolbaronShowfunction movieoverlaywrapperfadeIn100 Affordable software training Easytounderstand video tutorials ONLINE Get full access to our entire library DOWNLOAD Save to your own drive or device USB Portable training on the move Thanks VTC Ive learned more stuff in here and much faster than if I had bought a book or slept through a class Keep up the good work and keep on Arellano Torres more LEARN MORE ONLINE Get full access to our entire library DOWNLOAD Save to your own drive or device USB Portable training on the move Individuals and students Learn anywhere at your own pace FAST No time consuming class schedules PORTABLE Train anywherewhenever you want CERTIFICATES Certificates uponcourse completion Microsoft Excel 2013 QuickStart Managing Financial Data in Excel QuickStart VTC Help Movies Adobe CC Film Production Audition CC Spring MVC QS Evernote MasterClass Microsoft Excel 2013 Pivot Tables LEARN MORE FAST No time consuming class schedules PORTABLE Train anywherewhenever you want CERTIFICATES Certificates uponcourse completion Microsoft Excel 2013 QuickStart Managing Financial Data in Excel QuickStart VTC Help Movies Adobe CC Film Production Audition CC Spring MVC QS Evernote MasterClass Microsoft Excel 2013 Pivot Tables Businesses and corporations Train your staff easily and affordably FLEXIBLE Staff can sharemulti user accounts PRACTICAL Reduce supportcalls and costs COMPATIBLE Works with Windows Mac and Linux CompTIA Linux Exam LX0102 Ableton FileMaker Pro 13 Beginner Introduction to Cloud Computing Corel Painter 2016 Microsoft Windows 7 Configuration Exam 70680 QuickStart Adobe Flash Professional CC QuickStart WordPress Multisite LEARN MORE FLEXIBLE Staff can sharemulti user accounts PRACTICAL Reduce supportcalls and costs COMPATIBLE Works with Windows Mac and Linux CompTIA Linux Exam LX0102 Ableton FileMaker Pro 13 Beginner Introduction to Cloud Computing Corel Painter 2016 Microsoft Windows 7 Configuration Exam 70680 QuickStart Adobe Flash Professional CC QuickStart WordPress Multisite Colleges and universities Educate groups of students easily LDAP LCMS Integrate with existing systems TRACKING Quickly monitor student progress EASY ADMIN Full peruser account control QuickStart Search Engine Optimization 2013 Service Oriented Architecture Part 2 QuickStart Adobe Media Encoder CS6 Quickbooks Online Microsoft Outlook 2013 QuickStart Adobe Flash Professional CS6 Red Hat Certified Engineer RHCE Exam EX300 Joomla 25 LEARN MORE LDAP LCMS Integrate with existing systems TRACKING Quickly monitor student progress EASY ADMIN Full peruser account control QuickStart Search Engine Optimization 2013 Service Oriented Architecture Part 2 QuickStart Adobe Media Encoder CS6 Quickbooks Online Microsoft Outlook 2013 QuickStart Adobe Flash Professional CS6 Red Hat Certified Engineer RHCE Exam EX300 Joomla 25 TRAINING TYPES FOR INDIVIDUALS FOR BUSINESS FOR COLLEGES Business Applications Quickstart Office 365 Programming Moodle Certification Red Hat Certified Engineer RHCE Exam EX300 Certification Oracle Introduction to Oracle SQL and PLSQL Programming Service Oriented Architecture Part 2 Audio Cubase 8 Feedback Become an Author Suggest a Course Verify Certificate Access Cards Authors Animation 3D Audio Bundles Business Applications CAD Certification Databases Game Design Development Graphics Page Layout Internet Web Design MasterClass Multimedia Video Networking Security Operating Systems Programming Project Management QuickStart Ableton Tutorials Adobe Tutorials Apache Tutorials Apple Tutorials Autodesk Tutorials Avid Tutorials Cakewalk Tutorials CompTIA Tutorials Corel Tutorials Dreamweaver Tutorials FileMaker Tutorials Java Tutorials Linux Tutorials Flash Tutorials Microsoft Tutorials MySQL Tutorials Oracle Tutorials Photoshop Tutorials PHP Tutorials Sony Tutorials Professional Podcasting Quickbooks Online Quickstart Dropbox Corel Painter 2016 Zencart Service Oriented Architecture Cubase 8 College Preparation Course Getting Started with Office 36 VTC Player VTC iPad App Access Card Verify Certificate Become a VTC Author Site Map About Us Support FAQ Contact Terms and Conditions Facebook Twitter LinkedIn Blog Sign up Username Password Remember me After Login Go to my home page Stay on current page Forgot password Thanks VTC Ive learned more stuff in here and much faster than if I had bought a book or slept through a class Keep up the good work and keep on Arellano Torres more Client and visitor information gathered by VTC is used ONLY by VTC our lists are never rented or sold For more information view our privacy policy TERMS CONDITIONS OF USE BY SUBSCRIBING TO THIS SERVICE YOU ARE CONSENTING TO BE BOUND BY AND ARE BECOMING A PARTY TO THIS AGREEMENT THE TERMS AND CONDITIONS OF WHICH SHALL PREVAIL IN GOVERNING YOUR RIGHTS OF USE BY CLICKING THE BECOME A MEMBER BUTTON THE INDIVIDUAL OR ENTITY LICENSING THE PRODUCT YOU IS CONSENTING TO BE BOUND BY AND IS BECOMING A PARTY TO THIS AGREEMENT IF LICENSEE DOES NOT AGREE TO ALL OF THE TERMS OF THIS AGREEMENT THE BUTTON INDICATING BECOME A MEMBER MUST NOT BE SELECTED AND LICENSEE MUST NOT INSTALL OR USE THE SOFTWARE 1 DEFINITIONS VTC refers to Virtual Training Company Inc You refers to the user or subscriber Software refers to the VTC training content and software 2 LICENSE VTC hereby grants to You a worldwide nonroyalty bearing nonexclusive license to use the Software according to the provisions contained herein and subject to payment of the applicable subscription fees 3 RESTRICTIONS You may not do any of the following Save the Software to Your hard disk or other storage medium permit others to use the Software except as specified by addendum modify reverse engineer decompile or disassemble the Software make derivative works based on the Software publish or otherwise disseminate the Software VTC Inc VTC Online University and the Virtual Training Company site is owned and operated by VTC Inc as a corporation of record All materials on this site are the property of VTC unless otherwise specified No material from these pages may be copied reproduced republished downloaded uploaded posted transmitted or distributed in any way Modification of the materials or use of the materials for any other purpose is a violation of US copyright law and other proprietary rights For purposes of this Agreement the use of any such material on any other web site or networked computer environment is prohibited 4 FEES The rights granted under this Agreement are effective only upon payment of the subscription fees which are strictly nonrefundable other than as expressly provided herein The term monthly subscription is defined as any 30 day period The term yearly subscription is defined as one 365 day period A yearly subscription ends on the same numerical date as it began example July 28 2004 to July 28 2005 The VTC Online University is access to every VTC training tutorial in our library You pay a flat fee for access to these titles You are billed according to your renewal selection below and can renew monthly yearly or in any other increment offered If you choose to be billed monthly you will be billed every 30 days for the subscription until you request the subscription be cancelled Our terms of service state that you must cancel a monthly subscription at least two business days before your renewal date These two days give us enough time to ensure that you will not be charged again 5 LIMITED WARRANTY VTC warrants that the Software if operated as directed will substantially achieve the functionality described VTC does not warrant however that Your use of the Software will be uninterrupted or that the operation of the Software will be errorfree or secure In addition the security mechanisms implemented by the Software have inherent limitations and You must determine that the Software sufficiently meets Your requirements VTC also warrants that the media containing the Software if provided by VTC is free from defects in material from the date You acquired the Software VTCs sole liability for any breach of this warranty shall be in VTCs sole discretion i to replace Your defective media or Software or ii to advise You how to achieve substantially the same functionality with the Software as described or iii if the above remedies are impracticable to refund the subscription fee You paid for the Software Only if You inform VTC of Your problem with the Software during the applicable subscription period will VTC be obligated to honor this warranty VTC will use reasonable commercial efforts to repair replace advise or refund pursuant to the foregoing warranty within thirty 30 days of being so notified If any modifications are made to the Software by You during the warranty period if the medium is subjected to accident abuse or improper use or if You violate the terms of this Agreement then this warranty shall immediately terminate This warranty shall not apply if the Software is used on or in conjunction with hardware or software other than the unmodified version of hardware and software with which the Software was designed to be used as described THIS IS A LIMITED WARRANTY AND IT IS THE ONLY WARRANTY MADE BY VTC OR ITS SUPPLIERS VTC MAKES NO OTHER WARRANTIES EXPRESS OR IMPLIED INCLUDING BUT NOT LIMITED TO WARRANTIES OF MERCHANTABILITY FITNESS FOR A PARTICULAR PURPOSE AND NONINFRINGEMENT OF THIRD PARTIES RIGHTS YOU MAY HAVE OTHER STATUTORY RIGHTS HOWEVER TO THE FULL EXTENT PERMITTED BY LAW THE DURATION OF STATUTORILY REQUIRED WARRANTIES IF ANY SHALL BE LIMITED TO THE ABOVE LIMITED WARRANTY PERIOD MOREOVER IN NO EVENT WILL WARRANTIES PROVIDED BY LAW IF ANY APPLY UNLESS THEY ARE REQUIRED TO APPLY BY STATUTE NOTWITHSTANDING THEIR EXCLUSION BY CONTRACT NO DEALER AGENT OR EMPLOYEE OF VTC IS AUTHORIZED TO MAKE ANY MODIFICATIONS EXTENSIONS OR ADDITIONS TO THIS LIMITED WARRANTY 6 PROPRIETARY RIGHTS VTC reserves all proprietary rights in and to the Software is protected by copyright and other intellectual property laws and by international treaties VTC Inc Trademark Notice VTC Virtual Training Company Inc The VTC Logo and VTC Online University are trademarks of VTC Inc All other company and product names may be trademarks of their respective owners The information contained herein is subject to change without notice Copyright © 1995 2005 VTC Inc All rights reserved 7 TERMINATION This Agreement shall automatically terminate if You fail to comply with the restrictions described herein Your obligations to pay outstanding subscription fees shall survive any termination of this Agreement 8 LIMITATION OF LIABILITY UNDER NO CIRCUMSTANCES AND UNDER NO LEGAL THEORY TORT CONTRACT OR OTHERWISE SHALL VTC OR ITS SUPPLIERS OR RESELLERS BE LIABLE TO YOU OR ANY OTHER PERSON FOR ANY INDIRECT SPECIAL INCIDENTAL OR CONSEQUENTIAL DAMAGES OF ANY CHARACTER INCLUDING WITHOUT LIMITATION DAMAGES FOR LOSS OF GOODWILL WORK STOPPAGE COMPUTER FAILURE OR MALFUNCTION OR ANY AND ALL OTHER COMMERCIAL DAMAGES OR LOSSES IN NO EVENT WILL VTC BE LIABLE FOR ANY DAMAGES IN EXCESS OF THE AMOUNT VTC RECEIVED FROM YOU FOR A LICENSE TO THE SOFTWARE EVEN IF VTC SHALL HAVE BEEN INFORMED OF THE POSSIBILITY OF SUCH DAMAGES OR FOR ANY CLAIM BY ANY OTHER PARTY THIS LIMITATION OF LIABILITY SHALL NOT APPLY TO LIABILITY FOR DEATH OR PERSONAL INJURY RESULTING FROM VTCS NEGLIGENCE TO THE EXTENT APPLICABLE LAW PROHIBITS SUCH LIMITATION SOME JURISDICTIONS DO NOT ALLOW THE EXCLUSION OR LIMITATION OF INCIDENTAL OR CONSEQUENTIAL DAMAGES SO THIS EXCLUSION AND LIMITATION MAY NOT APPLY TO YOU 9 Links To Other Materials Linked sites found at the VTC site are not under the control of VTC and we are not responsible for the content of any linked site or any link contained in a linked site VTC may change links based solely on our discretion and we reserve the right to terminate any link or linking program at any time VTC does not by linking to sites endorse companies or products to which it links and reserves the right to note as such on its web pages If you decide to access any of the third party sites linked to this site you do this entirely at your own risk Forums and Chat are not always screened by VTC and we are not responsible for the content of any public or open forum content at the site VTC may change these public forums based solely on our discretion and we reserve the right to terminate any forum at any time VTC does not by allowing these forums endorse companies or products which may be mentioned in these forums and reserves the right to note as such on its web pages If you decide to access any of the public forums in this site or linked to this site you do this entirely at your own risk 9 GOVERNING LAW DISPUTE RESOLUTION This Agreement is governed by Virginia law All disputes between You and VTC shall be finally resolved through arbitration in Winchester Virginia This site is controlled by VTC from its offices within the United States of America VTC makes no representation that materials in the site are appropriate or available for use in other locations and access to them from territories where their content is illegal is prohibited Those who choose to access this site from other locations do so on their own initiative and are responsible for compliance with applicable local laws You may not use or export the Materials in violation of US export laws and regulations Any claim relating to the Materials shall be governed by the internal substantive laws of the Commonwealth of Virginia USA VTC may revise these Terms at any time by updating this posting You should visit this page from time to time to review the thencurrent Terms because they are binding on you Certain provisions of these Terms may be superseded by expressly designated legal notices or terms located on particular pages at this Site If you have any questions regarding this policy or your information specifically you may email us atadminvtccom Sign up Login Forgot password Home About Us Affiliates Information Register Login Send Feedback Customer Suggestions Technical Problems Support Contact Courses All Courses Categories Recent Releases Popular Courses In Development Animation 3D Audio Bundles Business Applications CAD Certification Databases Game Design Development Graphics Page Layout Internet Web Design MasterClass Multimedia Video Networking Security Operating Systems Programming Project Management QuickStart Professional Podcasting Quickbooks Online Quickstart Dropbox Corel Painter 2016 Zencart Service Oriented Architecture Part 2 Cubase 8 College Preparation Course Getting Started with Office 365 for Business QuickStart Adobe Flash Professional CC QuickStart Adobe Dreamweaver CC Installing and Configuring Windows Server 2012 Exam 70410 QuickStart Adobe Illustrator CC QuickStart Adobe Audition CC Advanced Java Programming Java SE 7 QuickStart Adobe Premiere CC Microsoft Project 2013 CompTIA Linux Exam LX0101 Moodle Avid Media Composer 6 Advanced Ethical Hacking QuickStart 3D Printing Wireless Hacking and Security Prince2� 2013 Foundation and Practitioner Exam Prep iOS 7 Microsoft Windows 7 Configuration Exam 70680 Configuring Microsoft Windows 8 Exam 70687 Pricing Help more LEARN MORE Microsoft Excel 2013 QuickStart Managing Financial Data in Excel QuickStart VTC Help Movies Adobe CC Film Production Audition CC Spring MVC QS Evernote MasterClass Microsoft Excel 2013 Pivot Tables LEARN MORE CompTIA Linux Exam LX0102 Ableton FileMaker Pro 13 Beginner Introduction to Cloud Computing Corel Painter 2016 Microsoft Windows 7 Configuration Exam 70680 QuickStart Adobe Flash Professional CC QuickStart WordPress Multisite LEARN MORE QuickStart Search Engine Optimization 2013 Service Oriented Architecture Part 2 QuickStart Adobe Media Encoder CS6 Quickbooks Online Microsoft Outlook 2013 QuickStart Adobe Flash Professional CS6 Red Hat Certified Engineer RHCE Exam EX300 Joomla 25 LEARN MORE TRAINING TYPES FOR INDIVIDUALS FOR BUSINESS FOR COLLEGES View All Courses Business Applications Quickstart Office 365 Programming Moodle Certification Red Hat Certified Engineer RHCE Exam EX300 Certification Oracle Introduction to Oracle SQL and PLSQL Programming Service Oriented Architecture Part 2 Audio Cubase 8 Feedback Become an Author Suggest a Course Verify Certificate Access Cards Authors Animation 3D Audio Bundles Business Applications CAD Certification Databases Game Design Development Graphics Page Layout Internet Web Design MasterClass Multimedia Video Networking Security Operating Systems Programming Project Management QuickStart Ableton Tutorials Adobe Tutorials Apache Tutorials Apple Tutorials Autodesk Tutorials Avid Tutorials Cakewalk Tutorials CompTIA Tutorials Corel Tutorials Dreamweaver Tutorials FileMaker Tutorials Java Tutorials Linux Tutorials Flash Tutorials Microsoft Tutorials MySQL Tutorials Oracle Tutorials Photoshop Tutorials PHP Tutorials Sony Tutorials Professional Podcasting Quickbooks Online Quickstart Dropbox Corel Painter 2016 Zencart Service Oriented Architecture Cubase 8 College Preparation Course Getting Started with Office 36 VTC Player VTC iPad App Access Card Verify Certificate Become a VTC Author Site Map About Us Support FAQ Contact Terms and Conditions Facebook Twitter LinkedIn Blog privacy policy VTC Terms and Conditions TERMS CONDITIONS OF USE BY SUBSCRIBING TO THIS SERVICE YOU ARE CONSENTING TO BE BOUND BY AND ARE BECOMING A PARTY TO THIS AGREEMENT THE TERMS AND CONDITIONS OF WHICH SHALL PREVAIL IN GOVERNING YOUR RIGHTS OF USE BY CLICKING THE BECOME A MEMBER BUTTON THE INDIVIDUAL OR ENTITY LICENSING THE PRODUCT YOU IS CONSENTING TO BE BOUND BY AND IS BECOMING A PARTY TO THIS AGREEMENT IF LICENSEE DOES NOT AGREE TO ALL OF THE TERMS OF THIS AGREEMENT THE BUTTON INDICATING BECOME A MEMBER MUST NOT BE SELECTED AND LICENSEE MUST NOT INSTALL OR USE THE SOFTWARE 1 DEFINITIONS VTC refers to Virtual Training Company Inc You refers to the user or subscriber Software refers to the VTC training content and software 2 LICENSE VTC hereby grants to You a worldwide nonroyalty bearing nonexclusive license to use the Software according to the provisions contained herein and subject to payment of the applicable subscription fees 3 RESTRICTIONS You may not do any of the following Save the Software to Your hard disk or other storage medium permit others to use the Software except as specified by addendum modify reverse engineer decompile or disassemble the Software make derivative works based on the Software publish or otherwise disseminate the Software VTC Inc VTC Online University and the Virtual Training Company site is owned and operated by VTC Inc as a corporation of record All materials on this site are the property of VTC unless otherwise specified No material from these pages may be copied reproduced republished downloaded uploaded posted transmitted or distributed in any way Modification of the materials or use of the materials for any other purpose is a violation of US copyright law and other proprietary rights For purposes of this Agreement the use of any such material on any other web site or networked computer environment is prohibited 4 FEES The rights granted under this Agreement are effective only upon payment of the subscription fees which are strictly nonrefundable other than as expressly provided herein The term monthly subscription is defined as any 30 day period The term yearly subscription is defined as one 365 day period A yearly subscription ends on the same numerical date as it began example July 28 2004 to July 28 2005 The VTC Online University is access to every VTC training tutorial in our library You pay a flat fee for access to these titles You are billed according to your renewal selection below and can renew monthly yearly or in any other increment offered If you choose to be billed monthly you will be billed every 30 days for the subscription until you request the subscription be cancelled Our terms of service state that you must cancel a monthly subscription at least two business days before your renewal date These two days give us enough time to ensure that you will not be charged again 5 LIMITED WARRANTY VTC warrants that the Software if operated as directed will substantially achieve the functionality described VTC does not warrant however that Your use of the Software will be uninterrupted or that the operation of the Software will be errorfree or secure In addition the security mechanisms implemented by the Software have inherent limitations and You must determine that the Software sufficiently meets Your requirements VTC also warrants that the media containing the Software if provided by VTC is free from defects in material from the date You acquired the Software VTCs sole liability for any breach of this warranty shall be in VTCs sole discretion i to replace Your defective media or Software or ii to advise You how to achieve substantially the same functionality with the Software as described or iii if the above remedies are impracticable to refund the subscription fee You paid for the Software Only if You inform VTC of Your problem with the Software during the applicable subscription period will VTC be obligated to honor this warranty VTC will use reasonable commercial efforts to repair replace advise or refund pursuant to the foregoing warranty within thirty 30 days of being so notified If any modifications are made to the Software by You during the warranty period if the medium is subjected to accident abuse or improper use or if You violate the terms of this Agreement then this warranty shall immediately terminate This warranty shall not apply if the Software is used on or in conjunction with hardware or software other than the unmodified version of hardware and software with which the Software was designed to be used as described THIS IS A LIMITED WARRANTY AND IT IS THE ONLY WARRANTY MADE BY VTC OR ITS SUPPLIERS VTC MAKES NO OTHER WARRANTIES EXPRESS OR IMPLIED INCLUDING BUT NOT LIMITED TO WARRANTIES OF MERCHANTABILITY FITNESS FOR A PARTICULAR PURPOSE AND NONINFRINGEMENT OF THIRD PARTIES RIGHTS YOU MAY HAVE OTHER STATUTORY RIGHTS HOWEVER TO THE FULL EXTENT PERMITTED BY LAW THE DURATION OF STATUTORILY REQUIRED WARRANTIES IF ANY SHALL BE LIMITED TO THE ABOVE LIMITED WARRANTY PERIOD MOREOVER IN NO EVENT WILL WARRANTIES PROVIDED BY LAW IF ANY APPLY UNLESS THEY ARE REQUIRED TO APPLY BY STATUTE NOTWITHSTANDING THEIR EXCLUSION BY CONTRACT NO DEALER AGENT OR EMPLOYEE OF VTC IS AUTHORIZED TO MAKE ANY MODIFICATIONS EXTENSIONS OR ADDITIONS TO THIS LIMITED WARRANTY 6 PROPRIETARY RIGHTS VTC reserves all proprietary rights in and to the Software is protected by copyright and other intellectual property laws and by international treaties VTC Inc Trademark Notice VTC Virtual Training Company Inc The VTC Logo and VTC Online University are trademarks of VTC Inc All other company and product names may be trademarks of their respective owners The information contained herein is subject to change without notice Copyright © 1995 2005 VTC Inc All rights reserved 7 TERMINATION This Agreement shall automatically terminate if You fail to comply with the restrictions described herein Your obligations to pay outstanding subscription fees shall survive any termination of this Agreement 8 LIMITATION OF LIABILITY UNDER NO CIRCUMSTANCES AND UNDER NO LEGAL THEORY TORT CONTRACT OR OTHERWISE SHALL VTC OR ITS SUPPLIERS OR RESELLERS BE LIABLE TO YOU OR ANY OTHER PERSON FOR ANY INDIRECT SPECIAL INCIDENTAL OR CONSEQUENTIAL DAMAGES OF ANY CHARACTER INCLUDING WITHOUT LIMITATION DAMAGES FOR LOSS OF GOODWILL WORK STOPPAGE COMPUTER FAILURE OR MALFUNCTION OR ANY AND ALL OTHER COMMERCIAL DAMAGES OR LOSSES IN NO EVENT WILL VTC BE LIABLE FOR ANY DAMAGES IN EXCESS OF THE AMOUNT VTC RECEIVED FROM YOU FOR A LICENSE TO THE SOFTWARE EVEN IF VTC SHALL HAVE BEEN INFORMED OF THE POSSIBILITY OF SUCH DAMAGES OR FOR ANY CLAIM BY ANY OTHER PARTY THIS LIMITATION OF LIABILITY SHALL NOT APPLY TO LIABILITY FOR DEATH OR PERSONAL INJURY RESULTING FROM VTCS NEGLIGENCE TO THE EXTENT APPLICABLE LAW PROHIBITS SUCH LIMITATION SOME JURISDICTIONS DO NOT ALLOW THE EXCLUSION OR LIMITATION OF INCIDENTAL OR CONSEQUENTIAL DAMAGES SO THIS EXCLUSION AND LIMITATION MAY NOT APPLY TO YOU 9 Links To Other Materials Linked sites found at the VTC site are not under the control of VTC and we are not responsible for the content of any linked site or any link contained in a linked site VTC may change links based solely on our discretion and we reserve the right to terminate any link or linking program at any time VTC does not by linking to sites endorse companies or products to which it links and reserves the right to note as such on its web pages If you decide to access any of the third party sites linked to this site you do this entirely at your own risk Forums and Chat are not always screened by VTC and we are not responsible for the content of any public or open forum content at the site VTC may change these public forums based solely on our discretion and we reserve the right to terminate any forum at any time VTC does not by allowing these forums endorse companies or products which may be mentioned in these forums and reserves the right to note as such on its web pages If you decide to access any of the public forums in this site or linked to this site you do this entirely at your own risk 9 GOVERNING LAW DISPUTE RESOLUTION This Agreement is governed by Virginia law All disputes between You and VTC shall be finally resolved through arbitration in Winchester Virginia This site is controlled by VTC from its offices within the United States of America VTC makes no representation that materials in the site are appropriate or available for use in other locations and access to them from territories where their content is illegal is prohibited Those who choose to access this site from other locations do so on their own initiative and are responsible for compliance with applicable local laws You may not use or export the Materials in violation of US export laws and regulations Any claim relating to the Materials shall be governed by the internal substantive laws of the Commonwealth of Virginia USA VTC may revise these Terms at any time by updating this posting You should visit this page from time to time to review the thencurrent Terms because they are binding on you Certain provisions of these Terms may be superseded by expressly designated legal notices or terms located on particular pages at this Site If you have any questions regarding this policy or your information specifically you may email us atadminvtccom adminvtccom Courses FOR FOR FOR Facebook Twitter LinkedIn Blog</v>
       </c>
     </row>
     <row r="21">
@@ -773,16 +611,7 @@
         <v>Training and dev</v>
       </c>
       <c r="C21" t="str">
-        <v xml:space="preserve">Microsoft Virtual Academy – Free IT Training, Online Learning of Microsoft Technologies  Microsoft Virtual Academy provides free, self-paced, online training to help Developers, IT and Data Professionals, and students learn the latest technology, build their skills, and advance their careers.                    Free Microsoft Training Delivered by Experts                                       Find new courses every week! Data Science and Machine Learning Essentials Microsoft Cloud Roadshow Windows 10 Development for Absolute Beginners C++/DirectX Game Development Series Running Linux in Microsoft Azure                      See how others are learning with MVA                      World-class experts, real-world training                      Be a part of this vibrant community Welcome to the new Microsoft Virtual Academy home page :) Member Only Offer Mobile &amp; Web Developers Game Developers Network, Infrastructure, &amp; Cloud Engineers Database Admins, Architects, &amp; Developers Students interested in a career in technology                                                  Windows 10                                                  Cloud Development                                                  Game Development                                                  Web Development                                                  Database Development                                                  C# / XAML                                                  Visual Studio                                                  HTML5 &amp; CSS3                                                  For Beginners                                                  Windows 10                                                  Virtualization                                                  Identity &amp; Access Management                                                  Enterprise Security                                                  Desktop &amp; Device Management                                                  Azure for ITPros                                                  Office 365 for ITPros                                                  DevOps                                                  Server Infrastructure                                                  Database Administration                                                  Database Development                                                  Business Intelligence                                                  Advanced Analytics                                                  Big Data                                                  Azure for Data Pros                                                  SharePoint                                                  Power BI                                                  SQL Server                                                  Learn to Code                                                  Reign in the Cloud                                                  Validate your skills                                                  Educator Resources A Developer‘s Guide to Windows 10 Introduction to ASP.NET 5 Introduction to Mobile App Development Building Windows 10 Games with Unity 5 Creating Your First 2D Game with GameMaker Developing Games with Construct 2 Windows Server 2012 R2 Essentials Server Virtualization with Windows Server Hyper-V and System Center Getting Started with PowerShell 3.0 Jump Start Querying with Transact-SQL Developing Microsoft SQL Server Databases Designing Database Solutions for SQL Server C# Fundamentals for Absolute Beginners Security Fundamentals Database Fundamentals 50% 40% Want to manage your learning plans? Support                              Courses                                                       Live Events                                                       Books                                                                                        Home                                                                                                                                             For Beginners                                                                                  38                                                                                                                            Hybrid Cloud Automation                                                                                  27                                                                                                                            Database Development                                                                                  9                                                                                                                            Database Administration                                                                                  9                                                                                                                            Big Data                                                                                  8                                                                                                                            Advanced Analytics                                                                                  6                                                                                                                            Imagine - Educator Resources                                                                                  37                                                                                                                            Imagine - Validate your skills                                                                                  7                                                                                                                            Imagine - Reign in the Cloud                                                                                  7                                                                                                                            Imagine - Learn to Code                                                                                  13                                                                                                                            Enterprise Security                                                                                  20                                                                                                                            Mobile Device Management                                                                                  43                                                                                                                            HTML5                                                                                  19                                                                                                                            C# / XAML                                                                                  35                                                                                                                            App Development                                                                                  73                                                                                                                            Server Infrastructure                                                                                  86                                                                                                                            Virtualization                                                                                  38                                                                                                                            Game Development                                                                                  36                                                                                                                            Cloud App Development                                                                                  49                                                                                                                            Mobile App Development                                                                                  73                                                                                                                            Web Development                                                                                  88                                                                                                                            DevOps                                                                                  19                                                                                                                            Private Cloud                                                                                  27                                                                                                                            Hybrid Cloud                                                                                  20                                                                                                                            Identity and Access Management                                                                                  16                                                                                                                            Desktop and Device Management                                                                                  57                                                                                                                            Quick Start Challenges                                                                                  11                                                                                                                            Business Intelligence                                                                                  42                                                                                                                            Collaboration                                                                                  98                                                                                                                            Small Business                                                                                  34                                                                                                                            Licensing                                                                                  3                                                                                                                    Windows                                                                          82                                                                                                                Power BI                                                                          6                                                                                                                Windows Server                                                                          90                                                                                                                System Center                                                                          58                                                                                                                Microsoft Azure                                                                          115                                                                                                                Visual Studio                                                                          163                                                                                                                Windows Store Apps Development                                                                          38                                                                                                                Windows Phone Development                                                                          21                                                                                                                SQL Server                                                                          48                                                                                                                Office 365 for End Users                                                                          44                                                                                                                Office 365 for IT Pros                                                                          62                                                                                                                Office 365 for Developers                                                                          9                                                                                                                SharePoint                                                                          25                                                                                                                Skype for Business                                                                          13                                                                                                                Exchange                                                                          16                                                                                                                Microsoft Dynamics                                                                          13                                                                                                                C# Fundamentals for Absolute Beginners                                                                                                                                                     Windows 10 Development for Absolute Beginners                                                                                                                                                     Getting Started with PowerShell 3.0 Jump Start                                                                                                                                                     Introduction to ASP.NET MVC                                                                                                                                                     Database Fundamentals                                                                                                                                                     Introduction to AngularJS                                                                                                                                                     Web API Design Jump Start                                                                                                                                                     Hour of Code with TouchDevelop                                                                                                                                                     Programming in C# Jump Start                                                                                                                                                     Developing in HTML5 with JavaScript and CSS3 Jump Start                                                                                                                                                             App Development                                                                                                                                                                     Microsoft Azure                                                                                                                                                                     Microsoft System Center                                                                                                                                                                     Windows                                                                                                                                                                     Windows Server                                                                                                                                                                     SQL Server                                                                                                                                                                                                                                                        See All                                                                                                       See All                                                                                                                                                                          Windows Server                                                                                                                                                     Windows PowerShell                                                                                                                                                     App Development                                                                                                                                                     SQL Server and Azure SQL Database                                                                                                                                                     Windows                                                                                                                                                     SharePoint Server                                                                                                                                                     Exam Preparation                                                                                                                                                     Exchange Server                                                                                                                                                                                                                                                See All                                                                                                          See All                                                                                           Get unlimited access to content Join live events Track your progress Take self-assessments Participate in forums Receive discounts on books                                      Developers                                                                       IT Pros                                                                       Data Pros                                                                       Students                                                                                                                        C# Fundamentals for Absolute Beginners                                                                                                                                                                     Windows 10 Development for Absolute Beginners                                                                                                                                                                     Getting Started with PowerShell 3.0 Jump Start                                                                                                                                                                     Introduction to ASP.NET MVC                                                                                                                                                                     Database Fundamentals                                                                               FAQs                              Forums                                                       Feedback                                                           Sitemap                                                           Privacy &amp; Cookies                                                                      Terms of use                                                       Trademarks                          Microsoft Virtual Academy Get 50% off eBooks plus   40% off print books at   The Microsoft Press Store                        With hundreds of courses to choose from, you´re sure to find what you need!                  Join Steve Elston and Cynthia Rudin Build your cloud skills Join Bob Tabor Join Bryan Griffiths and Mickey MacDonald With Anton Boyko and Lucian Daia                      Microsoft Virtual Academy provides free, online training to help Developers, IT and Data Professionals, and students learn the latest technology, build their skills, and advance their careers.                                       Get your questions answered! Learn from teams of industry experts, see engaging demos, explore real-world scenarios, and get the training you need to apply your new skills right away.                                       It's not just you against the world anymore. Get your questions answered by our instructors and your peers, join the conversation, and share your knowledge with others.                                                   9 New Windows 10 Courses For Developers: 8 Short Ones and 1 Long One                                                                                                    08 Jan 2016 | Matthew Calder (MVA)                                                       Registered Microsoft Virtual Academy Students                                                       Likes                                                               Followers                                                                Subscribers                                                               Members                                                                                                                This was my first video course. For me the trick was two monitors and learning how to pause often! The HTML5 and CSS3 course was excellent! Bob's pace is perfect, he sticks to the pertinent material and has an 'easy to listen to' voice. Thanks!!                                                                                                                            Terry Bieritz                                                                                       United States                                                                                                                            I’ve been a C# developer for years now but have decided that I really was missing a trick by not knowing JavaScript, so I am actively trying to address that right now. The “Developing in HTML5 with JavaScript and CSS3 Jump Start” was exactly what I needed. Fast paced, enthusiastic and fun! Thanks!                                                                                                                            Martin Stickley                                                                                       United Kingdom                                                                                                                            The Microsoft Virtual Academy’s concept and ease of use encouraged me to learn in a fun and competitive environment. The Academy is indeed an innovative idea. I have asked my staff members to register and learn at the Academy.                                                                                                                            Ong Teck Soon                                                                                       Singapore                                          Back to top This is just the first step in our efforts to make the site easier for you to navigate. Stay tuned for more! All the great content that you expect is still here, so feel free to explore. Have feedback? We’d love to hear from you! Just select the Support link in the footer.                      Microsoft Virtual Academy                                       Courses                                                                    Sign in                                               Home                                              For Beginners                                                                                       Hybrid Cloud Automation                                                                                       Database Development                                                                                       Database Administration                                                                                       Big Data                                                                                       Advanced Analytics                                                                                       Imagine - Educator Resources                                                                                       Imagine - Validate your skills                                                                                       Imagine - Reign in the Cloud                                                                                       Imagine - Learn to Code                                                                                       Enterprise Security                                                                                       Mobile Device Management                                                                                       HTML5                                                                                       C# / XAML                                                                                       App Development                                                                                       Server Infrastructure                                                                                       Virtualization                                                                                       Game Development                                                                                       Cloud App Development                                                                                       Mobile App Development                                                                                       Web Development                                                                                       DevOps                                                                                       Private Cloud                                                                                       Hybrid Cloud                                                                                       Identity and Access Management                                                                                       Desktop and Device Management                                                                                       Quick Start Challenges                                                                                       Business Intelligence                                                                                       Collaboration                                                                                       Small Business                                                                                       Licensing                                                                                   Windows                                                                               Power BI                                                                               Windows Server                                                                               System Center                                                                               Microsoft Azure                                                                               Visual Studio                                                                               Windows Store Apps Development                                                                               Windows Phone Development                                                                               SQL Server                                                                               Office 365 for End Users                                                                               Office 365 for IT Pros                                                                               Office 365 for Developers                                                                               SharePoint                                                                               Skype for Business                                                                               Exchange                                                                               Microsoft Dynamics                                                                               C# Fundamentals for Absolute Beginners                                                                               Windows 10 Development for Absolute Beginners                                                                               Getting Started with PowerShell 3.0 Jump Start                                                                               Introduction to ASP.NET MVC                                                                               Database Fundamentals                                                                                                                                                              See All Courses                                                                                           See All Courses                                                                                                Introduction to AngularJS                                                                               Web API Design Jump Start                                                                               Hour of Code with TouchDevelop                                                                               Programming in C# Jump Start                                                                               Developing in HTML5 with JavaScript and CSS3 Jump Start                                                                                                                                                               See All Live Events                                                                                            See All Live Events                                                                                                    App Development                                                                                       Microsoft Azure                                                                                       Microsoft System Center                                                                                       Windows                                                                                       Windows Server                                                                                       SQL Server                                                                                                                                                                                      See All                                                                 </v>
-      </c>
-      <c r="D21" t="str">
-        <v xml:space="preserve">                                      See All                                                                                                            Windows Server                                                                               Windows PowerShell                                                                               App Development                                                                               SQL Server and Azure SQL Database                                                                               Windows                                                                               SharePoint Server                                                                               Exam Preparation                                                                               Exchange Server                                                                                                                                                                                  See All                                                                                                          See All                                                                  Become a Member Today Join now                                                                                                                                                                                                                                                                       Windows 10                                                                                                                                                                                                                                                                                                                                                     Cloud Development                                                                                                                                                                                                                                                                                                                                                     Game Development                                                                                                                                                                                                                                                                                                                                                     Web Development                                                                                                                                                                                                                                                                                                                                                     Database Development                                                                                                                                                                                                                                                                                                                                                     C# / XAML                                                                                                                                                                                                                                                                                                                                                     Visual Studio                                                                                                                                                                                                                                                                                                                                                     HTML5 &amp; CSS3                                                                                                                                                                                                                                                                                                                                                     For Beginners                                                                                                                                                                                                                                                                                                                                                     Windows 10                                                                                                                                                                                                                                                                                                                                                     Virtualization                                                                                                                                                                                                                                                                                                                                                     Identity &amp; Access Management                                                                                                                                                                                                                                                                                                                                                     Enterprise Security                                                                                                                                                                                                                                                                                                                                                     Desktop &amp; Device Management                                                                                                                                                                                                                                                                                                                                                     Azure for ITPros                                                                                                                                                                                                                                                                                                                                                     Office 365 for ITPros                                                                                                                                                                                                                                                                                                                                                     DevOps                                                                                                                                                                                                                                                                                                                                                     Server Infrastructure                                                                                                                                                                                                                                                                                                                                                     Database Administration                                                                                                                                                                                                                                                                                                                                                     Database Development                                                                                                                                                                                                                                                                                                                                                     Business Intelligence                                                                                                                                                                                                                                                                                                                                                     Advanced Analytics                                                                                                                                                                                                                                                                                                                                                     Big Data                                                                                                                                                                                                                                                                                                                                                     Azure for Data Pros                                                                                                                                                                                                                                                                                                                                                     SharePoint                                                                                                                                                                                                                                                                                                                                                     Power BI                                                                                                                                                                                                                                                                                                                                                     SQL Server                                                                                                                                                                                                                                                                                                                                                     Learn to Code                                                                                                                                                                                                                                                                                                                                                     Reign in the Cloud                                                                                                                                                                                                                                                                                                                                                     Validate your skills                                                                                                                                                                                                                                                                                                                                                     Educator Resources                                                                                                                                                     Browse all courses                                                                      Browse all courses                                                               Learn More                                                                               Most Popular                                                                                                                Most Popular                                                                                                                                              C# Fundamentals for Absolute Beginners                                                                                       Windows 10 Development for Absolute Beginners                                                                                       Getting Started with PowerShell 3.0 Jump Start                                                                                       Introduction to ASP.NET MVC                                                                                       Database Fundamentals                                           Watch now &gt;   Learn more &gt;   Watch now &gt;   Watch now &gt;   Watch now &gt;                                                                                                                              Mobile &amp; Web Developers                                                                                                                                                          Game Developers                                                                                                                                                          Network, Infrastructure, &amp; Cloud Engineers                                                                                                                                                          Database Admins, Architects, &amp; Developers                                                                                                                                                          Students interested in a career in technology                               app and mobile development training courses                                                                                                                             A Developer‘s Guide to Windows 10                                                                                                                                                      Introduction to ASP.NET 5                                                                                                                                                  Introduction to Mobile App Development                          Check out game development courses                                                                                                                             Building Windows 10 Games with Unity 5                                                                                                                                                      Creating Your First 2D Game with GameMaker                                                                                                                                                  Developing Games with Construct 2                          learn how to extend your datacenter to the cloud                                                                                                                             Windows Server 2012 R2 Essentials                                                                                                                                                      Server Virtualization with Windows Server Hyper-V and System Center                                                                                                                                                  Getting Started with PowerShell 3.0 Jump Start                          how to easily build predictive analytics solutions                                                                                                                             Querying with Transact-SQL                                                                                                                                                      Developing Microsoft SQL Server Databases                                                                                                                                                  Designing Database Solutions for SQL Server                          beginner technology training courses                                                                                                                             C# Fundamentals for Absolute Beginners                                                                                                                                                      Security Fundamentals                                                                                                                                                  Database Fundamentals                          Tweets by @MSVirtAcademy                                                                                                                                      Latest blog post                              9 New Windows 10 Courses For Developers: 8 Short Ones and 1 Long One read more Read more                                                                                                                                                                                   209,304                                                                                           Likes                                                                                                                                                                                                                                                              90,916                                                                                           Followers                                                                                                                                                                                                                                                               5,139                                                                                           Subscribers                                                                                                                                                                                                                                                              2,845                                                                                           Members                                                                                                                  Back to top                 Back to top              Chinese - Simplified Chinese - Traditional Czech French German Italian Japanese Korean Polish Portuguese (Brazil) Russian Spanish Turkish FAQs Forums Feedback Sitemap Privacy &amp; Cookies Terms of use Trademarks Courses Sign in 38 27 9 9 8 6 37 7 7 13 20 43 19 35 73 86 38 36 49 73 88 19 27 20 16 57 11 42 98 34 3 82 6 90 58 115 163 38 21 48 44 62 9 25 13 16 13 Get unlimited access to content Join live events Track your progress Take self-assessments Participate in forums Receive discounts on books                                      Browse all courses                                          Most Popular Watch now &gt; Learn more &gt; Watch now &gt; Watch now &gt; Watch now &gt; Previous Next                                      Latest blog post                                      08 Jan 2016 | Matthew Calder (MVA)                                  Read more                          Success Stories                      Back to top Get Started English English Support</v>
-      </c>
-      <c r="E21" t="str">
-        <v xml:space="preserve">                                      See All                                                                                                            Windows Server                                                                               Windows PowerShell                                                                               App Development                                                                               SQL Server and Azure SQL Database                                                                               Windows                                                                               SharePoint Server                                                                               Exam Preparation                                                                               Exchange Server                                                                                                                                                                                  See All                                                                                                          See All                                                                  Become a Member Today Join now                                                                                                                                                                                                                                                                       Windows 10                                                                                                                                                                                                                                                                                                                                                     Cloud Development                                                                                                                                                                                                                                                                                                                                                     Game Development                                                                                                                                                                                                                                                                                                                                                     Web Development                                                                                                                                                                                                                                                                                                                                                     Database Development                                                                                                                                                                                                                                                                                                                                                     C# / XAML                                                                                                                                                                                                                                                                                                                                                     Visual Studio                                                                                                                                                                                                                                                                                                                                                     HTML5 &amp; CSS3                                                                                                                                                                                                                                                                                                                                                     For Beginners                                                                                                                                                                                                                                                                                                                                                     Windows 10                                                                                                                                                                                                                                                                                                                                                     Virtualization                                                                                                                                                                                                                                                                                                                                                     Identity &amp; Access Management                                                                                                                                                                                                                                                                                                                                                     Enterprise Security                                                                                                                                                                                                                                                                                                                                                     Desktop &amp; Device Management                                                                                                                                                                                                                                                                                                                                                     Azure for ITPros                                                                                                                                                                                                                                                                                                                                                     Office 365 for ITPros                                                                                                                                                                                                                                                                                                                                                     DevOps                                                                                                                                                                                                                                                                                                                                                     Server Infrastructure                                                                                                                                                                                                                                                                                                                                                     Database Administration                                                                                                                                                                                                                                                                                                                                                     Database Development                                                                                                                                                                                                                                                                                                                                                     Business Intelligence                                                                                                                                                                                                                                                                                                                                                     Advanced Analytics                                                                                                                                                                                                                                                                                                                                                     Big Data                                                                                                                                                                                                                                                                                                                                                     Azure for Data Pros                                                                                                                                                                                                                                                                                                                                                     SharePoint                                                                                                                                                                                                                                                                                                                                                     Power BI                                                                                                                                                                                                                                                                                                                                                     SQL Server                                                                                                                                                                                                                                                                                                                                                     Learn to Code                                                                                                                                                                                                                                                                                                                                                     Reign in the Cloud                                                                                                                                                                                                                                                                                                                                                     Validate your skills                                                                                                                                                                                                                                                                                                                                                     Educator Resources                                                                                                                                                     Browse all courses                                                                      Browse all courses                                                               Learn More                                                                               Most Popular                                                                                                                Most Popular                                                                                                                                              C# Fundamentals for Absolute Beginners                                                                                       Windows 10 Development for Absolute Beginners                                                                                       Getting Started with PowerShell 3.0 Jump Start                                                                                       Introduction to ASP.NET MVC                                                                                       Database Fundamentals                                           Watch now &gt;   Learn more &gt;   Watch now &gt;   Watch now &gt;   Watch now &gt;                                                                                                                              Mobile &amp; Web Developers                                                                                                                                                          Game Developers                                                                                                                                                          Network, Infrastructure, &amp; Cloud Engineers                                                                                                                                                          Database Admins, Architects, &amp; Developers                                                                                                                                                          Students interested in a career in technology                               app and mobile development training courses                                                                                                                             A Developer‘s Guide to Windows 10                                                                                                                                                      Introduction to ASP.NET 5                                                                                                                                                  Introduction to Mobile App Development                          Check out game development courses                                                                                                                             Building Windows 10 Games with Unity 5                                                                                                                                                      Creating Your First 2D Game with GameMaker                                                                                                                                                  Developing Games with Construct 2                          learn how to extend your datacenter to the cloud                                                                                                                             Windows Server 2012 R2 Essentials                                                                                                                                                      Server Virtualization with Windows Server Hyper-V and System Center                                                                                                                                                  Getting Started with PowerShell 3.0 Jump Start                          how to easily build predictive analytics solutions                                                                                                                             Querying with Transact-SQL                                                                                                                                                      Developing Microsoft SQL Server Databases                                                                                                                                                  Designing Database Solutions for SQL Server                          beginner technology training courses                                                                                                                             C# Fundamentals for Absolute Beginners                                                                                                                                                      Security Fundamentals                                                                                                                                                  Database Fundamentals                          Tweets by @MSVirtAcademy                                                                                                                                      Latest blog post                              9 New Windows 10 Courses For Developers: 8 Short Ones and 1 Long One read more Read more                                                                                                                                                                                   209,304                                                                                           Likes                                                                                                                                                                                                                                                              90,916                                                                                           Followers                                                                                                                                                                                                                                                               5,139                                                                                           Subscribers                                                                                                                                                                                                                                                              2,845                                                                                           Members                                                                                                                  Back to top                 Back to top              Chinese - Simplified Chinese - Traditional Czech French German Italian Japanese Korean Polish Portuguese (Brazil) Russian Spanish Turkish FAQs Forums Feedback Sitemap Privacy &amp; Cookies Terms of use Trademarks Courses Sign in 38 27 9 9 8 6 37 7 7 13 20 43 19 35 73 86 38 36 49 73 88 19 27 20 16 57 11 42 98 34 3 82 6 90 58 115 163 38 21 48 44 62 9 25 13 16 13 Get unlimited access to content Join live events Track your progress Take self-assessments Participate in forums Receive discounts on books                                      Browse all courses                                          Most Popular Watch now &gt; Learn more &gt; Watch now &gt; Watch now &gt; Watch now &gt; Previous Next                                      Latest blog post                                      08 Jan 2016 | Matthew Calder (MVA)                                  Read more                          Success Stories                      Back to top Get Started English English Support</v>
-      </c>
-      <c r="F21" t="str">
-        <v xml:space="preserve">                                      See All                                                                                                            Windows Server                                                                               Windows PowerShell                                                                               App Development                                                                               SQL Server and Azure SQL Database                                                                               Windows                                                                               SharePoint Server                                                                               Exam Preparation                                                                               Exchange Server                                                                                                                                                                                  See All                                                                                                          See All                                                                  Become a Member Today Join now                                                                                                                                                                                                                                                                       Windows 10                                                                                                                                                                                                                                                                                                                                                     Cloud Development                                                                                                                                                                                                                                                                                                                                                     Game Development                                                                                                                                                                                                                                                                                                                                                     Web Development                                                                                                                                                                                                                                                                                                                                                     Database Development                                                                                                                                                                                                                                                                                                                                                     C# / XAML                                                                                                                                                                                                                                                                                                                                                     Visual Studio                                                                                                                                                                                                                                                                                                                                                     HTML5 &amp; CSS3                                                                                                                                                                                                                                                                                                                                                     For Beginners                                                                                                                                                                                                                                                                                                                                                     Windows 10                                                                                                                                                                                                                                                                                                                                                     Virtualization                                                                                                                                                                                                                                                                                                                                                     Identity &amp; Access Management                                                                                                                                                                                                                                                                                                                                                     Enterprise Security                                                                                                                                                                                                                                                                                                                                                     Desktop &amp; Device Management                                                                                                                                                                                                                                                                                                                                                     Azure for ITPros                                                                                                                                                                                                                                                                                                                                                     Office 365 for ITPros                                                                                                                                                                                                                                                                                                                                                     DevOps                                                                                                                                                                                                                                                                                                                                                     Server Infrastructure                                                                                                                                                                                                                                                                                                                                                     Database Administration                                                                                                                                                                                                                                                                                                                                                     Database Development                                                                                                                                                                                                                                                                                                                                                     Business Intelligence                                                                                                                                                                                                                                                                                                                                                     Advanced Analytics                                                                                                                                                                                                                                                                                                                                                     Big Data                                                                                                                                                                                                                                                                                                                                                     Azure for Data Pros                                                                                                                                                                                                                                                                                                                                                     SharePoint                                                                                                                                                                                                                                                                                                                                                     Power BI                                                                                                                                                                                                                                                                                                                                                     SQL Server                                                                                                                                                                                                                                                                                                                                                     Learn to Code                                                                                                                                                                                                                                                                                                                                                     Reign in the Cloud                                                                                                                                                                                                                                                                                                                                                     Validate your skills                                                                                                                                                                                                                                                                                                                                                     Educator Resources                                                                                                                                                     Browse all courses                                                                      Browse all courses                                                               Learn More                                                                               Most Popular                                                                                                                Most Popular                                                                                                                                              C# Fundamentals for Absolute Beginners                                                                                       Windows 10 Development for Absolute Beginners                                                                                       Getting Started with PowerShell 3.0 Jump Start                                                                                       Introduction to ASP.NET MVC                                                                                       Database Fundamentals                                           Watch now &gt;   Learn more &gt;   Watch now &gt;   Watch now &gt;   Watch now &gt;                                                                                                                              Mobile &amp; Web Developers                                                                                                                                                          Game Developers                                                                                                                                                          Network, Infrastructure, &amp; Cloud Engineers                                                                                                                                                          Database Admins, Architects, &amp; Developers                                                                                                                                                          Students interested in a career in technology                               app and mobile development training courses                                                                                                                             A Developer‘s Guide to Windows 10                                                                                                                                                      Introduction to ASP.NET 5                                                                                                                                                  Introduction to Mobile App Development                          Check out game development courses                                                                                                                             Building Windows 10 Games with Unity 5                                                                                                                                                      Creating Your First 2D Game with GameMaker                                                                                                                                                  Developing Games with Construct 2                          learn how to extend your datacenter to the cloud                                                                                                                             Windows Server 2012 R2 Essentials                                                                                                                                                      Server Virtualization with Windows Server Hyper-V and System Center                                                                                                                                                  Getting Started with PowerShell 3.0 Jump Start                          how to easily build predictive analytics solutions                                                                                                                             Querying with Transact-SQL                                                                                                                                                      Developing Microsoft SQL Server Databases                                                                                                                                                  Designing Database Solutions for SQL Server                          beginner technology training courses                                                                                                                             C# Fundamentals for Absolute Beginners                                                                                                                                                      Security Fundamentals                                                                                                                                                  Database Fundamentals                          Tweets by @MSVirtAcademy                                                                                                                                      Latest blog post                              9 New Windows 10 Courses For Developers: 8 Short Ones and 1 Long One read more Read more                                                                                                                                                                                   209,304                                                                                           Likes                                                                                                                                                                                                                                                              90,916                                                                                           Followers                                                                                                                                                                                                                                                               5,139                                                                                           Subscribers                                                                                                                                                                                                                                                              2,845                                                                                           Members                                                                                                                  Back to top                 Back to top              Chinese - Simplified Chinese - Traditional Czech French German Italian Japanese Korean Polish Portuguese (Brazil) Russian Spanish Turkish FAQs Forums Feedback Sitemap Privacy &amp; Cookies Terms of use Trademarks Courses Sign in 38 27 9 9 8 6 37 7 7 13 20 43 19 35 73 86 38 36 49 73 88 19 27 20 16 57 11 42 98 34 3 82 6 90 58 115 163 38 21 48 44 62 9 25 13 16 13 Get unlimited access to content Join live events Track your progress Take self-assessments Participate in forums Receive discounts on books                                      Browse all courses                                          Most Popular Watch now &gt; Learn more &gt; Watch now &gt; Watch now &gt; Watch now &gt; Previous Next                                      Latest blog post                                      08 Jan 2016 | Matthew Calder (MVA)                                  Read more                          Success Stories                      Back to top Get Started English English Support</v>
+        <v>Microsoft Virtual Academy Free IT Training Online Learning of Microsoft Technologies Microsoft Virtual Academy provides free selfpaced online training to help Developers IT and Data Professionals and students learn the latest technology build their skills and advance their careers Free Microsoft Training Delivered by Experts Find new courses every week Data Science and Machine Learning Essentials Microsoft Cloud Roadshow Windows 10 Development for Absolute Beginners CDirectX Game Development Series Running Linux in Microsoft Azure See how others are learning with MVA Worldclass experts realworld training Be a part of this vibrant community Welcome to the new Microsoft Virtual Academy home page Member Only Offer Mobile Web Developers Game Developers Network Infrastructure Cloud Engineers Database Admins Architects Developers Students interested in a career in technology Windows 10 Cloud Development Game Development Web Development Database Development C XAML Visual Studio HTML5 CSS3 For Beginners Windows 10 Virtualization Identity Access Management Enterprise Security Desktop Device Management Azure for ITPros Office 365 for ITPros DevOps Server Infrastructure Database Administration Database Development Business Intelligence Advanced Analytics Big Data Azure for Data Pros SharePoint Power BI SQL Server Learn to Code Reign in the Cloud Validate your skills Educator Resources A Developer‘s Guide to Windows 10 Introduction to ASPNET 5 Introduction to Mobile App Development Building Windows 10 Games with Unity 5 Creating Your First 2D Game with GameMaker Developing Games with Construct 2 Windows Server 2012 R2 Essentials Server Virtualization with Windows Server HyperV and System Center Getting Started with PowerShell 30 Jump Start Querying with TransactSQL Developing Microsoft SQL Server Databases Designing Database Solutions for SQL Server C Fundamentals for Absolute Beginners Security Fundamentals Database Fundamentals 50 40 Want to manage your learning plans Support Courses Live Events Books Home For Beginners 38 Hybrid Cloud Automation 27 Database Development 9 Database Administration 9 Big Data 8 Advanced Analytics 6 Imagine Educator Resources 37 Imagine Validate your skills 7 Imagine Reign in the Cloud 7 Imagine Learn to Code 13 Enterprise Security 20 Mobile Device Management 43 HTML5 19 C XAML 35 App Development 73 Server Infrastructure 86 Virtualization 38 Game Development 36 Cloud App Development 49 Mobile App Development 73 Web Development 88 DevOps 19 Private Cloud 27 Hybrid Cloud 20 Identity and Access Management 16 Desktop and Device Management 57 Quick Start Challenges 11 Business Intelligence 42 Collaboration 98 Small Business 34 Licensing 3 Windows 82 Power BI 6 Windows Server 90 System Center 58 Microsoft Azure 115 Visual Studio 163 Windows Store Apps Development 38 Windows Phone Development 21 SQL Server 48 Office 365 for End Users 44 Office 365 for IT Pros 62 Office 365 for Developers 9 SharePoint 25 Skype for Business 13 Exchange 16 Microsoft Dynamics 13 C Fundamentals for Absolute Beginners Windows 10 Development for Absolute Beginners Getting Started with PowerShell 30 Jump Start Introduction to ASPNET MVC Database Fundamentals Introduction to AngularJS Web API Design Jump Start Hour of Code with TouchDevelop Programming in C Jump Start Developing in HTML5 with JavaScript and CSS3 Jump Start App Development Microsoft Azure Microsoft System Center Windows Windows Server SQL Server See All See All Windows Server Windows PowerShell App Development SQL Server and Azure SQL Database Windows SharePoint Server Exam Preparation Exchange Server See All See All Get unlimited access to content Join live events Track your progress Take selfassessments Participate in forums Receive discounts on books Developers IT Pros Data Pros Students C Fundamentals for Absolute Beginners Windows 10 Development for Absolute Beginners Getting Started with PowerShell 30 Jump Start Introduction to ASPNET MVC Database Fundamentals FAQs Forums Feedback Sitemap Privacy Cookies Terms of use Trademarks Microsoft Virtual Academy Get 50 off eBooks plus 40 off print books at The Microsoft Press Store With hundreds of courses to choose from you´re sure to find what you need Join Steve Elston and Cynthia Rudin Build your cloud skills Join Bob Tabor Join Bryan Griffiths and Mickey MacDonald With Anton Boyko and Lucian Daia Microsoft Virtual Academy provides free online training to help Developers IT and Data Professionals and students learn the latest technology build their skills and advance their careers Get your questions answered Learn from teams of industry experts see engaging demos explore realworld scenarios and get the training you need to apply your new skills right away Its not just you against the world anymore Get your questions answered by our instructors and your peers join the conversation and share your knowledge with others 9 New Windows 10 Courses For Developers 8 Short Ones and 1 Long One 08 Jan 2016 Matthew Calder MVA Registered Microsoft Virtual Academy Students Likes Followers Subscribers Members This was my first video course For me the trick was two monitors and learning how to pause often The HTML5 and CSS3 course was excellent Bobs pace is perfect he sticks to the pertinent material and has an easy to listen to voice Thanks Terry Bieritz United States I’ve been a C developer for years now but have decided that I really was missing a trick by not knowing JavaScript so I am actively trying to address that right now The “Developing in HTML5 with JavaScript and CSS3 Jump Start” was exactly what I needed Fast paced enthusiastic and fun Thanks Martin Stickley United Kingdom The Microsoft Virtual Academy’s concept and ease of use encouraged me to learn in a fun and competitive environment The Academy is indeed an innovative idea I have asked my staff members to register and learn at the Academy Ong Teck Soon Singapore Back to top This is just the first step in our efforts to make the site easier for you to navigate Stay tuned for more All the great content that you expect is still here so feel free to explore Have feedback We’d love to hear from you Just select the Support link in the footer Microsoft Virtual Academy Courses Sign in Home For Beginners Hybrid Cloud Automation Database Development Database Administration Big Data Advanced Analytics Imagine Educator Resources Imagine Validate your skills Imagine Reign in the Cloud Imagine Learn to Code Enterprise Security Mobile Device Management HTML5 C XAML App Development Server Infrastructure Virtualization Game Development Cloud App Development Mobile App Development Web Development DevOps Private Cloud Hybrid Cloud Identity and Access Management Desktop and Device Management Quick Start Challenges Business Intelligence Collaboration Small Business Licensing Windows Power BI Windows Server System Center Microsoft Azure Visual Studio Windows Store Apps Development Windows Phone Development SQL Server Office 365 for End Users Office 365 for IT Pros Office 365 for Developers SharePoint Skype for Business Exchange Microsoft Dynamics C Fundamentals for Absolute Beginners Windows 10 Development for Absolute Beginners Getting Started with PowerShell 30 Jump Start Introduction to ASPNET MVC Database Fundamentals See All Courses See All Courses Introduction to AngularJS Web API Design Jump Start Hour of Code with TouchDevelop Programming in C Jump Start Developing in HTML5 with JavaScript and CSS3 Jump Start See All Live Events See All Live Events App Development Microsoft Azure Microsoft System Center Windows Windows Server SQL Server See All See All Windows Server Windows PowerShell App Development SQL Server and Azure SQL Database Windows SharePoint Server Exam Preparation Exchange Server See All See All Become a Member Today Join now Windows 10 Cloud Development Game Development Web Development Database Development C XAML Visual Studio HTML5 CSS3 For Beginners Windows 10 Virtualization Identity Access Management Enterprise Security Desktop Device Management Azure for ITPros Office 365 for ITPros DevOps Server Infrastructure Database Administration Database Development Business Intelligence Advanced Analytics Big Data Azure for Data Pros SharePoint Power BI SQL Server Learn to Code Reign in the Cloud Validate your skills Educator Resources Browse all courses Browse all courses Learn More Most Popular Most Popular C Fundamentals for Absolute Beginners Windows 10 Development for Absolute Beginners Getting Started with PowerShell 30 Jump Start Introduction to ASPNET MVC Database Fundamentals Watch now Learn more Watch now Watch now Watch now Mobile Web Developers Game Developers Network Infrastructure Cloud Engineers Database Admins Architects Developers Students interested in a career in technology app and mobile development training courses A Developer‘s Guide to Windows 10 Introduction to ASPNET 5 Introduction to Mobile App Development Check out game development courses Building Windows 10 Games with Unity 5 Creating Your First 2D Game with GameMaker Developing Games with Construct 2 learn how to extend your datacenter to the cloud Windows Server 2012 R2 Essentials Server Virtualization with Windows Server HyperV and System Center Getting Started with PowerShell 30 Jump Start how to easily build predictive analytics solutions Querying with TransactSQL Developing Microsoft SQL Server Databases Designing Database Solutions for SQL Server beginner technology training courses C Fundamentals for Absolute Beginners Security Fundamentals Database Fundamentals Tweets by MSVirtAcademy Latest blog post 9 New Windows 10 Courses For Developers 8 Short Ones and 1 Long One read more Read more 209304 Likes 90916 Followers 5139 Subscribers 2845 Members Back to top Back to top Chinese Simplified Chinese Traditional Czech French German Italian Japanese Korean Polish Portuguese Brazil Russian Spanish Turkish FAQs Forums Feedback Sitemap Privacy Cookies Terms of use Trademarks Courses Sign in 38 27 9 9 8 6 37 7 7 13 20 43 19 35 73 86 38 36 49 73 88 19 27 20 16 57 11 42 98 34 3 82 6 90 58 115 163 38 21 48 44 62 9 25 13 16 13 Get unlimited access to content Join live events Track your progress Take selfassessments Participate in forums Receive discounts on books Browse all courses Most Popular Watch now Learn more Watch now Watch now Watch now Previous Next Latest blog post 08 Jan 2016 Matthew Calder MVA Read more Success Stories Back to top Get Started English English Support</v>
       </c>
     </row>
     <row r="22">
@@ -793,16 +622,7 @@
         <v>IT and systems support</v>
       </c>
       <c r="C22" t="str">
-        <v>Computer Support, IT Consulting, Network Services - Guelph, Kitchener, Waterloo | HLB System Solutions HLB System Solutions specializes in IT Consulting, providing business Computer Support and Network Services in Guelph, Kitchener, Waterloo, Cambridge, Fergus and Arthur. “Are You Searching For An IT Support FirmBut You Don’t Know Who You Can Trust To Fix It Fast? Thank you Guelph for voting HLB as Best In Class! Office 365 Solution Industry leading collaboration suite – often copied never equalled How fast can you be back up and running after your system goes down? Most importantly, how much is it going to cost you? Why Choose HLB? Your One Stop Shop For All Your Technology Needs See what other business owners are saying about us... We're proud to partner with the best businesses in the industry. HLB System Solutions Microsoft Support has ended! Call Us Today At 519-822-3450! Managed Services Business Continuity Planning IT Consulting Cloud Computing Contact Info Navigation We’re Hiring! Support Center Is This You? How We Work Services Managed Services Business Continuity Planning Beyond Backup IT Consulting  Security On Demand Services Office Moves   Virtualization Email / Spam Protection Cloud Computing Web and Software Development  Managed Services Business Continuity Planning Beyond Backup IT Consulting  Security On Demand Services Office Moves   Security On Demand Services Office Moves Virtualization Email / Spam Protection Cloud Computing Web and Software Development 7 Things We Do Better Free Stuff   Newsletter Archive  Newsletter Archive Our Clients About Us   Job Opportunities Our Team Partners &amp; Certifications Referral Program Contact Us Support Center  Job Opportunities Our Team Partners &amp; Certifications Referral Program Contact Us Support Center Blog       “Are You Searching For An IT Support FirmBut You Don’t Know Who You Can Trust To Fix It Fast? Call Now to Speak to a Live Representative                  Microsoft Support has ended! What should you do?                    Thank you Guelph  for voting HLB as Best In Class!                 Office 365 Solution Industry leading collaboration suite – often copied never equalled Enhance work efficiency today               How fast can you be back up and running after your system goes down? Most importantly, how much is it going to cost you? Let's find out        Putting an end to your IT worries and dealing with your technology from A to Z. Bringing predictability to your IT budget with technology support that’s proactive and dependable. Investing in the future of your company with IT solutions that are built to last. Managed IT Services Cloud Computing Data Backup Solutions Disaster Recovery Planning Desktop Support Server Support Email/Spam Protection Network Security Website Design Virtualization HLB System Solutions  50 Malcolm RoadUnit 1Guelph, Ontario  N1K 1A9 Phone: 519-822-3450 Fax: 519-822-8861 About Us Services Support Center Contact Us Privacy Policy Website by Pronto Privacy Policy Website by Pronto Submit a Support RequestContact Us HLB System Solutions  50 Malcolm RoadUnit 1Guelph, Ontario Canada 519-822-3450 Get Directions Call Now to Speak to a Live Representative What should you do?  Enhance work efficiency today  Let's find out  With Managed Services from HLB System Solutions, you transfer the day-to-day management of your technology to us. Learn how your business can benefit. read more Protect all you've worked for, with Business Continuity Planning that ensures your company can weather any storm. read more Take your technology strategy to the next level with comprehensive, long-term IT Consulting from HLB System Solutions. read more Discover how Cloud Computing solutions can help you save money, increase productivity and simplify your business. read more Our true passion is playing a part in our clients’ success. We are only successful when our clients are successful! That is why our entire organization is built around aligning our goals with yours. As a small business owner myself, I share the same expectations from our own partners, as you would expect from an IT service company. I believe that great relationships are the foundations for great business, and trust can only be earned through action. That’s why at HLB, “We do what we say, we finish what we start, we show up on time and we say please and thank you." Lennart Berglund President, HLB System Solutions "HLB has filled all of our IT needs." HLB System Solutions has been servicing and supporting Ag Energy for almost a decade and most notably helped develop their CIS software application. When Ag Energy’s IT manager left the organization, it was suggested they consider utilizing HLB System Solutions managed services option rather than replacing their IT manager. After careful review and consideration, they opted to try the managed service program for a period of time until they could determine what their needs were. Rose Gage CEO, Ag Energy "They have been instrumental to our growth…" HLB has been a part of our team for many years now and truly understands our business. They have been instrumental to our growth and continue to provide innovative ideas on how to move us forward. We can comfortably focus on our business and let the friendly staff at HLB take care of our IT systems.  Manager of a local healthcare company "HLB help support our in-house IT personnel and also looks after all of our hardware needs..." We have been a client of HLBSS since early 2000. Currently they come in every morning to help support our in-house IT personnel and also look after all of our hardware needs. They also designed our website and our intranet site. I highly recommend them for either your sole IT support or as additional support to any in-house IT resources you may have.  RLB LLP, Chartered Accountants and Business Advisors !function ($) { $(function() {$("#partners-partners-certifications-slider").carousel()})}(window.jQuery)  ©2016 HLB System Solutions. All Rights Reserved. ©2016 HLB System Solutions. All Rights Reserved. We’re Hiring! Support Center Is This You? How We Work Services  Managed Services Business Continuity Planning Beyond Backup IT Consulting Security On Demand Services Office Moves Virtualization Email / Spam Protection Cloud Computing Web and Software Development 7 Things We Do Better Free Stuff  Newsletter Archive Our Clients About Us  Job Opportunities Our Team Partners &amp; Certifications Referral Program Contact Us Support Center Blog Submit a Support Request Contact Us 519-822-3450 Get Directions What should you do? Enhance work efficiency today Let's find out read more read more read more read more Read more testimonials About Us Services Support Center Contact Us Tweets by @HLBSolutions Privacy Policy Website by Pronto Privacy Policy Website by Pronto HLB System Solutions  50 Malcolm RoadUnit 1 Guelph Ontario  Canada for voting HLB as Best In Class! Most importantly, 519-822-3450! Managed IT Services Cloud Computing Data Backup Solutions Disaster Recovery Planning Desktop Support Server Support Email/Spam Protection Network Security Website Design Virtualization HLB System Solutions  50 Malcolm RoadUnit 1 Guelph Ontario  N1K 1A9 519-822-3450 519-822-8861</v>
-      </c>
-      <c r="D22" t="str">
-        <v>Computer Support, IT Consulting, Network Services - Guelph, Kitchener, Waterloo | HLB System Solutions HLB System Solutions specializes in IT Consulting, providing business Computer Support and Network Services in Guelph, Kitchener, Waterloo, Cambridge, Fergus and Arthur. “Are You Searching For An IT Support FirmBut You Don’t Know Who You Can Trust To Fix It Fast? Thank you Guelph for voting HLB as Best In Class! Office 365 Solution Industry leading collaboration suite – often copied never equalled How fast can you be back up and running after your system goes down? Most importantly, how much is it going to cost you? Why Choose HLB? Your One Stop Shop For All Your Technology Needs See what other business owners are saying about us... We're proud to partner with the best businesses in the industry. HLB System Solutions Microsoft Support has ended! Call Us Today At 519-822-3450! Managed Services Business Continuity Planning IT Consulting Cloud Computing Contact Info Navigation We’re Hiring! Support Center Is This You? How We Work Services Managed Services Business Continuity Planning Beyond Backup IT Consulting  Security On Demand Services Office Moves   Virtualization Email / Spam Protection Cloud Computing Web and Software Development  Managed Services Business Continuity Planning Beyond Backup IT Consulting  Security On Demand Services Office Moves   Security On Demand Services Office Moves Virtualization Email / Spam Protection Cloud Computing Web and Software Development 7 Things We Do Better Free Stuff   Newsletter Archive  Newsletter Archive Our Clients About Us   Job Opportunities Our Team Partners &amp; Certifications Referral Program Contact Us Support Center  Job Opportunities Our Team Partners &amp; Certifications Referral Program Contact Us Support Center Blog       “Are You Searching For An IT Support FirmBut You Don’t Know Who You Can Trust To Fix It Fast? Call Now to Speak to a Live Representative                  Microsoft Support has ended! What should you do?                    Thank you Guelph  for voting HLB as Best In Class!                 Office 365 Solution Industry leading collaboration suite – often copied never equalled Enhance work efficiency today               How fast can you be back up and running after your system goes down? Most importantly, how much is it going to cost you? Let's find out        Putting an end to your IT worries and dealing with your technology from A to Z. Bringing predictability to your IT budget with technology support that’s proactive and dependable. Investing in the future of your company with IT solutions that are built to last. Managed IT Services Cloud Computing Data Backup Solutions Disaster Recovery Planning Desktop Support Server Support Email/Spam Protection Network Security Website Design Virtualization HLB System Solutions  50 Malcolm RoadUnit 1Guelph, Ontario  N1K 1A9 Phone: 519-822-3450 Fax: 519-822-8861 About Us Services Support Center Contact Us Privacy Policy Website by Pronto Privacy Policy Website by Pronto Submit a Support RequestContact Us HLB System Solutions  50 Malcolm RoadUnit 1Guelph, Ontario Canada 519-822-3450 Get Directions Call Now to Speak to a Live Representative What should you do?  Enhance work efficiency today  Let's find out  With Managed Services from HLB System Solutions, you transfer the day-to-day management of your technology to us. Learn how your business can benefit. read more Protect all you've worked for, with Business Continuity Planning that ensures your company can weather any storm. read more Take your technology strategy to the next level with comprehensive, long-term IT Consulting from HLB System Solutions. read more Discover how Cloud Computing solutions can help you save money, increase productivity and simplify your business. read more Our true passion is playing a part in our clients’ success. We are only successful when our clients are successful! That is why our entire organization is built around aligning our goals with yours. As a small business owner myself, I share the same expectations from our own partners, as you would expect from an IT service company. I believe that great relationships are the foundations for great business, and trust can only be earned through action. That’s why at HLB, “We do what we say, we finish what we start, we show up on time and we say please and thank you." Lennart Berglund President, HLB System Solutions "HLB has filled all of our IT needs." HLB System Solutions has been servicing and supporting Ag Energy for almost a decade and most notably helped develop their CIS software application. When Ag Energy’s IT manager left the organization, it was suggested they consider utilizing HLB System Solutions managed services option rather than replacing their IT manager. After careful review and consideration, they opted to try the managed service program for a period of time until they could determine what their needs were. Rose Gage CEO, Ag Energy "They have been instrumental to our growth…" HLB has been a part of our team for many years now and truly understands our business. They have been instrumental to our growth and continue to provide innovative ideas on how to move us forward. We can comfortably focus on our business and let the friendly staff at HLB take care of our IT systems.  Manager of a local healthcare company "HLB help support our in-house IT personnel and also looks after all of our hardware needs..." We have been a client of HLBSS since early 2000. Currently they come in every morning to help support our in-house IT personnel and also look after all of our hardware needs. They also designed our website and our intranet site. I highly recommend them for either your sole IT support or as additional support to any in-house IT resources you may have.  RLB LLP, Chartered Accountants and Business Advisors !function ($) { $(function() {$("#partners-partners-certifications-slider").carousel()})}(window.jQuery)  ©2016 HLB System Solutions. All Rights Reserved. ©2016 HLB System Solutions. All Rights Reserved. We’re Hiring! Support Center Is This You? How We Work Services  Managed Services Business Continuity Planning Beyond Backup IT Consulting Security On Demand Services Office Moves Virtualization Email / Spam Protection Cloud Computing Web and Software Development 7 Things We Do Better Free Stuff  Newsletter Archive Our Clients About Us  Job Opportunities Our Team Partners &amp; Certifications Referral Program Contact Us Support Center Blog Submit a Support Request Contact Us 519-822-3450 Get Directions What should you do? Enhance work efficiency today Let's find out read more read more read more read more Read more testimonials About Us Services Support Center Contact Us Tweets by @HLBSolutions Privacy Policy Website by Pronto Privacy Policy Website by Pronto HLB System Solutions  50 Malcolm RoadUnit 1 Guelph Ontario  Canada for voting HLB as Best In Class! Most importantly, 519-822-3450! Managed IT Services Cloud Computing Data Backup Solutions Disaster Recovery Planning Desktop Support Server Support Email/Spam Protection Network Security Website Design Virtualization HLB System Solutions  50 Malcolm RoadUnit 1 Guelph Ontario  N1K 1A9 519-822-3450 519-822-8861</v>
-      </c>
-      <c r="E22" t="str">
-        <v>Computer Support, IT Consulting, Network Services - Guelph, Kitchener, Waterloo | HLB System Solutions HLB System Solutions specializes in IT Consulting, providing business Computer Support and Network Services in Guelph, Kitchener, Waterloo, Cambridge, Fergus and Arthur. “Are You Searching For An IT Support FirmBut You Don’t Know Who You Can Trust To Fix It Fast? Thank you Guelph for voting HLB as Best In Class! Office 365 Solution Industry leading collaboration suite – often copied never equalled How fast can you be back up and running after your system goes down? Most importantly, how much is it going to cost you? Why Choose HLB? Your One Stop Shop For All Your Technology Needs See what other business owners are saying about us... We're proud to partner with the best businesses in the industry. HLB System Solutions Microsoft Support has ended! Call Us Today At 519-822-3450! Managed Services Business Continuity Planning IT Consulting Cloud Computing Contact Info Navigation We’re Hiring! Support Center Is This You? How We Work Services Managed Services Business Continuity Planning Beyond Backup IT Consulting  Security On Demand Services Office Moves   Virtualization Email / Spam Protection Cloud Computing Web and Software Development  Managed Services Business Continuity Planning Beyond Backup IT Consulting  Security On Demand Services Office Moves   Security On Demand Services Office Moves Virtualization Email / Spam Protection Cloud Computing Web and Software Development 7 Things We Do Better Free Stuff   Newsletter Archive  Newsletter Archive Our Clients About Us   Job Opportunities Our Team Partners &amp; Certifications Referral Program Contact Us Support Center  Job Opportunities Our Team Partners &amp; Certifications Referral Program Contact Us Support Center Blog       “Are You Searching For An IT Support FirmBut You Don’t Know Who You Can Trust To Fix It Fast? Call Now to Speak to a Live Representative                  Microsoft Support has ended! What should you do?                    Thank you Guelph  for voting HLB as Best In Class!                 Office 365 Solution Industry leading collaboration suite – often copied never equalled Enhance work efficiency today               How fast can you be back up and running after your system goes down? Most importantly, how much is it going to cost you? Let's find out        Putting an end to your IT worries and dealing with your technology from A to Z. Bringing predictability to your IT budget with technology support that’s proactive and dependable. Investing in the future of your company with IT solutions that are built to last. Managed IT Services Cloud Computing Data Backup Solutions Disaster Recovery Planning Desktop Support Server Support Email/Spam Protection Network Security Website Design Virtualization HLB System Solutions  50 Malcolm RoadUnit 1Guelph, Ontario  N1K 1A9 Phone: 519-822-3450 Fax: 519-822-8861 About Us Services Support Center Contact Us Privacy Policy Website by Pronto Privacy Policy Website by Pronto Submit a Support RequestContact Us HLB System Solutions  50 Malcolm RoadUnit 1Guelph, Ontario Canada 519-822-3450 Get Directions Call Now to Speak to a Live Representative What should you do?  Enhance work efficiency today  Let's find out  With Managed Services from HLB System Solutions, you transfer the day-to-day management of your technology to us. Learn how your business can benefit. read more Protect all you've worked for, with Business Continuity Planning that ensures your company can weather any storm. read more Take your technology strategy to the next level with comprehensive, long-term IT Consulting from HLB System Solutions. read more Discover how Cloud Computing solutions can help you save money, increase productivity and simplify your business. read more Our true passion is playing a part in our clients’ success. We are only successful when our clients are successful! That is why our entire organization is built around aligning our goals with yours. As a small business owner myself, I share the same expectations from our own partners, as you would expect from an IT service company. I believe that great relationships are the foundations for great business, and trust can only be earned through action. That’s why at HLB, “We do what we say, we finish what we start, we show up on time and we say please and thank you." Lennart Berglund President, HLB System Solutions "HLB has filled all of our IT needs." HLB System Solutions has been servicing and supporting Ag Energy for almost a decade and most notably helped develop their CIS software application. When Ag Energy’s IT manager left the organization, it was suggested they consider utilizing HLB System Solutions managed services option rather than replacing their IT manager. After careful review and consideration, they opted to try the managed service program for a period of time until they could determine what their needs were. Rose Gage CEO, Ag Energy "They have been instrumental to our growth…" HLB has been a part of our team for many years now and truly understands our business. They have been instrumental to our growth and continue to provide innovative ideas on how to move us forward. We can comfortably focus on our business and let the friendly staff at HLB take care of our IT systems.  Manager of a local healthcare company "HLB help support our in-house IT personnel and also looks after all of our hardware needs..." We have been a client of HLBSS since early 2000. Currently they come in every morning to help support our in-house IT personnel and also look after all of our hardware needs. They also designed our website and our intranet site. I highly recommend them for either your sole IT support or as additional support to any in-house IT resources you may have.  RLB LLP, Chartered Accountants and Business Advisors !function ($) { $(function() {$("#partners-partners-certifications-slider").carousel()})}(window.jQuery)  ©2016 HLB System Solutions. All Rights Reserved. ©2016 HLB System Solutions. All Rights Reserved. We’re Hiring! Support Center Is This You? How We Work Services  Managed Services Business Continuity Planning Beyond Backup IT Consulting Security On Demand Services Office Moves Virtualization Email / Spam Protection Cloud Computing Web and Software Development 7 Things We Do Better Free Stuff  Newsletter Archive Our Clients About Us  Job Opportunities Our Team Partners &amp; Certifications Referral Program Contact Us Support Center Blog Submit a Support Request Contact Us 519-822-3450 Get Directions What should you do? Enhance work efficiency today Let's find out read more read more read more read more Read more testimonials About Us Services Support Center Contact Us Tweets by @HLBSolutions Privacy Policy Website by Pronto Privacy Policy Website by Pronto HLB System Solutions  50 Malcolm RoadUnit 1 Guelph Ontario  Canada for voting HLB as Best In Class! Most importantly, 519-822-3450! Managed IT Services Cloud Computing Data Backup Solutions Disaster Recovery Planning Desktop Support Server Support Email/Spam Protection Network Security Website Design Virtualization HLB System Solutions  50 Malcolm RoadUnit 1 Guelph Ontario  N1K 1A9 519-822-3450 519-822-8861</v>
-      </c>
-      <c r="F22" t="str">
-        <v>Computer Support, IT Consulting, Network Services - Guelph, Kitchener, Waterloo | HLB System Solutions HLB System Solutions specializes in IT Consulting, providing business Computer Support and Network Services in Guelph, Kitchener, Waterloo, Cambridge, Fergus and Arthur. “Are You Searching For An IT Support FirmBut You Don’t Know Who You Can Trust To Fix It Fast? Thank you Guelph for voting HLB as Best In Class! Office 365 Solution Industry leading collaboration suite – often copied never equalled How fast can you be back up and running after your system goes down? Most importantly, how much is it going to cost you? Why Choose HLB? Your One Stop Shop For All Your Technology Needs See what other business owners are saying about us... We're proud to partner with the best businesses in the industry. HLB System Solutions Microsoft Support has ended! Call Us Today At 519-822-3450! Managed Services Business Continuity Planning IT Consulting Cloud Computing Contact Info Navigation We’re Hiring! Support Center Is This You? How We Work Services Managed Services Business Continuity Planning Beyond Backup IT Consulting  Security On Demand Services Office Moves   Virtualization Email / Spam Protection Cloud Computing Web and Software Development  Managed Services Business Continuity Planning Beyond Backup IT Consulting  Security On Demand Services Office Moves   Security On Demand Services Office Moves Virtualization Email / Spam Protection Cloud Computing Web and Software Development 7 Things We Do Better Free Stuff   Newsletter Archive  Newsletter Archive Our Clients About Us   Job Opportunities Our Team Partners &amp; Certifications Referral Program Contact Us Support Center  Job Opportunities Our Team Partners &amp; Certifications Referral Program Contact Us Support Center Blog       “Are You Searching For An IT Support FirmBut You Don’t Know Who You Can Trust To Fix It Fast? Call Now to Speak to a Live Representative                  Microsoft Support has ended! What should you do?                    Thank you Guelph  for voting HLB as Best In Class!                 Office 365 Solution Industry leading collaboration suite – often copied never equalled Enhance work efficiency today               How fast can you be back up and running after your system goes down? Most importantly, how much is it going to cost you? Let's find out        Putting an end to your IT worries and dealing with your technology from A to Z. Bringing predictability to your IT budget with technology support that’s proactive and dependable. Investing in the future of your company with IT solutions that are built to last. Managed IT Services Cloud Computing Data Backup Solutions Disaster Recovery Planning Desktop Support Server Support Email/Spam Protection Network Security Website Design Virtualization HLB System Solutions  50 Malcolm RoadUnit 1Guelph, Ontario  N1K 1A9 Phone: 519-822-3450 Fax: 519-822-8861 About Us Services Support Center Contact Us Privacy Policy Website by Pronto Privacy Policy Website by Pronto Submit a Support RequestContact Us HLB System Solutions  50 Malcolm RoadUnit 1Guelph, Ontario Canada 519-822-3450 Get Directions Call Now to Speak to a Live Representative What should you do?  Enhance work efficiency today  Let's find out  With Managed Services from HLB System Solutions, you transfer the day-to-day management of your technology to us. Learn how your business can benefit. read more Protect all you've worked for, with Business Continuity Planning that ensures your company can weather any storm. read more Take your technology strategy to the next level with comprehensive, long-term IT Consulting from HLB System Solutions. read more Discover how Cloud Computing solutions can help you save money, increase productivity and simplify your business. read more Our true passion is playing a part in our clients’ success. We are only successful when our clients are successful! That is why our entire organization is built around aligning our goals with yours. As a small business owner myself, I share the same expectations from our own partners, as you would expect from an IT service company. I believe that great relationships are the foundations for great business, and trust can only be earned through action. That’s why at HLB, “We do what we say, we finish what we start, we show up on time and we say please and thank you." Lennart Berglund President, HLB System Solutions "HLB has filled all of our IT needs." HLB System Solutions has been servicing and supporting Ag Energy for almost a decade and most notably helped develop their CIS software application. When Ag Energy’s IT manager left the organization, it was suggested they consider utilizing HLB System Solutions managed services option rather than replacing their IT manager. After careful review and consideration, they opted to try the managed service program for a period of time until they could determine what their needs were. Rose Gage CEO, Ag Energy "They have been instrumental to our growth…" HLB has been a part of our team for many years now and truly understands our business. They have been instrumental to our growth and continue to provide innovative ideas on how to move us forward. We can comfortably focus on our business and let the friendly staff at HLB take care of our IT systems.  Manager of a local healthcare company "HLB help support our in-house IT personnel and also looks after all of our hardware needs..." We have been a client of HLBSS since early 2000. Currently they come in every morning to help support our in-house IT personnel and also look after all of our hardware needs. They also designed our website and our intranet site. I highly recommend them for either your sole IT support or as additional support to any in-house IT resources you may have.  RLB LLP, Chartered Accountants and Business Advisors !function ($) { $(function() {$("#partners-partners-certifications-slider").carousel()})}(window.jQuery)  ©2016 HLB System Solutions. All Rights Reserved. ©2016 HLB System Solutions. All Rights Reserved. We’re Hiring! Support Center Is This You? How We Work Services  Managed Services Business Continuity Planning Beyond Backup IT Consulting Security On Demand Services Office Moves Virtualization Email / Spam Protection Cloud Computing Web and Software Development 7 Things We Do Better Free Stuff  Newsletter Archive Our Clients About Us  Job Opportunities Our Team Partners &amp; Certifications Referral Program Contact Us Support Center Blog Submit a Support Request Contact Us 519-822-3450 Get Directions What should you do? Enhance work efficiency today Let's find out read more read more read more read more Read more testimonials About Us Services Support Center Contact Us Tweets by @HLBSolutions Privacy Policy Website by Pronto Privacy Policy Website by Pronto HLB System Solutions  50 Malcolm RoadUnit 1 Guelph Ontario  Canada for voting HLB as Best In Class! Most importantly, 519-822-3450! Managed IT Services Cloud Computing Data Backup Solutions Disaster Recovery Planning Desktop Support Server Support Email/Spam Protection Network Security Website Design Virtualization HLB System Solutions  50 Malcolm RoadUnit 1 Guelph Ontario  N1K 1A9 519-822-3450 519-822-8861</v>
+        <v>Computer Support IT Consulting Network Services Guelph Kitchener Waterloo HLB System Solutions HLB System Solutions specializes in IT Consulting providing business Computer Support and Network Services in Guelph Kitchener Waterloo Cambridge Fergus and Arthur “Are You Searching For An IT Support FirmBut You Don’t Know Who You Can Trust To Fix It Fast Thank you Guelph for voting HLB as Best In Class Office 365 Solution Industry leading collaboration suite often copied never equalled How fast can you be back up and running after your system goes down Most importantly how much is it going to cost you Why Choose HLB Your One Stop Shop For All Your Technology Needs See what other business owners are saying about us Were proud to partner with the best businesses in the industry HLB System Solutions Microsoft Support has ended Call Us Today At 5198223450 Managed Services Business Continuity Planning IT Consulting Cloud Computing Contact Info Navigation We’re Hiring Support Center Is This You How We Work Services Managed Services Business Continuity Planning Beyond Backup IT Consulting Security On Demand Services Office Moves Virtualization Email Spam Protection Cloud Computing Web and Software Development Managed Services Business Continuity Planning Beyond Backup IT Consulting Security On Demand Services Office Moves Security On Demand Services Office Moves Virtualization Email Spam Protection Cloud Computing Web and Software Development 7 Things We Do Better Free Stuff Newsletter Archive Newsletter Archive Our Clients About Us Job Opportunities Our Team Partners Certifications Referral Program Contact Us Support Center Job Opportunities Our Team Partners Certifications Referral Program Contact Us Support Center Blog “Are You Searching For An IT Support FirmBut You Don’t Know Who You Can Trust To Fix It Fast Call Now to Speak to a Live Representative Microsoft Support has ended What should you do Thank you Guelph for voting HLB as Best In Class Office 365 Solution Industry leading collaboration suite often copied never equalled Enhance work efficiency today How fast can you be back up and running after your system goes down Most importantly how much is it going to cost you Lets find out Putting an end to your IT worries and dealing with your technology from A to Z Bringing predictability to your IT budget with technology support that’s proactive and dependable Investing in the future of your company with IT solutions that are built to last Managed IT Services Cloud Computing Data Backup Solutions Disaster Recovery Planning Desktop Support Server Support EmailSpam Protection Network Security Website Design Virtualization HLB System Solutions 50 Malcolm RoadUnit 1Guelph Ontario N1K 1A9 Phone 5198223450 Fax 5198228861 About Us Services Support Center Contact Us Privacy Policy Website by Pronto Privacy Policy Website by Pronto Submit a Support RequestContact Us HLB System Solutions 50 Malcolm RoadUnit 1Guelph Ontario Canada 5198223450 Get Directions Call Now to Speak to a Live Representative What should you do Enhance work efficiency today Lets find out With Managed Services from HLB System Solutions you transfer the daytoday management of your technology to us Learn how your business can benefit read more Protect all youve worked for with Business Continuity Planning that ensures your company can weather any storm read more Take your technology strategy to the next level with comprehensive longterm IT Consulting from HLB System Solutions read more Discover how Cloud Computing solutions can help you save money increase productivity and simplify your business read more Our true passion is playing a part in our clients’ success We are only successful when our clients are successful That is why our entire organization is built around aligning our goals with yours As a small business owner myself I share the same expectations from our own partners as you would expect from an IT service company I believe that great relationships are the foundations for great business and trust can only be earned through action That’s why at HLB “We do what we say we finish what we start we show up on time and we say please and thank you Lennart Berglund President HLB System Solutions HLB has filled all of our IT needs HLB System Solutions has been servicing and supporting Ag Energy for almost a decade and most notably helped develop their CIS software application When Ag Energy’s IT manager left the organization it was suggested they consider utilizing HLB System Solutions managed services option rather than replacing their IT manager After careful review and consideration they opted to try the managed service program for a period of time until they could determine what their needs were Rose Gage CEO Ag Energy They have been instrumental to our growth… HLB has been a part of our team for many years now and truly understands our business They have been instrumental to our growth and continue to provide innovative ideas on how to move us forward We can comfortably focus on our business and let the friendly staff at HLB take care of our IT systems Manager of a local healthcare company HLB help support our inhouse IT personnel and also looks after all of our hardware needs We have been a client of HLBSS since early 2000 Currently they come in every morning to help support our inhouse IT personnel and also look after all of our hardware needs They also designed our website and our intranet site I highly recommend them for either your sole IT support or as additional support to any inhouse IT resources you may have RLB LLP Chartered Accountants and Business Advisors function function partnerspartnerscertificationsslidercarouselwindowjQuery ©2016 HLB System Solutions All Rights Reserved ©2016 HLB System Solutions All Rights Reserved We’re Hiring Support Center Is This You How We Work Services Managed Services Business Continuity Planning Beyond Backup IT Consulting Security On Demand Services Office Moves Virtualization Email Spam Protection Cloud Computing Web and Software Development 7 Things We Do Better Free Stuff Newsletter Archive Our Clients About Us Job Opportunities Our Team Partners Certifications Referral Program Contact Us Support Center Blog Submit a Support Request Contact Us 5198223450 Get Directions What should you do Enhance work efficiency today Lets find out read more read more read more read more Read more testimonials About Us Services Support Center Contact Us Tweets by HLBSolutions Privacy Policy Website by Pronto Privacy Policy Website by Pronto HLB System Solutions 50 Malcolm RoadUnit 1 Guelph Ontario Canada for voting HLB as Best In Class Most importantly 5198223450 Managed IT Services Cloud Computing Data Backup Solutions Disaster Recovery Planning Desktop Support Server Support EmailSpam Protection Network Security Website Design Virtualization HLB System Solutions 50 Malcolm RoadUnit 1 Guelph Ontario N1K 1A9 5198223450 5198228861</v>
       </c>
     </row>
     <row r="23">
@@ -813,16 +633,7 @@
         <v>IT and systems support</v>
       </c>
       <c r="C23" t="str">
-        <v>Homepage | Systems Support Corporation Not Ready To Call Us Just Yet? Feeling Like You’ve Outgrown Your Current IT Support Firm? 6 Reasons to Trust Systems Support Corporation to Support Your Computer Network Systems Support Corporation: trusted computer support for businesses throughout Eastern Massachusetts and Cape Cod – Let us help you today! See what other business owners are saying about us… Call Us Today At 781-837-0069 Our Services Download YourFree Copy Now Contact Latest Articles Hyatt Joins the Long List of Hacked Companies Windows 10 – The Most Successful OS Launch in Microsoft’s History Social Media Newsletter 1 2 3 4 5 6 Home Is This You? Services  Managed Services  Cloud Computing   Pure Cloud   Private Cloud   Custom Cloud     Network Solutions  E-Mail  Data Backup and Recovery  Mobile Device Management  Video Surveillance  VoIP Services  Website Services     Website Service Features      Managed Services Cloud Computing     Pure Cloud   Private Cloud   Custom Cloud    Pure Cloud Private Cloud Custom Cloud Network Solutions E-Mail Data Backup and Recovery Mobile Device Management Video Surveillance VoIP Services Website Services     Website Service Features    Website Service Features Why Choose Us? Our Clients Resources   Cloud Readiness Assessment  Cloud based email  Cloud Computing Guide for Construction  Backup and Disaster Recovery Plan  Whitepaper download : The 10 Disaster Planning Essentials For A Small Business Network  Free Network Health Check  Free BC/DR Assessment  Protect Your Network  Protect Your Identity  Blog   Cloud Readiness Assessment Cloud based email Cloud Computing Guide for Construction Backup and Disaster Recovery Plan Whitepaper download : The 10 Disaster Planning Essentials For A Small Business Network Free Network Health Check Free BC/DR Assessment Protect Your Network Protect Your Identity Blog About Us   Affiliations  Referral Program  Contact Us   Affiliations Referral Program Contact Us 781-837-0069 781-837-0069 Home Is This You? Services   Managed Services  Cloud Computing     Pure Cloud   Private Cloud   Custom Cloud     Network Solutions  E-Mail  Data Backup and Recovery  Mobile Device Management  Video Surveillance  VoIP Services  Website Services     Website Service Features      Managed Services Cloud Computing     Pure Cloud   Private Cloud   Custom Cloud    Pure Cloud Private Cloud Custom Cloud Network Solutions E-Mail Data Backup and Recovery Mobile Device Management Video Surveillance VoIP Services Website Services     Website Service Features    Website Service Features Why Choose Us? Our Clients Resources   Cloud Readiness Assessment  Cloud based email  Cloud Computing Guide for Construction  Backup and Disaster Recovery Plan  Whitepaper download : The 10 Disaster Planning Essentials For A Small Business Network  Free Network Health Check  Free BC/DR Assessment  Protect Your Network  Protect Your Identity  Blog   Cloud Readiness Assessment Cloud based email Cloud Computing Guide for Construction Backup and Disaster Recovery Plan Whitepaper download : The 10 Disaster Planning Essentials For A Small Business Network Free Network Health Check Free BC/DR Assessment Protect Your Network Protect Your Identity Blog About Us   Affiliations  Referral Program  Contact Us   Affiliations Referral Program Contact Us Download YourFree Copy Now Name* Email*                                                       Phone Company NameThis field is for validation purposes and should be left unchanged.  462 Plain Street Suite 206Marshfield, MA 02050 Phone: 781-837-0069 Phone: 781-837-0069 Email: info@systemsupport.com No Other IT Consulting Firm In Eastern Massachusetts And Cape Cod Can Touch Our Fast Response Time, Range Of Experience, Quality Customer Service, Or Our Ability To Deliver Technology Solutions That Work EXACTLY The Way You Want Them To. 1 One Stop Shop – We handle all aspects of your IT infrastructure including hardware and software management, vendor relationships for your internet connectivity, business software, phone systems, and any other related technology needs. We focus on your IT so you can focus on your business. 2 Reputable – We have been around since 1989, a respected leader in the community and the industry. Our proudest accomplishment is the large number of long term clients who year after year put their trust in us. 3 Proactive – Our service philosophy is proactive, not reactive. With state-of-the-art network monitoring and management, we manage your network 24/7 to identify issues and address them BEFORE they become problems, rather than putting out fires. 4 100% Satisfaction Guarantee – We want you to be completely satisfied with our services. We will do whatever it takes to make you happy. No hassles, no problems. 5 Quick response – Emergency response time is one hour or less guaranteed. A live person will answer your call. We can log in to your PC or server remotely and resolve many issues immediately without the wait for a technician to travel to your location. 6 Comprehensive project management – Our extensive experience managing all types of complex projects means we will handle every detail and coordinate all vendors so you can rest assured that your project will be completed on time and on budget.             We’ll manage all of your IT services for a flat-rate fee.             Our solutions are fully scalable and available for a flat-rate fee.             We deliver the innovative infrastructure solutions.             We provide a variety of email solutions to suit your needs. Maybe you’re concerned with the current rising costs of your IT services, or maybe you are just running short on time because of your expanding business and need to hand over the reins of some services to someone else. Whatever your reason, we can help you with quality IT services today. Your business can save money and time today with Systems Support Corporation’s managed services, network solutions, IT support and more. FIND OUT MORE We use SSC’s hosted cloud email and private cloud access and phone solutions for our remote sites. Now everybody gets all their information immediately and in one place. It’s like everybody’s in the office without being in the office. WOW! That is all I can say about SSC. It’s so nice to know that my entire network is handled so I can focus on business. I’ve worked with a number of other computer consultants in the past and no one can touch their level of service or expertise. Before hiring SSC, our network would go down frequently, run slow, and even run into the occasional virus. Since signing up on their network maintenance plan, we haven’t had one single issue. I’m VERY glad we hired these guys to support our network. Read More Testimonials If so, we would at least like to send you a copy of our recently published report, What Every Business Owner MUST Know To Protect Against Online Identity Theft. This informational booklet will outline in plain, non-technical English common mistakes that many small business owners make with their computer and network security that puts their personal information and identity at risk of being stolen. It will also further explain what identity theft is, and how you can prevent it from happening to you and your business. Simply fill out the form here and we’ll send you a copy today! January 23rd, 2016 January 22nd, 2016 Join our Newsletter to get the latest technology news and special offers. Home Is This You? Services Managed Services Cloud Computing Pure Cloud Private Cloud Custom Cloud Network Solutions E-Mail Data Backup and Recovery Mobile Device Management Video Surveillance VoIP Services Website Services Website Service Features Why Choose Us? Our Clients Resources Cloud Readiness Assessment Cloud based email Cloud Computing Guide for Construction Backup and Disaster Recovery Plan Whitepaper download : The 10 Disaster Planning Essentials For A Small Business Network Free Network Health Check Free BC/DR Assessment Protect Your Network Protect Your Identity Blog About Us Affiliations Referral Program Contact Us 781-837-0069 Home Is This You? Services Managed Services Cloud Computing Pure Cloud Private Cloud Custom Cloud Network Solutions E-Mail Data Backup and Recovery Mobile Device Management Video Surveillance VoIP Services Website Services Website Service Features Why Choose Us? Our Clients Resources Cloud Readiness Assessment Cloud based email Cloud Computing Guide for Construction Backup and Disaster Recovery Plan Whitepaper download : The 10 Disaster Planning Essentials For A Small Business Network Free Network Health Check Free BC/DR Assessment Protect Your Network Protect Your Identity Blog About Us Affiliations Referral Program Contact Us                                         FIND OUT MORE Read More Testimonials 781-837-0069 info@systemsupport.com Hyatt Joins the Long List of Hacked Companies Windows 10 – The Most Successful OS Launch in Microsoft’s History 781-837-0069 781-837-0069 No Other IT Consulting Firm In Eastern Massachusetts And Cape Cod Can Touch Our Fast Response Time, Range Of Experience, Quality Customer Service, Or Our Ability To Deliver Technology Solutions That Work EXACTLY The Way You Want Them To. 1 2 3 4 5 6                                 PresidentG&amp;R Construction Kennedy Carpets Morgan &amp; Morgan P.C. * * Systems Support Corporation Systems Support Corporation 462 Plain Street Suite 206 Marshfield MA 02050 781-837-0069 781-837-0069 info@systemsupport.com</v>
-      </c>
-      <c r="D23" t="str">
-        <v>Homepage | Systems Support Corporation Not Ready To Call Us Just Yet? Feeling Like You’ve Outgrown Your Current IT Support Firm? 6 Reasons to Trust Systems Support Corporation to Support Your Computer Network Systems Support Corporation: trusted computer support for businesses throughout Eastern Massachusetts and Cape Cod – Let us help you today! See what other business owners are saying about us… Call Us Today At 781-837-0069 Our Services Download YourFree Copy Now Contact Latest Articles Hyatt Joins the Long List of Hacked Companies Windows 10 – The Most Successful OS Launch in Microsoft’s History Social Media Newsletter 1 2 3 4 5 6 Home Is This You? Services  Managed Services  Cloud Computing   Pure Cloud   Private Cloud   Custom Cloud     Network Solutions  E-Mail  Data Backup and Recovery  Mobile Device Management  Video Surveillance  VoIP Services  Website Services     Website Service Features      Managed Services Cloud Computing     Pure Cloud   Private Cloud   Custom Cloud    Pure Cloud Private Cloud Custom Cloud Network Solutions E-Mail Data Backup and Recovery Mobile Device Management Video Surveillance VoIP Services Website Services     Website Service Features    Website Service Features Why Choose Us? Our Clients Resources   Cloud Readiness Assessment  Cloud based email  Cloud Computing Guide for Construction  Backup and Disaster Recovery Plan  Whitepaper download : The 10 Disaster Planning Essentials For A Small Business Network  Free Network Health Check  Free BC/DR Assessment  Protect Your Network  Protect Your Identity  Blog   Cloud Readiness Assessment Cloud based email Cloud Computing Guide for Construction Backup and Disaster Recovery Plan Whitepaper download : The 10 Disaster Planning Essentials For A Small Business Network Free Network Health Check Free BC/DR Assessment Protect Your Network Protect Your Identity Blog About Us   Affiliations  Referral Program  Contact Us   Affiliations Referral Program Contact Us 781-837-0069 781-837-0069 Home Is This You? Services   Managed Services  Cloud Computing     Pure Cloud   Private Cloud   Custom Cloud     Network Solutions  E-Mail  Data Backup and Recovery  Mobile Device Management  Video Surveillance  VoIP Services  Website Services     Website Service Features      Managed Services Cloud Computing     Pure Cloud   Private Cloud   Custom Cloud    Pure Cloud Private Cloud Custom Cloud Network Solutions E-Mail Data Backup and Recovery Mobile Device Management Video Surveillance VoIP Services Website Services     Website Service Features    Website Service Features Why Choose Us? Our Clients Resources   Cloud Readiness Assessment  Cloud based email  Cloud Computing Guide for Construction  Backup and Disaster Recovery Plan  Whitepaper download : The 10 Disaster Planning Essentials For A Small Business Network  Free Network Health Check  Free BC/DR Assessment  Protect Your Network  Protect Your Identity  Blog   Cloud Readiness Assessment Cloud based email Cloud Computing Guide for Construction Backup and Disaster Recovery Plan Whitepaper download : The 10 Disaster Planning Essentials For A Small Business Network Free Network Health Check Free BC/DR Assessment Protect Your Network Protect Your Identity Blog About Us   Affiliations  Referral Program  Contact Us   Affiliations Referral Program Contact Us Download YourFree Copy Now Name* Email*                                                       Phone Company NameThis field is for validation purposes and should be left unchanged.  462 Plain Street Suite 206Marshfield, MA 02050 Phone: 781-837-0069 Phone: 781-837-0069 Email: info@systemsupport.com No Other IT Consulting Firm In Eastern Massachusetts And Cape Cod Can Touch Our Fast Response Time, Range Of Experience, Quality Customer Service, Or Our Ability To Deliver Technology Solutions That Work EXACTLY The Way You Want Them To. 1 One Stop Shop – We handle all aspects of your IT infrastructure including hardware and software management, vendor relationships for your internet connectivity, business software, phone systems, and any other related technology needs. We focus on your IT so you can focus on your business. 2 Reputable – We have been around since 1989, a respected leader in the community and the industry. Our proudest accomplishment is the large number of long term clients who year after year put their trust in us. 3 Proactive – Our service philosophy is proactive, not reactive. With state-of-the-art network monitoring and management, we manage your network 24/7 to identify issues and address them BEFORE they become problems, rather than putting out fires. 4 100% Satisfaction Guarantee – We want you to be completely satisfied with our services. We will do whatever it takes to make you happy. No hassles, no problems. 5 Quick response – Emergency response time is one hour or less guaranteed. A live person will answer your call. We can log in to your PC or server remotely and resolve many issues immediately without the wait for a technician to travel to your location. 6 Comprehensive project management – Our extensive experience managing all types of complex projects means we will handle every detail and coordinate all vendors so you can rest assured that your project will be completed on time and on budget.             We’ll manage all of your IT services for a flat-rate fee.             Our solutions are fully scalable and available for a flat-rate fee.             We deliver the innovative infrastructure solutions.             We provide a variety of email solutions to suit your needs. Maybe you’re concerned with the current rising costs of your IT services, or maybe you are just running short on time because of your expanding business and need to hand over the reins of some services to someone else. Whatever your reason, we can help you with quality IT services today. Your business can save money and time today with Systems Support Corporation’s managed services, network solutions, IT support and more. FIND OUT MORE We use SSC’s hosted cloud email and private cloud access and phone solutions for our remote sites. Now everybody gets all their information immediately and in one place. It’s like everybody’s in the office without being in the office. WOW! That is all I can say about SSC. It’s so nice to know that my entire network is handled so I can focus on business. I’ve worked with a number of other computer consultants in the past and no one can touch their level of service or expertise. Before hiring SSC, our network would go down frequently, run slow, and even run into the occasional virus. Since signing up on their network maintenance plan, we haven’t had one single issue. I’m VERY glad we hired these guys to support our network. Read More Testimonials If so, we would at least like to send you a copy of our recently published report, What Every Business Owner MUST Know To Protect Against Online Identity Theft. This informational booklet will outline in plain, non-technical English common mistakes that many small business owners make with their computer and network security that puts their personal information and identity at risk of being stolen. It will also further explain what identity theft is, and how you can prevent it from happening to you and your business. Simply fill out the form here and we’ll send you a copy today! January 23rd, 2016 January 22nd, 2016 Join our Newsletter to get the latest technology news and special offers. Home Is This You? Services Managed Services Cloud Computing Pure Cloud Private Cloud Custom Cloud Network Solutions E-Mail Data Backup and Recovery Mobile Device Management Video Surveillance VoIP Services Website Services Website Service Features Why Choose Us? Our Clients Resources Cloud Readiness Assessment Cloud based email Cloud Computing Guide for Construction Backup and Disaster Recovery Plan Whitepaper download : The 10 Disaster Planning Essentials For A Small Business Network Free Network Health Check Free BC/DR Assessment Protect Your Network Protect Your Identity Blog About Us Affiliations Referral Program Contact Us 781-837-0069 Home Is This You? Services Managed Services Cloud Computing Pure Cloud Private Cloud Custom Cloud Network Solutions E-Mail Data Backup and Recovery Mobile Device Management Video Surveillance VoIP Services Website Services Website Service Features Why Choose Us? Our Clients Resources Cloud Readiness Assessment Cloud based email Cloud Computing Guide for Construction Backup and Disaster Recovery Plan Whitepaper download : The 10 Disaster Planning Essentials For A Small Business Network Free Network Health Check Free BC/DR Assessment Protect Your Network Protect Your Identity Blog About Us Affiliations Referral Program Contact Us                                         FIND OUT MORE Read More Testimonials 781-837-0069 info@systemsupport.com Hyatt Joins the Long List of Hacked Companies Windows 10 – The Most Successful OS Launch in Microsoft’s History 781-837-0069 781-837-0069 No Other IT Consulting Firm In Eastern Massachusetts And Cape Cod Can Touch Our Fast Response Time, Range Of Experience, Quality Customer Service, Or Our Ability To Deliver Technology Solutions That Work EXACTLY The Way You Want Them To. 1 2 3 4 5 6                                 PresidentG&amp;R Construction Kennedy Carpets Morgan &amp; Morgan P.C. * * Systems Support Corporation Systems Support Corporation 462 Plain Street Suite 206 Marshfield MA 02050 781-837-0069 781-837-0069 info@systemsupport.com</v>
-      </c>
-      <c r="E23" t="str">
-        <v>Homepage | Systems Support Corporation Not Ready To Call Us Just Yet? Feeling Like You’ve Outgrown Your Current IT Support Firm? 6 Reasons to Trust Systems Support Corporation to Support Your Computer Network Systems Support Corporation: trusted computer support for businesses throughout Eastern Massachusetts and Cape Cod – Let us help you today! See what other business owners are saying about us… Call Us Today At 781-837-0069 Our Services Download YourFree Copy Now Contact Latest Articles Hyatt Joins the Long List of Hacked Companies Windows 10 – The Most Successful OS Launch in Microsoft’s History Social Media Newsletter 1 2 3 4 5 6 Home Is This You? Services  Managed Services  Cloud Computing   Pure Cloud   Private Cloud   Custom Cloud     Network Solutions  E-Mail  Data Backup and Recovery  Mobile Device Management  Video Surveillance  VoIP Services  Website Services     Website Service Features      Managed Services Cloud Computing     Pure Cloud   Private Cloud   Custom Cloud    Pure Cloud Private Cloud Custom Cloud Network Solutions E-Mail Data Backup and Recovery Mobile Device Management Video Surveillance VoIP Services Website Services     Website Service Features    Website Service Features Why Choose Us? Our Clients Resources   Cloud Readiness Assessment  Cloud based email  Cloud Computing Guide for Construction  Backup and Disaster Recovery Plan  Whitepaper download : The 10 Disaster Planning Essentials For A Small Business Network  Free Network Health Check  Free BC/DR Assessment  Protect Your Network  Protect Your Identity  Blog   Cloud Readiness Assessment Cloud based email Cloud Computing Guide for Construction Backup and Disaster Recovery Plan Whitepaper download : The 10 Disaster Planning Essentials For A Small Business Network Free Network Health Check Free BC/DR Assessment Protect Your Network Protect Your Identity Blog About Us   Affiliations  Referral Program  Contact Us   Affiliations Referral Program Contact Us 781-837-0069 781-837-0069 Home Is This You? Services   Managed Services  Cloud Computing     Pure Cloud   Private Cloud   Custom Cloud     Network Solutions  E-Mail  Data Backup and Recovery  Mobile Device Management  Video Surveillance  VoIP Services  Website Services     Website Service Features      Managed Services Cloud Computing     Pure Cloud   Private Cloud   Custom Cloud    Pure Cloud Private Cloud Custom Cloud Network Solutions E-Mail Data Backup and Recovery Mobile Device Management Video Surveillance VoIP Services Website Services     Website Service Features    Website Service Features Why Choose Us? Our Clients Resources   Cloud Readiness Assessment  Cloud based email  Cloud Computing Guide for Construction  Backup and Disaster Recovery Plan  Whitepaper download : The 10 Disaster Planning Essentials For A Small Business Network  Free Network Health Check  Free BC/DR Assessment  Protect Your Network  Protect Your Identity  Blog   Cloud Readiness Assessment Cloud based email Cloud Computing Guide for Construction Backup and Disaster Recovery Plan Whitepaper download : The 10 Disaster Planning Essentials For A Small Business Network Free Network Health Check Free BC/DR Assessment Protect Your Network Protect Your Identity Blog About Us   Affiliations  Referral Program  Contact Us   Affiliations Referral Program Contact Us Download YourFree Copy Now Name* Email*                                                       Phone Company NameThis field is for validation purposes and should be left unchanged.  462 Plain Street Suite 206Marshfield, MA 02050 Phone: 781-837-0069 Phone: 781-837-0069 Email: info@systemsupport.com No Other IT Consulting Firm In Eastern Massachusetts And Cape Cod Can Touch Our Fast Response Time, Range Of Experience, Quality Customer Service, Or Our Ability To Deliver Technology Solutions That Work EXACTLY The Way You Want Them To. 1 One Stop Shop – We handle all aspects of your IT infrastructure including hardware and software management, vendor relationships for your internet connectivity, business software, phone systems, and any other related technology needs. We focus on your IT so you can focus on your business. 2 Reputable – We have been around since 1989, a respected leader in the community and the industry. Our proudest accomplishment is the large number of long term clients who year after year put their trust in us. 3 Proactive – Our service philosophy is proactive, not reactive. With state-of-the-art network monitoring and management, we manage your network 24/7 to identify issues and address them BEFORE they become problems, rather than putting out fires. 4 100% Satisfaction Guarantee – We want you to be completely satisfied with our services. We will do whatever it takes to make you happy. No hassles, no problems. 5 Quick response – Emergency response time is one hour or less guaranteed. A live person will answer your call. We can log in to your PC or server remotely and resolve many issues immediately without the wait for a technician to travel to your location. 6 Comprehensive project management – Our extensive experience managing all types of complex projects means we will handle every detail and coordinate all vendors so you can rest assured that your project will be completed on time and on budget.             We’ll manage all of your IT services for a flat-rate fee.             Our solutions are fully scalable and available for a flat-rate fee.             We deliver the innovative infrastructure solutions.             We provide a variety of email solutions to suit your needs. Maybe you’re concerned with the current rising costs of your IT services, or maybe you are just running short on time because of your expanding business and need to hand over the reins of some services to someone else. Whatever your reason, we can help you with quality IT services today. Your business can save money and time today with Systems Support Corporation’s managed services, network solutions, IT support and more. FIND OUT MORE We use SSC’s hosted cloud email and private cloud access and phone solutions for our remote sites. Now everybody gets all their information immediately and in one place. It’s like everybody’s in the office without being in the office. WOW! That is all I can say about SSC. It’s so nice to know that my entire network is handled so I can focus on business. I’ve worked with a number of other computer consultants in the past and no one can touch their level of service or expertise. Before hiring SSC, our network would go down frequently, run slow, and even run into the occasional virus. Since signing up on their network maintenance plan, we haven’t had one single issue. I’m VERY glad we hired these guys to support our network. Read More Testimonials If so, we would at least like to send you a copy of our recently published report, What Every Business Owner MUST Know To Protect Against Online Identity Theft. This informational booklet will outline in plain, non-technical English common mistakes that many small business owners make with their computer and network security that puts their personal information and identity at risk of being stolen. It will also further explain what identity theft is, and how you can prevent it from happening to you and your business. Simply fill out the form here and we’ll send you a copy today! January 23rd, 2016 January 22nd, 2016 Join our Newsletter to get the latest technology news and special offers. Home Is This You? Services Managed Services Cloud Computing Pure Cloud Private Cloud Custom Cloud Network Solutions E-Mail Data Backup and Recovery Mobile Device Management Video Surveillance VoIP Services Website Services Website Service Features Why Choose Us? Our Clients Resources Cloud Readiness Assessment Cloud based email Cloud Computing Guide for Construction Backup and Disaster Recovery Plan Whitepaper download : The 10 Disaster Planning Essentials For A Small Business Network Free Network Health Check Free BC/DR Assessment Protect Your Network Protect Your Identity Blog About Us Affiliations Referral Program Contact Us 781-837-0069 Home Is This You? Services Managed Services Cloud Computing Pure Cloud Private Cloud Custom Cloud Network Solutions E-Mail Data Backup and Recovery Mobile Device Management Video Surveillance VoIP Services Website Services Website Service Features Why Choose Us? Our Clients Resources Cloud Readiness Assessment Cloud based email Cloud Computing Guide for Construction Backup and Disaster Recovery Plan Whitepaper download : The 10 Disaster Planning Essentials For A Small Business Network Free Network Health Check Free BC/DR Assessment Protect Your Network Protect Your Identity Blog About Us Affiliations Referral Program Contact Us                                         FIND OUT MORE Read More Testimonials 781-837-0069 info@systemsupport.com Hyatt Joins the Long List of Hacked Companies Windows 10 – The Most Successful OS Launch in Microsoft’s History 781-837-0069 781-837-0069 No Other IT Consulting Firm In Eastern Massachusetts And Cape Cod Can Touch Our Fast Response Time, Range Of Experience, Quality Customer Service, Or Our Ability To Deliver Technology Solutions That Work EXACTLY The Way You Want Them To. 1 2 3 4 5 6                                 PresidentG&amp;R Construction Kennedy Carpets Morgan &amp; Morgan P.C. * * Systems Support Corporation Systems Support Corporation 462 Plain Street Suite 206 Marshfield MA 02050 781-837-0069 781-837-0069 info@systemsupport.com</v>
-      </c>
-      <c r="F23" t="str">
-        <v>Homepage | Systems Support Corporation Not Ready To Call Us Just Yet? Feeling Like You’ve Outgrown Your Current IT Support Firm? 6 Reasons to Trust Systems Support Corporation to Support Your Computer Network Systems Support Corporation: trusted computer support for businesses throughout Eastern Massachusetts and Cape Cod – Let us help you today! See what other business owners are saying about us… Call Us Today At 781-837-0069 Our Services Download YourFree Copy Now Contact Latest Articles Hyatt Joins the Long List of Hacked Companies Windows 10 – The Most Successful OS Launch in Microsoft’s History Social Media Newsletter 1 2 3 4 5 6 Home Is This You? Services  Managed Services  Cloud Computing   Pure Cloud   Private Cloud   Custom Cloud     Network Solutions  E-Mail  Data Backup and Recovery  Mobile Device Management  Video Surveillance  VoIP Services  Website Services     Website Service Features      Managed Services Cloud Computing     Pure Cloud   Private Cloud   Custom Cloud    Pure Cloud Private Cloud Custom Cloud Network Solutions E-Mail Data Backup and Recovery Mobile Device Management Video Surveillance VoIP Services Website Services     Website Service Features    Website Service Features Why Choose Us? Our Clients Resources   Cloud Readiness Assessment  Cloud based email  Cloud Computing Guide for Construction  Backup and Disaster Recovery Plan  Whitepaper download : The 10 Disaster Planning Essentials For A Small Business Network  Free Network Health Check  Free BC/DR Assessment  Protect Your Network  Protect Your Identity  Blog   Cloud Readiness Assessment Cloud based email Cloud Computing Guide for Construction Backup and Disaster Recovery Plan Whitepaper download : The 10 Disaster Planning Essentials For A Small Business Network Free Network Health Check Free BC/DR Assessment Protect Your Network Protect Your Identity Blog About Us   Affiliations  Referral Program  Contact Us   Affiliations Referral Program Contact Us 781-837-0069 781-837-0069 Home Is This You? Services   Managed Services  Cloud Computing     Pure Cloud   Private Cloud   Custom Cloud     Network Solutions  E-Mail  Data Backup and Recovery  Mobile Device Management  Video Surveillance  VoIP Services  Website Services     Website Service Features      Managed Services Cloud Computing     Pure Cloud   Private Cloud   Custom Cloud    Pure Cloud Private Cloud Custom Cloud Network Solutions E-Mail Data Backup and Recovery Mobile Device Management Video Surveillance VoIP Services Website Services     Website Service Features    Website Service Features Why Choose Us? Our Clients Resources   Cloud Readiness Assessment  Cloud based email  Cloud Computing Guide for Construction  Backup and Disaster Recovery Plan  Whitepaper download : The 10 Disaster Planning Essentials For A Small Business Network  Free Network Health Check  Free BC/DR Assessment  Protect Your Network  Protect Your Identity  Blog   Cloud Readiness Assessment Cloud based email Cloud Computing Guide for Construction Backup and Disaster Recovery Plan Whitepaper download : The 10 Disaster Planning Essentials For A Small Business Network Free Network Health Check Free BC/DR Assessment Protect Your Network Protect Your Identity Blog About Us   Affiliations  Referral Program  Contact Us   Affiliations Referral Program Contact Us Download YourFree Copy Now Name* Email*                                                       Phone Company NameThis field is for validation purposes and should be left unchanged.  462 Plain Street Suite 206Marshfield, MA 02050 Phone: 781-837-0069 Phone: 781-837-0069 Email: info@systemsupport.com No Other IT Consulting Firm In Eastern Massachusetts And Cape Cod Can Touch Our Fast Response Time, Range Of Experience, Quality Customer Service, Or Our Ability To Deliver Technology Solutions That Work EXACTLY The Way You Want Them To. 1 One Stop Shop – We handle all aspects of your IT infrastructure including hardware and software management, vendor relationships for your internet connectivity, business software, phone systems, and any other related technology needs. We focus on your IT so you can focus on your business. 2 Reputable – We have been around since 1989, a respected leader in the community and the industry. Our proudest accomplishment is the large number of long term clients who year after year put their trust in us. 3 Proactive – Our service philosophy is proactive, not reactive. With state-of-the-art network monitoring and management, we manage your network 24/7 to identify issues and address them BEFORE they become problems, rather than putting out fires. 4 100% Satisfaction Guarantee – We want you to be completely satisfied with our services. We will do whatever it takes to make you happy. No hassles, no problems. 5 Quick response – Emergency response time is one hour or less guaranteed. A live person will answer your call. We can log in to your PC or server remotely and resolve many issues immediately without the wait for a technician to travel to your location. 6 Comprehensive project management – Our extensive experience managing all types of complex projects means we will handle every detail and coordinate all vendors so you can rest assured that your project will be completed on time and on budget.             We’ll manage all of your IT services for a flat-rate fee.             Our solutions are fully scalable and available for a flat-rate fee.             We deliver the innovative infrastructure solutions.             We provide a variety of email solutions to suit your needs. Maybe you’re concerned with the current rising costs of your IT services, or maybe you are just running short on time because of your expanding business and need to hand over the reins of some services to someone else. Whatever your reason, we can help you with quality IT services today. Your business can save money and time today with Systems Support Corporation’s managed services, network solutions, IT support and more. FIND OUT MORE We use SSC’s hosted cloud email and private cloud access and phone solutions for our remote sites. Now everybody gets all their information immediately and in one place. It’s like everybody’s in the office without being in the office. WOW! That is all I can say about SSC. It’s so nice to know that my entire network is handled so I can focus on business. I’ve worked with a number of other computer consultants in the past and no one can touch their level of service or expertise. Before hiring SSC, our network would go down frequently, run slow, and even run into the occasional virus. Since signing up on their network maintenance plan, we haven’t had one single issue. I’m VERY glad we hired these guys to support our network. Read More Testimonials If so, we would at least like to send you a copy of our recently published report, What Every Business Owner MUST Know To Protect Against Online Identity Theft. This informational booklet will outline in plain, non-technical English common mistakes that many small business owners make with their computer and network security that puts their personal information and identity at risk of being stolen. It will also further explain what identity theft is, and how you can prevent it from happening to you and your business. Simply fill out the form here and we’ll send you a copy today! January 23rd, 2016 January 22nd, 2016 Join our Newsletter to get the latest technology news and special offers. Home Is This You? Services Managed Services Cloud Computing Pure Cloud Private Cloud Custom Cloud Network Solutions E-Mail Data Backup and Recovery Mobile Device Management Video Surveillance VoIP Services Website Services Website Service Features Why Choose Us? Our Clients Resources Cloud Readiness Assessment Cloud based email Cloud Computing Guide for Construction Backup and Disaster Recovery Plan Whitepaper download : The 10 Disaster Planning Essentials For A Small Business Network Free Network Health Check Free BC/DR Assessment Protect Your Network Protect Your Identity Blog About Us Affiliations Referral Program Contact Us 781-837-0069 Home Is This You? Services Managed Services Cloud Computing Pure Cloud Private Cloud Custom Cloud Network Solutions E-Mail Data Backup and Recovery Mobile Device Management Video Surveillance VoIP Services Website Services Website Service Features Why Choose Us? Our Clients Resources Cloud Readiness Assessment Cloud based email Cloud Computing Guide for Construction Backup and Disaster Recovery Plan Whitepaper download : The 10 Disaster Planning Essentials For A Small Business Network Free Network Health Check Free BC/DR Assessment Protect Your Network Protect Your Identity Blog About Us Affiliations Referral Program Contact Us                                         FIND OUT MORE Read More Testimonials 781-837-0069 info@systemsupport.com Hyatt Joins the Long List of Hacked Companies Windows 10 – The Most Successful OS Launch in Microsoft’s History 781-837-0069 781-837-0069 No Other IT Consulting Firm In Eastern Massachusetts And Cape Cod Can Touch Our Fast Response Time, Range Of Experience, Quality Customer Service, Or Our Ability To Deliver Technology Solutions That Work EXACTLY The Way You Want Them To. 1 2 3 4 5 6                                 PresidentG&amp;R Construction Kennedy Carpets Morgan &amp; Morgan P.C. * * Systems Support Corporation Systems Support Corporation 462 Plain Street Suite 206 Marshfield MA 02050 781-837-0069 781-837-0069 info@systemsupport.com</v>
+        <v>Homepage Systems Support Corporation Not Ready To Call Us Just Yet Feeling Like You’ve Outgrown Your Current IT Support Firm 6 Reasons to Trust Systems Support Corporation to Support Your Computer Network Systems Support Corporation trusted computer support for businesses throughout Eastern Massachusetts and Cape Cod Let us help you today See what other business owners are saying about us… Call Us Today At 7818370069 Our Services Download YourFree Copy Now Contact Latest Articles Hyatt Joins the Long List of Hacked Companies Windows 10 The Most Successful OS Launch in Microsoft’s History Social Media Newsletter 1 2 3 4 5 6 Home Is This You Services Managed Services Cloud Computing Pure Cloud Private Cloud Custom Cloud Network Solutions EMail Data Backup and Recovery Mobile Device Management Video Surveillance VoIP Services Website Services Website Service Features Managed Services Cloud Computing Pure Cloud Private Cloud Custom Cloud Pure Cloud Private Cloud Custom Cloud Network Solutions EMail Data Backup and Recovery Mobile Device Management Video Surveillance VoIP Services Website Services Website Service Features Website Service Features Why Choose Us Our Clients Resources Cloud Readiness Assessment Cloud based email Cloud Computing Guide for Construction Backup and Disaster Recovery Plan Whitepaper download The 10 Disaster Planning Essentials For A Small Business Network Free Network Health Check Free BCDR Assessment Protect Your Network Protect Your Identity Blog Cloud Readiness Assessment Cloud based email Cloud Computing Guide for Construction Backup and Disaster Recovery Plan Whitepaper download The 10 Disaster Planning Essentials For A Small Business Network Free Network Health Check Free BCDR Assessment Protect Your Network Protect Your Identity Blog About Us Affiliations Referral Program Contact Us Affiliations Referral Program Contact Us 7818370069 7818370069 Home Is This You Services Managed Services Cloud Computing Pure Cloud Private Cloud Custom Cloud Network Solutions EMail Data Backup and Recovery Mobile Device Management Video Surveillance VoIP Services Website Services Website Service Features Managed Services Cloud Computing Pure Cloud Private Cloud Custom Cloud Pure Cloud Private Cloud Custom Cloud Network Solutions EMail Data Backup and Recovery Mobile Device Management Video Surveillance VoIP Services Website Services Website Service Features Website Service Features Why Choose Us Our Clients Resources Cloud Readiness Assessment Cloud based email Cloud Computing Guide for Construction Backup and Disaster Recovery Plan Whitepaper download The 10 Disaster Planning Essentials For A Small Business Network Free Network Health Check Free BCDR Assessment Protect Your Network Protect Your Identity Blog Cloud Readiness Assessment Cloud based email Cloud Computing Guide for Construction Backup and Disaster Recovery Plan Whitepaper download The 10 Disaster Planning Essentials For A Small Business Network Free Network Health Check Free BCDR Assessment Protect Your Network Protect Your Identity Blog About Us Affiliations Referral Program Contact Us Affiliations Referral Program Contact Us Download YourFree Copy Now Name Email Phone Company CommentsThis field is for validation purposes and should be left unchanged 462 Plain Street Suite 206Marshfield MA 02050 Phone 7818370069 Phone 7818370069 Email infosystemsupportcom No Other IT Consulting Firm In Eastern Massachusetts And Cape Cod Can Touch Our Fast Response Time Range Of Experience Quality Customer Service Or Our Ability To Deliver Technology Solutions That Work EXACTLY The Way You Want Them To 1 One Stop Shop We handle all aspects of your IT infrastructure including hardware and software management vendor relationships for your internet connectivity business software phone systems and any other related technology needs We focus on your IT so you can focus on your business 2 Reputable We have been around since 1989 a respected leader in the community and the industry Our proudest accomplishment is the large number of long term clients who year after year put their trust in us 3 Proactive Our service philosophy is proactive not reactive With stateoftheart network monitoring and management we manage your network 247 to identify issues and address them BEFORE they become problems rather than putting out fires 4 100 Satisfaction Guarantee We want you to be completely satisfied with our services We will do whatever it takes to make you happy No hassles no problems 5 Quick response Emergency response time is one hour or less guaranteed A live person will answer your call We can log in to your PC or server remotely and resolve many issues immediately without the wait for a technician to travel to your location 6 Comprehensive project management Our extensive experience managing all types of complex projects means we will handle every detail and coordinate all vendors so you can rest assured that your project will be completed on time and on budget We’ll manage all of your IT services for a flatrate fee Our solutions are fully scalable and available for a flatrate fee We deliver the innovative infrastructure solutions We provide a variety of email solutions to suit your needs Maybe you’re concerned with the current rising costs of your IT services or maybe you are just running short on time because of your expanding business and need to hand over the reins of some services to someone else Whatever your reason we can help you with quality IT services today Your business can save money and time today with Systems Support Corporation’s managed services network solutions IT support and more FIND OUT MORE We use SSC’s hosted cloud email and private cloud access and phone solutions for our remote sites Now everybody gets all their information immediately and in one place It’s like everybody’s in the office without being in the office WOW That is all I can say about SSC It’s so nice to know that my entire network is handled so I can focus on business I’ve worked with a number of other computer consultants in the past and no one can touch their level of service or expertise Before hiring SSC our network would go down frequently run slow and even run into the occasional virus Since signing up on their network maintenance plan we haven’t had one single issue I’m VERY glad we hired these guys to support our network Read More Testimonials If so we would at least like to send you a copy of our recently published report What Every Business Owner MUST Know To Protect Against Online Identity Theft This informational booklet will outline in plain nontechnical English common mistakes that many small business owners make with their computer and network security that puts their personal information and identity at risk of being stolen It will also further explain what identity theft is and how you can prevent it from happening to you and your business Simply fill out the form here and we’ll send you a copy today January 23rd 2016 January 22nd 2016 Join our Newsletter to get the latest technology news and special offers Home Is This You Services Managed Services Cloud Computing Pure Cloud Private Cloud Custom Cloud Network Solutions EMail Data Backup and Recovery Mobile Device Management Video Surveillance VoIP Services Website Services Website Service Features Why Choose Us Our Clients Resources Cloud Readiness Assessment Cloud based email Cloud Computing Guide for Construction Backup and Disaster Recovery Plan Whitepaper download The 10 Disaster Planning Essentials For A Small Business Network Free Network Health Check Free BCDR Assessment Protect Your Network Protect Your Identity Blog About Us Affiliations Referral Program Contact Us 7818370069 Home Is This You Services Managed Services Cloud Computing Pure Cloud Private Cloud Custom Cloud Network Solutions EMail Data Backup and Recovery Mobile Device Management Video Surveillance VoIP Services Website Services Website Service Features Why Choose Us Our Clients Resources Cloud Readiness Assessment Cloud based email Cloud Computing Guide for Construction Backup and Disaster Recovery Plan Whitepaper download The 10 Disaster Planning Essentials For A Small Business Network Free Network Health Check Free BCDR Assessment Protect Your Network Protect Your Identity Blog About Us Affiliations Referral Program Contact Us FIND OUT MORE Read More Testimonials 7818370069 infosystemsupportcom Hyatt Joins the Long List of Hacked Companies Windows 10 The Most Successful OS Launch in Microsoft’s History 7818370069 7818370069 No Other IT Consulting Firm In Eastern Massachusetts And Cape Cod Can Touch Our Fast Response Time Range Of Experience Quality Customer Service Or Our Ability To Deliver Technology Solutions That Work EXACTLY The Way You Want Them To 1 2 3 4 5 6 PresidentGR Construction Kennedy Carpets Morgan Morgan PC Systems Support Corporation Systems Support Corporation 462 Plain Street Suite 206 Marshfield MA 02050 7818370069 7818370069 infosystemsupportcom</v>
       </c>
     </row>
     <row r="24">
@@ -833,16 +644,7 @@
         <v>IT and systems support</v>
       </c>
       <c r="C24" t="str">
-        <v>IT Services Canada – Montreal – Quebec – Ottawa - Maritimes Need a trusted technology partner for your business? Nashen offers complete IT consulting services and support to the Montreal, Quebec, Ottawa and Maritimes regions of Canada. IT Services Canada, IT services Montreal, IT services Quebec, IT services Ottawa, IT services Maritimes IT Services Customized technology for all business needs Our Value Proposition News room World’s Most Innovative Companies Listen Solve Integrate Published March 26 2013 Français | Support | Portal Home Corporate profile Solutions Services Partners News Room Contact us                    Listen, Solve, Integrate. ››                           Collaborate and innovate. ››                           A better way of doing business. ››                           Mobility and peace of mind.  ››          Site map Terms of use Portal Our mission is to help you achieve your business objectives in the most effective manner. We start by listening to you until we fully comprehend the challenges you face and the goals you seek. We understand that one size does not fit all – especially when it comes to IT services. Nashen’s experienced  consultants partner with you to implement the optimum solutions to address your most critical  business issues. With nearly 30 years experience, we can deliver the most efficient, lowest-risk IT services and solutions. Nashen doesn’t just implement solutions. We encourage companies to improve business processes to maximize efficiencies and promote growth and competitiveness. In many cases, the best way to do this is by integrating new technologies into existing workflows. Nashen serves the Montreal and Quebec regions of Canada. VMware has been identified in the field of Computing as one of 2013’s 50 Disruptive Companies, MIT Technology Review’s annual list of the world’s most innovative technology companies. The honorees are nominated by MIT Technology Review’s editors, who look for companies that have demonstrated original and valuable technology over the last year, are bringing that [...]        Virtualization e-book       “Getting More From Less”              Virtualization white paper       “The Virtualization Journey”       Nashen Technologies  3400, Jean-Talon West, Suite 203 Montreal, Quebec H3R 2E8   Phone: 514-345-8826 Toll-free: 1-877-545-8826   solutions@nashen.com  © 2016 All rights reserved Nashen + Nashen Consultants Inc.    Français Support Portal Home Corporate profile Solutions Services Partners News Room Contact us                  Listen, Solve, Integrate. ››                  Collaborate and innovate. ››                  A better way of doing business. ››                  Mobility and peace of mind.  ››      World’s Most Innovative Companies Read more + Read all news + Download now Download now Site map Terms of use Portal solutions@nashen.com Listen, Solve, Integrate. ›› Collaborate and innovate. ›› A better way of doing business. ›› Mobility and peace of mind.  ›› Read more + Read all news + Virtualization e-book “Getting More From Less” Download now Virtualization white paper “The Virtualization Journey” Download now</v>
-      </c>
-      <c r="D24" t="str">
-        <v>IT Services Canada – Montreal – Quebec – Ottawa - Maritimes Need a trusted technology partner for your business? Nashen offers complete IT consulting services and support to the Montreal, Quebec, Ottawa and Maritimes regions of Canada. IT Services Canada, IT services Montreal, IT services Quebec, IT services Ottawa, IT services Maritimes IT Services Customized technology for all business needs Our Value Proposition News room World’s Most Innovative Companies Listen Solve Integrate Published March 26 2013 Français | Support | Portal Home Corporate profile Solutions Services Partners News Room Contact us                    Listen, Solve, Integrate. ››                           Collaborate and innovate. ››                           A better way of doing business. ››                           Mobility and peace of mind.  ››          Site map Terms of use Portal Our mission is to help you achieve your business objectives in the most effective manner. We start by listening to you until we fully comprehend the challenges you face and the goals you seek. We understand that one size does not fit all – especially when it comes to IT services. Nashen’s experienced  consultants partner with you to implement the optimum solutions to address your most critical  business issues. With nearly 30 years experience, we can deliver the most efficient, lowest-risk IT services and solutions. Nashen doesn’t just implement solutions. We encourage companies to improve business processes to maximize efficiencies and promote growth and competitiveness. In many cases, the best way to do this is by integrating new technologies into existing workflows. Nashen serves the Montreal and Quebec regions of Canada. VMware has been identified in the field of Computing as one of 2013’s 50 Disruptive Companies, MIT Technology Review’s annual list of the world’s most innovative technology companies. The honorees are nominated by MIT Technology Review’s editors, who look for companies that have demonstrated original and valuable technology over the last year, are bringing that [...]        Virtualization e-book       “Getting More From Less”              Virtualization white paper       “The Virtualization Journey”       Nashen Technologies  3400, Jean-Talon West, Suite 203 Montreal, Quebec H3R 2E8   Phone: 514-345-8826 Toll-free: 1-877-545-8826   solutions@nashen.com  © 2016 All rights reserved Nashen + Nashen Consultants Inc.    Français Support Portal Home Corporate profile Solutions Services Partners News Room Contact us                  Listen, Solve, Integrate. ››                  Collaborate and innovate. ››                  A better way of doing business. ››                  Mobility and peace of mind.  ››      World’s Most Innovative Companies Read more + Read all news + Download now Download now Site map Terms of use Portal solutions@nashen.com Listen, Solve, Integrate. ›› Collaborate and innovate. ›› A better way of doing business. ›› Mobility and peace of mind.  ›› Read more + Read all news + Virtualization e-book “Getting More From Less” Download now Virtualization white paper “The Virtualization Journey” Download now</v>
-      </c>
-      <c r="E24" t="str">
-        <v>IT Services Canada – Montreal – Quebec – Ottawa - Maritimes Need a trusted technology partner for your business? Nashen offers complete IT consulting services and support to the Montreal, Quebec, Ottawa and Maritimes regions of Canada. IT Services Canada, IT services Montreal, IT services Quebec, IT services Ottawa, IT services Maritimes IT Services Customized technology for all business needs Our Value Proposition News room World’s Most Innovative Companies Listen Solve Integrate Published March 26 2013 Français | Support | Portal Home Corporate profile Solutions Services Partners News Room Contact us                    Listen, Solve, Integrate. ››                           Collaborate and innovate. ››                           A better way of doing business. ››                           Mobility and peace of mind.  ››          Site map Terms of use Portal Our mission is to help you achieve your business objectives in the most effective manner. We start by listening to you until we fully comprehend the challenges you face and the goals you seek. We understand that one size does not fit all – especially when it comes to IT services. Nashen’s experienced  consultants partner with you to implement the optimum solutions to address your most critical  business issues. With nearly 30 years experience, we can deliver the most efficient, lowest-risk IT services and solutions. Nashen doesn’t just implement solutions. We encourage companies to improve business processes to maximize efficiencies and promote growth and competitiveness. In many cases, the best way to do this is by integrating new technologies into existing workflows. Nashen serves the Montreal and Quebec regions of Canada. VMware has been identified in the field of Computing as one of 2013’s 50 Disruptive Companies, MIT Technology Review’s annual list of the world’s most innovative technology companies. The honorees are nominated by MIT Technology Review’s editors, who look for companies that have demonstrated original and valuable technology over the last year, are bringing that [...]        Virtualization e-book       “Getting More From Less”              Virtualization white paper       “The Virtualization Journey”       Nashen Technologies  3400, Jean-Talon West, Suite 203 Montreal, Quebec H3R 2E8   Phone: 514-345-8826 Toll-free: 1-877-545-8826   solutions@nashen.com  © 2016 All rights reserved Nashen + Nashen Consultants Inc.    Français Support Portal Home Corporate profile Solutions Services Partners News Room Contact us                  Listen, Solve, Integrate. ››                  Collaborate and innovate. ››                  A better way of doing business. ››                  Mobility and peace of mind.  ››      World’s Most Innovative Companies Read more + Read all news + Download now Download now Site map Terms of use Portal solutions@nashen.com Listen, Solve, Integrate. ›› Collaborate and innovate. ›› A better way of doing business. ›› Mobility and peace of mind.  ›› Read more + Read all news + Virtualization e-book “Getting More From Less” Download now Virtualization white paper “The Virtualization Journey” Download now</v>
-      </c>
-      <c r="F24" t="str">
-        <v>IT Services Canada – Montreal – Quebec – Ottawa - Maritimes Need a trusted technology partner for your business? Nashen offers complete IT consulting services and support to the Montreal, Quebec, Ottawa and Maritimes regions of Canada. IT Services Canada, IT services Montreal, IT services Quebec, IT services Ottawa, IT services Maritimes IT Services Customized technology for all business needs Our Value Proposition News room World’s Most Innovative Companies Listen Solve Integrate Published March 26 2013 Français | Support | Portal Home Corporate profile Solutions Services Partners News Room Contact us                    Listen, Solve, Integrate. ››                           Collaborate and innovate. ››                           A better way of doing business. ››                           Mobility and peace of mind.  ››          Site map Terms of use Portal Our mission is to help you achieve your business objectives in the most effective manner. We start by listening to you until we fully comprehend the challenges you face and the goals you seek. We understand that one size does not fit all – especially when it comes to IT services. Nashen’s experienced  consultants partner with you to implement the optimum solutions to address your most critical  business issues. With nearly 30 years experience, we can deliver the most efficient, lowest-risk IT services and solutions. Nashen doesn’t just implement solutions. We encourage companies to improve business processes to maximize efficiencies and promote growth and competitiveness. In many cases, the best way to do this is by integrating new technologies into existing workflows. Nashen serves the Montreal and Quebec regions of Canada. VMware has been identified in the field of Computing as one of 2013’s 50 Disruptive Companies, MIT Technology Review’s annual list of the world’s most innovative technology companies. The honorees are nominated by MIT Technology Review’s editors, who look for companies that have demonstrated original and valuable technology over the last year, are bringing that [...]        Virtualization e-book       “Getting More From Less”              Virtualization white paper       “The Virtualization Journey”       Nashen Technologies  3400, Jean-Talon West, Suite 203 Montreal, Quebec H3R 2E8   Phone: 514-345-8826 Toll-free: 1-877-545-8826   solutions@nashen.com  © 2016 All rights reserved Nashen + Nashen Consultants Inc.    Français Support Portal Home Corporate profile Solutions Services Partners News Room Contact us                  Listen, Solve, Integrate. ››                  Collaborate and innovate. ››                  A better way of doing business. ››                  Mobility and peace of mind.  ››      World’s Most Innovative Companies Read more + Read all news + Download now Download now Site map Terms of use Portal solutions@nashen.com Listen, Solve, Integrate. ›› Collaborate and innovate. ›› A better way of doing business. ›› Mobility and peace of mind.  ›› Read more + Read all news + Virtualization e-book “Getting More From Less” Download now Virtualization white paper “The Virtualization Journey” Download now</v>
+        <v>IT Services Canada Montreal Quebec Ottawa Maritimes Need a trusted technology partner for your business Nashen offers complete IT consulting services and support to the Montreal Quebec Ottawa and Maritimes regions of Canada IT Services Canada IT services Montreal IT services Quebec IT services Ottawa IT services Maritimes IT Services Customized technology for all business needs Our Value Proposition News room World’s Most Innovative Companies Listen Solve Integrate Published March 26 2013 Français Support Portal Home Corporate profile Solutions Services Partners News Room Contact us Listen Solve Integrate ›› Collaborate and innovate ›› A better way of doing business ›› Mobility and peace of mind ›› Site map Terms of use Portal Our mission is to help you achieve your business objectives in the most effective manner We start by listening to you until we fully comprehend the challenges you face and the goals you seek We understand that one size does not fit all especially when it comes to IT services Nashen’s experienced consultants partner with you to implement the optimum solutions to address your most critical business issues With nearly 30 years experience we can deliver the most efficient lowestrisk IT services and solutions Nashen doesn’t just implement solutions We encourage companies to improve business processes to maximize efficiencies and promote growth and competitiveness In many cases the best way to do this is by integrating new technologies into existing workflows Nashen serves the Montreal and Quebec regions of Canada VMware has been identified in the field of Computing as one of 2013’s 50 Disruptive Companies MIT Technology Review’s annual list of the world’s most innovative technology companies The honorees are nominated by MIT Technology Review’s editors who look for companies that have demonstrated original and valuable technology over the last year are bringing that Virtualization ebook “Getting More From Less” Virtualization white paper “The Virtualization Journey” Nashen Technologies 3400 JeanTalon West Suite 203 Montreal Quebec H3R 2E8 Phone 5143458826 Tollfree 18775458826 solutionsnashencom © 2016 All rights reserved Nashen Nashen Consultants Inc Français Support Portal Home Corporate profile Solutions Services Partners News Room Contact us Listen Solve Integrate ›› Collaborate and innovate ›› A better way of doing business ›› Mobility and peace of mind ›› World’s Most Innovative Companies Read more Read all news Download now Download now Site map Terms of use Portal solutionsnashencom Listen Solve Integrate ›› Collaborate and innovate ›› A better way of doing business ›› Mobility and peace of mind ›› Read more Read all news Virtualization ebook “Getting More From Less” Download now Virtualization white paper “The Virtualization Journey” Download now</v>
       </c>
     </row>
     <row r="25">
@@ -853,16 +655,7 @@
         <v>IT and systems support</v>
       </c>
       <c r="C25" t="str">
-        <v>Vancouver IT Company | (604) 986-8170 | IT Managed Services Looking for the best Vancouver IT Support available? Call Compunet right now at (604) 986-8170. Top Vancouver IT Services. Vancouver IT Services and Consulting Backup Solutions Managed IT Cloud Solutions VoIP Systems Do You Think Dependable IT Support In Vancouver, Burnaby And Richmond Is Impossible To Find? What Our Clients Are Saying Yes! Sign Me Up For A Free 90 Minute Consultation Free Home About Us Why Choose Us?  How We Work  Is This You?  Testimonials   Why Choose Us? How We Work Is This You? Testimonials IT Solutions   Consulting Services  Disaster Avoidance Planning  Information Security  Cloud Services  Hosted Solutions  Business Telephones  Virtualization Services  Email Security Solutions   Consulting Services Disaster Avoidance Planning Information Security Cloud Services Hosted Solutions Business Telephones Virtualization Services Email Security Solutions Our Clients   Law Firms  Accounting Firms  Mining &amp; Exploration  Manufacturing  Engineering/Architectural   Law Firms Accounting Firms Mining &amp; Exploration Manufacturing Engineering/Architectural Our Blog Contact Us Vancouver IT Support Law Firm IT Services Accounting IT Support IT Services Mining Site Map We’ll contact you within 15 minutes guaranteed!100% Free! NO obligation. NO commitment. Don’t let a disaster put you out of business Cost-Effective IT Management and Network Maintenance Simplifying your transition to the cloud Telephony systems designed with your business in mind Compunet InfoTech is the company you can trust for all your IT Solutions. “Can’t I get one simple solution for Computer Support from one single company?” Ever wondered about this? We’re always there for you, with Managed Services to make running your business in Vancouver, Burnaby and Richmond worry-free. “Compunet is very focused on what they do best. Their cloud solutions allow us to offer services that we would not be able to provide to our clients. I wouldn’t hesitate to recommend Compunet to any business that needs IT Services”. Home About Us Why Choose Us? How We Work Is This You? Testimonials IT Solutions Consulting Services Disaster Avoidance Planning Information Security Cloud Services Hosted Solutions Business Telephones Virtualization Services Email Security Solutions Our Clients Law Firms Accounting Firms Mining &amp; Exploration Manufacturing Engineering/Architectural Our Blog Contact Us Click For Details Backup Solutions Managed IT Cloud Solutions VoIP Systems Vancouver IT Support Law Firm IT Services Accounting IT Support IT Services Mining Site Map "MSP Marketing" Website analytics software (604) 986-_8170 _ Click For Details — Merv Richter (604) 986-_8170 _ 888-378-_5507 _</v>
-      </c>
-      <c r="D25" t="str">
-        <v>Vancouver IT Company | (604) 986-8170 | IT Managed Services Looking for the best Vancouver IT Support available? Call Compunet right now at (604) 986-8170. Top Vancouver IT Services. Vancouver IT Services and Consulting Backup Solutions Managed IT Cloud Solutions VoIP Systems Do You Think Dependable IT Support In Vancouver, Burnaby And Richmond Is Impossible To Find? What Our Clients Are Saying Yes! Sign Me Up For A Free 90 Minute Consultation Free Home About Us Why Choose Us?  How We Work  Is This You?  Testimonials   Why Choose Us? How We Work Is This You? Testimonials IT Solutions   Consulting Services  Disaster Avoidance Planning  Information Security  Cloud Services  Hosted Solutions  Business Telephones  Virtualization Services  Email Security Solutions   Consulting Services Disaster Avoidance Planning Information Security Cloud Services Hosted Solutions Business Telephones Virtualization Services Email Security Solutions Our Clients   Law Firms  Accounting Firms  Mining &amp; Exploration  Manufacturing  Engineering/Architectural   Law Firms Accounting Firms Mining &amp; Exploration Manufacturing Engineering/Architectural Our Blog Contact Us Vancouver IT Support Law Firm IT Services Accounting IT Support IT Services Mining Site Map We’ll contact you within 15 minutes guaranteed!100% Free! NO obligation. NO commitment. Don’t let a disaster put you out of business Cost-Effective IT Management and Network Maintenance Simplifying your transition to the cloud Telephony systems designed with your business in mind Compunet InfoTech is the company you can trust for all your IT Solutions. “Can’t I get one simple solution for Computer Support from one single company?” Ever wondered about this? We’re always there for you, with Managed Services to make running your business in Vancouver, Burnaby and Richmond worry-free. “Compunet is very focused on what they do best. Their cloud solutions allow us to offer services that we would not be able to provide to our clients. I wouldn’t hesitate to recommend Compunet to any business that needs IT Services”. Home About Us Why Choose Us? How We Work Is This You? Testimonials IT Solutions Consulting Services Disaster Avoidance Planning Information Security Cloud Services Hosted Solutions Business Telephones Virtualization Services Email Security Solutions Our Clients Law Firms Accounting Firms Mining &amp; Exploration Manufacturing Engineering/Architectural Our Blog Contact Us Click For Details Backup Solutions Managed IT Cloud Solutions VoIP Systems Vancouver IT Support Law Firm IT Services Accounting IT Support IT Services Mining Site Map "MSP Marketing" Website analytics software (604) 986-_8170 _ Click For Details — Merv Richter (604) 986-_8170 _ 888-378-_5507 _</v>
-      </c>
-      <c r="E25" t="str">
-        <v>Vancouver IT Company | (604) 986-8170 | IT Managed Services Looking for the best Vancouver IT Support available? Call Compunet right now at (604) 986-8170. Top Vancouver IT Services. Vancouver IT Services and Consulting Backup Solutions Managed IT Cloud Solutions VoIP Systems Do You Think Dependable IT Support In Vancouver, Burnaby And Richmond Is Impossible To Find? What Our Clients Are Saying Yes! Sign Me Up For A Free 90 Minute Consultation Free Home About Us Why Choose Us?  How We Work  Is This You?  Testimonials   Why Choose Us? How We Work Is This You? Testimonials IT Solutions   Consulting Services  Disaster Avoidance Planning  Information Security  Cloud Services  Hosted Solutions  Business Telephones  Virtualization Services  Email Security Solutions   Consulting Services Disaster Avoidance Planning Information Security Cloud Services Hosted Solutions Business Telephones Virtualization Services Email Security Solutions Our Clients   Law Firms  Accounting Firms  Mining &amp; Exploration  Manufacturing  Engineering/Architectural   Law Firms Accounting Firms Mining &amp; Exploration Manufacturing Engineering/Architectural Our Blog Contact Us Vancouver IT Support Law Firm IT Services Accounting IT Support IT Services Mining Site Map We’ll contact you within 15 minutes guaranteed!100% Free! NO obligation. NO commitment. Don’t let a disaster put you out of business Cost-Effective IT Management and Network Maintenance Simplifying your transition to the cloud Telephony systems designed with your business in mind Compunet InfoTech is the company you can trust for all your IT Solutions. “Can’t I get one simple solution for Computer Support from one single company?” Ever wondered about this? We’re always there for you, with Managed Services to make running your business in Vancouver, Burnaby and Richmond worry-free. “Compunet is very focused on what they do best. Their cloud solutions allow us to offer services that we would not be able to provide to our clients. I wouldn’t hesitate to recommend Compunet to any business that needs IT Services”. Home About Us Why Choose Us? How We Work Is This You? Testimonials IT Solutions Consulting Services Disaster Avoidance Planning Information Security Cloud Services Hosted Solutions Business Telephones Virtualization Services Email Security Solutions Our Clients Law Firms Accounting Firms Mining &amp; Exploration Manufacturing Engineering/Architectural Our Blog Contact Us Click For Details Backup Solutions Managed IT Cloud Solutions VoIP Systems Vancouver IT Support Law Firm IT Services Accounting IT Support IT Services Mining Site Map "MSP Marketing" Website analytics software (604) 986-_8170 _ Click For Details — Merv Richter (604) 986-_8170 _ 888-378-_5507 _</v>
-      </c>
-      <c r="F25" t="str">
-        <v>Vancouver IT Company | (604) 986-8170 | IT Managed Services Looking for the best Vancouver IT Support available? Call Compunet right now at (604) 986-8170. Top Vancouver IT Services. Vancouver IT Services and Consulting Backup Solutions Managed IT Cloud Solutions VoIP Systems Do You Think Dependable IT Support In Vancouver, Burnaby And Richmond Is Impossible To Find? What Our Clients Are Saying Yes! Sign Me Up For A Free 90 Minute Consultation Free Home About Us Why Choose Us?  How We Work  Is This You?  Testimonials   Why Choose Us? How We Work Is This You? Testimonials IT Solutions   Consulting Services  Disaster Avoidance Planning  Information Security  Cloud Services  Hosted Solutions  Business Telephones  Virtualization Services  Email Security Solutions   Consulting Services Disaster Avoidance Planning Information Security Cloud Services Hosted Solutions Business Telephones Virtualization Services Email Security Solutions Our Clients   Law Firms  Accounting Firms  Mining &amp; Exploration  Manufacturing  Engineering/Architectural   Law Firms Accounting Firms Mining &amp; Exploration Manufacturing Engineering/Architectural Our Blog Contact Us Vancouver IT Support Law Firm IT Services Accounting IT Support IT Services Mining Site Map We’ll contact you within 15 minutes guaranteed!100% Free! NO obligation. NO commitment. Don’t let a disaster put you out of business Cost-Effective IT Management and Network Maintenance Simplifying your transition to the cloud Telephony systems designed with your business in mind Compunet InfoTech is the company you can trust for all your IT Solutions. “Can’t I get one simple solution for Computer Support from one single company?” Ever wondered about this? We’re always there for you, with Managed Services to make running your business in Vancouver, Burnaby and Richmond worry-free. “Compunet is very focused on what they do best. Their cloud solutions allow us to offer services that we would not be able to provide to our clients. I wouldn’t hesitate to recommend Compunet to any business that needs IT Services”. Home About Us Why Choose Us? How We Work Is This You? Testimonials IT Solutions Consulting Services Disaster Avoidance Planning Information Security Cloud Services Hosted Solutions Business Telephones Virtualization Services Email Security Solutions Our Clients Law Firms Accounting Firms Mining &amp; Exploration Manufacturing Engineering/Architectural Our Blog Contact Us Click For Details Backup Solutions Managed IT Cloud Solutions VoIP Systems Vancouver IT Support Law Firm IT Services Accounting IT Support IT Services Mining Site Map "MSP Marketing" Website analytics software (604) 986-_8170 _ Click For Details — Merv Richter (604) 986-_8170 _ 888-378-_5507 _</v>
+        <v>Vancouver IT Company 604 9868170 IT Managed Services Looking for the best Vancouver IT Support available Call Compunet right now at 604 9868170 Top Vancouver IT Services Vancouver IT Services and Consulting Backup Solutions Managed IT Cloud Solutions VoIP Systems Do You Think Dependable IT Support In Vancouver Burnaby And Richmond Is Impossible To Find What Our Clients Are Saying Yes Sign Me Up For A Free 90 Minute Consultation Free Home About Us Why Choose Us How We Work Is This You Testimonials Why Choose Us How We Work Is This You Testimonials IT Solutions Consulting Services Disaster Avoidance Planning Information Security Cloud Services Hosted Solutions Business Telephones Virtualization Services Email Security Solutions Consulting Services Disaster Avoidance Planning Information Security Cloud Services Hosted Solutions Business Telephones Virtualization Services Email Security Solutions Our Clients Law Firms Accounting Firms Mining Exploration Manufacturing EngineeringArchitectural Law Firms Accounting Firms Mining Exploration Manufacturing EngineeringArchitectural Our Blog Contact Us Vancouver IT Support Law Firm IT Services Accounting IT Support IT Services Mining Site Map We’ll contact you within 15 minutes guaranteed100 Free NO obligation NO commitment Don’t let a disaster put you out of business CostEffective IT Management and Network Maintenance Simplifying your transition to the cloud Telephony systems designed with your business in mind Compunet InfoTech is the company you can trust for all your IT Solutions “Can’t I get one simple solution for Computer Support from one single company” Ever wondered about this We’re always there for you with Managed Services to make running your business in Vancouver Burnaby and Richmond worryfree “We can count on them for reliability and security They are 100 reliable they provide 247 service and the eliminate worry We depend on their reliability to fix our problems and make things operate smoothly We are happy we don’t have any bad experiences and count on them as they are our lifeblood100 accessibility” Home About Us Why Choose Us How We Work Is This You Testimonials IT Solutions Consulting Services Disaster Avoidance Planning Information Security Cloud Services Hosted Solutions Business Telephones Virtualization Services Email Security Solutions Our Clients Law Firms Accounting Firms Mining Exploration Manufacturing EngineeringArchitectural Our Blog Contact Us Click For Details Backup Solutions Managed IT Cloud Solutions VoIP Systems Vancouver IT Support Law Firm IT Services Accounting IT Support IT Services Mining Site Map MSP Marketing website statistics 604 9868170 Click For Details Jonn Kunicky 604 9868170 8883785507</v>
       </c>
     </row>
     <row r="26">
@@ -873,16 +666,7 @@
         <v>IT and systems support</v>
       </c>
       <c r="C26" t="str">
-        <v>Muller Systems - Full IT Support Muller Systems offers full IT support services for Small to Medium and Enterprise in Canada and the US Health Care IT Retail IT Manufacturing &amp; Engineering IT Muller Live Support for Windows Passcode Solutions                                          Franchise Support                       Health Care IT                       Retail IT                       Manufacturing &amp; Engineering                                           Franchise Support Health Care IT Retail IT Manufacturing &amp; Engineering Services                                            Managed Services                       IT Service Management                       Hosting                       Website Maintenance                                           Managed Services IT Service Management Hosting Website Maintenance Products                      Partners                                           About Us                                                                                   Connect                                            Worldwide Support                       Contact Us                       Employment Opportunities                                       Worldwide Support Contact Us Employment Opportunities Muller QS » Windows Thin Clients Mac OS X Live Support Worldwide Support 1.800.668.6954      RMS (Resale Management Software) is a fully functional suite for any buy/sell store, franchise or pawn shop. It is safe and secure to use, all for a low monthly cost, no software purchase required!  For more information, clickhere            With Managed Services from Muller Systems, companies will spend less time worrying about their technology and more time focusing on their business. A proactive approach to supporting your technology ensures success for you and your business.   For more information click here           Muller Systems offers IT Service Management for your company. If you require a resource to be on site to resolve issues on an Ad-Hoc basis or if a crisis occurs and remote support is needed, don’t wait any longer, just give us a call.For more information click here.           If you are looking for an environment to host your server infrastructure or business critical applications, then look to Muller Systems.  Our data center provides redundant and backup power supplies, and data communications all environmentally controlled, while providing the security you require for your equipment.For more information click here           Do you require an affordable, specialized and reliable Point of Sale solution?   Whether you are a small retail outlet or a multi-national franchise, we have the solution for you.  It is easy to setup and deploy in your business.For more information click here      Muller Health Care IT has you covered from the cabling and infrastructure to the computers, peripherals and Electronic Medical Records software implementation and support. more info Mullers has been supporting the Buy and Sell Retail market for over 20 years.  Looking for an all-in-one software, hardware and support solution? Muller’s Retail Management software has it all.   more info Mullers understands that Manufacturing and Engineering firms require their technology to work as hard as they do.  Our full IT support services allow us to keep the technology up and running to meet the ever growing manufacturing industry.  Our full range of IT services is suited to meet your needs.  more info            Launching Muller Live Support will cause your computer to connect to a Muller Systems support representative and allow them temporary control of your computer to fix the problem. When they are finished, they will close the connection and the Muller Live Support software will be automatically removed from your system. When you click on the link, you will have the option to Run, Open or Save the file. Please hit Open or Run. You may get a warning that the file may be dangerous. This is normal and this warning is shown by your browser when any .EXE is opened. Do not launch Muller Live Support unless you've been asked to do so by a support technician.                                 Home | Client Upload | Privacy                                                                                                                                                                                                                                         Solutions                                            Franchise Support                       Health Care IT                       Retail IT                       Manufacturing &amp; Engineering                                                             Services                                            Managed Services                       IT Service Management                       Hosting                       Website Maintenance                                                             Products                                        Partners                                                                                                                                                                                                                           About Us                                                                                                     Connect                                            Worldwide Support                       Contact Us                       Employment Opportunities                                                                                                                                                                   RMS (Resale Management Software) is a fully functional suite for any buy/sell store, franchise or pawn shop. It is safe and secure to use, all for a low monthly cost, no software purchase required!  For more information, clickhere                        With Managed Services from Muller Systems, companies will spend less time worrying about their technology and more time focusing on their business. A proactive approach to supporting your technology ensures success for you and your business.   For more information click here                       Muller Systems offers IT Service Management for your company. If you require a resource to be on site to resolve issues on an Ad-Hoc basis or if a crisis occurs and remote support is needed, don’t wait any longer, just give us a call.For more information click here.                       If you are looking for an environment to host your server infrastructure or business critical applications, then look to Muller Systems.  Our data center provides redundant and backup power supplies, and data communications all environmentally controlled, while providing the security you require for your equipment.For more information click here                       Do you require an affordable, specialized and reliable Point of Sale solution?   Whether you are a small retail outlet or a multi-national franchise, we have the solution for you.  It is easy to setup and deploy in your business.For more information click here                                                                                Health Care IT             Muller Health Care IT has you covered from the cabling and infrastructure to the computers, peripherals and Electronic Medical Records software implementation and support. more info                                   Retail IT              Mullers has been supporting the Buy and Sell Retail market for over 20 years.  Looking for an all-in-one software, hardware and support solution? Muller’s Retail Management software has it all.   more info                                   Manufacturing &amp; Engineering IT             Mullers understands that Manufacturing and Engineering firms require their technology to work as hard as they do.  Our full IT support services allow us to keep the technology up and running to meet the ever growing manufacturing industry.  Our full range of IT services is suited to meet your needs.  more info                                              © Muller Systems Corporation Inc, 2016                                                            Muller QS »           Windows           Thin Clients           Mac OS X                      Live Support                      Worldwide Support 1.800.668.6954                                                                                                                         ×     Muller Live Support for Windows           Launching Muller Live Support will cause your computer to connect to a Muller Systems support representative and allow them temporary control of your computer to fix the problem. When they are finished, they will close the connection and the Muller Live Support software will be automatically removed from your system.     When you click on the link, you will have the option to Run, Open or Save the file. Please hit Open or Run. You may get a warning that the file may be dangerous. This is normal and this warning is shown by your browser when any .EXE is opened.     Do not launch Muller Live Support unless you've been asked to do so by a support technician.                  Passcode                        Launch       Close                                                                                  $("a[rel=popover]").popover();       var _gaq = _gaq || [],           previous_menu = null;       function menuTouched(e) {         e.preventDefault();         var t = this;         if (previous_menu != null) {           $(previous_menu).children('ul').toggleClass('touched');         }         previous_menu = this;         $(this).children('ul').toggleClass('touched');         $(this).unbind('touchend');         $(this).children('a').bind('touchend', function(e) {           e.preventDefault();           $(t).children('a').unbind('touchend');           $(t).toggleClass('touched');           $(t).bind('touchend',menuTouched);         });         setTimeout(function(){closeMenu(t);},5000);       }       function closeMenu(menu) {         if ($(menu).children('ul').hasClass('touched')) {           $(menu).children('a').unbind('touchend');           $(menu).children('ul').toggleClass('touched');           $(menu).bind('touchend',menuTouched);           previous_menu = null;         }       }       $(document).ready(function() {           _gaq.push(['_setAccount', 'UA-17575700-3']); _gaq.push(['_trackPageview']); var ga = document.createElement('script'); ga.type = 'text/javascript'; ga.async = true; ga.src = ('https:' == document.location.protocol ? 'https://ssl' : 'http://www') + '.google-analytics.com/ga.js'; var s = document.getElementsByTagName('script')[0]; s.parentNode.insertBefore(ga, s);                   $('li.menu a.item').click(function(e) {           e.preventDefault();         });                  $('a.modals.clickable').click(function(e) {           e.preventDefault();           $('#livesupport').modal();         });          $('#launch').click(function(e) {   e.preventDefault();   $.ajax({     type: 'POST',     url: '/forms/submit/livesupport/',     data: $('#livesupportform').serialize(),     success: function(msg) {       if (msg == '!windows') {         alert('We have determined you are attempting to use an unsupported operating system for this support service. Please check that you are currently logged into Windows based computer and try again.')         $('div.modal-body input[type="text"]').val('');         $('#livesupport').modal('hide');       } else if (msg !== 'false') {         window.location.href = msg;       }     }   }); });        });        $(document).ready(function(data) {    $('#slides').slides({             preload: true,             preloadImage:             generateNextPrev: true,             play: 10000,           });  });          Home Client Upload Privacy                                                                    Solutions Franchise Support Health Care IT Retail IT Manufacturing &amp; Engineering Services Managed Services IT Service Management Hosting Website Maintenance Products Partners About Us Connect Worldwide Support Contact Us Employment Opportunities here  here here here here more info more info more info Muller QS » Windows Thin Clients Mac OS X Live Support Worldwide Support 1.800.668.6954 × Launch Close | |</v>
-      </c>
-      <c r="D26" t="str">
-        <v>Muller Systems - Full IT Support Muller Systems offers full IT support services for Small to Medium and Enterprise in Canada and the US Health Care IT Retail IT Manufacturing &amp; Engineering IT Muller Live Support for Windows Passcode Solutions                                          Franchise Support                       Health Care IT                       Retail IT                       Manufacturing &amp; Engineering                                           Franchise Support Health Care IT Retail IT Manufacturing &amp; Engineering Services                                            Managed Services                       IT Service Management                       Hosting                       Website Maintenance                                           Managed Services IT Service Management Hosting Website Maintenance Products                      Partners                                           About Us                                                                                   Connect                                            Worldwide Support                       Contact Us                       Employment Opportunities                                       Worldwide Support Contact Us Employment Opportunities Muller QS » Windows Thin Clients Mac OS X Live Support Worldwide Support 1.800.668.6954      RMS (Resale Management Software) is a fully functional suite for any buy/sell store, franchise or pawn shop. It is safe and secure to use, all for a low monthly cost, no software purchase required!  For more information, clickhere            With Managed Services from Muller Systems, companies will spend less time worrying about their technology and more time focusing on their business. A proactive approach to supporting your technology ensures success for you and your business.   For more information click here           Muller Systems offers IT Service Management for your company. If you require a resource to be on site to resolve issues on an Ad-Hoc basis or if a crisis occurs and remote support is needed, don’t wait any longer, just give us a call.For more information click here.           If you are looking for an environment to host your server infrastructure or business critical applications, then look to Muller Systems.  Our data center provides redundant and backup power supplies, and data communications all environmentally controlled, while providing the security you require for your equipment.For more information click here           Do you require an affordable, specialized and reliable Point of Sale solution?   Whether you are a small retail outlet or a multi-national franchise, we have the solution for you.  It is easy to setup and deploy in your business.For more information click here      Muller Health Care IT has you covered from the cabling and infrastructure to the computers, peripherals and Electronic Medical Records software implementation and support. more info Mullers has been supporting the Buy and Sell Retail market for over 20 years.  Looking for an all-in-one software, hardware and support solution? Muller’s Retail Management software has it all.   more info Mullers understands that Manufacturing and Engineering firms require their technology to work as hard as they do.  Our full IT support services allow us to keep the technology up and running to meet the ever growing manufacturing industry.  Our full range of IT services is suited to meet your needs.  more info            Launching Muller Live Support will cause your computer to connect to a Muller Systems support representative and allow them temporary control of your computer to fix the problem. When they are finished, they will close the connection and the Muller Live Support software will be automatically removed from your system. When you click on the link, you will have the option to Run, Open or Save the file. Please hit Open or Run. You may get a warning that the file may be dangerous. This is normal and this warning is shown by your browser when any .EXE is opened. Do not launch Muller Live Support unless you've been asked to do so by a support technician.                                 Home | Client Upload | Privacy                                                                                                                                                                                                                                         Solutions                                            Franchise Support                       Health Care IT                       Retail IT                       Manufacturing &amp; Engineering                                                             Services                                            Managed Services                       IT Service Management                       Hosting                       Website Maintenance                                                             Products                                        Partners                                                                                                                                                                                                                           About Us                                                                                                     Connect                                            Worldwide Support                       Contact Us                       Employment Opportunities                                                                                                                                                                   RMS (Resale Management Software) is a fully functional suite for any buy/sell store, franchise or pawn shop. It is safe and secure to use, all for a low monthly cost, no software purchase required!  For more information, clickhere                        With Managed Services from Muller Systems, companies will spend less time worrying about their technology and more time focusing on their business. A proactive approach to supporting your technology ensures success for you and your business.   For more information click here                       Muller Systems offers IT Service Management for your company. If you require a resource to be on site to resolve issues on an Ad-Hoc basis or if a crisis occurs and remote support is needed, don’t wait any longer, just give us a call.For more information click here.                       If you are looking for an environment to host your server infrastructure or business critical applications, then look to Muller Systems.  Our data center provides redundant and backup power supplies, and data communications all environmentally controlled, while providing the security you require for your equipment.For more information click here                       Do you require an affordable, specialized and reliable Point of Sale solution?   Whether you are a small retail outlet or a multi-national franchise, we have the solution for you.  It is easy to setup and deploy in your business.For more information click here                                                                                Health Care IT             Muller Health Care IT has you covered from the cabling and infrastructure to the computers, peripherals and Electronic Medical Records software implementation and support. more info                                   Retail IT              Mullers has been supporting the Buy and Sell Retail market for over 20 years.  Looking for an all-in-one software, hardware and support solution? Muller’s Retail Management software has it all.   more info                                   Manufacturing &amp; Engineering IT             Mullers understands that Manufacturing and Engineering firms require their technology to work as hard as they do.  Our full IT support services allow us to keep the technology up and running to meet the ever growing manufacturing industry.  Our full range of IT services is suited to meet your needs.  more info                                              © Muller Systems Corporation Inc, 2016                                                            Muller QS »           Windows           Thin Clients           Mac OS X                      Live Support                      Worldwide Support 1.800.668.6954                                                                                                                         ×     Muller Live Support for Windows           Launching Muller Live Support will cause your computer to connect to a Muller Systems support representative and allow them temporary control of your computer to fix the problem. When they are finished, they will close the connection and the Muller Live Support software will be automatically removed from your system.     When you click on the link, you will have the option to Run, Open or Save the file. Please hit Open or Run. You may get a warning that the file may be dangerous. This is normal and this warning is shown by your browser when any .EXE is opened.     Do not launch Muller Live Support unless you've been asked to do so by a support technician.                  Passcode                        Launch       Close                                                                                  $("a[rel=popover]").popover();       var _gaq = _gaq || [],           previous_menu = null;       function menuTouched(e) {         e.preventDefault();         var t = this;         if (previous_menu != null) {           $(previous_menu).children('ul').toggleClass('touched');         }         previous_menu = this;         $(this).children('ul').toggleClass('touched');         $(this).unbind('touchend');         $(this).children('a').bind('touchend', function(e) {           e.preventDefault();           $(t).children('a').unbind('touchend');           $(t).toggleClass('touched');           $(t).bind('touchend',menuTouched);         });         setTimeout(function(){closeMenu(t);},5000);       }       function closeMenu(menu) {         if ($(menu).children('ul').hasClass('touched')) {           $(menu).children('a').unbind('touchend');           $(menu).children('ul').toggleClass('touched');           $(menu).bind('touchend',menuTouched);           previous_menu = null;         }       }       $(document).ready(function() {           _gaq.push(['_setAccount', 'UA-17575700-3']); _gaq.push(['_trackPageview']); var ga = document.createElement('script'); ga.type = 'text/javascript'; ga.async = true; ga.src = ('https:' == document.location.protocol ? 'https://ssl' : 'http://www') + '.google-analytics.com/ga.js'; var s = document.getElementsByTagName('script')[0]; s.parentNode.insertBefore(ga, s);                   $('li.menu a.item').click(function(e) {           e.preventDefault();         });                  $('a.modals.clickable').click(function(e) {           e.preventDefault();           $('#livesupport').modal();         });          $('#launch').click(function(e) {   e.preventDefault();   $.ajax({     type: 'POST',     url: '/forms/submit/livesupport/',     data: $('#livesupportform').serialize(),     success: function(msg) {       if (msg == '!windows') {         alert('We have determined you are attempting to use an unsupported operating system for this support service. Please check that you are currently logged into Windows based computer and try again.')         $('div.modal-body input[type="text"]').val('');         $('#livesupport').modal('hide');       } else if (msg !== 'false') {         window.location.href = msg;       }     }   }); });        });        $(document).ready(function(data) {    $('#slides').slides({             preload: true,             preloadImage:             generateNextPrev: true,             play: 10000,           });  });          Home Client Upload Privacy                                                                    Solutions Franchise Support Health Care IT Retail IT Manufacturing &amp; Engineering Services Managed Services IT Service Management Hosting Website Maintenance Products Partners About Us Connect Worldwide Support Contact Us Employment Opportunities here  here here here here more info more info more info Muller QS » Windows Thin Clients Mac OS X Live Support Worldwide Support 1.800.668.6954 × Launch Close | |</v>
-      </c>
-      <c r="E26" t="str">
-        <v>Muller Systems - Full IT Support Muller Systems offers full IT support services for Small to Medium and Enterprise in Canada and the US Health Care IT Retail IT Manufacturing &amp; Engineering IT Muller Live Support for Windows Passcode Solutions                                          Franchise Support                       Health Care IT                       Retail IT                       Manufacturing &amp; Engineering                                           Franchise Support Health Care IT Retail IT Manufacturing &amp; Engineering Services                                            Managed Services                       IT Service Management                       Hosting                       Website Maintenance                                           Managed Services IT Service Management Hosting Website Maintenance Products                      Partners                                           About Us                                                                                   Connect                                            Worldwide Support                       Contact Us                       Employment Opportunities                                       Worldwide Support Contact Us Employment Opportunities Muller QS » Windows Thin Clients Mac OS X Live Support Worldwide Support 1.800.668.6954      RMS (Resale Management Software) is a fully functional suite for any buy/sell store, franchise or pawn shop. It is safe and secure to use, all for a low monthly cost, no software purchase required!  For more information, clickhere            With Managed Services from Muller Systems, companies will spend less time worrying about their technology and more time focusing on their business. A proactive approach to supporting your technology ensures success for you and your business.   For more information click here           Muller Systems offers IT Service Management for your company. If you require a resource to be on site to resolve issues on an Ad-Hoc basis or if a crisis occurs and remote support is needed, don’t wait any longer, just give us a call.For more information click here.           If you are looking for an environment to host your server infrastructure or business critical applications, then look to Muller Systems.  Our data center provides redundant and backup power supplies, and data communications all environmentally controlled, while providing the security you require for your equipment.For more information click here           Do you require an affordable, specialized and reliable Point of Sale solution?   Whether you are a small retail outlet or a multi-national franchise, we have the solution for you.  It is easy to setup and deploy in your business.For more information click here      Muller Health Care IT has you covered from the cabling and infrastructure to the computers, peripherals and Electronic Medical Records software implementation and support. more info Mullers has been supporting the Buy and Sell Retail market for over 20 years.  Looking for an all-in-one software, hardware and support solution? Muller’s Retail Management software has it all.   more info Mullers understands that Manufacturing and Engineering firms require their technology to work as hard as they do.  Our full IT support services allow us to keep the technology up and running to meet the ever growing manufacturing industry.  Our full range of IT services is suited to meet your needs.  more info            Launching Muller Live Support will cause your computer to connect to a Muller Systems support representative and allow them temporary control of your computer to fix the problem. When they are finished, they will close the connection and the Muller Live Support software will be automatically removed from your system. When you click on the link, you will have the option to Run, Open or Save the file. Please hit Open or Run. You may get a warning that the file may be dangerous. This is normal and this warning is shown by your browser when any .EXE is opened. Do not launch Muller Live Support unless you've been asked to do so by a support technician.                                 Home | Client Upload | Privacy                                                                                                                                                                                                                                         Solutions                                            Franchise Support                       Health Care IT                       Retail IT                       Manufacturing &amp; Engineering                                                             Services                                            Managed Services                       IT Service Management                       Hosting                       Website Maintenance                                                             Products                                        Partners                                                                                                                                                                                                                           About Us                                                                                                     Connect                                            Worldwide Support                       Contact Us                       Employment Opportunities                                                                                                                                                                   RMS (Resale Management Software) is a fully functional suite for any buy/sell store, franchise or pawn shop. It is safe and secure to use, all for a low monthly cost, no software purchase required!  For more information, clickhere                        With Managed Services from Muller Systems, companies will spend less time worrying about their technology and more time focusing on their business. A proactive approach to supporting your technology ensures success for you and your business.   For more information click here                       Muller Systems offers IT Service Management for your company. If you require a resource to be on site to resolve issues on an Ad-Hoc basis or if a crisis occurs and remote support is needed, don’t wait any longer, just give us a call.For more information click here.                       If you are looking for an environment to host your server infrastructure or business critical applications, then look to Muller Systems.  Our data center provides redundant and backup power supplies, and data communications all environmentally controlled, while providing the security you require for your equipment.For more information click here                       Do you require an affordable, specialized and reliable Point of Sale solution?   Whether you are a small retail outlet or a multi-national franchise, we have the solution for you.  It is easy to setup and deploy in your business.For more information click here                                                                                Health Care IT             Muller Health Care IT has you covered from the cabling and infrastructure to the computers, peripherals and Electronic Medical Records software implementation and support. more info                                   Retail IT              Mullers has been supporting the Buy and Sell Retail market for over 20 years.  Looking for an all-in-one software, hardware and support solution? Muller’s Retail Management software has it all.   more info                                   Manufacturing &amp; Engineering IT             Mullers understands that Manufacturing and Engineering firms require their technology to work as hard as they do.  Our full IT support services allow us to keep the technology up and running to meet the ever growing manufacturing industry.  Our full range of IT services is suited to meet your needs.  more info                                              © Muller Systems Corporation Inc, 2016                                                            Muller QS »           Windows           Thin Clients           Mac OS X                      Live Support                      Worldwide Support 1.800.668.6954                                                                                                                         ×     Muller Live Support for Windows           Launching Muller Live Support will cause your computer to connect to a Muller Systems support representative and allow them temporary control of your computer to fix the problem. When they are finished, they will close the connection and the Muller Live Support software will be automatically removed from your system.     When you click on the link, you will have the option to Run, Open or Save the file. Please hit Open or Run. You may get a warning that the file may be dangerous. This is normal and this warning is shown by your browser when any .EXE is opened.     Do not launch Muller Live Support unless you've been asked to do so by a support technician.                  Passcode                        Launch       Close                                                                                  $("a[rel=popover]").popover();       var _gaq = _gaq || [],           previous_menu = null;       function menuTouched(e) {         e.preventDefault();         var t = this;         if (previous_menu != null) {           $(previous_menu).children('ul').toggleClass('touched');         }         previous_menu = this;         $(this).children('ul').toggleClass('touched');         $(this).unbind('touchend');         $(this).children('a').bind('touchend', function(e) {           e.preventDefault();           $(t).children('a').unbind('touchend');           $(t).toggleClass('touched');           $(t).bind('touchend',menuTouched);         });         setTimeout(function(){closeMenu(t);},5000);       }       function closeMenu(menu) {         if ($(menu).children('ul').hasClass('touched')) {           $(menu).children('a').unbind('touchend');           $(menu).children('ul').toggleClass('touched');           $(menu).bind('touchend',menuTouched);           previous_menu = null;         }       }       $(document).ready(function() {           _gaq.push(['_setAccount', 'UA-17575700-3']); _gaq.push(['_trackPageview']); var ga = document.createElement('script'); ga.type = 'text/javascript'; ga.async = true; ga.src = ('https:' == document.location.protocol ? 'https://ssl' : 'http://www') + '.google-analytics.com/ga.js'; var s = document.getElementsByTagName('script')[0]; s.parentNode.insertBefore(ga, s);                   $('li.menu a.item').click(function(e) {           e.preventDefault();         });                  $('a.modals.clickable').click(function(e) {           e.preventDefault();           $('#livesupport').modal();         });          $('#launch').click(function(e) {   e.preventDefault();   $.ajax({     type: 'POST',     url: '/forms/submit/livesupport/',     data: $('#livesupportform').serialize(),     success: function(msg) {       if (msg == '!windows') {         alert('We have determined you are attempting to use an unsupported operating system for this support service. Please check that you are currently logged into Windows based computer and try again.')         $('div.modal-body input[type="text"]').val('');         $('#livesupport').modal('hide');       } else if (msg !== 'false') {         window.location.href = msg;       }     }   }); });        });        $(document).ready(function(data) {    $('#slides').slides({             preload: true,             preloadImage:             generateNextPrev: true,             play: 10000,           });  });          Home Client Upload Privacy                                                                    Solutions Franchise Support Health Care IT Retail IT Manufacturing &amp; Engineering Services Managed Services IT Service Management Hosting Website Maintenance Products Partners About Us Connect Worldwide Support Contact Us Employment Opportunities here  here here here here more info more info more info Muller QS » Windows Thin Clients Mac OS X Live Support Worldwide Support 1.800.668.6954 × Launch Close | |</v>
-      </c>
-      <c r="F26" t="str">
-        <v>Muller Systems - Full IT Support Muller Systems offers full IT support services for Small to Medium and Enterprise in Canada and the US Health Care IT Retail IT Manufacturing &amp; Engineering IT Muller Live Support for Windows Passcode Solutions                                          Franchise Support                       Health Care IT                       Retail IT                       Manufacturing &amp; Engineering                                           Franchise Support Health Care IT Retail IT Manufacturing &amp; Engineering Services                                            Managed Services                       IT Service Management                       Hosting                       Website Maintenance                                           Managed Services IT Service Management Hosting Website Maintenance Products                      Partners                                           About Us                                                                                   Connect                                            Worldwide Support                       Contact Us                       Employment Opportunities                                       Worldwide Support Contact Us Employment Opportunities Muller QS » Windows Thin Clients Mac OS X Live Support Worldwide Support 1.800.668.6954      RMS (Resale Management Software) is a fully functional suite for any buy/sell store, franchise or pawn shop. It is safe and secure to use, all for a low monthly cost, no software purchase required!  For more information, clickhere            With Managed Services from Muller Systems, companies will spend less time worrying about their technology and more time focusing on their business. A proactive approach to supporting your technology ensures success for you and your business.   For more information click here           Muller Systems offers IT Service Management for your company. If you require a resource to be on site to resolve issues on an Ad-Hoc basis or if a crisis occurs and remote support is needed, don’t wait any longer, just give us a call.For more information click here.           If you are looking for an environment to host your server infrastructure or business critical applications, then look to Muller Systems.  Our data center provides redundant and backup power supplies, and data communications all environmentally controlled, while providing the security you require for your equipment.For more information click here           Do you require an affordable, specialized and reliable Point of Sale solution?   Whether you are a small retail outlet or a multi-national franchise, we have the solution for you.  It is easy to setup and deploy in your business.For more information click here      Muller Health Care IT has you covered from the cabling and infrastructure to the computers, peripherals and Electronic Medical Records software implementation and support. more info Mullers has been supporting the Buy and Sell Retail market for over 20 years.  Looking for an all-in-one software, hardware and support solution? Muller’s Retail Management software has it all.   more info Mullers understands that Manufacturing and Engineering firms require their technology to work as hard as they do.  Our full IT support services allow us to keep the technology up and running to meet the ever growing manufacturing industry.  Our full range of IT services is suited to meet your needs.  more info            Launching Muller Live Support will cause your computer to connect to a Muller Systems support representative and allow them temporary control of your computer to fix the problem. When they are finished, they will close the connection and the Muller Live Support software will be automatically removed from your system. When you click on the link, you will have the option to Run, Open or Save the file. Please hit Open or Run. You may get a warning that the file may be dangerous. This is normal and this warning is shown by your browser when any .EXE is opened. Do not launch Muller Live Support unless you've been asked to do so by a support technician.                                 Home | Client Upload | Privacy                                                                                                                                                                                                                                         Solutions                                            Franchise Support                       Health Care IT                       Retail IT                       Manufacturing &amp; Engineering                                                             Services                                            Managed Services                       IT Service Management                       Hosting                       Website Maintenance                                                             Products                                        Partners                                                                                                                                                                                                                           About Us                                                                                                     Connect                                            Worldwide Support                       Contact Us                       Employment Opportunities                                                                                                                                                                   RMS (Resale Management Software) is a fully functional suite for any buy/sell store, franchise or pawn shop. It is safe and secure to use, all for a low monthly cost, no software purchase required!  For more information, clickhere                        With Managed Services from Muller Systems, companies will spend less time worrying about their technology and more time focusing on their business. A proactive approach to supporting your technology ensures success for you and your business.   For more information click here                       Muller Systems offers IT Service Management for your company. If you require a resource to be on site to resolve issues on an Ad-Hoc basis or if a crisis occurs and remote support is needed, don’t wait any longer, just give us a call.For more information click here.                       If you are looking for an environment to host your server infrastructure or business critical applications, then look to Muller Systems.  Our data center provides redundant and backup power supplies, and data communications all environmentally controlled, while providing the security you require for your equipment.For more information click here                       Do you require an affordable, specialized and reliable Point of Sale solution?   Whether you are a small retail outlet or a multi-national franchise, we have the solution for you.  It is easy to setup and deploy in your business.For more information click here                                                                                Health Care IT             Muller Health Care IT has you covered from the cabling and infrastructure to the computers, peripherals and Electronic Medical Records software implementation and support. more info                                   Retail IT              Mullers has been supporting the Buy and Sell Retail market for over 20 years.  Looking for an all-in-one software, hardware and support solution? Muller’s Retail Management software has it all.   more info                                   Manufacturing &amp; Engineering IT             Mullers understands that Manufacturing and Engineering firms require their technology to work as hard as they do.  Our full IT support services allow us to keep the technology up and running to meet the ever growing manufacturing industry.  Our full range of IT services is suited to meet your needs.  more info                                              © Muller Systems Corporation Inc, 2016                                                            Muller QS »           Windows           Thin Clients           Mac OS X                      Live Support                      Worldwide Support 1.800.668.6954                                                                                                                         ×     Muller Live Support for Windows           Launching Muller Live Support will cause your computer to connect to a Muller Systems support representative and allow them temporary control of your computer to fix the problem. When they are finished, they will close the connection and the Muller Live Support software will be automatically removed from your system.     When you click on the link, you will have the option to Run, Open or Save the file. Please hit Open or Run. You may get a warning that the file may be dangerous. This is normal and this warning is shown by your browser when any .EXE is opened.     Do not launch Muller Live Support unless you've been asked to do so by a support technician.                  Passcode                        Launch       Close                                                                                  $("a[rel=popover]").popover();       var _gaq = _gaq || [],           previous_menu = null;       function menuTouched(e) {         e.preventDefault();         var t = this;         if (previous_menu != null) {           $(previous_menu).children('ul').toggleClass('touched');         }         previous_menu = this;         $(this).children('ul').toggleClass('touched');         $(this).unbind('touchend');         $(this).children('a').bind('touchend', function(e) {           e.preventDefault();           $(t).children('a').unbind('touchend');           $(t).toggleClass('touched');           $(t).bind('touchend',menuTouched);         });         setTimeout(function(){closeMenu(t);},5000);       }       function closeMenu(menu) {         if ($(menu).children('ul').hasClass('touched')) {           $(menu).children('a').unbind('touchend');           $(menu).children('ul').toggleClass('touched');           $(menu).bind('touchend',menuTouched);           previous_menu = null;         }       }       $(document).ready(function() {           _gaq.push(['_setAccount', 'UA-17575700-3']); _gaq.push(['_trackPageview']); var ga = document.createElement('script'); ga.type = 'text/javascript'; ga.async = true; ga.src = ('https:' == document.location.protocol ? 'https://ssl' : 'http://www') + '.google-analytics.com/ga.js'; var s = document.getElementsByTagName('script')[0]; s.parentNode.insertBefore(ga, s);                   $('li.menu a.item').click(function(e) {           e.preventDefault();         });                  $('a.modals.clickable').click(function(e) {           e.preventDefault();           $('#livesupport').modal();         });          $('#launch').click(function(e) {   e.preventDefault();   $.ajax({     type: 'POST',     url: '/forms/submit/livesupport/',     data: $('#livesupportform').serialize(),     success: function(msg) {       if (msg == '!windows') {         alert('We have determined you are attempting to use an unsupported operating system for this support service. Please check that you are currently logged into Windows based computer and try again.')         $('div.modal-body input[type="text"]').val('');         $('#livesupport').modal('hide');       } else if (msg !== 'false') {         window.location.href = msg;       }     }   }); });        });        $(document).ready(function(data) {    $('#slides').slides({             preload: true,             preloadImage:             generateNextPrev: true,             play: 10000,           });  });          Home Client Upload Privacy                                                                    Solutions Franchise Support Health Care IT Retail IT Manufacturing &amp; Engineering Services Managed Services IT Service Management Hosting Website Maintenance Products Partners About Us Connect Worldwide Support Contact Us Employment Opportunities here  here here here here more info more info more info Muller QS » Windows Thin Clients Mac OS X Live Support Worldwide Support 1.800.668.6954 × Launch Close | |</v>
+        <v>Muller Systems Full IT Support Muller Systems offers full IT support services for Small to Medium and Enterprise in Canada and the US Health Care IT Retail IT Manufacturing Engineering IT Muller Live Support for Windows Passcode Solutions Franchise Support Health Care IT Retail IT Manufacturing Engineering Franchise Support Health Care IT Retail IT Manufacturing Engineering Services Managed Services IT Service Management Hosting Website Maintenance Managed Services IT Service Management Hosting Website Maintenance Products Partners About Us Connect Worldwide Support Contact Us Employment Opportunities Worldwide Support Contact Us Employment Opportunities Muller QS » Windows Thin Clients Mac OS X Live Support Worldwide Support 18006686954 RMS Resale Management Software is a fully functional suite for any buysell store franchise or pawn shop It is safe and secure to use all for a low monthly cost no software purchase required For more information clickhere With Managed Services from Muller Systems companies will spend less time worrying about their technology and more time focusing on their business A proactive approach to supporting your technology ensures success for you and your business For more information click here Muller Systems offers IT Service Management for your company If you require a resource to be on site to resolve issues on an AdHoc basis or if a crisis occurs and remote support is needed don’t wait any longer just give us a callFor more information click here If you are looking for an environment to host your server infrastructure or business critical applications then look to Muller Systems Our data center provides redundant and backup power supplies and data communications all environmentally controlled while providing the security you require for your equipmentFor more information click here Do you require an affordable specialized and reliable Point of Sale solution Whether you are a small retail outlet or a multinational franchise we have the solution for you It is easy to setup and deploy in your businessFor more information click here Muller Health Care IT has you covered from the cabling and infrastructure to the computers peripherals and Electronic Medical Records software implementation and support more info Mullers has been supporting the Buy and Sell Retail market for over 20 years Looking for an allinone software hardware and support solution Muller’s Retail Management software has it all more info Mullers understands that Manufacturing and Engineering firms require their technology to work as hard as they do Our full IT support services allow us to keep the technology up and running to meet the ever growing manufacturing industry Our full range of IT services is suited to meet your needs more info Launching Muller Live Support will cause your computer to connect to a Muller Systems support representative and allow them temporary control of your computer to fix the problem When they are finished they will close the connection and the Muller Live Support software will be automatically removed from your system When you click on the link you will have the option to Run Open or Save the file Please hit Open or Run You may get a warning that the file may be dangerous This is normal and this warning is shown by your browser when any EXE is opened Do not launch Muller Live Support unless youve been asked to do so by a support technician Home Client Upload Privacy Solutions Franchise Support Health Care IT Retail IT Manufacturing Engineering Services Managed Services IT Service Management Hosting Website Maintenance Products Partners About Us Connect Worldwide Support Contact Us Employment Opportunities RMS Resale Management Software is a fully functional suite for any buysell store franchise or pawn shop It is safe and secure to use all for a low monthly cost no software purchase required For more information clickhere With Managed Services from Muller Systems companies will spend less time worrying about their technology and more time focusing on their business A proactive approach to supporting your technology ensures success for you and your business For more information click here Muller Systems offers IT Service Management for your company If you require a resource to be on site to resolve issues on an AdHoc basis or if a crisis occurs and remote support is needed don’t wait any longer just give us a callFor more information click here If you are looking for an environment to host your server infrastructure or business critical applications then look to Muller Systems Our data center provides redundant and backup power supplies and data communications all environmentally controlled while providing the security you require for your equipmentFor more information click here Do you require an affordable specialized and reliable Point of Sale solution Whether you are a small retail outlet or a multinational franchise we have the solution for you It is easy to setup and deploy in your businessFor more information click here Health Care IT Muller Health Care IT has you covered from the cabling and infrastructure to the computers peripherals and Electronic Medical Records software implementation and support more info Retail IT Mullers has been supporting the Buy and Sell Retail market for over 20 years Looking for an allinone software hardware and support solution Muller’s Retail Management software has it all more info Manufacturing Engineering IT Mullers understands that Manufacturing and Engineering firms require their technology to work as hard as they do Our full IT support services allow us to keep the technology up and running to meet the ever growing manufacturing industry Our full range of IT services is suited to meet your needs more info © Muller Systems Corporation Inc 2016 Muller QS » Windows Thin Clients Mac OS X Live Support Worldwide Support 18006686954 × Muller Live Support for Windows Launching Muller Live Support will cause your computer to connect to a Muller Systems support representative and allow them temporary control of your computer to fix the problem When they are finished they will close the connection and the Muller Live Support software will be automatically removed from your system When you click on the link you will have the option to Run Open or Save the file Please hit Open or Run You may get a warning that the file may be dangerous This is normal and this warning is shown by your browser when any EXE is opened Do not launch Muller Live Support unless youve been asked to do so by a support technician Passcode Launch Close arelpopoverpopover var gaq gaq previousmenu null function menuTouchede epreventDefault var t this if previousmenu null previousmenuchildrenultoggleClasstouched previousmenu this thischildrenultoggleClasstouched thisunbindtouchend thischildrenabindtouchend functione epreventDefault tchildrenaunbindtouchend ttoggleClasstouched tbindtouchendmenuTouched setTimeoutfunctioncloseMenut5000 function closeMenumenu if menuchildrenulhasClasstouched menuchildrenaunbindtouchend menuchildrenultoggleClasstouched menubindtouchendmenuTouched previousmenu null documentreadyfunction gaqpushsetAccount UA175757003 gaqpushtrackPageview var ga documentcreateElementscript gatype textjavascript gaasync true gasrc https documentlocationprotocol httpsssl httpwww googleanalyticscomgajs var s documentgetElementsByTagNamescript0 sparentNodeinsertBeforega s limenu aitemclickfunctione epreventDefault amodalsclickableclickfunctione epreventDefault livesupportmodal launchclickfunctione epreventDefault ajax type POST url formssubmitlivesupport data livesupportformserialize success functionmsg if msg windows alertWe have determined you are attempting to use an unsupported operating system for this support service Please check that you are currently logged into Windows based computer and try again divmodalbody inputtypetextval livesupportmodalhide else if msg false windowlocationhref msg documentreadyfunctiondata slidesslides preload true preloadImage generateNextPrev true play 10000 Home Client Upload Privacy Solutions Franchise Support Health Care IT Retail IT Manufacturing Engineering Services Managed Services IT Service Management Hosting Website Maintenance Products Partners About Us Connect Worldwide Support Contact Us Employment Opportunities here here here here here more info more info more info Muller QS » Windows Thin Clients Mac OS X Live Support Worldwide Support 18006686954 × Launch Close</v>
       </c>
     </row>
     <row r="27">
@@ -893,16 +677,7 @@
         <v>IT and systems support</v>
       </c>
       <c r="C27" t="str">
-        <v>Managed Services, IT Consulting &amp; Computer Support Ottawa Revolution Networks is Ottawa's premium provider of managed services, IT consulting and computer support in Ottawa. Our Advantages Features Your Local IT Support Experts Reliable Support To Enhance Your Business Prompt Response When You Need It Most Latest Posts: Location: Computer Support Network Services IT Services Managed Services IT Assessments Remote Backup Microsoft Office 365 Emergency Services Anti-Virus/Anti-Spam Exchange Hosting Network Design/Build Network Monitoring Network Wiring IT Consulting On-Site Computer Services sales@revnet.ca613-321-6198 sales@revnet.ca 613-321-6198 Home About Us Services Cloud Services     Microsoft Office 365   Managed Workstation   Exchange Hosting   Remote Backup   Anti-Virus/Anti-Spam   Network Monitoring     IT Consulting     IT Assessments &amp; Audits   VOIP Services   CCTV Camera Systems   CTO/CIO Services   Network Cabling   Disaster Recovery Planning     On-Site Services     Network Support   IT Staff Augmentation   Network Design/Build   Emergency Services   Technical Projects   Office Moves and Network Wiring      Support Blog Contact HomeAbout UsServices             Cloud Services               Microsoft Office 365  Managed Workstation  Exchange Hosting  Remote Backup  Anti-Virus/Anti-Spam  Network Monitoring   IT Consulting               IT Assessments &amp; Audits  VOIP Services  CCTV Camera Systems  CTO/CIO Services  Network Cabling  Disaster Recovery Planning   On-Site Services               Network Support  IT Staff Augmentation  Network Design/Build  Emergency Services  Technical Projects  Office Moves and Network Wiring   SupportBlogContact Home About Us Services    Cloud Services     Microsoft Office 365   Managed Workstation   Exchange Hosting   Remote Backup   Anti-Virus/Anti-Spam   Network Monitoring     IT Consulting     IT Assessments &amp; Audits   VOIP Services   CCTV Camera Systems   CTO/CIO Services   Network Cabling   Disaster Recovery Planning     On-Site Services     Network Support   IT Staff Augmentation   Network Design/Build   Emergency Services   Technical Projects   Office Moves and Network Wiring      Cloud Services     Microsoft Office 365   Managed Workstation   Exchange Hosting   Remote Backup   Anti-Virus/Anti-Spam   Network Monitoring    Microsoft Office 365 Managed Workstation Exchange Hosting Remote Backup Anti-Virus/Anti-Spam Network Monitoring IT Consulting     IT Assessments &amp; Audits   VOIP Services   CCTV Camera Systems   CTO/CIO Services   Network Cabling   Disaster Recovery Planning    IT Assessments &amp; Audits VOIP Services CCTV Camera Systems CTO/CIO Services Network Cabling Disaster Recovery Planning On-Site Services     Network Support   IT Staff Augmentation   Network Design/Build   Emergency Services   Technical Projects   Office Moves and Network Wiring    Network Support IT Staff Augmentation Network Design/Build Emergency Services Technical Projects Office Moves and Network Wiring Support Blog Contact Home About Us Services             Cloud Services               Microsoft Office 365  Managed Workstation  Exchange Hosting  Remote Backup  Anti-Virus/Anti-Spam  Network Monitoring   IT Consulting               IT Assessments &amp; Audits  VOIP Services  CCTV Camera Systems  CTO/CIO Services  Network Cabling  Disaster Recovery Planning   On-Site Services               Network Support  IT Staff Augmentation  Network Design/Build  Emergency Services  Technical Projects  Office Moves and Network Wiring    Cloud Services               Microsoft Office 365  Managed Workstation  Exchange Hosting  Remote Backup  Anti-Virus/Anti-Spam  Network Monitoring   Microsoft Office 365 Managed Workstation Exchange Hosting Remote Backup Anti-Virus/Anti-Spam Network Monitoring IT Consulting               IT Assessments &amp; Audits  VOIP Services  CCTV Camera Systems  CTO/CIO Services  Network Cabling  Disaster Recovery Planning   IT Assessments &amp; Audits VOIP Services CCTV Camera Systems CTO/CIO Services Network Cabling Disaster Recovery Planning On-Site Services               Network Support  IT Staff Augmentation  Network Design/Build  Emergency Services  Technical Projects  Office Moves and Network Wiring   Network Support IT Staff Augmentation Network Design/Build Emergency Services Technical Projects Office Moves and Network Wiring Support Blog Contact                                                               Go                                              Reliable Support           Call us at: 613.321.6198                                  Prompt Response           Call us at: 613.321.6198                                  Efficient Services           Call us at: 613.321.6198                                  Professional Solutions           Call us at: 613.321.6198            File Encryption: How Can I Protect My Data?             How Firewalls Can Help Protect the Perimeter             Why Are Cloud Based Solutions So Popular?             5 Common Web Attacks to Watch Out For             Welcome to the team, Chris!        Microsoft Office 365 Managed Workstation Exchange Hosting Remote Backup Anti-virus/Anti-spam Network Monitoring IT Assessments VOIP Services Camera Systems CTO/CIO Services Network Cabling Disaster Recovery Planning Network Support IT Staff Augmentation Network Design/Build Emergency Services Technical Projects Office Moves and Network Wiring Rely on our IT experts to assist you with their experience and masterful knowledge. Our reliable solutions will result in immediate improvements for your business. Our help desk technicians are always standing by, ready to provide you with the highest quality personal assistance at any moment you suffer technical difficulties. We are a trusted advisor to hundreds of local businesses, offering on-going support &amp; advice for all IT-related needs. We work with businesses in a variety of industries, including healthcare, restaurants, professional services, legal, technology and manufacturing. © Copyright 2015. Revolution Networks. Online Marketing by seoplus+ sales@revnet.ca Home About Us Services  Cloud Services Microsoft Office 365 Managed Workstation Exchange Hosting Remote Backup Anti-Virus/Anti-Spam Network Monitoring IT Consulting IT Assessments &amp; Audits VOIP Services CCTV Camera Systems CTO/CIO Services Network Cabling Disaster Recovery Planning On-Site Services Network Support IT Staff Augmentation Network Design/Build Emergency Services Technical Projects Office Moves and Network Wiring Support Blog Contact Home About Us Services Cloud Services Microsoft Office 365 Managed Workstation Exchange Hosting Remote Backup Anti-Virus/Anti-Spam Network Monitoring IT Consulting IT Assessments &amp; Audits VOIP Services CCTV Camera Systems CTO/CIO Services Network Cabling Disaster Recovery Planning On-Site Services Network Support IT Staff Augmentation Network Design/Build Emergency Services Technical Projects Office Moves and Network Wiring Support Blog Contact 613.321.6198 613.321.6198 613.321.6198 613.321.6198 Microsoft Office 365 Managed Workstation Exchange Hosting Remote Backup Anti-virus/Anti-spam Network Monitoring Learn More IT Assessments VOIP Services Camera Systems CTO/CIO Services Network Cabling Disaster Recovery Planning Learn More Network Support IT Staff Augmentation Network Design/Build Emergency Services Technical Projects Office Moves and Network Wiring Learn More Learn More Learn More Learn More Learn More Learn More Learn More Learn More Learn More Learn More Learn More Learn More Learn More Contact us File Encryption: How Can I Protect My Data? How Firewalls Can Help Protect the Perimeter Why Are Cloud Based Solutions So Popular? 5 Common Web Attacks to Watch Out For Welcome to the team, Chris! 613.321.6198 sales@revnet.ca seoplus+ Toggle navigation Menu                                                          Go</v>
-      </c>
-      <c r="D27" t="str">
-        <v>Managed Services, IT Consulting &amp; Computer Support Ottawa Revolution Networks is Ottawa's premium provider of managed services, IT consulting and computer support in Ottawa. Our Advantages Features Your Local IT Support Experts Reliable Support To Enhance Your Business Prompt Response When You Need It Most Latest Posts: Location: Computer Support Network Services IT Services Managed Services IT Assessments Remote Backup Microsoft Office 365 Emergency Services Anti-Virus/Anti-Spam Exchange Hosting Network Design/Build Network Monitoring Network Wiring IT Consulting On-Site Computer Services sales@revnet.ca613-321-6198 sales@revnet.ca 613-321-6198 Home About Us Services Cloud Services     Microsoft Office 365   Managed Workstation   Exchange Hosting   Remote Backup   Anti-Virus/Anti-Spam   Network Monitoring     IT Consulting     IT Assessments &amp; Audits   VOIP Services   CCTV Camera Systems   CTO/CIO Services   Network Cabling   Disaster Recovery Planning     On-Site Services     Network Support   IT Staff Augmentation   Network Design/Build   Emergency Services   Technical Projects   Office Moves and Network Wiring      Support Blog Contact HomeAbout UsServices             Cloud Services               Microsoft Office 365  Managed Workstation  Exchange Hosting  Remote Backup  Anti-Virus/Anti-Spam  Network Monitoring   IT Consulting               IT Assessments &amp; Audits  VOIP Services  CCTV Camera Systems  CTO/CIO Services  Network Cabling  Disaster Recovery Planning   On-Site Services               Network Support  IT Staff Augmentation  Network Design/Build  Emergency Services  Technical Projects  Office Moves and Network Wiring   SupportBlogContact Home About Us Services    Cloud Services     Microsoft Office 365   Managed Workstation   Exchange Hosting   Remote Backup   Anti-Virus/Anti-Spam   Network Monitoring     IT Consulting     IT Assessments &amp; Audits   VOIP Services   CCTV Camera Systems   CTO/CIO Services   Network Cabling   Disaster Recovery Planning     On-Site Services     Network Support   IT Staff Augmentation   Network Design/Build   Emergency Services   Technical Projects   Office Moves and Network Wiring      Cloud Services     Microsoft Office 365   Managed Workstation   Exchange Hosting   Remote Backup   Anti-Virus/Anti-Spam   Network Monitoring    Microsoft Office 365 Managed Workstation Exchange Hosting Remote Backup Anti-Virus/Anti-Spam Network Monitoring IT Consulting     IT Assessments &amp; Audits   VOIP Services   CCTV Camera Systems   CTO/CIO Services   Network Cabling   Disaster Recovery Planning    IT Assessments &amp; Audits VOIP Services CCTV Camera Systems CTO/CIO Services Network Cabling Disaster Recovery Planning On-Site Services     Network Support   IT Staff Augmentation   Network Design/Build   Emergency Services   Technical Projects   Office Moves and Network Wiring    Network Support IT Staff Augmentation Network Design/Build Emergency Services Technical Projects Office Moves and Network Wiring Support Blog Contact Home About Us Services             Cloud Services               Microsoft Office 365  Managed Workstation  Exchange Hosting  Remote Backup  Anti-Virus/Anti-Spam  Network Monitoring   IT Consulting               IT Assessments &amp; Audits  VOIP Services  CCTV Camera Systems  CTO/CIO Services  Network Cabling  Disaster Recovery Planning   On-Site Services               Network Support  IT Staff Augmentation  Network Design/Build  Emergency Services  Technical Projects  Office Moves and Network Wiring    Cloud Services               Microsoft Office 365  Managed Workstation  Exchange Hosting  Remote Backup  Anti-Virus/Anti-Spam  Network Monitoring   Microsoft Office 365 Managed Workstation Exchange Hosting Remote Backup Anti-Virus/Anti-Spam Network Monitoring IT Consulting               IT Assessments &amp; Audits  VOIP Services  CCTV Camera Systems  CTO/CIO Services  Network Cabling  Disaster Recovery Planning   IT Assessments &amp; Audits VOIP Services CCTV Camera Systems CTO/CIO Services Network Cabling Disaster Recovery Planning On-Site Services               Network Support  IT Staff Augmentation  Network Design/Build  Emergency Services  Technical Projects  Office Moves and Network Wiring   Network Support IT Staff Augmentation Network Design/Build Emergency Services Technical Projects Office Moves and Network Wiring Support Blog Contact                                                               Go                                              Reliable Support           Call us at: 613.321.6198                                  Prompt Response           Call us at: 613.321.6198                                  Efficient Services           Call us at: 613.321.6198                                  Professional Solutions           Call us at: 613.321.6198            File Encryption: How Can I Protect My Data?             How Firewalls Can Help Protect the Perimeter             Why Are Cloud Based Solutions So Popular?             5 Common Web Attacks to Watch Out For             Welcome to the team, Chris!        Microsoft Office 365 Managed Workstation Exchange Hosting Remote Backup Anti-virus/Anti-spam Network Monitoring IT Assessments VOIP Services Camera Systems CTO/CIO Services Network Cabling Disaster Recovery Planning Network Support IT Staff Augmentation Network Design/Build Emergency Services Technical Projects Office Moves and Network Wiring Rely on our IT experts to assist you with their experience and masterful knowledge. Our reliable solutions will result in immediate improvements for your business. Our help desk technicians are always standing by, ready to provide you with the highest quality personal assistance at any moment you suffer technical difficulties. We are a trusted advisor to hundreds of local businesses, offering on-going support &amp; advice for all IT-related needs. We work with businesses in a variety of industries, including healthcare, restaurants, professional services, legal, technology and manufacturing. © Copyright 2015. Revolution Networks. Online Marketing by seoplus+ sales@revnet.ca Home About Us Services  Cloud Services Microsoft Office 365 Managed Workstation Exchange Hosting Remote Backup Anti-Virus/Anti-Spam Network Monitoring IT Consulting IT Assessments &amp; Audits VOIP Services CCTV Camera Systems CTO/CIO Services Network Cabling Disaster Recovery Planning On-Site Services Network Support IT Staff Augmentation Network Design/Build Emergency Services Technical Projects Office Moves and Network Wiring Support Blog Contact Home About Us Services Cloud Services Microsoft Office 365 Managed Workstation Exchange Hosting Remote Backup Anti-Virus/Anti-Spam Network Monitoring IT Consulting IT Assessments &amp; Audits VOIP Services CCTV Camera Systems CTO/CIO Services Network Cabling Disaster Recovery Planning On-Site Services Network Support IT Staff Augmentation Network Design/Build Emergency Services Technical Projects Office Moves and Network Wiring Support Blog Contact 613.321.6198 613.321.6198 613.321.6198 613.321.6198 Microsoft Office 365 Managed Workstation Exchange Hosting Remote Backup Anti-virus/Anti-spam Network Monitoring Learn More IT Assessments VOIP Services Camera Systems CTO/CIO Services Network Cabling Disaster Recovery Planning Learn More Network Support IT Staff Augmentation Network Design/Build Emergency Services Technical Projects Office Moves and Network Wiring Learn More Learn More Learn More Learn More Learn More Learn More Learn More Learn More Learn More Learn More Learn More Learn More Learn More Contact us File Encryption: How Can I Protect My Data? How Firewalls Can Help Protect the Perimeter Why Are Cloud Based Solutions So Popular? 5 Common Web Attacks to Watch Out For Welcome to the team, Chris! 613.321.6198 sales@revnet.ca seoplus+ Toggle navigation Menu                                                          Go</v>
-      </c>
-      <c r="E27" t="str">
-        <v>Managed Services, IT Consulting &amp; Computer Support Ottawa Revolution Networks is Ottawa's premium provider of managed services, IT consulting and computer support in Ottawa. Our Advantages Features Your Local IT Support Experts Reliable Support To Enhance Your Business Prompt Response When You Need It Most Latest Posts: Location: Computer Support Network Services IT Services Managed Services IT Assessments Remote Backup Microsoft Office 365 Emergency Services Anti-Virus/Anti-Spam Exchange Hosting Network Design/Build Network Monitoring Network Wiring IT Consulting On-Site Computer Services sales@revnet.ca613-321-6198 sales@revnet.ca 613-321-6198 Home About Us Services Cloud Services     Microsoft Office 365   Managed Workstation   Exchange Hosting   Remote Backup   Anti-Virus/Anti-Spam   Network Monitoring     IT Consulting     IT Assessments &amp; Audits   VOIP Services   CCTV Camera Systems   CTO/CIO Services   Network Cabling   Disaster Recovery Planning     On-Site Services     Network Support   IT Staff Augmentation   Network Design/Build   Emergency Services   Technical Projects   Office Moves and Network Wiring      Support Blog Contact HomeAbout UsServices             Cloud Services               Microsoft Office 365  Managed Workstation  Exchange Hosting  Remote Backup  Anti-Virus/Anti-Spam  Network Monitoring   IT Consulting               IT Assessments &amp; Audits  VOIP Services  CCTV Camera Systems  CTO/CIO Services  Network Cabling  Disaster Recovery Planning   On-Site Services               Network Support  IT Staff Augmentation  Network Design/Build  Emergency Services  Technical Projects  Office Moves and Network Wiring   SupportBlogContact Home About Us Services    Cloud Services     Microsoft Office 365   Managed Workstation   Exchange Hosting   Remote Backup   Anti-Virus/Anti-Spam   Network Monitoring     IT Consulting     IT Assessments &amp; Audits   VOIP Services   CCTV Camera Systems   CTO/CIO Services   Network Cabling   Disaster Recovery Planning     On-Site Services     Network Support   IT Staff Augmentation   Network Design/Build   Emergency Services   Technical Projects   Office Moves and Network Wiring      Cloud Services     Microsoft Office 365   Managed Workstation   Exchange Hosting   Remote Backup   Anti-Virus/Anti-Spam   Network Monitoring    Microsoft Office 365 Managed Workstation Exchange Hosting Remote Backup Anti-Virus/Anti-Spam Network Monitoring IT Consulting     IT Assessments &amp; Audits   VOIP Services   CCTV Camera Systems   CTO/CIO Services   Network Cabling   Disaster Recovery Planning    IT Assessments &amp; Audits VOIP Services CCTV Camera Systems CTO/CIO Services Network Cabling Disaster Recovery Planning On-Site Services     Network Support   IT Staff Augmentation   Network Design/Build   Emergency Services   Technical Projects   Office Moves and Network Wiring    Network Support IT Staff Augmentation Network Design/Build Emergency Services Technical Projects Office Moves and Network Wiring Support Blog Contact Home About Us Services             Cloud Services               Microsoft Office 365  Managed Workstation  Exchange Hosting  Remote Backup  Anti-Virus/Anti-Spam  Network Monitoring   IT Consulting               IT Assessments &amp; Audits  VOIP Services  CCTV Camera Systems  CTO/CIO Services  Network Cabling  Disaster Recovery Planning   On-Site Services               Network Support  IT Staff Augmentation  Network Design/Build  Emergency Services  Technical Projects  Office Moves and Network Wiring    Cloud Services               Microsoft Office 365  Managed Workstation  Exchange Hosting  Remote Backup  Anti-Virus/Anti-Spam  Network Monitoring   Microsoft Office 365 Managed Workstation Exchange Hosting Remote Backup Anti-Virus/Anti-Spam Network Monitoring IT Consulting               IT Assessments &amp; Audits  VOIP Services  CCTV Camera Systems  CTO/CIO Services  Network Cabling  Disaster Recovery Planning   IT Assessments &amp; Audits VOIP Services CCTV Camera Systems CTO/CIO Services Network Cabling Disaster Recovery Planning On-Site Services               Network Support  IT Staff Augmentation  Network Design/Build  Emergency Services  Technical Projects  Office Moves and Network Wiring   Network Support IT Staff Augmentation Network Design/Build Emergency Services Technical Projects Office Moves and Network Wiring Support Blog Contact                                                               Go                                              Reliable Support           Call us at: 613.321.6198                                  Prompt Response           Call us at: 613.321.6198                                  Efficient Services           Call us at: 613.321.6198                                  Professional Solutions           Call us at: 613.321.6198            File Encryption: How Can I Protect My Data?             How Firewalls Can Help Protect the Perimeter             Why Are Cloud Based Solutions So Popular?             5 Common Web Attacks to Watch Out For             Welcome to the team, Chris!        Microsoft Office 365 Managed Workstation Exchange Hosting Remote Backup Anti-virus/Anti-spam Network Monitoring IT Assessments VOIP Services Camera Systems CTO/CIO Services Network Cabling Disaster Recovery Planning Network Support IT Staff Augmentation Network Design/Build Emergency Services Technical Projects Office Moves and Network Wiring Rely on our IT experts to assist you with their experience and masterful knowledge. Our reliable solutions will result in immediate improvements for your business. Our help desk technicians are always standing by, ready to provide you with the highest quality personal assistance at any moment you suffer technical difficulties. We are a trusted advisor to hundreds of local businesses, offering on-going support &amp; advice for all IT-related needs. We work with businesses in a variety of industries, including healthcare, restaurants, professional services, legal, technology and manufacturing. © Copyright 2015. Revolution Networks. Online Marketing by seoplus+ sales@revnet.ca Home About Us Services  Cloud Services Microsoft Office 365 Managed Workstation Exchange Hosting Remote Backup Anti-Virus/Anti-Spam Network Monitoring IT Consulting IT Assessments &amp; Audits VOIP Services CCTV Camera Systems CTO/CIO Services Network Cabling Disaster Recovery Planning On-Site Services Network Support IT Staff Augmentation Network Design/Build Emergency Services Technical Projects Office Moves and Network Wiring Support Blog Contact Home About Us Services Cloud Services Microsoft Office 365 Managed Workstation Exchange Hosting Remote Backup Anti-Virus/Anti-Spam Network Monitoring IT Consulting IT Assessments &amp; Audits VOIP Services CCTV Camera Systems CTO/CIO Services Network Cabling Disaster Recovery Planning On-Site Services Network Support IT Staff Augmentation Network Design/Build Emergency Services Technical Projects Office Moves and Network Wiring Support Blog Contact 613.321.6198 613.321.6198 613.321.6198 613.321.6198 Microsoft Office 365 Managed Workstation Exchange Hosting Remote Backup Anti-virus/Anti-spam Network Monitoring Learn More IT Assessments VOIP Services Camera Systems CTO/CIO Services Network Cabling Disaster Recovery Planning Learn More Network Support IT Staff Augmentation Network Design/Build Emergency Services Technical Projects Office Moves and Network Wiring Learn More Learn More Learn More Learn More Learn More Learn More Learn More Learn More Learn More Learn More Learn More Learn More Learn More Contact us File Encryption: How Can I Protect My Data? How Firewalls Can Help Protect the Perimeter Why Are Cloud Based Solutions So Popular? 5 Common Web Attacks to Watch Out For Welcome to the team, Chris! 613.321.6198 sales@revnet.ca seoplus+ Toggle navigation Menu                                                          Go</v>
-      </c>
-      <c r="F27" t="str">
-        <v>Managed Services, IT Consulting &amp; Computer Support Ottawa Revolution Networks is Ottawa's premium provider of managed services, IT consulting and computer support in Ottawa. Our Advantages Features Your Local IT Support Experts Reliable Support To Enhance Your Business Prompt Response When You Need It Most Latest Posts: Location: Computer Support Network Services IT Services Managed Services IT Assessments Remote Backup Microsoft Office 365 Emergency Services Anti-Virus/Anti-Spam Exchange Hosting Network Design/Build Network Monitoring Network Wiring IT Consulting On-Site Computer Services sales@revnet.ca613-321-6198 sales@revnet.ca 613-321-6198 Home About Us Services Cloud Services     Microsoft Office 365   Managed Workstation   Exchange Hosting   Remote Backup   Anti-Virus/Anti-Spam   Network Monitoring     IT Consulting     IT Assessments &amp; Audits   VOIP Services   CCTV Camera Systems   CTO/CIO Services   Network Cabling   Disaster Recovery Planning     On-Site Services     Network Support   IT Staff Augmentation   Network Design/Build   Emergency Services   Technical Projects   Office Moves and Network Wiring      Support Blog Contact HomeAbout UsServices             Cloud Services               Microsoft Office 365  Managed Workstation  Exchange Hosting  Remote Backup  Anti-Virus/Anti-Spam  Network Monitoring   IT Consulting               IT Assessments &amp; Audits  VOIP Services  CCTV Camera Systems  CTO/CIO Services  Network Cabling  Disaster Recovery Planning   On-Site Services               Network Support  IT Staff Augmentation  Network Design/Build  Emergency Services  Technical Projects  Office Moves and Network Wiring   SupportBlogContact Home About Us Services    Cloud Services     Microsoft Office 365   Managed Workstation   Exchange Hosting   Remote Backup   Anti-Virus/Anti-Spam   Network Monitoring     IT Consulting     IT Assessments &amp; Audits   VOIP Services   CCTV Camera Systems   CTO/CIO Services   Network Cabling   Disaster Recovery Planning     On-Site Services     Network Support   IT Staff Augmentation   Network Design/Build   Emergency Services   Technical Projects   Office Moves and Network Wiring      Cloud Services     Microsoft Office 365   Managed Workstation   Exchange Hosting   Remote Backup   Anti-Virus/Anti-Spam   Network Monitoring    Microsoft Office 365 Managed Workstation Exchange Hosting Remote Backup Anti-Virus/Anti-Spam Network Monitoring IT Consulting     IT Assessments &amp; Audits   VOIP Services   CCTV Camera Systems   CTO/CIO Services   Network Cabling   Disaster Recovery Planning    IT Assessments &amp; Audits VOIP Services CCTV Camera Systems CTO/CIO Services Network Cabling Disaster Recovery Planning On-Site Services     Network Support   IT Staff Augmentation   Network Design/Build   Emergency Services   Technical Projects   Office Moves and Network Wiring    Network Support IT Staff Augmentation Network Design/Build Emergency Services Technical Projects Office Moves and Network Wiring Support Blog Contact Home About Us Services             Cloud Services               Microsoft Office 365  Managed Workstation  Exchange Hosting  Remote Backup  Anti-Virus/Anti-Spam  Network Monitoring   IT Consulting               IT Assessments &amp; Audits  VOIP Services  CCTV Camera Systems  CTO/CIO Services  Network Cabling  Disaster Recovery Planning   On-Site Services               Network Support  IT Staff Augmentation  Network Design/Build  Emergency Services  Technical Projects  Office Moves and Network Wiring    Cloud Services               Microsoft Office 365  Managed Workstation  Exchange Hosting  Remote Backup  Anti-Virus/Anti-Spam  Network Monitoring   Microsoft Office 365 Managed Workstation Exchange Hosting Remote Backup Anti-Virus/Anti-Spam Network Monitoring IT Consulting               IT Assessments &amp; Audits  VOIP Services  CCTV Camera Systems  CTO/CIO Services  Network Cabling  Disaster Recovery Planning   IT Assessments &amp; Audits VOIP Services CCTV Camera Systems CTO/CIO Services Network Cabling Disaster Recovery Planning On-Site Services               Network Support  IT Staff Augmentation  Network Design/Build  Emergency Services  Technical Projects  Office Moves and Network Wiring   Network Support IT Staff Augmentation Network Design/Build Emergency Services Technical Projects Office Moves and Network Wiring Support Blog Contact                                                               Go                                              Reliable Support           Call us at: 613.321.6198                                  Prompt Response           Call us at: 613.321.6198                                  Efficient Services           Call us at: 613.321.6198                                  Professional Solutions           Call us at: 613.321.6198            File Encryption: How Can I Protect My Data?             How Firewalls Can Help Protect the Perimeter             Why Are Cloud Based Solutions So Popular?             5 Common Web Attacks to Watch Out For             Welcome to the team, Chris!        Microsoft Office 365 Managed Workstation Exchange Hosting Remote Backup Anti-virus/Anti-spam Network Monitoring IT Assessments VOIP Services Camera Systems CTO/CIO Services Network Cabling Disaster Recovery Planning Network Support IT Staff Augmentation Network Design/Build Emergency Services Technical Projects Office Moves and Network Wiring Rely on our IT experts to assist you with their experience and masterful knowledge. Our reliable solutions will result in immediate improvements for your business. Our help desk technicians are always standing by, ready to provide you with the highest quality personal assistance at any moment you suffer technical difficulties. We are a trusted advisor to hundreds of local businesses, offering on-going support &amp; advice for all IT-related needs. We work with businesses in a variety of industries, including healthcare, restaurants, professional services, legal, technology and manufacturing. © Copyright 2015. Revolution Networks. Online Marketing by seoplus+ sales@revnet.ca Home About Us Services  Cloud Services Microsoft Office 365 Managed Workstation Exchange Hosting Remote Backup Anti-Virus/Anti-Spam Network Monitoring IT Consulting IT Assessments &amp; Audits VOIP Services CCTV Camera Systems CTO/CIO Services Network Cabling Disaster Recovery Planning On-Site Services Network Support IT Staff Augmentation Network Design/Build Emergency Services Technical Projects Office Moves and Network Wiring Support Blog Contact Home About Us Services Cloud Services Microsoft Office 365 Managed Workstation Exchange Hosting Remote Backup Anti-Virus/Anti-Spam Network Monitoring IT Consulting IT Assessments &amp; Audits VOIP Services CCTV Camera Systems CTO/CIO Services Network Cabling Disaster Recovery Planning On-Site Services Network Support IT Staff Augmentation Network Design/Build Emergency Services Technical Projects Office Moves and Network Wiring Support Blog Contact 613.321.6198 613.321.6198 613.321.6198 613.321.6198 Microsoft Office 365 Managed Workstation Exchange Hosting Remote Backup Anti-virus/Anti-spam Network Monitoring Learn More IT Assessments VOIP Services Camera Systems CTO/CIO Services Network Cabling Disaster Recovery Planning Learn More Network Support IT Staff Augmentation Network Design/Build Emergency Services Technical Projects Office Moves and Network Wiring Learn More Learn More Learn More Learn More Learn More Learn More Learn More Learn More Learn More Learn More Learn More Learn More Learn More Contact us File Encryption: How Can I Protect My Data? How Firewalls Can Help Protect the Perimeter Why Are Cloud Based Solutions So Popular? 5 Common Web Attacks to Watch Out For Welcome to the team, Chris! 613.321.6198 sales@revnet.ca seoplus+ Toggle navigation Menu                                                          Go</v>
+        <v>Managed Services IT Consulting Computer Support Ottawa Revolution Networks is Ottawas premium provider of managed services IT consulting and computer support in Ottawa Our Advantages Features Your Local IT Support Experts Reliable Support To Enhance Your Business Prompt Response When You Need It Most Latest Posts Location Computer Support Network Services IT Services Managed Services IT Assessments Remote Backup Microsoft Office 365 Emergency Services AntiVirusAntiSpam Exchange Hosting Network DesignBuild Network Monitoring Network Wiring IT Consulting OnSite Computer Services salesrevnetca6133216198 salesrevnetca 6133216198 Home About Us Services Cloud Services Microsoft Office 365 Managed Workstation Exchange Hosting Remote Backup AntiVirusAntiSpam Network Monitoring IT Consulting IT Assessments Audits VOIP Services CCTV Camera Systems CTOCIO Services Network Cabling Disaster Recovery Planning OnSite Services Network Support IT Staff Augmentation Network DesignBuild Emergency Services Technical Projects Office Moves and Network Wiring Support Blog Contact HomeAbout UsServices Cloud Services Microsoft Office 365 Managed Workstation Exchange Hosting Remote Backup AntiVirusAntiSpam Network Monitoring IT Consulting IT Assessments Audits VOIP Services CCTV Camera Systems CTOCIO Services Network Cabling Disaster Recovery Planning OnSite Services Network Support IT Staff Augmentation Network DesignBuild Emergency Services Technical Projects Office Moves and Network Wiring SupportBlogContact Home About Us Services Cloud Services Microsoft Office 365 Managed Workstation Exchange Hosting Remote Backup AntiVirusAntiSpam Network Monitoring IT Consulting IT Assessments Audits VOIP Services CCTV Camera Systems CTOCIO Services Network Cabling Disaster Recovery Planning OnSite Services Network Support IT Staff Augmentation Network DesignBuild Emergency Services Technical Projects Office Moves and Network Wiring Cloud Services Microsoft Office 365 Managed Workstation Exchange Hosting Remote Backup AntiVirusAntiSpam Network Monitoring Microsoft Office 365 Managed Workstation Exchange Hosting Remote Backup AntiVirusAntiSpam Network Monitoring IT Consulting IT Assessments Audits VOIP Services CCTV Camera Systems CTOCIO Services Network Cabling Disaster Recovery Planning IT Assessments Audits VOIP Services CCTV Camera Systems CTOCIO Services Network Cabling Disaster Recovery Planning OnSite Services Network Support IT Staff Augmentation Network DesignBuild Emergency Services Technical Projects Office Moves and Network Wiring Network Support IT Staff Augmentation Network DesignBuild Emergency Services Technical Projects Office Moves and Network Wiring Support Blog Contact Home About Us Services Cloud Services Microsoft Office 365 Managed Workstation Exchange Hosting Remote Backup AntiVirusAntiSpam Network Monitoring IT Consulting IT Assessments Audits VOIP Services CCTV Camera Systems CTOCIO Services Network Cabling Disaster Recovery Planning OnSite Services Network Support IT Staff Augmentation Network DesignBuild Emergency Services Technical Projects Office Moves and Network Wiring Cloud Services Microsoft Office 365 Managed Workstation Exchange Hosting Remote Backup AntiVirusAntiSpam Network Monitoring Microsoft Office 365 Managed Workstation Exchange Hosting Remote Backup AntiVirusAntiSpam Network Monitoring IT Consulting IT Assessments Audits VOIP Services CCTV Camera Systems CTOCIO Services Network Cabling Disaster Recovery Planning IT Assessments Audits VOIP Services CCTV Camera Systems CTOCIO Services Network Cabling Disaster Recovery Planning OnSite Services Network Support IT Staff Augmentation Network DesignBuild Emergency Services Technical Projects Office Moves and Network Wiring Network Support IT Staff Augmentation Network DesignBuild Emergency Services Technical Projects Office Moves and Network Wiring Support Blog Contact Go Reliable Support Call us at 6133216198 Prompt Response Call us at 6133216198 Efficient Services Call us at 6133216198 Professional Solutions Call us at 6133216198 File Encryption How Can I Protect My Data How Firewalls Can Help Protect the Perimeter Why Are Cloud Based Solutions So Popular 5 Common Web Attacks to Watch Out For Welcome to the team Chris Microsoft Office 365 Managed Workstation Exchange Hosting Remote Backup AntivirusAntispam Network Monitoring IT Assessments VOIP Services Camera Systems CTOCIO Services Network Cabling Disaster Recovery Planning Network Support IT Staff Augmentation Network DesignBuild Emergency Services Technical Projects Office Moves and Network Wiring Rely on our IT experts to assist you with their experience and masterful knowledge Our reliable solutions will result in immediate improvements for your business Our help desk technicians are always standing by ready to provide you with the highest quality personal assistance at any moment you suffer technical difficulties We are a trusted advisor to hundreds of local businesses offering ongoing support advice for all ITrelated needs We work with businesses in a variety of industries including healthcare restaurants professional services legal technology and manufacturing © Copyright 2015 Revolution Networks Online Marketing by seoplus salesrevnetca Home About Us Services Cloud Services Microsoft Office 365 Managed Workstation Exchange Hosting Remote Backup AntiVirusAntiSpam Network Monitoring IT Consulting IT Assessments Audits VOIP Services CCTV Camera Systems CTOCIO Services Network Cabling Disaster Recovery Planning OnSite Services Network Support IT Staff Augmentation Network DesignBuild Emergency Services Technical Projects Office Moves and Network Wiring Support Blog Contact Home About Us Services Cloud Services Microsoft Office 365 Managed Workstation Exchange Hosting Remote Backup AntiVirusAntiSpam Network Monitoring IT Consulting IT Assessments Audits VOIP Services CCTV Camera Systems CTOCIO Services Network Cabling Disaster Recovery Planning OnSite Services Network Support IT Staff Augmentation Network DesignBuild Emergency Services Technical Projects Office Moves and Network Wiring Support Blog Contact 6133216198 6133216198 6133216198 6133216198 Microsoft Office 365 Managed Workstation Exchange Hosting Remote Backup AntivirusAntispam Network Monitoring Learn More IT Assessments VOIP Services Camera Systems CTOCIO Services Network Cabling Disaster Recovery Planning Learn More Network Support IT Staff Augmentation Network DesignBuild Emergency Services Technical Projects Office Moves and Network Wiring Learn More Learn More Learn More Learn More Learn More Learn More Learn More Learn More Learn More Learn More Learn More Learn More Learn More Contact us File Encryption How Can I Protect My Data How Firewalls Can Help Protect the Perimeter Why Are Cloud Based Solutions So Popular 5 Common Web Attacks to Watch Out For Welcome to the team Chris 6133216198 salesrevnetca seoplus Toggle navigation Menu Go</v>
       </c>
     </row>
     <row r="28">
@@ -913,16 +688,7 @@
         <v>Match true</v>
       </c>
       <c r="C28" t="str">
-        <v>App Annie - The App Analytics and App Data Industry Standard App Annie is the standard in app analytics and app market data, giving you one easy-to-use platform for running every stage of your app business. App Annie, App Analytics, App Data                                        Market Data                         Analytics                         Insights                              Tours                                                            Market Data                                                    Store Stats                                                        Store Stats Pro From $59                                                        ASO                                                                                                                                    Enterprise Market Data Premium                                                    Store Intelligence                                                        Usage Intelligence                                                        Audience Intelligence                                                                                                                                    App Analytics Platform                                                    App Store Analytics                                                        Advertising Analytics                                                        In-App Analytics Beta                                                                                                                                 Market Data                                                    Store Stats                                                        Store Stats Pro From $59                                                        ASO                                                                                                                                   Store Stats                                       Store Stats Pro From $59                                       ASO                                                                      Enterprise Market Data Premium                                                    Store Intelligence                                                        Usage Intelligence                                                        Audience Intelligence                                                                                                                                   Store Intelligence                                       Usage Intelligence                                       Audience Intelligence                                                                      App Analytics Platform                                                    App Store Analytics                                                        Advertising Analytics                                                        In-App Analytics Beta                                                                                                                                   App Store Analytics                                       Advertising Analytics                                       In-App Analytics Beta                                                                       Pricing                              About                                                                                                                        About                                                                                                          Leadership                                                                                                          Jobs                                                                                                          Customers                                                                                                          Partnerships                                                                                                          Press                                                                                                          Contact                                                                                                       About                                                                                                 Leadership                                                                                                 Jobs                                                                                                 Customers                                                                                                 Partnerships                                                                                                 Press                                                                                                 Contact                                      Blog                              Market Data                                       Analytics                                       Insights                                       Register                                       Login                                       Logout                                                                                                                                                         RegisterLogin                                                                                                                                                                                                                                                                         Store Stats                                                                                                                                                                                                                                                                                   Store Stats                                                                                                                                                                                                                                                                 Index                                                                                                                                                                                                                                                                                   Index                                                                                                                                                                                                                                                                                                                                                                                                                                                        Premium                                     Intelligence                                                                                                                                                                                                                                                                                                                                                         Premium                                     Intelligence                                                                                                                                                                                                                                                                                                                                                 App Analytics                                                                                                                                                                                                                                                                                   App Analytics                                                                                                                                                                                                                                                                 Advertising Analytics                                                                                                                                                                                                                                                                                   Advertising Analytics                                                                                                                                                                                                                                                                                                                                                Market Data                                                                                                                                                                                                                                                                                                                                                      Store Stats                                                                                                                                                                                                                                                                                                Store Stats Pro From $59                                                                                                                                                                                                                                                                                                ASO                                                                                                                                                                                                                                                                                                                                                                                                                           Market Data                                                                                                                                                                                                                                                                                                                         Store Stats                                                                                                                                                                                                                                                                                                Store Stats Pro From $59                                                                                                                                                                                                                                                                                                ASO                                                                                                                                                                                                                                                                                                                                                           Store Stats                                                                                                                                                                                                                                                           Store Stats Pro From $59                                                                                                                                                                                                                                                           ASO                                                                                                                                                                                                                                                                         Enterprise Market Data Premium                                                                                                                                                                                                                                                                                                                                                      Store Intelligence                                                                                                                                                                                                                                                                                                Usage Intelligence                                                                                                                                                                                                                                                                                                Audience Intelligence                                                                                                                                                                                                                                                                                                                                                                                           Enterprise Market Data Premium                                                                                                                                                                                                                                                                                                                         Store Intelligence                                                                                                                                                                                                                                                                                                Usage Intelligence                                                                                                                                                                                                                                                                                                Audience Intelligence                                                                                                                                                                                                                                                                                                                                                           Store Intelligence                                                                                                                                                                                                                                                           Usage Intelligence                                                                                                                                                                                                                                                           Audience Intelligence                                                                                                                                                                                                                                                                         App Analytics Platform                                                                                                                                                                                                                                                                                                                                                      App Store Analytics                                                                                                                                                                                                                                                                                                Advertising Analytics                                                                                                                                                                                                                                                                                                In-App Analytics Beta                                                                                                                                                                                                                                                                                                                                                                                           App Analytics Platform                                                                                                                                                                                                                                                                                                                         App Store Analytics                                                                                                                                                                                                                                                                                                Advertising Analytics                                                                                                                                                                                                                                                                                                In-App Analytics Beta                                                                                                                                                                                                                                                                                                                                                           App Store Analytics                                                                                                                                                                                                                                                           Advertising Analytics                                                                                                                                                                                                                                                           In-App Analytics Beta                                                                                                                                                                                                                                                                                                                        About                                                                                                                                                                                                                                                                                   About                                                                                                                                                                                                                                                             Leadership                                                                                                                                                                                                                                                                               Leadership                                                                                                                                                                                                                                                                 Jobs                                                                                                                                                                                                                                                                                   Jobs                                                                                                                                                                                                                                                                 Customers                                                                                                                                                                                                                                                                                   Customers                                                                                                                                                                                                                                                                 Partnerships                                                                                                                                                                                                                                                                                   Partnerships                                                                                                                                                                                                                                                                 Press                                                                                                                                                                                                                                                                                   Press                                                                                                                                                                                                                                                                 Contact                                                                                                                                                                                                                                                                                   Contact                                                                                                                                                                                                                                                                                    Store Stats FREE           Monitor the app ecosystem and your competitors.           Check hourly or daily top charts as well as ranking history, search keywords and featured placements for millions of apps.                                                                         More details                                                   Use for free                                                                                                                                                 More details                               Use for free                                                                                                                                                                                                                     Store Stats Pro FROM $59           Track your competitors’ performance in the app stores.           Instantly access precise estimates of your competitors' daily app downloads and revenue to understand app performance, starting from $59 per month.                                                                         More details                                                   Purchase now                                                                                                                                                 More details                               Purchase now                                                                                                                                                                                                                     Store Intelligence PREMIUM            Complete app store transparency on every download and dollar.            Unparalleled insight with the most accurate estimates of app sales and revenue performance. Available for millions of apps, hundreds of thousands of companies, 155 countries and over 40 categories.                                                                         More details                                                   Schedule a demo                                                                                                                                                 More details                               Schedule a demo                                                                                                                                                                                                                     Usage Intelligence NEW            A revolutionary understanding of mobile app and device usage.           Deep insights into an app's users, engagement, reach and retention. Follow daily, weekly and monthly updates on the apps you care about, broken down by app, device and country.                                                                         More details                                                   Schedule a demo                                                                                                                                                 More details                               Schedule a demo                                                                                                                                                                                                                     Audience Intelligence PREMIUM            Detailed data about who is using every major mobile app.            Estimates on user demographics, cross-app adoption, and users' opinions of app quality. Get app-level data for thousands of apps to understand everything from user gender and age to income and education level.                                                                         More details                                                   Schedule a demo                                                                                                                                                 More details                               Schedule a demo                                                                                                                                                                                                                     App Store Analytics Free           Powerful visualizations to analyze your app store sales data — all in one place.           Monitor downloads, revenue, reviews, search keywords and more across your entire app portfolio, simply organized in one dashboard and without the need for an SDK.                                                                         More details                                                   Set up your dashboard                                                                                                                                                 More details                               Set up your dashboard                                                                                                                                                                                                                     Advertising Analytics Free           Unified dashboard for all your mobile advertising and monetization data.           No more manual aggregation ever! Get your ad spend, revenue, CPI, eCPM, and fill rates from multiple ad platforms automatically in one single dashboard.                                                                         More details                                                   Connect your advertising data                                                                                                                                                 More details                               Connect your advertising data                                                                                                                                                                                                                     In-App Analytics BETA           Monitor the usage metrics that matter most for your app business.           Track the health of your user base by adding app usage metrics to your App Analytics dashboard. Instantly surface insights such as whether version updates impact your average session duration, or how active users correlate with revenue.                                                                         Learn more                                                    Connect your usage metrics                                                                                                                                                 Learn more                                Connect your usage metrics                       Home                            Market Data                        Enterprise Market Data                            App Analytics Platform                        Pricing               About               Leadership               Jobs               Partnerships               Press               Contact               Blog               Support               Intelligence FAQ               Analytics API               Intelligence API               Intelligence Announcements               Security               Data Usage Policy               Copyright Policy                            English                                     日本語                                     한국어                                     中文(简体)                                     Pусский                                     Français                                     Deutsch                        © 2016 App Annie               Terms of Service               Privacy Policy                                                                                                                                                                                                                                                                                                                                                                                                                                  Market Data           Analytics           Insights                    Tours                                 Market Data Store Stats Store Stats Pro From $59 ASO Enterprise Market Data Premium Store Intelligence Usage Intelligence Audience Intelligence App Analytics Platform App Store Analytics Advertising Analytics In-App Analytics Beta          Pricing                        About                                 About Leadership Jobs Customers Partnerships Press Contact          Blog                        Market Data                                 Analytics                                 Insights                                 Register                                 Login                                 Logout                                       Register Login Store Stats Index                                      Premium                                     Intelligence                                  App Analytics Advertising Analytics Market Data Store Stats Store Stats Pro From $59 ASO Enterprise Market Data Premium Store Intelligence Usage Intelligence Audience Intelligence App Analytics Platform App Store Analytics Advertising Analytics In-App Ana</v>
-      </c>
-      <c r="D28" t="str">
-        <v>lytics Beta About Leadership Jobs Customers Partnerships Press Contact                    Sign up, it's free!               Download &amp; discover top app trends.                    JOIN OUR TEAM. SEE ALL JOBS.               More details Use for free More details Purchase now More details Schedule a demo More details Schedule a demo More details Schedule a demo More details Set up your dashboard More details Connect your advertising data Learn more  Connect your usage metrics Take me there                    Sign up for free               Home              Market Data          Enterprise Market Data              App Analytics Platform          Pricing About Leadership Jobs Partnerships Press Contact Blog Support Intelligence FAQ Analytics API Intelligence API Intelligence Announcements Security Data Usage Policy Copyright Policy              English                       日本語                       한국어                       中文(简体)                       Pусский                       Français                       Deutsch          Terms of Service Privacy Policy                                                                                                                                                                                                        Toggle navigation Market Data Analytics Insights Tours Market Data From $59 Premium App Analytics Platform Beta Pricing About                                                                                                                                                                                                                                                                                                                                                 Blog Market Data Analytics Insights Register Login Logout                                                                                                                                                                                                                                                                                                                                     Premium                                                                                                                                                                                                                                                                                                                                                             Market Data                                                                                                                                                                                                                                                                         From $59                                                                                                                                                                                                                                                 Premium                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                         App Analytics Platform                                                                                                                                                                                                                                                                                                                                                                                                             Beta                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                     Sign up, it's free!     1,000,000  1,000,000     94%  94%     500,000      500,000  500,000 JOIN OUR TEAM. SEE ALL JOBS. FREE FROM $59 PREMIUM NEW PREMIUM Free Free BETA Sign up for free Market Data App Analytics Platform English 日本語 한국어 中文(简体) Pусский Français Deutsch © 2016 App Annie</v>
-      </c>
-      <c r="E28" t="str">
-        <v>lytics Beta About Leadership Jobs Customers Partnerships Press Contact                    Sign up, it's free!               Download &amp; discover top app trends.                    JOIN OUR TEAM. SEE ALL JOBS.               More details Use for free More details Purchase now More details Schedule a demo More details Schedule a demo More details Schedule a demo More details Set up your dashboard More details Connect your advertising data Learn more  Connect your usage metrics Take me there                    Sign up for free               Home              Market Data          Enterprise Market Data              App Analytics Platform          Pricing About Leadership Jobs Partnerships Press Contact Blog Support Intelligence FAQ Analytics API Intelligence API Intelligence Announcements Security Data Usage Policy Copyright Policy              English                       日本語                       한국어                       中文(简体)                       Pусский                       Français                       Deutsch          Terms of Service Privacy Policy                                                                                                                                                                                                        Toggle navigation Market Data Analytics Insights Tours Market Data From $59 Premium App Analytics Platform Beta Pricing About                                                                                                                                                                                                                                                                                                                                                 Blog Market Data Analytics Insights Register Login Logout                                                                                                                                                                                                                                                                                                                                     Premium                                                                                                                                                                                                                                                                                                                                                             Market Data                                                                                                                                                                                                                                                                         From $59                                                                                                                                                                                                                                                 Premium                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                         App Analytics Platform                                                                                                                                                                                                                                                                                                                                                                                                             Beta                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                     Sign up, it's free!     1,000,000  1,000,000     94%  94%     500,000      500,000  500,000 JOIN OUR TEAM. SEE ALL JOBS. FREE FROM $59 PREMIUM NEW PREMIUM Free Free BETA Sign up for free Market Data App Analytics Platform English 日本語 한국어 中文(简体) Pусский Français Deutsch © 2016 App Annie</v>
-      </c>
-      <c r="F28" t="str">
-        <v>lytics Beta About Leadership Jobs Customers Partnerships Press Contact                    Sign up, it's free!               Download &amp; discover top app trends.                    JOIN OUR TEAM. SEE ALL JOBS.               More details Use for free More details Purchase now More details Schedule a demo More details Schedule a demo More details Schedule a demo More details Set up your dashboard More details Connect your advertising data Learn more  Connect your usage metrics Take me there                    Sign up for free               Home              Market Data          Enterprise Market Data              App Analytics Platform          Pricing About Leadership Jobs Partnerships Press Contact Blog Support Intelligence FAQ Analytics API Intelligence API Intelligence Announcements Security Data Usage Policy Copyright Policy              English                       日本語                       한국어                       中文(简体)                       Pусский                       Français                       Deutsch          Terms of Service Privacy Policy                                                                                                                                                                                                        Toggle navigation Market Data Analytics Insights Tours Market Data From $59 Premium App Analytics Platform Beta Pricing About                                                                                                                                                                                                                                                                                                                                                 Blog Market Data Analytics Insights Register Login Logout                                                                                                                                                                                                                                                                                                                                     Premium                                                                                                                                                                                                                                                                                                                                                             Market Data                                                                                                                                                                                                                                                                         From $59                                                                                                                                                                                                                                                 Premium                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                         App Analytics Platform                                                                                                                                                                                                                                                                                                                                                                                                             Beta                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                     Sign up, it's free!     1,000,000  1,000,000     94%  94%     500,000      500,000  500,000 JOIN OUR TEAM. SEE ALL JOBS. FREE FROM $59 PREMIUM NEW PREMIUM Free Free BETA Sign up for free Market Data App Analytics Platform English 日本語 한국어 中文(简体) Pусский Français Deutsch © 2016 App Annie</v>
+        <v>App Annie The App Analytics and App Data Industry Standard App Annie is the standard in app analytics and app market data giving you one easytouse platform for running every stage of your app business App Annie App Analytics App Data Market Data Analytics Insights Tours Market Data Store Stats Store Stats Pro From 59 ASO Enterprise Market Data Premium Store Intelligence Usage Intelligence Audience Intelligence App Analytics Platform App Store Analytics Advertising Analytics InApp Analytics Beta Market Data Store Stats Store Stats Pro From 59 ASO Store Stats Store Stats Pro From 59 ASO Enterprise Market Data Premium Store Intelligence Usage Intelligence Audience Intelligence Store Intelligence Usage Intelligence Audience Intelligence App Analytics Platform App Store Analytics Advertising Analytics InApp Analytics Beta App Store Analytics Advertising Analytics InApp Analytics Beta Pricing About About Leadership Jobs Customers Partnerships Press Contact About Leadership Jobs Customers Partnerships Press Contact Blog Market Data Analytics Insights Register Login Logout RegisterLogin Store Stats Store Stats Index Index Premium Intelligence Premium Intelligence App Analytics App Analytics Advertising Analytics Advertising Analytics Market Data Store Stats Store Stats Pro From 59 ASO Market Data Store Stats Store Stats Pro From 59 ASO Store Stats Store Stats Pro From 59 ASO Enterprise Market Data Premium Store Intelligence Usage Intelligence Audience Intelligence Enterprise Market Data Premium Store Intelligence Usage Intelligence Audience Intelligence Store Intelligence Usage Intelligence Audience Intelligence App Analytics Platform App Store Analytics Advertising Analytics InApp Analytics Beta App Analytics Platform App Store Analytics Advertising Analytics InApp Analytics Beta App Store Analytics Advertising Analytics InApp Analytics Beta About About Leadership Leadership Jobs Jobs Customers Customers Partnerships Partnerships Press Press Contact Contact Store Stats FREE Monitor the app ecosystem and your competitors Check hourly or daily top charts as well as ranking history search keywords and featured placements for millions of apps More details Use for free More details Use for free Store Stats Pro FROM 59 Track your competitors’ performance in the app stores Instantly access precise estimates of your competitors daily app downloads and revenue to understand app performance starting from 59 per month More details Purchase now More details Purchase now Store Intelligence PREMIUM Complete app store transparency on every download and dollar Unparalleled insight with the most accurate estimates of app sales and revenue performance Available for millions of apps hundreds of thousands of companies 155 countries and over 40 categories More details Schedule a demo More details Schedule a demo Usage Intelligence NEW A revolutionary understanding of mobile app and device usage Deep insights into an apps users engagement reach and retention Follow daily weekly and monthly updates on the apps you care about broken down by app device and country More details Schedule a demo More details Schedule a demo Audience Intelligence PREMIUM Detailed data about who is using every major mobile app Estimates on user demographics crossapp adoption and users opinions of app quality Get applevel data for thousands of apps to understand everything from user gender and age to income and education level More details Schedule a demo More details Schedule a demo App Store Analytics Free Powerful visualizations to analyze your app store sales data all in one place Monitor downloads revenue reviews search keywords and more across your entire app portfolio simply organized in one dashboard and without the need for an SDK More details Set up your dashboard More details Set up your dashboard Advertising Analytics Free Unified dashboard for all your mobile advertising and monetization data No more manual aggregation ever Get your ad spend revenue CPI eCPM and fill rates from multiple ad platforms automatically in one single dashboard More details Connect your advertising data More details Connect your advertising data InApp Analytics BETA Monitor the usage metrics that matter most for your app business Track the health of your user base by adding app usage metrics to your App Analytics dashboard Instantly surface insights such as whether version updates impact your average session duration or how active users correlate with revenue Learn more Connect your usage metrics Learn more Connect your usage metrics Home Market Data Enterprise Market Data App Analytics Platform Pricing About Leadership Jobs Partnerships Press Contact Blog Support Intelligence FAQ Analytics API Intelligence API Intelligence Announcements Security Data Usage Policy Copyright Policy English 日本語 한국어 中文简体 Pусский Français Deutsch © 2016 App Annie Terms of Service Privacy Policy Market Data Analytics Insights Tours Market Data Store Stats Store Stats Pro From 59 ASO Enterprise Market Data Premium Store Intelligence Usage Intelligence Audience Intelligence App Analytics Platform App Store Analytics Advertising Analytics InApp Analytics Beta Pricing About About Leadership Jobs Customers Partnerships Press Contact Blog Market Data Analytics Insights Register Login Logout Register Login Store Stats Index Premium Intelligence App Analytics Advertising Analytics Market Data Store Stats Store Stats Pro From 59 ASO Enterprise Market Data Premium Store Intelligence Usage Intelligence Audience Intelligence App Analytics Platform App Store Analytics Advertising Analytics InApp Analytics Beta About Leadership Jobs Customers Partnerships Press Contact Sign up its free Download discover top app trends JOIN OUR TEAM SEE ALL JOBS More details Use for free More details Purchase now More details Schedule a demo More details Schedule a demo More details Schedule a demo More details Set up your dashboard More details Connect your advertising data Learn more Connect your usage metrics Take me there Sign up for free Home Market Data Enterprise Market Data App Analytics Platform Pricing About Leadership Jobs Partnerships Press Contact Blog Support Intelligence FAQ Analytics API Intelligence API Intelligence Announcements Security Data Usage Policy Copyright Policy English 日本語 한국어 中文简体 Pусский Français Deutsch Terms of Service Privacy Policy Toggle navigation Market Data Analytics Insights Tours Market Data From 59 Premium App Analytics Platform Beta Pricing About Blog Market Data Analytics Insights Register Login Logout Premium Market Data From 59 Premium App Analytics Platform Beta Sign up its free 1000000 1000000 94 94 500000 500000 500000 JOIN OUR TEAM SEE ALL JOBS FREE FROM 59 PREMIUM NEW PREMIUM Free Free BETA Sign up for free Market Data App Analytics Platform English 日本語 한국어 中文简体 Pусский Français Deutsch © 2016 App Annie</v>
       </c>
     </row>
   </sheetData>

</xml_diff>